<commit_message>
Songs, pipeline and stuff
</commit_message>
<xml_diff>
--- a/data/02_intermediate/cleaned_2zer_Washington_songs.xlsx
+++ b/data/02_intermediate/cleaned_2zer_Washington_songs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Grünt #11</t>
+          <t>Démarre</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Les ados rêvent de packs d'eau, c'est rare qu'on rafle l'oseille Pauvre dans l'apparence, enchaîne série d'abdomens, achète du Ralph Lauren Un peu d'Poliakov et j'm'évade, pas d'Maybach, c'est pas trop hardcore J'préfère Ärsenik, les polos Lacoste Avec les femmes j'ai pas trop la côte Pas grave, j'ai fait un tas d'choix Comme Brassens, dis leur Bazoo, c'est les potos d'abord Si tu m'trahis, j'te pardonne pas, j'suis pas fou et con T'auras fait ton temps mais j'coupe les ponts J'pense pas qu'les clodos m'adorent On s'en fout des s'condes, c'qui fait mal c'est quand l'passé surgit L'Rap j'suis fou d'lui et c'est pas d'sa faute, si on fait qu'se frapper sous tise Entre schlags, les sous-fifres, j'tourne en rond, comme la BAC dans le tiek's J'veux pas quitter Paris, j'veux juste un appart' dans le 16 Entre nous y a pas dentraide, le problème, c'est que j'dors plus et qu'les rêves j'ai peur d'en faire En plus j'ai pas attendu qu'mes parents crèvent pour pleurer, j'suis écuré Quand ma tête est en paix, mon cur et mes couilles partent en guerre J'me sens sale quand je cède à mes plus sombres désirs Ici, les gens se trompent et dérivent, car c'est le vice qui comble les vides Et le temps passe, ouais, je peux te dire que je veux le titre d'innovateur Moi, sous beuh je rime avant qu'le feu se vide, faut qu'on m'idolâtre J'évite les mythomanes, ils perdent des kilogrammes À force de nous envier et de mendier, c'est immoral J'prends ça à la rigolade, vu que ces psychopathes Disent de la merde, microphone en guise de vibromasseur J'ai ce sentiment de faire mauvaise impression Mais pourtant pour qu'j'fasse de la merde faudrait droguer l'ingé' son J'aime fracasser la rime et saccager Paris J'vais pas passer ma vie à me poser plein d'questions Mais je sais que je suis l'un des meilleurs Tous les mecs qui me suivent, flinguent les haters Pour cramer tous tes mensonges Y a même pas besoin d'un détecteur Comme d'habitude j'remue le couteau dans la plaie Trop de flow, j'baise des tas d'tes-pu sous l'eau, en apnée La poisse me hante quand la chance me manque Si j'suis pauvre je braque une banque Ramène ta bande dans ma planque Y a d'la blanche, y a d'la plante La légende j'prends gent-gent-ar Comme un gen-gendarme, j'ai mon arme Ma tante gère ton ron-da pour avoir les fafs, normal J'jette mon sac quand j'rentre chez moi J'ai eu mon bac, j'sais pas pourquoi J'viens d'la où mes profs n'iront pas, nieront pas Que du sale en moi, grosse casquette à l'endroit J'suis pas la mode, gros, c'est elle qui suit mes endroits Dans le film Troie, j'peux être qu'Achille Si j'étais un pays, j'serais la Chine Trop technique, fuck le Brazil Chez nous c'est pas les femmes qui font la cuisine T'as jamais vu mon slogan, j'maîtrise le flow comme un volant Quand t'as d'la peu-fra, les négros deviennent collants J'brille comme mon schlass, négro, t'as rien d'innovant Fuck le présent, on s'reverra dans 10 ans Dans 10 ans, j'aurais des femmes, une terre, un état Comme Moïse ouvre la mer J'ouvre les flammes comme un Sheïtan Les conseils les moins précis sont les plus précipités Fumer un joint, ça fait du bien, fumer une meuf, ça fait pitié Ouais, ouais, la vie rose comme du PQ Leur morale j'me torche avec Donne un quart de ton salaire et la Porsche qui va avec Entre la main et l'cendrier, ma main fait la navette La Mannschaft, on vise dans le mille Ramène une pomme, une arbalète Une console et deux manettes que la nuit soit plus rapide Des massas et de la garett', des canettes de chez Rachid Rageant, quand pas d'argent mais, après l'orage, beau temps Des potos, j'en ai beaucoup alors ça fera du boucan Si t'es comme moi, tu comprends, si t'es maso, t'es content Tu perds tes dents après ce couplet tu peux plus manger croquant Les petits de Paris qui aiment baiser les lois, monter sur les toits Ou descendre dans l'parking, le résultat sera le même Un oint-j de pollen une canette de coca Candidat à la principauté d'la ville comme les mecs du 1-1-3 Le monde tourne à l'envers mais j'ai la cervelle à l'endroit C'est la rue qui m'emploie, le vent sur mon 33 On s'aimera et après, la pillave comme seul remède J'appelle mon soss Arcel pour une soirée Jack Daniels Alors buvons, festoyons jusqu'à l'épuisement Attention à l'ascension d'mes garnements Imminente et rapide, musicothérapie Ils sont bons qu'à rapper, racler pour des raclis C'est des pédales, yeuf et garette-ci J'fume avec Pégase et Yeuk Au 18e étage, j'ai tout baisé, j'avais pas l'âge 7-5 capitale, ouais ouais, y a d'la came Des vils-ci dans les parages du lobby en dépannage La vie, c'est une étape, faut faire un bon démarrage RDV à l'arrivée pour le vol à l'étalage de l'année Celui qui nous ref'ra J'avais faim j'ai sauté le repas, j'ai mangé le refrain Fais une photo, où je tape la pose Tah les anciens avec mon joint On grandit vite parce que ça nous va bien Du 14e, j'suis toujours dans mon coin Ou pas loin vers les quartiers voisins Nous, on bosse, demande à Sélin, sous un soleil d'hiver J'ai mis une p'tite paire de lunettes vertes Nique sa mère c'est L'Animal, j'fume de la verte ou du taga Les MC, on les tabasse, poto On vient reprendre le taff que les saletés s'approprient J'aime le Rap, moi, je m'en tape des sapes d'AAP Rocky J'suis pas un mec à Nike, moi, j'suis un mec à meufs J'roule des mécaniques avec mes canailles Petit bisou dans l'cou et les 'tagasses gémissent Eux, ils baisent des miss dont le clito' fait la taille d'un pénis C'est pour mes muslim, mes 'feu-j et mes catho' Qui pé-ra le soir, tu ne connais pas, gros On apprécie l'ancienne école et les sciences hideuses Ambiance pestilentielle comme un pet silencieux C'est notre passion donc on a mis des loves La chienne est la meilleure amie de l'homme Ça rappe H24, mes collègues sont épuisants On élargit le réseau donc les connexions sont puissantes Cousin, ça gère la pub, Cheval de Troie pour faire la une Tu baves ? J'ai vu ta mère la pute racoler sous des buissons OK, c'est sus-Vers qu'enclenche le processus vers l'ascension Au lieu d'cer-su, les frères, vous devriez tous faire attention Chouf, mec, la tension monte à chaque apparition Ça devient plus foulek comme une russe roulette Gare aux bombes Gros, c'est Tristan Tzara, j'suis triste quand ça rappe mal Dédicace à tous mes bicots, juifs, bambaras, man Qui savent faire la maille et qui n'aiment pas qu'on les dévisage En gros, tous les mecs qui s'tapent tard la night Fils, sache qu'à la base on est pas des salauds C'est juste le goût dans notre bouche qui est salé Donc on s'laisse aller, on vit ça à l'arrache On est devenus des mecs tout bizarres Les prototypes à la vache chaude Tu joues les mauvais garçons, espèce de pédé Mais devant mon avance y aura plus personne pour t'aider Gros, c'est automatique, la rime hors pair Provoque chez toi des dégâts post-traumatiques Poste sur ma clique, breh, on t'dépose sur l'maquis J'ai le mic' dans la paume, des grosses phases dans la peau Là, si t'attends ta dose, signé Framal quand ta go À son biberon, à son p'tit-déj', trop d'auditions au poste Des missions en bande, j'donne mon opinion à l'opinel Check mes phases je t'étale des vrais versets crades Et t'es pas né, moi, c'est Framal, j'ai des tas de techniques Mon talent t'épate, le Rap c'est ma life et t'es pas prêt J'prends ta femme pour nettoyer mes meubles Déjà en primaire ça parlait d'moi dans les toilettes des meufs Les temps changent, malheureusement, les gens aussi J'la baise, elle a pas ses règles, elle est pourtant en sang sur me Trop d'pépins, j'avais la pèche, j'ai bouffé l'noyau En sueur parce que y a pas qu'à la piscine Qu'on mouille le maillot C'est quoi les bili-bails ? Tu comptes cer-per comme a-ç ? Non, l'amour c'est pas gratuit, demande à ces chères connasses Paré pour l'décollage, une teille de Zubrow, plus d'lycée J'suis sous l'porche, nique sa mère, j'rendais fou l'prof Tu vois l'délire ou pas ? Les banques, c'est démodé J'suis pour Paris mais c'est la crise, faut braquer les émirs au Parc Plus l'temps que j'baraude, tout s'répète, j'suis perplexe Les réflexes du jardinier tu m'plantes, je t'arrose J'fume tant d'garrots mais je l'ai pas au bras Tu dis être sombre comme l'ombre du baobab On t'croise toujours tout pâle au bar Elles sont toutes dans l'ciel, ici bas, y a pas d'stars Et parce qu'y a gosses, les tes-pu goûtent ton sexe Loin d'être un vrai, ta mère aurait dû faire une fausse couche En plus, tu pues la merde La vie d'mon derche, t'es pire qu'une grosse mouche Pas du genre à crier au secours sur l'capot des keufs Ton mec a pas d'cul Ils t'payent des keuss qui coûtent la peau des seufs Bande de sacrées putes avec vos sales réput' On vous court pas après, on court plutôt quand ça crie plus Ouais, ici, la BAC passe mais ça passe pas l'bac Parle pas, passage à tabac pour une Malba, on n'oublie pas Seul ton HIV s'avoue au card-pla La concurrence se brise mais s'répare pas, compte pas sur Carglass Wesh, Daymolition, welcome, listen Les meufs, c'est toutes les mêmes Il m'en faut une ni conne ni cheum À présent, on est dans l'futur, personne peut nous dépasser J'te parle de vue quand j'te dis qu'personne veut la voir B.A.C Depuis la naissance, on a les crocs car plus d'unité Peut-être pour ça qu'aux appels à l'aide les potes décrochent pas La monnaie a plus de charme qu'Eva Mendes On va s'foutre le Rap en groupe Notre album s'appellera Gang Bang On veut l'million tah les Rolling Stones Le bruit s'habille en écho lorsque les broliques causent Punchline sur punchline Pourtant les vues sur YouTube n'augmentent pas Entre les juifs et Hitler, y avait d'eau dans l'gaz Woop ! Woop ! Y a les keufs pas Meek Mill Le crime paie, armé d'un mic', les bitches j'kille On a les nerfs, khoya Si un keuf canne, logiquement, des frérots j'tappe J'ai dit une phrase à double sens, merde J'suis pas un élève Usain Bolt, j'fais 100 mètres J'aime pas les beurettes donc faut qu'ces pouffiasses m'entendent Y a qu'dans Aladdin que t'en verras une kiffer sur un mendiant Y a plus d'respect entre les daronnes, les petites d'16 piges Normal que les petites fesses clean Se prennent pour Britney Spears De nos jours, les vrais se comptent sur les doigts d'un amputé Poto, j'traîne pas au Marais mais pourtant j'vois qu'des enculés Y a qu'des bonhommes au cro-mi, pas d'bobo qu'on lobotomise Et quand tu braques, il t'manque une case prison Comme au Monopoly Bah ouais, ils sont graves contents quand l'arabe s'tait J'suis un arabe que tu comprends pas donc j'suis un art abstrait Ton maillot est fabriqué en Chine Tes mythos faut pas qu'on y croit J'sais plus qui est qui, comme un schizophrène devant son miroir On traîne qu'avec des faux, on est même habillé en falsh Même les yeux dans le dos, poto, j'vois la réalité en face J'répète, faut tej' les faux comme l'OM doit tej' Gignac Dans ma ville y a qu'des tacleurs Ma sur, mets tes protège-tibias Le morceau n'est qu'un remix, y a aucune parodie On s'écarte de l'Enfer comme les dents d'Vanessa Paradis Averse de punchline, sortez vos parapluies Genre t'as connu Rap Line dans la Star Academy J'ai fait mon chemin un peu dans l'noir comme Ray Charles J'taffe l'jour pour conclure que j'finirai dans... Feu de ouf, t'as le seum de nos hassoul Si tu veux la guerre, j'la fais Appelle-moi Walaz Massoud J'suis d'humeur matinale, tous les jours j'me ve-le tôt La force à l'heure de fajr, une fois que j'ai fait le dos Toujours un jaloux qui parle sur mon dos Et si j'connais le succès, y en aura bien sûrement d'autres Pourquoi tu parles si t'as sucé tel et tel chibre ? Faire de la belle zik est exigé, dommage Que ton rappeur fétiche ne fasse que réciter le JT Y en a qui lèchent bien l'fion, nous, on perce les curs J'fais plein d'sons car faut faire des textes avant d'faire des buzz J'représente les peuls et les bons humains Moi j'suis un ex-Expendable J'ai mes connexions dans les bas-fonds d'Dublin Jusqu'au Staples Center, c'est là où joue Kobe Bryant Comme lui, j'dois briller pour sortir mes frères de la noyade Chaque jour, le doute m'oblige à taffer comme un chien J'ai pas d'pouf mobile, j'veux pas être le king de ma ville Juste Alpha Wann, j'trouve ça plus stylé Visualise-moi, toute la nuit durant, me triturant ligne par ligne J'suis pas une petite frappe mais, dès six heures, j'suis fini Enfoiré, j'ai des switcheurs, des zig-zag, des phillies Rien qu'mes bougs s'agitent que quand ils touchent de la verte Gars, j'ai des trous, j'navigue entre le gouffre et la vraie vie J'fais des tours d'magie, ils font des tours d'la ville Pour d'la weed, j'tourne la vis pour qu'ils me doutent la paix Quoi ? Tout cela paie, du coup, j'ai grave d'la rime Traîne qu'avec des asthmatiques apatrides pour te la mettre Mais wesh, on s'exporte, laisse les trimer comme des sex toys Toujours dans l'même sens Pour se faire gifler par les mêmes porcs Les frères dorment tous sournois comme la douceur de la corde Souple, les corps souffrent morts saouls J'attends que les portes s'ouvrent Puis j'ai pas envie d'marcher devant Sache qu'on boit pas dans l'même verre si t'as craché dedans Même si t'as taffé, je sens que tu vas caner, le temps À parler, à blabater sur mes frères au lieu d'garder le rang Nique le système carcéral, j'ai pris flemme de passer à-l Je préfère les décibels et puis les péritels des caméras Ne m'colle pas d'étiquette, j'bicrave des citernes de came, hélas J'baise les fliquettes, et vi'-ser des criquets de chaque tier-quar Nous allons nous équiper comme les petits mecs des favelas Le ballon, je l'ai esquivé, j'ai fait vibrer des tas d'pétasses Wesh kafass ? Moi, j'froisse des spliffs La poisse m'esquive, j'suis la poussière dans l'mauvais il Tous les yeux m'guettent, à croire qu'je m'exhibe Bandes de sales vermines Que pourrez-vous faire quand j'aurai l'seum ? Nada ! Ça va trouer des shnecks et puis clouer des becs T'es dégoûté, t'es déf', venez goûter mes textes Allez, courez les mecs, ça va couper des têtes Tout est prétexte à jouer les chefs, ouais, masquez vos pulsions J'viens pas rouler des pelles Dans l'trou de tes fesses, j'fais ma révolution Ouais, mate l'élocution, t'es un petit mytho si t'oses dire Qu'on est pas des pros du son, moi, j'te critique au micro, petit J'vais pas m'défiler, méfiez-vous, faut pas m'défier J'ai ves-qui les cours pour des filles, des sous, et des billets pourpres Rev'là le singe hurleur maniaque, vu Toujours obscur et grognon Je laisse mon ombre occuper vos pions Loin devant j'opère comme les tueurs d'mafia russe D'humeur glaciale, j'tue sans aucune émotion Mais ma vie a un goût de houblon, j'ai un joujou sous l'blouson Je shoote tout c'qui bouge pour pouvoir être toujours bon 2Fingz prend l'mic', juste des rimes qui frappent Nan, on change pas une équipe qui couche tout le monde J'sors de ma douche mais, merde, ouais, c'est trop nocif Les haines que j'ai quand j'sors d'une douche froide, alléluia Quand certains s'plaignent de leur maman au ciel Moi, j'le fais pour des coupures EDF et l'chauffe-eau vide Alors que j'ai qu'des couplets crades Comme la bouche de la plus belle femme Qui suce une bite pour une dose de crack Caché au fond d'un survêt' Nike Mais que fait la police ? J'me l'demande et j'vois Les petits du tier-quar qui s'alcoolisent, qui arrachent ton sac Comme on aurait pu le faire en classe de 4e Pour ces bulles d'air, ouais, qu'on rêvait d'avoir En bas d'une barre d'immeubles Les cheveux aussi courts qu'le destin d'Hamza Qu'est-ce qu'on a pu lâcher des larmes Et des vraies quand on était seuls Pendant qu'les salopes qui baisaient Parlaient que de lui dans leur pseudo MSN Y a des soirs où j'ai pensé à partir Ma mère comprenait pas ma souffrance Alors souvent, ouais, j'me vengeais dans la nuit On s'casse la voix en guise de SOS, le Sheitan A niqué mes valeurs familiales et j'me dis qu'ça ira Pour l'instant faut faire avec, j'ai juste dû jeter mes rêves Comme mes habits crades dans une rue sombre de Stalingrad Où l'amour et la passion n'ont jamais montré l'bout du nez Car l'argent fait pas l'bonheur Mais pas d'bonheur sans s'foutu blé Toujours les mêmes dictons qui nous montent à la tête Ouais, c'est triste, ma caille Si à 20 ans t'as toujours des envies de braquage Anonyme comme Zorro, complice muet comme Fernando Comme du bon vin, c'est dans la cave que l'projet fermente, gros Habillés à l'envers du slip au manteau Comme une putain qui demande à chard-clo si l'hiver tient chaud Nouveau maillot taché, j'suis vert comme un martien Ou comme ce machin malsain que j'consomme parfois l'matin Et c'est ça qui m'atteint, pas les critiques des rageux Que j'déglingue et momifie comme le scoot à Martin Rime au marteau-piqueur dans la rue, après l'Pan Tu vas rejoindre Peter dans l'monde des enfants perdus Sample de jazz, percu, j'suis perché, je m'y suis cru Cracheur de feu au ci-ci-ci-circus On veut baiser l'circuit, éponger nos dettes Difficile sous la pluie, finir pauvre et honnête C'est sec comme un biscuit mais ça paye au long terme Dans l'tunnel de l'effort japerçois la lanterne Du bonheur, du bonheur, c'est L'Animal, poto Tu veux m'baise, faudra t'lever d'bonne heure Équipe de charbonneurs, Milmo Areno, on les baisera, gros Combien de corps recroquevillés cèdent sous le sort Pendant qu'des hordes de propriétaires touchent de l'or Tu dis que j'ai tort, que notre vie est belle, regarde dehors Sans t'esquiver, frère, j'te parle de morts pour des billets verts Pendant qu'on sort pour s'ennuyer ferme, à crier fort La nuit éclaire les pauvres qui dorment sous un pilier de fer Imbibés de bière, qui se traînent parmi la pisse des clebs Donc quand je fais la fête, j'leur jette une petite quantité d'pièces On est impliqués, merde, j'peux pas m'incliner même Si lÉtat sème le doute, que toute tentative est vaine On rentre dans c'vivier d'dettes, on fantalise l'échec On rentre dans ce vivier terne, ils parlent d'émeutes Je n'vois qu'des bleus qui vandalisent des êtres Le mal, c'est eux, la faim dans l'monde c'est pas une idée d'Ken J'connais pas la suite, t'inquiète pas, mec, j'suis un génie Donc j'enchaîne tranquillement, fuck tous les ingénus J'en ai rien à foutre, l'ingé mue quand j'pose ce putain d'truc Faut qu'ça enchaîne le mic', qu'on fasse tourner les choses Rien à foutre, mon pote, j'balance une dose, écoute la prose J'te dis même pas bats les pattes mais n'mets pas les ieps Dans mon tiek's où on rit dans la rue Mais où rudes sont les balayettes Je m'exprime au clair de lune quand les MC rangent leur plume J'les allume sans rancune Donc sale pute maintenant qu'est-ce t'as ? Vous pouvez m'guet', toi et tes lascards, lâche car Faut pas test si tu n'encaisses pas, j'ai la rime Technique, c'est pour ça qu'je t'exprime et t'explique que On rigole pas, négro, c'est dangereux et grand reu' Pense à tous les mecs qui canent à cause de leur endettement Réfléchis, ferme-la avant d'te faire enfoncer bêtement T'es con ou quoi ? Tu t'fais taper par les tits-pe d'chez oi-m Et après tu veux m'test, mais t'es fou, toi Mec de tess ? Haha, tu m'fais rire Moi, c'est , mec de tiek's, t'es dans ma ligne de mire Est-ce que j'vais t'tabasser car tu checkes ma meuf sur l'net ? Question bête comme me demander si j'rappe mieux qu' Un verre de sky sec, mec, à ta santé M'fais pas m'impatienter pour t'la raconter On m'a justement raconté qu'tu faisais moins l'malin quand t'es Seul tout et j'te dis sur l'coup, tes jours sont comptés Mais j'me la raconte pas, hé, demande à mon gars Veusti Comment j'suis deuspi dans l'art du combat Et viens au contact et t'apprendra, petit Qu'dans un hall, le nombre ne compte pas Paris capitale, capital sous l'oreiller J'vends des cauchemars à des shlags toujours éveillés Gros sons d'2Pac pour me réveiller Et j'suis en mode spartiate, énervé 7.5 meu-ar feu-shnou bah ouais Gros , je m'arrache, négro, ça l'fait Pheno, cessez d'parler, les frères J'donne mon corps à la science car j'suis trop frais C'est l'Enfer si t'as les dents à Vanessa Et l'Paradis si t'habites à Denfert Mon cur veut la perdre, ma queue la garder Même avec les menottes, j'continue à la mater Je m'envole dans les hautesses, me crash dans les infirmières Le bonheur est près et j'dirais, il est éphémère J'ai pas les poches pleines mais j'suis pas en hess Parfois, c'est la merde, j'mets l'Rap entre parenthèse À fond dans les flammes mais j'me brûle pas Le ghetto m'acclame, la richesse me calcule pas Il faut qu'tu notes ce texte O.G Wann Kenoby l'noir, bien sûr que j'ai la force, peut-êt' Que plein d'MC sont devenus cordonniers dans l'espoir De pouvoir analyser mes bottes secrètes Tu m'vois partout mais j'suis l'homme invisible C'est comme ça qu'me surnomme mes voisins J'me donne les moyens d'réussir, j'suis un homme averti Une pierre fait deux coups, une clope fait trois joints Leur truc est à gerber, tu kiffes ? Laisse-leur lancer des piques J'perds pas mes repères, j'fais d'la RER B musique Fontenay, Bagneux, Auber', j'connais la ligne Plus d'argent, plus de problèmes, frère, tu connais la ligne Tu crois qu't'as les habits, l'style, crari Vraiment, frère, avec une paire de chaussures Calvin Klein Pompe et astique, tu veux dénoncer la mif Note donc les blazes, le nom c'est Art, prénom c'est Patrick Hatai, c'est Paname, t'es pas tout seul À force de penser qu'à ta poire, t'as pas vu venir la banane T'as un tas d'arme, c'est pas des conneries Toi, tu parles de tonnes de weed Mais t'es qu'un acteur comme Sean Connery Et c'est pas fini, j'envoie des punchlines en plaquette Pendant que t'envoies les petites acheter des paninis Demande à lel-Bi, à Mehdi, on tabasse les gueush Check mon kamas de peuf', ici, on arrache les keus, une tasse C'est comme un boomerang, elle revient quand tu la tèj C'est pas normal, j'me sens si bien quand j'encule la teille Et c'est la merde depuis que j'suis déscolarisé Sur la carrière d'Escobar, j'ai vu des ex-taulards miser Nan, j'suis pas voué à l'échec, j'ai jamais aimé ça J'me dis putain, pourquoi je l'ai ken Quand la keh remet ses sapes Avec le buzz, elle m'tourne autour comme un satellite L'amour c'est , montre ta chatte et vite Hello ! C'est Yassi Yass alias le boucher tounsi On veut des go's, des liasses sans oublier l'bout d'shit Négro, fais pas le man, on peut t'découper tout d'suite Mac Cain, y a des fournées sur la liste Mais j'reste cool, y a le S-Crew et Doumam's sur la piste Les bitches veulent des billets, voir les bling-bling briller Mais faut surtout pas oublier qu'on peut tout faire la suite Demande à , on peut tout faire dans la suite Mais t'es mon bro ou pas ? Yes, yes il était pas à-l, j'te parle pas de Framal Passe le cohiba, je t'enverrai pas de faire-part Enfile ton gilet pare-balles, s'il faut que je t'arrose au FAMAS Je t'aurais tôt ou tard, rien ne sert d'courir C'est pas bon pour l business, loin des rêves de l'oubli Le charbon, c'est mon fitness, personne m'enlève le sourire Avec mes frères, on peut se nourrir à 15 sur un bifteck Les tits-pe arrêtent le collège À 12 ans, veulent qu'on les reconnaisse Frère, c'est trop laid, j'attends l'prophète Ils prennent Nabilla comme modèle Comme Ayem, tu veux des seins contrefaits t'façon Princesse, ton conte de fée deviendra conte de fellation Et en plus, le gouvernement veut niquer nos repères Le mariage pour tous, c'est comme nos couilles Pas besoin d'avoir deux pères J'ai oublié mon texte mais j'pars en impro', poto L'instru' j'la baise, bah ouais, c'est une nympho C'est Limsa, mes reufrés savent, j'ai de l'imagination Poto, j'suis trop far quand j'pars en improvisation J'passe le mic' à S.A.L.I.M J'fous l'feu au mic' comme d'habitude Gravé dans la roche, hmm, Excalibur C'est plus des rimes que j'lâche, non, l'ami, c'est des Golden Avec le numéro 93 j'atterrirai dans le top ten Bordel, écartez les mômes, les femmes, les bombes pleuvent Mortelles sont mes phases mais... Fuck Charlie, où est la maille, c'est elle que j'veux trouver J'aime faire des feat vu que j'aime faire l'amour J'ai pas l'temps mais comme Dolby, j'suis à la bourre On a couché des tas d'mecs Teddy Riner Demande à Crysto, le clan des kickeurs Fuck les Illuminatis, lÉtat, les lois comme ça c'est dit J'rappe depuis pour rivaliser le Milan, j'ai assez d'titres J'rêve J'préviens d'office, j'ai des grosses rimes solides C'est du haut niveau, les rivaux j'laisse immobiles Je t'ai mis dans les cordes, wha-wha-what's my nigga ? Profites-en, prends-en une et pends-toi avec T'es dans les bacs, fils, j'suis dans les blocs T'aimerais vendre des disques mais tu vends tes potes Shimmy shimmy yo, shimmy yeah, j'manie l'mic' J'élimine les faux, j'vise les têtes pas les pattes En quelques lignes je fous l'boucan, j'ai pas ton temps Logique que tu n'sois pas content 9.3, bats les couilles si la balle est dans ton camp Et si c'est l'Rap, les man, j'avoue c'est facile Dans mon clan y a tous les Dans le tien, y a tous les has been Motherfuck, j'ai zéro dans l'porte-feuille J'vais t'en faire voir d'toutes les couleurs Tu vas pas aimer comme Hortefeux OK, gros, faut que j'me casse, les choses se compliquent À cause d'ces cons d'flics, en gros, trop d'choses se passent J'deviens claustro, j'me tasse dans ma galère, j'en ai pas l'air Mais les gens m'disent que j'suis trop bon, faut que j'me fâche Mais c'est pas dans ma nature, moi J'suis plutôt un mec posé que s'retient par peur d'exploser T'as choisi d'grandir à la dure, toi, de t'exposer Traîner, dealer dans la 'u-r, moi, j'ai pas eu l'choix J'ai grandi sans l'daron et sans mon reuf, meuf À la tête d'la mif donc normal qu'j'finisse expert en bluff Mais bon, mes soldats ont toujours été là dans tous les coups durs Et ça, c'est l'amitié sous toutes ses coutures, c'est grâce à a-ç J'ai tenu, ça graillait a'-p, sa race, chez nous et pour ne pas qu'ça lasse J'ai du du crack salace à la Marcello Et ça, remarque, chez nous, c'est pas des masses à faire Pour que les liasses s'amassent Les pieds en France, la tête en Allemagne J'pense qu'aux gros bolides, à buzzer sur Paname Tasse-pé dans mon lit, le futur m'a choisi La misère me bannit quand j'commence à dormir Ma vie dans c'journal, j'me lève du pied gauche Toujours à parler mal comme les South Park Pheno, record, retour en arrière Le Rap, c'est mieux quand y a pas d'suceur, sa mère J'suis tout seul dans ton viseur, t'attends quoi pour tirer ? Mais si j'meurs, comment l'peu-Ra va s'en tirer ? J'vous mets à l'amende, en retard à ton rencard Ta langue en attente car les loves m'attendent Gov dans mon veau-cer, toss devant mes yeux Les pauvres prennent la grosse tête, les riches font des aveux Pas besoin d'avion pour prendre mon envol Les profs m'en voulaient, les grands m'disaient Reste à l'école J'ai confiance en personne sauf en mes darons Trouve-moi un plavon, j'vais pas ramasser l'savon C'que j'fais, c'est bavon, demande aux javons J'parle mal aux commi's, aux profs pas aux darons C'est mon secteur qui débarque comme dans la guerre des mondes De l'improviste qui s'démarque et enterre tes modes On s'demande, c'est qui cette équipe qui nous emmerde tellement Ma rime, un martèlement loin de chez Sony Entertainement Dans mon 18, la rime n'est pas nourrie aux phéromones Les MC n'font pas du creux juste histoire de s'faire aux normes On veut des thunes mais t'attends à me voir faire l'aumône Ni même faire le môme ou sur un plateau télé à faire l'homo' C'est pour mon département, 7.5 débarquement Ma rime provoque des déportements Ici, on cherche tous l'issue mais les portes manquent S'ils te disent tous fichus, c'est que les porcs te mentent Notre secteur est vecteur d'un potentiel en croissance Et si tu crois mon Rap sectaire, c'est qu'tu n'y cherches pas trois sens On a tous connu les larmes, les frérots, la traîtrise Des drames, un tournevis dans l'Sergio Tacchini D'la tise de merde et c'est parti pour les prises de têtes Histoire de meufs ou d'shit Vu y a qu'ça pour nous faire croire à la vie de rêve C'qui m'passionne, c'est pas Disney, moi C'est observer la ville des toits Avec mes renégats quand Paris s'nettoie Alors ça rime très tard quand les premiers métros s'tirent Ça tise les fonds d'canettes si y a pas d'mégot d'spliff Une semaine que j'ai pas vu mon lit J'préfère les trains qu'on fraude Moi et les contrôleurs, compare pas les singes aux fauves Et tes rappeurs ont des faux airs de lâches Comment leur dire qu'en 90 Ils rentraient pas dans les concerts de Rap Alors ça gaze, ma caille ? Tu t'es fais poucave ? Nan mais les shtars, c'est tes potos Qui prennent des photos via Instagram Ma p'tite gueule c'est ça la vie d'thug, un jus d'fruit, une liqueur Et j'te raconte ma vie, bah oui, ce son c'est Twitter Écoute pas c'que les boloss disent, ils pourront tout dire Mais ils savent pas que pour s'nourrir Georgio vole à Monoprix J'pourrais parler d'mes origines mais c'est pas ta vie Ces bâtards disent que j'fais rebeu Mais moi, j'suis fier d'venir de Pointe à Pitre Alors parle pas sur mes chicos et la barbe que j'ai pas eu Dis-toi chez moi c'est Mexico, bicrave du crack au bout d'ma rue La misère c'est pas mon fond d'commerce Mais j'ai pas envie d'parler d'bonheur Quand j'suis dehors et que j'croise des parents ivres J'cogite trop j'en fais des rimes, c'est mieux qu'd'aller chez l'psychiatre Suffit qu'tu tombes pour que les bleus sautent de joie, comme quand Chelsea marque Tu vois l'truc ? Accro au crime, aux femmes, à la nicotine On fait d'la 'sique au stud, on gère des putes, puis on les nique au 'tel Sa mère, on a les flics au derch', mé-cra par la bicrave Sache qu'un homme qui porte pas ses couilles, dit-leur , ça fait vite trav' N'envisage pas de relation propre si t'aimes les bites crades J'te prendrais pas le tienne, j'me ferais ma place même si c'est ric-rac Fuck Rick Ross, le temps passe trop vite et ça fait tic-tac P'tite frappe, flippe a'-p, les flics traquent la street Crois pas qu'la street craque Reste unique, elles ont des termites dans la schnek Depuis que les langues de bois font des cuni' Tous unis pourtant j'ai besoin d'un vrai bol d'air Sonner la révolte frère Les douiller devient trop facile, j'ai l'regard revolver Faut pas qu'les hommes de Sarko sachent tout ce que mes narcos cachent Tout ça c'est trash, et on reste sombre même dans le dernier Chaque MC voulant feater se découvre des talents d'lover J'reste fidèle au tro-mé et j'boycotte un Range Rover Dans l'Hip-Hop, ça pue J'rappe mais j'me porte pas garant d'l'odeur Voyant les gars d'avance bagarrant J'avance comme 40 moteurs, j'les vois bavardant Guette si c'est pas navrant, généreux soi-disant Mais rien qu'ça parle d'argent C'est chiant qu'ces wacks vénéneux soient vivants Vas-y, laisse tenter un dièse, j'viens à 'aise chanter un 16 Dans l'peu-Ra, t'es inconnu, j'peux t'appeler 31 On est des hommes pauvres qui veulent des femmes à fric Et puis des fanatiques, on veut des tas d'articles Dans l'journal car les gars d'la clique En ont marre des wacks qui roulent les mots, c'est trop facile À paumer des mots, mon flow fascine Des phases de malades et les faux s'vaccinent Les quettes-pla arrondissent le mois Garantissent un bon glissement À bon prix se vendent autour des arrondissements J'lâche des vilains couplets, chouf J'ai une vie à couper l'souffle Toi, tu veux rapper mais tes darons disent Nan Si mon fric, cétait ton fric avant quje recompte la somme Me sors pas dsornette, que la honte tassomme Mais si lon fuit ces immondices, si lon sfie à ses complices On oublie ces visions tristes, y compris les immondes vices Avance sans perdre de temps avec la mode des écrits usuels On emmerde les banques mais on saccorde un crédit mutuel Jai demandé Il est bien c'monde ?, le silence était insolent Mais un seul empruntant le bien se rince dans leau étincelante Éteins seulement un instant linsensé engin qui t'force J'suis bien quand cest simple, sans dédain Jsuis rien sans ces frangins qui mportent Vu qules méchants sont maîtres, mes aveux ont lair de ruse Je nvois que des aveugles à perte de vue Merde, jsais pas quoi faire de plus Être le premier pour aider son prochain dans latmosphère de ruse C'est vrai qu'ma rime est assez triste, j'suis affaibli sous caféine J'fais l'amnésique quand mes parents me d'mandent si j'suis aux ASSEDIC Ma tragédie c'est d'éviter la fucking vie, ses maléfices Aulnay-sous' frère on aime pas les flics J'aimerais chanter, savoir aimer, un peu comme Florent Pagny Mais j'sais pas faire donc ramène des pouffiasses au Campanile J'suis pas le genre de mec qui mourrait pour sa petite amie J'ai peur de l'eau et des glaçons, j'suis pas comme Jack dans Titanic Pourtant j'connais que des meufs ches-lou, avec des têtes bizarroïde Tu vois l'genre de meufs ? Celle qu'on a pas besoin de masque pour Halloween Y a qu'des blancs dans leurs films, frère j't'avoue qu'c'est épatant Les renois meurent en premier, les rebeus on est même pas d'dans Ok c'est Limsa la famille, j'débarque et j'kicke sale à Paris Avec mon </t>
+          <t>Eh Don, Don, Don Dada 2zer Washington Don, Don, Don Dada Seine Zoo Records, ouais ouais ouais Faut qu'tu niques tout, personne va l'faire à ta place Si les négros étaient des caisses On sort du concessionnaire et vous êtes à la casse dawg Faux billet plug en Uganda pas d'extradition Copyright le flow Seine Zoo sur la partition Technique comme Harlem, tu connais la tradition sisi Profil New York MCs, fuck les imitratrices De retour dans l'BX on aime quand les vils-ci balisent Sisi la team, huit heures de conduite Chauffeur haïtien, traphouse à Cincinnati Business de faux chèques, vacances à Aspen Cigare cubain comme le bracelet Escroc de luxe, j'en ai l'aspect Billets de toutes les couleurs, mon négro vas-y brasse-les Style de killa pour qui chaque vie se paie Ta meuf imagine le game okay Négro, t'es pas OG juste parce que t'étais là back in the days À la limite, et au-delà, jusqu'à l'au-delà J'vendrai le parfum du hood, j'appellerais ça Eau De Larmes Balance l'instru', j'me comporte comme un boucher avec Sors un disque, j'sais pas combien j'vais toucher avec La meuf à mon bras, j'vais t'faire loucher avec J'en ai marre d'elle même avant d'avoir couché avec Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage T'approches pas de mon cur si t'as peur du vide Mon horloge biologique indique l'heure du crime, hmm Petit opportuniste, écoute ce son faut pas qu'tu meurs stupide Mon cur comme stylo, mon sang en guise d'ancre Plus j'vide mes veines, plus j'me sens vivant Sans ça, je n'ai plus de sentiments Pourtant, on est tous nés en criant Trois heures du mat' dans une ruelle parisienne L'odeur te gene, dans la rue, y'a pas d'hygiène Como esta si esta bien Même si la vie m'a prouvé qu'il n'y a jamais d'happy end Pas d'heures précises pour les criminels Qui ont le cur assez froid pour aimer l'hiver Pas de rappeurs pressés pour les midinettes Qui veulent éliminer les préliminaires Le début d'la fin, négro l'alpha et l'oméga t'inflige des gros dégâts Démarre le biz devant l'entrée du Bodega, déter' comme Gogeta ouais ouais Tu veux d'l'automatique, tu trafiques le jouet Esclave du système, c'est pour mieux te contrôler qu'il agite le fouet Les faux passeports sont fournis par des zaïrois Les cheques lavés par mes gars d'l'Afrique de l'Ouest Seine Zoo perception, parle pas d'règles négro, j'suis l'exception J'arrive LuXe comme, tu connais l'expression Rappe à la perfection Hustla, couche tard, y'aura qu'mes frérots là où j'pars J'suis né réfugié politique, la Syrie Comment tu veux qu'ça m'touche pas ? Tes démons sont trop visibles mais le succès les maquillera Accompagné d'une Shakira sur la moto rouge d'Akira LuuuXe Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage Yeah, Seine Zoo Records Don Dada on dit quoi ? VM le Don, disquette le proc, lui fais croire qu'j'suis légal Qu'y'a pas d'business de drogues</t>
         </is>
       </c>
     </row>
@@ -543,7 +543,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Démarre</t>
+          <t>Du vécu</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Du vécu</t>
+          <t>CDGLAXJFKHNDATH</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Eh Don, Don, Don Dada 2zer Washington Don, Don, Don Dada Seine Zoo Records, ouais ouais ouais Faut qu'tu niques tout, personne va l'faire à ta place Si les négros étaient des caisses On sort du concessionnaire et vous êtes à la casse dawg Faux billet plug en Uganda pas d'extradition Copyright le flow Seine Zoo sur la partition Technique comme Harlem, tu connais la tradition sisi Profil New York MCs, fuck les imitratrices De retour dans l'BX on aime quand les vils-ci balisent Sisi la team, huit heures de conduite Chauffeur haïtien, traphouse à Cincinnati Business de faux chèques, vacances à Aspen Cigare cubain comme le bracelet Escroc de luxe, j'en ai l'aspect Billets de toutes les couleurs, mon négro vas-y brasse-les Style de killa pour qui chaque vie se paie Ta meuf imagine le game okay Négro, t'es pas OG juste parce que t'étais là back in the days À la limite, et au-delà, jusqu'à l'au-delà J'vendrai le parfum du hood, j'appellerais ça Eau De Larmes Balance l'instru', j'me comporte comme un boucher avec Sors un disque, j'sais pas combien j'vais toucher avec La meuf à mon bras, j'vais t'faire loucher avec J'en ai marre d'elle même avant d'avoir couché avec Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage T'approches pas de mon cur si t'as peur du vide Mon horloge biologique indique l'heure du crime, hmm Petit opportuniste, écoute ce son faut pas qu'tu meurs stupide Mon cur comme stylo, mon sang en guise d'ancre Plus j'vide mes veines, plus j'me sens vivant Sans ça, je n'ai plus de sentiments Pourtant, on est tous nés en criant Trois heures du mat' dans une ruelle parisienne L'odeur te gene, dans la rue, y'a pas d'hygiène Como esta si esta bien Même si la vie m'a prouvé qu'il n'y a jamais d'happy end Pas d'heures précises pour les criminels Qui ont le cur assez froid pour aimer l'hiver Pas de rappeurs pressés pour les midinettes Qui veulent éliminer les préliminaires Le début d'la fin, négro l'alpha et l'oméga t'inflige des gros dégâts Démarre le biz devant l'entrée du Bodega, déter' comme Gogeta ouais ouais Tu veux d'l'automatique, tu trafiques le jouet Esclave du système, c'est pour mieux te contrôler qu'il agite le fouet Les faux passeports sont fournis par des zaïrois Les cheques lavés par mes gars d'l'Afrique de l'Ouest Seine Zoo perception, parle pas d'règles négro, j'suis l'exception J'arrive LuXe comme, tu connais l'expression Rappe à la perfection Hustla, couche tard, y'aura qu'mes frérots là où j'pars J'suis né réfugié politique, la Syrie Comment tu veux qu'ça m'touche pas ? Tes démons sont trop visibles mais le succès les maquillera Accompagné d'une Shakira sur la moto rouge d'Akira LuuuXe Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage Yeah, Seine Zoo Records Don Dada on dit quoi ? VM le Don, disquette le proc, lui fais croire qu'j'suis légal Qu'y'a pas d'business de drogues</t>
+          <t>Tu peux m'croiser à C.D.G. ou L.A.X. ou L.A.X. J.F.K, Haneda, toujours avec les mêmes avec le Mélange pas l'roi des animaux avec les hyènes avec les hyènes, boy Tu veux savoir d'où j'viens, check le BPM 7-5, 7-5 de Paname à Bethléem 7-5, boy, internationaux sont mes DM drrr Tizi ou Darsalam, toujours avec les mêmes avec les mêmes Tu veux savoir d'où j'viens, check le BPM J'garde les pieds sur terre, j'observe le moindre pas C'qui s'passe à Paname m'affecte, même si je suis loin de ça C.D.G., Benito-Juarez, money, hélico, soirée Autour de nous, que des go soignées, on s'la joue Rico Suave J'en ai marre de Paname et des coups bas, j'aime m'sentir libre comme Cuba Excès de vitesse dans la ture-voi, la policia, on la soudoie Pas l'temps d'rattraper l'décalage, faut qu'j'm'endorme avant l'décollage On vole en business class, avant c'était vol à l'étalage Y'a qu'sur les plages du succès qu'on échoue Tu vis la fast life quand ton escale dure autant qu'ton séjour et qu'ta meuf essuie ses joues Tu dis qu't'es fidèle mais en boîte t'enlève ton alliance, mmh T'a pris moins qu'tes complices et tu dis qu't'as pas balance Les gens manquent pas de cu-lot, j'les guette par le hu-blot Ils m'ont déçu comme Hu-lot, t'façon bientôt y a plus d'eau Tu peux m'croiser à C.D.G. ou L.A.X. ou L.A.X. J.F.K, Haneda, toujours avec les mêmes avec les mêmes Mélange pas l'roi des animaux avec les hyènes avec les hyènes, boy Tu veux savoir d'où j'viens, check le BPM 7-5, 7-5 de Paname à Bethléem 7-5, boy, internationaux sont mes DM sont mes DM Tizi ou Darsalam, toujours avec les mêmes Tu veux savoir d'où j'viens, check le BPM 7-5, tu l'avais senti, Mersko, c'est la hess en juillet-août, on est frais dans la veste en cuir, gros, de ceux qui voulaient s'enfuir Empiler les billets, on saute dans le vide sans filets Dans l'quartier, on s'y fait, dans l'but de vite s'en tirer, hey Qui aurait pu penser que nos destins soient liés ? Qu'on les ferait danser ce que certains voient briller Pas d'sous en poche, on s'débrouillait pour s'habiller Pas d'téléphone, on déboule sur ton palier Une copine de la copine de ma copine veut qu'on passe au Brésil J'ai promis qu'j'arriverai à la fin d'l'été comme passion brisée Invité par ma voisine, elle m'a fait cuire du poisson braisé J'pose un couplet pour le et j'm'arrache d'Europe façon Brexit Ouais, ma vie, c'est le rap et je rappe par amour, j'ai de l'amour pour mes amis, ouais, mes amis pour la vie J'ai des projets pour mon label, mon label pour le business, le business pour la monnaie, la monnaie pour la mif pow Tu peux m'croiser à C.D.G. ou L.A.X. ou L.A.X. J.F.K, Haneda, toujours avec les mêmes avec le Mélange pas l'roi des animaux avec les hyènes avec les hyènes, boy Tu veux savoir d'où j'viens, check le BPM 7-5, 7-5 de Paname à Bethléem 7-5, boy, internationaux sont mes DM drrr Tizi ou Darsalam, toujours avec les mêmes avec les mêmes Tu veux savoir d'où j'viens, check le BPM 7-5, 7-5 Wesh, ? Fian'so, on dit quoi ? 7-5 Moussy-mouss Moussolini4</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CDGLAXJFKHNDATH</t>
+          <t>Fausse note</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Tu peux m'croiser à C.D.G. ou L.A.X. ou L.A.X. J.F.K, Haneda, toujours avec les mêmes avec le Mélange pas l'roi des animaux avec les hyènes avec les hyènes, boy Tu veux savoir d'où j'viens, check le BPM 7-5, 7-5 de Paname à Bethléem 7-5, boy, internationaux sont mes DM drrr Tizi ou Darsalam, toujours avec les mêmes avec les mêmes Tu veux savoir d'où j'viens, check le BPM J'garde les pieds sur terre, j'observe le moindre pas C'qui s'passe à Paname m'affecte, même si je suis loin de ça C.D.G., Benito-Juarez, money, hélico, soirée Autour de nous, que des go soignées, on s'la joue Rico Suave J'en ai marre de Paname et des coups bas, j'aime m'sentir libre comme Cuba Excès de vitesse dans la ture-voi, la policia, on la soudoie Pas l'temps d'rattraper l'décalage, faut qu'j'm'endorme avant l'décollage On vole en business class, avant c'était vol à l'étalage Y'a qu'sur les plages du succès qu'on échoue Tu vis la fast life quand ton escale dure autant qu'ton séjour et qu'ta meuf essuie ses joues Tu dis qu't'es fidèle mais en boîte t'enlève ton alliance, mmh T'a pris moins qu'tes complices et tu dis qu't'as pas balance Les gens manquent pas de cu-lot, j'les guette par le hu-blot Ils m'ont déçu comme Hu-lot, t'façon bientôt y a plus d'eau Tu peux m'croiser à C.D.G. ou L.A.X. ou L.A.X. J.F.K, Haneda, toujours avec les mêmes avec les mêmes Mélange pas l'roi des animaux avec les hyènes avec les hyènes, boy Tu veux savoir d'où j'viens, check le BPM 7-5, 7-5 de Paname à Bethléem 7-5, boy, internationaux sont mes DM sont mes DM Tizi ou Darsalam, toujours avec les mêmes Tu veux savoir d'où j'viens, check le BPM 7-5, tu l'avais senti, Mersko, c'est la hess en juillet-août, on est frais dans la veste en cuir, gros, de ceux qui voulaient s'enfuir Empiler les billets, on saute dans le vide sans filets Dans l'quartier, on s'y fait, dans l'but de vite s'en tirer, hey Qui aurait pu penser que nos destins soient liés ? Qu'on les ferait danser ce que certains voient briller Pas d'sous en poche, on s'débrouillait pour s'habiller Pas d'téléphone, on déboule sur ton palier Une copine de la copine de ma copine veut qu'on passe au Brésil J'ai promis qu'j'arriverai à la fin d'l'été comme passion brisée Invité par ma voisine, elle m'a fait cuire du poisson braisé J'pose un couplet pour le et j'm'arrache d'Europe façon Brexit Ouais, ma vie, c'est le rap et je rappe par amour, j'ai de l'amour pour mes amis, ouais, mes amis pour la vie J'ai des projets pour mon label, mon label pour le business, le business pour la monnaie, la monnaie pour la mif pow Tu peux m'croiser à C.D.G. ou L.A.X. ou L.A.X. J.F.K, Haneda, toujours avec les mêmes avec le Mélange pas l'roi des animaux avec les hyènes avec les hyènes, boy Tu veux savoir d'où j'viens, check le BPM 7-5, 7-5 de Paname à Bethléem 7-5, boy, internationaux sont mes DM drrr Tizi ou Darsalam, toujours avec les mêmes avec les mêmes Tu veux savoir d'où j'viens, check le BPM 7-5, 7-5 Wesh, ? Fian'so, on dit quoi ? 7-5 Moussy-mouss Moussolini4</t>
+          <t>Yeah, Zerzer Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour ds choses abominables, sèche ms larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais ZerZer volume 1 dispo partout la miff' DJ Élite aux platines Eh, eh Ok, ok, yeah Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Nique ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce gosse en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Brrrr Comme d'habitude, Hugz à la prod Eh, eh, eh Depuis l'époque de Décisions Yeah, yeah, yeah Han, han, Zerzer Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Ok, yeah, yeah, yeah Ça, c'est pour les anciens, ceux qui étaient là depuis l'époque Eh, eh Yeah Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie Yeah, yeah, yeah, yeah Ok, Reeko à la prod Hahaha, tu connais les bails Ouais, ouais, yeah Eh L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais Wooouh ! Han, han Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Yeah, yeah Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woouuh, -Crew, 2zer, Framal Brrraaa Brreh, brreh, brreh, brreh Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Letsguill ! Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Letsguill, Letsguill Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle 2zer Washington Ça sent la lorage, ca sent laverse jsuis dans ma tête Saboteurs Je ne bouge pas' jattends quca vienne Eh, eh, eh Sur le droit chemin, en sens inverse Grozomozo, Ratu, Saboteur gang Yeah, yeah, yeah Letsguill DJ Elite, balance la suite Han, han, tu connais Toujours la même, rien n'a changé Toujours les mêmes ons-s, toujours la même cons', eh Ouais, toujours les mêmes têtes Blackbird, Saboteur, Seine Zoo Hugz, ça dit quoi mon pote ? J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Eh, Grünt, sisi Han, han, ZerZer volume 1, dispo partout la miff' Yeah, han, han, han Saboteur gang, Seine Zoo Saboteur gang, Seine Zoo Hugz, ça dit quoi ? Yeah</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fausse note</t>
+          <t>Nés pour mener</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Yeah, Zerzer Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour ds choses abominables, sèche ms larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais ZerZer volume 1 dispo partout la miff' DJ Élite aux platines Eh, eh Ok, ok, yeah Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Nique ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce gosse en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Brrrr Comme d'habitude, Hugz à la prod Eh, eh, eh Depuis l'époque de Décisions Yeah, yeah, yeah Han, han, Zerzer Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Ok, yeah, yeah, yeah Ça, c'est pour les anciens, ceux qui étaient là depuis l'époque Eh, eh Yeah Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie Yeah, yeah, yeah, yeah Ok, Reeko à la prod Hahaha, tu connais les bails Ouais, ouais, yeah Eh L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais Wooouh ! Han, han Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Yeah, yeah Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woouuh, -Crew, 2zer, Framal Brrraaa Brreh, brreh, brreh, brreh Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Letsguill ! Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Letsguill, Letsguill Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle 2zer Washington Ça sent la lorage, ca sent laverse jsuis dans ma tête Saboteurs Je ne bouge pas' jattends quca vienne Eh, eh, eh Sur le droit chemin, en sens inverse Grozomozo, Ratu, Saboteur gang Yeah, yeah, yeah Letsguill DJ Elite, balance la suite Han, han, tu connais Toujours la même, rien n'a changé Toujours les mêmes ons-s, toujours la même cons', eh Ouais, toujours les mêmes têtes Blackbird, Saboteur, Seine Zoo Hugz, ça dit quoi mon pote ? J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Eh, Grünt, sisi Han, han, ZerZer volume 1, dispo partout la miff' Yeah, han, han, han Saboteur gang, Seine Zoo Saboteur gang, Seine Zoo Hugz, ça dit quoi ? Yeah</t>
+          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Nés pour mener</t>
+          <t>Jusqu’au bout</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Jusqu’au bout</t>
+          <t>Les rois</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>2zer Washington Parlez-vous cefran? Hein, hein, parlez-vous cefran? DJ noise -crew boyyyy, tu connais les bails Personne ne peut stopper ma force Mais j'vous cache ma rage Comme tous mes côtés atroces et où j'passe à l'acte Mais tout ça, ça marque On n'résout pas sa life En jouant l'toréador Les coups partent, bâtard Rappelle-moi tous tes coups ratés Quand l'état voulait nous fater La vendetta de mes fous à lier Double ge-ra à défourailler J'ai coulé d'la marchandise Depuis j'me suis attendri Pour pas que le maton m'dise Tenez-vous droit, venez vous laver J'ai la force H24 sous adrénaline J'ai toujours la gouache sans mettre de poudre à mes narines J'veux soulager ma vie sans outrager la rime J'ai la force pour taffer la nuit Quand vous allez dormir On est d'accord Framal Apportez l'fric, là j'vais saboter l'biz Trop paro j'débite Que des sales projets, approchez Là j'promets, droite, gauche, et Nekfeu arme soviétique ! En guise de rime, en titre de chemise J'enfile mon jean rempli d'centimes Et gratte ce rap trop technique La prose est clean, j'tape trop de spliff Là je t'assomme ? ? Nekfeu que des balles trop précises ! J'ai le sabre dans la gorge Mec, prends garde, j't'encastre Il m'faut du cash dans la pocket J'veux des thunes d'apache Déçu d'la life, toi tu cé-su J't'exécute à l'épluche-patate Mékra Seine zoo dans les bacs Y'a pas d'nana dans mon équipe que des ? On a la rage d'un Apache Toi t'as la bouche ouverte Faudra nachave, prendre un appart' Et ça à toute vitesse J'rappe sous ivresse, quoi tu m'crois pas? ? Hey, nique les strass et les paillettes Moi j'suis ? j'ai les manières D'un soc' ? Ecoute mon clan, on arrive On va couler l'bateau des traîtres Tu veux prendre ton tarif Ca va t'coûter la peau des fesses, ma miss On est frais, bah oui Ca c'est pour mes frères d'Afrique On a tous été trahis Par toutes ces ? hemi Et tu m'verras, toujours partant pour les re-frè Nekfeu Pas l'temps pour les regrets, hein J'suis posé sans contrainte, à cent contre un J'attends pas l'embonpoint J'arrête de rapper mes textes dans mon coin Avec ma tête de fennec j'suis scred' Donc quand je squatte des quartiers chics J'écarte les cuisses des femelles du 16 On reste vrais grâce à nos actes On a nos façons d'voir le rap Pas d'casanova, tu faisais quoi à notre âge, mon gars? Arrête de rager, vu? Ici, c'est ris-Pa J'suis pas l'élu juste un p'tit gars muni de ses 10 doigts Et quoi qu'tu dises on s'est fait connaître sans radio Moi, j'suis un artiste pas comme tes collègues en major Il faut que le message s'exporte Pour qu'les petits frelons kiffent le son La vie, c'est pas que ? Je kick pour le freestyle Pire encore, fist Ma vie est un 2zer freestyle qui m'renforce ? Je kick pour le freestyle Pire encore, fist Ma vie est Mékra un freestyle qui m'renforce Hein, parlez-vous cefran? Seine zoo, allez-vous ser-dan? Check, check, l'entourage bébé</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Les rois</t>
+          <t>Les parisiennes</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2zer Washington Parlez-vous cefran? Hein, hein, parlez-vous cefran? DJ noise -crew boyyyy, tu connais les bails Personne ne peut stopper ma force Mais j'vous cache ma rage Comme tous mes côtés atroces et où j'passe à l'acte Mais tout ça, ça marque On n'résout pas sa life En jouant l'toréador Les coups partent, bâtard Rappelle-moi tous tes coups ratés Quand l'état voulait nous fater La vendetta de mes fous à lier Double ge-ra à défourailler J'ai coulé d'la marchandise Depuis j'me suis attendri Pour pas que le maton m'dise Tenez-vous droit, venez vous laver J'ai la force H24 sous adrénaline J'ai toujours la gouache sans mettre de poudre à mes narines J'veux soulager ma vie sans outrager la rime J'ai la force pour taffer la nuit Quand vous allez dormir On est d'accord Framal Apportez l'fric, là j'vais saboter l'biz Trop paro j'débite Que des sales projets, approchez Là j'promets, droite, gauche, et Nekfeu arme soviétique ! En guise de rime, en titre de chemise J'enfile mon jean rempli d'centimes Et gratte ce rap trop technique La prose est clean, j'tape trop de spliff Là je t'assomme ? ? Nekfeu que des balles trop précises ! J'ai le sabre dans la gorge Mec, prends garde, j't'encastre Il m'faut du cash dans la pocket J'veux des thunes d'apache Déçu d'la life, toi tu cé-su J't'exécute à l'épluche-patate Mékra Seine zoo dans les bacs Y'a pas d'nana dans mon équipe que des ? On a la rage d'un Apache Toi t'as la bouche ouverte Faudra nachave, prendre un appart' Et ça à toute vitesse J'rappe sous ivresse, quoi tu m'crois pas? ? Hey, nique les strass et les paillettes Moi j'suis ? j'ai les manières D'un soc' ? Ecoute mon clan, on arrive On va couler l'bateau des traîtres Tu veux prendre ton tarif Ca va t'coûter la peau des fesses, ma miss On est frais, bah oui Ca c'est pour mes frères d'Afrique On a tous été trahis Par toutes ces ? hemi Et tu m'verras, toujours partant pour les re-frè Nekfeu Pas l'temps pour les regrets, hein J'suis posé sans contrainte, à cent contre un J'attends pas l'embonpoint J'arrête de rapper mes textes dans mon coin Avec ma tête de fennec j'suis scred' Donc quand je squatte des quartiers chics J'écarte les cuisses des femelles du 16 On reste vrais grâce à nos actes On a nos façons d'voir le rap Pas d'casanova, tu faisais quoi à notre âge, mon gars? Arrête de rager, vu? Ici, c'est ris-Pa J'suis pas l'élu juste un p'tit gars muni de ses 10 doigts Et quoi qu'tu dises on s'est fait connaître sans radio Moi, j'suis un artiste pas comme tes collègues en major Il faut que le message s'exporte Pour qu'les petits frelons kiffent le son La vie, c'est pas que ? Je kick pour le freestyle Pire encore, fist Ma vie est un 2zer freestyle qui m'renforce ? Je kick pour le freestyle Pire encore, fist Ma vie est Mékra un freestyle qui m'renforce Hein, parlez-vous cefran? Seine zoo, allez-vous ser-dan? Check, check, l'entourage bébé</t>
+          <t>Eh Don, Don, Don Dada 2zer Washington Don, Don, Don Dada Seine Zoo Records, ouais ouais ouais Faut qu'tu niques tout, personne va l'faire à ta place Si les négros étaient des caisses On sort du concessionnaire et vous êtes à la casse dawg Faux billet plug en Uganda pas d'extradition Copyright le flow Seine Zoo sur la partition Technique comme Harlem, tu connais la tradition sisi Profil New York MCs, fuck les imitratrices De retour dans l'BX on aime quand les vils-ci balisent Sisi la team, huit heures de conduite Chauffeur haïtien, traphouse à Cincinnati Business de faux chèques, vacances à Aspen Cigare cubain comme le bracelet Escroc de luxe, j'en ai l'aspect Billets de toutes les couleurs, mon négro vas-y brasse-les Style de killa pour qui chaque vie se paie Ta meuf imagine le game okay Négro, t'es pas OG juste parce que t'étais là back in the days À la limite, et au-delà, jusqu'à l'au-delà J'vendrai le parfum du hood, j'appellerais ça Eau De Larmes Balance l'instru', j'me comporte comme un boucher avec Sors un disque, j'sais pas combien j'vais toucher avec La meuf à mon bras, j'vais t'faire loucher avec J'en ai marre d'elle même avant d'avoir couché avec Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage T'approches pas de mon cur si t'as peur du vide Mon horloge biologique indique l'heure du crime, hmm Petit opportuniste, écoute ce son faut pas qu'tu meurs stupide Mon cur comme stylo, mon sang en guise d'ancre Plus j'vide mes veines, plus j'me sens vivant Sans ça, je n'ai plus de sentiments Pourtant, on est tous nés en criant Trois heures du mat' dans une ruelle parisienne L'odeur te gene, dans la rue, y'a pas d'hygiène Como esta si esta bien Même si la vie m'a prouvé qu'il n'y a jamais d'happy end Pas d'heures précises pour les criminels Qui ont le cur assez froid pour aimer l'hiver Pas de rappeurs pressés pour les midinettes Qui veulent éliminer les préliminaires Le début d'la fin, négro l'alpha et l'oméga t'inflige des gros dégâts Démarre le biz devant l'entrée du Bodega, déter' comme Gogeta ouais ouais Tu veux d'l'automatique, tu trafiques le jouet Esclave du système, c'est pour mieux te contrôler qu'il agite le fouet Les faux passeports sont fournis par des zaïrois Les cheques lavés par mes gars d'l'Afrique de l'Ouest Seine Zoo perception, parle pas d'règles négro, j'suis l'exception J'arrive LuXe comme, tu connais l'expression Rappe à la perfection Hustla, couche tard, y'aura qu'mes frérots là où j'pars J'suis né réfugié politique, la Syrie Comment tu veux qu'ça m'touche pas ? Tes démons sont trop visibles mais le succès les maquillera Accompagné d'une Shakira sur la moto rouge d'Akira LuuuXe Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage Yeah, Seine Zoo Records Don Dada on dit quoi ? VM le Don, disquette le proc, lui fais croire qu'j'suis légal Qu'y'a pas d'business de drogues</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Les parisiennes</t>
+          <t>Une étoile</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Eh Don, Don, Don Dada 2zer Washington Don, Don, Don Dada Seine Zoo Records, ouais ouais ouais Faut qu'tu niques tout, personne va l'faire à ta place Si les négros étaient des caisses On sort du concessionnaire et vous êtes à la casse dawg Faux billet plug en Uganda pas d'extradition Copyright le flow Seine Zoo sur la partition Technique comme Harlem, tu connais la tradition sisi Profil New York MCs, fuck les imitratrices De retour dans l'BX on aime quand les vils-ci balisent Sisi la team, huit heures de conduite Chauffeur haïtien, traphouse à Cincinnati Business de faux chèques, vacances à Aspen Cigare cubain comme le bracelet Escroc de luxe, j'en ai l'aspect Billets de toutes les couleurs, mon négro vas-y brasse-les Style de killa pour qui chaque vie se paie Ta meuf imagine le game okay Négro, t'es pas OG juste parce que t'étais là back in the days À la limite, et au-delà, jusqu'à l'au-delà J'vendrai le parfum du hood, j'appellerais ça Eau De Larmes Balance l'instru', j'me comporte comme un boucher avec Sors un disque, j'sais pas combien j'vais toucher avec La meuf à mon bras, j'vais t'faire loucher avec J'en ai marre d'elle même avant d'avoir couché avec Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage T'approches pas de mon cur si t'as peur du vide Mon horloge biologique indique l'heure du crime, hmm Petit opportuniste, écoute ce son faut pas qu'tu meurs stupide Mon cur comme stylo, mon sang en guise d'ancre Plus j'vide mes veines, plus j'me sens vivant Sans ça, je n'ai plus de sentiments Pourtant, on est tous nés en criant Trois heures du mat' dans une ruelle parisienne L'odeur te gene, dans la rue, y'a pas d'hygiène Como esta si esta bien Même si la vie m'a prouvé qu'il n'y a jamais d'happy end Pas d'heures précises pour les criminels Qui ont le cur assez froid pour aimer l'hiver Pas de rappeurs pressés pour les midinettes Qui veulent éliminer les préliminaires Le début d'la fin, négro l'alpha et l'oméga t'inflige des gros dégâts Démarre le biz devant l'entrée du Bodega, déter' comme Gogeta ouais ouais Tu veux d'l'automatique, tu trafiques le jouet Esclave du système, c'est pour mieux te contrôler qu'il agite le fouet Les faux passeports sont fournis par des zaïrois Les cheques lavés par mes gars d'l'Afrique de l'Ouest Seine Zoo perception, parle pas d'règles négro, j'suis l'exception J'arrive LuXe comme, tu connais l'expression Rappe à la perfection Hustla, couche tard, y'aura qu'mes frérots là où j'pars J'suis né réfugié politique, la Syrie Comment tu veux qu'ça m'touche pas ? Tes démons sont trop visibles mais le succès les maquillera Accompagné d'une Shakira sur la moto rouge d'Akira LuuuXe Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage Yeah, Seine Zoo Records Don Dada on dit quoi ? VM le Don, disquette le proc, lui fais croire qu'j'suis légal Qu'y'a pas d'business de drogues</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -679,7 +679,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Une étoile</t>
+          <t>L’art et la manière</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>L’art et la manière</t>
+          <t>Gros freestyle de Nekfeu en live dans Planète Rap</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gros freestyle de Nekfeu en live dans Planète Rap</t>
+          <t>J’ai le seum</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
+          <t>Moi, j'me sens libre quand j'écris ces mots A la prod', tu l'as senti, ouais, c'est DJ Lo' C'est l'Entourage, bébé, on s'enfouraille On encourage les vrais 2zer Washington, tu connais t'façon Comme l'Homme de l'Est, j'attends l'apocalypse Je profite avant qu'on m'refroidisse, avant qu'ma peau palisse Dans mon ciboulot, j'suis mitigé, oui, si j'ai un petit boulot Un salaire, j'irais prendre l'air même si j'vivais ma vie sous l'eau Le Rap me dégoûte comme les pires aspects des filles gâtées J'vais vite gratter malgré que j'dérive, là, mais j'déprime jamais Les vices cachés des miss fâchées, ça entraine des vies gâchées Dédicacer des petites tasses-pé ? Autant caner déshydraté Ma vie d'avant, merde ! J'peux pas la quitter Zer-2 va rappliquer, faire de l'art appliqué J'vais devoir jouer les crevards, plus qu'deux lattes à tirer Tous maladifs, touche pas la mif' ou j'vais te ratatiner Noichintok, jusqu'au Népal, je gère Poto, tu connais pas 2-Zer !? X2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon Ouais, tu connais pas 2-Zer ? Comment ça, tu connais pas 2-Zer ? Faut que j'devienne légendaire, que j'éclaire les lanternes mais Ici, c'est l'enfer depuis qu'j'vois mes frères s'faire enfermer Nique le système carcéral, j'ai pris flemme de passer àl Je préféré les décibels et puis les péritels des caméras Ne m'colle pas d'étiquette, j'bicrave des citernes de came hélas J'baise les fliquettes, éviscère des criquets de chaque tié-quar Nous allons nous équiper comme les p'tits mecs des favelas Le ballon, j'l'ai esquivé, j'ai fait vibrer des tas d'pétasses Wesh kafass ? Moi, j'froisse des spliffs La poisse m'esquive, j'suis la poussière dans l'mauvais il Tous les yeux m'guettent, à croire que j'm'exhibe Bandes de sales vermines, que pourrez-vous faire quand j'aurai l'seum ? Nada... Tu connais pas 2-Zer ? Écoute ça, c'est mamen 2-Zer x2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon Attention, je débarque ça va trouer des schnecks Et puis clouer des becs, t'es dégouté, t'es dèf Venez gouter mes textes, allez, courez les mecs Ca va couper des têtes, tout est prétexte à jouer les chefs Ouais, masquez vos pulsions, j'viens pas rouler des pelles Dans l'trou de tes fesses j'fait ma révolution Ouais, mate l'élocution, t'es un petit mytho si t'oses dire Qu'on est pas des pros du son, moi, j'te critique au micro, p'tit J'vai pas m'défiler, méfiez-vous, faut pas m'défier J'ai ves-qui les cours pour des filles, des sous Et des billets pourpres, j'ai mis d'côté les plaisirs des foufs Car j'en ai qu'une mais j'sais qu'vous m'désirez toutes L'argent, les thunes, mon but... Ouais, tu connais pas 2-Zer ? X2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon2</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>J’ai le seum</t>
+          <t>Enorme freestyle de Nekfeu en live dans Planète Rap !</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Moi, j'me sens libre quand j'écris ces mots A la prod', tu l'as senti, ouais, c'est DJ Lo' C'est l'Entourage, bébé, on s'enfouraille On encourage les vrais 2zer Washington, tu connais t'façon Comme l'Homme de l'Est, j'attends l'apocalypse Je profite avant qu'on m'refroidisse, avant qu'ma peau palisse Dans mon ciboulot, j'suis mitigé, oui, si j'ai un petit boulot Un salaire, j'irais prendre l'air même si j'vivais ma vie sous l'eau Le Rap me dégoûte comme les pires aspects des filles gâtées J'vais vite gratter malgré que j'dérive, là, mais j'déprime jamais Les vices cachés des miss fâchées, ça entraine des vies gâchées Dédicacer des petites tasses-pé ? Autant caner déshydraté Ma vie d'avant, merde ! J'peux pas la quitter Zer-2 va rappliquer, faire de l'art appliqué J'vais devoir jouer les crevards, plus qu'deux lattes à tirer Tous maladifs, touche pas la mif' ou j'vais te ratatiner Noichintok, jusqu'au Népal, je gère Poto, tu connais pas 2-Zer !? X2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon Ouais, tu connais pas 2-Zer ? Comment ça, tu connais pas 2-Zer ? Faut que j'devienne légendaire, que j'éclaire les lanternes mais Ici, c'est l'enfer depuis qu'j'vois mes frères s'faire enfermer Nique le système carcéral, j'ai pris flemme de passer àl Je préféré les décibels et puis les péritels des caméras Ne m'colle pas d'étiquette, j'bicrave des citernes de came hélas J'baise les fliquettes, éviscère des criquets de chaque tié-quar Nous allons nous équiper comme les p'tits mecs des favelas Le ballon, j'l'ai esquivé, j'ai fait vibrer des tas d'pétasses Wesh kafass ? Moi, j'froisse des spliffs La poisse m'esquive, j'suis la poussière dans l'mauvais il Tous les yeux m'guettent, à croire que j'm'exhibe Bandes de sales vermines, que pourrez-vous faire quand j'aurai l'seum ? Nada... Tu connais pas 2-Zer ? Écoute ça, c'est mamen 2-Zer x2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon Attention, je débarque ça va trouer des schnecks Et puis clouer des becs, t'es dégouté, t'es dèf Venez gouter mes textes, allez, courez les mecs Ca va couper des têtes, tout est prétexte à jouer les chefs Ouais, masquez vos pulsions, j'viens pas rouler des pelles Dans l'trou de tes fesses j'fait ma révolution Ouais, mate l'élocution, t'es un petit mytho si t'oses dire Qu'on est pas des pros du son, moi, j'te critique au micro, p'tit J'vai pas m'défiler, méfiez-vous, faut pas m'défier J'ai ves-qui les cours pour des filles, des sous Et des billets pourpres, j'ai mis d'côté les plaisirs des foufs Car j'en ai qu'une mais j'sais qu'vous m'désirez toutes L'argent, les thunes, mon but... Ouais, tu connais pas 2-Zer ? X2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon2</t>
+          <t>×4 J'suis sorti du ventre de ma mère pour vous faire l'album de l'année Les autres vendent de la merde, je l'ai fait sur mon propre label Dis-moi, c'est quoi l'album de l'année ? Feu ! Feu ! Feu ! Feu ! Comme Walter White, j'ai mes Clarks Wallabees Sur, serre-moi la main, frère, claque-moi la bise Je ne côtoie que des avions à la carlingue parfaite J'ai beaucoup plus de goût que Karl Lagerfeld Le monde de l'art est vantard, il te vend du street-art Mais ne veulent surtout pas voir mes scarlas graffer en vandale Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Tu peux ressentir l'aura dans nos raps, sortez les anoraks On aura bientôt l'orage selon l'oracle Ma conscience m'a dit Qui es-tu ? Veux-tu vivre dans le vice ou dans la quiétude ? Ça dépend où est l'pèze, on doit être bêtes, ouais, p't-être Mais ma plume peut clouer l'bec de Houellebecq Ici, on est vite tentés, il vaut mieux que tu vives ta quête J'ai entendu Vide ta caisse, le lendemain, les flics enquêtent ×2 C'est quand j'aurai des millions que j'me questionnerai Dans quelques années, je me demande qu'est-ce qu'on aura Si je n'savais pas que les keufs m'espionneraient Jamais j'démissionerais même s'ils veulent mon aura La voix d'la tess' dans l'oreille Faut qu'on encaisse dans le Rap Mental d'acier tah les chefs de guerre Dis-moi tu vas ken lequel ? Je n'vois que des merdeux gueh Tu vois pas comme les chiennes te guettent ? Elles rêvent d'être avec moi comme dans des fiançailles Pour que je ne regarde plus mes finances InchAllah, je ne mettrai qu'une fille enceinte J'prie mon Dieu mais je reste silencieux Pris dans l'jeu, c'était une évidence Pris dans l'feu, qui sort seul Méfiance, faut qu'tu prennes tes distances Vie d'malfrat en noir et blanc comme les films anciens Quand on est sur scène c'est l'empire byzantin Mon équipe rend dingues les pires depuis bambins La nuit, je sors sans but comme un somnambule Y'a certains rêves que les Hommes n'ont plus J'ai vu cette fille, on était seuls dans l'bus Elle avait les yeux rouges, elle avait pas seulement bu Elle avait de la came dans un sac Balenciaga Elle s'est fait caner, c'est ça d'balancer un gars Dans Paname, y'en a qui s'perdent, y'en a qu'espèrent Péter des sapes Agnès B., des Nike SB Dehors, c'est froid, y'a plus d'humanité Un homme est mort inanimé devant un immeuble inhabité C'est la crise ! La crise ? Qui est-ce qu'elle atteint ? Toi, moi ou le suicidaire qui escalade un toit ? Si Dieu veut, jusqu'à 120 ans voilà mon espérance de vie Toujours dans l'excellence, tu connais mes préférences On est vraiment des références de style Dans l'équipe, aucune déviance, nan On ne tolère pas la médisance, nan On est méfiants, choisis ton camp Au lieu de rester entre deux fils, nan Tant que je n'ai pas de millions Mes egotrips resteront de l'autodérision Besoin de causes et regrets pour quitter ce monde de merde Je me laisse aller avant de prendre une autre décision Trop de menaces et de coups de crasse pour des loves Je le sens tout d'suite quand un traitre tape mon épaule Ne le vois-tu pas ? De quoi tu parles à part de ton ego ? Moi, rester à ma place, ce n'est pas dans mon créneau J'veux que Def Jam signe mon chèque, ouais, mon putain d'chèque J'veux qu'la SACEM signe un chèque, ouais, mon putain d'chèque J'veux que Def Jam signe un chèque, ouais, mon putain d'chèque J'veux qu'la Def Jam signe un chèque, ouais, mon putain d'chèque Négro, faut d'la maille, ouais, mon négro, faut d'la maille Rebeu, faut d'la maille, ouais, mon rebeu, faut d'la maille Babtou, faut d'la maille, ouais, mon babtou, faut d'la maille Babtou, faut d'la maille, ouais, mon babtou, faut d'la maille J'dors les yeux ouverts, j'parle avec les esprits J'ai fait souffrir car j'ai souffert J'ai fait des erreurs aujourd'hui j'en paie l'prix J'suis bon qu'à rapper c'que j'suis Mes raisons, mes torts, c'est ça être vrai, couz' Et foutre des foufs dans mes clips Que moi-même je n'voudrais ni comme sur ni comme épouse J'suis qu'un fou parmi des cons En vrai, j'sais même pas dans quoi j'suis Ces bâtards m'critiquent, si j'les laisse ouvrir leurs gueules C'est juste que j'aime savoir dans quoi j'chie J'lâche des perles en stud' Mais j'crois qu'l'industrie n'y voit qu'tchi Et ma voisine du dessus Me regarde comme si j'étais un frère Kouachi On apprend à s'faire tous seuls, vu qu'le système nous néglige On deale en croyant être screds Alors qu'on s'fait remarquer comme une pute dans une église J'rappe pour mes rabzouzs J'rappe pour mes niggas Black, blanche ou beurre, j'les aime toutes Du moment qu'elles remplissent leurs leggings J'ai l'inspi' à Tupac, flow sale comme l'argent d'la bicrave Frais dans les clips à t'en faire croire Qu'être négro en France n'a jamais été un handicap J'pratique le haut-débit, Numéricable Toi, t'es un faux mac mais ne pute véritable J'me mets à nu, mais j'suis pudique Un peu comme une actrice X en Niqab Beaucoup qui font les hlels mais qui les baise en chette-ca ? Y'a ton ADN sous la semelle de ma sket-ba Micro semi-auto, j'appuie sur la chette-ga J'ai perdu au loto donc j'ai bibi la sel3a J'suis avec mes potos, capuché, squette-ca Trop chaud, loco, abusé, teste pas Ton équipe est et prête à gober des chibres Mon équipe est glauque et prête à t'voler tes litrons Tu veux tester mes salauds, ça fait bang, genre saloon Frère, si je t'allume c'est que j'suis prêt pour l'salut T'es pas d'la mif, parle-moi biff ou parle-moi d'profit Dix kilos d'weed, un kilo d'shit, le tout sera blanchi On fume le matos, mes vatos vont brûler ces rappeurs Ça sera du gâteau comme rotte-ca le de l'éducateur A bord d'une Merco Benz, vitres teintées, grosse boisson C'est la moisson, les mousseux sont d'sortie, ouais eh mistinguette Rentre dans le VIP si tu veux changer de vie Si tu rentres dans le lit, sache qu'on rentre dans le mille J'suis un hot nigga Mes gavas derrière oim ne craignent que God, nigga Mon équipe pète les scores pendant qu'tu t'fichas, kho Rebeu, renois, babtous, chicanos Tes négros softs ont des chichas roses Suffit pas d'pomper tous les rappeurs de Chicago Cassos, plaques et matraques la capitale est yomb Ici ni fleuve ni lac, juste une scène lasse-dèg donc allons-y, fuyons Entre les putes, les connasses, les gars, nous trions Vie lassante nous rions donc j'accomplis mon triomphe comme l'Arc Imagine la Tour Eiffel se faire amputer Boumbadaboum ! Encore un keuf vient d'se faire buter Le pognon, c'est l'thème L'opinion d'ces débiles n'est pas essentielle Sans gène, c'est l'défilé des pigeons avec ou sans ailes Certains, pris de dégout, deviendront des scélérats Sortis des égouts, les bourges nous regardent En s'disant C'est ça les rats... La street a mauvais ragout, passe tes thunes et ça l'aidera A assaisonner de plus de gout, ça vaut le coup mais, ça, c'est rare J'voulais porter le stard-co mais les keufs m'ont mis les pinces On n'écoute pas Sarko, ici, seul le Parc est un prince Au plus profond d'mes songes, j'ai vu cette lueur lunaire Sans aucune honte J'vous présente le côté sombre de la ville lumière ×2 D'ici à Châtelet, des deux côtés du périph' on gronde Drogue, sexe et Noctambus voici la capitale du monde L'hiver est rude, la neige tombe et s'faufile par le zen Les mecs sont prudes et puis Te plombent dans les nuits parisiennes Paris, ville lumière, ouais, bienvenu dans la capitale On t'attrape comme Thiago Silva, porte le brassard d'el capitan Tout porte à croire qu'c'est mondain Donc les touristes dépensent plus devant ces sangsues Donc j'pense plus comme Rodin Les clochards gisent sur le sol, les dealers dans la zeb Des péniches en façade cachant les cadavres enfouis dans la Seine La fréquence des contrôles varie d'Passy à bès-Bar Entre le 16ème et l'18ème, y'a qu'le 17 qui sépare Yo, embrasse le peuple de Dakar à Brazza Une odeur de bazar, ici, ça fouette comme la madrassa Ouais, c'est Paname, ça des rats aux dimensions de macro Assume la cité des arts, un concert par rame de métro Efface le cliché béret, gondole et cornemuse Et, pour les fraudes de bus, devant les leurs On change de blaze comme Cassius A la différence de Totti, ici, les roms vident les bennes Et c'est pas les gars du 19 qui t'diront qu'la vie est belle Dans les dédales de Paname, j'n'ai pas d'égal, j'me balade Pas loin des halles, où les daleux parle mal de la femme Et je déballe des tas d'phases, au départ, j'n'avais pas d'bases Mais je taffe et les raps sales que je lâche te laisse patraque Je n'aime pas les paperasses, parlez pas d'ça J'ai le bac mais le choix d'ma vie c'est d'rapper la night Ouais, ça c'est ma life, j'ai pris des tas de claques Prié tard le soir, grillé par la BAC, c'est pas marrant J'ai gratté pas mal de phases de malades Si j'ai dragué ta femme, c'est un acte banal Je plane dans le calme, flâne quand je dave-bé J'ai pas le temps de parler aux fans à part aux tasses-pé La vie est ainsi faite, envier les alliés du système Chaque matinée sur lpallier, lcur habillé de tristesse Les yeux rouges écarlates, rentrant dune soirée banale Boire et foirer sa life dans lespoir de croiser la joie Gars, jte croyais capable Pourquoi tu t'détruis pas comme nous ? Réduits dans des débris dalcool croyant que Dieu pardonne tout Jattends que les juges de mon âme me condamnent Quils se demandent si jsuis têtu ou si jai fait le bon choix Me convoitant pour que débute un constat immoral Comme mes pensées emprisonnées dans les cellules de mon crâne Mes gars se foutent de la sentence Toi, quoi la peur, yo, cest tout cque tas dans lventre ? Jme suis retrouvé en présence de la démence Chemin faisant dans lindécence La roue tourne mais dans quel sens ? Est-ce quon avance ou on recule dans cet enfer ? Le temps nous joue des tours et la roue tourne à lenvers Tes du-per si tu crois qujrécupère des écus Lorsque jénumère mon vécu, mec, jaurais dû faire des études Dans les rues jerre sans vrai but, la vérité, cest quça me rend fou Comme ces rageux méprisants Me disant que jferai pas de grands coups Jveux pas dune vie fade et sans gout Jcraque, des fois jpète mon câble Sans tromper pour compter du fric comme un expert-comptable La vie, une pêche frontale, ils font les fiers Mais tous mes frères ont mal Pas dcur de pierre face aux pierres tombales Les mains sales et la rime propre, Paris Nord en pleine forme Comme d'hab, le ciel est gris comme ton Macintosh J'm'active, bosse car dans l'Bronx, les macs, les putes Le crack, ses thunes, mate, c'est stupide mais j'connais ça Malgré l'omerta, t'inquiète que nos mères savent Viens tester les nôtres, j't'assure ton corps sera méconnaissable Toujours dans les business bizarres Crise d'nerfs, inhale, j'ai plus l'temps Ni même de visage, je vis ma vie chaque milliseconde Les négros qui agissent comme des bitches me gonflent Je reste vrai même si c'est vrai Qu'les vrais négros irritent ce monde Le contraire se tient aussi J'sors une veste en cuir peinte sur un Tachini comme Saïd On bicrave même à l'aid, la débrouillardise du Pirates des caraïbes Hustler de luxe, longtemps que j'cogite sur l'métier On loue un appart' en face du comico pour les surveiller Trouve-moi dans un sombre côté du square J'ai le crack en solde si ta meuf a du mal à perdre du poids Issue dramatique, l'automatique m'a dit La technique est stricte, break, beat et spliffs, esquive les flics Et les balances même si des fois c'est pas si facile. J'préfère ça qu'être celui qui reste passif assis Sur l'banc à regarder les gros culs et les dollars qui passent j'rime salace, mes taulards bicravent Même à l'intérieur, qui suis-je pourn'pas mailler en liberté ? Si t'aimes pas, t'es un illetré, cousin Est-ce que tu captes, on veut du calme Tire deux fois dans le ciel, négro, j'ai cru y voir les yeux du Diable 86 Joon speaks Set that nigga in history 86, call me 86 Or Joon bitch you can take your pic Or take a pic, post a Insta flick Got your girl all on my hip Don't act like you ain't heard that For when I speak you niggas pissed Flippin this dawg you had it I got it no worry who watchin' ? So sophisticated Ain't no one watchin' Still niggas wanna hate you ? Tell somebody comes naughty I aint a gangster but Ill break neck I worked for mine, deserve all these checks Took chances nigga, won all my bets I'm a man nigga so I owe my threats Ain't worried about it, look at me I pay no mind and kept my eyes on me And you're still broke, and that talk is cheap Piss me I'mma tryna go get Ali Fist fight in that mirror nigga Like Rick Hill, rockin' Hilfiger I'm DMX Tous tes rappeurs c'est des mythomanes en puissance Qui rêveraient d'avoir le flow et l'épopée de qui j'pense Beaucoup trop longtemps que j'erre Et que j'leur mets des distances J'veux l'million maintenant je bosse avec... Heureusement que j'ai des gavas qui sont là pour moi Cette michto, elle veut mon porte-monnaie pas la bague au doigt Tes rappeurs, les éliminer ça n'me fait pas peur du tout Pour trafic tu prends la même peine que Marc Dutroux Comme d'hab, j'suis posé à PDM Et bisous aux haineux qui la ferment et qui laissent passer les hyènes On a le cur mort et les mains dans la merde A chacun de nos actes on se rapproche de l'enfer Perdu dans ma matrice, j'ai la grise mine de Gandalf Tu veux un feat ? Pose ton SMIC qu'on en reparle Parait que j'suis un prodige mais j'ai déjà déconné Donc, bébé, suce pas trop ma bite Même si je sais que je suis pas comme les autres Et que le médecin l'avait dit lors de léchographie ×2 J'ai des plaies, j'peux les rapper des heures Approche et apprends que j'ai jamais voulu être célèbre J'me réveille dans une Mercedes neuve Car hier j'ai noyé ma peine dans la Belvédère Ouais je bois des litres de vodka A la santé de ceux qui voulaient nous mettre des rottes-ca On vole pas aux voleurs, va t'occuper d'autres gars Moi si je suis un rappeur, je suis un rappeur haut de gamme J'ai la tête sur les épaules et les épaules dans la piscine Pâtes au pesto dans un resto de la city Tu côtoies des vieilles gos, moi mes khos n'ont que des missiles On fréquente des tel-hô mais tu me verras jamais à l'Ibis J'ai la monnaie, collègue, rien qu'on fume le pollen On est sept sur scène et parait qu'on est en colère Toujours OP j'opère, direction le soleil Je rappe sept sur sept, je suis le meilleur depuis le collège Jamais à l'heure à mes rendez-vous, excusez-moi monsieur J'avais mieux à faire, je suis aller manger sur les quais Après je comptais venir, mais y'avait des fans sur mes côtes Ils voulaient des photos et je suis mauvais à ce jeu Si tu me vois dans la rue, s'il te plait ne m'arrête pas Fais tes bails, j'ai ma tranquillité et ma rette-ba Si ce flic ouvre sa gueule, mettez le dans la caisse noire Nous n'avons que notre liberté en guise d'espoir Appel inconnu, salope de plus me parasite A peine reconnu, les jaloux sont plus J'ai pas lu l'avenir mais ça s'voit qu'ce monde est condamné Donc avant d'partir, j'dois finir tout c'que j'ai commencé Issu d'là où ça pue la mort, la drogue et les keufs Là où les peuples s'entendent entre musulmans, chrétiens et feujs Fils, le prestige se gagne en travaillant pas si tu suces Le crime paie mais y'a rien d'glorieux dans c'ness-busi Sont tous hors-jeu car j'suis défenseur avec un gun T'es défoncé sous rhum, j'écrirai mes versets sous l'porche On a tous bicrave alors pourquoi tu t'sens pousser des couilles ? Biatch, reste cool, c'est pas la Gucci qui fait l'lascar Alors qu'on s'serre les coudes, sert à rien vu qu'tu sers à rien Putain, vraie tantouze fais du boucan juste pour être craints Moi, j'ai le cran, la haine, le seum, quand j'serai grand J'voudrais le biff, être à l'abri afin d'claquer ses seufs Panama Bende on est sept, on peut t'faire chier toute la semaine Comme une merde dans laquelle j'viens d'marcher Les MC's sont tous sous ma semelle Le mic, on m'la donné, OK, rappons Mon Rap est frais, mon Rap pétille à consommer avec modération Sinon tu risques de t'blesser, le beat j'veux l'dresser Sache que même si j'flippe tu m'verras pas les yeux baissés Hey l'internaute, si t'aimes le Rap viens voir ma page Dans mon équipe on garde la tête haute Dans l'espoir de pas boire la tasse Écoute ce beat, mes khos kickent stone Mais ça, ça ne bouge pas depuis les Beattles ou les Rolling Stone J'connais mes bases, j'ai relu ma leçon et j'vote la paix Fais comme moi, écoute ces basses Mets l'volume à fond et hoche la tête J'lâche que des phases qui te fascinent, effacent tous les blazes Écoute les MC's sont sous plaques d'égouts Et n'ont qu'des placements faciles Perdre sa valeur dans c'monde,où l'argent fascine J'aime trop cette tension dans la salle Lorsque les fans attendent l'artiste 18 ans à peine, tu vois que l'âge ne fait rien Le beat prend déjà tarif et pourtant là je n'fais rien Jeune terrien qui n'aime pas rester seul, ouais Un frère au tel' dans la main gauche Et avec l'autre, ma belle, j'caresse tes seufs C'est l'binôme infernal, sors l'matos, prends le bédo J'préviens qu'ça va faire mal comme le lapin dans le métro C'est pour mes gars d'mmerce-Co Qui font du biff, arrêtent la hess Tu kiffes avec la tête, c'est qu'on kicke avec la tech Hassanettes sur hassanettes, j'les fais ap, j'les ferai Pour l'instant, j'suis dans l'optique de gérer des khenzettes La recette, on cherche tous à s'la procurer Fuck le procureur, trop d'curieux, ça a trop duré Au stud, j'me dis tue-les tous, j'compte même plus les douzes C'est pour tous mes couz équipés d'un putain d'bulletproof Faut-il un style sophistiqué ? Ouais, trop d'estime On est ssif-ma, nocif pour les flics, vont-ils kiffer ? Hein, c'est c'que j'me demande Quand j'me dit qu'faut que j'les démonte Dès l'tin-ma, j'reçois plein d'amendes, on massera pas la loi J'suis pas un padawan, wallah, rien d'un Balavoine J'parle à toi quand t'as pas la gnaque, tu passeras pas la douane C'est leur bel équilibre, j'viens de Berriz City J'suis le best, tu veux test, en un bang je t'élimine C'est pour tous mes reufs qui fument de l'herbe à l'air frais J'aime quand une voiture de keufs me laisse traverser Parfois j'ai envie de tout faire péter pour qu'il reste rien de ce désordre Ils s'battent pas pour... Mais restreindre ceux des autres Ok ça foire mais c'est pas grave j'pars c'est pour ma poire J'me fends la poire rien à faire mec, ... je vois Ah c'est comme ça qu'ça s'passe mec j'compte pas pour du bois C'est pour mes potes qui prennent du poids Hey, qui va kicker ça ? Gagne un peu de temps pour le prochain C'est comme ça qu'ça s'passe, ceux qui s'font crosser, j'aime aussi les gros seins J'suis pas skin même en polo Fred Perry, tu le sais J'suis le best, elle est loin l'époque de Hail Mary Jexpérimente des flows qui vont t'faire périr Pour les faux, ça risque d'être terrible T'es en vogue si t'as nos jers' et nos vestes teddy Meilleurs textes, meilleurs textiles, l'dernier cri Qu'ces MC's pousseront risquerait d'me faire plaisir Gardez vos bitches, j'suis l'homme qu'elles désirent J'débarque, elles deviennent célib, la vie c'est si hard Estime-toi frais si t'as ta mif et des biffs à faire Eff Gee, stop ! Fuck tout ça ! Quand j'gratte, c'est d'la frappe, il faut qu'ça cogne tout-par Face au Eff du L, qu'est-ce tu testes ? Mec, tu perds Tu fais l'fou mais t'es trop doux, tes potos t'appellent my boo Mes bulles d'air restent sur Terre, frère, tu sais Trop s'étonnent des babtous qui rappent et cassent tout Pff... Comme si on allait s'arrêter J'vais pas m'abaisser à ça mais j'vous mets la fessée Elles veulent caresser ma barbe car il paraît que c'est d'la balle Voudraient s'faire graisser la patte, au moins s'faire lécher la chatte Laissez-moi ! J'kiffe pour mes homies Tes sons soûlent plus qu'une bouteille d'eau-de-vie J'les écoute, fonce-dé, pour m'faire vomir Je sais c'que j'ai à perdre, je sais c'que j'ai à gagner Toujours pas d'Rolex au poignet, j'sirote ma mauresque au Panier Restons calmes, restons parés, que les commères restent au palier J'ai la fierté dans le sang tout comme mes collègues Oranais Leur Rap Game, c'est un putain d'truc de putarelle En une semaine de Planète Rap J'vois plus de putes qu'à Bucarest, j'me prends plus la tête Ça vaut plus la peine, tu crois qu'tu m'arrêtes J'te coupe un bras et puis je t'encule avec J'te crève un il avec ton propre orteil All black comme le croque-mort, requiem post-mortem J'suis fort, j'suis formel, je n'sors qu'des trésors d'orfèvre J'commence doucement, j'finis gore comme Hostel ou Dorcel Présente-moi tes jolies potes, j'leur présenterai mon lollipop J'ai mis ma eue-qu dans tellement d'gorges Elles m'appellent toutes le polyglotte J'maîtrise la langue jusqu'aux litotes, la France jusqu'aux iPod's J'redonne de l'espoir au Game, j'redéfinis le mot Hip-Hop Burbigo, j'vais les ken jusqu'à c'que j'bande plus Ils vont tous crier mon blaze comme s'ils étaient mes plans cul Qu'ils crèvent avec leurs 16 jetables J'rêve de les voir en sang, les soigner avec du sel de table Me cherche pas ou tu risques de perdre Tout l'monde a vu mes RC, j'ai percé sans sucer d'verge Qui peut en dire autant ? Sûrement pas ces tire-au-flancs Je tire au but, je tire au centre depuis qu'la faim m'a pris au ventre J'suis rieur, c'est curieux Jeune déviant, retourne chez tes vieux Nah, sérieux, j'suis meilleur même si je fais rien Jump dans c'buiz' comme un cop dans l'six, ou un mafieux Méfiant comme un il myope dans l'viseur Il y a des milliards de choses que j'veux illico presto Mini-bar, gov' chromé, whisky, frappe, resto Ils s'blessent pour des valeurs ajoutées Mais j'laisse faire, il m'reste quelques rappeurs à shooter J'me fiche de l'égalité des chances, j'vis Pour les lyrics et la qualité des jantes J'me relaxe, spliff sur quais d'Seine Et on m'a dit que jexcellais Quand j'rappe, t'es vexé, désolé, j'suis l'next level Roule de longues battes pour éviter qu'on bosse Et ça fait double contact entre ma bite et ton gloss Chillance, avec les vilains prend d'la distance On parle de filles ienbs, de filles minces et de finance5</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Enorme freestyle de Nekfeu en live dans Planète Rap !</t>
+          <t>Plus pareil</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>×4 J'suis sorti du ventre de ma mère pour vous faire l'album de l'année Les autres vendent de la merde, je l'ai fait sur mon propre label Dis-moi, c'est quoi l'album de l'année ? Feu ! Feu ! Feu ! Feu ! Comme Walter White, j'ai mes Clarks Wallabees Sur, serre-moi la main, frère, claque-moi la bise Je ne côtoie que des avions à la carlingue parfaite J'ai beaucoup plus de goût que Karl Lagerfeld Le monde de l'art est vantard, il te vend du street-art Mais ne veulent surtout pas voir mes scarlas graffer en vandale Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Feu ! Tu peux ressentir l'aura dans nos raps, sortez les anoraks On aura bientôt l'orage selon l'oracle Ma conscience m'a dit Qui es-tu ? Veux-tu vivre dans le vice ou dans la quiétude ? Ça dépend où est l'pèze, on doit être bêtes, ouais, p't-être Mais ma plume peut clouer l'bec de Houellebecq Ici, on est vite tentés, il vaut mieux que tu vives ta quête J'ai entendu Vide ta caisse, le lendemain, les flics enquêtent ×2 C'est quand j'aurai des millions que j'me questionnerai Dans quelques années, je me demande qu'est-ce qu'on aura Si je n'savais pas que les keufs m'espionneraient Jamais j'démissionerais même s'ils veulent mon aura La voix d'la tess' dans l'oreille Faut qu'on encaisse dans le Rap Mental d'acier tah les chefs de guerre Dis-moi tu vas ken lequel ? Je n'vois que des merdeux gueh Tu vois pas comme les chiennes te guettent ? Elles rêvent d'être avec moi comme dans des fiançailles Pour que je ne regarde plus mes finances InchAllah, je ne mettrai qu'une fille enceinte J'prie mon Dieu mais je reste silencieux Pris dans l'jeu, c'était une évidence Pris dans l'feu, qui sort seul Méfiance, faut qu'tu prennes tes distances Vie d'malfrat en noir et blanc comme les films anciens Quand on est sur scène c'est l'empire byzantin Mon équipe rend dingues les pires depuis bambins La nuit, je sors sans but comme un somnambule Y'a certains rêves que les Hommes n'ont plus J'ai vu cette fille, on était seuls dans l'bus Elle avait les yeux rouges, elle avait pas seulement bu Elle avait de la came dans un sac Balenciaga Elle s'est fait caner, c'est ça d'balancer un gars Dans Paname, y'en a qui s'perdent, y'en a qu'espèrent Péter des sapes Agnès B., des Nike SB Dehors, c'est froid, y'a plus d'humanité Un homme est mort inanimé devant un immeuble inhabité C'est la crise ! La crise ? Qui est-ce qu'elle atteint ? Toi, moi ou le suicidaire qui escalade un toit ? Si Dieu veut, jusqu'à 120 ans voilà mon espérance de vie Toujours dans l'excellence, tu connais mes préférences On est vraiment des références de style Dans l'équipe, aucune déviance, nan On ne tolère pas la médisance, nan On est méfiants, choisis ton camp Au lieu de rester entre deux fils, nan Tant que je n'ai pas de millions Mes egotrips resteront de l'autodérision Besoin de causes et regrets pour quitter ce monde de merde Je me laisse aller avant de prendre une autre décision Trop de menaces et de coups de crasse pour des loves Je le sens tout d'suite quand un traitre tape mon épaule Ne le vois-tu pas ? De quoi tu parles à part de ton ego ? Moi, rester à ma place, ce n'est pas dans mon créneau J'veux que Def Jam signe mon chèque, ouais, mon putain d'chèque J'veux qu'la SACEM signe un chèque, ouais, mon putain d'chèque J'veux que Def Jam signe un chèque, ouais, mon putain d'chèque J'veux qu'la Def Jam signe un chèque, ouais, mon putain d'chèque Négro, faut d'la maille, ouais, mon négro, faut d'la maille Rebeu, faut d'la maille, ouais, mon rebeu, faut d'la maille Babtou, faut d'la maille, ouais, mon babtou, faut d'la maille Babtou, faut d'la maille, ouais, mon babtou, faut d'la maille J'dors les yeux ouverts, j'parle avec les esprits J'ai fait souffrir car j'ai souffert J'ai fait des erreurs aujourd'hui j'en paie l'prix J'suis bon qu'à rapper c'que j'suis Mes raisons, mes torts, c'est ça être vrai, couz' Et foutre des foufs dans mes clips Que moi-même je n'voudrais ni comme sur ni comme épouse J'suis qu'un fou parmi des cons En vrai, j'sais même pas dans quoi j'suis Ces bâtards m'critiquent, si j'les laisse ouvrir leurs gueules C'est juste que j'aime savoir dans quoi j'chie J'lâche des perles en stud' Mais j'crois qu'l'industrie n'y voit qu'tchi Et ma voisine du dessus Me regarde comme si j'étais un frère Kouachi On apprend à s'faire tous seuls, vu qu'le système nous néglige On deale en croyant être screds Alors qu'on s'fait remarquer comme une pute dans une église J'rappe pour mes rabzouzs J'rappe pour mes niggas Black, blanche ou beurre, j'les aime toutes Du moment qu'elles remplissent leurs leggings J'ai l'inspi' à Tupac, flow sale comme l'argent d'la bicrave Frais dans les clips à t'en faire croire Qu'être négro en France n'a jamais été un handicap J'pratique le haut-débit, Numéricable Toi, t'es un faux mac mais ne pute véritable J'me mets à nu, mais j'suis pudique Un peu comme une actrice X en Niqab Beaucoup qui font les hlels mais qui les baise en chette-ca ? Y'a ton ADN sous la semelle de ma sket-ba Micro semi-auto, j'appuie sur la chette-ga J'ai perdu au loto donc j'ai bibi la sel3a J'suis avec mes potos, capuché, squette-ca Trop chaud, loco, abusé, teste pas Ton équipe est et prête à gober des chibres Mon équipe est glauque et prête à t'voler tes litrons Tu veux tester mes salauds, ça fait bang, genre saloon Frère, si je t'allume c'est que j'suis prêt pour l'salut T'es pas d'la mif, parle-moi biff ou parle-moi d'profit Dix kilos d'weed, un kilo d'shit, le tout sera blanchi On fume le matos, mes vatos vont brûler ces rappeurs Ça sera du gâteau comme rotte-ca le de l'éducateur A bord d'une Merco Benz, vitres teintées, grosse boisson C'est la moisson, les mousseux sont d'sortie, ouais eh mistinguette Rentre dans le VIP si tu veux changer de vie Si tu rentres dans le lit, sache qu'on rentre dans le mille J'suis un hot nigga Mes gavas derrière oim ne craignent que God, nigga Mon équipe pète les scores pendant qu'tu t'fichas, kho Rebeu, renois, babtous, chicanos Tes négros softs ont des chichas roses Suffit pas d'pomper tous les rappeurs de Chicago Cassos, plaques et matraques la capitale est yomb Ici ni fleuve ni lac, juste une scène lasse-dèg donc allons-y, fuyons Entre les putes, les connasses, les gars, nous trions Vie lassante nous rions donc j'accomplis mon triomphe comme l'Arc Imagine la Tour Eiffel se faire amputer Boumbadaboum ! Encore un keuf vient d'se faire buter Le pognon, c'est l'thème L'opinion d'ces débiles n'est pas essentielle Sans gène, c'est l'défilé des pigeons avec ou sans ailes Certains, pris de dégout, deviendront des scélérats Sortis des égouts, les bourges nous regardent En s'disant C'est ça les rats... La street a mauvais ragout, passe tes thunes et ça l'aidera A assaisonner de plus de gout, ça vaut le coup mais, ça, c'est rare J'voulais porter le stard-co mais les keufs m'ont mis les pinces On n'écoute pas Sarko, ici, seul le Parc est un prince Au plus profond d'mes songes, j'ai vu cette lueur lunaire Sans aucune honte J'vous présente le côté sombre de la ville lumière ×2 D'ici à Châtelet, des deux côtés du périph' on gronde Drogue, sexe et Noctambus voici la capitale du monde L'hiver est rude, la neige tombe et s'faufile par le zen Les mecs sont prudes et puis Te plombent dans les nuits parisiennes Paris, ville lumière, ouais, bienvenu dans la capitale On t'attrape comme Thiago Silva, porte le brassard d'el capitan Tout porte à croire qu'c'est mondain Donc les touristes dépensent plus devant ces sangsues Donc j'pense plus comme Rodin Les clochards gisent sur le sol, les dealers dans la zeb Des péniches en façade cachant les cadavres enfouis dans la Seine La fréquence des contrôles varie d'Passy à bès-Bar Entre le 16ème et l'18ème, y'a qu'le 17 qui sépare Yo, embrasse le peuple de Dakar à Brazza Une odeur de bazar, ici, ça fouette comme la madrassa Ouais, c'est Paname, ça des rats aux dimensions de macro Assume la cité des arts, un concert par rame de métro Efface le cliché béret, gondole et cornemuse Et, pour les fraudes de bus, devant les leurs On change de blaze comme Cassius A la différence de Totti, ici, les roms vident les bennes Et c'est pas les gars du 19 qui t'diront qu'la vie est belle Dans les dédales de Paname, j'n'ai pas d'égal, j'me balade Pas loin des halles, où les daleux parle mal de la femme Et je déballe des tas d'phases, au départ, j'n'avais pas d'bases Mais je taffe et les raps sales que je lâche te laisse patraque Je n'aime pas les paperasses, parlez pas d'ça J'ai le bac mais le choix d'ma vie c'est d'rapper la night Ouais, ça c'est ma life, j'ai pris des tas de claques Prié tard le soir, grillé par la BAC, c'est pas marrant J'ai gratté pas mal de phases de malades Si j'ai dragué ta femme, c'est un acte banal Je plane dans le calme, flâne quand je dave-bé J'ai pas le temps de parler aux fans à part aux tasses-pé La vie est ainsi faite, envier les alliés du système Chaque matinée sur lpallier, lcur habillé de tristesse Les yeux rouges écarlates, rentrant dune soirée banale Boire et foirer sa life dans lespoir de croiser la joie Gars, jte croyais capable Pourquoi tu t'détruis pas comme nous ? Réduits dans des débris dalcool croyant que Dieu pardonne tout Jattends que les juges de mon âme me condamnent Quils se demandent si jsuis têtu ou si jai fait le bon choix Me convoitant pour que débute un constat immoral Comme mes pensées emprisonnées dans les cellules de mon crâne Mes gars se foutent de la sentence Toi, quoi la peur, yo, cest tout cque tas dans lventre ? Jme suis retrouvé en présence de la démence Chemin faisant dans lindécence La roue tourne mais dans quel sens ? Est-ce quon avance ou on recule dans cet enfer ? Le temps nous joue des tours et la roue tourne à lenvers Tes du-per si tu crois qujrécupère des écus Lorsque jénumère mon vécu, mec, jaurais dû faire des études Dans les rues jerre sans vrai but, la vérité, cest quça me rend fou Comme ces rageux méprisants Me disant que jferai pas de grands coups Jveux pas dune vie fade et sans gout Jcraque, des fois jpète mon câble Sans tromper pour compter du fric comme un expert-comptable La vie, une pêche frontale, ils font les fiers Mais tous mes frères ont mal Pas dcur de pierre face aux pierres tombales Les mains sales et la rime propre, Paris Nord en pleine forme Comme d'hab, le ciel est gris comme ton Macintosh J'm'active, bosse car dans l'Bronx, les macs, les putes Le crack, ses thunes, mate, c'est stupide mais j'connais ça Malgré l'omerta, t'inquiète que nos mères savent Viens tester les nôtres, j't'assure ton corps sera méconnaissable Toujours dans les business bizarres Crise d'nerfs, inhale, j'ai plus l'temps Ni même de visage, je vis ma vie chaque milliseconde Les négros qui agissent comme des bitches me gonflent Je reste vrai même si c'est vrai Qu'les vrais négros irritent ce monde Le contraire se tient aussi J'sors une veste en cuir peinte sur un Tachini comme Saïd On bicrave même à l'aid, la débrouillardise du Pirates des caraïbes Hustler de luxe, longtemps que j'cogite sur l'métier On loue un appart' en face du comico pour les surveiller Trouve-moi dans un sombre côté du square J'ai le crack en solde si ta meuf a du mal à perdre du poids Issue dramatique, l'automatique m'a dit La technique est stricte, break, beat et spliffs, esquive les flics Et les balances même si des fois c'est pas si facile. J'préfère ça qu'être celui qui reste passif assis Sur l'banc à regarder les gros culs et les dollars qui passent j'rime salace, mes taulards bicravent Même à l'intérieur, qui suis-je pourn'pas mailler en liberté ? Si t'aimes pas, t'es un illetré, cousin Est-ce que tu captes, on veut du calme Tire deux fois dans le ciel, négro, j'ai cru y voir les yeux du Diable 86 Joon speaks Set that nigga in history 86, call me 86 Or Joon bitch you can take your pic Or take a pic, post a Insta flick Got your girl all on my hip Don't act like you ain't heard that For when I speak you niggas pissed Flippin this dawg you had it I got it no worry who watchin' ? So sophisticated Ain't no one watchin' Still niggas wanna hate you ? Tell somebody comes naughty I aint a gangster but Ill break neck I worked for mine, deserve all these checks Took chances nigga, won all my bets I'm a man nigga so I owe my threats Ain't worried about it, look at me I pay no mind and kept my eyes on me And you're still broke, and that talk is cheap Piss me I'mma tryna go get Ali Fist fight in that mirror nigga Like Rick Hill, rockin' Hilfiger I'm DMX Tous tes rappeurs c'est des mythomanes en puissance Qui rêveraient d'avoir le flow et l'épopée de qui j'pense Beaucoup trop longtemps que j'erre Et que j'leur mets des distances J'veux l'million maintenant je bosse avec... Heureusement que j'ai des gavas qui sont là pour moi Cette michto, elle veut mon porte-monnaie pas la bague au doigt Tes rappeurs, les éliminer ça n'me fait pas peur du tout Pour trafic tu prends la même peine que Marc Dutroux Comme d'hab, j'suis posé à PDM Et bisous aux haineux qui la ferment et qui laissent passer les hyènes On a le cur mort et les mains dans la merde A chacun de nos actes on se rapproche de l'enfer Perdu dans ma matrice, j'ai la grise mine de Gandalf Tu veux un feat ? Pose ton SMIC qu'on en reparle Parait que j'suis un prodige mais j'ai déjà déconné Donc, bébé, suce pas trop ma bite Même si je sais que je suis pas comme les autres Et que le médecin l'avait dit lors de léchographie ×2 J'ai des plaies, j'peux les rapper des heures Approche et apprends que j'ai jamais voulu être célèbre J'me réveille dans une Mercedes neuve Car hier j'ai noyé ma peine dans la Belvédère Ouais je bois des litres de vodka A la santé de ceux qui voulaient nous mettre des rottes-ca On vole pas aux voleurs, va t'occuper d'autres gars Moi si je suis un rappeur, je suis un rappeur haut de gamme J'ai la tête sur les épaules et les épaules dans la piscine Pâtes au pesto dans un resto de la city Tu côtoies des vieilles gos, moi mes khos n'ont que des missiles On fréquente des tel-hô mais tu me verras jamais à l'Ibis J'ai la monnaie, collègue, rien qu'on fume le pollen On est sept sur scène et parait qu'on est en colère Toujours OP j'opère, direction le soleil Je rappe sept sur sept, je suis le meilleur depuis le collège Jamais à l'heure à mes rendez-vous, excusez-moi monsieur J'avais mieux à faire, je suis aller manger sur les quais Après je comptais venir, mais y'avait des fans sur mes côtes Ils voulaient des photos et je suis mauvais à ce jeu Si tu me vois dans la rue, s'il te plait ne m'arrête pas Fais tes bails, j'ai ma tranquillité et ma rette-ba Si ce flic ouvre sa gueule, mettez le dans la caisse noire Nous n'avons que notre liberté en guise d'espoir Appel inconnu, salope de plus me parasite A peine reconnu, les jaloux sont plus J'ai pas lu l'avenir mais ça s'voit qu'ce monde est condamné Donc avant d'partir, j'dois finir tout c'que j'ai commencé Issu d'là où ça pue la mort, la drogue et les keufs Là où les peuples s'entendent entre musulmans, chrétiens et feujs Fils, le prestige se gagne en travaillant pas si tu suces Le crime paie mais y'a rien d'glorieux dans c'ness-busi Sont tous hors-jeu car j'suis défenseur avec un gun T'es défoncé sous rhum, j'écrirai mes versets sous l'porche On a tous bicrave alors pourquoi tu t'sens pousser des couilles ? Biatch, reste cool, c'est pas la Gucci qui fait l'lascar Alors qu'on s'serre les coudes, sert à rien vu qu'tu sers à rien Putain, vraie tantouze fais du boucan juste pour être craints Moi, j'ai le cran, la haine, le seum, quand j'serai grand J'voudrais le biff, être à l'abri afin d'claquer ses seufs Panama Bende on est sept, on peut t'faire chier toute la semaine Comme une merde dans laquelle j'viens d'marcher Les MC's sont tous sous ma semelle Le mic, on m'la donné, OK, rappons Mon Rap est frais, mon Rap pétille à consommer avec modération Sinon tu risques de t'blesser, le beat j'veux l'dresser Sache que même si j'flippe tu m'verras pas les yeux baissés Hey l'internaute, si t'aimes le Rap viens voir ma page Dans mon équipe on garde la tête haute Dans l'espoir de pas boire la tasse Écoute ce beat, mes khos kickent stone Mais ça, ça ne bouge pas depuis les Beattles ou les Rolling Stone J'connais mes bases, j'ai relu ma leçon et j'vote la paix Fais comme moi, écoute ces basses Mets l'volume à fond et hoche la tête J'lâche que des phases qui te fascinent, effacent tous les blazes Écoute les MC's sont sous plaques d'égouts Et n'ont qu'des placements faciles Perdre sa valeur dans c'monde,où l'argent fascine J'aime trop cette tension dans la salle Lorsque les fans attendent l'artiste 18 ans à peine, tu vois que l'âge ne fait rien Le beat prend déjà tarif et pourtant là je n'fais rien Jeune terrien qui n'aime pas rester seul, ouais Un frère au tel' dans la main gauche Et avec l'autre, ma belle, j'caresse tes seufs C'est l'binôme infernal, sors l'matos, prends le bédo J'préviens qu'ça va faire mal comme le lapin dans le métro C'est pour mes gars d'mmerce-Co Qui font du biff, arrêtent la hess Tu kiffes avec la tête, c'est qu'on kicke avec la tech Hassanettes sur hassanettes, j'les fais ap, j'les ferai Pour l'instant, j'suis dans l'optique de gérer des khenzettes La recette, on cherche tous à s'la procurer Fuck le procureur, trop d'curieux, ça a trop duré Au stud, j'me dis tue-les tous, j'compte même plus les douzes C'est pour tous mes couz équipés d'un putain d'bulletproof Faut-il un style sophistiqué ? Ouais, trop d'estime On est ssif-ma, nocif pour les flics, vont-ils kiffer ? Hein, c'est c'que j'me demande Quand j'me dit qu'faut que j'les démonte Dès l'tin-ma, j'reçois plein d'amendes, on massera pas la loi J'suis pas un padawan, wallah, rien d'un Balavoine J'parle à toi quand t'as pas la gnaque, tu passeras pas la douane C'est leur bel équilibre, j'viens de Berriz City J'suis le best, tu veux test, en un bang je t'élimine C'est pour tous mes reufs qui fument de l'herbe à l'air frais J'aime quand une voiture de keufs me laisse traverser Parfois j'ai envie de tout faire péter pour qu'il reste rien de ce désordre Ils s'battent pas pour... Mais restreindre ceux des autres Ok ça foire mais c'est pas grave j'pars c'est pour ma poire J'me fends la poire rien à faire mec, ... je vois Ah c'est comme ça qu'ça s'passe mec j'compte pas pour du bois C'est pour mes potes qui prennent du poids Hey, qui va kicker ça ? Gagne un peu de temps pour le prochain C'est comme ça qu'ça s'passe, ceux qui s'font crosser, j'aime aussi les gros seins J'suis pas skin même en polo Fred Perry, tu le sais J'suis le best, elle est loin l'époque de Hail Mary Jexpérimente des flows qui vont t'faire périr Pour les faux, ça risque d'être terrible T'es en vogue si t'as nos jers' et nos vestes teddy Meilleurs textes, meilleurs textiles, l'dernier cri Qu'ces MC's pousseront risquerait d'me faire plaisir Gardez vos bitches, j'suis l'homme qu'elles désirent J'débarque, elles deviennent célib, la vie c'est si hard Estime-toi frais si t'as ta mif et des biffs à faire Eff Gee, stop ! Fuck tout ça ! Quand j'gratte, c'est d'la frappe, il faut qu'ça cogne tout-par Face au Eff du L, qu'est-ce tu testes ? Mec, tu perds Tu fais l'fou mais t'es trop doux, tes potos t'appellent my boo Mes bulles d'air restent sur Terre, frère, tu sais Trop s'étonnent des babtous qui rappent et cassent tout Pff... Comme si on allait s'arrêter J'vais pas m'abaisser à ça mais j'vous mets la fessée Elles veulent caresser ma barbe car il paraît que c'est d'la balle Voudraient s'faire graisser la patte, au moins s'faire lécher la chatte Laissez-moi ! J'kiffe pour mes homies Tes sons soûlent plus qu'une bouteille d'eau-de-vie J'les écoute, fonce-dé, pour m'faire vomir Je sais c'que j'ai à perdre, je sais c'que j'ai à gagner Toujours pas d'Rolex au poignet, j'sirote ma mauresque au Panier Restons calmes, restons parés, que les commères restent au palier J'ai la fierté dans le sang tout comme mes collègues Oranais Leur Rap Game, c'est un putain d'truc de putarelle En une semaine de Planète Rap J'vois plus de putes qu'à Bucarest, j'me prends plus la tête Ça vaut plus la peine, tu crois qu'tu m'arrêtes J'te coupe un bras et puis je t'encule avec J'te crève un il avec ton propre orteil All black comme le croque-mort, requiem post-mortem J'suis fort, j'suis formel, je n'sors qu'des trésors d'orfèvre J'commence doucement, j'finis gore comme Hostel ou Dorcel Présente-moi tes jolies potes, j'leur présenterai mon lollipop J'ai mis ma eue-qu dans tellement d'gorges Elles m'appellent toutes le polyglotte J'maîtrise la langue jusqu'aux litotes, la France jusqu'aux iPod's J'redonne de l'espoir au Game, j'redéfinis le mot Hip-Hop Burbigo, j'vais les ken jusqu'à c'que j'bande plus Ils vont tous crier mon blaze comme s'ils étaient mes plans cul Qu'ils crèvent avec leurs 16 jetables J'rêve de les voir en sang, les soigner avec du sel de table Me cherche pas ou tu risques de perdre Tout l'monde a vu mes RC, j'ai percé sans sucer d'verge Qui peut en dire autant ? Sûrement pas ces tire-au-flancs Je tire au but, je tire au centre depuis qu'la faim m'a pris au ventre J'suis rieur, c'est curieux Jeune déviant, retourne chez tes vieux Nah, sérieux, j'suis meilleur même si je fais rien Jump dans c'buiz' comme un cop dans l'six, ou un mafieux Méfiant comme un il myope dans l'viseur Il y a des milliards de choses que j'veux illico presto Mini-bar, gov' chromé, whisky, frappe, resto Ils s'blessent pour des valeurs ajoutées Mais j'laisse faire, il m'reste quelques rappeurs à shooter J'me fiche de l'égalité des chances, j'vis Pour les lyrics et la qualité des jantes J'me relaxe, spliff sur quais d'Seine Et on m'a dit que jexcellais Quand j'rappe, t'es vexé, désolé, j'suis l'next level Roule de longues battes pour éviter qu'on bosse Et ça fait double contact entre ma bite et ton gloss Chillance, avec les vilains prend d'la distance On parle de filles ienbs, de filles minces et de finance5</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Plus pareil</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Tu suces, tu sers à rien T'es microscopique tel un acarien Je brasse et je brasse et je brasse, mais toi tu n'es rien qu'un arlequin J'débarque à l'improviste comme Billy Cocaïne J'ai pas reçu d'invit donc j'me codéine J'ai mélangé prométhazine sprite et codé pour en faire un excellent lean J'débite les rimes, oui je n'suis pas clean, j'immite les humanoïdes Dix bites dans la teush à l'ennemi, limonade à liqueur d'opioïde Devant la TV je n'matte qu'On n'Est Pas Couché, enfumé sous gnax en m'servant un double rre-vé Trop bourré sur l'pc j'regarde la MMA et j'en profite pour taper d'la bonne C Mauvais délires et débile sous LSD je vois et je vais encaisser les low kicks J'entends dans ma tête des rires et des rires et des rires, il me semble que j'suis sick Dans ma tête ils sont six, and three d'entre eux sont accros aux sticks Ces trois là très souvent me réclament de rouler un spliff comme si la weed était gratuite, comme si la weed était gratuite Le regard dans le vide j'ai le cerveau de freezer, légèrement schizoïde il y a sûrement une erreur Une erreur ça prend deux R comme terreur et 2zer Washington Mon corps et mon esprit sont dissociés je pèse deux tones J'suis complètement vidé, l'acide dans les recepteurs deux goutes de diéthylamide bad trip de 3h Faudrait p't'etre que j'fasse un truc car la redescente est assez difficile Si mes parents me voyaient dans cet état c'est sur qu'ils m'auraient déjà kill Ma mère m'a souvent dit les drogues c'est mal et ça peut même être létal Elle me disait aussi que ça nous rendait bête et pas normal, comme le racisme juif et anti-black Sévissant depuis des siècles celui-ci n'est pas légal, cent fois plus dangereux que les drogues et la galle Si présent pourtant, certains méritent des claques plutôt qu'un mac 22 octobre 2k16 j'assistais excité à mon premier pèlerinage musicale L'Guizi foncedé débitait des rimes et des rimes sous gros shit, oui j'étais à la Cigale Désormais j'attends qu'le gremlins fassent les backs avant le bac Le 16 décembre à la fnac pour pecho l'album-black On écrit, on tté-fri On roule des spliffs et je fais l'trie Boulette ? Pas boulette, sur le sol j'retrouve des têtes J'tabasse tellement les wacks qu'on m'appelle souvent l'nouveau Nek' Je fume, je rime, tu déprimes, j'bois du lean avec ma team Ces rappeurs sont has been, ma teen a le même boule que Kim Je trend set et oui j'me la pète, oui j'pète mon teh d'OG Kush J'ai kiffé sa bonne beuh-er, j'en rachète 500 meujs Tu flippes quand je dégaine, m'esquive quand je kick t'en sortira pas indemne Tellement d'hasch dans les veines, tes textes sentent la merde même à 100 kilomètres d'la seine ou dix, vernon zooo Si j'te croise j'te ferais mal à la manière de Framal J'te troue de trente balles, tu fall et devient tout pâle Donc cale toi ça dans l'crâne tu canes et je plane tel l'Empreur du Sale J'suis preneur de soufflette profesional et oui je fly comme Phall à la Don Dada Imperturbable même quand le cell sonne J'lâche un dab quand j'applique le cellophane Incompris j'me sens comme Cell, sans phone J'me présente mon blaze c'est Kagame-san J'comprends qu'tu sois fan mais dorénavant appelle moi Kami-sama Ces faux mc sont mauvais, flagrant comme l'obésité morbide à la big mama Sa mère ça suce, z'ont pas d'inspi donc sans cesse parle de tess d'ecsta et de cess C'est pas sensé même défoncé leurs faussent lyrics sont nasent ils croient qu'ils pèsent Si ça te plait pas t'as qu'à diskliker, carte visa dans la main j'fais taffer l'caissier T'aimes te ficha au lycée t'es pas ma tasse d'café j'préfère les filles discrète, mignonne, brunette pas trop maquillé Tu kiffes les beurettes pas belles kiffant faire la fête, la fête se fera bien dans leur chatte mouillées Au bout de deux trois verres ces salopes sont toutes sous l'emprise du Jack D Je crois avoir définit la définition du mot taspé, une keh sous mojito ou plutôt Mojito sur keh Ce fils de pute c'est ma beurette de luxe, suce j'arrive Yass comme Luxe pendant qu't'écoutes des bails claqués Je trouve ce son bien trop étrange, c'est donc la fin de ce mauvais mélange</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>J’avais un rêve</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Tu suces, tu sers à rien T'es microscopique tel un acarien Je brasse et je brasse et je brasse, mais toi tu n'es rien qu'un arlequin J'débarque à l'improviste comme Billy Cocaïne J'ai pas reçu d'invit donc j'me codéine J'ai mélangé prométhazine sprite et codé pour en faire un excellent lean J'débite les rimes, oui je n'suis pas clean, j'immite les humanoïdes Dix bites dans la teush à l'ennemi, limonade à liqueur d'opioïde Devant la TV je n'matte qu'On n'Est Pas Couché, enfumé sous gnax en m'servant un double rre-vé Trop bourré sur l'pc j'regarde la MMA et j'en profite pour taper d'la bonne C Mauvais délires et débile sous LSD je vois et je vais encaisser les low kicks J'entends dans ma tête des rires et des rires et des rires, il me semble que j'suis sick Dans ma tête ils sont six, and three d'entre eux sont accros aux sticks Ces trois là très souvent me réclament de rouler un spliff comme si la weed était gratuite, comme si la weed était gratuite Le regard dans le vide j'ai le cerveau de freezer, légèrement schizoïde il y a sûrement une erreur Une erreur ça prend deux R comme terreur et 2zer Washington Mon corps et mon esprit sont dissociés je pèse deux tones J'suis complètement vidé, l'acide dans les recepteurs deux goutes de diéthylamide bad trip de 3h Faudrait p't'etre que j'fasse un truc car la redescente est assez difficile Si mes parents me voyaient dans cet état c'est sur qu'ils m'auraient déjà kill Ma mère m'a souvent dit les drogues c'est mal et ça peut même être létal Elle me disait aussi que ça nous rendait bête et pas normal, comme le racisme juif et anti-black Sévissant depuis des siècles celui-ci n'est pas légal, cent fois plus dangereux que les drogues et la galle Si présent pourtant, certains méritent des claques plutôt qu'un mac 22 octobre 2k16 j'assistais excité à mon premier pèlerinage musicale L'Guizi foncedé débitait des rimes et des rimes sous gros shit, oui j'étais à la Cigale Désormais j'attends qu'le gremlins fassent les backs avant le bac Le 16 décembre à la fnac pour pecho l'album-black On écrit, on tté-fri On roule des spliffs et je fais l'trie Boulette ? Pas boulette, sur le sol j'retrouve des têtes J'tabasse tellement les wacks qu'on m'appelle souvent l'nouveau Nek' Je fume, je rime, tu déprimes, j'bois du lean avec ma team Ces rappeurs sont has been, ma teen a le même boule que Kim Je trend set et oui j'me la pète, oui j'pète mon teh d'OG Kush J'ai kiffé sa bonne beuh-er, j'en rachète 500 meujs Tu flippes quand je dégaine, m'esquive quand je kick t'en sortira pas indemne Tellement d'hasch dans les veines, tes textes sentent la merde même à 100 kilomètres d'la seine ou dix, vernon zooo Si j'te croise j'te ferais mal à la manière de Framal J'te troue de trente balles, tu fall et devient tout pâle Donc cale toi ça dans l'crâne tu canes et je plane tel l'Empreur du Sale J'suis preneur de soufflette profesional et oui je fly comme Phall à la Don Dada Imperturbable même quand le cell sonne J'lâche un dab quand j'applique le cellophane Incompris j'me sens comme Cell, sans phone J'me présente mon blaze c'est Kagame-san J'comprends qu'tu sois fan mais dorénavant appelle moi Kami-sama Ces faux mc sont mauvais, flagrant comme l'obésité morbide à la big mama Sa mère ça suce, z'ont pas d'inspi donc sans cesse parle de tess d'ecsta et de cess C'est pas sensé même défoncé leurs faussent lyrics sont nasent ils croient qu'ils pèsent Si ça te plait pas t'as qu'à diskliker, carte visa dans la main j'fais taffer l'caissier T'aimes te ficha au lycée t'es pas ma tasse d'café j'préfère les filles discrète, mignonne, brunette pas trop maquillé Tu kiffes les beurettes pas belles kiffant faire la fête, la fête se fera bien dans leur chatte mouillées Au bout de deux trois verres ces salopes sont toutes sous l'emprise du Jack D Je crois avoir définit la définition du mot taspé, une keh sous mojito ou plutôt Mojito sur keh Ce fils de pute c'est ma beurette de luxe, suce j'arrive Yass comme Luxe pendant qu't'écoutes des bails claqués Je trouve ce son bien trop étrange, c'est donc la fin de ce mauvais mélange</t>
+          <t>La vrai fraternité, c'est déjà terminé On voit si t'as l'sang chaud une fois tes artères vidées C'est la guerre contre ces réfractaires givrés J'les met à terre s'ils déblatèrent sur mes affaires privées C'est la merde! Non j'veux pas m'faire des idées Détailler c'est risqué mais j'ai pas l'air d'hésiter Mais là frère c'que je vis c'est la célébrité J'lai mérité pour ça pas d'sérénité J'baise ta cacophonie j'vis ma vie Et j'te rends dingue comme une pathologie psychiatrique Putain y'as trop d'folies! Mais face aux phobies j'y arrive Tu cherches la merde, c'est que c'est la sodomie qui t'attire! Mon clan t'rentre dedans, sans prendre de gants C'est sanglant nan nan franchement Il est grand temps que j'me venge! Nekfeu, Framal et Mekra, S-Crew, nerveux f'ra vla les dégâts On va tout niquer, et j'le pense amplement! Faut pas nous banaliser, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Analisez, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Si ton malheur m'affecte, c'est par peur que ça m'arrive J'combat je maltraite, ceux qui condamnent le faciès Mes sons d'ailleurs achètent, les rappeurs que t'analyse Saveurs de cannabis, ces vapeurs me canalisent! Le diable est dans ton déhanché miss J'vais pas m'estomper j'vais dompter et plomber l'antéchrist, non c'est triste! Avant y'avait les meufs qui m'bâchaient et ces chiens qui m'ignoraient Maintenant j'me fais draguer par des bitchs aux seins siliconés! Unis dans l'biz mais on ne sait plus à qui se référencer Comme un uni-jambiste qui veut choisir sur quel pied danser Pas là pour plaisanter, ou bien quémander Ne propose pas un steak à un édenté! J'ai fréquenter les pires endroits J'ai vu des dérangés qui étranglaient des filles dans l'bois! Quand ta vie s'en va, t'es pris de l'angoisse Que ta miss conçoit, l'avenir sans toi! La vie d'rêve frangin, c'est 2zer Washington! Tu connais t'façons, L'Entourage bébé S-Crew booy! Framal est dans la place! Crapo', toujours monosourcilé! Blackbird bébé, Blackbirdddd, tu connais t'façons! Mekra, j'sais pas t'es où t'es toujours en retard Et Fennek, t'es en tournée, et Bsahtek, on va tout baiser ! S-Crew!1</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>J’avais un rêve</t>
+          <t>Si j’écris ce texte</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>La vrai fraternité, c'est déjà terminé On voit si t'as l'sang chaud une fois tes artères vidées C'est la guerre contre ces réfractaires givrés J'les met à terre s'ils déblatèrent sur mes affaires privées C'est la merde! Non j'veux pas m'faire des idées Détailler c'est risqué mais j'ai pas l'air d'hésiter Mais là frère c'que je vis c'est la célébrité J'lai mérité pour ça pas d'sérénité J'baise ta cacophonie j'vis ma vie Et j'te rends dingue comme une pathologie psychiatrique Putain y'as trop d'folies! Mais face aux phobies j'y arrive Tu cherches la merde, c'est que c'est la sodomie qui t'attire! Mon clan t'rentre dedans, sans prendre de gants C'est sanglant nan nan franchement Il est grand temps que j'me venge! Nekfeu, Framal et Mekra, S-Crew, nerveux f'ra vla les dégâts On va tout niquer, et j'le pense amplement! Faut pas nous banaliser, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Analisez, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Si ton malheur m'affecte, c'est par peur que ça m'arrive J'combat je maltraite, ceux qui condamnent le faciès Mes sons d'ailleurs achètent, les rappeurs que t'analyse Saveurs de cannabis, ces vapeurs me canalisent! Le diable est dans ton déhanché miss J'vais pas m'estomper j'vais dompter et plomber l'antéchrist, non c'est triste! Avant y'avait les meufs qui m'bâchaient et ces chiens qui m'ignoraient Maintenant j'me fais draguer par des bitchs aux seins siliconés! Unis dans l'biz mais on ne sait plus à qui se référencer Comme un uni-jambiste qui veut choisir sur quel pied danser Pas là pour plaisanter, ou bien quémander Ne propose pas un steak à un édenté! J'ai fréquenter les pires endroits J'ai vu des dérangés qui étranglaient des filles dans l'bois! Quand ta vie s'en va, t'es pris de l'angoisse Que ta miss conçoit, l'avenir sans toi! La vie d'rêve frangin, c'est 2zer Washington! Tu connais t'façons, L'Entourage bébé S-Crew booy! Framal est dans la place! Crapo', toujours monosourcilé! Blackbird bébé, Blackbirdddd, tu connais t'façons! Mekra, j'sais pas t'es où t'es toujours en retard Et Fennek, t'es en tournée, et Bsahtek, on va tout baiser ! S-Crew!1</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Si j’écris ce texte</t>
+          <t>La roue tourne trop vite</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Hé, c'est toi Neslet ? Hé franchement, j'kiffe c'que tu fais J'adore ton travail tout ça Ça fait penser à Matthieu Kassovitz, Kourtrajmé Tout ça, c'est la même chose franchement Hé tu connais pas 2zer ? Tu connais pas 2zer ? Hé tu connais pas 2zer ? Tu connais pas 2zer ? C'est quoi les bails ? C'est quoi les bails ? OK, 2-Zer Toi même tu sais comment ça aif', mon pote OK, dans ma vie, pff... J'en ai fait des erreurs Plein, plein, plein... OK Mais ma plus grosse erreur C'est de n'pas suivre l'exemple que mes parents m'montrent Puis j'ai compris qu'à part eux pour m'soutenir, y'avait pas grand monde J'vis dans le passé, j'm'en bats les couilles de la mode contemporaine Si mon ex-meuf refait sa vie, j'serai jamais content pour elle Ma vie c'est un croquis mal dessiné, j'en ai marre du ciné J'dois suivre ma destinée et combler ma dulcinée J'suis comme mon frère, on est dans l'vent, on a l'cerveau climatisé Et quand ça gueule j'suis dans l'espace, j'entends pas les cris d'ma fusée Moi, j'suis du-per depuis qu'la maladie a attrapé Maman C'est là qu'le destin m'a mis à terre et m'a frappé malement J'verse une larme, là, quand j'prie, moi j'suis trop incompris Pourtant j'parle français, c'est pas comme si je rappais l'allemand J'veux finir en terre promise mais ces bâtards me laissent trimer J'voudrais dire Je t'aime trop, miss mais j'ai du mal à l'exprimer Le bonheur ça dure deux secondes dans n'importe quelle situation J'pense qu'on devrait m'écouter, ouais, t'es un bon si tu as l'son X2 La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents Les gens, ça va, ça vient Tous les jours tu fais de bonnes ou de mauvaises rencontres Choisis bien ceux qui tentourent Observe bien, écoute bien c'quils disent Ne reste jamais dans un endroit où tu tsens mal à laise Jamais, non ! Les gens savent mentir donc apprends à mentir aussi Tout est éphémère Tout, tout, tout, tout... Même lamour et lamitié, frère... Malheureusement... Écoute ça, écoute ça... Donc si t'as pas les boules, dégage avant que mes gars t'les mettent Moi, j'bicrave, c'est bien ! Nan, en fait, je gratte les miettes Mon flow est alléchant, crois-en tes papilles gustatives Faut que j'sois actif, pour l'instant j'connais pas d'vie plus statique Moi, sans renoncer j'arpente les rues d'la capitale J'dois, remonter la pente c'qui est dans mon cas vital J'vois ma vie de l'extérieur, j'suis impuissant comme un soixantenaire Faut qu'j'sois sans colère face à ceux qui s'barrent quand ça sent l'tonnerre Si j'avais pu, j't'aurais dit l'mot Je t'aime et tous ses synonymes Mais tu t'fous de ma gueule, on apprend pas l'langage des signes aux mimes J'ai recollé les morceaux donc les pots ne devraient plus s'casser Nan, j'me vois pas aux puces taffer mais d'ma vie j'en ai plus qu'assez Putain, avec le temps les problèmes auraient dû s'tasser J'veux p'tit dèj' croissant plus café et l'soir grailler des crustacés 2-Zer Washington... C'est comme ça que les chacals m'appellent J'kiffe quand l'Entourage m'encourage, c'est c'qui fait que j'garde la pêche X2 La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents Hahahaha, 2-Zer ! Les gens, ça va, ça vient Tu connais t'façon, pas besoin d't'expliquer OK La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents8</t>
         </is>
       </c>
     </row>
@@ -832,12 +832,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>La roue tourne trop vite</t>
+          <t>Déçus par la vie</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Hé, c'est toi Neslet ? Hé franchement, j'kiffe c'que tu fais J'adore ton travail tout ça Ça fait penser à Matthieu Kassovitz, Kourtrajmé Tout ça, c'est la même chose franchement Hé tu connais pas 2zer ? Tu connais pas 2zer ? Hé tu connais pas 2zer ? Tu connais pas 2zer ? C'est quoi les bails ? C'est quoi les bails ? OK, 2-Zer Toi même tu sais comment ça aif', mon pote OK, dans ma vie, pff... J'en ai fait des erreurs Plein, plein, plein... OK Mais ma plus grosse erreur C'est de n'pas suivre l'exemple que mes parents m'montrent Puis j'ai compris qu'à part eux pour m'soutenir, y'avait pas grand monde J'vis dans le passé, j'm'en bats les couilles de la mode contemporaine Si mon ex-meuf refait sa vie, j'serai jamais content pour elle Ma vie c'est un croquis mal dessiné, j'en ai marre du ciné J'dois suivre ma destinée et combler ma dulcinée J'suis comme mon frère, on est dans l'vent, on a l'cerveau climatisé Et quand ça gueule j'suis dans l'espace, j'entends pas les cris d'ma fusée Moi, j'suis du-per depuis qu'la maladie a attrapé Maman C'est là qu'le destin m'a mis à terre et m'a frappé malement J'verse une larme, là, quand j'prie, moi j'suis trop incompris Pourtant j'parle français, c'est pas comme si je rappais l'allemand J'veux finir en terre promise mais ces bâtards me laissent trimer J'voudrais dire Je t'aime trop, miss mais j'ai du mal à l'exprimer Le bonheur ça dure deux secondes dans n'importe quelle situation J'pense qu'on devrait m'écouter, ouais, t'es un bon si tu as l'son X2 La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents Les gens, ça va, ça vient Tous les jours tu fais de bonnes ou de mauvaises rencontres Choisis bien ceux qui tentourent Observe bien, écoute bien c'quils disent Ne reste jamais dans un endroit où tu tsens mal à laise Jamais, non ! Les gens savent mentir donc apprends à mentir aussi Tout est éphémère Tout, tout, tout, tout... Même lamour et lamitié, frère... Malheureusement... Écoute ça, écoute ça... Donc si t'as pas les boules, dégage avant que mes gars t'les mettent Moi, j'bicrave, c'est bien ! Nan, en fait, je gratte les miettes Mon flow est alléchant, crois-en tes papilles gustatives Faut que j'sois actif, pour l'instant j'connais pas d'vie plus statique Moi, sans renoncer j'arpente les rues d'la capitale J'dois, remonter la pente c'qui est dans mon cas vital J'vois ma vie de l'extérieur, j'suis impuissant comme un soixantenaire Faut qu'j'sois sans colère face à ceux qui s'barrent quand ça sent l'tonnerre Si j'avais pu, j't'aurais dit l'mot Je t'aime et tous ses synonymes Mais tu t'fous de ma gueule, on apprend pas l'langage des signes aux mimes J'ai recollé les morceaux donc les pots ne devraient plus s'casser Nan, j'me vois pas aux puces taffer mais d'ma vie j'en ai plus qu'assez Putain, avec le temps les problèmes auraient dû s'tasser J'veux p'tit dèj' croissant plus café et l'soir grailler des crustacés 2-Zer Washington... C'est comme ça que les chacals m'appellent J'kiffe quand l'Entourage m'encourage, c'est c'qui fait que j'garde la pêche X2 La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents Hahahaha, 2-Zer ! Les gens, ça va, ça vient Tu connais t'façon, pas besoin d't'expliquer OK La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents8</t>
+          <t>B-Boy, B-Girl, scarla, scarlette T'es toujours à l'écoute de la Mixtape 2Fingz Et la 75ème Sess' te remercie Si t'as un truc à fumer, roule cette merde maintenant Si t'as une 'teille dans l'frigo, t'as juste le temps d'aller la chercher Et si tu kiffes juste l'oxygène, mets-toi à l'aise et écoute le son C'est parti, S-Crew, 2Fingz Il est temps d'leur montrer d'quoi vous êtes capables Mario, balance l'instru Framal Tu peux entendre mes balles dans l'gun, pas l'temps de dire ouf J'suis comme un battement d'cur, ta tempe se dissout Attends le discours d'un savant, j'suis vite saoulé Par les vacances, moi, j'veux de l'argent puis des foufs Mon passe-temps est pour l'appart des parents J'nique la France et les cours, qu'on parle franc Appelle-moi l'hémorroïde quand j'viens bloquer ta sortie Assorti au, fucking décor flamboyant, ça déborde sur la langue Tu viens d'sucker ma grosse bite, la grosse bitch prend la porte J'baise les porcs, on les prend comme un tarif à bon prix T'as compris, écoute le bruit des Ducati Sous les plumards y'a plus d'cash, j'me bute la nuit Ouais, j'me couche tard, les coups d'schlass te fourguent, l'ami Que des coups d'rage, écoute ça, que de l'outrage Sors mon pouchka, on nous regarde, sur tout Paris 2Zer Washington Quand mes pensées s'assombrissent, y'a danger, ça s'complique La vie m'a mutilé mais j'suis cultivé, je n'rangerai pas mon bic Ma vendetta s'combine pendant qu'ces sales cons friment J'suis déçu de la vie comme Une nympho devant des caleçons vides Ma vie, c'est rapper ou taffer l'développé-couché J'suis l'buf qui vient désosser et dévorer l'boucher J'ai les oreilles bouchées car le Rap met la pression On parlera d'mes agressions quand j'aurais dégommé Clooney Et détrôné tous mes adversaires J'suis un sale pervers car tes gars se laissent faire Quand j'leur fais des attouchements textuels J'rappe doucement car souvent ma Douce France est cruelle Mekra J'ai les pensées d'un polygame, j'aime trop les femmes, ma gueule J'suis pas comique mais trop bizarre, j'ai promis, j'cane la feuille C'est Mekra, j'aime pas l'État, fais gaffe, j'suis pas légal, pédale Je gratte des phases où le Sheitan m'accueille, c'est sale Tu veux lire dans mes pensées, fais bellek, c'est un film d'horreur Des trucs de psychopathes, ça passe du rire aux larmes Ça vire au drame quand j'me dis que les vigos meurent Tu trouve que j'suis fou, normal, je le suis Tu boudes là, petite zouz ? Goûte le bre-chi Ouais, j'ai des pensées perverses, j'ai dépensé De l'espèce pour des 'teilles pour que j'essaye De songer à des pensées pépères, faut m'laisser, les mecs Dans mes dièses, j'suis débranché, les frères KLM Dégomme des rangées d', des tonnes de pensées obscures Animent mon veau-cer mais je n'ai que faire Elle passe ap' le duo au stud' Des sons, d'la sape, ça bosse dur Sans borne, j'leur zappe leur posture Qui che-lâ ses shabs après une sale imposture Des post-it partout dans la breuch, un crachat dans une teuch Une overdose de geushs et ta clique de porcs à la broche Voilà c'que je vois quand Chivas est à l'approche Tétanisé sur la brèche, j'accélère et passe aux proches Un big up, ouais ! C'est qu'ils veulent çà A 19 time, j'serai peut-être toujours qué-cho par les loches Mais bref, j'me détends, j'rallume la téloche Les flammes du mal me lèchent J'peux t'dire qu'elles tarissent pas d'éloges Doum's Ça sent la merde, toi-même t'as senti Que mon esprit n'est pas tranquille Tard en ville, j'pars en vrille, ouais, presbyte, j'te garantis Que si tu t'approches trop, tu vas pas en revenir T'as capté ce stème-sy ? J'suis pas d'humeur à blaguer J'peux te smasher, attardé, si tu me respectes pas assez Avec ma horde de basanés, on va bien te fracasser MC, ramassez les mixtures sur le canapé, je m'immisce Merde, frère... J'ai rattrapé ces bitchs Qui m'parlaient d'un plan à 3, j'crois qu'ça se passe dans les bois Mon côté obscur a pris l'dessus, je t'assure, j'voulais ap' J'suis tombé dans les arcades de la folie, à l'agonie J'fais des arnaques à la Yonea4</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Déçus par la vie</t>
+          <t>Maintenant</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -866,12 +866,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Maintenant</t>
+          <t>Le vicieux</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>B-Boy, B-Girl, scarla, scarlette T'es toujours à l'écoute de la Mixtape 2Fingz Et la 75ème Sess' te remercie Si t'as un truc à fumer, roule cette merde maintenant Si t'as une 'teille dans l'frigo, t'as juste le temps d'aller la chercher Et si tu kiffes juste l'oxygène, mets-toi à l'aise et écoute le son C'est parti, S-Crew, 2Fingz Il est temps d'leur montrer d'quoi vous êtes capables Mario, balance l'instru Framal Tu peux entendre mes balles dans l'gun, pas l'temps de dire ouf J'suis comme un battement d'cur, ta tempe se dissout Attends le discours d'un savant, j'suis vite saoulé Par les vacances, moi, j'veux de l'argent puis des foufs Mon passe-temps est pour l'appart des parents J'nique la France et les cours, qu'on parle franc Appelle-moi l'hémorroïde quand j'viens bloquer ta sortie Assorti au, fucking décor flamboyant, ça déborde sur la langue Tu viens d'sucker ma grosse bite, la grosse bitch prend la porte J'baise les porcs, on les prend comme un tarif à bon prix T'as compris, écoute le bruit des Ducati Sous les plumards y'a plus d'cash, j'me bute la nuit Ouais, j'me couche tard, les coups d'schlass te fourguent, l'ami Que des coups d'rage, écoute ça, que de l'outrage Sors mon pouchka, on nous regarde, sur tout Paris 2Zer Washington Quand mes pensées s'assombrissent, y'a danger, ça s'complique La vie m'a mutilé mais j'suis cultivé, je n'rangerai pas mon bic Ma vendetta s'combine pendant qu'ces sales cons friment J'suis déçu de la vie comme Une nympho devant des caleçons vides Ma vie, c'est rapper ou taffer l'développé-couché J'suis l'buf qui vient désosser et dévorer l'boucher J'ai les oreilles bouchées car le Rap met la pression On parlera d'mes agressions quand j'aurais dégommé Clooney Et détrôné tous mes adversaires J'suis un sale pervers car tes gars se laissent faire Quand j'leur fais des attouchements textuels J'rappe doucement car souvent ma Douce France est cruelle Mekra J'ai les pensées d'un polygame, j'aime trop les femmes, ma gueule J'suis pas comique mais trop bizarre, j'ai promis, j'cane la feuille C'est Mekra, j'aime pas l'État, fais gaffe, j'suis pas légal, pédale Je gratte des phases où le Sheitan m'accueille, c'est sale Tu veux lire dans mes pensées, fais bellek, c'est un film d'horreur Des trucs de psychopathes, ça passe du rire aux larmes Ça vire au drame quand j'me dis que les vigos meurent Tu trouve que j'suis fou, normal, je le suis Tu boudes là, petite zouz ? Goûte le bre-chi Ouais, j'ai des pensées perverses, j'ai dépensé De l'espèce pour des 'teilles pour que j'essaye De songer à des pensées pépères, faut m'laisser, les mecs Dans mes dièses, j'suis débranché, les frères KLM Dégomme des rangées d', des tonnes de pensées obscures Animent mon veau-cer mais je n'ai que faire Elle passe ap' le duo au stud' Des sons, d'la sape, ça bosse dur Sans borne, j'leur zappe leur posture Qui che-lâ ses shabs après une sale imposture Des post-it partout dans la breuch, un crachat dans une teuch Une overdose de geushs et ta clique de porcs à la broche Voilà c'que je vois quand Chivas est à l'approche Tétanisé sur la brèche, j'accélère et passe aux proches Un big up, ouais ! C'est qu'ils veulent çà A 19 time, j'serai peut-être toujours qué-cho par les loches Mais bref, j'me détends, j'rallume la téloche Les flammes du mal me lèchent J'peux t'dire qu'elles tarissent pas d'éloges Doum's Ça sent la merde, toi-même t'as senti Que mon esprit n'est pas tranquille Tard en ville, j'pars en vrille, ouais, presbyte, j'te garantis Que si tu t'approches trop, tu vas pas en revenir T'as capté ce stème-sy ? J'suis pas d'humeur à blaguer J'peux te smasher, attardé, si tu me respectes pas assez Avec ma horde de basanés, on va bien te fracasser MC, ramassez les mixtures sur le canapé, je m'immisce Merde, frère... J'ai rattrapé ces bitchs Qui m'parlaient d'un plan à 3, j'crois qu'ça se passe dans les bois Mon côté obscur a pris l'dessus, je t'assure, j'voulais ap' J'suis tombé dans les arcades de la folie, à l'agonie J'fais des arnaques à la Yonea4</t>
+          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
         </is>
       </c>
     </row>
@@ -883,12 +883,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Le vicieux</t>
+          <t>L’entourage</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
+          <t>L'Entourage, on vient pour percer ou tout bouleverser, couz Faut qu'tu cours vers ces bougs qui veulent tous faire des sous T'as déconné, t'aurais voulu nous détrôner Mais dans ce pe-Ra, t'es paumé, bouge, mec, t'es fou J'ai pleins d'défauts, je veux bien mais j'sors des flows de gue-din J'vais pas m'ver-sau mais ter-sau et puis per-stop le venin Mec, sur le tempo, j'aime trop faire ser-po de vrais pros Même chose, j'prends le métro, pas d'resto Merco mais faut que j'détrône les faux Ouais, fils, j'ouvre les cuisses des bitches allemandes J'fais des french kisses aux métisses, j'maîtrise la langue J'fais des tris sélectifs chez les miss et je m'esquive Elles m'épuisent mais miskine, j'les méprise salement Lents, on prend notre temps, tous les gens du clan Rage on t'rentre dedans avec des flows de gue-din On a de la bonne de meda, trop de jeunes pour tes vieux gars Ceux qui fument de la gue-dro quitte à quer-cho, qui font des ffs-gra L'envie de gagner, toubabs et basanés Rage mis dans le panier, épaule nos hommes de mains On a de la bonne de meda, trop de jeunes pour tes vieux gars Ceux qui fument de la gue-dro quitte à qué-cho, qui font des ffs-gra Yo, c'est L'Entourage, Burbigo pour mon poto Guizmo J'étale trop de style flow, c'est la faute au shit, gros J'élabore des discographies pour mes gars qui poussent Le paki toujours tapis dans des trafics locaux d'ssiste-gro J'rapplique au cromi-phone la fougue d'un smicard qui roule La ville tard sous jogo d'popo, je m'autosponsorise, gros Personne pourra dire qu'il m'a mis à manger dans l'assiette Trop à penser dans la tête, quelque chose à changer dans l'faciès Bronzé dans ma chair, j'ai songé à ma perte et plongé dans ma quête J'arrêterai quand j'serai rangé sous la terre Si j'me plante, j'ai pas de plan B donc j'ai foncé pour la tess Tu m'as croisé peut-être dans l'quartier, j'suis pas passé pour la fête Allez, ramenez toute la presse, on va rafler toute la fraîche Élimine les débilités qu'éditent leurs foutus labels Mais fuck, les trous duc' s'ramènent, j'les laisse tous bouches cousues à terre On va dealer d'la qualité, seul but d'nos foutues carrière Lents, on prend notre temps, tous les gens du clan Rage on t'rentre dedans avec des flows de gue-din On a de la bonne de meda, trop de jeunes pour tes vieux gars Ceux qui fument de la gue-dro quitte à quer-cho, qui font des ffs-gra L'envie de gagner, toubabs et basanés Rage mis dans le panier, épaule nos hommes de mains On a de la bonne de meda, trop de jeune pour tes vieux gars Ceux qui fument de la gue-dro quitte à qué-cho, qui font des ffs-gra Ça péra pour vivre, malgré ça, j'suis lassé d'ma routine J'vais braquer la boutique, ne passez pas de coups de fil Ça s'pe-ta sous tise, ça bédave Amnézia ou shit Capuché les yeux rouges plissés par des tas d'soucis Pisté par les schtars, j'cours vite sinon c'est hors de la maison En plus, lors de l'agression, j'lui ai mis 4 coups d'crique Mais rien d'grave, c'est juste que des fois il faut jouer des coudes Et puisque c'est ça, on va goomer des bouches Et vu qu'la roue tourne, on finira par s'faire goomer aussi C'est fou et nocif de jouer nos vies Shootés au spliff, on va goûter au pire Car on est fous et hostiles au lieu d'rester doux et dociles ×5 Lents, on prend notre temps, tous les gens du clan Rage on t'rentre dedans avec des flows de gue-din On a de la bonne de meda, trop de jeunes pour tes vieux gars Ceux qui fument de la gue-dro quitte à quer-cho, qui font des ffs-gra L'envie de gagner, toubabs et basanés Rage mis dans le panier, épaule nos hommes de mains On a de la bonne de meda, trop de jeune pour tes vieux gars Ceux qui fument de la gue-dro quitte à qué-cho, qui font des ffs-gra4</t>
         </is>
       </c>
     </row>
@@ -900,12 +900,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>L’entourage</t>
+          <t>Incompris</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>L'Entourage, on vient pour percer ou tout bouleverser, couz Faut qu'tu cours vers ces bougs qui veulent tous faire des sous T'as déconné, t'aurais voulu nous détrôner Mais dans ce pe-Ra, t'es paumé, bouge, mec, t'es fou J'ai pleins d'défauts, je veux bien mais j'sors des flows de gue-din J'vais pas m'ver-sau mais ter-sau et puis per-stop le venin Mec, sur le tempo, j'aime trop faire ser-po de vrais pros Même chose, j'prends le métro, pas d'resto Merco mais faut que j'détrône les faux Ouais, fils, j'ouvre les cuisses des bitches allemandes J'fais des french kisses aux métisses, j'maîtrise la langue J'fais des tris sélectifs chez les miss et je m'esquive Elles m'épuisent mais miskine, j'les méprise salement Lents, on prend notre temps, tous les gens du clan Rage on t'rentre dedans avec des flows de gue-din On a de la bonne de meda, trop de jeunes pour tes vieux gars Ceux qui fument de la gue-dro quitte à quer-cho, qui font des ffs-gra L'envie de gagner, toubabs et basanés Rage mis dans le panier, épaule nos hommes de mains On a de la bonne de meda, trop de jeunes pour tes vieux gars Ceux qui fument de la gue-dro quitte à qué-cho, qui font des ffs-gra Yo, c'est L'Entourage, Burbigo pour mon poto Guizmo J'étale trop de style flow, c'est la faute au shit, gros J'élabore des discographies pour mes gars qui poussent Le paki toujours tapis dans des trafics locaux d'ssiste-gro J'rapplique au cromi-phone la fougue d'un smicard qui roule La ville tard sous jogo d'popo, je m'autosponsorise, gros Personne pourra dire qu'il m'a mis à manger dans l'assiette Trop à penser dans la tête, quelque chose à changer dans l'faciès Bronzé dans ma chair, j'ai songé à ma perte et plongé dans ma quête J'arrêterai quand j'serai rangé sous la terre Si j'me plante, j'ai pas de plan B donc j'ai foncé pour la tess Tu m'as croisé peut-être dans l'quartier, j'suis pas passé pour la fête Allez, ramenez toute la presse, on va rafler toute la fraîche Élimine les débilités qu'éditent leurs foutus labels Mais fuck, les trous duc' s'ramènent, j'les laisse tous bouches cousues à terre On va dealer d'la qualité, seul but d'nos foutues carrière Lents, on prend notre temps, tous les gens du clan Rage on t'rentre dedans avec des flows de gue-din On a de la bonne de meda, trop de jeunes pour tes vieux gars Ceux qui fument de la gue-dro quitte à quer-cho, qui font des ffs-gra L'envie de gagner, toubabs et basanés Rage mis dans le panier, épaule nos hommes de mains On a de la bonne de meda, trop de jeune pour tes vieux gars Ceux qui fument de la gue-dro quitte à qué-cho, qui font des ffs-gra Ça péra pour vivre, malgré ça, j'suis lassé d'ma routine J'vais braquer la boutique, ne passez pas de coups de fil Ça s'pe-ta sous tise, ça bédave Amnézia ou shit Capuché les yeux rouges plissés par des tas d'soucis Pisté par les schtars, j'cours vite sinon c'est hors de la maison En plus, lors de l'agression, j'lui ai mis 4 coups d'crique Mais rien d'grave, c'est juste que des fois il faut jouer des coudes Et puisque c'est ça, on va goomer des bouches Et vu qu'la roue tourne, on finira par s'faire goomer aussi C'est fou et nocif de jouer nos vies Shootés au spliff, on va goûter au pire Car on est fous et hostiles au lieu d'rester doux et dociles ×5 Lents, on prend notre temps, tous les gens du clan Rage on t'rentre dedans avec des flows de gue-din On a de la bonne de meda, trop de jeunes pour tes vieux gars Ceux qui fument de la gue-dro quitte à quer-cho, qui font des ffs-gra L'envie de gagner, toubabs et basanés Rage mis dans le panier, épaule nos hommes de mains On a de la bonne de meda, trop de jeune pour tes vieux gars Ceux qui fument de la gue-dro quitte à qué-cho, qui font des ffs-gra4</t>
+          <t>Tu suces, tu sers à rien T'es microscopique tel un acarien Je brasse et je brasse et je brasse, mais toi tu n'es rien qu'un arlequin J'débarque à l'improviste comme Billy Cocaïne J'ai pas reçu d'invit donc j'me codéine J'ai mélangé prométhazine sprite et codé pour en faire un excellent lean J'débite les rimes, oui je n'suis pas clean, j'immite les humanoïdes Dix bites dans la teush à l'ennemi, limonade à liqueur d'opioïde Devant la TV je n'matte qu'On n'Est Pas Couché, enfumé sous gnax en m'servant un double rre-vé Trop bourré sur l'pc j'regarde la MMA et j'en profite pour taper d'la bonne C Mauvais délires et débile sous LSD je vois et je vais encaisser les low kicks J'entends dans ma tête des rires et des rires et des rires, il me semble que j'suis sick Dans ma tête ils sont six, and three d'entre eux sont accros aux sticks Ces trois là très souvent me réclament de rouler un spliff comme si la weed était gratuite, comme si la weed était gratuite Le regard dans le vide j'ai le cerveau de freezer, légèrement schizoïde il y a sûrement une erreur Une erreur ça prend deux R comme terreur et 2zer Washington Mon corps et mon esprit sont dissociés je pèse deux tones J'suis complètement vidé, l'acide dans les recepteurs deux goutes de diéthylamide bad trip de 3h Faudrait p't'etre que j'fasse un truc car la redescente est assez difficile Si mes parents me voyaient dans cet état c'est sur qu'ils m'auraient déjà kill Ma mère m'a souvent dit les drogues c'est mal et ça peut même être létal Elle me disait aussi que ça nous rendait bête et pas normal, comme le racisme juif et anti-black Sévissant depuis des siècles celui-ci n'est pas légal, cent fois plus dangereux que les drogues et la galle Si présent pourtant, certains méritent des claques plutôt qu'un mac 22 octobre 2k16 j'assistais excité à mon premier pèlerinage musicale L'Guizi foncedé débitait des rimes et des rimes sous gros shit, oui j'étais à la Cigale Désormais j'attends qu'le gremlins fassent les backs avant le bac Le 16 décembre à la fnac pour pecho l'album-black On écrit, on tté-fri On roule des spliffs et je fais l'trie Boulette ? Pas boulette, sur le sol j'retrouve des têtes J'tabasse tellement les wacks qu'on m'appelle souvent l'nouveau Nek' Je fume, je rime, tu déprimes, j'bois du lean avec ma team Ces rappeurs sont has been, ma teen a le même boule que Kim Je trend set et oui j'me la pète, oui j'pète mon teh d'OG Kush J'ai kiffé sa bonne beuh-er, j'en rachète 500 meujs Tu flippes quand je dégaine, m'esquive quand je kick t'en sortira pas indemne Tellement d'hasch dans les veines, tes textes sentent la merde même à 100 kilomètres d'la seine ou dix, vernon zooo Si j'te croise j'te ferais mal à la manière de Framal J'te troue de trente balles, tu fall et devient tout pâle Donc cale toi ça dans l'crâne tu canes et je plane tel l'Empreur du Sale J'suis preneur de soufflette profesional et oui je fly comme Phall à la Don Dada Imperturbable même quand le cell sonne J'lâche un dab quand j'applique le cellophane Incompris j'me sens comme Cell, sans phone J'me présente mon blaze c'est Kagame-san J'comprends qu'tu sois fan mais dorénavant appelle moi Kami-sama Ces faux mc sont mauvais, flagrant comme l'obésité morbide à la big mama Sa mère ça suce, z'ont pas d'inspi donc sans cesse parle de tess d'ecsta et de cess C'est pas sensé même défoncé leurs faussent lyrics sont nasent ils croient qu'ils pèsent Si ça te plait pas t'as qu'à diskliker, carte visa dans la main j'fais taffer l'caissier T'aimes te ficha au lycée t'es pas ma tasse d'café j'préfère les filles discrète, mignonne, brunette pas trop maquillé Tu kiffes les beurettes pas belles kiffant faire la fête, la fête se fera bien dans leur chatte mouillées Au bout de deux trois verres ces salopes sont toutes sous l'emprise du Jack D Je crois avoir définit la définition du mot taspé, une keh sous mojito ou plutôt Mojito sur keh Ce fils de pute c'est ma beurette de luxe, suce j'arrive Yass comme Luxe pendant qu't'écoutes des bails claqués Je trouve ce son bien trop étrange, c'est donc la fin de ce mauvais mélange</t>
         </is>
       </c>
     </row>
@@ -917,12 +917,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Incompris</t>
+          <t>Toujours là</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tu suces, tu sers à rien T'es microscopique tel un acarien Je brasse et je brasse et je brasse, mais toi tu n'es rien qu'un arlequin J'débarque à l'improviste comme Billy Cocaïne J'ai pas reçu d'invit donc j'me codéine J'ai mélangé prométhazine sprite et codé pour en faire un excellent lean J'débite les rimes, oui je n'suis pas clean, j'immite les humanoïdes Dix bites dans la teush à l'ennemi, limonade à liqueur d'opioïde Devant la TV je n'matte qu'On n'Est Pas Couché, enfumé sous gnax en m'servant un double rre-vé Trop bourré sur l'pc j'regarde la MMA et j'en profite pour taper d'la bonne C Mauvais délires et débile sous LSD je vois et je vais encaisser les low kicks J'entends dans ma tête des rires et des rires et des rires, il me semble que j'suis sick Dans ma tête ils sont six, and three d'entre eux sont accros aux sticks Ces trois là très souvent me réclament de rouler un spliff comme si la weed était gratuite, comme si la weed était gratuite Le regard dans le vide j'ai le cerveau de freezer, légèrement schizoïde il y a sûrement une erreur Une erreur ça prend deux R comme terreur et 2zer Washington Mon corps et mon esprit sont dissociés je pèse deux tones J'suis complètement vidé, l'acide dans les recepteurs deux goutes de diéthylamide bad trip de 3h Faudrait p't'etre que j'fasse un truc car la redescente est assez difficile Si mes parents me voyaient dans cet état c'est sur qu'ils m'auraient déjà kill Ma mère m'a souvent dit les drogues c'est mal et ça peut même être létal Elle me disait aussi que ça nous rendait bête et pas normal, comme le racisme juif et anti-black Sévissant depuis des siècles celui-ci n'est pas légal, cent fois plus dangereux que les drogues et la galle Si présent pourtant, certains méritent des claques plutôt qu'un mac 22 octobre 2k16 j'assistais excité à mon premier pèlerinage musicale L'Guizi foncedé débitait des rimes et des rimes sous gros shit, oui j'étais à la Cigale Désormais j'attends qu'le gremlins fassent les backs avant le bac Le 16 décembre à la fnac pour pecho l'album-black On écrit, on tté-fri On roule des spliffs et je fais l'trie Boulette ? Pas boulette, sur le sol j'retrouve des têtes J'tabasse tellement les wacks qu'on m'appelle souvent l'nouveau Nek' Je fume, je rime, tu déprimes, j'bois du lean avec ma team Ces rappeurs sont has been, ma teen a le même boule que Kim Je trend set et oui j'me la pète, oui j'pète mon teh d'OG Kush J'ai kiffé sa bonne beuh-er, j'en rachète 500 meujs Tu flippes quand je dégaine, m'esquive quand je kick t'en sortira pas indemne Tellement d'hasch dans les veines, tes textes sentent la merde même à 100 kilomètres d'la seine ou dix, vernon zooo Si j'te croise j'te ferais mal à la manière de Framal J'te troue de trente balles, tu fall et devient tout pâle Donc cale toi ça dans l'crâne tu canes et je plane tel l'Empreur du Sale J'suis preneur de soufflette profesional et oui je fly comme Phall à la Don Dada Imperturbable même quand le cell sonne J'lâche un dab quand j'applique le cellophane Incompris j'me sens comme Cell, sans phone J'me présente mon blaze c'est Kagame-san J'comprends qu'tu sois fan mais dorénavant appelle moi Kami-sama Ces faux mc sont mauvais, flagrant comme l'obésité morbide à la big mama Sa mère ça suce, z'ont pas d'inspi donc sans cesse parle de tess d'ecsta et de cess C'est pas sensé même défoncé leurs faussent lyrics sont nasent ils croient qu'ils pèsent Si ça te plait pas t'as qu'à diskliker, carte visa dans la main j'fais taffer l'caissier T'aimes te ficha au lycée t'es pas ma tasse d'café j'préfère les filles discrète, mignonne, brunette pas trop maquillé Tu kiffes les beurettes pas belles kiffant faire la fête, la fête se fera bien dans leur chatte mouillées Au bout de deux trois verres ces salopes sont toutes sous l'emprise du Jack D Je crois avoir définit la définition du mot taspé, une keh sous mojito ou plutôt Mojito sur keh Ce fils de pute c'est ma beurette de luxe, suce j'arrive Yass comme Luxe pendant qu't'écoutes des bails claqués Je trouve ce son bien trop étrange, c'est donc la fin de ce mauvais mélange</t>
+          <t>2zer Washington Parlez-vous cefran? Hein, hein, parlez-vous cefran? DJ noise -crew boyyyy, tu connais les bails Personne ne peut stopper ma force Mais j'vous cache ma rage Comme tous mes côtés atroces et où j'passe à l'acte Mais tout ça, ça marque On n'résout pas sa life En jouant l'toréador Les coups partent, bâtard Rappelle-moi tous tes coups ratés Quand l'état voulait nous fater La vendetta de mes fous à lier Double ge-ra à défourailler J'ai coulé d'la marchandise Depuis j'me suis attendri Pour pas que le maton m'dise Tenez-vous droit, venez vous laver J'ai la force H24 sous adrénaline J'ai toujours la gouache sans mettre de poudre à mes narines J'veux soulager ma vie sans outrager la rime J'ai la force pour taffer la nuit Quand vous allez dormir On est d'accord Framal Apportez l'fric, là j'vais saboter l'biz Trop paro j'débite Que des sales projets, approchez Là j'promets, droite, gauche, et Nekfeu arme soviétique ! En guise de rime, en titre de chemise J'enfile mon jean rempli d'centimes Et gratte ce rap trop technique La prose est clean, j'tape trop de spliff Là je t'assomme ? ? Nekfeu que des balles trop précises ! J'ai le sabre dans la gorge Mec, prends garde, j't'encastre Il m'faut du cash dans la pocket J'veux des thunes d'apache Déçu d'la life, toi tu cé-su J't'exécute à l'épluche-patate Mékra Seine zoo dans les bacs Y'a pas d'nana dans mon équipe que des ? On a la rage d'un Apache Toi t'as la bouche ouverte Faudra nachave, prendre un appart' Et ça à toute vitesse J'rappe sous ivresse, quoi tu m'crois pas? ? Hey, nique les strass et les paillettes Moi j'suis ? j'ai les manières D'un soc' ? Ecoute mon clan, on arrive On va couler l'bateau des traîtres Tu veux prendre ton tarif Ca va t'coûter la peau des fesses, ma miss On est frais, bah oui Ca c'est pour mes frères d'Afrique On a tous été trahis Par toutes ces ? hemi Et tu m'verras, toujours partant pour les re-frè Nekfeu Pas l'temps pour les regrets, hein J'suis posé sans contrainte, à cent contre un J'attends pas l'embonpoint J'arrête de rapper mes textes dans mon coin Avec ma tête de fennec j'suis scred' Donc quand je squatte des quartiers chics J'écarte les cuisses des femelles du 16 On reste vrais grâce à nos actes On a nos façons d'voir le rap Pas d'casanova, tu faisais quoi à notre âge, mon gars? Arrête de rager, vu? Ici, c'est ris-Pa J'suis pas l'élu juste un p'tit gars muni de ses 10 doigts Et quoi qu'tu dises on s'est fait connaître sans radio Moi, j'suis un artiste pas comme tes collègues en major Il faut que le message s'exporte Pour qu'les petits frelons kiffent le son La vie, c'est pas que ? Je kick pour le freestyle Pire encore, fist Ma vie est un 2zer freestyle qui m'renforce ? Je kick pour le freestyle Pire encore, fist Ma vie est Mékra un freestyle qui m'renforce Hein, parlez-vous cefran? Seine zoo, allez-vous ser-dan? Check, check, l'entourage bébé</t>
         </is>
       </c>
     </row>
@@ -934,12 +934,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Toujours là</t>
+          <t>Personne</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2zer Washington Parlez-vous cefran? Hein, hein, parlez-vous cefran? DJ noise -crew boyyyy, tu connais les bails Personne ne peut stopper ma force Mais j'vous cache ma rage Comme tous mes côtés atroces et où j'passe à l'acte Mais tout ça, ça marque On n'résout pas sa life En jouant l'toréador Les coups partent, bâtard Rappelle-moi tous tes coups ratés Quand l'état voulait nous fater La vendetta de mes fous à lier Double ge-ra à défourailler J'ai coulé d'la marchandise Depuis j'me suis attendri Pour pas que le maton m'dise Tenez-vous droit, venez vous laver J'ai la force H24 sous adrénaline J'ai toujours la gouache sans mettre de poudre à mes narines J'veux soulager ma vie sans outrager la rime J'ai la force pour taffer la nuit Quand vous allez dormir On est d'accord Framal Apportez l'fric, là j'vais saboter l'biz Trop paro j'débite Que des sales projets, approchez Là j'promets, droite, gauche, et Nekfeu arme soviétique ! En guise de rime, en titre de chemise J'enfile mon jean rempli d'centimes Et gratte ce rap trop technique La prose est clean, j'tape trop de spliff Là je t'assomme ? ? Nekfeu que des balles trop précises ! J'ai le sabre dans la gorge Mec, prends garde, j't'encastre Il m'faut du cash dans la pocket J'veux des thunes d'apache Déçu d'la life, toi tu cé-su J't'exécute à l'épluche-patate Mékra Seine zoo dans les bacs Y'a pas d'nana dans mon équipe que des ? On a la rage d'un Apache Toi t'as la bouche ouverte Faudra nachave, prendre un appart' Et ça à toute vitesse J'rappe sous ivresse, quoi tu m'crois pas? ? Hey, nique les strass et les paillettes Moi j'suis ? j'ai les manières D'un soc' ? Ecoute mon clan, on arrive On va couler l'bateau des traîtres Tu veux prendre ton tarif Ca va t'coûter la peau des fesses, ma miss On est frais, bah oui Ca c'est pour mes frères d'Afrique On a tous été trahis Par toutes ces ? hemi Et tu m'verras, toujours partant pour les re-frè Nekfeu Pas l'temps pour les regrets, hein J'suis posé sans contrainte, à cent contre un J'attends pas l'embonpoint J'arrête de rapper mes textes dans mon coin Avec ma tête de fennec j'suis scred' Donc quand je squatte des quartiers chics J'écarte les cuisses des femelles du 16 On reste vrais grâce à nos actes On a nos façons d'voir le rap Pas d'casanova, tu faisais quoi à notre âge, mon gars? Arrête de rager, vu? Ici, c'est ris-Pa J'suis pas l'élu juste un p'tit gars muni de ses 10 doigts Et quoi qu'tu dises on s'est fait connaître sans radio Moi, j'suis un artiste pas comme tes collègues en major Il faut que le message s'exporte Pour qu'les petits frelons kiffent le son La vie, c'est pas que ? Je kick pour le freestyle Pire encore, fist Ma vie est un 2zer freestyle qui m'renforce ? Je kick pour le freestyle Pire encore, fist Ma vie est Mékra un freestyle qui m'renforce Hein, parlez-vous cefran? Seine zoo, allez-vous ser-dan? Check, check, l'entourage bébé</t>
+          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Personne</t>
+          <t>Tudo Bem</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
+          <t>2-zer, tu connais t'facon, hein Pour moi, tudo bem, pour l'instant, tout baigne BlackBird, S-Crew La vie m'a appris à ne jamais tourner le dos, y'a que le mur qui peut mater mes fesses Mais je laisse la bédave cramer tout mes neurones, ouais, ouais, j'préfère ça que d'me gratter les veines J'fais c'que j'sais faire le plus gratter des 16 qui te pètent le cul Ouais sans cesse on encaisse mais j'reste concentré, j'ai une tête et un sexe de mule J'ai souffert dans le calme, ça prouve que mon parcours est crédible Coup de pelle dans le crâne pour qu'ces jaloux soient ouvert d'esprit Si tu banalises c'que j'dis, on te malmène jusqu'à ramper, quand le cannabis fleurit, poto, ça freine la santé Véritable vécu, j'en garde les stigmates, de plus, j'apprécie les paysages et j'fume de l'herbe médicale On reste insaisissables et têtus, toujours en indé, minable Partage équitable des thunes comme dans Breaking Bad J'lèche des tétons d'minettes en toute modestie, là, j'y prends goût J'ai l'Expression Direkt depuis qu'mon esprit est parti en couille Jusque là, j't'aimais mais t'as blasphémé, j't'avais dit que personne ne pourrait m'arrêter Râgeux, je t'offre le droit de te moquer si tu m'passes le code de ta CB x2 Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Les leçons de la vie, on les apprend nous mêmes Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Bouteille de Jack grande ouverte Quand y'en a marre de la grisaille, on quitte Paris au calme On bouge à Rio voir mes Cariocas Là gros, c'est bon, j'me vois déjà sur les ges-pla d'Ipanema La peau zée-bron, non, fallait pas m'amener là-bas, j'y dierai pas C'est le chômage à Paname, moi, j'fais l'sauvage à la plage Tes potes passent à la barre quand j'suis à Copacabana Quand je serai sur Paris, j'dirai vrai aux femmes qui m'aiment trop Mon amour, ma vie c'est Mirelle Do Nascimento À Mexico, on ferra un magique voyage, oye chico ! A mí me gusta marijuana Hombre viva la vida ! Dónde estas las chicas ? Ma tequila à la main, fonce-dé, j'bédave mon cigare x2 Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Les leçons de la vie, on les apprend nous mêmes Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Bouteille de Jack grande ouverte10</t>
         </is>
       </c>
     </row>
@@ -968,12 +968,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tudo Bem</t>
+          <t>Mourir demain</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2-zer, tu connais t'facon, hein Pour moi, tudo bem, pour l'instant, tout baigne BlackBird, S-Crew La vie m'a appris à ne jamais tourner le dos, y'a que le mur qui peut mater mes fesses Mais je laisse la bédave cramer tout mes neurones, ouais, ouais, j'préfère ça que d'me gratter les veines J'fais c'que j'sais faire le plus gratter des 16 qui te pètent le cul Ouais sans cesse on encaisse mais j'reste concentré, j'ai une tête et un sexe de mule J'ai souffert dans le calme, ça prouve que mon parcours est crédible Coup de pelle dans le crâne pour qu'ces jaloux soient ouvert d'esprit Si tu banalises c'que j'dis, on te malmène jusqu'à ramper, quand le cannabis fleurit, poto, ça freine la santé Véritable vécu, j'en garde les stigmates, de plus, j'apprécie les paysages et j'fume de l'herbe médicale On reste insaisissables et têtus, toujours en indé, minable Partage équitable des thunes comme dans Breaking Bad J'lèche des tétons d'minettes en toute modestie, là, j'y prends goût J'ai l'Expression Direkt depuis qu'mon esprit est parti en couille Jusque là, j't'aimais mais t'as blasphémé, j't'avais dit que personne ne pourrait m'arrêter Râgeux, je t'offre le droit de te moquer si tu m'passes le code de ta CB x2 Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Les leçons de la vie, on les apprend nous mêmes Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Bouteille de Jack grande ouverte Quand y'en a marre de la grisaille, on quitte Paris au calme On bouge à Rio voir mes Cariocas Là gros, c'est bon, j'me vois déjà sur les ges-pla d'Ipanema La peau zée-bron, non, fallait pas m'amener là-bas, j'y dierai pas C'est le chômage à Paname, moi, j'fais l'sauvage à la plage Tes potes passent à la barre quand j'suis à Copacabana Quand je serai sur Paris, j'dirai vrai aux femmes qui m'aiment trop Mon amour, ma vie c'est Mirelle Do Nascimento À Mexico, on ferra un magique voyage, oye chico ! A mí me gusta marijuana Hombre viva la vida ! Dónde estas las chicas ? Ma tequila à la main, fonce-dé, j'bédave mon cigare x2 Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Les leçons de la vie, on les apprend nous mêmes Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Pour moi, tudo bem, pour l'instant, tout baigne Bouteille de Jack grande ouverte10</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -985,12 +985,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Mourir demain</t>
+          <t>Porte de Paris</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Yo, toi avec ton p'tit boule d'actrice, viens par ici tirer sur ma Big Buddah Cheese Laissons de côté les sujets qui nous attristent, sur ma baguette enchantée, j'ai besoin d'un bisou magique J'ai dit, yo, toi avec ton p'tit boule d'actrice, viens par ici tirer sur ma Big Buddah Cheese Laissons de côté les sujets qui nous attristent, sur ma baguette enchantée, j'ai besoin d'un bisou magique À chaque porte de Paris, j'ai une concubine, ça va d'la blonde stupide à la ronde pudique Des meufs compulsives qui veulent qu'on s'unisse, elles savent que moi et la rue, on a rompu vite J'connais une meuf coquine vers Porte Dauphine, Elle tape dans les drogues dures et boit de la codéine Quant à la cocaïne, elle croit que c'est comestible Une blondinette zombifiée pour qui j'ai pas trop d'estime À lopposée, j'connais une beurette à Porte de Clichy Elle a des formes, qu'est c'qu'elle est bonne mais peu importe le physique Avec elle, j'me tape des barres et on bédave des lattes, j'ai d'jà essayé mais pas moyen que j'lui écarte les pattes À Porte d'Auteuil, j'vais te présenter une portugaise, mordue de sexe, sans faire aucun effort, tu baises J'dois me faire discret, j'ai la dégaine d'un dealer de me-seu, elle habite une loge de gardienne d'un immeuble de vieux Tes tuteurs le savent, je suis un séducteur de femmes, tes lèvres fines toute douces m'excitent T'aurais dû l'prévoir, c'est plus fort que oi-m, fevant une belle fille, je sors toujours le même speech Yo, toi avec ton p'tit boule d'actrice, viens par ici tirer sur ma Big Buddah Cheese Laissons de côté les sujets qui nous attristent, sur ma baguette enchantée, j'ai besoin d'un bisou magique J'ai dit, hey, toi avec ton p'tit boule d'actrice, viens par ici tirer sur ma Big Buddah Cheese Laissons de côté les sujets qui nous attristent, sur ma baguette enchantée, j'ai besoin d'un bisou magique Porte de Pantin, y'a une meuf un peu garçon manqué Elle va peut-être tomber pour avoir ppé-fra son banquier Les gens saints d'esprits l'appellent sens interdit Quand tu la vois, fais demi-tour ou tu perds tes dents, j't'avertis J'prends l'périph direction Porte d'Italie, c'est l'heure du thé, j'vais capter une salope britannique Elle comprend pas quand j'rappe donc j'sors des pures folies Posé sur le divan, bon vivant comme Berlusconi Porte de la Muette, dans le duplex d'une brunette sexy Y'a de la buée sur mes lunettes quand la fumée s'expire C'est la plus belle, j'y tiens comme à la prunelle de mes yeux C'est un tunnel sans fin quand l'adultère se fait vieux Tes tuteurs le savent, je suis un séducteur de femmes, tes lèvres fines toute douces m'excitent T'aurais dû l'prévoir, c'est plus fort que oi-m, fevant une belle fille, je sors toujours le même speech 4</t>
         </is>
       </c>
     </row>
@@ -1002,12 +1002,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Porte de Paris</t>
+          <t>Nekfeu, S-Crew, S.Pri Noir… en freestyle dans Planète Rap</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Yo, toi avec ton p'tit boule d'actrice, viens par ici tirer sur ma Big Buddah Cheese Laissons de côté les sujets qui nous attristent, sur ma baguette enchantée, j'ai besoin d'un bisou magique J'ai dit, yo, toi avec ton p'tit boule d'actrice, viens par ici tirer sur ma Big Buddah Cheese Laissons de côté les sujets qui nous attristent, sur ma baguette enchantée, j'ai besoin d'un bisou magique À chaque porte de Paris, j'ai une concubine, ça va d'la blonde stupide à la ronde pudique Des meufs compulsives qui veulent qu'on s'unisse, elles savent que moi et la rue, on a rompu vite J'connais une meuf coquine vers Porte Dauphine, Elle tape dans les drogues dures et boit de la codéine Quant à la cocaïne, elle croit que c'est comestible Une blondinette zombifiée pour qui j'ai pas trop d'estime À lopposée, j'connais une beurette à Porte de Clichy Elle a des formes, qu'est c'qu'elle est bonne mais peu importe le physique Avec elle, j'me tape des barres et on bédave des lattes, j'ai d'jà essayé mais pas moyen que j'lui écarte les pattes À Porte d'Auteuil, j'vais te présenter une portugaise, mordue de sexe, sans faire aucun effort, tu baises J'dois me faire discret, j'ai la dégaine d'un dealer de me-seu, elle habite une loge de gardienne d'un immeuble de vieux Tes tuteurs le savent, je suis un séducteur de femmes, tes lèvres fines toute douces m'excitent T'aurais dû l'prévoir, c'est plus fort que oi-m, fevant une belle fille, je sors toujours le même speech Yo, toi avec ton p'tit boule d'actrice, viens par ici tirer sur ma Big Buddah Cheese Laissons de côté les sujets qui nous attristent, sur ma baguette enchantée, j'ai besoin d'un bisou magique J'ai dit, hey, toi avec ton p'tit boule d'actrice, viens par ici tirer sur ma Big Buddah Cheese Laissons de côté les sujets qui nous attristent, sur ma baguette enchantée, j'ai besoin d'un bisou magique Porte de Pantin, y'a une meuf un peu garçon manqué Elle va peut-être tomber pour avoir ppé-fra son banquier Les gens saints d'esprits l'appellent sens interdit Quand tu la vois, fais demi-tour ou tu perds tes dents, j't'avertis J'prends l'périph direction Porte d'Italie, c'est l'heure du thé, j'vais capter une salope britannique Elle comprend pas quand j'rappe donc j'sors des pures folies Posé sur le divan, bon vivant comme Berlusconi Porte de la Muette, dans le duplex d'une brunette sexy Y'a de la buée sur mes lunettes quand la fumée s'expire C'est la plus belle, j'y tiens comme à la prunelle de mes yeux C'est un tunnel sans fin quand l'adultère se fait vieux Tes tuteurs le savent, je suis un séducteur de femmes, tes lèvres fines toute douces m'excitent T'aurais dû l'prévoir, c'est plus fort que oi-m, fevant une belle fille, je sors toujours le même speech 4</t>
+          <t>Avant d'commencer c'son, j'avais un thème Un truc sombre sur la vendetta Dans la tête d'un jeune qui a la vingtaine Puis j'ai fumé un joint d'jaune avec untel Ou p't-être un joint d'zeb suivi d'un fond d'teille Et j'ai zappé, sa mère Faudrait qu'j'arrête cette merde avant d'dead On est seuls, c'qui fait qu'on est tristes Le mauvais il, ça l'fait kiffer qu'on s'détruise Dis-toi qu't'as tout pour toi, c'est important Quand est-ce qu'on va s'unir ? Il faut un temps pour tout, on forme un tout pourtant Faut qu'on soit formatés dans l'système, ils disent Ça m'fait flipper comme la montée d'l'antisémitisme On va en boîte, on s'fait chier Alors on fout l'zbeul, on finit dans les fichiers des colboks Comportement à l'école bof On s'bute à Call of en buvant des alcools forts Et les filles, je ne sais pas c'qu'elles veulent Mais je m'en fiche tant que j'enfile des baskets neuves Mais dès qu'j'ai mis la paire, ça y est, elle est plus neuve Problème épineux, dans ce shop y'aura p't-être une mieux On est continuellement frustrés consommer pour s'consoler J'm'amuse jamais dans les soirées mais j'continue d'm'incruster C'est pas bénéfique, les voisins débarquent avec La ferme intention de dire La ferme, attention, j'appelle les flics ! Je compte même plus les moments d'absence Je t'aime ça compte plus, les mots n'ont pas d'sens J'agrippe un Scud pendant qu'mon groupuscule Graille une crêpe au stud', face à Dieu Mes têtes lisses et crépues scrutent le même crépuscule J'ai mes résultats, tes raisons, mon réseau dans tes reilles-o Ce soir, dans ma tête, c'est sombre, j'ai mon majeur en érection J'gratte mes textes dans des allées coupe-gorge De la pure cocaïne sous l'eau Pas très loin de la coupole à l'époque de la Cool Co' J'aperçois la tombe, il faut pas faire d'erreur Toujours avec mes reufs même devant des balles à plomb Y'a qu'pour la victoire qu'on perd du grand cru T'as cru qu'on allait lever l'ancre A chaque fois qu'j'en rentre une Maintenant, tu sauras que j'prends de l'élan Un cycle interminable, j'ramène un flow impérial Dans une riade en mode survie comme Call of sur les terres d'Irak Y'a plus d'élégance à l'heure où on éteint les lampes Trop de métiers lents quand tu veux faire des millions Ils sont tombés des nues quand on a fait tomber des murs Tu veux nous voir en cert-con ? Viens nous voir à la tombée d'la nuit J'fais partie d'ces gens trop sincères pour ce monde de vicieux Donc j'ai pas prévu d'plan B mais tu m'as jamais vu tremper Pourtant une vie peut s'échanger contre 10 000E Pendant que j'longe le vide, viens pas m'parler du danger Vos débats souffrent d'une atroce stérilité Pour te du-per, c'est les filles biens Qu'les salopes ne cessent d'imiter J'suis qu'un homme, j'aime les femmes à forte fertilité Mais j'préfère mon équipe que seule la mort devrait diviser Et j'prétends pas résoudre les problèmes du monde J'veux juste être honnête avec mes collègues Ne jamais déconner pour le gros derche d'une blonde J'ai une dent contre ce pays que les commerces surplombent Microphonique prise de contact, j'envoie une mosaïque de rimes Cinématographiques dans les panoramiques de ton casque J'veux vivre de mes textes, kicker, faire de belles perf Nique le Medef, y'a que l'épicier que j'appelle chef J'ai mis le rap avant tout, la fac, les shabs, les femmes Mec, des fois ça rend fou, yo, laissez place à mon crew Nique la passivité, j'suis toujours en activité Mec, j'dois faire mon taff, question d'responsabilité Tu peux m'estampiller, couz, on est validé Ils donnent dans la quantité, nous, dans la qualité Et y'a du pain sur la planche, on inclut ma bande Parmi les pointures qui te ceinturent Et te mettent le flingue sur la tempe Laisse les potos taffer, tu peux photographier Yo, on brûle tous vos textes, mec autodafé ! Ouais, j'suis devenu un homme, faut que je tue l'insomnie Donc j'fais des putains d'bonnes rimes puis je débute un somme Mon rap, écoute-le, j'vais bouffer tout le jeu, mec Tu te doutes que on goûte beaucoup de beuh avant le couvre feu Le coup est douloureux, t'es choqué mais j'peux sauter plus haut Les gars toqués, approchez, osez roder à côté du fauve J'vais grogner pour donner du flow, étoffer mon palmarès Mes projets apparaissent, pas d'overdose car aucune maladresse J'ai de la sagesse, mais je suis de la nouvelle école J'vais redoubler d'effort avant de monter retrouver les morts Cocaïne Flow conçu pour du cash pour du pez pour du gros C'est Fougères dans la base, mec, nous défier qui ose ? On a la meilleure frappe khey, everybody knows Tu cherchais le meilleur kickeur, mon pote, tu t'es pas trompé J'ai voulu grimper dans la drogue, mais je ne suis pas tombé Nous on bosse à plein temps, clinquants, pimpants C'est Paris 20, mon pote, loin de Saint-Tropez I'm D.M.X. before the world got 'em Batman before he found Robin Got no problems, cop, bullet addiction Money, weed and rad bitches Slap dons, serving pillows for loot Stacking bread but I ain't drive in a Coupe Nothing under my mattress But a ratchet, gotta have it This America, you dumb niggas Where cops pull up just to kill niggas Not them so you know I got the heater All these niggas better see me Cause you know I'm gonna beat 'em, I'mma beam 'em Niggas better back up, back up before you get your fucked up Let me knock, cost too much and 'bout to spit the shit You niggas better know that I'm too lit Woo, my mouth got caught up Let me get back on the beat and let me show you what is up I'm here right now in Paris straight from L.A So you niggas know that I'm not scary And I'm chilling on the streets Niggas better see while I'm killing on the beat Niggas know I get it, you can walk up on my feet Nigga I'mma do it all the time Fuck la foule, j'aime les rues désertes Je m'en bats les couilles d'être le plus célèbre Tant que sur mes vers j'me dépense tellement Que j'ai l'impression d'gratter sur des chèques Si tu vis, vise la lune Le peu-Ra te fait pas sentir la thune Rien ne change dans nos vies, juste On bosse album dans des villas de luxe Entourage, Vincent Chase J'pars à l'aventure avec mes 10 collègues L'Entourage, Eff Gee Ça n'a rien à voir avec ces MC's Être les meilleurs, c'est ça qu'on fait Pour nous battre peu d'espoir C'est le L, on a quatre concerts Dans quatre villes le même soir Fais groover le dièse, les seules taches validées Sur les t-shirts sont entourées de têtes On veut toucher le ciel, faire notre truc maintenant Pour pas se dire plus tard qu'on pouvait le faire Je n'veux plus qu'on m'enferme, le système Veut m'dompter mais obéir Moi, je n'sais pas comment faire Nan, je n'sais pas comment faire J'veux sortir de là sans l'vice, pour l'instant Je n'sais pas comment faire, le Coran Est rempli d'instructions pourtant Je n'sais pas comment faire Ma graine se trouve toujours en terre Hustler jusqu'à c'que l'on m'enterre , c'est l'enfer, on m'dit changer Bébé, je n'sais pas comment faire Nan nan, je n'sais pas comment faire Nan, je n'sais pas comment faire Ma mère veut qu'j'fasse attention Et je n'sais pas comment faire Ouais, sale dynamique dans mon quartier Pas grand chose à part ma réputation Mais mes OG's m'ont montré Comment faire votre éducation Mec, tu sais, j'assassine, l'homme est assez Stupide pour s'faire expulser du Paradis Bien et Mal provoquent une émulation Donc vis par le gun, meurs par le gun Vite, passe ? ce thug a le seum Inhale le blunt. Je ne cherche pas midi à deux heures C'est biz à gogo, drogue, armes, ces MC's Écartent les jambes comme le logo Jordan J'glisse des disquettes vite fait J'vis une vie qu'les petits de mon bat kiffent Immunité diplomatique comme Dipset, Dipset Qu'un vrai négro subisse sans miauler? On a des égos surdimensionnés T'as dévalé la ville en scred, le silence est dans le respect Canalisé par le cannabis, je n'ai pas d'immenses rêves J'ai regardé l'évidence vraie mais la vérité sent la pisse T'auras beau laver cela dit T'as la , t'forniquer toute la nuit J'suis pas là pour t'guider ton ami, nan La belle n'a pas lavé le khalis, ouais Bah, repasse à la caisse, tu salives comme tes potes J'me vide sur ma feuille comme si j'étais aux chiottes J'ai gratté la massa, le départ est instable Pas sur le même piédestal et je pars sur des bases fats T'es comme le Joker face à Batman, l'idée ne passe pas Criblé de balles par nous, tu n'étais pas dans le coup Mais bon, j'étais là où les plus compétents Les bidons veulent le guidon, mon con Je ne dévale pas la ville avec les moutons Démarre la machine avec un pouce dans l'boul J'ai des frissons, le pacte est pas rompu Pendus par les pattes et les couilles sont tes équipiers Plus de balles dans le barillet, tous mes alliés sont prêts Les mots je manie et des dégâts sur ton palier, palier J'suis dans une suite de malade Canapé en cuir en dessous d'ses cuisses de mama Odeur de weed, de salade Mélangée à l'huile de massage Les corps se rapprochent, on est tous en sueur Ça prend tout son sens pour ma puissance J'aime les bons rapports dans la distance Quand t'avales, j'veux entendre Oui, mon maître ou tais-toi Fais ça gentiment, tu seras une petite poulette qui décoiffe Déscolarisé, rebeu, renoi, babtou, romanichel Dans les halls la misère On manigance pour les loves à Bill Gates Pour les modalités, fuck la moralité Che7ma dans le bolide, mordille-toi les lèvres Audi noire et beige, sors nous ton regard exotique Tu veux nous ressembler ? Bandes de nazes Si y'a des femmes mûres, j'veux prendre de l'age Si t'es qu'une sale pute, tu peux prendre ton tahma Si y'a pas de pub je reste un gentleman Tous les jours je remercie le ciel De permettre à la daronne de se lever de son lit Matin-midi, sortez pour l'oseille Conflit permanent avec la police Les rappeurs français sont dans l'agonie Piégés dans la trappe des chiens, tenus par des laisses Ils font les thugs faisant les macaques, j'en ai ma claque J'rafale dans le tas comme Tony, tant pis si j'y reste On fait nos bails en freelance Traqués par le ministère des finances Voir les pleurs de la daronne, ma peine est si dense Arrivés au monde, on crie, on meurt en silence Ta maman peut bien te cajoler Si tu fais le grand, ici, si tu finis foisonné Attiré par la merde, Des embrouilles, privé d'amour, la rue m'a façonné Fuck les balances et les lopettes du sentiment est perdu loin dans mes murs J'ai laissé la compassion sur l'tec' Aucun miroir n'est assez grand pour refléter mes erreurs J'rappe à mes heures perdues Étant donné que j'ai du temps à perdre Ouais, négro, j'ai du temps à tuer Avant qu'l'oseille me mène à ma perte Les démons dans ma te-tê viennent que quand j'pose J'suis loin des billets verts, j'ai pas les gants d'boxe Pour ne pas baisser les bras, j'ai fumé trop Guidé par le ballon, comme F.A., j'suis sincère quand j'cause Y'a qu'pour mes fêlés que j'fais des bad On a tisé dans la bouteille, c'était pas d'l'eau C'est pour mes vrais gars qu'on la passe et on l'attaque Ouais ouais, Dojo Family, y'a pas ta ce-pla dans le paquebot T'as cru qu'on allait rester al' ? Nan Il faut des billets pour qu'le véhicule soit allemand Besoin de crier qu'on est doux et que les places manquent Loin d'ici j'écris, je sais qu'ça finira brutalement J'ai Nekfeu pour me rendre pro Tout est ici, j'esquive les putes, les balles, comme Rambo Tous mes gavas, là, sont ready, contre la cage grognent Placer des coups bas ta jalousie provoque ta propre mort Primo, moi, j'aime pas ta tête secundo, j'aime pas ta tête Arrache-toi, jai pas de plaquette, boloss, mate la tech Dans ma bande, ya pas de tapettes Quand on rackette, ça dure pas 5 sets J'veux les 4-5 chiffres, après le 1, mets 4-5 chiffres Tous mes quatrains t'giflent, si tu veux du rap saint, siffle Petite catin, mon débit vaut bien plus que tes placements d'shit J'assassine les basses d'l'auto, j'ai le son qui passe au zoo Chez les cas sociaux, j'ai fait toutes mes classes au zoo C'est le 20 que t'entends mais j'ai vécu dans le 1 ocho Au milieu des putes, des règlements d'compte chauds Près des canailles et des Karaïs qui portent pas de poncho Près des quartiers gangs, des fous, des dingues Des sales dégaines, du bruit des flics Du bruit des flingues et puis des placements de dope Mon phrasé vient les désosser, pour ceux qu'ont fait les 400 coups Du deal, au vol de portable, une claque et on éteint ton pouls Même si t'as le jeu de jambes de Van Damme Pratique est la vente d'armes S'il paie pas ses dettes dans les délais, fais jouer les contacts C'est du sport de contact, serre les fesses et contracte Tu peux m'appeler gros cash, gros crack, coca, Sosa J'rentre pas dans leur quota, on vient pénétrer ton domicile Au pied d'biche, au gros missile, c'est l'équipe des gros, sisi Belek, j'officie, viens pas jouer les auch ici 75 zone d'homicide, c'est l'il ouvert qu'on dort Renoi, c'est le sang qui ruisselle sous les ponts d'or Bienvenue à Paris, fais péter tous les compteurs Tous les jours on s'entraîne à maîtriser nos peurs Tu peux voir mes ieps fouler le 7-5 Tu vas m'dire cest la vie, mais t'es pas 2 Chainz Les mecs séradiquent pour les mêmes scenari Pendant qu'le plus riche de tous se pète les narines En train d'baiser la ville sans même baisser la vitre Tu veux l'cayenne yo t'auras la couchette Plus belle quAyem nan t'auras la poussette Pas dBMFerrari quand la haine fait la bise Ouais la paye fait la diff', la plus vieille fée l'a dit, bang Cuit comme Willy Denzey la miff Lequel de mes gavas voudra ken ses amis J'vois des têtes de salive, plein de Bentley salignent Trop d'belles caisses à livrer, mais quels spécialistes ? Guette cest ça lhymne, quitte a vexer sa miss On s'reconnait plus lorsque les excès saniment Sexe et famille riment comme stress et vanille Donc pourquoi les mélanger, pourquoi les textes se salissent ? Moral dans les baskets mec Les problèmes de la vie rendront les casses-têtes clairs Au fond de labîme personne de classe taime, t'aide La couleur de ma rime tu t'manges une balle pleine tête Demande à Sheldon, demande au Panama On vient remplacer l'boss, prendre la force au padawan Viens pas tester Salim et sa punch des abysses J'suis dans la dans des restes de Paris Le soir, j'pisse du cool-al, convoitises d'une bonnasse Trop d'connards font naufrage, ça flippe vu nos armes A quinze dans un zin-gam, vous serez comme mon blaze Posés dans un gamos 'vec potes-bombasses Chien de la casse, tu siffles les moches et ça c'est illégal J'aime les femmes qui kiffent les hommes Mais pas les petites pédales T'as pas d'talent, connasse, mais qu'est-ce qu'tu veux savoir ? J'fais pas d'cunnilingus, j'donne pas ma langue au chat J'aime pas l'état et la bédave et toutes ces tass sheitanisées Tu fais l'vrai gars mais les vrais savent Tu fais qu'ler-par et baliser C'est quoi les bails, j'fais que pe-ra, saha, j'remplis des salles Petit, j'avais toujours les mêmes sapes Comme un héros d'dessin animé Tu mets des coups d'épée dans l'eau, l'affreux, on s'propage Prépare tes adieux, on fout le feu comme des Ghostriders Il faut que toutes les mains se lèvent haut Rimes façon West Coast, Gangsta à la Death Row Fuck les ennemis, miskine, ils se croient peut-être drôles Ca cartonne comme au rallye, au Carlton même sans khaliss Mes alliés se rallient, mental de patron On ne dit pas pardon, y'a que comme ça que tu seras libre Si j'tombe à Fleury, c'est qu'y a un beau million à prendre Ou qu'y a une tombe à fleurir, les tes-trai vont prendre des pralines J'ai pas vu d'boulot tendre, faut prendre pas l'9ar9ob Ils ont la boule au ventre, on a les abdos Alors ensuite on bosse, on pète le truc à la Mobb Deep C'est le mort, le Glock est raide A tout moment, la scène sera morbide P.A.N.A.M.A.B.E.N.D.E, les gars c'est grave Mais là je crois que c'est tes bavons qui sucent et ça m'écure En place, je fly, les autres croient que je vibe Tu veux continuer à insulter ? T'auras des noises de taille Gros excès de drogue et hérésie, ma caille c'est grave Moi je veux juste la renommée de Led Zeppelin Ou bien même celle des Red Devils Avoir le salaire de Gattuso, fuir jusqu'à Acapulco La France c'est dead, j'ai dis, je préfère Itchi à Naruto Je suis unanime, je rêve de me baigner, chiller sur la rive Obus d'haschich, brandit, fumant comme un feu de forêt Mais même avec ça j'oublie pas que je veux la carrière de Ludacris Obitaki sur ton papa, l'fétichiste de la campagne Reste ici, je rappe encore concocte des attentats Je suis un rappeur cyborg avec une pointe d'humanisme J'aime me fonce-dé sur un track du Kaaris Fume le zat pur, et mets des claques au buraliste Marre d'être déprimé, Seigneur, m'entends-tu ? Je me détruis même au détriment de mon art J'aimerais agir autrement... Peut-être que les mecs te mentent Et, nan, y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant... File-moi un rre-ve que je décolle Frère, j'me sens plus près d'la maison de retraite que de l'école Tous les soirs j'me bousille mais je n'regrette que de vrais torts Acteur de ma vie avant qu'on me jette dans le décor J'dois éviter le mesquin, dans ce film ton énigme c'est le destin Peut-être est-ce Dieu qui le rédige et nous prédit peu de belles fins Mes couplets j'les ai trouvé en route Le souffle d'un taureau, entre deux tains-p avec des sous-vêtements rouges Tu vois le topo, mec, on roule tricards en coupé dans l'hood Salaire de smicard avec un lifestyle de courtier en bourse C'est pour mes lèves-tard trop dégoûtés Par les journées sans flouze On veut l'milliard mais je n'vois que quelques dinars Sous le coussin, genre camouflés en douce J'suis c'prisonnier du ciment, tu devrais parler gentiment Tranquillement, j'ride avec des meufs que j'ai dragué en sifflant De temps il m'reste peu à vivre, j'laisse mon esprit s'évader J'écris des pavés, inspiré par ceux d'ma ville J'ai des problèmes dans ma vie Mais j'regarde le monde et me dis qu'c'est rien J'allume ma télé, j'vois qu'des vies s'éteindre Ouais, j'vois qu'du rouge, y'a plus d'rose J'vois qu'ça serre la ceinture J'vois des sous derrière un bureau J'vois un peuple derrière un mur J'vois qu'un daron vient chercher ta petite A l'école pour la violer dans un champ Il va la bruler donc tu la reverras jamais dans sa chambre S'écraser dans la pente, c'est tout c'qu'on va faire Société cracher dans la fente Et j'arrête pas d't'irriter, mes phases touchent ce qui t'blesse J'ai des facilités dans l'rap donc j'peux dire ce qu'il m'plait Et j'en profite, les gens parlent bien mais les gens profitent Faudrait qu'je change de pays si un jour j'veux faire un gros feat Nan, j'déconne, j'laisse un peu d'côté l'égotrip Là, j'laisse juste parler mon cur, j'me fous d'savoir si les gos kiffent Dans Paname, les gens cavalent, moi, j'm'y pavane Slow down comme le Roi dans son palace Errant sans dame et sans valet autour d'la table carrée J'suis pas un as mais un taré Pourquoi tout l'monde veut prendre ma place ? Je suis Roronoa donc je fuck Konoha Le One Piece, on l'aura à la force de nos bras Mon équipage booste mon aura Jusqu'à la trente-sixième bre-cham Puis brandit, bien devant moi, l'emblème de mon peu-ra J'démonte à coups d'bre-sa, qui veux tester le samouraï-ninja ? J'fais l'amour aux tines-pla, remballe tes diam's tous falsh J'te rentre des tas d'ouvrage tout comme le Père stor-Ca Qu'ils viennent des tours du torze-qua et de ses entourages Viens filme en tournage, mes yeux sont à la caméra Retranscrivant, d'la capitale, rouages, vices et aléas J'lévite, médite mes dires car il y a pire, c'est triste et là C'est les favelas, loin d'la Baltique, des Maldives aux Baléares Y'a qu'pour l'oseille que j'ai d'l'appétit, 300 000 E juste pou Si t'es un pédé comme Eddy, la balle se propage dans ta rétine Le lash-ka est sous mon parka, traces de sang sur mon parquet Sur le rain-t' on est le Barça donc il faut penser à s'démarquer counia, counia, counia counia, counia manman'w Atterrissage Pukhet-Ibiza t'es bizarre T'attends le dernier moment Pour prendre ton billet, le billet que tu m'dois, négro Tu sais que j'vais pas oublié, j'ai juste fait semblant , mourir d'un travail te mitraille comme , si tu survis c'est un miracle 4-7 AK comme en Irak, bienvenu dans l'bateau pirate Dieu seul sait où est-ce qu'on ira, jette re-co dans le virage La haine comme Tony pour Elvira C'est toi qui m'a dit que tout se paiera Bats les couilles, bats les couilles Qu'est-ce que vous avez tous ? Allez vous Faire enculer, j'vais ken des re-mè J'suis très rancunier, j'ai l'veau-cer en fumée clic-clic bah s'faire enrhumer J'ai pas d'amis, j'compte sur ma famille et sur mon famas Sur ma famille pour amasser du kamas Personne ne peut aimer le rap plus que moi je l'aime Il a flagellé mon âme lors des abus de ma jeunesse Il m'a ramené dans l'art, il m'a rappelé au calme Immature témoin des images dures de l'armée demoniaque Et peut-être que l'rap, certains l'font pour rire Mais, moi, j'cautionne pas Est-ce que quelque part dans ce monde pourri Des gens pensent comme moi ? J'entends les foules hurler... J'fous le boucan, j'vous l'ai juré1</t>
         </is>
       </c>
     </row>
@@ -1019,12 +1019,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Nekfeu, S-Crew, S.Pri Noir… en freestyle dans Planète Rap</t>
+          <t>Clan</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Avant d'commencer c'son, j'avais un thème Un truc sombre sur la vendetta Dans la tête d'un jeune qui a la vingtaine Puis j'ai fumé un joint d'jaune avec untel Ou p't-être un joint d'zeb suivi d'un fond d'teille Et j'ai zappé, sa mère Faudrait qu'j'arrête cette merde avant d'dead On est seuls, c'qui fait qu'on est tristes Le mauvais il, ça l'fait kiffer qu'on s'détruise Dis-toi qu't'as tout pour toi, c'est important Quand est-ce qu'on va s'unir ? Il faut un temps pour tout, on forme un tout pourtant Faut qu'on soit formatés dans l'système, ils disent Ça m'fait flipper comme la montée d'l'antisémitisme On va en boîte, on s'fait chier Alors on fout l'zbeul, on finit dans les fichiers des colboks Comportement à l'école bof On s'bute à Call of en buvant des alcools forts Et les filles, je ne sais pas c'qu'elles veulent Mais je m'en fiche tant que j'enfile des baskets neuves Mais dès qu'j'ai mis la paire, ça y est, elle est plus neuve Problème épineux, dans ce shop y'aura p't-être une mieux On est continuellement frustrés consommer pour s'consoler J'm'amuse jamais dans les soirées mais j'continue d'm'incruster C'est pas bénéfique, les voisins débarquent avec La ferme intention de dire La ferme, attention, j'appelle les flics ! Je compte même plus les moments d'absence Je t'aime ça compte plus, les mots n'ont pas d'sens J'agrippe un Scud pendant qu'mon groupuscule Graille une crêpe au stud', face à Dieu Mes têtes lisses et crépues scrutent le même crépuscule J'ai mes résultats, tes raisons, mon réseau dans tes reilles-o Ce soir, dans ma tête, c'est sombre, j'ai mon majeur en érection J'gratte mes textes dans des allées coupe-gorge De la pure cocaïne sous l'eau Pas très loin de la coupole à l'époque de la Cool Co' J'aperçois la tombe, il faut pas faire d'erreur Toujours avec mes reufs même devant des balles à plomb Y'a qu'pour la victoire qu'on perd du grand cru T'as cru qu'on allait lever l'ancre A chaque fois qu'j'en rentre une Maintenant, tu sauras que j'prends de l'élan Un cycle interminable, j'ramène un flow impérial Dans une riade en mode survie comme Call of sur les terres d'Irak Y'a plus d'élégance à l'heure où on éteint les lampes Trop de métiers lents quand tu veux faire des millions Ils sont tombés des nues quand on a fait tomber des murs Tu veux nous voir en cert-con ? Viens nous voir à la tombée d'la nuit J'fais partie d'ces gens trop sincères pour ce monde de vicieux Donc j'ai pas prévu d'plan B mais tu m'as jamais vu tremper Pourtant une vie peut s'échanger contre 10 000E Pendant que j'longe le vide, viens pas m'parler du danger Vos débats souffrent d'une atroce stérilité Pour te du-per, c'est les filles biens Qu'les salopes ne cessent d'imiter J'suis qu'un homme, j'aime les femmes à forte fertilité Mais j'préfère mon équipe que seule la mort devrait diviser Et j'prétends pas résoudre les problèmes du monde J'veux juste être honnête avec mes collègues Ne jamais déconner pour le gros derche d'une blonde J'ai une dent contre ce pays que les commerces surplombent Microphonique prise de contact, j'envoie une mosaïque de rimes Cinématographiques dans les panoramiques de ton casque J'veux vivre de mes textes, kicker, faire de belles perf Nique le Medef, y'a que l'épicier que j'appelle chef J'ai mis le rap avant tout, la fac, les shabs, les femmes Mec, des fois ça rend fou, yo, laissez place à mon crew Nique la passivité, j'suis toujours en activité Mec, j'dois faire mon taff, question d'responsabilité Tu peux m'estampiller, couz, on est validé Ils donnent dans la quantité, nous, dans la qualité Et y'a du pain sur la planche, on inclut ma bande Parmi les pointures qui te ceinturent Et te mettent le flingue sur la tempe Laisse les potos taffer, tu peux photographier Yo, on brûle tous vos textes, mec autodafé ! Ouais, j'suis devenu un homme, faut que je tue l'insomnie Donc j'fais des putains d'bonnes rimes puis je débute un somme Mon rap, écoute-le, j'vais bouffer tout le jeu, mec Tu te doutes que on goûte beaucoup de beuh avant le couvre feu Le coup est douloureux, t'es choqué mais j'peux sauter plus haut Les gars toqués, approchez, osez roder à côté du fauve J'vais grogner pour donner du flow, étoffer mon palmarès Mes projets apparaissent, pas d'overdose car aucune maladresse J'ai de la sagesse, mais je suis de la nouvelle école J'vais redoubler d'effort avant de monter retrouver les morts Cocaïne Flow conçu pour du cash pour du pez pour du gros C'est Fougères dans la base, mec, nous défier qui ose ? On a la meilleure frappe khey, everybody knows Tu cherchais le meilleur kickeur, mon pote, tu t'es pas trompé J'ai voulu grimper dans la drogue, mais je ne suis pas tombé Nous on bosse à plein temps, clinquants, pimpants C'est Paris 20, mon pote, loin de Saint-Tropez I'm D.M.X. before the world got 'em Batman before he found Robin Got no problems, cop, bullet addiction Money, weed and rad bitches Slap dons, serving pillows for loot Stacking bread but I ain't drive in a Coupe Nothing under my mattress But a ratchet, gotta have it This America, you dumb niggas Where cops pull up just to kill niggas Not them so you know I got the heater All these niggas better see me Cause you know I'm gonna beat 'em, I'mma beam 'em Niggas better back up, back up before you get your fucked up Let me knock, cost too much and 'bout to spit the shit You niggas better know that I'm too lit Woo, my mouth got caught up Let me get back on the beat and let me show you what is up I'm here right now in Paris straight from L.A So you niggas know that I'm not scary And I'm chilling on the streets Niggas better see while I'm killing on the beat Niggas know I get it, you can walk up on my feet Nigga I'mma do it all the time Fuck la foule, j'aime les rues désertes Je m'en bats les couilles d'être le plus célèbre Tant que sur mes vers j'me dépense tellement Que j'ai l'impression d'gratter sur des chèques Si tu vis, vise la lune Le peu-Ra te fait pas sentir la thune Rien ne change dans nos vies, juste On bosse album dans des villas de luxe Entourage, Vincent Chase J'pars à l'aventure avec mes 10 collègues L'Entourage, Eff Gee Ça n'a rien à voir avec ces MC's Être les meilleurs, c'est ça qu'on fait Pour nous battre peu d'espoir C'est le L, on a quatre concerts Dans quatre villes le même soir Fais groover le dièse, les seules taches validées Sur les t-shirts sont entourées de têtes On veut toucher le ciel, faire notre truc maintenant Pour pas se dire plus tard qu'on pouvait le faire Je n'veux plus qu'on m'enferme, le système Veut m'dompter mais obéir Moi, je n'sais pas comment faire Nan, je n'sais pas comment faire J'veux sortir de là sans l'vice, pour l'instant Je n'sais pas comment faire, le Coran Est rempli d'instructions pourtant Je n'sais pas comment faire Ma graine se trouve toujours en terre Hustler jusqu'à c'que l'on m'enterre , c'est l'enfer, on m'dit changer Bébé, je n'sais pas comment faire Nan nan, je n'sais pas comment faire Nan, je n'sais pas comment faire Ma mère veut qu'j'fasse attention Et je n'sais pas comment faire Ouais, sale dynamique dans mon quartier Pas grand chose à part ma réputation Mais mes OG's m'ont montré Comment faire votre éducation Mec, tu sais, j'assassine, l'homme est assez Stupide pour s'faire expulser du Paradis Bien et Mal provoquent une émulation Donc vis par le gun, meurs par le gun Vite, passe ? ce thug a le seum Inhale le blunt. Je ne cherche pas midi à deux heures C'est biz à gogo, drogue, armes, ces MC's Écartent les jambes comme le logo Jordan J'glisse des disquettes vite fait J'vis une vie qu'les petits de mon bat kiffent Immunité diplomatique comme Dipset, Dipset Qu'un vrai négro subisse sans miauler? On a des égos surdimensionnés T'as dévalé la ville en scred, le silence est dans le respect Canalisé par le cannabis, je n'ai pas d'immenses rêves J'ai regardé l'évidence vraie mais la vérité sent la pisse T'auras beau laver cela dit T'as la , t'forniquer toute la nuit J'suis pas là pour t'guider ton ami, nan La belle n'a pas lavé le khalis, ouais Bah, repasse à la caisse, tu salives comme tes potes J'me vide sur ma feuille comme si j'étais aux chiottes J'ai gratté la massa, le départ est instable Pas sur le même piédestal et je pars sur des bases fats T'es comme le Joker face à Batman, l'idée ne passe pas Criblé de balles par nous, tu n'étais pas dans le coup Mais bon, j'étais là où les plus compétents Les bidons veulent le guidon, mon con Je ne dévale pas la ville avec les moutons Démarre la machine avec un pouce dans l'boul J'ai des frissons, le pacte est pas rompu Pendus par les pattes et les couilles sont tes équipiers Plus de balles dans le barillet, tous mes alliés sont prêts Les mots je manie et des dégâts sur ton palier, palier J'suis dans une suite de malade Canapé en cuir en dessous d'ses cuisses de mama Odeur de weed, de salade Mélangée à l'huile de massage Les corps se rapprochent, on est tous en sueur Ça prend tout son sens pour ma puissance J'aime les bons rapports dans la distance Quand t'avales, j'veux entendre Oui, mon maître ou tais-toi Fais ça gentiment, tu seras une petite poulette qui décoiffe Déscolarisé, rebeu, renoi, babtou, romanichel Dans les halls la misère On manigance pour les loves à Bill Gates Pour les modalités, fuck la moralité Che7ma dans le bolide, mordille-toi les lèvres Audi noire et beige, sors nous ton regard exotique Tu veux nous ressembler ? Bandes de nazes Si y'a des femmes mûres, j'veux prendre de l'age Si t'es qu'une sale pute, tu peux prendre ton tahma Si y'a pas de pub je reste un gentleman Tous les jours je remercie le ciel De permettre à la daronne de se lever de son lit Matin-midi, sortez pour l'oseille Conflit permanent avec la police Les rappeurs français sont dans l'agonie Piégés dans la trappe des chiens, tenus par des laisses Ils font les thugs faisant les macaques, j'en ai ma claque J'rafale dans le tas comme Tony, tant pis si j'y reste On fait nos bails en freelance Traqués par le ministère des finances Voir les pleurs de la daronne, ma peine est si dense Arrivés au monde, on crie, on meurt en silence Ta maman peut bien te cajoler Si tu fais le grand, ici, si tu finis foisonné Attiré par la merde, Des embrouilles, privé d'amour, la rue m'a façonné Fuck les balances et les lopettes du sentiment est perdu loin dans mes murs J'ai laissé la compassion sur l'tec' Aucun miroir n'est assez grand pour refléter mes erreurs J'rappe à mes heures perdues Étant donné que j'ai du temps à perdre Ouais, négro, j'ai du temps à tuer Avant qu'l'oseille me mène à ma perte Les démons dans ma te-tê viennent que quand j'pose J'suis loin des billets verts, j'ai pas les gants d'boxe Pour ne pas baisser les bras, j'ai fumé trop Guidé par le ballon, comme F.A., j'suis sincère quand j'cause Y'a qu'pour mes fêlés que j'fais des bad On a tisé dans la bouteille, c'était pas d'l'eau C'est pour mes vrais gars qu'on la passe et on l'attaque Ouais ouais, Dojo Family, y'a pas ta ce-pla dans le paquebot T'as cru qu'on allait rester al' ? Nan Il faut des billets pour qu'le véhicule soit allemand Besoin de crier qu'on est doux et que les places manquent Loin d'ici j'écris, je sais qu'ça finira brutalement J'ai Nekfeu pour me rendre pro Tout est ici, j'esquive les putes, les balles, comme Rambo Tous mes gavas, là, sont ready, contre la cage grognent Placer des coups bas ta jalousie provoque ta propre mort Primo, moi, j'aime pas ta tête secundo, j'aime pas ta tête Arrache-toi, jai pas de plaquette, boloss, mate la tech Dans ma bande, ya pas de tapettes Quand on rackette, ça dure pas 5 sets J'veux les 4-5 chiffres, après le 1, mets 4-5 chiffres Tous mes quatrains t'giflent, si tu veux du rap saint, siffle Petite catin, mon débit vaut bien plus que tes placements d'shit J'assassine les basses d'l'auto, j'ai le son qui passe au zoo Chez les cas sociaux, j'ai fait toutes mes classes au zoo C'est le 20 que t'entends mais j'ai vécu dans le 1 ocho Au milieu des putes, des règlements d'compte chauds Près des canailles et des Karaïs qui portent pas de poncho Près des quartiers gangs, des fous, des dingues Des sales dégaines, du bruit des flics Du bruit des flingues et puis des placements de dope Mon phrasé vient les désosser, pour ceux qu'ont fait les 400 coups Du deal, au vol de portable, une claque et on éteint ton pouls Même si t'as le jeu de jambes de Van Damme Pratique est la vente d'armes S'il paie pas ses dettes dans les délais, fais jouer les contacts C'est du sport de contact, serre les fesses et contracte Tu peux m'appeler gros cash, gros crack, coca, Sosa J'rentre pas dans leur quota, on vient pénétrer ton domicile Au pied d'biche, au gros missile, c'est l'équipe des gros, sisi Belek, j'officie, viens pas jouer les auch ici 75 zone d'homicide, c'est l'il ouvert qu'on dort Renoi, c'est le sang qui ruisselle sous les ponts d'or Bienvenue à Paris, fais péter tous les compteurs Tous les jours on s'entraîne à maîtriser nos peurs Tu peux voir mes ieps fouler le 7-5 Tu vas m'dire cest la vie, mais t'es pas 2 Chainz Les mecs séradiquent pour les mêmes scenari Pendant qu'le plus riche de tous se pète les narines En train d'baiser la ville sans même baisser la vitre Tu veux l'cayenne yo t'auras la couchette Plus belle quAyem nan t'auras la poussette Pas dBMFerrari quand la haine fait la bise Ouais la paye fait la diff', la plus vieille fée l'a dit, bang Cuit comme Willy Denzey la miff Lequel de mes gavas voudra ken ses amis J'vois des têtes de salive, plein de Bentley salignent Trop d'belles caisses à livrer, mais quels spécialistes ? Guette cest ça lhymne, quitte a vexer sa miss On s'reconnait plus lorsque les excès saniment Sexe et famille riment comme stress et vanille Donc pourquoi les mélanger, pourquoi les textes se salissent ? Moral dans les baskets mec Les problèmes de la vie rendront les casses-têtes clairs Au fond de labîme personne de classe taime, t'aide La couleur de ma rime tu t'manges une balle pleine tête Demande à Sheldon, demande au Panama On vient remplacer l'boss, prendre la force au padawan Viens pas tester Salim et sa punch des abysses J'suis dans la dans des restes de Paris Le soir, j'pisse du cool-al, convoitises d'une bonnasse Trop d'connards font naufrage, ça flippe vu nos armes A quinze dans un zin-gam, vous serez comme mon blaze Posés dans un gamos 'vec potes-bombasses Chien de la casse, tu siffles les moches et ça c'est illégal J'aime les femmes qui kiffent les hommes Mais pas les petites pédales T'as pas d'talent, connasse, mais qu'est-ce qu'tu veux savoir ? J'fais pas d'cunnilingus, j'donne pas ma langue au chat J'aime pas l'état et la bédave et toutes ces tass sheitanisées Tu fais l'vrai gars mais les vrais savent Tu fais qu'ler-par et baliser C'est quoi les bails, j'fais que pe-ra, saha, j'remplis des salles Petit, j'avais toujours les mêmes sapes Comme un héros d'dessin animé Tu mets des coups d'épée dans l'eau, l'affreux, on s'propage Prépare tes adieux, on fout le feu comme des Ghostriders Il faut que toutes les mains se lèvent haut Rimes façon West Coast, Gangsta à la Death Row Fuck les ennemis, miskine, ils se croient peut-être drôles Ca cartonne comme au rallye, au Carlton même sans khaliss Mes alliés se rallient, mental de patron On ne dit pas pardon, y'a que comme ça que tu seras libre Si j'tombe à Fleury, c'est qu'y a un beau million à prendre Ou qu'y a une tombe à fleurir, les tes-trai vont prendre des pralines J'ai pas vu d'boulot tendre, faut prendre pas l'9ar9ob Ils ont la boule au ventre, on a les abdos Alors ensuite on bosse, on pète le truc à la Mobb Deep C'est le mort, le Glock est raide A tout moment, la scène sera morbide P.A.N.A.M.A.B.E.N.D.E, les gars c'est grave Mais là je crois que c'est tes bavons qui sucent et ça m'écure En place, je fly, les autres croient que je vibe Tu veux continuer à insulter ? T'auras des noises de taille Gros excès de drogue et hérésie, ma caille c'est grave Moi je veux juste la renommée de Led Zeppelin Ou bien même celle des Red Devils Avoir le salaire de Gattuso, fuir jusqu'à Acapulco La France c'est dead, j'ai dis, je préfère Itchi à Naruto Je suis unanime, je rêve de me baigner, chiller sur la rive Obus d'haschich, brandit, fumant comme un feu de forêt Mais même avec ça j'oublie pas que je veux la carrière de Ludacris Obitaki sur ton papa, l'fétichiste de la campagne Reste ici, je rappe encore concocte des attentats Je suis un rappeur cyborg avec une pointe d'humanisme J'aime me fonce-dé sur un track du Kaaris Fume le zat pur, et mets des claques au buraliste Marre d'être déprimé, Seigneur, m'entends-tu ? Je me détruis même au détriment de mon art J'aimerais agir autrement... Peut-être que les mecs te mentent Et, nan, y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant... File-moi un rre-ve que je décolle Frère, j'me sens plus près d'la maison de retraite que de l'école Tous les soirs j'me bousille mais je n'regrette que de vrais torts Acteur de ma vie avant qu'on me jette dans le décor J'dois éviter le mesquin, dans ce film ton énigme c'est le destin Peut-être est-ce Dieu qui le rédige et nous prédit peu de belles fins Mes couplets j'les ai trouvé en route Le souffle d'un taureau, entre deux tains-p avec des sous-vêtements rouges Tu vois le topo, mec, on roule tricards en coupé dans l'hood Salaire de smicard avec un lifestyle de courtier en bourse C'est pour mes lèves-tard trop dégoûtés Par les journées sans flouze On veut l'milliard mais je n'vois que quelques dinars Sous le coussin, genre camouflés en douce J'suis c'prisonnier du ciment, tu devrais parler gentiment Tranquillement, j'ride avec des meufs que j'ai dragué en sifflant De temps il m'reste peu à vivre, j'laisse mon esprit s'évader J'écris des pavés, inspiré par ceux d'ma ville J'ai des problèmes dans ma vie Mais j'regarde le monde et me dis qu'c'est rien J'allume ma télé, j'vois qu'des vies s'éteindre Ouais, j'vois qu'du rouge, y'a plus d'rose J'vois qu'ça serre la ceinture J'vois des sous derrière un bureau J'vois un peuple derrière un mur J'vois qu'un daron vient chercher ta petite A l'école pour la violer dans un champ Il va la bruler donc tu la reverras jamais dans sa chambre S'écraser dans la pente, c'est tout c'qu'on va faire Société cracher dans la fente Et j'arrête pas d't'irriter, mes phases touchent ce qui t'blesse J'ai des facilités dans l'rap donc j'peux dire ce qu'il m'plait Et j'en profite, les gens parlent bien mais les gens profitent Faudrait qu'je change de pays si un jour j'veux faire un gros feat Nan, j'déconne, j'laisse un peu d'côté l'égotrip Là, j'laisse juste parler mon cur, j'me fous d'savoir si les gos kiffent Dans Paname, les gens cavalent, moi, j'm'y pavane Slow down comme le Roi dans son palace Errant sans dame et sans valet autour d'la table carrée J'suis pas un as mais un taré Pourquoi tout l'monde veut prendre ma place ? Je suis Roronoa donc je fuck Konoha Le One Piece, on l'aura à la force de nos bras Mon équipage booste mon aura Jusqu'à la trente-sixième bre-cham Puis brandit, bien devant moi, l'emblème de mon peu-ra J'démonte à coups d'bre-sa, qui veux tester le samouraï-ninja ? J'fais l'amour aux tines-pla, remballe tes diam's tous falsh J'te rentre des tas d'ouvrage tout comme le Père stor-Ca Qu'ils viennent des tours du torze-qua et de ses entourages Viens filme en tournage, mes yeux sont à la caméra Retranscrivant, d'la capitale, rouages, vices et aléas J'lévite, médite mes dires car il y a pire, c'est triste et là C'est les favelas, loin d'la Baltique, des Maldives aux Baléares Y'a qu'pour l'oseille que j'ai d'l'appétit, 300 000 E juste pou Si t'es un pédé comme Eddy, la balle se propage dans ta rétine Le lash-ka est sous mon parka, traces de sang sur mon parquet Sur le rain-t' on est le Barça donc il faut penser à s'démarquer counia, counia, counia counia, counia manman'w Atterrissage Pukhet-Ibiza t'es bizarre T'attends le dernier moment Pour prendre ton billet, le billet que tu m'dois, négro Tu sais que j'vais pas oublié, j'ai juste fait semblant , mourir d'un travail te mitraille comme , si tu survis c'est un miracle 4-7 AK comme en Irak, bienvenu dans l'bateau pirate Dieu seul sait où est-ce qu'on ira, jette re-co dans le virage La haine comme Tony pour Elvira C'est toi qui m'a dit que tout se paiera Bats les couilles, bats les couilles Qu'est-ce que vous avez tous ? Allez vous Faire enculer, j'vais ken des re-mè J'suis très rancunier, j'ai l'veau-cer en fumée clic-clic bah s'faire enrhumer J'ai pas d'amis, j'compte sur ma famille et sur mon famas Sur ma famille pour amasser du kamas Personne ne peut aimer le rap plus que moi je l'aime Il a flagellé mon âme lors des abus de ma jeunesse Il m'a ramené dans l'art, il m'a rappelé au calme Immature témoin des images dures de l'armée demoniaque Et peut-être que l'rap, certains l'font pour rire Mais, moi, j'cautionne pas Est-ce que quelque part dans ce monde pourri Des gens pensent comme moi ? J'entends les foules hurler... J'fous le boucan, j'vous l'ai juré1</t>
+          <t>J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien Pense au passé, souviens-toi du futur yeah, j'suis dans le phrasé, hier, j'étais foutu eh ouais On a tout cassé, on a tout vu, est-c'que tu vois la fraternité qu'on a cousue ? Rien n's'efface, on est shrab depuis eh, on les passe quand le mal te suit ah ouais On est frères plutôt que des bons amis, on est solides yeah, yeah T'as payé cher la fausse compagnie si t'aimes la solitude -Crew, 2001 J'représenterai jusqu'à la mort mes res-frè yeah Ouais, c'est mon sang, mon repère C'est dans le sale qu'on opère Beaucoup sont là par intérêt Y a qu'la maille qui les intéresse Vices et sourires pour s'insérer Combien de vrais khos sincères ? Combien ? J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien Saper les frères en vrai, c'est cile-fa, combien sont partis une fois la peur présente ? J'écoute leurs sons, j'm'identifie pas, y a que les miens qui me représentent T'admires les mauvaises étoiles, t'en as perdu le nord perdu le nord Parle pas de la street à un frère qui a vécu dehors vécu dehors, eh Pour construire le futur, on se sert du passé tout en profitant du moment présent yeah Quand tu viens me parler, c'est par nécessité, fais pas genre tu veux savoir comment j'me sens Fin de couplet, pas besoin de m'étaler, on reste soudés, notre amour est métallique Tu sais, chez eux, le prix du respect varie, le même produit mais c'est pas le même tarif J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Clan</t>
+          <t>Grünt Hors-Série 日本 🇯🇵 (Japon)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien Pense au passé, souviens-toi du futur yeah, j'suis dans le phrasé, hier, j'étais foutu eh ouais On a tout cassé, on a tout vu, est-c'que tu vois la fraternité qu'on a cousue ? Rien n's'efface, on est shrab depuis eh, on les passe quand le mal te suit ah ouais On est frères plutôt que des bons amis, on est solides yeah, yeah T'as payé cher la fausse compagnie si t'aimes la solitude -Crew, 2001 J'représenterai jusqu'à la mort mes res-frè yeah Ouais, c'est mon sang, mon repère C'est dans le sale qu'on opère Beaucoup sont là par intérêt Y a qu'la maille qui les intéresse Vices et sourires pour s'insérer Combien de vrais khos sincères ? Combien ? J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien Saper les frères en vrai, c'est cile-fa, combien sont partis une fois la peur présente ? J'écoute leurs sons, j'm'identifie pas, y a que les miens qui me représentent T'admires les mauvaises étoiles, t'en as perdu le nord perdu le nord Parle pas de la street à un frère qui a vécu dehors vécu dehors, eh Pour construire le futur, on se sert du passé tout en profitant du moment présent yeah Quand tu viens me parler, c'est par nécessité, fais pas genre tu veux savoir comment j'me sens Fin de couplet, pas besoin de m'étaler, on reste soudés, notre amour est métallique Tu sais, chez eux, le prix du respect varie, le même produit mais c'est pas le même tarif J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien j'étais rien J'représenterai toujours pour les miens pour les miens Pour eux, j'étais tout quand j'étais rien, j'étais rien</t>
+          <t>Tout d'abord, j'en place une pour tout ceux qui sont partis trop tôt Force aux frolos, la vie, c'est comme un Loto Poto, ça va trop vite un jour, tu bédaves du popo Tu deviens claustro', le lendemain, ça s'ra l'hosto On n'a pas bibi par choix, ne l'oublie pas p'tit frère Maintenant qu'on est yo, on n'a plus b'soin d'ces choses, p'tit frère Pendant des années, en faisant du mal, j'ai fait du bien Fallait bien payer l'loyer, maintenant, c'est fini Y'en a très peu que j'considère comme mes grands frères Les liens du sang qui découlent de la grand-mère J'suis ni très vieux ni très pieux mais je sais quand m'taire Un gain de temps quand tu grandis dans la gangrène Obligé d'brûler cette substance pour trouver l'sommeil Ce monde est glauque, imagine un glock posé sur ton globe oculaire Sans aucune aide, c'est moi et ma chance Va-t-il trembler ou juste prendre l'blé ? La grande délinquance Implique des dangers, fils d'étrangers, j'veux gonfler ma panse Quoi d'autre, quoi d'autre, quoi d'autre ? Avant d'dompter la France Frère, on bédave comme si c'était légal mais c'est pas Me-da Des zones de non droit où les Hongrois cachent les murders Frère, c'est Paname et ses aléas On te banane si tu t'balades trop près de nos allées crades Niggiz, j't'ai dit c'est Paname et ses aléas Pour une garre-ba ou une kehba? ça s'canarde jusqu'au carnage Y'a pas d'partage avec ces sasa' J'les tabasse comme mon taga Doums alias Morgan pour les tagasses SuperSound niggiz, Seine Zoo c'est l'souk, call les cops niggiz J't'ai dit c'est SuperSound niggiz, Seine Zoo c'est l'souk, call les cops niggiz SuperSound niggiz, Seine Zoo c'est l'souk, call les cops niggiz Un vrai repère le Rap, y'a trop d'faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Ouais, 'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des seaux de larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme Ouais, c'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'je pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Solitaire qui traîne en bande, j'ai pas l'air sympathique En effet, c'est vrai j'aime pas la fée mais les fanatiques J'arrive tel un tsunami, fallait t'méfier d'l'eau qui dort Après avoir vu les filles défiler j'veux des los-ki d'or J'ai pas eu l'enfant du mec riche, plein de vices, très mal élevé Quand les vengeances du rire que le pardon pour les arrêter J'aime pas faire semblant, j'suis vrai, j'suis pas la honte de ma ruelle À croire qu'c'est en vendant du rêve que le tien deviendra réel J'm'appelle Mekra, j'suis né pour baffer les plafs Les faux frères, ouais, tout ces mecs la tous J'suis un félin femelle, on t'fera la fête Si t'as le boule bombé, ça f'ra l'affaire Ça a mal commencé comme un check raté Ça va mal finir comme une histoire de dette Si tu t'demandes où j'suis, j'suis dans ta tête le reste, c'est dépassé Les lignes sont pré-tracées Ils m'demandent c'est comment ? j'leur réponds tkt T'as quoi en plus une fois les nerfs passés ? J'vois des pantins éphémères s'bâcher Devenir mongol comme le kop de Fenerbahçe En bas d'chez moi, y'a plus de richesse depuis qu'c'est la crise Si tu t'demandais d'où venait mon cynisme et mon envie d'prêcher L'envie d'faire mieux et la haine dessinent des motifs Certains mélangent les deux, y trouvent la motiv' Un jour, on dira tous au revoir, on mettra pas d'emoji Avant laisse-moi l'temps d'arriver, j'suis juiced up, j'ai fait les modifs Cette bande de fake ass va danser l'lean-back Plus de putes que dans les Vine de King Bach Gros, y'a pas d'subli, y'a que des flip-flap Vingt milles lieues sous la merde dans la trixe-ma Dans la trix-ma, j'les graille comme un Kit Kat Flip-flap j'kick aç, c'est comme aç comme un dique-sa C'est Nek le Fenek j'prends le mic, improvise Avec mes gavas, tu sais qu'on atomise toutes ces salopes, c'est promis C'est quoi les dises ? Balance la suite mon gava faut qu'tu brûles les cliques J't'ai dit, on atomise j'aime pas quand les nanas tho-my, hein Baise ton anatomie, fuck les thos-my, j'prends le cro-mi C'est promis, ça r'vient j'suis comme un putain de cro-ma, et ouais j'les traumat' J'fais mon bail en direct du toit, qu'est-c'tu vois ? Fuck les lois, fuck toi Fuck tout ceux qui veulent pas comprendre que c'est nous, le putain de crew J'fais mes bails, j'fais des trous dans leurs curs de hum, aah C'est nous les rois, mais à quoi elles jouent, on les troue C'est tous des oufs, bellek là c'est l'crew de Doums Écoute les bails, on est posés, on est calmes Tu fais le fou, tu vas goûter quelques pas Ça va siffler dans ton oreille, c'est quoi les g's avec mes gavas, c'est toujours la même On est à Tokyo, freestyle Grünt, on va les baiser c'est des laisse et freine C'est quoi les g's, j'ai plus les mots, Ken l'a déjà dit les French OVO sur toutes ces hoes Laisse-nous faire les choses, c'est de l'impro Arrête de faire celui qu'a trop de flouze J'rappe, j'ai trop de flow, j'ai mon eau de source Tu vois bien que c'est toujours pour le Doums Tu vois bien que c'est toujours pour le crew Y'a Alpha qui arrive avec un banda rose Il fait ça pour tous les putains d'bandero C'est comme ça qu'je le fait, j't'ai vu bander kho C'est chelou, c'est comment qu'on l'fait ? J'fais le fric et j'vais pas d'mander trop, nan J'vais pas demander d'crocs, là y'a le nouveau kho On vient de débarquer dans l'bail, ça va être trop trop chaud C'est quoi le bail le Phall ? Est-c'que t'es prêt mon gars ? À balancer quelques impros, ouais pour tous les kho Sisisi, j'voulais aller au Mcdo, mais j'me suis paumé Donc j'suis allé chez dennis Nike pour la paire de Tennis, il frémissent Alph Lauren, toujours le vêtement qui hennit En fait la té-véri, c'est qu'j'ai monté les marches, donc j'suis encore essoufflé, hey Dans l'appart', hey, je vais séjourner, on va les shooter La carrière de ces wack MC's va être écourtée On va les découper avec les couplets ou avec les impros Sur le fil du rasoir, sur le fil du couperet C'est quoi les bails ? Il faut riposter On est prêts sur le bail avec le Feu C'est quoi les ? On va donner c'que l'on veut C'est vrai, il faut tripoter, il faut riposter, il faut tricoter, il faut hiphoper Il faut fricoter, même ricosser, j'suis un putain de Grec et aussi Ecossais Avec les vrais bitches, on va fricoter, toi-même tu sais, on est les types côtés Les rimes vont ricocher, on est pas les types cokés J'en place une pour l'cameraman au rik à love J'en place une pour Timothé, même si j'sais pas qui c'est J'en place une pour les biatchs qui sont team Hôtel Team hôtel, c'est facile on va les immoler Philly Flingue jamais de demi molle, j'arrive, pas d'mimolette Vas-y molo, c'est comme ça qu'on l'fait, pas de trémolo J'en place une pour mon frais, mon Lo', qui vient de partir J'en place une aussi pour les frémologues Les vrais frolos qui sont al' dans Tokyo Même air, L-I-S avec tous les kho Toi-même tu sais, toujours le crew à Tokyo On est tellement bien, on mange des sushis, on boit de l'eau bio Je flingue ta tête et j'vise tes lobes, yo J'viens te fumer un peu comme l'opium Et j'arrive comme Sébastien Loeb, yo Donc je finis sur le podium Dur de lire c'qu'y'a sur mes labialles, c'est la mafia Tellement d'style, on mange un plat de nouilles, on dirait qu'on mange du caviar Et tu t'agenouilles, bang bang, un tas de douilles Philly Flingue, Alph le Tigre, Alph le Loup, non jamais de paires de Afflelou Là, il raffle tout, c'est un freestyle ou des textes Tu t'demandes c'est quoi les dises, écoute les couz, on est les meilleurs, pas de coups de coudes On reste coude à coude Sisisi, que des impros pas de textes, on flex, avec ta futur motherfuckin ex Restaurant Tex Mex, en provenance d'une tasse qui vient de Aix-en-Provence Moi, j'viens du Nord de Paris, neuvième zone où je gravite Pour faire du biff, ça s'agite, black and white dans le sachet Pendant qu'tu dragues que des rousses moi, j'lui gratte des bouts d'clope Nous, c'est la Jack ou la ruskov, on niaxe sur le rooftop Pour atteindre le sommet, en équipe ça va d'soi Faut vesqui l'abattoir, quitte à en perdre le sommeil Avec deux-trois gavas, posés à Montmartre Il se fait tard, on est fêtard rien qu'ça féraille avec Fera, on est veinard yeah Toute la s'maine, tous les jours du mois ou toute l'année Tu veux un check ? Niggiz, touche du bois La mif comme moteur, coffre la fraîche Les flics arrivent si vite sur les hauteurs, nos regrets s'effritent avec le shit, motherfucker J'me suis trompé de pellicule, j'vois tout en négatif Et mon seul sédatif, c'est de recompter les thunes Pas facile d'être un artiste on charbonne, on est actif Après une tempête de sable, il faut remonter les dunes Je ne veux pas du monde à mes pieds Je veux que mon nom, tout le monde sache l'épeler Ouais, j'ai un train de vie de fêlé La vie, c'est pas la télé mais j'veux zapper quand ça me déplaît Ouais, j'vais pas rentrer dans l'détail mais on a plié de la féraille Que mon train de vie en déraille, yeah On m'avait dit dans tes rêves mais j'ai la tête dure Comme sur Twitter, toujours en TT Seul passager de mon train de vie Toujours plus vite retiens la devise Trop de bons souvenirs, le stockage est bientôt saturé Donc j'ai déjà zappé tout ce que je viens de vivre J'essaie de bien m'tenir mais c'est rien de l'dire Un homme qui n'agit pas, il n'y a rien de pire Tu prends de l'âge et ça tu ne le vois pas venir Le temps qui passe te fera breaker comme une feinte de tir Tu peux prononcer mon nom sauf si t'es devant un bleu Ils ont vu passer mon ombre comme la fumée dans le blunt J'ai dû prendre de l'ampleur quand j'ai vu qu'dans ses yeux il pleuvait Efficace dans le biz donc j'ai une emprise sur le plug On doit s'entendre sur les termes mais sinon gringo ça peut l'faire On veut du biff jusqu'au plafond, notre musique, c'est de la peuf' La came part en fumée, dans nos caves ou dans celle des stups Ce qui nous arrive c'est l'destin, on laisse les salles en feu, ouais Certains vivent dans l'passé, d'autres veulent vivre dans l'futur On vit l'instant présent, tous aux Zéniths pour le Feu Tour Ma vie, je la chante et le peuple la vit comme il l'entend Si t'attends ta chance, c'est sûrement qu'la peur sommeille en toi Pourquoi mon cur a-t-il sombré ? Quand j'leur pose la question, c'est juste pour savoir si ils sont vrais Même si on a fait du racket, je viens pas jouer les durs à cuire Beaucoup ont dû raquer, j'suis dans les histoires dures à croire Bébé, je reste en ville que pour quelques jours Je veux lire mon nom sur tes lèvres douces J'veux que t'écoutes ce son et que tes fesses bougent Et qu'on amène le bendo dans les fêtes de bourges J'attrape la Mustang par la crinière Décapotable, j'ai le vent comme soin capillaire Monte du côté passager mais fais-toi discrète Tu m'dis que t'aimes flirter bien que tu sois fidèle Tu tiens le volant pendant que je roule mon spliff Je te dis que tu m'attires et que t'es plutôt mon style Ma fierté m'aura p't-être un jour J'préfère ça que de vivre à genoux J'suis pas comme vous, non, j'suis pas un gnou Quand la coupe est pleine, on plaide la self-défonce Ouais l'affreux, j't'efface, en un quart de s'conde J'viens d'passer l'quart de siècle toujours la même routine J'me mets à faire du sport, j'arrête la semaine d'après J'fume la verte, l'amnes' pour oublier mes soucis Et j'en ai beaucoup, frérot, oui, j'en ai beaucoup Ça chauffe, c'est l'insolation mais c'est pas l'Afghanistan J'te bibi ta consommation pour toi, c'est comme un talisman Pas de deuxième sommation, la soumission s'ra la seule issue La solution, c'est l'khaliss mais c'est salissant Même les voleurs ont des valeurs À Paris centre, Paris centre, Paris J'te dis que même mes voleurs ont des valeurs À Paris centre, Paris centre, Paris J'irai haut comme une montgolfière Maman, t'auras la clé des coffres, tu remonteras mon col, fière Demain, on va jouer au golf, après-demain on dira qu'on a joué au golf hier J'vais pas sauver l'monde et le monde va pas m'sauver On s'remplit comme nos ventres, froid comme novembre J'ai grandi dans les orties, j'les sens plus Hey, on est dans l'truc, le gang est de sortie Tiser des litres, sniffer des lignes ? Nan Prendre des drogues aux effets psychédéliques ? Nan J'vais expliquer l'délire niquer l'élite Qui a gardé le fric et les livres ? On fraudait déjà l'bus au C.P. vu qu'nos C.V. sont vides Hey, vu qu'nos C.V. sont vides J'oublie mon texte et j'reviens avec dou-Mama, on fait le feat On glisse sur l'instru de Mad Skillz Car j'ai beaucoup d'lyrics et de shit dans la chambre Y'a du chrome sur les jantes, négro Eh, c'est comme ça qu'on voit l'motherfucking futur Faut qu'le truc dure Mes motherfucking impro sont comme un motherfucking boa constrictor au niveau d'la structure Car il n'y en a pas, le truc est infini, balance un vinyle Hey, qu'on l'fasse tourner, Philly Flingue, j'ai fumé plein d'phillies Blunt, j'ai fumé plein d'phillies blunt J'ai fumé plein d'phillies blunt, plein d'phillies blunt x4 Trop de lyrics et de shit dans ma chambre chambre Ça swingue swingue à souhait souhait, soin soin Ah cette prod, on l'a kickée maintes fois avec Phaal Rien à foutre que ces salopes sont nymphos et Ça n'm'intéresse pas, j'aime pas trop les folles Avec mes gavas en impro, rien qu'on décolle On décolle, on décolle comme les profits J'suis au Mont Fuji, je bois du blended coffee C'est comme ça qu's'appelle la motherfucking canette J'veux faire de la maille comme Michael et Janet De la maille comme Michael et Janet ou bien Danette Rien à foutre d'ces salopes, moi, j'suis pas de la même planète J'fume que du brocolis, on dirait un Namek Nan, j'suis trop chaud, j'suis comme Broly, nique ta mère Sisisi c'est pour les faux khos, non c'est pour les vrais zins On est au Mont Fuji, on boit des canettes de Fanta raisin En fait, mon faux vaut plus d'cent balles Avant, c'était une canette et maintenant, c'est plus qu'un cendar Car tout se construit et se re-transforme Philly Flingue au microphone, tu sais, oui, je suis en forme J'avance avec dou-Mama Toi-même tu sais, fuck toutes ces petites pétasses qui ont l'trou d'balle large x4 Trop de lyrics et de shit dans ma chambre chambre Ça swingue swingue à souhait souhait, soin soin Ramène-nous les végétales, ouais les végétales Avec mon gava Phaal la fusion, c'est mode Vegetto Car c'est que des freestyles crades, rien à foutre de toutes ces 'tasses On va pas t'lâcher des... nan, on va t'lâcher que des flammes Sisisi toi-même tu sais, tu t'demandes si c'est légal Vu comment ça débite, faut qu'tu apprécies le flow du Mali, d'la Guinée et du Sénégal Philly Flingue, on les traite comme si c'était du bétail Ah ouais du bétail, genre un petit vache J'ai pas parlé français, SO le JBax Y'a pas de souci, on est posé, il faut qu'ça claque Vas-y ramène-moi de la weed, du shit ou d'la wax Si Phaal Philly s'mêle du shit alors c'est pour de vrai Donc R.E.P. Jean-Philippe Smet, car Tout l'monde, un jour va finir en Haut Philly Flingue, j'veux pas finir dans un motherfucking enclos Enclos, nan nan, rien à foutre de ces salauds qui veulent nous enfermer Ouais le landau, il est préparé pour eux Rien à foutre de la Place Vendôme et des Toi-même tu sais qu'j'ai mon nouveau bandeau J'arrive, j'récupère pas mon prix, j'envoie une meuf comme Marlon Brando aux Oscars Et j'suis un vrai négro, j'suis pas une fausse star On n'est pas des fausses stars, toujours en costard La beuh est dans l'pochtard Ok poto, j'balance un putain de d'xte-te Toi-même tu sais c'que j'fais Le vice est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenue dans l'pays des relations extra-conjugales Où ta femme et son amant festoient et baisent dans ton plumard Enlève ton autotune, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé' nous colle au cul Jamais de drogues dures hein, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Fais de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina chez Yass dans le Bronx Aïe, j'me rappelle de c'couplet à New York C'était plutôt pas mal, c'était vers la ligne Et c'est classe ouais, et j'ai le vice et j'ai la vertu Petite pause pshiiit, canette ouverture Philly Flingue, me tester tu sais que c'est perdu Oh merde, vas-y Doumamaf envoie l'truc Faut qu'j'envoie la verte, faut qu'j'envoie les bails Rien à foutre que je perde tant qu'j'suis avec mes frères Tu vois c'que j'veux dire on n'change pas une équipe qui perd Demande à Mekra, on va baiser toutes les paires Air plus fluide, il faut qu'je sois plus speed Qu'est-c'qui s'passe ? On les utilise comme des serpillières Eh toi-même tu sais, j'trafiquais avec des Serbes hier Et demain ce s'ra p't-être avec des Moldaves ou des Hongrois Ou des Hongrois, fuck c'qu'on croit Bonjour, bonsoir, tu sais qu'j'ai l'bon swag Philly Flingue au microphone donc j'repasse avec le bonjour J'ai mis un bandeau parce qu'il m'faut des contours Au Japon, j'sais pas qui peut m'faire le cut Hey, Philly Flingue en live de la Grünt5</t>
         </is>
       </c>
     </row>
@@ -1053,12 +1053,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Grünt Hors-Série 日本 🇯🇵 (Japon)</t>
+          <t>Encore</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Tout d'abord, j'en place une pour tout ceux qui sont partis trop tôt Force aux frolos, la vie, c'est comme un Loto Poto, ça va trop vite un jour, tu bédaves du popo Tu deviens claustro', le lendemain, ça s'ra l'hosto On n'a pas bibi par choix, ne l'oublie pas p'tit frère Maintenant qu'on est yo, on n'a plus b'soin d'ces choses, p'tit frère Pendant des années, en faisant du mal, j'ai fait du bien Fallait bien payer l'loyer, maintenant, c'est fini Y'en a très peu que j'considère comme mes grands frères Les liens du sang qui découlent de la grand-mère J'suis ni très vieux ni très pieux mais je sais quand m'taire Un gain de temps quand tu grandis dans la gangrène Obligé d'brûler cette substance pour trouver l'sommeil Ce monde est glauque, imagine un glock posé sur ton globe oculaire Sans aucune aide, c'est moi et ma chance Va-t-il trembler ou juste prendre l'blé ? La grande délinquance Implique des dangers, fils d'étrangers, j'veux gonfler ma panse Quoi d'autre, quoi d'autre, quoi d'autre ? Avant d'dompter la France Frère, on bédave comme si c'était légal mais c'est pas Me-da Des zones de non droit où les Hongrois cachent les murders Frère, c'est Paname et ses aléas On te banane si tu t'balades trop près de nos allées crades Niggiz, j't'ai dit c'est Paname et ses aléas Pour une garre-ba ou une kehba? ça s'canarde jusqu'au carnage Y'a pas d'partage avec ces sasa' J'les tabasse comme mon taga Doums alias Morgan pour les tagasses SuperSound niggiz, Seine Zoo c'est l'souk, call les cops niggiz J't'ai dit c'est SuperSound niggiz, Seine Zoo c'est l'souk, call les cops niggiz SuperSound niggiz, Seine Zoo c'est l'souk, call les cops niggiz Un vrai repère le Rap, y'a trop d'faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Ouais, 'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des seaux de larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme Ouais, c'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'je pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Solitaire qui traîne en bande, j'ai pas l'air sympathique En effet, c'est vrai j'aime pas la fée mais les fanatiques J'arrive tel un tsunami, fallait t'méfier d'l'eau qui dort Après avoir vu les filles défiler j'veux des los-ki d'or J'ai pas eu l'enfant du mec riche, plein de vices, très mal élevé Quand les vengeances du rire que le pardon pour les arrêter J'aime pas faire semblant, j'suis vrai, j'suis pas la honte de ma ruelle À croire qu'c'est en vendant du rêve que le tien deviendra réel J'm'appelle Mekra, j'suis né pour baffer les plafs Les faux frères, ouais, tout ces mecs la tous J'suis un félin femelle, on t'fera la fête Si t'as le boule bombé, ça f'ra l'affaire Ça a mal commencé comme un check raté Ça va mal finir comme une histoire de dette Si tu t'demandes où j'suis, j'suis dans ta tête le reste, c'est dépassé Les lignes sont pré-tracées Ils m'demandent c'est comment ? j'leur réponds tkt T'as quoi en plus une fois les nerfs passés ? J'vois des pantins éphémères s'bâcher Devenir mongol comme le kop de Fenerbahçe En bas d'chez moi, y'a plus de richesse depuis qu'c'est la crise Si tu t'demandais d'où venait mon cynisme et mon envie d'prêcher L'envie d'faire mieux et la haine dessinent des motifs Certains mélangent les deux, y trouvent la motiv' Un jour, on dira tous au revoir, on mettra pas d'emoji Avant laisse-moi l'temps d'arriver, j'suis juiced up, j'ai fait les modifs Cette bande de fake ass va danser l'lean-back Plus de putes que dans les Vine de King Bach Gros, y'a pas d'subli, y'a que des flip-flap Vingt milles lieues sous la merde dans la trixe-ma Dans la trix-ma, j'les graille comme un Kit Kat Flip-flap j'kick aç, c'est comme aç comme un dique-sa C'est Nek le Fenek j'prends le mic, improvise Avec mes gavas, tu sais qu'on atomise toutes ces salopes, c'est promis C'est quoi les dises ? Balance la suite mon gava faut qu'tu brûles les cliques J't'ai dit, on atomise j'aime pas quand les nanas tho-my, hein Baise ton anatomie, fuck les thos-my, j'prends le cro-mi C'est promis, ça r'vient j'suis comme un putain de cro-ma, et ouais j'les traumat' J'fais mon bail en direct du toit, qu'est-c'tu vois ? Fuck les lois, fuck toi Fuck tout ceux qui veulent pas comprendre que c'est nous, le putain de crew J'fais mes bails, j'fais des trous dans leurs curs de hum, aah C'est nous les rois, mais à quoi elles jouent, on les troue C'est tous des oufs, bellek là c'est l'crew de Doums Écoute les bails, on est posés, on est calmes Tu fais le fou, tu vas goûter quelques pas Ça va siffler dans ton oreille, c'est quoi les g's avec mes gavas, c'est toujours la même On est à Tokyo, freestyle Grünt, on va les baiser c'est des laisse et freine C'est quoi les g's, j'ai plus les mots, Ken l'a déjà dit les French OVO sur toutes ces hoes Laisse-nous faire les choses, c'est de l'impro Arrête de faire celui qu'a trop de flouze J'rappe, j'ai trop de flow, j'ai mon eau de source Tu vois bien que c'est toujours pour le Doums Tu vois bien que c'est toujours pour le crew Y'a Alpha qui arrive avec un banda rose Il fait ça pour tous les putains d'bandero C'est comme ça qu'je le fait, j't'ai vu bander kho C'est chelou, c'est comment qu'on l'fait ? J'fais le fric et j'vais pas d'mander trop, nan J'vais pas demander d'crocs, là y'a le nouveau kho On vient de débarquer dans l'bail, ça va être trop trop chaud C'est quoi le bail le Phall ? Est-c'que t'es prêt mon gars ? À balancer quelques impros, ouais pour tous les kho Sisisi, j'voulais aller au Mcdo, mais j'me suis paumé Donc j'suis allé chez dennis Nike pour la paire de Tennis, il frémissent Alph Lauren, toujours le vêtement qui hennit En fait la té-véri, c'est qu'j'ai monté les marches, donc j'suis encore essoufflé, hey Dans l'appart', hey, je vais séjourner, on va les shooter La carrière de ces wack MC's va être écourtée On va les découper avec les couplets ou avec les impros Sur le fil du rasoir, sur le fil du couperet C'est quoi les bails ? Il faut riposter On est prêts sur le bail avec le Feu C'est quoi les ? On va donner c'que l'on veut C'est vrai, il faut tripoter, il faut riposter, il faut tricoter, il faut hiphoper Il faut fricoter, même ricosser, j'suis un putain de Grec et aussi Ecossais Avec les vrais bitches, on va fricoter, toi-même tu sais, on est les types côtés Les rimes vont ricocher, on est pas les types cokés J'en place une pour l'cameraman au rik à love J'en place une pour Timothé, même si j'sais pas qui c'est J'en place une pour les biatchs qui sont team Hôtel Team hôtel, c'est facile on va les immoler Philly Flingue jamais de demi molle, j'arrive, pas d'mimolette Vas-y molo, c'est comme ça qu'on l'fait, pas de trémolo J'en place une pour mon frais, mon Lo', qui vient de partir J'en place une aussi pour les frémologues Les vrais frolos qui sont al' dans Tokyo Même air, L-I-S avec tous les kho Toi-même tu sais, toujours le crew à Tokyo On est tellement bien, on mange des sushis, on boit de l'eau bio Je flingue ta tête et j'vise tes lobes, yo J'viens te fumer un peu comme l'opium Et j'arrive comme Sébastien Loeb, yo Donc je finis sur le podium Dur de lire c'qu'y'a sur mes labialles, c'est la mafia Tellement d'style, on mange un plat de nouilles, on dirait qu'on mange du caviar Et tu t'agenouilles, bang bang, un tas de douilles Philly Flingue, Alph le Tigre, Alph le Loup, non jamais de paires de Afflelou Là, il raffle tout, c'est un freestyle ou des textes Tu t'demandes c'est quoi les dises, écoute les couz, on est les meilleurs, pas de coups de coudes On reste coude à coude Sisisi, que des impros pas de textes, on flex, avec ta futur motherfuckin ex Restaurant Tex Mex, en provenance d'une tasse qui vient de Aix-en-Provence Moi, j'viens du Nord de Paris, neuvième zone où je gravite Pour faire du biff, ça s'agite, black and white dans le sachet Pendant qu'tu dragues que des rousses moi, j'lui gratte des bouts d'clope Nous, c'est la Jack ou la ruskov, on niaxe sur le rooftop Pour atteindre le sommet, en équipe ça va d'soi Faut vesqui l'abattoir, quitte à en perdre le sommeil Avec deux-trois gavas, posés à Montmartre Il se fait tard, on est fêtard rien qu'ça féraille avec Fera, on est veinard yeah Toute la s'maine, tous les jours du mois ou toute l'année Tu veux un check ? Niggiz, touche du bois La mif comme moteur, coffre la fraîche Les flics arrivent si vite sur les hauteurs, nos regrets s'effritent avec le shit, motherfucker J'me suis trompé de pellicule, j'vois tout en négatif Et mon seul sédatif, c'est de recompter les thunes Pas facile d'être un artiste on charbonne, on est actif Après une tempête de sable, il faut remonter les dunes Je ne veux pas du monde à mes pieds Je veux que mon nom, tout le monde sache l'épeler Ouais, j'ai un train de vie de fêlé La vie, c'est pas la télé mais j'veux zapper quand ça me déplaît Ouais, j'vais pas rentrer dans l'détail mais on a plié de la féraille Que mon train de vie en déraille, yeah On m'avait dit dans tes rêves mais j'ai la tête dure Comme sur Twitter, toujours en TT Seul passager de mon train de vie Toujours plus vite retiens la devise Trop de bons souvenirs, le stockage est bientôt saturé Donc j'ai déjà zappé tout ce que je viens de vivre J'essaie de bien m'tenir mais c'est rien de l'dire Un homme qui n'agit pas, il n'y a rien de pire Tu prends de l'âge et ça tu ne le vois pas venir Le temps qui passe te fera breaker comme une feinte de tir Tu peux prononcer mon nom sauf si t'es devant un bleu Ils ont vu passer mon ombre comme la fumée dans le blunt J'ai dû prendre de l'ampleur quand j'ai vu qu'dans ses yeux il pleuvait Efficace dans le biz donc j'ai une emprise sur le plug On doit s'entendre sur les termes mais sinon gringo ça peut l'faire On veut du biff jusqu'au plafond, notre musique, c'est de la peuf' La came part en fumée, dans nos caves ou dans celle des stups Ce qui nous arrive c'est l'destin, on laisse les salles en feu, ouais Certains vivent dans l'passé, d'autres veulent vivre dans l'futur On vit l'instant présent, tous aux Zéniths pour le Feu Tour Ma vie, je la chante et le peuple la vit comme il l'entend Si t'attends ta chance, c'est sûrement qu'la peur sommeille en toi Pourquoi mon cur a-t-il sombré ? Quand j'leur pose la question, c'est juste pour savoir si ils sont vrais Même si on a fait du racket, je viens pas jouer les durs à cuire Beaucoup ont dû raquer, j'suis dans les histoires dures à croire Bébé, je reste en ville que pour quelques jours Je veux lire mon nom sur tes lèvres douces J'veux que t'écoutes ce son et que tes fesses bougent Et qu'on amène le bendo dans les fêtes de bourges J'attrape la Mustang par la crinière Décapotable, j'ai le vent comme soin capillaire Monte du côté passager mais fais-toi discrète Tu m'dis que t'aimes flirter bien que tu sois fidèle Tu tiens le volant pendant que je roule mon spliff Je te dis que tu m'attires et que t'es plutôt mon style Ma fierté m'aura p't-être un jour J'préfère ça que de vivre à genoux J'suis pas comme vous, non, j'suis pas un gnou Quand la coupe est pleine, on plaide la self-défonce Ouais l'affreux, j't'efface, en un quart de s'conde J'viens d'passer l'quart de siècle toujours la même routine J'me mets à faire du sport, j'arrête la semaine d'après J'fume la verte, l'amnes' pour oublier mes soucis Et j'en ai beaucoup, frérot, oui, j'en ai beaucoup Ça chauffe, c'est l'insolation mais c'est pas l'Afghanistan J'te bibi ta consommation pour toi, c'est comme un talisman Pas de deuxième sommation, la soumission s'ra la seule issue La solution, c'est l'khaliss mais c'est salissant Même les voleurs ont des valeurs À Paris centre, Paris centre, Paris J'te dis que même mes voleurs ont des valeurs À Paris centre, Paris centre, Paris J'irai haut comme une montgolfière Maman, t'auras la clé des coffres, tu remonteras mon col, fière Demain, on va jouer au golf, après-demain on dira qu'on a joué au golf hier J'vais pas sauver l'monde et le monde va pas m'sauver On s'remplit comme nos ventres, froid comme novembre J'ai grandi dans les orties, j'les sens plus Hey, on est dans l'truc, le gang est de sortie Tiser des litres, sniffer des lignes ? Nan Prendre des drogues aux effets psychédéliques ? Nan J'vais expliquer l'délire niquer l'élite Qui a gardé le fric et les livres ? On fraudait déjà l'bus au C.P. vu qu'nos C.V. sont vides Hey, vu qu'nos C.V. sont vides J'oublie mon texte et j'reviens avec dou-Mama, on fait le feat On glisse sur l'instru de Mad Skillz Car j'ai beaucoup d'lyrics et de shit dans la chambre Y'a du chrome sur les jantes, négro Eh, c'est comme ça qu'on voit l'motherfucking futur Faut qu'le truc dure Mes motherfucking impro sont comme un motherfucking boa constrictor au niveau d'la structure Car il n'y en a pas, le truc est infini, balance un vinyle Hey, qu'on l'fasse tourner, Philly Flingue, j'ai fumé plein d'phillies Blunt, j'ai fumé plein d'phillies blunt J'ai fumé plein d'phillies blunt, plein d'phillies blunt x4 Trop de lyrics et de shit dans ma chambre chambre Ça swingue swingue à souhait souhait, soin soin Ah cette prod, on l'a kickée maintes fois avec Phaal Rien à foutre que ces salopes sont nymphos et Ça n'm'intéresse pas, j'aime pas trop les folles Avec mes gavas en impro, rien qu'on décolle On décolle, on décolle comme les profits J'suis au Mont Fuji, je bois du blended coffee C'est comme ça qu's'appelle la motherfucking canette J'veux faire de la maille comme Michael et Janet De la maille comme Michael et Janet ou bien Danette Rien à foutre d'ces salopes, moi, j'suis pas de la même planète J'fume que du brocolis, on dirait un Namek Nan, j'suis trop chaud, j'suis comme Broly, nique ta mère Sisisi c'est pour les faux khos, non c'est pour les vrais zins On est au Mont Fuji, on boit des canettes de Fanta raisin En fait, mon faux vaut plus d'cent balles Avant, c'était une canette et maintenant, c'est plus qu'un cendar Car tout se construit et se re-transforme Philly Flingue au microphone, tu sais, oui, je suis en forme J'avance avec dou-Mama Toi-même tu sais, fuck toutes ces petites pétasses qui ont l'trou d'balle large x4 Trop de lyrics et de shit dans ma chambre chambre Ça swingue swingue à souhait souhait, soin soin Ramène-nous les végétales, ouais les végétales Avec mon gava Phaal la fusion, c'est mode Vegetto Car c'est que des freestyles crades, rien à foutre de toutes ces 'tasses On va pas t'lâcher des... nan, on va t'lâcher que des flammes Sisisi toi-même tu sais, tu t'demandes si c'est légal Vu comment ça débite, faut qu'tu apprécies le flow du Mali, d'la Guinée et du Sénégal Philly Flingue, on les traite comme si c'était du bétail Ah ouais du bétail, genre un petit vache J'ai pas parlé français, SO le JBax Y'a pas de souci, on est posé, il faut qu'ça claque Vas-y ramène-moi de la weed, du shit ou d'la wax Si Phaal Philly s'mêle du shit alors c'est pour de vrai Donc R.E.P. Jean-Philippe Smet, car Tout l'monde, un jour va finir en Haut Philly Flingue, j'veux pas finir dans un motherfucking enclos Enclos, nan nan, rien à foutre de ces salauds qui veulent nous enfermer Ouais le landau, il est préparé pour eux Rien à foutre de la Place Vendôme et des Toi-même tu sais qu'j'ai mon nouveau bandeau J'arrive, j'récupère pas mon prix, j'envoie une meuf comme Marlon Brando aux Oscars Et j'suis un vrai négro, j'suis pas une fausse star On n'est pas des fausses stars, toujours en costard La beuh est dans l'pochtard Ok poto, j'balance un putain de d'xte-te Toi-même tu sais c'que j'fais Le vice est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenue dans l'pays des relations extra-conjugales Où ta femme et son amant festoient et baisent dans ton plumard Enlève ton autotune, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé' nous colle au cul Jamais de drogues dures hein, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Fais de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina chez Yass dans le Bronx Aïe, j'me rappelle de c'couplet à New York C'était plutôt pas mal, c'était vers la ligne Et c'est classe ouais, et j'ai le vice et j'ai la vertu Petite pause pshiiit, canette ouverture Philly Flingue, me tester tu sais que c'est perdu Oh merde, vas-y Doumamaf envoie l'truc Faut qu'j'envoie la verte, faut qu'j'envoie les bails Rien à foutre que je perde tant qu'j'suis avec mes frères Tu vois c'que j'veux dire on n'change pas une équipe qui perd Demande à Mekra, on va baiser toutes les paires Air plus fluide, il faut qu'je sois plus speed Qu'est-c'qui s'passe ? On les utilise comme des serpillières Eh toi-même tu sais, j'trafiquais avec des Serbes hier Et demain ce s'ra p't-être avec des Moldaves ou des Hongrois Ou des Hongrois, fuck c'qu'on croit Bonjour, bonsoir, tu sais qu'j'ai l'bon swag Philly Flingue au microphone donc j'repasse avec le bonjour J'ai mis un bandeau parce qu'il m'faut des contours Au Japon, j'sais pas qui peut m'faire le cut Hey, Philly Flingue en live de la Grünt5</t>
+          <t>S-Crew, boy, sur du Screwball Écoute ça, Candy Cotton Happy Face Record, 1.9.9.5, encore une fois, mon gars Balance un autre joint ×3 N'écoute pas les autres MC's, c'est d'la fumée aux yeux Voici le seul et unique freestyle numéro 2 Mon cur a payé la facture, j'ai des fractures et on m'a dit sheh ! Mais je vais m'acharner comme l'état sur les romanichels Je t'assure on traumatise sec, t'as vu, l'euro m'a mis cher J'me répands sur YouTube comme un virus informatique, mec Pas le format type, moi, j'suis de l'école de IV My People Pas d'automatique, poto, ma clique supporte ma petite gueule J'ai de l'amour pour les frères, si tu veux m'parler, je t'écoute Mais si t'insultes, j'fais comme ta mère J'irai te chercher après les cours Tu te demandes C'est qui ce mec qui kicke avec ses tifs longs ? Qui glisse des disquettes aux filles qui visent les biftons ? Nek de l'Entourage, gars, sache qu'on m'emboucane pas Tu clashes mais, matte les wacks Je les frappe comme San Ku Kai, man Pas un grand toubab mais, en tout cas Je rentre tout-par parce que mon crew rappe Pendant qu'tu parles mal devant l'ouvrage Stupide, oh, tu parles dans le dos, quand je passe, tu dis Yo J'fais des freestyles vidéos parce qu'on a pas d'studio Je confonds mes rêves et mes souvenirs Les yeux fermés n'ont qu'à s'ouvrir Mes cauchemars ressemblent souvent Aux films de Mathieu Kassovitz Ça s'est de la tuerie, mon gars sûr, 2Zer Washington Je t'assure, pour nous, c'est pas dur de s'faire ta pine-co Si y'a des coccyx brisés, j'suis à proximité C'est Nek le Fennek envoyé par Zoxea, j'y vais J'suis c'toubab qui se sépare du game, yeah C'est Boom Back façon Sëar lui-même Quand la foudre part, c'est juste le S-Crew qui rappe Moi, j'rappe comme les cains-ri, j'fais rimer les sous titrages quoi...2</t>
         </is>
       </c>
     </row>
@@ -1070,12 +1070,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Encore</t>
+          <t>Comme ça</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>S-Crew, boy, sur du Screwball Écoute ça, Candy Cotton Happy Face Record, 1.9.9.5, encore une fois, mon gars Balance un autre joint ×3 N'écoute pas les autres MC's, c'est d'la fumée aux yeux Voici le seul et unique freestyle numéro 2 Mon cur a payé la facture, j'ai des fractures et on m'a dit sheh ! Mais je vais m'acharner comme l'état sur les romanichels Je t'assure on traumatise sec, t'as vu, l'euro m'a mis cher J'me répands sur YouTube comme un virus informatique, mec Pas le format type, moi, j'suis de l'école de IV My People Pas d'automatique, poto, ma clique supporte ma petite gueule J'ai de l'amour pour les frères, si tu veux m'parler, je t'écoute Mais si t'insultes, j'fais comme ta mère J'irai te chercher après les cours Tu te demandes C'est qui ce mec qui kicke avec ses tifs longs ? Qui glisse des disquettes aux filles qui visent les biftons ? Nek de l'Entourage, gars, sache qu'on m'emboucane pas Tu clashes mais, matte les wacks Je les frappe comme San Ku Kai, man Pas un grand toubab mais, en tout cas Je rentre tout-par parce que mon crew rappe Pendant qu'tu parles mal devant l'ouvrage Stupide, oh, tu parles dans le dos, quand je passe, tu dis Yo J'fais des freestyles vidéos parce qu'on a pas d'studio Je confonds mes rêves et mes souvenirs Les yeux fermés n'ont qu'à s'ouvrir Mes cauchemars ressemblent souvent Aux films de Mathieu Kassovitz Ça s'est de la tuerie, mon gars sûr, 2Zer Washington Je t'assure, pour nous, c'est pas dur de s'faire ta pine-co Si y'a des coccyx brisés, j'suis à proximité C'est Nek le Fennek envoyé par Zoxea, j'y vais J'suis c'toubab qui se sépare du game, yeah C'est Boom Back façon Sëar lui-même Quand la foudre part, c'est juste le S-Crew qui rappe Moi, j'rappe comme les cains-ri, j'fais rimer les sous titrages quoi...2</t>
+          <t>Hé, c'est toi Neslet ? Hé franchement, j'kiffe c'que tu fais J'adore ton travail tout ça Ça fait penser à Matthieu Kassovitz, Kourtrajmé Tout ça, c'est la même chose franchement Hé tu connais pas 2zer ? Tu connais pas 2zer ? Hé tu connais pas 2zer ? Tu connais pas 2zer ? C'est quoi les bails ? C'est quoi les bails ? OK, 2-Zer Toi même tu sais comment ça aif', mon pote OK, dans ma vie, pff... J'en ai fait des erreurs Plein, plein, plein... OK Mais ma plus grosse erreur C'est de n'pas suivre l'exemple que mes parents m'montrent Puis j'ai compris qu'à part eux pour m'soutenir, y'avait pas grand monde J'vis dans le passé, j'm'en bats les couilles de la mode contemporaine Si mon ex-meuf refait sa vie, j'serai jamais content pour elle Ma vie c'est un croquis mal dessiné, j'en ai marre du ciné J'dois suivre ma destinée et combler ma dulcinée J'suis comme mon frère, on est dans l'vent, on a l'cerveau climatisé Et quand ça gueule j'suis dans l'espace, j'entends pas les cris d'ma fusée Moi, j'suis du-per depuis qu'la maladie a attrapé Maman C'est là qu'le destin m'a mis à terre et m'a frappé malement J'verse une larme, là, quand j'prie, moi j'suis trop incompris Pourtant j'parle français, c'est pas comme si je rappais l'allemand J'veux finir en terre promise mais ces bâtards me laissent trimer J'voudrais dire Je t'aime trop, miss mais j'ai du mal à l'exprimer Le bonheur ça dure deux secondes dans n'importe quelle situation J'pense qu'on devrait m'écouter, ouais, t'es un bon si tu as l'son X2 La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents Les gens, ça va, ça vient Tous les jours tu fais de bonnes ou de mauvaises rencontres Choisis bien ceux qui tentourent Observe bien, écoute bien c'quils disent Ne reste jamais dans un endroit où tu tsens mal à laise Jamais, non ! Les gens savent mentir donc apprends à mentir aussi Tout est éphémère Tout, tout, tout, tout... Même lamour et lamitié, frère... Malheureusement... Écoute ça, écoute ça... Donc si t'as pas les boules, dégage avant que mes gars t'les mettent Moi, j'bicrave, c'est bien ! Nan, en fait, je gratte les miettes Mon flow est alléchant, crois-en tes papilles gustatives Faut que j'sois actif, pour l'instant j'connais pas d'vie plus statique Moi, sans renoncer j'arpente les rues d'la capitale J'dois, remonter la pente c'qui est dans mon cas vital J'vois ma vie de l'extérieur, j'suis impuissant comme un soixantenaire Faut qu'j'sois sans colère face à ceux qui s'barrent quand ça sent l'tonnerre Si j'avais pu, j't'aurais dit l'mot Je t'aime et tous ses synonymes Mais tu t'fous de ma gueule, on apprend pas l'langage des signes aux mimes J'ai recollé les morceaux donc les pots ne devraient plus s'casser Nan, j'me vois pas aux puces taffer mais d'ma vie j'en ai plus qu'assez Putain, avec le temps les problèmes auraient dû s'tasser J'veux p'tit dèj' croissant plus café et l'soir grailler des crustacés 2-Zer Washington... C'est comme ça que les chacals m'appellent J'kiffe quand l'Entourage m'encourage, c'est c'qui fait que j'garde la pêche X2 La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents Hahahaha, 2-Zer ! Les gens, ça va, ça vient Tu connais t'façon, pas besoin d't'expliquer OK La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents8</t>
         </is>
       </c>
     </row>
@@ -1087,12 +1087,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Comme ça</t>
+          <t>Ma force</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Hé, c'est toi Neslet ? Hé franchement, j'kiffe c'que tu fais J'adore ton travail tout ça Ça fait penser à Matthieu Kassovitz, Kourtrajmé Tout ça, c'est la même chose franchement Hé tu connais pas 2zer ? Tu connais pas 2zer ? Hé tu connais pas 2zer ? Tu connais pas 2zer ? C'est quoi les bails ? C'est quoi les bails ? OK, 2-Zer Toi même tu sais comment ça aif', mon pote OK, dans ma vie, pff... J'en ai fait des erreurs Plein, plein, plein... OK Mais ma plus grosse erreur C'est de n'pas suivre l'exemple que mes parents m'montrent Puis j'ai compris qu'à part eux pour m'soutenir, y'avait pas grand monde J'vis dans le passé, j'm'en bats les couilles de la mode contemporaine Si mon ex-meuf refait sa vie, j'serai jamais content pour elle Ma vie c'est un croquis mal dessiné, j'en ai marre du ciné J'dois suivre ma destinée et combler ma dulcinée J'suis comme mon frère, on est dans l'vent, on a l'cerveau climatisé Et quand ça gueule j'suis dans l'espace, j'entends pas les cris d'ma fusée Moi, j'suis du-per depuis qu'la maladie a attrapé Maman C'est là qu'le destin m'a mis à terre et m'a frappé malement J'verse une larme, là, quand j'prie, moi j'suis trop incompris Pourtant j'parle français, c'est pas comme si je rappais l'allemand J'veux finir en terre promise mais ces bâtards me laissent trimer J'voudrais dire Je t'aime trop, miss mais j'ai du mal à l'exprimer Le bonheur ça dure deux secondes dans n'importe quelle situation J'pense qu'on devrait m'écouter, ouais, t'es un bon si tu as l'son X2 La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents Les gens, ça va, ça vient Tous les jours tu fais de bonnes ou de mauvaises rencontres Choisis bien ceux qui tentourent Observe bien, écoute bien c'quils disent Ne reste jamais dans un endroit où tu tsens mal à laise Jamais, non ! Les gens savent mentir donc apprends à mentir aussi Tout est éphémère Tout, tout, tout, tout... Même lamour et lamitié, frère... Malheureusement... Écoute ça, écoute ça... Donc si t'as pas les boules, dégage avant que mes gars t'les mettent Moi, j'bicrave, c'est bien ! Nan, en fait, je gratte les miettes Mon flow est alléchant, crois-en tes papilles gustatives Faut que j'sois actif, pour l'instant j'connais pas d'vie plus statique Moi, sans renoncer j'arpente les rues d'la capitale J'dois, remonter la pente c'qui est dans mon cas vital J'vois ma vie de l'extérieur, j'suis impuissant comme un soixantenaire Faut qu'j'sois sans colère face à ceux qui s'barrent quand ça sent l'tonnerre Si j'avais pu, j't'aurais dit l'mot Je t'aime et tous ses synonymes Mais tu t'fous de ma gueule, on apprend pas l'langage des signes aux mimes J'ai recollé les morceaux donc les pots ne devraient plus s'casser Nan, j'me vois pas aux puces taffer mais d'ma vie j'en ai plus qu'assez Putain, avec le temps les problèmes auraient dû s'tasser J'veux p'tit dèj' croissant plus café et l'soir grailler des crustacés 2-Zer Washington... C'est comme ça que les chacals m'appellent J'kiffe quand l'Entourage m'encourage, c'est c'qui fait que j'garde la pêche X2 La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents Hahahaha, 2-Zer ! Les gens, ça va, ça vient Tu connais t'façon, pas besoin d't'expliquer OK La roue tourne plus que rapidement, j'suis pas happy devant Celle qui revend les sentiments et à prix dément J'ai couru après l'démon, pourquoi j'ai pas pris l'devant ? Ce bâtard a pris plus de vies qu'il n'a pris de vents8</t>
+          <t>2zer Washington Parlez-vous cefran? Hein, hein, parlez-vous cefran? DJ noise -crew boyyyy, tu connais les bails Personne ne peut stopper ma force Mais j'vous cache ma rage Comme tous mes côtés atroces et où j'passe à l'acte Mais tout ça, ça marque On n'résout pas sa life En jouant l'toréador Les coups partent, bâtard Rappelle-moi tous tes coups ratés Quand l'état voulait nous fater La vendetta de mes fous à lier Double ge-ra à défourailler J'ai coulé d'la marchandise Depuis j'me suis attendri Pour pas que le maton m'dise Tenez-vous droit, venez vous laver J'ai la force H24 sous adrénaline J'ai toujours la gouache sans mettre de poudre à mes narines J'veux soulager ma vie sans outrager la rime J'ai la force pour taffer la nuit Quand vous allez dormir On est d'accord Framal Apportez l'fric, là j'vais saboter l'biz Trop paro j'débite Que des sales projets, approchez Là j'promets, droite, gauche, et Nekfeu arme soviétique ! En guise de rime, en titre de chemise J'enfile mon jean rempli d'centimes Et gratte ce rap trop technique La prose est clean, j'tape trop de spliff Là je t'assomme ? ? Nekfeu que des balles trop précises ! J'ai le sabre dans la gorge Mec, prends garde, j't'encastre Il m'faut du cash dans la pocket J'veux des thunes d'apache Déçu d'la life, toi tu cé-su J't'exécute à l'épluche-patate Mékra Seine zoo dans les bacs Y'a pas d'nana dans mon équipe que des ? On a la rage d'un Apache Toi t'as la bouche ouverte Faudra nachave, prendre un appart' Et ça à toute vitesse J'rappe sous ivresse, quoi tu m'crois pas? ? Hey, nique les strass et les paillettes Moi j'suis ? j'ai les manières D'un soc' ? Ecoute mon clan, on arrive On va couler l'bateau des traîtres Tu veux prendre ton tarif Ca va t'coûter la peau des fesses, ma miss On est frais, bah oui Ca c'est pour mes frères d'Afrique On a tous été trahis Par toutes ces ? hemi Et tu m'verras, toujours partant pour les re-frè Nekfeu Pas l'temps pour les regrets, hein J'suis posé sans contrainte, à cent contre un J'attends pas l'embonpoint J'arrête de rapper mes textes dans mon coin Avec ma tête de fennec j'suis scred' Donc quand je squatte des quartiers chics J'écarte les cuisses des femelles du 16 On reste vrais grâce à nos actes On a nos façons d'voir le rap Pas d'casanova, tu faisais quoi à notre âge, mon gars? Arrête de rager, vu? Ici, c'est ris-Pa J'suis pas l'élu juste un p'tit gars muni de ses 10 doigts Et quoi qu'tu dises on s'est fait connaître sans radio Moi, j'suis un artiste pas comme tes collègues en major Il faut que le message s'exporte Pour qu'les petits frelons kiffent le son La vie, c'est pas que ? Je kick pour le freestyle Pire encore, fist Ma vie est un 2zer freestyle qui m'renforce ? Je kick pour le freestyle Pire encore, fist Ma vie est Mékra un freestyle qui m'renforce Hein, parlez-vous cefran? Seine zoo, allez-vous ser-dan? Check, check, l'entourage bébé</t>
         </is>
       </c>
     </row>
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Ma force</t>
+          <t>On est ensemble</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2zer Washington Parlez-vous cefran? Hein, hein, parlez-vous cefran? DJ noise -crew boyyyy, tu connais les bails Personne ne peut stopper ma force Mais j'vous cache ma rage Comme tous mes côtés atroces et où j'passe à l'acte Mais tout ça, ça marque On n'résout pas sa life En jouant l'toréador Les coups partent, bâtard Rappelle-moi tous tes coups ratés Quand l'état voulait nous fater La vendetta de mes fous à lier Double ge-ra à défourailler J'ai coulé d'la marchandise Depuis j'me suis attendri Pour pas que le maton m'dise Tenez-vous droit, venez vous laver J'ai la force H24 sous adrénaline J'ai toujours la gouache sans mettre de poudre à mes narines J'veux soulager ma vie sans outrager la rime J'ai la force pour taffer la nuit Quand vous allez dormir On est d'accord Framal Apportez l'fric, là j'vais saboter l'biz Trop paro j'débite Que des sales projets, approchez Là j'promets, droite, gauche, et Nekfeu arme soviétique ! En guise de rime, en titre de chemise J'enfile mon jean rempli d'centimes Et gratte ce rap trop technique La prose est clean, j'tape trop de spliff Là je t'assomme ? ? Nekfeu que des balles trop précises ! J'ai le sabre dans la gorge Mec, prends garde, j't'encastre Il m'faut du cash dans la pocket J'veux des thunes d'apache Déçu d'la life, toi tu cé-su J't'exécute à l'épluche-patate Mékra Seine zoo dans les bacs Y'a pas d'nana dans mon équipe que des ? On a la rage d'un Apache Toi t'as la bouche ouverte Faudra nachave, prendre un appart' Et ça à toute vitesse J'rappe sous ivresse, quoi tu m'crois pas? ? Hey, nique les strass et les paillettes Moi j'suis ? j'ai les manières D'un soc' ? Ecoute mon clan, on arrive On va couler l'bateau des traîtres Tu veux prendre ton tarif Ca va t'coûter la peau des fesses, ma miss On est frais, bah oui Ca c'est pour mes frères d'Afrique On a tous été trahis Par toutes ces ? hemi Et tu m'verras, toujours partant pour les re-frè Nekfeu Pas l'temps pour les regrets, hein J'suis posé sans contrainte, à cent contre un J'attends pas l'embonpoint J'arrête de rapper mes textes dans mon coin Avec ma tête de fennec j'suis scred' Donc quand je squatte des quartiers chics J'écarte les cuisses des femelles du 16 On reste vrais grâce à nos actes On a nos façons d'voir le rap Pas d'casanova, tu faisais quoi à notre âge, mon gars? Arrête de rager, vu? Ici, c'est ris-Pa J'suis pas l'élu juste un p'tit gars muni de ses 10 doigts Et quoi qu'tu dises on s'est fait connaître sans radio Moi, j'suis un artiste pas comme tes collègues en major Il faut que le message s'exporte Pour qu'les petits frelons kiffent le son La vie, c'est pas que ? Je kick pour le freestyle Pire encore, fist Ma vie est un 2zer freestyle qui m'renforce ? Je kick pour le freestyle Pire encore, fist Ma vie est Mékra un freestyle qui m'renforce Hein, parlez-vous cefran? Seine zoo, allez-vous ser-dan? Check, check, l'entourage bébé</t>
+          <t>Yeah, Zerzer Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour ds choses abominables, sèche ms larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais ZerZer volume 1 dispo partout la miff' DJ Élite aux platines Eh, eh Ok, ok, yeah Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Nique ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce gosse en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Brrrr Comme d'habitude, Hugz à la prod Eh, eh, eh Depuis l'époque de Décisions Yeah, yeah, yeah Han, han, Zerzer Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Ok, yeah, yeah, yeah Ça, c'est pour les anciens, ceux qui étaient là depuis l'époque Eh, eh Yeah Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie Yeah, yeah, yeah, yeah Ok, Reeko à la prod Hahaha, tu connais les bails Ouais, ouais, yeah Eh L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais Wooouh ! Han, han Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Yeah, yeah Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woouuh, -Crew, 2zer, Framal Brrraaa Brreh, brreh, brreh, brreh Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Letsguill ! Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Letsguill, Letsguill Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle 2zer Washington Ça sent la lorage, ca sent laverse jsuis dans ma tête Saboteurs Je ne bouge pas' jattends quca vienne Eh, eh, eh Sur le droit chemin, en sens inverse Grozomozo, Ratu, Saboteur gang Yeah, yeah, yeah Letsguill DJ Elite, balance la suite Han, han, tu connais Toujours la même, rien n'a changé Toujours les mêmes ons-s, toujours la même cons', eh Ouais, toujours les mêmes têtes Blackbird, Saboteur, Seine Zoo Hugz, ça dit quoi mon pote ? J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Eh, Grünt, sisi Han, han, ZerZer volume 1, dispo partout la miff' Yeah, han, han, han Saboteur gang, Seine Zoo Saboteur gang, Seine Zoo Hugz, ça dit quoi ? Yeah</t>
         </is>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>On est ensemble</t>
+          <t>Du monde en Freestyle dans le Planète Rap de Nekfeu</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Yeah, Zerzer Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour ds choses abominables, sèche ms larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais ZerZer volume 1 dispo partout la miff' DJ Élite aux platines Eh, eh Ok, ok, yeah Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Nique ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce gosse en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Brrrr Comme d'habitude, Hugz à la prod Eh, eh, eh Depuis l'époque de Décisions Yeah, yeah, yeah Han, han, Zerzer Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Ok, yeah, yeah, yeah Ça, c'est pour les anciens, ceux qui étaient là depuis l'époque Eh, eh Yeah Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie Yeah, yeah, yeah, yeah Ok, Reeko à la prod Hahaha, tu connais les bails Ouais, ouais, yeah Eh L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais Wooouh ! Han, han Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Yeah, yeah Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woouuh, -Crew, 2zer, Framal Brrraaa Brreh, brreh, brreh, brreh Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Letsguill ! Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Letsguill, Letsguill Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle 2zer Washington Ça sent la lorage, ca sent laverse jsuis dans ma tête Saboteurs Je ne bouge pas' jattends quca vienne Eh, eh, eh Sur le droit chemin, en sens inverse Grozomozo, Ratu, Saboteur gang Yeah, yeah, yeah Letsguill DJ Elite, balance la suite Han, han, tu connais Toujours la même, rien n'a changé Toujours les mêmes ons-s, toujours la même cons', eh Ouais, toujours les mêmes têtes Blackbird, Saboteur, Seine Zoo Hugz, ça dit quoi mon pote ? J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Eh, Grünt, sisi Han, han, ZerZer volume 1, dispo partout la miff' Yeah, han, han, han Saboteur gang, Seine Zoo Saboteur gang, Seine Zoo Hugz, ça dit quoi ? Yeah</t>
+          <t>Même si t'as tout fait pour les gens A la moindre dispute, ils oublieront Déçu de ceux qui rampent On veut d'la soupe, il faut des sous qui rentrent C'est l'souk, j'veux pas d'une zouz exubérante qui zouke Sinon, j'devrai couper le souffle aux soupirants Ils m'supplieront d'les épargner mais j'suis pas économe Hey, connards, laissez parler les vrais bonhommes Tu sais, tant qu'un frère a du cur, j'ai rien à foutre de ses stats' On a passé l'stade de s'demander qui sait s'tape On s'estime et les doutes s'estompent J'suis pas assez stable, sista, cesse donc d'envier ces stars Au fond du trou, à part le Ciel, tu veux qu'j'me tourne vers qui ? Envie d'repartir à zéro comme un converti Le traître négocie les trêves, le journaliste grossit les traits Comme un coké, que connait-il D'la philosophie des gosses illettrés ? Sait-il c'qu'il s'passe chaque fois qu'un petit s'fait renvoyer ? Connaît-il la souffrance de l'enfance De mes petites surs en foyer, hein ?! Comme mon homonyme, des cicatrices, j'en ai bezef Même avec les cordes vocales coupées, je serai un mec de parole J'me retourne dans mon lit en m'demandant si j'dois les baiser Vu qu'la nuit porte conseil, j'me lève avec le barreau Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y a des seaux de larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots J'crois bien que le danger vient de mes proches Rien ne m'étonne tout c'qui m'entoure n'est qu'un simple décor Craindre l'effort ce n'est pas pour moi donc je blinde mes forces Poto, tu pues la défaite Tout c'que j'peux faire, c'est plaindre tes gosses A force de manier l'argent sale, j'commence à m'en laver les mains C'est un nouveau départ dans l'Rap On va embrasser le destin J'compte plus le nombre de fois Que j'me pète la tête et m'défonce le foie Mec, j'arrête de faire la fête Avec ma secte, on est fonces-dé le soir S - C.R.E.W Tous ces mecs illettrés rêvent de nous bluffer Le vice peux m'taper dans lil donc j'abaisse pas ma garde La vie un long fleuve tranquille qu'on traverse à la nage Les man, à vos phases, voilà Nekfeu, partez Pétasse, allez, twerke, bouge ton bête de tard-pé C'est E.2.F, ne tente pas d'contrer 7.5.0.19 si tu cherches la contrée Pompez, pompez, pompez, c'est le L Que des flammes bleues, appelle les pompiers Nekflamme, Bazz, Flav', Deen 2zer, Alpha, Doums Mekra, Framal, Gee On est là pour longtemps Faut qu't'achètes Feu si tu veux payer comptant On fait des erreurs mais, quand on chante On est les meilleurs même quand on s'branle Nique toutes vos notions d'loi, bitch Du plus profond d'moi, je veux finir au plus profond d'toi On terminera l'parcours à la morgue Mais avant ça, on est revenus mettre les babtous à la mode Trop d'actions, peu de débats, l'avenir Mais la patience est une vertu que peu Depuis tout petit, 2015, l'année du L, bientôt le Jour Gee C'est facile de les faire rager, ouais, ça, j'sais l'faire J'arrive avec les Versace et les sachets verts Vous êtes tous gâtés, bande de merdeux du net A travers ma paire de lunettes Cartier, j'vois des lunes écartées Double scotch, j'ouvre le score quand mon équipe rentre Le toit est en feu, le sol brûle, ma clique flambe Les gens nous guettent et n'veulent ap' s'ambiancer Ils veulent connaitre nos raps, nos sapes Nos placements financiers Fuck toutes ces débilités d'espionnage Notre crédibilité n'est même pas questionnable Nique les normes, on cherche des deals énormes Dis aux hyènes de déclarer forfait, j'suis là pour un millenium J'ai bien dit un millenium, dès qu'ça parle argent Ils ont des voix bizarres, c'est comme s'ils avaient prit de l'hélium Faut qu'on les plume vite, colors Don Dada On va faire tomber les colosses, yeah Je culmine, ils pourront ap' me battre On pratique le rap de patron Anti-personnel comme une mine J'suis boss, pas intérimaire Quand j'suis dans l'périmètre y'a que des playmates J'écris plus de refrains, j'peins à l'instinct A 25 piges, j'ai déjà signé 25 eins' Nekfeu, c'est le Planète Rap Philly Flingue au microphone, personne arrêtera Y'a pas d'problème quand c'est le Planète Rap Tu sais qu'c'est Mekra, tu sais que personne l'arrêtera C'est Mekra, l'mec rare au micro, parlez pas d'bédave, je picole J'suis qu'un brave qu'a pas d'biff, j'te fais khaf comme à Rio J'suis pas black ni latino, j'suis un bicot qu'a la dalle A c'qui paraît, tous ces mythos passent des kilos par la douane Rien dans l'frigo, y'a pas d'maille, on veut chill au Panama Piner J-Lo, s'il faut killer l'beat, mon stylo gratte un max M.E.K.R.A, et t'as mé-cra cette putain d'caille-ra Ça ira, j'suis faya, pas d'mariage, on salira la Zaia De Paris à Bahia, on a l'image de cannibale Et c'est khatal tah Al-Qaïda Et t'as pas idée, à ris-Pa on a des qualités Le barillet fait baliser tes p'tits, ils restent tétanisés Le sale diable va t'habiter si t'as pas la gnaque, il sait J'travaille mes patates sur un sac à la salle, j'y vais J'ai plein d'buts mais pas d'marques et pas d'thunes, c'est la life J'veux une Féfé, j'ai un PC, j'suis pas une pute, j'ai pas d'MAC Et mate ma démarche de barge, savoir ne pas parler De tes bails, c'est un choix, crois-moi, c'est pas gagné Sale tass, tu parles mal, j't'avais dit, y'a pas d'amour à Paname Donc pas besoin de t'attacher Pas que les gallons, tacle les gars qui jactent et ça bédave, petit T'es tarté, les balles te visent, fais l'chaud et attends-toi au mieux A l'aise, j't'éclate le pif, j'suis chaud donc j'ai pas froid aux yeux J'ai pas froid aux yeux Encore un soir où je tente d'écrire mais ma page reste blanche Peu d'inspi, le ventre vide, il m'reste un sachet à vendre J'me dirige vers le 6, là bas un los-bar m'attend J'vais m'remplir le bide et l'frigo devant la porte On se voit, on monte chez Los', la transaction se passe en balle Puis j'fonce dans l'trom', rejoindre tous mes gars en bas Ça roule des cônes ou plutôt, devrais-je plutôt dire des battes Goûte cette dope qui me fait relativiser La cam c'est mal, on l'sait tous mais cela dit j'y vais Fuck tes probabilités, je tenterais ce pari risqué Il m'faut des pepettes pour graille, j'suis pas du style lève tôt J'garde ma conscience pour moi donc fais de même, frérot Petit toine-An a fait ses classes au mic, gentil mais pas naïf Pas du genre à perdre une occas' de faire de la maille Pas du genre à gémir, à fléchir ou à s'taire A frémir, depuis mes seize balais, j'prépare la guerre Me compare pas à tes assoces, mec, j'suis au-dessus Car j'ai la vision, l'ambition, la tech, maitrise le processus Clic-clic-boom, l'offensive est lancée C'est L'Entourage, couz, sur un ouvrage classique du Rap français J'sais pas en qui, en quoi tu crois mais, demain J'me vois loin mille-fa, villa soignée, Saint-Domingue Après l'show, on sèche le whiskas C'est là qu'j'fais mes plans, j'suis prêt, j'avance Pas à pas, ouvre les yeux, serre les dents et tu l'sais Ici, survivre est un exploit, faut pas lâcher On m'a dit c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur l'canapé après une dure journée Un jour, elle m'a dit je t'aime et tes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme J'suis sur YouTube, j'fais du zapping, ouais, ça pique Le rap que j'vois est nul mais, y'a cinq ans, j'trouvais ça pire Ce truc va tourner comme une éolienne, les autres Ils manquent pas d'toupet, leurs couplets sont coupés au miel Qu'ils aillent s'faire mettre, mes concerts dans ta ville chiffrent Mes frères m'aident, j'rappe la vraie merde, la real shit Babylone me chuchote Prends ton cash, dépense-le, vas-y. Comme toi, toutes ces histoires de braquage de banque me fascinent Plante le raciste, prends-le assis, trempe-le dans de l'acide Noir en France plus facile de prendre l'avion que d'prendre le taxi J'vais pas appeler à l'aide ou attendre qu'on m'paye J'me sens ni dans mon pays ni sur ma planète J'dois rentrer où on entre ap' et entreprendre 400 ans d'retard, pas l'temps d'me branler, mon ventre rappe J'l'entends sous mon manteau, ouais Il faut que j'me serve dans l'pot Les noirs intouchables, c'est du cinéma ou c'est des fantômes J'viens d'la pyramide, ça gère la famine ou la lice-po On sait qui a l'pouvoir, les anciennes familles d'aristo' Le niveau d'la vie hausse, tout l'monde fraude Personne peut assumer l'tarif, les gosses haïssent la vie tôt Dis-moi c'est quelle vie, les jeunes ken vite Haine viscérale envers l'système scolaire Les contacts se font quand les phones-tel' vibrent Ils s'tuent la semaine et le week-end vivent Pour dormir contre les 'teilles d'Heinekein vides Ni slow ni slam, juste des flows, des flammes Pour les hommes, les femmes Aucune pitié, zin, y'a que les sommes qu'j'épargne J'donne tout c'que j'ai dans mes raps Pour, un jour, peser dans les charts Lâche ton billet, Feu est dans les bacs On est ravis de l'fêter, les seules qu'on va laisser Nous empêcher de briller sont les maquilleuses télé La réussite des miens vaut plus de dix émeraudes, khey C'est la fierté des nôtres comme le disait Rohff, ouais Le groove leur fout des coups d'schlass, demande à ta petite amie Mes couches-tard découpent des bouts d'zat Gros comme le rocher qu'a fait sombrer le Titanic Dans leurs crews d'nazes, personne s'est fait tirer dessus Pourtant j'y vois plus d'un trou d'balle Et leurs albums n'valent même pas mes prout-lines Quand on rappe, renois, rabzas, babtous bougent On est pas l'renouveau du boom-bap On est l'renouveau du rap tout court On nous a pris pour des intrus Les autres sont passés à la Trap et j'parle pas que d'leur instrus Feu, t'as fait un album presque parfait chapeau, l'artiste J'dis presque parfait parce qu'il manque Bigo sur la tracklist Tu vois, mec ici, y'a pas de rap lisse J'ai zappé mon gars Bigo d'la tracklist Mais j'l'ai pas zappé car y'a les textes qui arrivent Y'a les featurings de fou sur chaque rive de Paname L'Entourage, mon gars, quelle plus grande fierté Que voir les frères faire des couplets écrits, mec, et gratter Pour l'occasion, l'album est dans les bacs, va le per-cho C'est comme ça qu'ça s'passe, j'vais te quer-cho Laisse-moi décompresser La vie d'un jeune entrepreneur est complexe Entre les embrouilles 'vec la justice et les embrouilles 'vec mon ex Et les embrouilles 'vec mes fournisseurs Les embrouilles pour des samples J'suis dans un monde étourdissant Tu peux tout remonter, tout redescendre J'redescendrai plus jamais, mon ex m'a dit J't'en prie, ne t'en va pas Vingt-quatre piges à peine, je travaille déjà plus que ton papa Difficile de m'avoir, impossible de me marier Cette mannequin faisait des manières Maintenant m'invite dans son manoir J'sais pas c'qui s'est passé, j'apprécie les dièses Le pastis est glacé, la piscine est tiède Elle veut être avec Feu mais, moi, j'veux plus être en ple-cou Sa main dans mes cheveux, j'la laisse abîmer ma pe-cou Ses copines me regardent, genre Quand est-ce qu'elle l'épouse ? Ses copains me regardent, genre Qu'est-ce qu'elle lui trouve ? Je bédave tout ce caramelo Et j'écris sur la nouvelle douceur qu'a ramené Lo' J'aime comment tu danses, bébé, détends-toi Le toit est en feu, le feu est en toi J'aime comment tu danses, bébé, détends-toi Le toit est en feu, le feu est en toi La vie m'a appris à ne jamais tourner le dos Y'a que le mur qui peut mater mes fesses Mais j'laisse la bédave cramer tous mes neurones Ouais ouais, j'préfère ça que de me gratter les veines J'fais ce que je sais faire le plus gratter des 16 qui te pètent le cul Ouais, sans cesse on encaisse mais j'reste concentré J'ai une tête et un sexe de mule J'ai souffert dans le calme Ça prouve que mon parcours est crédible Coup d'pelle dans le crâne Pour qu'ces jaloux soient ouverts d'esprit Si tu banalises c'que j'dis, on te malmène jusqu'à ramper Quand le cannabis fleurit, poto, ça freine la santé Véritable vécu, j'en garde les stigmates De plus, j'apprécie les paysages et j'fume de l'herbe médicale On reste insaisissables et têtus, toujours en indé, minable Partage équitable des thunes comme dans Breaking Bad J'lèche des tétons d'minettes en toute modestie, là, j'y prends goût J'ai l'Expression Direkt depuis qu'mon esprit est parti en couille Jusque là j't'aimais mais t'as blasphémé J't'avais dit que personne ne pourrait m'arrêter Râgeux, je t'offre le droit de te moquer Si tu m'passes le code de ta CB Je mène pas une vie hyper saine, même si j'ai percé J'aperçois des personnes derrière les persiennes Seul dans mon appart sale, ma sur révise un partiel Y'a pas d'loi impartiale à part l'Ciel J'suis entouré de zonards sur le sonar Mais c'est trop tard quand les ennuis sont là Les accusés sont sur l'banc et transpirent comme au sauna Les mères pleurent comme Solaar T'es jamais à l'abri, le mal me l'a appris La me-la brille, une maman prie Pourquoi tu me l'as pris ? Ô Dieu, c'est pas le Ciel, c'est les Hommes Odieux, leur âme est scellée par le sexe et les sommes J'ai vu le seum, donné du sale C'est comme si leur cur avait regardé les deux yeux de Médusa Le courage et la peur ensembles sont mes deux armes Quand je me sens déraciné, je monte au sommet des arbres De là-haut, j'vois la mort, faut être prêt si elle approche La vie, c'est apprécier la vue, après scier la branche Tu veux tester mes salauds, ça fait bang, genre saloon Frère, si j't'allume c'est que j'suis prêt pour l'salut T'es pas d'la mif, parle-moi biff ou parle-moi d'profit Dix kilos d'weed, un kilo d'shit, le tout sera blanchi On fume le matos, mes vatos vont tuer ces rappeurs Ça sera du gâteau comme rotte-ca le de l'éducateur A bord d'une Merco Benz, vitres teintées, grosse boisson C'est la moisson, les mousseux sont d'sortie Fuck ton crew, sale pédale, ça bouge ap T'es tout naze, écoute, ça fait breh ! Rien qu'on fait des classiques, S-Crew, le nom d'mon gang Y'a que dans l'ombre qu'on tranche pour pas finir aux assises Souvent dans un camouflage vert kaki L'ambiance est pourave, y'a des toux grasses ça vi-ser d'la weed Ici, tu perds ta vie, on t'nique ta mère à 6 Une bonne paire de Nike Air dans la tête, c'est facile Le leust est entouré donc on fait ça à notre manière Bientôt le L est en tournée donc prenez garde à vos arrières Bitch ! Et toi, dis moi pourquoi tu causes On est au festival de Cannes, toi, tu traînes à la Foire du Trône3</t>
         </is>
       </c>
     </row>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Du monde en Freestyle dans le Planète Rap de Nekfeu</t>
+          <t>Chez nous</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Même si t'as tout fait pour les gens A la moindre dispute, ils oublieront Déçu de ceux qui rampent On veut d'la soupe, il faut des sous qui rentrent C'est l'souk, j'veux pas d'une zouz exubérante qui zouke Sinon, j'devrai couper le souffle aux soupirants Ils m'supplieront d'les épargner mais j'suis pas économe Hey, connards, laissez parler les vrais bonhommes Tu sais, tant qu'un frère a du cur, j'ai rien à foutre de ses stats' On a passé l'stade de s'demander qui sait s'tape On s'estime et les doutes s'estompent J'suis pas assez stable, sista, cesse donc d'envier ces stars Au fond du trou, à part le Ciel, tu veux qu'j'me tourne vers qui ? Envie d'repartir à zéro comme un converti Le traître négocie les trêves, le journaliste grossit les traits Comme un coké, que connait-il D'la philosophie des gosses illettrés ? Sait-il c'qu'il s'passe chaque fois qu'un petit s'fait renvoyer ? Connaît-il la souffrance de l'enfance De mes petites surs en foyer, hein ?! Comme mon homonyme, des cicatrices, j'en ai bezef Même avec les cordes vocales coupées, je serai un mec de parole J'me retourne dans mon lit en m'demandant si j'dois les baiser Vu qu'la nuit porte conseil, j'me lève avec le barreau Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y a des seaux de larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots J'crois bien que le danger vient de mes proches Rien ne m'étonne tout c'qui m'entoure n'est qu'un simple décor Craindre l'effort ce n'est pas pour moi donc je blinde mes forces Poto, tu pues la défaite Tout c'que j'peux faire, c'est plaindre tes gosses A force de manier l'argent sale, j'commence à m'en laver les mains C'est un nouveau départ dans l'Rap On va embrasser le destin J'compte plus le nombre de fois Que j'me pète la tête et m'défonce le foie Mec, j'arrête de faire la fête Avec ma secte, on est fonces-dé le soir S - C.R.E.W Tous ces mecs illettrés rêvent de nous bluffer Le vice peux m'taper dans lil donc j'abaisse pas ma garde La vie un long fleuve tranquille qu'on traverse à la nage Les man, à vos phases, voilà Nekfeu, partez Pétasse, allez, twerke, bouge ton bête de tard-pé C'est E.2.F, ne tente pas d'contrer 7.5.0.19 si tu cherches la contrée Pompez, pompez, pompez, c'est le L Que des flammes bleues, appelle les pompiers Nekflamme, Bazz, Flav', Deen 2zer, Alpha, Doums Mekra, Framal, Gee On est là pour longtemps Faut qu't'achètes Feu si tu veux payer comptant On fait des erreurs mais, quand on chante On est les meilleurs même quand on s'branle Nique toutes vos notions d'loi, bitch Du plus profond d'moi, je veux finir au plus profond d'toi On terminera l'parcours à la morgue Mais avant ça, on est revenus mettre les babtous à la mode Trop d'actions, peu de débats, l'avenir Mais la patience est une vertu que peu Depuis tout petit, 2015, l'année du L, bientôt le Jour Gee C'est facile de les faire rager, ouais, ça, j'sais l'faire J'arrive avec les Versace et les sachets verts Vous êtes tous gâtés, bande de merdeux du net A travers ma paire de lunettes Cartier, j'vois des lunes écartées Double scotch, j'ouvre le score quand mon équipe rentre Le toit est en feu, le sol brûle, ma clique flambe Les gens nous guettent et n'veulent ap' s'ambiancer Ils veulent connaitre nos raps, nos sapes Nos placements financiers Fuck toutes ces débilités d'espionnage Notre crédibilité n'est même pas questionnable Nique les normes, on cherche des deals énormes Dis aux hyènes de déclarer forfait, j'suis là pour un millenium J'ai bien dit un millenium, dès qu'ça parle argent Ils ont des voix bizarres, c'est comme s'ils avaient prit de l'hélium Faut qu'on les plume vite, colors Don Dada On va faire tomber les colosses, yeah Je culmine, ils pourront ap' me battre On pratique le rap de patron Anti-personnel comme une mine J'suis boss, pas intérimaire Quand j'suis dans l'périmètre y'a que des playmates J'écris plus de refrains, j'peins à l'instinct A 25 piges, j'ai déjà signé 25 eins' Nekfeu, c'est le Planète Rap Philly Flingue au microphone, personne arrêtera Y'a pas d'problème quand c'est le Planète Rap Tu sais qu'c'est Mekra, tu sais que personne l'arrêtera C'est Mekra, l'mec rare au micro, parlez pas d'bédave, je picole J'suis qu'un brave qu'a pas d'biff, j'te fais khaf comme à Rio J'suis pas black ni latino, j'suis un bicot qu'a la dalle A c'qui paraît, tous ces mythos passent des kilos par la douane Rien dans l'frigo, y'a pas d'maille, on veut chill au Panama Piner J-Lo, s'il faut killer l'beat, mon stylo gratte un max M.E.K.R.A, et t'as mé-cra cette putain d'caille-ra Ça ira, j'suis faya, pas d'mariage, on salira la Zaia De Paris à Bahia, on a l'image de cannibale Et c'est khatal tah Al-Qaïda Et t'as pas idée, à ris-Pa on a des qualités Le barillet fait baliser tes p'tits, ils restent tétanisés Le sale diable va t'habiter si t'as pas la gnaque, il sait J'travaille mes patates sur un sac à la salle, j'y vais J'ai plein d'buts mais pas d'marques et pas d'thunes, c'est la life J'veux une Féfé, j'ai un PC, j'suis pas une pute, j'ai pas d'MAC Et mate ma démarche de barge, savoir ne pas parler De tes bails, c'est un choix, crois-moi, c'est pas gagné Sale tass, tu parles mal, j't'avais dit, y'a pas d'amour à Paname Donc pas besoin de t'attacher Pas que les gallons, tacle les gars qui jactent et ça bédave, petit T'es tarté, les balles te visent, fais l'chaud et attends-toi au mieux A l'aise, j't'éclate le pif, j'suis chaud donc j'ai pas froid aux yeux J'ai pas froid aux yeux Encore un soir où je tente d'écrire mais ma page reste blanche Peu d'inspi, le ventre vide, il m'reste un sachet à vendre J'me dirige vers le 6, là bas un los-bar m'attend J'vais m'remplir le bide et l'frigo devant la porte On se voit, on monte chez Los', la transaction se passe en balle Puis j'fonce dans l'trom', rejoindre tous mes gars en bas Ça roule des cônes ou plutôt, devrais-je plutôt dire des battes Goûte cette dope qui me fait relativiser La cam c'est mal, on l'sait tous mais cela dit j'y vais Fuck tes probabilités, je tenterais ce pari risqué Il m'faut des pepettes pour graille, j'suis pas du style lève tôt J'garde ma conscience pour moi donc fais de même, frérot Petit toine-An a fait ses classes au mic, gentil mais pas naïf Pas du genre à perdre une occas' de faire de la maille Pas du genre à gémir, à fléchir ou à s'taire A frémir, depuis mes seize balais, j'prépare la guerre Me compare pas à tes assoces, mec, j'suis au-dessus Car j'ai la vision, l'ambition, la tech, maitrise le processus Clic-clic-boom, l'offensive est lancée C'est L'Entourage, couz, sur un ouvrage classique du Rap français J'sais pas en qui, en quoi tu crois mais, demain J'me vois loin mille-fa, villa soignée, Saint-Domingue Après l'show, on sèche le whiskas C'est là qu'j'fais mes plans, j'suis prêt, j'avance Pas à pas, ouvre les yeux, serre les dents et tu l'sais Ici, survivre est un exploit, faut pas lâcher On m'a dit c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur l'canapé après une dure journée Un jour, elle m'a dit je t'aime et tes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme J'suis sur YouTube, j'fais du zapping, ouais, ça pique Le rap que j'vois est nul mais, y'a cinq ans, j'trouvais ça pire Ce truc va tourner comme une éolienne, les autres Ils manquent pas d'toupet, leurs couplets sont coupés au miel Qu'ils aillent s'faire mettre, mes concerts dans ta ville chiffrent Mes frères m'aident, j'rappe la vraie merde, la real shit Babylone me chuchote Prends ton cash, dépense-le, vas-y. Comme toi, toutes ces histoires de braquage de banque me fascinent Plante le raciste, prends-le assis, trempe-le dans de l'acide Noir en France plus facile de prendre l'avion que d'prendre le taxi J'vais pas appeler à l'aide ou attendre qu'on m'paye J'me sens ni dans mon pays ni sur ma planète J'dois rentrer où on entre ap' et entreprendre 400 ans d'retard, pas l'temps d'me branler, mon ventre rappe J'l'entends sous mon manteau, ouais Il faut que j'me serve dans l'pot Les noirs intouchables, c'est du cinéma ou c'est des fantômes J'viens d'la pyramide, ça gère la famine ou la lice-po On sait qui a l'pouvoir, les anciennes familles d'aristo' Le niveau d'la vie hausse, tout l'monde fraude Personne peut assumer l'tarif, les gosses haïssent la vie tôt Dis-moi c'est quelle vie, les jeunes ken vite Haine viscérale envers l'système scolaire Les contacts se font quand les phones-tel' vibrent Ils s'tuent la semaine et le week-end vivent Pour dormir contre les 'teilles d'Heinekein vides Ni slow ni slam, juste des flows, des flammes Pour les hommes, les femmes Aucune pitié, zin, y'a que les sommes qu'j'épargne J'donne tout c'que j'ai dans mes raps Pour, un jour, peser dans les charts Lâche ton billet, Feu est dans les bacs On est ravis de l'fêter, les seules qu'on va laisser Nous empêcher de briller sont les maquilleuses télé La réussite des miens vaut plus de dix émeraudes, khey C'est la fierté des nôtres comme le disait Rohff, ouais Le groove leur fout des coups d'schlass, demande à ta petite amie Mes couches-tard découpent des bouts d'zat Gros comme le rocher qu'a fait sombrer le Titanic Dans leurs crews d'nazes, personne s'est fait tirer dessus Pourtant j'y vois plus d'un trou d'balle Et leurs albums n'valent même pas mes prout-lines Quand on rappe, renois, rabzas, babtous bougent On est pas l'renouveau du boom-bap On est l'renouveau du rap tout court On nous a pris pour des intrus Les autres sont passés à la Trap et j'parle pas que d'leur instrus Feu, t'as fait un album presque parfait chapeau, l'artiste J'dis presque parfait parce qu'il manque Bigo sur la tracklist Tu vois, mec ici, y'a pas de rap lisse J'ai zappé mon gars Bigo d'la tracklist Mais j'l'ai pas zappé car y'a les textes qui arrivent Y'a les featurings de fou sur chaque rive de Paname L'Entourage, mon gars, quelle plus grande fierté Que voir les frères faire des couplets écrits, mec, et gratter Pour l'occasion, l'album est dans les bacs, va le per-cho C'est comme ça qu'ça s'passe, j'vais te quer-cho Laisse-moi décompresser La vie d'un jeune entrepreneur est complexe Entre les embrouilles 'vec la justice et les embrouilles 'vec mon ex Et les embrouilles 'vec mes fournisseurs Les embrouilles pour des samples J'suis dans un monde étourdissant Tu peux tout remonter, tout redescendre J'redescendrai plus jamais, mon ex m'a dit J't'en prie, ne t'en va pas Vingt-quatre piges à peine, je travaille déjà plus que ton papa Difficile de m'avoir, impossible de me marier Cette mannequin faisait des manières Maintenant m'invite dans son manoir J'sais pas c'qui s'est passé, j'apprécie les dièses Le pastis est glacé, la piscine est tiède Elle veut être avec Feu mais, moi, j'veux plus être en ple-cou Sa main dans mes cheveux, j'la laisse abîmer ma pe-cou Ses copines me regardent, genre Quand est-ce qu'elle l'épouse ? Ses copains me regardent, genre Qu'est-ce qu'elle lui trouve ? Je bédave tout ce caramelo Et j'écris sur la nouvelle douceur qu'a ramené Lo' J'aime comment tu danses, bébé, détends-toi Le toit est en feu, le feu est en toi J'aime comment tu danses, bébé, détends-toi Le toit est en feu, le feu est en toi La vie m'a appris à ne jamais tourner le dos Y'a que le mur qui peut mater mes fesses Mais j'laisse la bédave cramer tous mes neurones Ouais ouais, j'préfère ça que de me gratter les veines J'fais ce que je sais faire le plus gratter des 16 qui te pètent le cul Ouais, sans cesse on encaisse mais j'reste concentré J'ai une tête et un sexe de mule J'ai souffert dans le calme Ça prouve que mon parcours est crédible Coup d'pelle dans le crâne Pour qu'ces jaloux soient ouverts d'esprit Si tu banalises c'que j'dis, on te malmène jusqu'à ramper Quand le cannabis fleurit, poto, ça freine la santé Véritable vécu, j'en garde les stigmates De plus, j'apprécie les paysages et j'fume de l'herbe médicale On reste insaisissables et têtus, toujours en indé, minable Partage équitable des thunes comme dans Breaking Bad J'lèche des tétons d'minettes en toute modestie, là, j'y prends goût J'ai l'Expression Direkt depuis qu'mon esprit est parti en couille Jusque là j't'aimais mais t'as blasphémé J't'avais dit que personne ne pourrait m'arrêter Râgeux, je t'offre le droit de te moquer Si tu m'passes le code de ta CB Je mène pas une vie hyper saine, même si j'ai percé J'aperçois des personnes derrière les persiennes Seul dans mon appart sale, ma sur révise un partiel Y'a pas d'loi impartiale à part l'Ciel J'suis entouré de zonards sur le sonar Mais c'est trop tard quand les ennuis sont là Les accusés sont sur l'banc et transpirent comme au sauna Les mères pleurent comme Solaar T'es jamais à l'abri, le mal me l'a appris La me-la brille, une maman prie Pourquoi tu me l'as pris ? Ô Dieu, c'est pas le Ciel, c'est les Hommes Odieux, leur âme est scellée par le sexe et les sommes J'ai vu le seum, donné du sale C'est comme si leur cur avait regardé les deux yeux de Médusa Le courage et la peur ensembles sont mes deux armes Quand je me sens déraciné, je monte au sommet des arbres De là-haut, j'vois la mort, faut être prêt si elle approche La vie, c'est apprécier la vue, après scier la branche Tu veux tester mes salauds, ça fait bang, genre saloon Frère, si j't'allume c'est que j'suis prêt pour l'salut T'es pas d'la mif, parle-moi biff ou parle-moi d'profit Dix kilos d'weed, un kilo d'shit, le tout sera blanchi On fume le matos, mes vatos vont tuer ces rappeurs Ça sera du gâteau comme rotte-ca le de l'éducateur A bord d'une Merco Benz, vitres teintées, grosse boisson C'est la moisson, les mousseux sont d'sortie Fuck ton crew, sale pédale, ça bouge ap T'es tout naze, écoute, ça fait breh ! Rien qu'on fait des classiques, S-Crew, le nom d'mon gang Y'a que dans l'ombre qu'on tranche pour pas finir aux assises Souvent dans un camouflage vert kaki L'ambiance est pourave, y'a des toux grasses ça vi-ser d'la weed Ici, tu perds ta vie, on t'nique ta mère à 6 Une bonne paire de Nike Air dans la tête, c'est facile Le leust est entouré donc on fait ça à notre manière Bientôt le L est en tournée donc prenez garde à vos arrières Bitch ! Et toi, dis moi pourquoi tu causes On est au festival de Cannes, toi, tu traînes à la Foire du Trône3</t>
+          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
         </is>
       </c>
     </row>
@@ -1155,12 +1155,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Chez nous</t>
+          <t>Tu pourras me suivre</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -1172,12 +1172,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Tu pourras me suivre</t>
+          <t>Leçon de vie</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie En autodidacte, tous mes frères sont coriaces La beuh, les meufs, le cognac Mon équipe est armée et dangerous Notorious donc profil bas New York diesel dans le Cohiba Tu vois les flammes dans nos yeuz On est dangerous, ne nous copie pas, nan Ne nous copie pas, on s'en beurre de l'audimat On prend pas de C, on n'a pas d'copyright On ne vendra pas nos images Entre nous et ces chiens, y'a un gros clivage Pas de copinage Et toi, bébé, fais-toi respecter si tu veux ma perle dans ton coquillage J'me lève le matin, un joint de pollen en guise de p'tit-déjeuner Ça me permet d'avoir moins de colère et de rester raisonné Les leçons de la vie s'apprennent seul et pas quand des vieux cons te parlent Mon équipage n'est pas battu par les flots donc le navire ne sombre pas x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie x2 En autodidacte, tous mes frères sont coriaces La beuh, les meufs, le cognac Mon équipe est armée et dangerous Notorious donc profil bas New York diesel dans le Cohiba Tu vois les flammes dans nos yeuz On est dangerous, ne nous copie pas, nan</t>
         </is>
       </c>
     </row>
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Leçon de vie</t>
+          <t>Anges &amp; démons</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie En autodidacte, tous mes frères sont coriaces La beuh, les meufs, le cognac Mon équipe est armée et dangerous Notorious donc profil bas New York diesel dans le Cohiba Tu vois les flammes dans nos yeuz On est dangerous, ne nous copie pas, nan Ne nous copie pas, on s'en beurre de l'audimat On prend pas de C, on n'a pas d'copyright On ne vendra pas nos images Entre nous et ces chiens, y'a un gros clivage Pas de copinage Et toi, bébé, fais-toi respecter si tu veux ma perle dans ton coquillage J'me lève le matin, un joint de pollen en guise de p'tit-déjeuner Ça me permet d'avoir moins de colère et de rester raisonné Les leçons de la vie s'apprennent seul et pas quand des vieux cons te parlent Mon équipage n'est pas battu par les flots donc le navire ne sombre pas x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie x2 En autodidacte, tous mes frères sont coriaces La beuh, les meufs, le cognac Mon équipe est armée et dangerous Notorious donc profil bas New York diesel dans le Cohiba Tu vois les flammes dans nos yeuz On est dangerous, ne nous copie pas, nan</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Anges &amp; démons</t>
+          <t>Les contraires ça tire</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1223,12 +1223,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Les contraires ça tire</t>
+          <t>Nekfeu, Doums, Alpha Wann, S-Crew &amp; Eff Gee en freestyle dans Planète Rap !</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Même si t'as tout fait pour les gens A la moindre dispute, ils oublieront Déçu de ceux qui rampent On veut d'la soupe, il faut des sous qui rentrent C'est l'souk, j'veux pas d'une zouz exubérante qui zouke Sinon, j'devrai couper le souffle aux soupirants Ils m'supplieront d'les épargner mais j'suis pas économe Hey, connards, laissez parler les vrais bonhommes Tu sais, tant qu'un frère a du cur, j'ai rien à foutre de ses stats' On a passé l'stade de s'demander qui sait s'tape On s'estime et les doutes s'estompent J'suis pas assez stable, sista, cesse donc d'envier ces stars Au fond du trou, à part le Ciel, tu veux qu'j'me tourne vers qui ? Envie d'repartir à zéro comme un converti Le traître négocie les trêves, le journaliste grossit les traits Comme un coké, que connait-il D'la philosophie des gosses illettrés ? Sait-il c'qu'il s'passe chaque fois qu'un petit s'fait renvoyer ? Connaît-il la souffrance de l'enfance De mes petites surs en foyer, hein ?! Comme mon homonyme, des cicatrices, j'en ai bezef Même avec les cordes vocales coupées, je serai un mec de parole J'me retourne dans mon lit en m'demandant si j'dois les baiser Vu qu'la nuit porte conseil, j'me lève avec le barreau Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y a des seaux de larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots J'crois bien que le danger vient de mes proches Rien ne m'étonne tout c'qui m'entoure n'est qu'un simple décor Craindre l'effort ce n'est pas pour moi donc je blinde mes forces Poto, tu pues la défaite Tout c'que j'peux faire, c'est plaindre tes gosses A force de manier l'argent sale, j'commence à m'en laver les mains C'est un nouveau départ dans l'Rap On va embrasser le destin J'compte plus le nombre de fois Que j'me pète la tête et m'défonce le foie Mec, j'arrête de faire la fête Avec ma secte, on est fonces-dé le soir S - C.R.E.W Tous ces mecs illettrés rêvent de nous bluffer Le vice peux m'taper dans lil donc j'abaisse pas ma garde La vie un long fleuve tranquille qu'on traverse à la nage Les man, à vos phases, voilà Nekfeu, partez Pétasse, allez, twerke, bouge ton bête de tard-pé C'est E.2.F, ne tente pas d'contrer 7.5.0.19 si tu cherches la contrée Pompez, pompez, pompez, c'est le L Que des flammes bleues, appelle les pompiers Nekflamme, Bazz, Flav', Deen 2zer, Alpha, Doums Mekra, Framal, Gee On est là pour longtemps Faut qu't'achètes Feu si tu veux payer comptant On fait des erreurs mais, quand on chante On est les meilleurs même quand on s'branle Nique toutes vos notions d'loi, bitch Du plus profond d'moi, je veux finir au plus profond d'toi On terminera l'parcours à la morgue Mais avant ça, on est revenus mettre les babtous à la mode Trop d'actions, peu de débats, l'avenir Mais la patience est une vertu que peu Depuis tout petit, 2015, l'année du L, bientôt le Jour Gee C'est facile de les faire rager, ouais, ça, j'sais l'faire J'arrive avec les Versace et les sachets verts Vous êtes tous gâtés, bande de merdeux du net A travers ma paire de lunettes Cartier, j'vois des lunes écartées Double scotch, j'ouvre le score quand mon équipe rentre Le toit est en feu, le sol brûle, ma clique flambe Les gens nous guettent et n'veulent ap' s'ambiancer Ils veulent connaitre nos raps, nos sapes Nos placements financiers Fuck toutes ces débilités d'espionnage Notre crédibilité n'est même pas questionnable Nique les normes, on cherche des deals énormes Dis aux hyènes de déclarer forfait, j'suis là pour un millenium J'ai bien dit un millenium, dès qu'ça parle argent Ils ont des voix bizarres, c'est comme s'ils avaient prit de l'hélium Faut qu'on les plume vite, colors Don Dada On va faire tomber les colosses, yeah Je culmine, ils pourront ap' me battre On pratique le rap de patron Anti-personnel comme une mine J'suis boss, pas intérimaire Quand j'suis dans l'périmètre y'a que des playmates J'écris plus de refrains, j'peins à l'instinct A 25 piges, j'ai déjà signé 25 eins' Nekfeu, c'est le Planète Rap Philly Flingue au microphone, personne arrêtera Y'a pas d'problème quand c'est le Planète Rap Tu sais qu'c'est Mekra, tu sais que personne l'arrêtera C'est Mekra, l'mec rare au micro, parlez pas d'bédave, je picole J'suis qu'un brave qu'a pas d'biff, j'te fais khaf comme à Rio J'suis pas black ni latino, j'suis un bicot qu'a la dalle A c'qui paraît, tous ces mythos passent des kilos par la douane Rien dans l'frigo, y'a pas d'maille, on veut chill au Panama Piner J-Lo, s'il faut killer l'beat, mon stylo gratte un max M.E.K.R.A, et t'as mé-cra cette putain d'caille-ra Ça ira, j'suis faya, pas d'mariage, on salira la Zaia De Paris à Bahia, on a l'image de cannibale Et c'est khatal tah Al-Qaïda Et t'as pas idée, à ris-Pa on a des qualités Le barillet fait baliser tes p'tits, ils restent tétanisés Le sale diable va t'habiter si t'as pas la gnaque, il sait J'travaille mes patates sur un sac à la salle, j'y vais J'ai plein d'buts mais pas d'marques et pas d'thunes, c'est la life J'veux une Féfé, j'ai un PC, j'suis pas une pute, j'ai pas d'MAC Et mate ma démarche de barge, savoir ne pas parler De tes bails, c'est un choix, crois-moi, c'est pas gagné Sale tass, tu parles mal, j't'avais dit, y'a pas d'amour à Paname Donc pas besoin de t'attacher Pas que les gallons, tacle les gars qui jactent et ça bédave, petit T'es tarté, les balles te visent, fais l'chaud et attends-toi au mieux A l'aise, j't'éclate le pif, j'suis chaud donc j'ai pas froid aux yeux J'ai pas froid aux yeux Encore un soir où je tente d'écrire mais ma page reste blanche Peu d'inspi, le ventre vide, il m'reste un sachet à vendre J'me dirige vers le 6, là bas un los-bar m'attend J'vais m'remplir le bide et l'frigo devant la porte On se voit, on monte chez Los', la transaction se passe en balle Puis j'fonce dans l'trom', rejoindre tous mes gars en bas Ça roule des cônes ou plutôt, devrais-je plutôt dire des battes Goûte cette dope qui me fait relativiser La cam c'est mal, on l'sait tous mais cela dit j'y vais Fuck tes probabilités, je tenterais ce pari risqué Il m'faut des pepettes pour graille, j'suis pas du style lève tôt J'garde ma conscience pour moi donc fais de même, frérot Petit toine-An a fait ses classes au mic, gentil mais pas naïf Pas du genre à perdre une occas' de faire de la maille Pas du genre à gémir, à fléchir ou à s'taire A frémir, depuis mes seize balais, j'prépare la guerre Me compare pas à tes assoces, mec, j'suis au-dessus Car j'ai la vision, l'ambition, la tech, maitrise le processus Clic-clic-boom, l'offensive est lancée C'est L'Entourage, couz, sur un ouvrage classique du Rap français J'sais pas en qui, en quoi tu crois mais, demain J'me vois loin mille-fa, villa soignée, Saint-Domingue Après l'show, on sèche le whiskas C'est là qu'j'fais mes plans, j'suis prêt, j'avance Pas à pas, ouvre les yeux, serre les dents et tu l'sais Ici, survivre est un exploit, faut pas lâcher On m'a dit c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur l'canapé après une dure journée Un jour, elle m'a dit je t'aime et tes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme J'suis sur YouTube, j'fais du zapping, ouais, ça pique Le rap que j'vois est nul mais, y'a cinq ans, j'trouvais ça pire Ce truc va tourner comme une éolienne, les autres Ils manquent pas d'toupet, leurs couplets sont coupés au miel Qu'ils aillent s'faire mettre, mes concerts dans ta ville chiffrent Mes frères m'aident, j'rappe la vraie merde, la real shit Babylone me chuchote Prends ton cash, dépense-le, vas-y. Comme toi, toutes ces histoires de braquage de banque me fascinent Plante le raciste, prends-le assis, trempe-le dans de l'acide Noir en France plus facile de prendre l'avion que d'prendre le taxi J'vais pas appeler à l'aide ou attendre qu'on m'paye J'me sens ni dans mon pays ni sur ma planète J'dois rentrer où on entre ap' et entreprendre 400 ans d'retard, pas l'temps d'me branler, mon ventre rappe J'l'entends sous mon manteau, ouais Il faut que j'me serve dans l'pot Les noirs intouchables, c'est du cinéma ou c'est des fantômes J'viens d'la pyramide, ça gère la famine ou la lice-po On sait qui a l'pouvoir, les anciennes familles d'aristo' Le niveau d'la vie hausse, tout l'monde fraude Personne peut assumer l'tarif, les gosses haïssent la vie tôt Dis-moi c'est quelle vie, les jeunes ken vite Haine viscérale envers l'système scolaire Les contacts se font quand les phones-tel' vibrent Ils s'tuent la semaine et le week-end vivent Pour dormir contre les 'teilles d'Heinekein vides Ni slow ni slam, juste des flows, des flammes Pour les hommes, les femmes Aucune pitié, zin, y'a que les sommes qu'j'épargne J'donne tout c'que j'ai dans mes raps Pour, un jour, peser dans les charts Lâche ton billet, Feu est dans les bacs On est ravis de l'fêter, les seules qu'on va laisser Nous empêcher de briller sont les maquilleuses télé La réussite des miens vaut plus de dix émeraudes, khey C'est la fierté des nôtres comme le disait Rohff, ouais Le groove leur fout des coups d'schlass, demande à ta petite amie Mes couches-tard découpent des bouts d'zat Gros comme le rocher qu'a fait sombrer le Titanic Dans leurs crews d'nazes, personne s'est fait tirer dessus Pourtant j'y vois plus d'un trou d'balle Et leurs albums n'valent même pas mes prout-lines Quand on rappe, renois, rabzas, babtous bougent On est pas l'renouveau du boom-bap On est l'renouveau du rap tout court On nous a pris pour des intrus Les autres sont passés à la Trap et j'parle pas que d'leur instrus Feu, t'as fait un album presque parfait chapeau, l'artiste J'dis presque parfait parce qu'il manque Bigo sur la tracklist Tu vois, mec ici, y'a pas de rap lisse J'ai zappé mon gars Bigo d'la tracklist Mais j'l'ai pas zappé car y'a les textes qui arrivent Y'a les featurings de fou sur chaque rive de Paname L'Entourage, mon gars, quelle plus grande fierté Que voir les frères faire des couplets écrits, mec, et gratter Pour l'occasion, l'album est dans les bacs, va le per-cho C'est comme ça qu'ça s'passe, j'vais te quer-cho Laisse-moi décompresser La vie d'un jeune entrepreneur est complexe Entre les embrouilles 'vec la justice et les embrouilles 'vec mon ex Et les embrouilles 'vec mes fournisseurs Les embrouilles pour des samples J'suis dans un monde étourdissant Tu peux tout remonter, tout redescendre J'redescendrai plus jamais, mon ex m'a dit J't'en prie, ne t'en va pas Vingt-quatre piges à peine, je travaille déjà plus que ton papa Difficile de m'avoir, impossible de me marier Cette mannequin faisait des manières Maintenant m'invite dans son manoir J'sais pas c'qui s'est passé, j'apprécie les dièses Le pastis est glacé, la piscine est tiède Elle veut être avec Feu mais, moi, j'veux plus être en ple-cou Sa main dans mes cheveux, j'la laisse abîmer ma pe-cou Ses copines me regardent, genre Quand est-ce qu'elle l'épouse ? Ses copains me regardent, genre Qu'est-ce qu'elle lui trouve ? Je bédave tout ce caramelo Et j'écris sur la nouvelle douceur qu'a ramené Lo' J'aime comment tu danses, bébé, détends-toi Le toit est en feu, le feu est en toi J'aime comment tu danses, bébé, détends-toi Le toit est en feu, le feu est en toi La vie m'a appris à ne jamais tourner le dos Y'a que le mur qui peut mater mes fesses Mais j'laisse la bédave cramer tous mes neurones Ouais ouais, j'préfère ça que de me gratter les veines J'fais ce que je sais faire le plus gratter des 16 qui te pètent le cul Ouais, sans cesse on encaisse mais j'reste concentré J'ai une tête et un sexe de mule J'ai souffert dans le calme Ça prouve que mon parcours est crédible Coup d'pelle dans le crâne Pour qu'ces jaloux soient ouverts d'esprit Si tu banalises c'que j'dis, on te malmène jusqu'à ramper Quand le cannabis fleurit, poto, ça freine la santé Véritable vécu, j'en garde les stigmates De plus, j'apprécie les paysages et j'fume de l'herbe médicale On reste insaisissables et têtus, toujours en indé, minable Partage équitable des thunes comme dans Breaking Bad J'lèche des tétons d'minettes en toute modestie, là, j'y prends goût J'ai l'Expression Direkt depuis qu'mon esprit est parti en couille Jusque là j't'aimais mais t'as blasphémé J't'avais dit que personne ne pourrait m'arrêter Râgeux, je t'offre le droit de te moquer Si tu m'passes le code de ta CB Je mène pas une vie hyper saine, même si j'ai percé J'aperçois des personnes derrière les persiennes Seul dans mon appart sale, ma sur révise un partiel Y'a pas d'loi impartiale à part l'Ciel J'suis entouré de zonards sur le sonar Mais c'est trop tard quand les ennuis sont là Les accusés sont sur l'banc et transpirent comme au sauna Les mères pleurent comme Solaar T'es jamais à l'abri, le mal me l'a appris La me-la brille, une maman prie Pourquoi tu me l'as pris ? Ô Dieu, c'est pas le Ciel, c'est les Hommes Odieux, leur âme est scellée par le sexe et les sommes J'ai vu le seum, donné du sale C'est comme si leur cur avait regardé les deux yeux de Médusa Le courage et la peur ensembles sont mes deux armes Quand je me sens déraciné, je monte au sommet des arbres De là-haut, j'vois la mort, faut être prêt si elle approche La vie, c'est apprécier la vue, après scier la branche Tu veux tester mes salauds, ça fait bang, genre saloon Frère, si j't'allume c'est que j'suis prêt pour l'salut T'es pas d'la mif, parle-moi biff ou parle-moi d'profit Dix kilos d'weed, un kilo d'shit, le tout sera blanchi On fume le matos, mes vatos vont tuer ces rappeurs Ça sera du gâteau comme rotte-ca le de l'éducateur A bord d'une Merco Benz, vitres teintées, grosse boisson C'est la moisson, les mousseux sont d'sortie Fuck ton crew, sale pédale, ça bouge ap T'es tout naze, écoute, ça fait breh ! Rien qu'on fait des classiques, S-Crew, le nom d'mon gang Y'a que dans l'ombre qu'on tranche pour pas finir aux assises Souvent dans un camouflage vert kaki L'ambiance est pourave, y'a des toux grasses ça vi-ser d'la weed Ici, tu perds ta vie, on t'nique ta mère à 6 Une bonne paire de Nike Air dans la tête, c'est facile Le leust est entouré donc on fait ça à notre manière Bientôt le L est en tournée donc prenez garde à vos arrières Bitch ! Et toi, dis moi pourquoi tu causes On est au festival de Cannes, toi, tu traînes à la Foire du Trône3</t>
         </is>
       </c>
     </row>
@@ -1240,12 +1240,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Nekfeu, Doums, Alpha Wann, S-Crew &amp; Eff Gee en freestyle dans Planète Rap !</t>
+          <t>Palm Trees (Remix)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Même si t'as tout fait pour les gens A la moindre dispute, ils oublieront Déçu de ceux qui rampent On veut d'la soupe, il faut des sous qui rentrent C'est l'souk, j'veux pas d'une zouz exubérante qui zouke Sinon, j'devrai couper le souffle aux soupirants Ils m'supplieront d'les épargner mais j'suis pas économe Hey, connards, laissez parler les vrais bonhommes Tu sais, tant qu'un frère a du cur, j'ai rien à foutre de ses stats' On a passé l'stade de s'demander qui sait s'tape On s'estime et les doutes s'estompent J'suis pas assez stable, sista, cesse donc d'envier ces stars Au fond du trou, à part le Ciel, tu veux qu'j'me tourne vers qui ? Envie d'repartir à zéro comme un converti Le traître négocie les trêves, le journaliste grossit les traits Comme un coké, que connait-il D'la philosophie des gosses illettrés ? Sait-il c'qu'il s'passe chaque fois qu'un petit s'fait renvoyer ? Connaît-il la souffrance de l'enfance De mes petites surs en foyer, hein ?! Comme mon homonyme, des cicatrices, j'en ai bezef Même avec les cordes vocales coupées, je serai un mec de parole J'me retourne dans mon lit en m'demandant si j'dois les baiser Vu qu'la nuit porte conseil, j'me lève avec le barreau Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y a des seaux de larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots J'crois bien que le danger vient de mes proches Rien ne m'étonne tout c'qui m'entoure n'est qu'un simple décor Craindre l'effort ce n'est pas pour moi donc je blinde mes forces Poto, tu pues la défaite Tout c'que j'peux faire, c'est plaindre tes gosses A force de manier l'argent sale, j'commence à m'en laver les mains C'est un nouveau départ dans l'Rap On va embrasser le destin J'compte plus le nombre de fois Que j'me pète la tête et m'défonce le foie Mec, j'arrête de faire la fête Avec ma secte, on est fonces-dé le soir S - C.R.E.W Tous ces mecs illettrés rêvent de nous bluffer Le vice peux m'taper dans lil donc j'abaisse pas ma garde La vie un long fleuve tranquille qu'on traverse à la nage Les man, à vos phases, voilà Nekfeu, partez Pétasse, allez, twerke, bouge ton bête de tard-pé C'est E.2.F, ne tente pas d'contrer 7.5.0.19 si tu cherches la contrée Pompez, pompez, pompez, c'est le L Que des flammes bleues, appelle les pompiers Nekflamme, Bazz, Flav', Deen 2zer, Alpha, Doums Mekra, Framal, Gee On est là pour longtemps Faut qu't'achètes Feu si tu veux payer comptant On fait des erreurs mais, quand on chante On est les meilleurs même quand on s'branle Nique toutes vos notions d'loi, bitch Du plus profond d'moi, je veux finir au plus profond d'toi On terminera l'parcours à la morgue Mais avant ça, on est revenus mettre les babtous à la mode Trop d'actions, peu de débats, l'avenir Mais la patience est une vertu que peu Depuis tout petit, 2015, l'année du L, bientôt le Jour Gee C'est facile de les faire rager, ouais, ça, j'sais l'faire J'arrive avec les Versace et les sachets verts Vous êtes tous gâtés, bande de merdeux du net A travers ma paire de lunettes Cartier, j'vois des lunes écartées Double scotch, j'ouvre le score quand mon équipe rentre Le toit est en feu, le sol brûle, ma clique flambe Les gens nous guettent et n'veulent ap' s'ambiancer Ils veulent connaitre nos raps, nos sapes Nos placements financiers Fuck toutes ces débilités d'espionnage Notre crédibilité n'est même pas questionnable Nique les normes, on cherche des deals énormes Dis aux hyènes de déclarer forfait, j'suis là pour un millenium J'ai bien dit un millenium, dès qu'ça parle argent Ils ont des voix bizarres, c'est comme s'ils avaient prit de l'hélium Faut qu'on les plume vite, colors Don Dada On va faire tomber les colosses, yeah Je culmine, ils pourront ap' me battre On pratique le rap de patron Anti-personnel comme une mine J'suis boss, pas intérimaire Quand j'suis dans l'périmètre y'a que des playmates J'écris plus de refrains, j'peins à l'instinct A 25 piges, j'ai déjà signé 25 eins' Nekfeu, c'est le Planète Rap Philly Flingue au microphone, personne arrêtera Y'a pas d'problème quand c'est le Planète Rap Tu sais qu'c'est Mekra, tu sais que personne l'arrêtera C'est Mekra, l'mec rare au micro, parlez pas d'bédave, je picole J'suis qu'un brave qu'a pas d'biff, j'te fais khaf comme à Rio J'suis pas black ni latino, j'suis un bicot qu'a la dalle A c'qui paraît, tous ces mythos passent des kilos par la douane Rien dans l'frigo, y'a pas d'maille, on veut chill au Panama Piner J-Lo, s'il faut killer l'beat, mon stylo gratte un max M.E.K.R.A, et t'as mé-cra cette putain d'caille-ra Ça ira, j'suis faya, pas d'mariage, on salira la Zaia De Paris à Bahia, on a l'image de cannibale Et c'est khatal tah Al-Qaïda Et t'as pas idée, à ris-Pa on a des qualités Le barillet fait baliser tes p'tits, ils restent tétanisés Le sale diable va t'habiter si t'as pas la gnaque, il sait J'travaille mes patates sur un sac à la salle, j'y vais J'ai plein d'buts mais pas d'marques et pas d'thunes, c'est la life J'veux une Féfé, j'ai un PC, j'suis pas une pute, j'ai pas d'MAC Et mate ma démarche de barge, savoir ne pas parler De tes bails, c'est un choix, crois-moi, c'est pas gagné Sale tass, tu parles mal, j't'avais dit, y'a pas d'amour à Paname Donc pas besoin de t'attacher Pas que les gallons, tacle les gars qui jactent et ça bédave, petit T'es tarté, les balles te visent, fais l'chaud et attends-toi au mieux A l'aise, j't'éclate le pif, j'suis chaud donc j'ai pas froid aux yeux J'ai pas froid aux yeux Encore un soir où je tente d'écrire mais ma page reste blanche Peu d'inspi, le ventre vide, il m'reste un sachet à vendre J'me dirige vers le 6, là bas un los-bar m'attend J'vais m'remplir le bide et l'frigo devant la porte On se voit, on monte chez Los', la transaction se passe en balle Puis j'fonce dans l'trom', rejoindre tous mes gars en bas Ça roule des cônes ou plutôt, devrais-je plutôt dire des battes Goûte cette dope qui me fait relativiser La cam c'est mal, on l'sait tous mais cela dit j'y vais Fuck tes probabilités, je tenterais ce pari risqué Il m'faut des pepettes pour graille, j'suis pas du style lève tôt J'garde ma conscience pour moi donc fais de même, frérot Petit toine-An a fait ses classes au mic, gentil mais pas naïf Pas du genre à perdre une occas' de faire de la maille Pas du genre à gémir, à fléchir ou à s'taire A frémir, depuis mes seize balais, j'prépare la guerre Me compare pas à tes assoces, mec, j'suis au-dessus Car j'ai la vision, l'ambition, la tech, maitrise le processus Clic-clic-boom, l'offensive est lancée C'est L'Entourage, couz, sur un ouvrage classique du Rap français J'sais pas en qui, en quoi tu crois mais, demain J'me vois loin mille-fa, villa soignée, Saint-Domingue Après l'show, on sèche le whiskas C'est là qu'j'fais mes plans, j'suis prêt, j'avance Pas à pas, ouvre les yeux, serre les dents et tu l'sais Ici, survivre est un exploit, faut pas lâcher On m'a dit c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur l'canapé après une dure journée Un jour, elle m'a dit je t'aime et tes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme J'suis sur YouTube, j'fais du zapping, ouais, ça pique Le rap que j'vois est nul mais, y'a cinq ans, j'trouvais ça pire Ce truc va tourner comme une éolienne, les autres Ils manquent pas d'toupet, leurs couplets sont coupés au miel Qu'ils aillent s'faire mettre, mes concerts dans ta ville chiffrent Mes frères m'aident, j'rappe la vraie merde, la real shit Babylone me chuchote Prends ton cash, dépense-le, vas-y. Comme toi, toutes ces histoires de braquage de banque me fascinent Plante le raciste, prends-le assis, trempe-le dans de l'acide Noir en France plus facile de prendre l'avion que d'prendre le taxi J'vais pas appeler à l'aide ou attendre qu'on m'paye J'me sens ni dans mon pays ni sur ma planète J'dois rentrer où on entre ap' et entreprendre 400 ans d'retard, pas l'temps d'me branler, mon ventre rappe J'l'entends sous mon manteau, ouais Il faut que j'me serve dans l'pot Les noirs intouchables, c'est du cinéma ou c'est des fantômes J'viens d'la pyramide, ça gère la famine ou la lice-po On sait qui a l'pouvoir, les anciennes familles d'aristo' Le niveau d'la vie hausse, tout l'monde fraude Personne peut assumer l'tarif, les gosses haïssent la vie tôt Dis-moi c'est quelle vie, les jeunes ken vite Haine viscérale envers l'système scolaire Les contacts se font quand les phones-tel' vibrent Ils s'tuent la semaine et le week-end vivent Pour dormir contre les 'teilles d'Heinekein vides Ni slow ni slam, juste des flows, des flammes Pour les hommes, les femmes Aucune pitié, zin, y'a que les sommes qu'j'épargne J'donne tout c'que j'ai dans mes raps Pour, un jour, peser dans les charts Lâche ton billet, Feu est dans les bacs On est ravis de l'fêter, les seules qu'on va laisser Nous empêcher de briller sont les maquilleuses télé La réussite des miens vaut plus de dix émeraudes, khey C'est la fierté des nôtres comme le disait Rohff, ouais Le groove leur fout des coups d'schlass, demande à ta petite amie Mes couches-tard découpent des bouts d'zat Gros comme le rocher qu'a fait sombrer le Titanic Dans leurs crews d'nazes, personne s'est fait tirer dessus Pourtant j'y vois plus d'un trou d'balle Et leurs albums n'valent même pas mes prout-lines Quand on rappe, renois, rabzas, babtous bougent On est pas l'renouveau du boom-bap On est l'renouveau du rap tout court On nous a pris pour des intrus Les autres sont passés à la Trap et j'parle pas que d'leur instrus Feu, t'as fait un album presque parfait chapeau, l'artiste J'dis presque parfait parce qu'il manque Bigo sur la tracklist Tu vois, mec ici, y'a pas de rap lisse J'ai zappé mon gars Bigo d'la tracklist Mais j'l'ai pas zappé car y'a les textes qui arrivent Y'a les featurings de fou sur chaque rive de Paname L'Entourage, mon gars, quelle plus grande fierté Que voir les frères faire des couplets écrits, mec, et gratter Pour l'occasion, l'album est dans les bacs, va le per-cho C'est comme ça qu'ça s'passe, j'vais te quer-cho Laisse-moi décompresser La vie d'un jeune entrepreneur est complexe Entre les embrouilles 'vec la justice et les embrouilles 'vec mon ex Et les embrouilles 'vec mes fournisseurs Les embrouilles pour des samples J'suis dans un monde étourdissant Tu peux tout remonter, tout redescendre J'redescendrai plus jamais, mon ex m'a dit J't'en prie, ne t'en va pas Vingt-quatre piges à peine, je travaille déjà plus que ton papa Difficile de m'avoir, impossible de me marier Cette mannequin faisait des manières Maintenant m'invite dans son manoir J'sais pas c'qui s'est passé, j'apprécie les dièses Le pastis est glacé, la piscine est tiède Elle veut être avec Feu mais, moi, j'veux plus être en ple-cou Sa main dans mes cheveux, j'la laisse abîmer ma pe-cou Ses copines me regardent, genre Quand est-ce qu'elle l'épouse ? Ses copains me regardent, genre Qu'est-ce qu'elle lui trouve ? Je bédave tout ce caramelo Et j'écris sur la nouvelle douceur qu'a ramené Lo' J'aime comment tu danses, bébé, détends-toi Le toit est en feu, le feu est en toi J'aime comment tu danses, bébé, détends-toi Le toit est en feu, le feu est en toi La vie m'a appris à ne jamais tourner le dos Y'a que le mur qui peut mater mes fesses Mais j'laisse la bédave cramer tous mes neurones Ouais ouais, j'préfère ça que de me gratter les veines J'fais ce que je sais faire le plus gratter des 16 qui te pètent le cul Ouais, sans cesse on encaisse mais j'reste concentré J'ai une tête et un sexe de mule J'ai souffert dans le calme Ça prouve que mon parcours est crédible Coup d'pelle dans le crâne Pour qu'ces jaloux soient ouverts d'esprit Si tu banalises c'que j'dis, on te malmène jusqu'à ramper Quand le cannabis fleurit, poto, ça freine la santé Véritable vécu, j'en garde les stigmates De plus, j'apprécie les paysages et j'fume de l'herbe médicale On reste insaisissables et têtus, toujours en indé, minable Partage équitable des thunes comme dans Breaking Bad J'lèche des tétons d'minettes en toute modestie, là, j'y prends goût J'ai l'Expression Direkt depuis qu'mon esprit est parti en couille Jusque là j't'aimais mais t'as blasphémé J't'avais dit que personne ne pourrait m'arrêter Râgeux, je t'offre le droit de te moquer Si tu m'passes le code de ta CB Je mène pas une vie hyper saine, même si j'ai percé J'aperçois des personnes derrière les persiennes Seul dans mon appart sale, ma sur révise un partiel Y'a pas d'loi impartiale à part l'Ciel J'suis entouré de zonards sur le sonar Mais c'est trop tard quand les ennuis sont là Les accusés sont sur l'banc et transpirent comme au sauna Les mères pleurent comme Solaar T'es jamais à l'abri, le mal me l'a appris La me-la brille, une maman prie Pourquoi tu me l'as pris ? Ô Dieu, c'est pas le Ciel, c'est les Hommes Odieux, leur âme est scellée par le sexe et les sommes J'ai vu le seum, donné du sale C'est comme si leur cur avait regardé les deux yeux de Médusa Le courage et la peur ensembles sont mes deux armes Quand je me sens déraciné, je monte au sommet des arbres De là-haut, j'vois la mort, faut être prêt si elle approche La vie, c'est apprécier la vue, après scier la branche Tu veux tester mes salauds, ça fait bang, genre saloon Frère, si j't'allume c'est que j'suis prêt pour l'salut T'es pas d'la mif, parle-moi biff ou parle-moi d'profit Dix kilos d'weed, un kilo d'shit, le tout sera blanchi On fume le matos, mes vatos vont tuer ces rappeurs Ça sera du gâteau comme rotte-ca le de l'éducateur A bord d'une Merco Benz, vitres teintées, grosse boisson C'est la moisson, les mousseux sont d'sortie Fuck ton crew, sale pédale, ça bouge ap T'es tout naze, écoute, ça fait breh ! Rien qu'on fait des classiques, S-Crew, le nom d'mon gang Y'a que dans l'ombre qu'on tranche pour pas finir aux assises Souvent dans un camouflage vert kaki L'ambiance est pourave, y'a des toux grasses ça vi-ser d'la weed Ici, tu perds ta vie, on t'nique ta mère à 6 Une bonne paire de Nike Air dans la tête, c'est facile Le leust est entouré donc on fait ça à notre manière Bientôt le L est en tournée donc prenez garde à vos arrières Bitch ! Et toi, dis moi pourquoi tu causes On est au festival de Cannes, toi, tu traînes à la Foire du Trône3</t>
+          <t>Bouge la tête et ressens ce frisson, j'aimerais te voir dans différentes positions J'démarre au quart de tour quand je prends le guidon, le son est entraînant et nous en profitons Tu fouilles mes affaires quand je sors ou tu prends des photos quand je dors Alors, écarte-toi de mon champ de vision ou mon poing et ta tête rentrent en collision Je passe à la radio, tu me vois à la télé mais tu peux me croiser dans le tro-mé Ou assis sur un banc parisien, fonce-dé, j'observe les gens se promener Je pense à la vie que Dieu m'a donné, trop souvent la souffrance m'a fait plier Je ne savais pas que ma destinée n'était qu'un navire que j'manuvrais Des fois, la douleur m'a fait perdre la foi, j'avais cette haine et j'étais fier de l'avoir Quand la folie m'attaquait, j'passais des nuits à rapper, jusqu'à ce que je m'en baise la voix Monter sur la scène avec une attelle à l'épaule, bien évidemment, c'est la passion qui me guide Je ne prends pas le mic', pour les femmes et la débauche, ma vie c'est le rap, t'as compris le risque T'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende J'répète, si t'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende Hein L'esprit hanté par des démons, des ondes qui montent à la tête dans la pénombre J'ai l'don, la manière, nique les barrières, mes sons estompent vos carrières En 2-4-6, j'sors le barillet, c'est la fin, Aladin, tue-les, par pitié J'suis le nouveau talent sur qui parier, les catins, au Parrain, veulent se marier Car y a trop d'types qui m'imitent et j'ai un gros style à la P. Diddy S'il y a les keufs, meuf, j'fais un murder, cache ton brolic sous ton bikini Sous ton bikini, j'fuck la police et les dirigistes Toujours primitif, mesdames, le rap, c'est pas difficile, guette ça Quand ma vie se déchire sur mon rap, j'ai le cur dans les ténèbres Et quand mon rap se déchire sur ma feuille, il est rare que je m'énerve Salope, j'ai pas le temps, les minutes vont plus vite quand t'es célèbre J'ai deux-trois trucs à faire afin même que mon business te pénètre Rien qu'j'les pénètre depuis le plus jeune âge, très peu d'temps pour que tu l'remarques Pour que tu me regardes, pourquoi tu m'reparles ? Parce que j'ai l'buzz et les putes ce soir Puff puff sur le oint-j, j'suis trop loin, dans ma matrice On m'dit Aladin, jusqu'à la fin, tu seras magique T'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende J'répète, si t'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende Han Beaucoup de ous-s dans ma tête, aux coups d'teau-cou, j'fais la fête J'suis à l'heure du Big Ben, j'veux la paye de T-Pain, pourquoi ? Pour que ta bitch me la tienne Tous les jours, j'suis en bas d'ton bâtiment, j'suis opé' du lundi à dimanche J'suis l'meilleur pratiquement, fumée blanche du Vatican Ma paye, j'la prends dans la street, j'ai d'la bue-her meilleure que celle de Maastricht Tous tes players ont peur de l'affiche, c'est la frayeur du succès, d'la frime On veut du cash, mon re-frè, du biff, tu captes, mon re-frè, tu piges ? On veut du cash mon re-frè, du biff, tu captes, mon re-frè, tu piges ? J'veux voir une fesse monter sur l'autre, baby, j'veux qu'tu twerkes J'ai le même bide que Rick Ross, t'as la même touffe que Rick James Première phase tous tes rappeurs sont terre-par, bang, bang, bang, bang, clashez-moi, faut qu'on dehka J'me suis souvent dis que le rap, c'était mon hobby, que ça m'amènerait pas à la Merco ou l'Audi Pas attendu l'rap pour faire de l'argent, demande à la rue, les poucaves et l'agent Si tu veux un feat', sors-moi si t'as l'mec, t'as dû voir ma gueule, si t'as l'net 500 000 vues, toujours pas à la SACEM, Panama en concert, il faut que ça saigne T'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende J'répète, si t'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende7</t>
         </is>
       </c>
     </row>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Palm Trees (Remix)</t>
+          <t>On reste vrai</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Bouge la tête et ressens ce frisson, j'aimerais te voir dans différentes positions J'démarre au quart de tour quand je prends le guidon, le son est entraînant et nous en profitons Tu fouilles mes affaires quand je sors ou tu prends des photos quand je dors Alors, écarte-toi de mon champ de vision ou mon poing et ta tête rentrent en collision Je passe à la radio, tu me vois à la télé mais tu peux me croiser dans le tro-mé Ou assis sur un banc parisien, fonce-dé, j'observe les gens se promener Je pense à la vie que Dieu m'a donné, trop souvent la souffrance m'a fait plier Je ne savais pas que ma destinée n'était qu'un navire que j'manuvrais Des fois, la douleur m'a fait perdre la foi, j'avais cette haine et j'étais fier de l'avoir Quand la folie m'attaquait, j'passais des nuits à rapper, jusqu'à ce que je m'en baise la voix Monter sur la scène avec une attelle à l'épaule, bien évidemment, c'est la passion qui me guide Je ne prends pas le mic', pour les femmes et la débauche, ma vie c'est le rap, t'as compris le risque T'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende J'répète, si t'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende Hein L'esprit hanté par des démons, des ondes qui montent à la tête dans la pénombre J'ai l'don, la manière, nique les barrières, mes sons estompent vos carrières En 2-4-6, j'sors le barillet, c'est la fin, Aladin, tue-les, par pitié J'suis le nouveau talent sur qui parier, les catins, au Parrain, veulent se marier Car y a trop d'types qui m'imitent et j'ai un gros style à la P. Diddy S'il y a les keufs, meuf, j'fais un murder, cache ton brolic sous ton bikini Sous ton bikini, j'fuck la police et les dirigistes Toujours primitif, mesdames, le rap, c'est pas difficile, guette ça Quand ma vie se déchire sur mon rap, j'ai le cur dans les ténèbres Et quand mon rap se déchire sur ma feuille, il est rare que je m'énerve Salope, j'ai pas le temps, les minutes vont plus vite quand t'es célèbre J'ai deux-trois trucs à faire afin même que mon business te pénètre Rien qu'j'les pénètre depuis le plus jeune âge, très peu d'temps pour que tu l'remarques Pour que tu me regardes, pourquoi tu m'reparles ? Parce que j'ai l'buzz et les putes ce soir Puff puff sur le oint-j, j'suis trop loin, dans ma matrice On m'dit Aladin, jusqu'à la fin, tu seras magique T'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende J'répète, si t'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende Han Beaucoup de ous-s dans ma tête, aux coups d'teau-cou, j'fais la fête J'suis à l'heure du Big Ben, j'veux la paye de T-Pain, pourquoi ? Pour que ta bitch me la tienne Tous les jours, j'suis en bas d'ton bâtiment, j'suis opé' du lundi à dimanche J'suis l'meilleur pratiquement, fumée blanche du Vatican Ma paye, j'la prends dans la street, j'ai d'la bue-her meilleure que celle de Maastricht Tous tes players ont peur de l'affiche, c'est la frayeur du succès, d'la frime On veut du cash, mon re-frè, du biff, tu captes, mon re-frè, tu piges ? On veut du cash mon re-frè, du biff, tu captes, mon re-frè, tu piges ? J'veux voir une fesse monter sur l'autre, baby, j'veux qu'tu twerkes J'ai le même bide que Rick Ross, t'as la même touffe que Rick James Première phase tous tes rappeurs sont terre-par, bang, bang, bang, bang, clashez-moi, faut qu'on dehka J'me suis souvent dis que le rap, c'était mon hobby, que ça m'amènerait pas à la Merco ou l'Audi Pas attendu l'rap pour faire de l'argent, demande à la rue, les poucaves et l'agent Si tu veux un feat', sors-moi si t'as l'mec, t'as dû voir ma gueule, si t'as l'net 500 000 vues, toujours pas à la SACEM, Panama en concert, il faut que ça saigne T'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende J'répète, si t'as l'appart', bébé, on débarque avec mes gavas mal élevés Nuits blanches, freestyles, c'est L'Entourage et le Panama Bende7</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -1274,12 +1274,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>On reste vrai</t>
+          <t>Fous la merde</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Georgio, Abou, 2-Zer C'est L'Entourage, S-Crew, boy Tu connais t'façon 75ème Session, girl Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Toutes les pétasses opèrent avec la même technique d'approche OK, j'suis le Roi des cons mais t'es la reine des p'tites salopes Ici, c'est Paris, la ville des soi-disant gangsters Qui manigancent pour te voir moisir en enfer C'est 2-Zer Washington et Georgio Armani Y'a d'la be-her, d'la picole et puis des morceaux d'cannabis Nos propos paralysent et font l'effet du tabagisme On t'attire comme une actrice porno amatrice Dans l'excellence, j'suis une référence textuelle Tes déchainements gestuels prouvent tes préférences sexuelles Errer dans des ruelles, nan, c'est pas l'paradis On fait qu'se plaindre car la vie est méchante et cruelle On fait pas d'Rap mais de la littérature moderne C'est ça l'dicton, pas d'addiction mais la rime et la rue m'obsèdent C'est pour Paris Nord mais c'couplet j'l'ai gratté dans l'15 Big up à mon S-Crew et ceux qui vont graffer dans l'train Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Assis dans l'métro, j'remercie Rosa Parks mais je serais heureux Quand on n'osera pas me dire non aux soirées hypes et grands apparts J'entends tellement de merdes, de faux Nekfeu J'ai peur qu'les gens vomissent, pas d'feat Je mélange pas mon champagne avec du Champomy Très loin des cours de catéchisme mes amis sombres, entre shit et garettes-ci J'ai quitté la maison, c'est la merde à vrai dire Quelques métaphores dans mes textes, on m'a dit Mets en d'autres En attendant on s'baise la tête, une chambre de bonne devenue maison close L'impression qu'tout le wagon m'fixe d'être à part Malgré qu'j'sois dans les normes avec mon pantalon-baskets-sweat bien sympa J'pense aux embrouilles d'hier, j'avais la tête vide à la base Et ma mère, j'comprends plus rien à c'qu'elle m'dit, v'la l'blabla Le monde s'achète, mets ton nom sous packaging, c'est tout pour la monnaie Alors qu'y'a qu'dans ces yeux qu'j'trouve un coin de paradis L'été, Paris sous les toits a des airs de Jamaïque J'ai fini d'rêver, j'aurais plus d'espoir si j'étais pas naïf x2 Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Oh qu'est-ce que tu fous, là !? Ça va pas ou quoi !? Quoi, j'fais rien d'mal ? J'veux juste réveiller le quartier ! Regarde, ouvre tes yeux, il est mort c'putain d'quartier !</t>
         </is>
       </c>
     </row>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Fous la merde</t>
+          <t>Tu connais t’facons</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Georgio, Abou, 2-Zer C'est L'Entourage, S-Crew, boy Tu connais t'façon 75ème Session, girl Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Toutes les pétasses opèrent avec la même technique d'approche OK, j'suis le Roi des cons mais t'es la reine des p'tites salopes Ici, c'est Paris, la ville des soi-disant gangsters Qui manigancent pour te voir moisir en enfer C'est 2-Zer Washington et Georgio Armani Y'a d'la be-her, d'la picole et puis des morceaux d'cannabis Nos propos paralysent et font l'effet du tabagisme On t'attire comme une actrice porno amatrice Dans l'excellence, j'suis une référence textuelle Tes déchainements gestuels prouvent tes préférences sexuelles Errer dans des ruelles, nan, c'est pas l'paradis On fait qu'se plaindre car la vie est méchante et cruelle On fait pas d'Rap mais de la littérature moderne C'est ça l'dicton, pas d'addiction mais la rime et la rue m'obsèdent C'est pour Paris Nord mais c'couplet j'l'ai gratté dans l'15 Big up à mon S-Crew et ceux qui vont graffer dans l'train Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Assis dans l'métro, j'remercie Rosa Parks mais je serais heureux Quand on n'osera pas me dire non aux soirées hypes et grands apparts J'entends tellement de merdes, de faux Nekfeu J'ai peur qu'les gens vomissent, pas d'feat Je mélange pas mon champagne avec du Champomy Très loin des cours de catéchisme mes amis sombres, entre shit et garettes-ci J'ai quitté la maison, c'est la merde à vrai dire Quelques métaphores dans mes textes, on m'a dit Mets en d'autres En attendant on s'baise la tête, une chambre de bonne devenue maison close L'impression qu'tout le wagon m'fixe d'être à part Malgré qu'j'sois dans les normes avec mon pantalon-baskets-sweat bien sympa J'pense aux embrouilles d'hier, j'avais la tête vide à la base Et ma mère, j'comprends plus rien à c'qu'elle m'dit, v'la l'blabla Le monde s'achète, mets ton nom sous packaging, c'est tout pour la monnaie Alors qu'y'a qu'dans ces yeux qu'j'trouve un coin de paradis L'été, Paris sous les toits a des airs de Jamaïque J'ai fini d'rêver, j'aurais plus d'espoir si j'étais pas naïf x2 Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Oh qu'est-ce que tu fous, là !? Ça va pas ou quoi !? Quoi, j'fais rien d'mal ? J'veux juste réveiller le quartier ! Regarde, ouvre tes yeux, il est mort c'putain d'quartier !</t>
+          <t>Moi, j'me sens libre quand j'écris ces mots A la prod', tu l'as senti, ouais, c'est DJ Lo' C'est l'Entourage, bébé, on s'enfouraille On encourage les vrais 2zer Washington, tu connais t'façon Comme l'Homme de l'Est, j'attends l'apocalypse Je profite avant qu'on m'refroidisse, avant qu'ma peau palisse Dans mon ciboulot, j'suis mitigé, oui, si j'ai un petit boulot Un salaire, j'irais prendre l'air même si j'vivais ma vie sous l'eau Le Rap me dégoûte comme les pires aspects des filles gâtées J'vais vite gratter malgré que j'dérive, là, mais j'déprime jamais Les vices cachés des miss fâchées, ça entraine des vies gâchées Dédicacer des petites tasses-pé ? Autant caner déshydraté Ma vie d'avant, merde ! J'peux pas la quitter Zer-2 va rappliquer, faire de l'art appliqué J'vais devoir jouer les crevards, plus qu'deux lattes à tirer Tous maladifs, touche pas la mif' ou j'vais te ratatiner Noichintok, jusqu'au Népal, je gère Poto, tu connais pas 2-Zer !? X2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon Ouais, tu connais pas 2-Zer ? Comment ça, tu connais pas 2-Zer ? Faut que j'devienne légendaire, que j'éclaire les lanternes mais Ici, c'est l'enfer depuis qu'j'vois mes frères s'faire enfermer Nique le système carcéral, j'ai pris flemme de passer àl Je préféré les décibels et puis les péritels des caméras Ne m'colle pas d'étiquette, j'bicrave des citernes de came hélas J'baise les fliquettes, éviscère des criquets de chaque tié-quar Nous allons nous équiper comme les p'tits mecs des favelas Le ballon, j'l'ai esquivé, j'ai fait vibrer des tas d'pétasses Wesh kafass ? Moi, j'froisse des spliffs La poisse m'esquive, j'suis la poussière dans l'mauvais il Tous les yeux m'guettent, à croire que j'm'exhibe Bandes de sales vermines, que pourrez-vous faire quand j'aurai l'seum ? Nada... Tu connais pas 2-Zer ? Écoute ça, c'est mamen 2-Zer x2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon Attention, je débarque ça va trouer des schnecks Et puis clouer des becs, t'es dégouté, t'es dèf Venez gouter mes textes, allez, courez les mecs Ca va couper des têtes, tout est prétexte à jouer les chefs Ouais, masquez vos pulsions, j'viens pas rouler des pelles Dans l'trou de tes fesses j'fait ma révolution Ouais, mate l'élocution, t'es un petit mytho si t'oses dire Qu'on est pas des pros du son, moi, j'te critique au micro, p'tit J'vai pas m'défiler, méfiez-vous, faut pas m'défier J'ai ves-qui les cours pour des filles, des sous Et des billets pourpres, j'ai mis d'côté les plaisirs des foufs Car j'en ai qu'une mais j'sais qu'vous m'désirez toutes L'argent, les thunes, mon but... Ouais, tu connais pas 2-Zer ? X2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon2</t>
         </is>
       </c>
     </row>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Tu connais t’facons</t>
+          <t>Les filles de Paris</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Les filles de Paris</t>
+          <t>2001</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Moi, j'me sens libre quand j'écris ces mots A la prod', tu l'as senti, ouais, c'est DJ Lo' C'est l'Entourage, bébé, on s'enfouraille On encourage les vrais 2zer Washington, tu connais t'façon Comme l'Homme de l'Est, j'attends l'apocalypse Je profite avant qu'on m'refroidisse, avant qu'ma peau palisse Dans mon ciboulot, j'suis mitigé, oui, si j'ai un petit boulot Un salaire, j'irais prendre l'air même si j'vivais ma vie sous l'eau Le Rap me dégoûte comme les pires aspects des filles gâtées J'vais vite gratter malgré que j'dérive, là, mais j'déprime jamais Les vices cachés des miss fâchées, ça entraine des vies gâchées Dédicacer des petites tasses-pé ? Autant caner déshydraté Ma vie d'avant, merde ! J'peux pas la quitter Zer-2 va rappliquer, faire de l'art appliqué J'vais devoir jouer les crevards, plus qu'deux lattes à tirer Tous maladifs, touche pas la mif' ou j'vais te ratatiner Noichintok, jusqu'au Népal, je gère Poto, tu connais pas 2-Zer !? X2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon Ouais, tu connais pas 2-Zer ? Comment ça, tu connais pas 2-Zer ? Faut que j'devienne légendaire, que j'éclaire les lanternes mais Ici, c'est l'enfer depuis qu'j'vois mes frères s'faire enfermer Nique le système carcéral, j'ai pris flemme de passer àl Je préféré les décibels et puis les péritels des caméras Ne m'colle pas d'étiquette, j'bicrave des citernes de came hélas J'baise les fliquettes, éviscère des criquets de chaque tié-quar Nous allons nous équiper comme les p'tits mecs des favelas Le ballon, j'l'ai esquivé, j'ai fait vibrer des tas d'pétasses Wesh kafass ? Moi, j'froisse des spliffs La poisse m'esquive, j'suis la poussière dans l'mauvais il Tous les yeux m'guettent, à croire que j'm'exhibe Bandes de sales vermines, que pourrez-vous faire quand j'aurai l'seum ? Nada... Tu connais pas 2-Zer ? Écoute ça, c'est mamen 2-Zer x2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon Attention, je débarque ça va trouer des schnecks Et puis clouer des becs, t'es dégouté, t'es dèf Venez gouter mes textes, allez, courez les mecs Ca va couper des têtes, tout est prétexte à jouer les chefs Ouais, masquez vos pulsions, j'viens pas rouler des pelles Dans l'trou de tes fesses j'fait ma révolution Ouais, mate l'élocution, t'es un petit mytho si t'oses dire Qu'on est pas des pros du son, moi, j'te critique au micro, p'tit J'vai pas m'défiler, méfiez-vous, faut pas m'défier J'ai ves-qui les cours pour des filles, des sous Et des billets pourpres, j'ai mis d'côté les plaisirs des foufs Car j'en ai qu'une mais j'sais qu'vous m'désirez toutes L'argent, les thunes, mon but... Ouais, tu connais pas 2-Zer ? X2 Tu connais t'facon, ici, ma vie c'est Rue, drogue et baston, putes bonnes et d'la skunk Du rhum des glaçons, tu t'butes à l'actu Tu m'as vu sur des tas de sons, le plus mauvais garçon2</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2001</t>
+          <t>Djadja</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>PAGE EN COURS DE CONSTRUCTION !!!Annotation typeCliquez sur la lettre de votre choix pour accéder directement au raccourciABCDEFGHIJKLMNOPQRSTUVWXYZ113 13 Block 100 Blaze 404Billy 1995 2CheeseMilkShake 2zer Washington 3010 47ter 75ème SessionAA2H Abou Debeing Abou Tall Ademo Aketo Aladin 135 Aladoum Alain de l'ombre A Little Rooster Alkpote Alibi Montana Alonzo Alpha Wann AP Arcane Areno Jazz Darryl Zeuja Arsn Ashh Ashkidd ASF Ateyaba Joke Aya NakamuraBBadjer Baek Bakar Barack Adama Balou Bedjik Beeby Ben-J Biffty Bigflo Bigflo Oli Big Budha Cheez Big Yuss Bil-K Bilel Biwai Black D XV Barbar Black Kent Black M Blacko Bolemvn Bramsito Brav' Brulux Busta Flex Butter Bullets B-BifaceCCaballero Cahiips Caly.exe K-LY Canardo Casseurs Flowters Cenza Cheu-B XV Barbar Chilla Chris Karjack ColumbineDD6 Dabs Dadju Damlif Damso Dany Dan Davodka Darryl Zeuja Areno Jazz DA Uzi Dead Obies Deen Burbigo Dehmo Demi Portion Demon One Derka Despo Rutti Di-Meh Diabi Diddi Trix DIL Dinos Punchlinovic Disiz DJ Weedim Djadja Dinaz DJ X-Men Doc Gynéco Doks Don Choa Doomams Dosseh Double Å Doudou Masta Doums L'Entourage Dr Beriz Driver Dry DTFEEden Dillinger Eff Gee Elams El Matador Elyo Espiiem Esso LuxueuxFF430 FA2L Fababy Fanny Polly Féfé Bess Fidji Fixpen Sill F.L.O Flynt Fonky Family Fonky Flav' Franglish Freeze Corleone FrizGGeezy Georgio Ghetto Phénomène Gianni Gradur GRËJ Gringe Gros Mo Grodash Grünt GuizmoHH Magnum Hache-P Hamza Hayce Lemsi Heuss L'Enfoiré Hologram Lo' Hooss Houari Hippocampe Fou HyacintheII.N.C.H Beats Infinit Inso Le Veritable IxzoJJames Izmad Jarod Jason Voriz Jazzy Bazz JeanJass Jeff Le Nerf Jehkyl Jewel Usain JMK Joe Lucazz JoeyStarr Jok'Air John K Jorrdee Josman JR O'Chrome Juicy P JulKKaaris Kaddour Hadadi HK Kalash Kalash Criminel Kamelanc' Keblack Kekra Keny Arkana Kery James Kikesa Kobo Koba LaD Kohndo Koma Kool Shen K-Point KrisyLLa Famax La Fouine La Mannschaft La Race Canine LaCraps Lacrim Lartiste Laylow Lasco La Massfa La Smala L'Algerino L'Entourage Leck Lefa Les Alchimistes Lesram Les Tontons Flingueurs Le Rat Luciano Limsa D'Aulnay Lomepal Lonepsi Lord Kossity Lorenzo Luidji Lino L.I.O. Pétrodollars Lucci LTF Lucio Bukowski L'UzineMMac Kregor Mac Tyer Maître Gims Makala Mala Manu Key Maska MC Jean Gab'1 Médine Melan Omerta-Muzik Melopheelo MHD Mike Lucazz Minch Missak Mista Flo Mister You M le Maudit MOH Moha La Squale Mokless Mokobé Morsay MZ MMZNNakk Naps Nasty Yass LuXe Néfaste RSKP Nekfeu Nemir Nessbeal Ninho Niska Niro NOR N.O.S Nubi NuskyOOGB Oli Ol' Kainry Orelsan Ormaz Oxmo PuccinoPPaco Panama Bende Passi Patee Gee Phénomène Bizness Pit Baccardi PLK PNL Psy 4 de la Rime PSO ThugQRRed Cross Remy Retro X R.E.D.K. Rim'K Rizla RK Rob-D Dante Sito Rocca Rockin' Squat Rohff Romeo Elvis RowjaySSadek SAF Saloon Sam's Sanka Sat L'Artificier Sch S-Crew Scylla Sefyu Selim du 9.4 Senamo SetMatch Seth Gueko Sexion d'Assaut Shay Shone Holocost Shotas Shurik'N Sianna Siboy Sidi Sid Sinik Sirap Sir'klo Skreally Boy Sneazzy Snel Carter Sniper Sofiane Soprano Soso Maness Soul G Specta S.Pri Noir Still Fresh Suik'on Blaze AD Sultan Swagg Man Swift GuadTTristvn9 Take A Mic Taipan Teddy Corona Timal Tito Prince TLF The Shin Sekaï Tiers monde Tortoz Triplego TunisianoUUskyVVald Vaati Varnish La Piscine Veazy Veerus Veust Vicelow Vicenzo VM the Don Vîrus Volts Face Vrax VSO Le VaisseauWWalid Wit. Wizman Worms TXXGangs XVBarbarYYL Youri Tsar YoussouphaZZamdane Zesau Zeu Zeurti Zekwé Ramos Zola Zoxea11</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Djadja</t>
+          <t>L’heure tourne</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>PAGE EN COURS DE CONSTRUCTION !!!Annotation typeCliquez sur la lettre de votre choix pour accéder directement au raccourciABCDEFGHIJKLMNOPQRSTUVWXYZ113 13 Block 100 Blaze 404Billy 1995 2CheeseMilkShake 2zer Washington 3010 47ter 75ème SessionAA2H Abou Debeing Abou Tall Ademo Aketo Aladin 135 Aladoum Alain de l'ombre A Little Rooster Alkpote Alibi Montana Alonzo Alpha Wann AP Arcane Areno Jazz Darryl Zeuja Arsn Ashh Ashkidd ASF Ateyaba Joke Aya NakamuraBBadjer Baek Bakar Barack Adama Balou Bedjik Beeby Ben-J Biffty Bigflo Bigflo Oli Big Budha Cheez Big Yuss Bil-K Bilel Biwai Black D XV Barbar Black Kent Black M Blacko Bolemvn Bramsito Brav' Brulux Busta Flex Butter Bullets B-BifaceCCaballero Cahiips Caly.exe K-LY Canardo Casseurs Flowters Cenza Cheu-B XV Barbar Chilla Chris Karjack ColumbineDD6 Dabs Dadju Damlif Damso Dany Dan Davodka Darryl Zeuja Areno Jazz DA Uzi Dead Obies Deen Burbigo Dehmo Demi Portion Demon One Derka Despo Rutti Di-Meh Diabi Diddi Trix DIL Dinos Punchlinovic Disiz DJ Weedim Djadja Dinaz DJ X-Men Doc Gynéco Doks Don Choa Doomams Dosseh Double Å Doudou Masta Doums L'Entourage Dr Beriz Driver Dry DTFEEden Dillinger Eff Gee Elams El Matador Elyo Espiiem Esso LuxueuxFF430 FA2L Fababy Fanny Polly Féfé Bess Fidji Fixpen Sill F.L.O Flynt Fonky Family Fonky Flav' Franglish Freeze Corleone FrizGGeezy Georgio Ghetto Phénomène Gianni Gradur GRËJ Gringe Gros Mo Grodash Grünt GuizmoHH Magnum Hache-P Hamza Hayce Lemsi Heuss L'Enfoiré Hologram Lo' Hooss Houari Hippocampe Fou HyacintheII.N.C.H Beats Infinit Inso Le Veritable IxzoJJames Izmad Jarod Jason Voriz Jazzy Bazz JeanJass Jeff Le Nerf Jehkyl Jewel Usain JMK Joe Lucazz JoeyStarr Jok'Air John K Jorrdee Josman JR O'Chrome Juicy P JulKKaaris Kaddour Hadadi HK Kalash Kalash Criminel Kamelanc' Keblack Kekra Keny Arkana Kery James Kikesa Kobo Koba LaD Kohndo Koma Kool Shen K-Point KrisyLLa Famax La Fouine La Mannschaft La Race Canine LaCraps Lacrim Lartiste Laylow Lasco La Massfa La Smala L'Algerino L'Entourage Leck Lefa Les Alchimistes Lesram Les Tontons Flingueurs Le Rat Luciano Limsa D'Aulnay Lomepal Lonepsi Lord Kossity Lorenzo Luidji Lino L.I.O. Pétrodollars Lucci LTF Lucio Bukowski L'UzineMMac Kregor Mac Tyer Maître Gims Makala Mala Manu Key Maska MC Jean Gab'1 Médine Melan Omerta-Muzik Melopheelo MHD Mike Lucazz Minch Missak Mista Flo Mister You M le Maudit MOH Moha La Squale Mokless Mokobé Morsay MZ MMZNNakk Naps Nasty Yass LuXe Néfaste RSKP Nekfeu Nemir Nessbeal Ninho Niska Niro NOR N.O.S Nubi NuskyOOGB Oli Ol' Kainry Orelsan Ormaz Oxmo PuccinoPPaco Panama Bende Passi Patee Gee Phénomène Bizness Pit Baccardi PLK PNL Psy 4 de la Rime PSO ThugQRRed Cross Remy Retro X R.E.D.K. Rim'K Rizla RK Rob-D Dante Sito Rocca Rockin' Squat Rohff Romeo Elvis RowjaySSadek SAF Saloon Sam's Sanka Sat L'Artificier Sch S-Crew Scylla Sefyu Selim du 9.4 Senamo SetMatch Seth Gueko Sexion d'Assaut Shay Shone Holocost Shotas Shurik'N Sianna Siboy Sidi Sid Sinik Sirap Sir'klo Skreally Boy Sneazzy Snel Carter Sniper Sofiane Soprano Soso Maness Soul G Specta S.Pri Noir Still Fresh Suik'on Blaze AD Sultan Swagg Man Swift GuadTTristvn9 Take A Mic Taipan Teddy Corona Timal Tito Prince TLF The Shin Sekaï Tiers monde Tortoz Triplego TunisianoUUskyVVald Vaati Varnish La Piscine Veazy Veerus Veust Vicelow Vicenzo VM the Don Vîrus Volts Face Vrax VSO Le VaisseauWWalid Wit. Wizman Worms TXXGangs XVBarbarYYL Youri Tsar YoussouphaZZamdane Zesau Zeu Zeurti Zekwé Ramos Zola Zoxea11</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>L’heure tourne</t>
+          <t>No sizzurp</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Pédale, moi, j'ai pas le time, j'suis l'meilleur des pivots Nique les rivaux, j'place des ciseaux dans leur lucarne Zlatan Ça zigzague dans les rues d'Paname Vite, frappe si une pute nègre parle mal Ça bicrave dans les rues d'Paname Les flics passent, piquent une boulette par àl Fais pas le fou bête, barre-toi J'te lâche des bootlegs par 3 C'est pour mes zoulettes, mes poulettes moites Nan, j'fais des doux rêves, parfois M'en voulez pas, c'est ma génération On est fooleks, ça se voit On passe du rire aux larmes dans ma ville le soir Pour un petit regard, les types se braquent Puisqu'on est bourrés d'mala Bourrés d'mala, bourrés d'mala, bourrés d'mala Frérot, j'te parle de mon time où les gars préfèrent la maille Plutôt qu'les vacances, gérer les placements Le genre de ressoi dans les parcs où ça s'die et dès que ça rappe T'entends les agents mais je n'ai que 20 ans Donc laissez-moi vivre, je n'ai que 20 ans et trop d'choses à dire Dans ma valise, pas d'cess, nan, juste des combos d'rimes Des copeaux d'shit, rien de méchant et faut se le dire Les pronostics sont édifiants donc on est méfiants J'me sens sale quand je cède à mes plus sombres désirs Ici, les gens se trompent et dérivent Car c'est le vice qui comble les vides Et le temps passe, ouais, je peux te dire Que je veux le titre d'innovateur Moi, sous beuh, je rime avant qu'le feu se vide Faut qu'on m'idolâtre J'évite les mythomanes, ils perdent des kilogrammes À force de nous envier et de mendier, c'est immoral J'prends ça à la rigolade vu que ces psychopathes Disent de la merde, microphone en guise de vibromasseur J'ai ce sentiment de faire mauvaise impression Mais pourtant pour que j'fasse de la merde Faudrait droguer l'ingé son J'aime fracasser la rime et saccager Paris, j'vais Pas passer ma vie à me poser pleins d'questions Mais je sais que je suis l'un des meilleurs Tous les mecs qui me suivent, flinguent les haters Pour cramer tous tes mensonges Y'a même pas besoin d'un détecteur Comme d'habitude j'remue l'couteau dans la plaie Trop de flow, j'baise des tas de tes-pu sous l'eau, en apnée Frérot, j'te parle de mon time où les gars préfèrent la maille Plutôt qu'les vacances, gérer les placements Le genre de ressoi dans les parcs où ça s'die et dès que ça rappe T'entends les agents mais je n'ai que 20 ans Donc laissez-moi vivre, je n'ai que 20 ans et trop d'choses à dire Dans ma valise, pas d'cess, nan, juste des combos d'rimes Des copeaux d'shit, rien de méchant et faut se le dire Les pronostics sont édifiants donc on est méfiants Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Frérot, j'te parle de mon time, une heure de montage La tête ailleurs et l'embonpoint d'un fumeur de bon tahs Contracte des tumeurs de comptables Ou bien gravir des montagnes Le time est devenu biff donc pour la suite tu me raconte-rraah ! Content mais toujours pas d'contrat En même temps je l'ai ap' ché-cher Veau-cer gé-char d'une atmosphère déter' Et j'gère les virages tant bien que mal, dans la fumée Sans calculer, acculer les débauches qu'on peut assumer La bouche fermée juste les jours fériés Ces jacteuses foutent le seum À croire qu'personne les baffent dans tout c'merdier Bla bla bla... Ils rêvent de double meurtre mais dès qu'le jour se lève On fait ça pour de vrai, ouais, frangin Frérot, j'te parle de mon time où les gars préfèrent la maille Plutôt qu'les vacances, gérer les placements Le genre de ressoi dans les parcs où ça s'die et dès que ça rappe T'entends les agents mais je n'ai que 20 ans Donc laissez-moi vivre, je n'ai que 20 ans et trop d'choses à dire Dans ma valise, pas d'cess, nan, juste des combos d'rimes Des copeaux d'shit, rien de méchant et faut se le dire Les pronostics sont édifiants donc on est méfiants Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam 2</t>
         </is>
       </c>
     </row>
@@ -1393,12 +1393,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>No sizzurp</t>
+          <t>La loi du plus fort</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Pédale, moi, j'ai pas le time, j'suis l'meilleur des pivots Nique les rivaux, j'place des ciseaux dans leur lucarne Zlatan Ça zigzague dans les rues d'Paname Vite, frappe si une pute nègre parle mal Ça bicrave dans les rues d'Paname Les flics passent, piquent une boulette par àl Fais pas le fou bête, barre-toi J'te lâche des bootlegs par 3 C'est pour mes zoulettes, mes poulettes moites Nan, j'fais des doux rêves, parfois M'en voulez pas, c'est ma génération On est fooleks, ça se voit On passe du rire aux larmes dans ma ville le soir Pour un petit regard, les types se braquent Puisqu'on est bourrés d'mala Bourrés d'mala, bourrés d'mala, bourrés d'mala Frérot, j'te parle de mon time où les gars préfèrent la maille Plutôt qu'les vacances, gérer les placements Le genre de ressoi dans les parcs où ça s'die et dès que ça rappe T'entends les agents mais je n'ai que 20 ans Donc laissez-moi vivre, je n'ai que 20 ans et trop d'choses à dire Dans ma valise, pas d'cess, nan, juste des combos d'rimes Des copeaux d'shit, rien de méchant et faut se le dire Les pronostics sont édifiants donc on est méfiants J'me sens sale quand je cède à mes plus sombres désirs Ici, les gens se trompent et dérivent Car c'est le vice qui comble les vides Et le temps passe, ouais, je peux te dire Que je veux le titre d'innovateur Moi, sous beuh, je rime avant qu'le feu se vide Faut qu'on m'idolâtre J'évite les mythomanes, ils perdent des kilogrammes À force de nous envier et de mendier, c'est immoral J'prends ça à la rigolade vu que ces psychopathes Disent de la merde, microphone en guise de vibromasseur J'ai ce sentiment de faire mauvaise impression Mais pourtant pour que j'fasse de la merde Faudrait droguer l'ingé son J'aime fracasser la rime et saccager Paris, j'vais Pas passer ma vie à me poser pleins d'questions Mais je sais que je suis l'un des meilleurs Tous les mecs qui me suivent, flinguent les haters Pour cramer tous tes mensonges Y'a même pas besoin d'un détecteur Comme d'habitude j'remue l'couteau dans la plaie Trop de flow, j'baise des tas de tes-pu sous l'eau, en apnée Frérot, j'te parle de mon time où les gars préfèrent la maille Plutôt qu'les vacances, gérer les placements Le genre de ressoi dans les parcs où ça s'die et dès que ça rappe T'entends les agents mais je n'ai que 20 ans Donc laissez-moi vivre, je n'ai que 20 ans et trop d'choses à dire Dans ma valise, pas d'cess, nan, juste des combos d'rimes Des copeaux d'shit, rien de méchant et faut se le dire Les pronostics sont édifiants donc on est méfiants Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Frérot, j'te parle de mon time, une heure de montage La tête ailleurs et l'embonpoint d'un fumeur de bon tahs Contracte des tumeurs de comptables Ou bien gravir des montagnes Le time est devenu biff donc pour la suite tu me raconte-rraah ! Content mais toujours pas d'contrat En même temps je l'ai ap' ché-cher Veau-cer gé-char d'une atmosphère déter' Et j'gère les virages tant bien que mal, dans la fumée Sans calculer, acculer les débauches qu'on peut assumer La bouche fermée juste les jours fériés Ces jacteuses foutent le seum À croire qu'personne les baffent dans tout c'merdier Bla bla bla... Ils rêvent de double meurtre mais dès qu'le jour se lève On fait ça pour de vrai, ouais, frangin Frérot, j'te parle de mon time où les gars préfèrent la maille Plutôt qu'les vacances, gérer les placements Le genre de ressoi dans les parcs où ça s'die et dès que ça rappe T'entends les agents mais je n'ai que 20 ans Donc laissez-moi vivre, je n'ai que 20 ans et trop d'choses à dire Dans ma valise, pas d'cess, nan, juste des combos d'rimes Des copeaux d'shit, rien de méchant et faut se le dire Les pronostics sont édifiants donc on est méfiants Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam Instagram, sticks et sticks en kilogrammes Bourré, bourré, j'me rétame, où ça ? À Amsterdam 2</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -1410,12 +1410,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>La loi du plus fort</t>
+          <t>30 minutes de Freestyle dans le Planète Rap de Nekfeu</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Fais-moi voir ton côté intelectuel J'veux pas voir ton cul mais ton QI Pourquoi tu mets des bas résilles sur ton cerveau ? J'fais du gyneco, pas d'la philo T'es l'gars devant la porte qu'essaie de rentrer Tu connais même pas leurs codes Même si t'as l'dress-code, ils vont te bloquer Ta date de naissance, le nom d'ta belle-mêre Essaie tous les chiffres que tu connais Mais sache que la porte ne s'ouvrira jamais Et si tu t'demandes comment j'suis rentré J'ai juste poussé la porte, t'as oublié d'essayé J'ai pas d'problèmes avec Gavalda Mais j'mets pas d'science dans mon peu-Ra J'fais partie des gens simples et j'réfléchis pas Fais un voyage d'étude à BLC, dans la zone 4, aux Michelettes De la droiture avant l'cash, quand la vie t'rend muet Mon nom sur une vitre embuée avant l'crash de la voiture C'est comme ça qu'j'vois le Rap une écriture insignifiante Avant qu'on parte, le dernier cri d'une jeunesse édifiante Personne t'explique la vie, c'est un chemin introspectif L'unique défi, schéma atroce Une ligne de fuite pour perspective d'avenir Nos vies sont crades donc on défonce notre crâne Et plus j'connais la musique, plus j'aime les fausses notes Ce soir, ça part en impro, parait qu'ça kicke pas mal Comme Doc Gyneco, j'veux atteindre le nirvana Ouais, mon gars, tu sais bien, c'est pour les tiques-fana Mais surtout pour les frères qui sont là depuis l'début, là-bas Ceux qui écoutent depuis Paname, qui mettent pas de soupape C'est l'tou-bab toujours coupable, tu vois bien qu'tout part Tout l'monde parle de ça, tout l'monde parle de nous C'est comme ça qu'ça s'passe, j'arrive à pas de loup Afflelou comme Alph Lau', c'est comme ça qu'ça s'passe On a l'flow, on a le Ralph Lau', vas-y, Doums, balance le flow OK, on balance ça avec le popo Rien à foutre de tous ces pédés, nique la po-po -lice, j'arrive avec mes gars, on est posés àl Pour l'album de Nekfeu, on crache weed et flammes Que aç avec mes gars laxistes Pourquoi tu veux nous tester, négro, là ? Oui, j'insiste Pour te dire que c'est le fire, putain, oui, c'est trop dar On est des mecs de Paname, t'inquiète qu'on a la flamme Olympique, on baise ces pitres, rien à foutre de ces bitchs J'arrive avec mes gars et j'te rackette depuis les Pitch's Fucked up, j'en place pour mes gavas du 9 Qui va kicker ça ? Vas-y, balance ça, mon reuf J'ai le flow embrumé, en plus, j'suis enrhumé On vient pas pour t'entuber, le studio est enfumé Car y'a Doums et y'a Doc Gyneco, c'est bon ça C'est pour tous les mecs qui nnait-co, c'est comme ça C'est comme ça qu'on l'fait, on a les codes, fuck l'école Fuck les cops quand ils sont pas sympas C'est comme ça qu'ça s'passe sur l'instru Framal, j'sens qu't'es prêt à partir, c'est l'départ Fais ça vite comme un guépard, yeah Hé, putain, j'suis chire-dé, j'suis fonce-dé Qu'est-ce qu'tu demandes de faire ? A cette heure-ci, putain, j'sais pas quoi faire On m'appelle Doc alors j'vais t'mettre à l'heure Mais t'es mon petit frère alors je t'aime et j'te parle avec le cur Putain, les phrases elles sont longues J'arrive à débiter mais j'sais pas quoi t'dire J'ai pas assez d'feuilles longues et j'peux pas fumer Merde, putain, vous êtes sûrs que j'peux pas donner ? Oh, et puis j'donne à l'ancienne, on dirait Lionel D Fuck ton crew, sale pédale, ça bouge ap T'es tout naze, écoute, ça fait breh ! Rien qu'on fait des classiques, S-Crew, le nom d'mon gang Y'a que dans l'ombre qu'on tranche pour pas finir aux assises Souvent dans un camouflage vert kaki L'ambiance est pourave, y'a des toux grasses ça vi-ser d'la weed Ici, tu perds ta vie, on t'nique ta mère à 6 Une bonne paire de Nike Air dans la tête, c'est facile Le leust est entouré donc on fait ça à notre manière Bientôt le L est en tournée donc prenez garde à vos arrières Bitch ! Et toi, dis moi pourquoi tu causes On est au festival de Cannes, toi, tu traînes à la Foire du Trône Comme l'Homme de l'Est, j'attends l'apocalypse Je profite avant qu'on m'refroidisse, avant qu'ma peau palisse Dans mon ciboulot, j'suis mitigé, oui, si j'ai un petit boulot Un salaire, j'irais prendre l'air même si j'vivais ma vie sous l'eau Le Rap me dégoûte comme les pires aspects des filles gâtées J'vais vite gratter malgré que j'dérive, là, mais j'déprime jamais Les vices cachés des miss fâchées, ça entraine des vies gâchées Dédicacer des petites tasses-pé ? Autant caner déshydraté Ma vie d'avant, merde ! J'peux pas la quitter Zer-2 va rappliquer, faire de l'art appliqué J'vais devoir jouer les crevards, plus qu'deux lattes à tirer Tous maladifs, touche pas la mif' ou j'vais te ratatiner Faut que j'devienne légendaire, que j'éclaire les lanternes mais Ici, c'est l'enfer depuis qu'j'vois mes frères s'faire enfermer Nique le système carcéral, j'ai pris flemme de passer àl Je préféré les décibels et puis les péritels des caméras Ne m'colle pas d'étiquette, j'bicrave des citernes de came hélas J'baise les fliquettes, éviscère des criquets de chaque tié-quar Nous allons nous équiper comme les p'tits mecs des favelas Le ballon, j'l'ai esquivé, j'ai fait vibrer des tas d'pétasses Wesh kafass ? Moi, j'froisse des spliffs La poisse m'esquive, j'suis la poussière dans l'mauvais il Tous les yeux m'guettent, à croire que j'm'exhibe Bandes de sales vermines, que pourrez-vous faire quand j'aurai l'seum ? Nada, ça va trouer des schnecks Et puis clouer des becs, t'es dégouté, t'es dèf Venez gouter mes textes, allez, courez les mecs Ca va couper des têtes, tout est prétexte à jouer les chefs Ouais, masquez vos pulsions, j'viens pas rouler des pelles Dans l'trou de tes fesses j'fait ma révolution Je suis ce shaolin intégrant le Rap aux arts martiaux Quand t'es déjà au lit, transformant le cro-mi en arme d'acier Que celui qui parle de la vie des autres regarde la sienne Trop d'astreintes, on passe plus de temps A s'plaindre qu'à remercier, que Dieu m'pardonne Dans la vie aucun format simple, mes reufs à l'instinct carnassier Vendent plus de drogue qu'un pharmacien J'ai qu'l'envie d'karna ces mêmes clones Coulée dhémoglobine, le mic' s'tache Un texte de Mac de mon clan clean Pendant qu'les mecs s'touchent Ça peut ler-par mon premier flow s'appelait placentas Je sors du sas et rentre dans l'south quand mon soss' place un tag Teubé sors ton nez d'la poudre J'suis un peu désordonné mais rien à tref' des ordres donnés J'entends que des remarques, personne le fait mieux, à part ça On m'appelle Dead Man, A.K.A le vieux bâtard sale On a pas d'manager et l'équipe fait sa com', ça-comme On a pas d'mal à gérer, c'est toujours 5050, ça cogne, ça cogne C'est comme quand les keufs courent te rattraper Le juge goûtera la joie quand, toi, tu goûteras ta peine Quelques gouttes de Rap, à peine Sauf que maintenant, c'est plus des essais On peut conclure en ce sens qu'la concurrence pue des aisselles Que faire de plus, gars ? À part les effacer Yo, sucez moi bien jusqu'à, la paralysie faciale ×2 T'es le boss de qui ? T'es le boss de quoi ? Tu te prends pour qui ? Tu te prends pour quoi ? Pourquoi tu tires ? Ici, ça tire Alors rentre chez 'oit c'est l'son du ghetto Et si tu connais pas mon blaze, c'est B.2O.Z.2O Si y'a d'la monnaie j'suis chaud, y'aura pas besoin d'me ffer-chau J'aime pas les fachos, veulent voir les blacks au cachot , c'est trop chaud mais, moi, j'suis dans l'pochon Je te ferai pas l'amour, bitch, t'as les pieds de cochon Le jour où je vais prendre du gallon Mes deux bras seront trop longs, frelon, j'vais ramener des ballons C'est pour mes gars sûrs et certains Bakary 93.150, on a des couilles en béton , j'lui montre ma tête de python Des billets violets dans un putain d'sac Louis Vuitton Rien à foutre même si ils ont débranché la table Faut pas déranger madame, faut pas mélanger la came C'est comme ça qu'ça s'passe, j'ai un truc macabre J'dis n'importe quoi pour gagner du temps car y'a blanco C'est comme ça qu'ça s'passe, c'est pour les gars de Blankok Tu vas bouncer jusqu'à Bangkok, t'sais, quand mon gang cogne C'est comme un gomme-cogne comme à Boston Retour des shinobis mais crois pas que c'est l'fric notre pilier J'compte plus les rivaux pliés encore immobiles On a acquis notre biz comme Nino B., Jack City Faut qu'on s'lance dans l'immobilier, faut qu'on multiplie nos billes Crois qu'les paillettes et les strass' vont aliéner mes srhabs Ils trouvent mes alliés détestables Ils s'disent Ça y est, c'est des stars On passe à base de tasses calientes, slash, variétés d'sapes On confond plus les Cayenne et les Smart Très vite, les bitchs voient que j'évite les filles d'joie J'effrite et puis j'bois, si l'ennemi s'précise Très vite l'équipe s'équipe, méfie-toi On fait l'beurre, on intercepte le cash, ton espèce De garce veut réchauffer mon cur et mon zgeg de glace On laissera les archives, ouais, Phaal gifle J'envoie les dragées, j'les laisse à l'état léthargique Trop d'écart j'les calcine, les garces s'écartent vite On est classes, on te-cla les gares-ci J'appelle ta pétasse Bécassine Oublie la paix, kho, on monte de 0 à 100 Verse pour les frérots absents pendant l'apéro J'ai la conscience qui part en couille, tu vas galérer pour m'cerner Regarde le diable partir en douce avant qu'tu t'enfonces dans le gouffre J'te regarde, t'as vraiment pas de fouf et j'me sens pas concerné J'ai vu des guesh en pleine se-cri, c'est par le nez qu'ils gerbaient Petit message pour toi raciste avec ta face d'alien Tu veux nous briser, maitriser, enculé d'ta race aryenne Regarde-moi Marianne, putain, non, je n'vais pas chipoter Ton pays m'rend toxico, t'es bien la pire des home sweet home La vie n'est pas un roman, tout s'accumule comme des briques donc tu laisses place à l'arrogance Le soir tu veilles, tu parles à ta 'teille, tu dragues dans ta tête T'espères la fortune de Karl Lagarfeld, c'est le carnage infernal Bien évidemment, cela va faire mal, j'en perds ma rancur comme le but de mon exercice On n'fait qu'm'exorciser pour qu'je m'éclaircisse Tu veux tester mes salauds, ça fait bang, genre saloon Frère, si je t'allume c'est que j'suis prêt pour l'salut T'es pas d'la mif, parle-moi biff ou parle-moi d'profit Dix kilos d'weed, un kilo d'shit, le tout sera blanchi On fume le matos, mes vatos vont tuer ces rappeurs Ça sera du gâteau comme rotte-ca le XXX de l'éducateur A bord d'une Merco Benz, vitres teintées, grosse boisson C'est la moisson, les mousseux sont d'sortie, ouais Rentre dans le VIP si tu veux changer de vie Si tu rentres dans le lit, sache qu'on rentre dans le mille J'suis un hot nigga Mes gavas derrière oim ne craignent que God, nigga Mon équipe pète les scores pendant qu'tu t'fichas, kho Rebeu, renois, babtous, chicanos Tes négros softs ont des chichas roses Suffit pas d'pomper tous les rappeurs de Chicago Bien souvent, c'est pour une poule que démarre un combat d'coq A Paname, ça s'embrouille autour d'une boite duf Si t'as l'moral dans l'zen, sache que je l'ai dans la poche mon boule, j'me confesse sur la prod Man, c'est D6 le barge Toujours posé fonce-dé dans ton canap' quand la pénombre se cache Un moment d'colère face à c'monde de lâche On dit qu'le vent l'emporte mais je ne suis qu'un rocher Resté accroché à un moule façonné par lÉlysée Pour eux, nous sommes des poules prêtes à s'faire plumer J'survis devant 2012, j'vis l'enfer C'est sur la Seine que les premières lueurs du matin déteignent L'humanité meurt depuis qu'on a quitté l'Jardin d'Éden On a le rêve dans le cur, le cauchemar dans les veines Mais plus je monte et plus j'm'identifie à Martin Eden Moi, j'suis un babtou à part j'vois plein de babtous pompeux Mais sache que les babtous comme moi N'aiment pas les babtous comme eux Surtout quand les babtous ont peur Tout l'monde m'invite dans les plans Fils de pute, bien sûr qu'c'est plus facile pour toi quand t'es blanc Les riches font partie des plus radins dans cet empire de piranhas Parfois, j'reconnais même plus ma patrie comme mon pote Iranien T'oublies tout tellement tu rappes, hein, obligé d'se mentir un peu Du genre si jamais j'mets c'panier du premier coup, tout ira bien J'ai jamais tté-gra, t'as rien quand tu taffes peu Il m'faut un casque intégral J'vais braquer l'industrie comme les Daft Punk J'ai la rage d'un animal, cannibale, poto, j'manie l'mic Mais j'suis resté sur l'carreau Comme une chemise de Charles Ingalls J'garde la foi comme Abidal, hélas, le cash est capital Rebeu, la carte bleu c'est la seule carte qui soit vitale Bah ouais, j'ai eu des bonnes notes sans ter-chan Trempé dans de sales affaires, j'ai eu mon bac en séchant J'péra c'est embêtant, j'aime pas danser j'suis lancé dans La vie, tout l'monde peut s'en sortir, j'veux juste lui rentrer dedans Car j'ai grandi à Aulnay-Sous, Emmaüs la favelas On nique les chevaliers, qu'ils soient d'la rue ou d'Athéna Compte pas sur nous pour parler quand les schtars débarquent Pas d'messes basses, les keufs tournent, silence des cathédrales J'ai compris qu'les faux potes et l'honneur font bande à part Quand la haine, l'amour et la jalousie font des plans à trois J'donne plus d'amour à la rue, elle m'le rendra pas Comment faire partie des meubles Sans finir dans un grand placard ? Dans l'peu-Ra, trop d'suceurs qui m'foutent le seum Fermez vos gueules, si on est cheum, vous êtes tous plus cheum J'suis ce jeune parisien, américain dans l'état d'esprit Prends rendez-vous avec ton médecin légiste Ici, en plus des gouttes de pluie, souvent les coups pleuvent Mon crew est fait de vrais amis, à ton avis Pourquoi les putes se retrouvent toutes seules ? J'écris des rimes, j'envoie des torgnoles de malade Et pourtant, j'ai pas lu d'livre depuis TomTom Nana J'sors du Mordor de Paname, viens la bonne drogue est par là Une grosse pensée à nos proches pour qui l'horloge s'emballa Moi, j'suis debout, au-dessus d'moi, je vois voler les corbeaux J'ai besoin de joindre les deux bouts avant d'recoller les morceaux Tu mets des coups d'épée dans l'eau, l'affreux, on s'propage Prépare tes adieux, on fout le feu comme des Ghostriders Il faut que toutes les mains se lèvent haut Rimes façon West Coast, Gangsta à la Death Row On fuck les ennemis, miskine, ils se croient peut-être drôles Ça cartonne comme au rallye, on cartonne même sans khaliss Mes alliés se rallient, mental de patron On ne dit pas pardon, y'a que comme ça que tu seras libre Si j'tombe à Fleury, c'est qu'y a un beau million à prendre Ou qu'y a une tombe à fleurir, les tes-trai vont prendre des pralines J'ai pas vu d'boulot tendre Faut prendre pas l'9ar9ob face à la drogue Ils ont la boule au ventre, on a des abdos Les traitres sont de vraies balances Wesh, mais tétais dla bande, ouais, ouais, ouais... Faut quon tsaigne avant qutu mènes la danse Lami est éphémère, yen a qui parlent derrière ton dos Yen a même qui tbaisent et prennent ton cash, bellek, mon soss Putain de merde ! Cest quoi ce délire de faire Le soss et voler dans les mêmes dièses, oser se dire deux frères ? Tous hypocrites, les gens thypnotisent Leurs masques cachent leurs émotions et se disent trop vif Yen a qui servent du charme et te font croire à des rêves dars Et yen a qui tcachent des choses, et ouais, pour pas te faire mal Trop dacteurs, de squatteurs, de bâtards, de gratteurs de biff Faut des valeurs, le malheur tarrache la peur de vivre</t>
         </is>
       </c>
     </row>
@@ -1427,12 +1427,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>30 minutes de Freestyle dans le Planète Rap de Nekfeu</t>
+          <t>Ton nouveau pote</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Fais-moi voir ton côté intelectuel J'veux pas voir ton cul mais ton QI Pourquoi tu mets des bas résilles sur ton cerveau ? J'fais du gyneco, pas d'la philo T'es l'gars devant la porte qu'essaie de rentrer Tu connais même pas leurs codes Même si t'as l'dress-code, ils vont te bloquer Ta date de naissance, le nom d'ta belle-mêre Essaie tous les chiffres que tu connais Mais sache que la porte ne s'ouvrira jamais Et si tu t'demandes comment j'suis rentré J'ai juste poussé la porte, t'as oublié d'essayé J'ai pas d'problèmes avec Gavalda Mais j'mets pas d'science dans mon peu-Ra J'fais partie des gens simples et j'réfléchis pas Fais un voyage d'étude à BLC, dans la zone 4, aux Michelettes De la droiture avant l'cash, quand la vie t'rend muet Mon nom sur une vitre embuée avant l'crash de la voiture C'est comme ça qu'j'vois le Rap une écriture insignifiante Avant qu'on parte, le dernier cri d'une jeunesse édifiante Personne t'explique la vie, c'est un chemin introspectif L'unique défi, schéma atroce Une ligne de fuite pour perspective d'avenir Nos vies sont crades donc on défonce notre crâne Et plus j'connais la musique, plus j'aime les fausses notes Ce soir, ça part en impro, parait qu'ça kicke pas mal Comme Doc Gyneco, j'veux atteindre le nirvana Ouais, mon gars, tu sais bien, c'est pour les tiques-fana Mais surtout pour les frères qui sont là depuis l'début, là-bas Ceux qui écoutent depuis Paname, qui mettent pas de soupape C'est l'tou-bab toujours coupable, tu vois bien qu'tout part Tout l'monde parle de ça, tout l'monde parle de nous C'est comme ça qu'ça s'passe, j'arrive à pas de loup Afflelou comme Alph Lau', c'est comme ça qu'ça s'passe On a l'flow, on a le Ralph Lau', vas-y, Doums, balance le flow OK, on balance ça avec le popo Rien à foutre de tous ces pédés, nique la po-po -lice, j'arrive avec mes gars, on est posés àl Pour l'album de Nekfeu, on crache weed et flammes Que aç avec mes gars laxistes Pourquoi tu veux nous tester, négro, là ? Oui, j'insiste Pour te dire que c'est le fire, putain, oui, c'est trop dar On est des mecs de Paname, t'inquiète qu'on a la flamme Olympique, on baise ces pitres, rien à foutre de ces bitchs J'arrive avec mes gars et j'te rackette depuis les Pitch's Fucked up, j'en place pour mes gavas du 9 Qui va kicker ça ? Vas-y, balance ça, mon reuf J'ai le flow embrumé, en plus, j'suis enrhumé On vient pas pour t'entuber, le studio est enfumé Car y'a Doums et y'a Doc Gyneco, c'est bon ça C'est pour tous les mecs qui nnait-co, c'est comme ça C'est comme ça qu'on l'fait, on a les codes, fuck l'école Fuck les cops quand ils sont pas sympas C'est comme ça qu'ça s'passe sur l'instru Framal, j'sens qu't'es prêt à partir, c'est l'départ Fais ça vite comme un guépard, yeah Hé, putain, j'suis chire-dé, j'suis fonce-dé Qu'est-ce qu'tu demandes de faire ? A cette heure-ci, putain, j'sais pas quoi faire On m'appelle Doc alors j'vais t'mettre à l'heure Mais t'es mon petit frère alors je t'aime et j'te parle avec le cur Putain, les phrases elles sont longues J'arrive à débiter mais j'sais pas quoi t'dire J'ai pas assez d'feuilles longues et j'peux pas fumer Merde, putain, vous êtes sûrs que j'peux pas donner ? Oh, et puis j'donne à l'ancienne, on dirait Lionel D Fuck ton crew, sale pédale, ça bouge ap T'es tout naze, écoute, ça fait breh ! Rien qu'on fait des classiques, S-Crew, le nom d'mon gang Y'a que dans l'ombre qu'on tranche pour pas finir aux assises Souvent dans un camouflage vert kaki L'ambiance est pourave, y'a des toux grasses ça vi-ser d'la weed Ici, tu perds ta vie, on t'nique ta mère à 6 Une bonne paire de Nike Air dans la tête, c'est facile Le leust est entouré donc on fait ça à notre manière Bientôt le L est en tournée donc prenez garde à vos arrières Bitch ! Et toi, dis moi pourquoi tu causes On est au festival de Cannes, toi, tu traînes à la Foire du Trône Comme l'Homme de l'Est, j'attends l'apocalypse Je profite avant qu'on m'refroidisse, avant qu'ma peau palisse Dans mon ciboulot, j'suis mitigé, oui, si j'ai un petit boulot Un salaire, j'irais prendre l'air même si j'vivais ma vie sous l'eau Le Rap me dégoûte comme les pires aspects des filles gâtées J'vais vite gratter malgré que j'dérive, là, mais j'déprime jamais Les vices cachés des miss fâchées, ça entraine des vies gâchées Dédicacer des petites tasses-pé ? Autant caner déshydraté Ma vie d'avant, merde ! J'peux pas la quitter Zer-2 va rappliquer, faire de l'art appliqué J'vais devoir jouer les crevards, plus qu'deux lattes à tirer Tous maladifs, touche pas la mif' ou j'vais te ratatiner Faut que j'devienne légendaire, que j'éclaire les lanternes mais Ici, c'est l'enfer depuis qu'j'vois mes frères s'faire enfermer Nique le système carcéral, j'ai pris flemme de passer àl Je préféré les décibels et puis les péritels des caméras Ne m'colle pas d'étiquette, j'bicrave des citernes de came hélas J'baise les fliquettes, éviscère des criquets de chaque tié-quar Nous allons nous équiper comme les p'tits mecs des favelas Le ballon, j'l'ai esquivé, j'ai fait vibrer des tas d'pétasses Wesh kafass ? Moi, j'froisse des spliffs La poisse m'esquive, j'suis la poussière dans l'mauvais il Tous les yeux m'guettent, à croire que j'm'exhibe Bandes de sales vermines, que pourrez-vous faire quand j'aurai l'seum ? Nada, ça va trouer des schnecks Et puis clouer des becs, t'es dégouté, t'es dèf Venez gouter mes textes, allez, courez les mecs Ca va couper des têtes, tout est prétexte à jouer les chefs Ouais, masquez vos pulsions, j'viens pas rouler des pelles Dans l'trou de tes fesses j'fait ma révolution Je suis ce shaolin intégrant le Rap aux arts martiaux Quand t'es déjà au lit, transformant le cro-mi en arme d'acier Que celui qui parle de la vie des autres regarde la sienne Trop d'astreintes, on passe plus de temps A s'plaindre qu'à remercier, que Dieu m'pardonne Dans la vie aucun format simple, mes reufs à l'instinct carnassier Vendent plus de drogue qu'un pharmacien J'ai qu'l'envie d'karna ces mêmes clones Coulée dhémoglobine, le mic' s'tache Un texte de Mac de mon clan clean Pendant qu'les mecs s'touchent Ça peut ler-par mon premier flow s'appelait placentas Je sors du sas et rentre dans l'south quand mon soss' place un tag Teubé sors ton nez d'la poudre J'suis un peu désordonné mais rien à tref' des ordres donnés J'entends que des remarques, personne le fait mieux, à part ça On m'appelle Dead Man, A.K.A le vieux bâtard sale On a pas d'manager et l'équipe fait sa com', ça-comme On a pas d'mal à gérer, c'est toujours 5050, ça cogne, ça cogne C'est comme quand les keufs courent te rattraper Le juge goûtera la joie quand, toi, tu goûteras ta peine Quelques gouttes de Rap, à peine Sauf que maintenant, c'est plus des essais On peut conclure en ce sens qu'la concurrence pue des aisselles Que faire de plus, gars ? À part les effacer Yo, sucez moi bien jusqu'à, la paralysie faciale ×2 T'es le boss de qui ? T'es le boss de quoi ? Tu te prends pour qui ? Tu te prends pour quoi ? Pourquoi tu tires ? Ici, ça tire Alors rentre chez 'oit c'est l'son du ghetto Et si tu connais pas mon blaze, c'est B.2O.Z.2O Si y'a d'la monnaie j'suis chaud, y'aura pas besoin d'me ffer-chau J'aime pas les fachos, veulent voir les blacks au cachot , c'est trop chaud mais, moi, j'suis dans l'pochon Je te ferai pas l'amour, bitch, t'as les pieds de cochon Le jour où je vais prendre du gallon Mes deux bras seront trop longs, frelon, j'vais ramener des ballons C'est pour mes gars sûrs et certains Bakary 93.150, on a des couilles en béton , j'lui montre ma tête de python Des billets violets dans un putain d'sac Louis Vuitton Rien à foutre même si ils ont débranché la table Faut pas déranger madame, faut pas mélanger la came C'est comme ça qu'ça s'passe, j'ai un truc macabre J'dis n'importe quoi pour gagner du temps car y'a blanco C'est comme ça qu'ça s'passe, c'est pour les gars de Blankok Tu vas bouncer jusqu'à Bangkok, t'sais, quand mon gang cogne C'est comme un gomme-cogne comme à Boston Retour des shinobis mais crois pas que c'est l'fric notre pilier J'compte plus les rivaux pliés encore immobiles On a acquis notre biz comme Nino B., Jack City Faut qu'on s'lance dans l'immobilier, faut qu'on multiplie nos billes Crois qu'les paillettes et les strass' vont aliéner mes srhabs Ils trouvent mes alliés détestables Ils s'disent Ça y est, c'est des stars On passe à base de tasses calientes, slash, variétés d'sapes On confond plus les Cayenne et les Smart Très vite, les bitchs voient que j'évite les filles d'joie J'effrite et puis j'bois, si l'ennemi s'précise Très vite l'équipe s'équipe, méfie-toi On fait l'beurre, on intercepte le cash, ton espèce De garce veut réchauffer mon cur et mon zgeg de glace On laissera les archives, ouais, Phaal gifle J'envoie les dragées, j'les laisse à l'état léthargique Trop d'écart j'les calcine, les garces s'écartent vite On est classes, on te-cla les gares-ci J'appelle ta pétasse Bécassine Oublie la paix, kho, on monte de 0 à 100 Verse pour les frérots absents pendant l'apéro J'ai la conscience qui part en couille, tu vas galérer pour m'cerner Regarde le diable partir en douce avant qu'tu t'enfonces dans le gouffre J'te regarde, t'as vraiment pas de fouf et j'me sens pas concerné J'ai vu des guesh en pleine se-cri, c'est par le nez qu'ils gerbaient Petit message pour toi raciste avec ta face d'alien Tu veux nous briser, maitriser, enculé d'ta race aryenne Regarde-moi Marianne, putain, non, je n'vais pas chipoter Ton pays m'rend toxico, t'es bien la pire des home sweet home La vie n'est pas un roman, tout s'accumule comme des briques donc tu laisses place à l'arrogance Le soir tu veilles, tu parles à ta 'teille, tu dragues dans ta tête T'espères la fortune de Karl Lagarfeld, c'est le carnage infernal Bien évidemment, cela va faire mal, j'en perds ma rancur comme le but de mon exercice On n'fait qu'm'exorciser pour qu'je m'éclaircisse Tu veux tester mes salauds, ça fait bang, genre saloon Frère, si je t'allume c'est que j'suis prêt pour l'salut T'es pas d'la mif, parle-moi biff ou parle-moi d'profit Dix kilos d'weed, un kilo d'shit, le tout sera blanchi On fume le matos, mes vatos vont tuer ces rappeurs Ça sera du gâteau comme rotte-ca le XXX de l'éducateur A bord d'une Merco Benz, vitres teintées, grosse boisson C'est la moisson, les mousseux sont d'sortie, ouais Rentre dans le VIP si tu veux changer de vie Si tu rentres dans le lit, sache qu'on rentre dans le mille J'suis un hot nigga Mes gavas derrière oim ne craignent que God, nigga Mon équipe pète les scores pendant qu'tu t'fichas, kho Rebeu, renois, babtous, chicanos Tes négros softs ont des chichas roses Suffit pas d'pomper tous les rappeurs de Chicago Bien souvent, c'est pour une poule que démarre un combat d'coq A Paname, ça s'embrouille autour d'une boite duf Si t'as l'moral dans l'zen, sache que je l'ai dans la poche mon boule, j'me confesse sur la prod Man, c'est D6 le barge Toujours posé fonce-dé dans ton canap' quand la pénombre se cache Un moment d'colère face à c'monde de lâche On dit qu'le vent l'emporte mais je ne suis qu'un rocher Resté accroché à un moule façonné par lÉlysée Pour eux, nous sommes des poules prêtes à s'faire plumer J'survis devant 2012, j'vis l'enfer C'est sur la Seine que les premières lueurs du matin déteignent L'humanité meurt depuis qu'on a quitté l'Jardin d'Éden On a le rêve dans le cur, le cauchemar dans les veines Mais plus je monte et plus j'm'identifie à Martin Eden Moi, j'suis un babtou à part j'vois plein de babtous pompeux Mais sache que les babtous comme moi N'aiment pas les babtous comme eux Surtout quand les babtous ont peur Tout l'monde m'invite dans les plans Fils de pute, bien sûr qu'c'est plus facile pour toi quand t'es blanc Les riches font partie des plus radins dans cet empire de piranhas Parfois, j'reconnais même plus ma patrie comme mon pote Iranien T'oublies tout tellement tu rappes, hein, obligé d'se mentir un peu Du genre si jamais j'mets c'panier du premier coup, tout ira bien J'ai jamais tté-gra, t'as rien quand tu taffes peu Il m'faut un casque intégral J'vais braquer l'industrie comme les Daft Punk J'ai la rage d'un animal, cannibale, poto, j'manie l'mic Mais j'suis resté sur l'carreau Comme une chemise de Charles Ingalls J'garde la foi comme Abidal, hélas, le cash est capital Rebeu, la carte bleu c'est la seule carte qui soit vitale Bah ouais, j'ai eu des bonnes notes sans ter-chan Trempé dans de sales affaires, j'ai eu mon bac en séchant J'péra c'est embêtant, j'aime pas danser j'suis lancé dans La vie, tout l'monde peut s'en sortir, j'veux juste lui rentrer dedans Car j'ai grandi à Aulnay-Sous, Emmaüs la favelas On nique les chevaliers, qu'ils soient d'la rue ou d'Athéna Compte pas sur nous pour parler quand les schtars débarquent Pas d'messes basses, les keufs tournent, silence des cathédrales J'ai compris qu'les faux potes et l'honneur font bande à part Quand la haine, l'amour et la jalousie font des plans à trois J'donne plus d'amour à la rue, elle m'le rendra pas Comment faire partie des meubles Sans finir dans un grand placard ? Dans l'peu-Ra, trop d'suceurs qui m'foutent le seum Fermez vos gueules, si on est cheum, vous êtes tous plus cheum J'suis ce jeune parisien, américain dans l'état d'esprit Prends rendez-vous avec ton médecin légiste Ici, en plus des gouttes de pluie, souvent les coups pleuvent Mon crew est fait de vrais amis, à ton avis Pourquoi les putes se retrouvent toutes seules ? J'écris des rimes, j'envoie des torgnoles de malade Et pourtant, j'ai pas lu d'livre depuis TomTom Nana J'sors du Mordor de Paname, viens la bonne drogue est par là Une grosse pensée à nos proches pour qui l'horloge s'emballa Moi, j'suis debout, au-dessus d'moi, je vois voler les corbeaux J'ai besoin de joindre les deux bouts avant d'recoller les morceaux Tu mets des coups d'épée dans l'eau, l'affreux, on s'propage Prépare tes adieux, on fout le feu comme des Ghostriders Il faut que toutes les mains se lèvent haut Rimes façon West Coast, Gangsta à la Death Row On fuck les ennemis, miskine, ils se croient peut-être drôles Ça cartonne comme au rallye, on cartonne même sans khaliss Mes alliés se rallient, mental de patron On ne dit pas pardon, y'a que comme ça que tu seras libre Si j'tombe à Fleury, c'est qu'y a un beau million à prendre Ou qu'y a une tombe à fleurir, les tes-trai vont prendre des pralines J'ai pas vu d'boulot tendre Faut prendre pas l'9ar9ob face à la drogue Ils ont la boule au ventre, on a des abdos Les traitres sont de vraies balances Wesh, mais tétais dla bande, ouais, ouais, ouais... Faut quon tsaigne avant qutu mènes la danse Lami est éphémère, yen a qui parlent derrière ton dos Yen a même qui tbaisent et prennent ton cash, bellek, mon soss Putain de merde ! Cest quoi ce délire de faire Le soss et voler dans les mêmes dièses, oser se dire deux frères ? Tous hypocrites, les gens thypnotisent Leurs masques cachent leurs émotions et se disent trop vif Yen a qui servent du charme et te font croire à des rêves dars Et yen a qui tcachent des choses, et ouais, pour pas te faire mal Trop dacteurs, de squatteurs, de bâtards, de gratteurs de biff Faut des valeurs, le malheur tarrache la peur de vivre</t>
+          <t>Yeah, Zerzer Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour ds choses abominables, sèche ms larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais ZerZer volume 1 dispo partout la miff' DJ Élite aux platines Eh, eh Ok, ok, yeah Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Nique ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce gosse en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Brrrr Comme d'habitude, Hugz à la prod Eh, eh, eh Depuis l'époque de Décisions Yeah, yeah, yeah Han, han, Zerzer Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Ok, yeah, yeah, yeah Ça, c'est pour les anciens, ceux qui étaient là depuis l'époque Eh, eh Yeah Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie Yeah, yeah, yeah, yeah Ok, Reeko à la prod Hahaha, tu connais les bails Ouais, ouais, yeah Eh L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais Wooouh ! Han, han Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Yeah, yeah Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woouuh, -Crew, 2zer, Framal Brrraaa Brreh, brreh, brreh, brreh Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Letsguill ! Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Letsguill, Letsguill Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle 2zer Washington Ça sent la lorage, ca sent laverse jsuis dans ma tête Saboteurs Je ne bouge pas' jattends quca vienne Eh, eh, eh Sur le droit chemin, en sens inverse Grozomozo, Ratu, Saboteur gang Yeah, yeah, yeah Letsguill DJ Elite, balance la suite Han, han, tu connais Toujours la même, rien n'a changé Toujours les mêmes ons-s, toujours la même cons', eh Ouais, toujours les mêmes têtes Blackbird, Saboteur, Seine Zoo Hugz, ça dit quoi mon pote ? J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Eh, Grünt, sisi Han, han, ZerZer volume 1, dispo partout la miff' Yeah, han, han, han Saboteur gang, Seine Zoo Saboteur gang, Seine Zoo Hugz, ça dit quoi ? Yeah</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Ton nouveau pote</t>
+          <t>Plus rien à faire</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Yeah, Zerzer Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour ds choses abominables, sèche ms larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais ZerZer volume 1 dispo partout la miff' DJ Élite aux platines Eh, eh Ok, ok, yeah Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Nique ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce gosse en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Brrrr Comme d'habitude, Hugz à la prod Eh, eh, eh Depuis l'époque de Décisions Yeah, yeah, yeah Han, han, Zerzer Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Ok, yeah, yeah, yeah Ça, c'est pour les anciens, ceux qui étaient là depuis l'époque Eh, eh Yeah Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie Yeah, yeah, yeah, yeah Ok, Reeko à la prod Hahaha, tu connais les bails Ouais, ouais, yeah Eh L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais Wooouh ! Han, han Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Yeah, yeah Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woouuh, -Crew, 2zer, Framal Brrraaa Brreh, brreh, brreh, brreh Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Letsguill ! Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Letsguill, Letsguill Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle 2zer Washington Ça sent la lorage, ca sent laverse jsuis dans ma tête Saboteurs Je ne bouge pas' jattends quca vienne Eh, eh, eh Sur le droit chemin, en sens inverse Grozomozo, Ratu, Saboteur gang Yeah, yeah, yeah Letsguill DJ Elite, balance la suite Han, han, tu connais Toujours la même, rien n'a changé Toujours les mêmes ons-s, toujours la même cons', eh Ouais, toujours les mêmes têtes Blackbird, Saboteur, Seine Zoo Hugz, ça dit quoi mon pote ? J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Eh, Grünt, sisi Han, han, ZerZer volume 1, dispo partout la miff' Yeah, han, han, han Saboteur gang, Seine Zoo Saboteur gang, Seine Zoo Hugz, ça dit quoi ? Yeah</t>
+          <t>Tu suces, tu sers à rien T'es microscopique tel un acarien Je brasse et je brasse et je brasse, mais toi tu n'es rien qu'un arlequin J'débarque à l'improviste comme Billy Cocaïne J'ai pas reçu d'invit donc j'me codéine J'ai mélangé prométhazine sprite et codé pour en faire un excellent lean J'débite les rimes, oui je n'suis pas clean, j'immite les humanoïdes Dix bites dans la teush à l'ennemi, limonade à liqueur d'opioïde Devant la TV je n'matte qu'On n'Est Pas Couché, enfumé sous gnax en m'servant un double rre-vé Trop bourré sur l'pc j'regarde la MMA et j'en profite pour taper d'la bonne C Mauvais délires et débile sous LSD je vois et je vais encaisser les low kicks J'entends dans ma tête des rires et des rires et des rires, il me semble que j'suis sick Dans ma tête ils sont six, and three d'entre eux sont accros aux sticks Ces trois là très souvent me réclament de rouler un spliff comme si la weed était gratuite, comme si la weed était gratuite Le regard dans le vide j'ai le cerveau de freezer, légèrement schizoïde il y a sûrement une erreur Une erreur ça prend deux R comme terreur et 2zer Washington Mon corps et mon esprit sont dissociés je pèse deux tones J'suis complètement vidé, l'acide dans les recepteurs deux goutes de diéthylamide bad trip de 3h Faudrait p't'etre que j'fasse un truc car la redescente est assez difficile Si mes parents me voyaient dans cet état c'est sur qu'ils m'auraient déjà kill Ma mère m'a souvent dit les drogues c'est mal et ça peut même être létal Elle me disait aussi que ça nous rendait bête et pas normal, comme le racisme juif et anti-black Sévissant depuis des siècles celui-ci n'est pas légal, cent fois plus dangereux que les drogues et la galle Si présent pourtant, certains méritent des claques plutôt qu'un mac 22 octobre 2k16 j'assistais excité à mon premier pèlerinage musicale L'Guizi foncedé débitait des rimes et des rimes sous gros shit, oui j'étais à la Cigale Désormais j'attends qu'le gremlins fassent les backs avant le bac Le 16 décembre à la fnac pour pecho l'album-black On écrit, on tté-fri On roule des spliffs et je fais l'trie Boulette ? Pas boulette, sur le sol j'retrouve des têtes J'tabasse tellement les wacks qu'on m'appelle souvent l'nouveau Nek' Je fume, je rime, tu déprimes, j'bois du lean avec ma team Ces rappeurs sont has been, ma teen a le même boule que Kim Je trend set et oui j'me la pète, oui j'pète mon teh d'OG Kush J'ai kiffé sa bonne beuh-er, j'en rachète 500 meujs Tu flippes quand je dégaine, m'esquive quand je kick t'en sortira pas indemne Tellement d'hasch dans les veines, tes textes sentent la merde même à 100 kilomètres d'la seine ou dix, vernon zooo Si j'te croise j'te ferais mal à la manière de Framal J'te troue de trente balles, tu fall et devient tout pâle Donc cale toi ça dans l'crâne tu canes et je plane tel l'Empreur du Sale J'suis preneur de soufflette profesional et oui je fly comme Phall à la Don Dada Imperturbable même quand le cell sonne J'lâche un dab quand j'applique le cellophane Incompris j'me sens comme Cell, sans phone J'me présente mon blaze c'est Kagame-san J'comprends qu'tu sois fan mais dorénavant appelle moi Kami-sama Ces faux mc sont mauvais, flagrant comme l'obésité morbide à la big mama Sa mère ça suce, z'ont pas d'inspi donc sans cesse parle de tess d'ecsta et de cess C'est pas sensé même défoncé leurs faussent lyrics sont nasent ils croient qu'ils pèsent Si ça te plait pas t'as qu'à diskliker, carte visa dans la main j'fais taffer l'caissier T'aimes te ficha au lycée t'es pas ma tasse d'café j'préfère les filles discrète, mignonne, brunette pas trop maquillé Tu kiffes les beurettes pas belles kiffant faire la fête, la fête se fera bien dans leur chatte mouillées Au bout de deux trois verres ces salopes sont toutes sous l'emprise du Jack D Je crois avoir définit la définition du mot taspé, une keh sous mojito ou plutôt Mojito sur keh Ce fils de pute c'est ma beurette de luxe, suce j'arrive Yass comme Luxe pendant qu't'écoutes des bails claqués Je trouve ce son bien trop étrange, c'est donc la fin de ce mauvais mélange</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Plus rien à faire</t>
+          <t>Je sais enfin ce que je voulais dire</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Tu suces, tu sers à rien T'es microscopique tel un acarien Je brasse et je brasse et je brasse, mais toi tu n'es rien qu'un arlequin J'débarque à l'improviste comme Billy Cocaïne J'ai pas reçu d'invit donc j'me codéine J'ai mélangé prométhazine sprite et codé pour en faire un excellent lean J'débite les rimes, oui je n'suis pas clean, j'immite les humanoïdes Dix bites dans la teush à l'ennemi, limonade à liqueur d'opioïde Devant la TV je n'matte qu'On n'Est Pas Couché, enfumé sous gnax en m'servant un double rre-vé Trop bourré sur l'pc j'regarde la MMA et j'en profite pour taper d'la bonne C Mauvais délires et débile sous LSD je vois et je vais encaisser les low kicks J'entends dans ma tête des rires et des rires et des rires, il me semble que j'suis sick Dans ma tête ils sont six, and three d'entre eux sont accros aux sticks Ces trois là très souvent me réclament de rouler un spliff comme si la weed était gratuite, comme si la weed était gratuite Le regard dans le vide j'ai le cerveau de freezer, légèrement schizoïde il y a sûrement une erreur Une erreur ça prend deux R comme terreur et 2zer Washington Mon corps et mon esprit sont dissociés je pèse deux tones J'suis complètement vidé, l'acide dans les recepteurs deux goutes de diéthylamide bad trip de 3h Faudrait p't'etre que j'fasse un truc car la redescente est assez difficile Si mes parents me voyaient dans cet état c'est sur qu'ils m'auraient déjà kill Ma mère m'a souvent dit les drogues c'est mal et ça peut même être létal Elle me disait aussi que ça nous rendait bête et pas normal, comme le racisme juif et anti-black Sévissant depuis des siècles celui-ci n'est pas légal, cent fois plus dangereux que les drogues et la galle Si présent pourtant, certains méritent des claques plutôt qu'un mac 22 octobre 2k16 j'assistais excité à mon premier pèlerinage musicale L'Guizi foncedé débitait des rimes et des rimes sous gros shit, oui j'étais à la Cigale Désormais j'attends qu'le gremlins fassent les backs avant le bac Le 16 décembre à la fnac pour pecho l'album-black On écrit, on tté-fri On roule des spliffs et je fais l'trie Boulette ? Pas boulette, sur le sol j'retrouve des têtes J'tabasse tellement les wacks qu'on m'appelle souvent l'nouveau Nek' Je fume, je rime, tu déprimes, j'bois du lean avec ma team Ces rappeurs sont has been, ma teen a le même boule que Kim Je trend set et oui j'me la pète, oui j'pète mon teh d'OG Kush J'ai kiffé sa bonne beuh-er, j'en rachète 500 meujs Tu flippes quand je dégaine, m'esquive quand je kick t'en sortira pas indemne Tellement d'hasch dans les veines, tes textes sentent la merde même à 100 kilomètres d'la seine ou dix, vernon zooo Si j'te croise j'te ferais mal à la manière de Framal J'te troue de trente balles, tu fall et devient tout pâle Donc cale toi ça dans l'crâne tu canes et je plane tel l'Empreur du Sale J'suis preneur de soufflette profesional et oui je fly comme Phall à la Don Dada Imperturbable même quand le cell sonne J'lâche un dab quand j'applique le cellophane Incompris j'me sens comme Cell, sans phone J'me présente mon blaze c'est Kagame-san J'comprends qu'tu sois fan mais dorénavant appelle moi Kami-sama Ces faux mc sont mauvais, flagrant comme l'obésité morbide à la big mama Sa mère ça suce, z'ont pas d'inspi donc sans cesse parle de tess d'ecsta et de cess C'est pas sensé même défoncé leurs faussent lyrics sont nasent ils croient qu'ils pèsent Si ça te plait pas t'as qu'à diskliker, carte visa dans la main j'fais taffer l'caissier T'aimes te ficha au lycée t'es pas ma tasse d'café j'préfère les filles discrète, mignonne, brunette pas trop maquillé Tu kiffes les beurettes pas belles kiffant faire la fête, la fête se fera bien dans leur chatte mouillées Au bout de deux trois verres ces salopes sont toutes sous l'emprise du Jack D Je crois avoir définit la définition du mot taspé, une keh sous mojito ou plutôt Mojito sur keh Ce fils de pute c'est ma beurette de luxe, suce j'arrive Yass comme Luxe pendant qu't'écoutes des bails claqués Je trouve ce son bien trop étrange, c'est donc la fin de ce mauvais mélange</t>
+          <t>Elle me tenait dans le creux de sa main et elle le savait. Je m'étais toujours moqué des gars qui parlaient d'amour. Rien que d'écrire le mot, je me sens impuissant mais c'est vrai. De toute ma vie, j'avais jamais ressenti ça pour qui que ce soit à part ma mère et ça ne me plaisait pas. Je l'pense du fond du cur. Ça m'donnait l'impression... l'impression d'être faible... Faut qujte dise combien jai mal, jaurais pas dû mattacher Une barre de fer dans lestomac, une grosse boule dans ma trachée Mes larmes coulent mais, s'te plait, ne mprends pas pour un faible Pour texpliquer, jy vais en douceur, jlaisserai pas les bourrins faire Je tavais déclaré ma flamme car on ma dit qutu bédavais Moi, jsuis peut-être parano mais jsuis pas teu-bé, navré Je fais que d'penser à toi et jarrive même plus à grailler Vu la dispute de lautre soir, ma tristesse sest agravée Bref, quest-ce que jvoulais dire ? Ouais, jpense que tas tout gâché Apparemment, tu ten foutais, moi, jmétais amouraché Repense à ce qui se passe, compare le bon et le mauvais Cest difficile mais, à part toi, jai que le son et le brevet Jétais fier dêtre avec toi, sache que ça me flatte à lidée Que jai pu tintéresser et il ny a pas dfatalité Jveux que tu prennes ça en compte, jespère que ma phrase ta guidée Même si jai été blessé et que jsuis rapta vite fait ×2 Jsais enfin cque jvoulais dire, jai retrouvé mes phases Ton absence est trop néfaste et la solitude mefface Peut-être que ça va trop vite mais vaut mieux ça quun trou vide Si on mprescrit la folie, bah, je massacre un toubib Comment tas pu me faire ça ? Au final, jdevais pas compter pour toi Jpourrais pas être ton ami et puis être, par bonté, courtois Putain jcrois que jpète un plomb, ma seule issue, cest dans le son Au final, jsuis peut-être qu'un con qui se fait trop dillusions Jai aperçu le bonheur mais on mla repris aussitôt Tu mas brisé quelque chose quon n'répare pas dans les hôpitaux Tu mas fait goûté lparadis et là jretombe en enfer Mes larmes coulent, pour les stopper, moi, jsais pas comment faire1</t>
         </is>
       </c>
     </row>
@@ -1478,12 +1478,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Je sais enfin ce que je voulais dire</t>
+          <t>L’effet pas d’pilon</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Elle me tenait dans le creux de sa main et elle le savait. Je m'étais toujours moqué des gars qui parlaient d'amour. Rien que d'écrire le mot, je me sens impuissant mais c'est vrai. De toute ma vie, j'avais jamais ressenti ça pour qui que ce soit à part ma mère et ça ne me plaisait pas. Je l'pense du fond du cur. Ça m'donnait l'impression... l'impression d'être faible... Faut qujte dise combien jai mal, jaurais pas dû mattacher Une barre de fer dans lestomac, une grosse boule dans ma trachée Mes larmes coulent mais, s'te plait, ne mprends pas pour un faible Pour texpliquer, jy vais en douceur, jlaisserai pas les bourrins faire Je tavais déclaré ma flamme car on ma dit qutu bédavais Moi, jsuis peut-être parano mais jsuis pas teu-bé, navré Je fais que d'penser à toi et jarrive même plus à grailler Vu la dispute de lautre soir, ma tristesse sest agravée Bref, quest-ce que jvoulais dire ? Ouais, jpense que tas tout gâché Apparemment, tu ten foutais, moi, jmétais amouraché Repense à ce qui se passe, compare le bon et le mauvais Cest difficile mais, à part toi, jai que le son et le brevet Jétais fier dêtre avec toi, sache que ça me flatte à lidée Que jai pu tintéresser et il ny a pas dfatalité Jveux que tu prennes ça en compte, jespère que ma phrase ta guidée Même si jai été blessé et que jsuis rapta vite fait ×2 Jsais enfin cque jvoulais dire, jai retrouvé mes phases Ton absence est trop néfaste et la solitude mefface Peut-être que ça va trop vite mais vaut mieux ça quun trou vide Si on mprescrit la folie, bah, je massacre un toubib Comment tas pu me faire ça ? Au final, jdevais pas compter pour toi Jpourrais pas être ton ami et puis être, par bonté, courtois Putain jcrois que jpète un plomb, ma seule issue, cest dans le son Au final, jsuis peut-être qu'un con qui se fait trop dillusions Jai aperçu le bonheur mais on mla repris aussitôt Tu mas brisé quelque chose quon n'répare pas dans les hôpitaux Tu mas fait goûté lparadis et là jretombe en enfer Mes larmes coulent, pour les stopper, moi, jsais pas comment faire1</t>
+          <t>XXX Depuis une semaine, plus dpilon, ouais, poto, les temps sont durs Mes associés se font soulever et dans la rue les tensions durent Pas dremords dans mon quartier, même Monsieur Propre a les mains sales Le Sheitan te tend un spliff et te demande Allume-moi ça Dans une heure jai rendez-vous un pote un pote marrange les 100 meujes Jaurais enfin de quoi m'rendre fier, cest marrant jme sens mieux Jsuis pas chez moi, jconnais sonne-per, faut que j'fasse profil bas Pourvu quces gars nen profitent pas, tfaçon, jai les crocs jfile pas Jmarchais tranquillement mais un fils de pute est venu minterpeler Il mdit Qu'est-ce que tas sur toi, poto ? On va tfaire pleurer Tu connais lpremier réflexe, patate dans les gencives Pas ltemps de discuter, moi, jtrace et les gens suivent Tu sais pas cque jai du faire pour protéger mes bénéfices Jvoulais pas autant dproblèmes, juste du biff et baiser l'fisc Bref, passons les blablas, jfinis la soirée sous Heineken et beu-her Tout se finit bien, sache que les biatchs aiment Ken et 2-zer Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Tous les papas l'diront, tout réside dans une histoire de Tarot Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Certains mdisent jsuis plus le même car jveux qu'les culs secs Les pucelles avalent la vie cul sec, vider mes cuves pleines, le cul règne Dans le Rap avant cétait NTM le suprême Maintenant cest Lyricalchimie, nattends pas qumon équipe te surprenne Jveux une existence plus quhumaine Mon manque de substances remplace par lenvie dken Jlance mes hadoken, 7 cicatrices pour ton abdomen Spliff et heineken grosse orgie parisienne où les ados ken La weed les épinards de Popeye, leffet pas dpilon S'infiltre dans tes oreilles, bordel, plus dcocon Mais dans une corbeille des ailes sectionnées, forcé d'marcher Avec des engelures aux orteils pour des enflures sélectionnées Cest leffet impossible dtoucher lsommet Avant le funéraire quand t'tej funiculaire vit à trois cent à lheure Déjà shooté par lherbe cest pas clair Cest leffet casse-tête pas leffet grasse herbe Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Tous les papas l'diront, tout réside dans une histoire de Tarot Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux A Paris, quand la nuit tombe, il se passe de sales histoires Quand il sagit dpas décevoir lénergie du samedi soir Il y a ce type désopilant fanatique de son pilon Qui organise une fête chez lui et se fait piquer son filon Obligé de bipper son pigeon pour soulager ses nerfs Il s'dit qula vie, cest trop bidon donc le roulage est sévère Et son boloss rentre chez lui en scoot, il s'penche et rit Il se tuera sur la route, écoute car le mal renchérit Et son pote va se mettre mal Encore un soir bête où le pet va rendre ce mec pâle Alors il fume, cest mieux que d'avoir pas dshit Mais comme il force sur la dose, il part en bad trip Des mecs en bas crient, ça fait monter sa rage Le genre de brave type qui te démonte et sarrache Mais il descend le pilon, cest du courage en barre Cest indécent le bilan car il mourra en bas Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Tous les papas l'diront, tout réside dans une histoire de Tarot Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Cest leffet pas pas dpilon1</t>
         </is>
       </c>
     </row>
@@ -1495,12 +1495,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>L’effet pas d’pilon</t>
+          <t>Compte sur nous</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>XXX Depuis une semaine, plus dpilon, ouais, poto, les temps sont durs Mes associés se font soulever et dans la rue les tensions durent Pas dremords dans mon quartier, même Monsieur Propre a les mains sales Le Sheitan te tend un spliff et te demande Allume-moi ça Dans une heure jai rendez-vous un pote un pote marrange les 100 meujes Jaurais enfin de quoi m'rendre fier, cest marrant jme sens mieux Jsuis pas chez moi, jconnais sonne-per, faut que j'fasse profil bas Pourvu quces gars nen profitent pas, tfaçon, jai les crocs jfile pas Jmarchais tranquillement mais un fils de pute est venu minterpeler Il mdit Qu'est-ce que tas sur toi, poto ? On va tfaire pleurer Tu connais lpremier réflexe, patate dans les gencives Pas ltemps de discuter, moi, jtrace et les gens suivent Tu sais pas cque jai du faire pour protéger mes bénéfices Jvoulais pas autant dproblèmes, juste du biff et baiser l'fisc Bref, passons les blablas, jfinis la soirée sous Heineken et beu-her Tout se finit bien, sache que les biatchs aiment Ken et 2-zer Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Tous les papas l'diront, tout réside dans une histoire de Tarot Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Certains mdisent jsuis plus le même car jveux qu'les culs secs Les pucelles avalent la vie cul sec, vider mes cuves pleines, le cul règne Dans le Rap avant cétait NTM le suprême Maintenant cest Lyricalchimie, nattends pas qumon équipe te surprenne Jveux une existence plus quhumaine Mon manque de substances remplace par lenvie dken Jlance mes hadoken, 7 cicatrices pour ton abdomen Spliff et heineken grosse orgie parisienne où les ados ken La weed les épinards de Popeye, leffet pas dpilon S'infiltre dans tes oreilles, bordel, plus dcocon Mais dans une corbeille des ailes sectionnées, forcé d'marcher Avec des engelures aux orteils pour des enflures sélectionnées Cest leffet impossible dtoucher lsommet Avant le funéraire quand t'tej funiculaire vit à trois cent à lheure Déjà shooté par lherbe cest pas clair Cest leffet casse-tête pas leffet grasse herbe Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Tous les papas l'diront, tout réside dans une histoire de Tarot Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux A Paris, quand la nuit tombe, il se passe de sales histoires Quand il sagit dpas décevoir lénergie du samedi soir Il y a ce type désopilant fanatique de son pilon Qui organise une fête chez lui et se fait piquer son filon Obligé de bipper son pigeon pour soulager ses nerfs Il s'dit qula vie, cest trop bidon donc le roulage est sévère Et son boloss rentre chez lui en scoot, il s'penche et rit Il se tuera sur la route, écoute car le mal renchérit Et son pote va se mettre mal Encore un soir bête où le pet va rendre ce mec pâle Alors il fume, cest mieux que d'avoir pas dshit Mais comme il force sur la dose, il part en bad trip Des mecs en bas crient, ça fait monter sa rage Le genre de brave type qui te démonte et sarrache Mais il descend le pilon, cest du courage en barre Cest indécent le bilan car il mourra en bas Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Tous les papas l'diront, tout réside dans une histoire de Tarot Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Cest leffet pas pas dpilon, quand on tpropose Tu peux pas pas dire non, cmonde est pas rose Si tas pas les cartes, tu restes sur le carreau Si tes pas sur tes gardes, tu finis derrière les barreaux Cest leffet pas pas dpilon1</t>
+          <t>La vrai fraternité, c'est déjà terminé On voit si t'as l'sang chaud une fois tes artères vidées C'est la guerre contre ces réfractaires givrés J'les met à terre s'ils déblatèrent sur mes affaires privées C'est la merde! Non j'veux pas m'faire des idées Détailler c'est risqué mais j'ai pas l'air d'hésiter Mais là frère c'que je vis c'est la célébrité J'lai mérité pour ça pas d'sérénité J'baise ta cacophonie j'vis ma vie Et j'te rends dingue comme une pathologie psychiatrique Putain y'as trop d'folies! Mais face aux phobies j'y arrive Tu cherches la merde, c'est que c'est la sodomie qui t'attire! Mon clan t'rentre dedans, sans prendre de gants C'est sanglant nan nan franchement Il est grand temps que j'me venge! Nekfeu, Framal et Mekra, S-Crew, nerveux f'ra vla les dégâts On va tout niquer, et j'le pense amplement! Faut pas nous banaliser, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Analisez, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Si ton malheur m'affecte, c'est par peur que ça m'arrive J'combat je maltraite, ceux qui condamnent le faciès Mes sons d'ailleurs achètent, les rappeurs que t'analyse Saveurs de cannabis, ces vapeurs me canalisent! Le diable est dans ton déhanché miss J'vais pas m'estomper j'vais dompter et plomber l'antéchrist, non c'est triste! Avant y'avait les meufs qui m'bâchaient et ces chiens qui m'ignoraient Maintenant j'me fais draguer par des bitchs aux seins siliconés! Unis dans l'biz mais on ne sait plus à qui se référencer Comme un uni-jambiste qui veut choisir sur quel pied danser Pas là pour plaisanter, ou bien quémander Ne propose pas un steak à un édenté! J'ai fréquenter les pires endroits J'ai vu des dérangés qui étranglaient des filles dans l'bois! Quand ta vie s'en va, t'es pris de l'angoisse Que ta miss conçoit, l'avenir sans toi! La vie d'rêve frangin, c'est 2zer Washington! Tu connais t'façons, L'Entourage bébé S-Crew booy! Framal est dans la place! Crapo', toujours monosourcilé! Blackbird bébé, Blackbirdddd, tu connais t'façons! Mekra, j'sais pas t'es où t'es toujours en retard Et Fennek, t'es en tournée, et Bsahtek, on va tout baiser ! S-Crew!1</t>
         </is>
       </c>
     </row>
@@ -1512,12 +1512,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Compte sur nous</t>
+          <t>Entêté</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>La vrai fraternité, c'est déjà terminé On voit si t'as l'sang chaud une fois tes artères vidées C'est la guerre contre ces réfractaires givrés J'les met à terre s'ils déblatèrent sur mes affaires privées C'est la merde! Non j'veux pas m'faire des idées Détailler c'est risqué mais j'ai pas l'air d'hésiter Mais là frère c'que je vis c'est la célébrité J'lai mérité pour ça pas d'sérénité J'baise ta cacophonie j'vis ma vie Et j'te rends dingue comme une pathologie psychiatrique Putain y'as trop d'folies! Mais face aux phobies j'y arrive Tu cherches la merde, c'est que c'est la sodomie qui t'attire! Mon clan t'rentre dedans, sans prendre de gants C'est sanglant nan nan franchement Il est grand temps que j'me venge! Nekfeu, Framal et Mekra, S-Crew, nerveux f'ra vla les dégâts On va tout niquer, et j'le pense amplement! Faut pas nous banaliser, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Analisez, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Si ton malheur m'affecte, c'est par peur que ça m'arrive J'combat je maltraite, ceux qui condamnent le faciès Mes sons d'ailleurs achètent, les rappeurs que t'analyse Saveurs de cannabis, ces vapeurs me canalisent! Le diable est dans ton déhanché miss J'vais pas m'estomper j'vais dompter et plomber l'antéchrist, non c'est triste! Avant y'avait les meufs qui m'bâchaient et ces chiens qui m'ignoraient Maintenant j'me fais draguer par des bitchs aux seins siliconés! Unis dans l'biz mais on ne sait plus à qui se référencer Comme un uni-jambiste qui veut choisir sur quel pied danser Pas là pour plaisanter, ou bien quémander Ne propose pas un steak à un édenté! J'ai fréquenter les pires endroits J'ai vu des dérangés qui étranglaient des filles dans l'bois! Quand ta vie s'en va, t'es pris de l'angoisse Que ta miss conçoit, l'avenir sans toi! La vie d'rêve frangin, c'est 2zer Washington! Tu connais t'façons, L'Entourage bébé S-Crew booy! Framal est dans la place! Crapo', toujours monosourcilé! Blackbird bébé, Blackbirdddd, tu connais t'façons! Mekra, j'sais pas t'es où t'es toujours en retard Et Fennek, t'es en tournée, et Bsahtek, on va tout baiser ! S-Crew!1</t>
+          <t>Yeah, Zer-2, tu connais t'façons -Crew, 2001 jusqu'à l'infini fois deux cousin Yeah, écoute, han, yeah Ne me parle pas de tes problèmes, j'en ai d'jà trop, j'en ai que faire Quand je veux parler des miens on m'dit que j'suis censé me taire Dis-moi comment avoir du cur sans se faire traiter de faible Eviter les cauchemars c'est tout c'que j'ai rêvé de faire On m'a dit T'as changé 2zer depuis qu'tu ne manques plus d'oseille Mais j'ai toujours le spliff au bec, un peu comme une enclume au pied Depuis que nos ennemis se sont pris des déculottées Plus de couteau sous l'pullover et mon équipe est plus qu'opée Personne n'aurait pu m'stopper, j'avais le mental Ma sincérité pouvait blesser, un vrai ne ment pas Toi tu fais que parler d'oseille mais ça tombe bien qu'tu m'en parles Y'a pas plus rentable que ma voix sur l'instrumentale Mon frère est disque de platine, d'un coup ma vie prend du sens hein hein Ce serait triste de partir donc on arrive en puissance C'est pas facile de bâtir un empire, ça prend du temps On veut la paix et on y arrivera en luttant x2 Entêté, j'veux briller avant d'être enterré Continuer dans ma lancée, avancer sans freiner Sans stresser, sans s'presser, c'est c'qu'on m'a enseigné Le savoir est une arme, une arme peut s'enrayer Yo, les uns parlent de tess', les autres parlent de sexe Y'en a qui parlent de caisses, moi qu'est-ce qui m'reste à part ce texte ? Les uns parlent de tess', les autres parlent de sexe Y'en a qui parlent de caisses, moi qu'est-ce qui m'reste à part ce texte ? Les uns parlent de tess', les autres parlent de sexe Y'en a qui parlent de caisses, moi qu'est-ce qui m'reste à part ce texte ? Les uns parlent de tess', les autres parlent de sexe Moi qu'est-ce qui m'reste yo ? Ça fait 8 ans que je n'fais que rapper, ça correspond à l'infini Je nie être célèbre même si toutes les preuves m'incriminent On dit qu'on débarque à 26, on débarque à 26 000 On a du shit qui fait planer et d'la weed qui rend invisible Que faire face au doute, à part l'ignorer ? Tu peux pas dépenser les sous que t'as pas mis d'côté Moi je savoure chaque moment que la vie m'a mijoté J'te laisse traficoter tant qu'tu viens pas m'asticoter x2 Entêté, j'veux briller avant d'être enterré Continuer dans ma lancée, avancer sans freiner Sans stresser, sans s'presser, c'est c'qu'on m'a enseigné Le savoir est une arme, une arme peut s'enrayer Hello, no one is available to take your call. Please leave a message after the tone1</t>
         </is>
       </c>
     </row>
@@ -1529,12 +1529,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Entêté</t>
+          <t>Freestyle de l’Entourage en live dans Planète Rap !</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Yeah, Zer-2, tu connais t'façons -Crew, 2001 jusqu'à l'infini fois deux cousin Yeah, écoute, han, yeah Ne me parle pas de tes problèmes, j'en ai d'jà trop, j'en ai que faire Quand je veux parler des miens on m'dit que j'suis censé me taire Dis-moi comment avoir du cur sans se faire traiter de faible Eviter les cauchemars c'est tout c'que j'ai rêvé de faire On m'a dit T'as changé 2zer depuis qu'tu ne manques plus d'oseille Mais j'ai toujours le spliff au bec, un peu comme une enclume au pied Depuis que nos ennemis se sont pris des déculottées Plus de couteau sous l'pullover et mon équipe est plus qu'opée Personne n'aurait pu m'stopper, j'avais le mental Ma sincérité pouvait blesser, un vrai ne ment pas Toi tu fais que parler d'oseille mais ça tombe bien qu'tu m'en parles Y'a pas plus rentable que ma voix sur l'instrumentale Mon frère est disque de platine, d'un coup ma vie prend du sens hein hein Ce serait triste de partir donc on arrive en puissance C'est pas facile de bâtir un empire, ça prend du temps On veut la paix et on y arrivera en luttant x2 Entêté, j'veux briller avant d'être enterré Continuer dans ma lancée, avancer sans freiner Sans stresser, sans s'presser, c'est c'qu'on m'a enseigné Le savoir est une arme, une arme peut s'enrayer Yo, les uns parlent de tess', les autres parlent de sexe Y'en a qui parlent de caisses, moi qu'est-ce qui m'reste à part ce texte ? Les uns parlent de tess', les autres parlent de sexe Y'en a qui parlent de caisses, moi qu'est-ce qui m'reste à part ce texte ? Les uns parlent de tess', les autres parlent de sexe Y'en a qui parlent de caisses, moi qu'est-ce qui m'reste à part ce texte ? Les uns parlent de tess', les autres parlent de sexe Moi qu'est-ce qui m'reste yo ? Ça fait 8 ans que je n'fais que rapper, ça correspond à l'infini Je nie être célèbre même si toutes les preuves m'incriminent On dit qu'on débarque à 26, on débarque à 26 000 On a du shit qui fait planer et d'la weed qui rend invisible Que faire face au doute, à part l'ignorer ? Tu peux pas dépenser les sous que t'as pas mis d'côté Moi je savoure chaque moment que la vie m'a mijoté J'te laisse traficoter tant qu'tu viens pas m'asticoter x2 Entêté, j'veux briller avant d'être enterré Continuer dans ma lancée, avancer sans freiner Sans stresser, sans s'presser, c'est c'qu'on m'a enseigné Le savoir est une arme, une arme peut s'enrayer Hello, no one is available to take your call. Please leave a message after the tone1</t>
+          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
         </is>
       </c>
     </row>
@@ -1546,12 +1546,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Freestyle de l’Entourage en live dans Planète Rap !</t>
+          <t>Ouais Boy</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
+          <t>B-Boy, B-Girl, scarla, scarlette T'es toujours à l'écoute de la Mixtape 2Fingz Et la 75ème Sess' te remercie Si t'as un truc à fumer, roule cette merde maintenant Si t'as une 'teille dans l'frigo, t'as juste le temps d'aller la chercher Et si tu kiffes juste l'oxygène, mets-toi à l'aise et écoute le son C'est parti, S-Crew, 2Fingz Il est temps d'leur montrer d'quoi vous êtes capables Mario, balance l'instru Framal Tu peux entendre mes balles dans l'gun, pas l'temps de dire ouf J'suis comme un battement d'cur, ta tempe se dissout Attends le discours d'un savant, j'suis vite saoulé Par les vacances, moi, j'veux de l'argent puis des foufs Mon passe-temps est pour l'appart des parents J'nique la France et les cours, qu'on parle franc Appelle-moi l'hémorroïde quand j'viens bloquer ta sortie Assorti au, fucking décor flamboyant, ça déborde sur la langue Tu viens d'sucker ma grosse bite, la grosse bitch prend la porte J'baise les porcs, on les prend comme un tarif à bon prix T'as compris, écoute le bruit des Ducati Sous les plumards y'a plus d'cash, j'me bute la nuit Ouais, j'me couche tard, les coups d'schlass te fourguent, l'ami Que des coups d'rage, écoute ça, que de l'outrage Sors mon pouchka, on nous regarde, sur tout Paris 2Zer Washington Quand mes pensées s'assombrissent, y'a danger, ça s'complique La vie m'a mutilé mais j'suis cultivé, je n'rangerai pas mon bic Ma vendetta s'combine pendant qu'ces sales cons friment J'suis déçu de la vie comme Une nympho devant des caleçons vides Ma vie, c'est rapper ou taffer l'développé-couché J'suis l'buf qui vient désosser et dévorer l'boucher J'ai les oreilles bouchées car le Rap met la pression On parlera d'mes agressions quand j'aurais dégommé Clooney Et détrôné tous mes adversaires J'suis un sale pervers car tes gars se laissent faire Quand j'leur fais des attouchements textuels J'rappe doucement car souvent ma Douce France est cruelle Mekra J'ai les pensées d'un polygame, j'aime trop les femmes, ma gueule J'suis pas comique mais trop bizarre, j'ai promis, j'cane la feuille C'est Mekra, j'aime pas l'État, fais gaffe, j'suis pas légal, pédale Je gratte des phases où le Sheitan m'accueille, c'est sale Tu veux lire dans mes pensées, fais bellek, c'est un film d'horreur Des trucs de psychopathes, ça passe du rire aux larmes Ça vire au drame quand j'me dis que les vigos meurent Tu trouve que j'suis fou, normal, je le suis Tu boudes là, petite zouz ? Goûte le bre-chi Ouais, j'ai des pensées perverses, j'ai dépensé De l'espèce pour des 'teilles pour que j'essaye De songer à des pensées pépères, faut m'laisser, les mecs Dans mes dièses, j'suis débranché, les frères KLM Dégomme des rangées d', des tonnes de pensées obscures Animent mon veau-cer mais je n'ai que faire Elle passe ap' le duo au stud' Des sons, d'la sape, ça bosse dur Sans borne, j'leur zappe leur posture Qui che-lâ ses shabs après une sale imposture Des post-it partout dans la breuch, un crachat dans une teuch Une overdose de geushs et ta clique de porcs à la broche Voilà c'que je vois quand Chivas est à l'approche Tétanisé sur la brèche, j'accélère et passe aux proches Un big up, ouais ! C'est qu'ils veulent çà A 19 time, j'serai peut-être toujours qué-cho par les loches Mais bref, j'me détends, j'rallume la téloche Les flammes du mal me lèchent J'peux t'dire qu'elles tarissent pas d'éloges Doum's Ça sent la merde, toi-même t'as senti Que mon esprit n'est pas tranquille Tard en ville, j'pars en vrille, ouais, presbyte, j'te garantis Que si tu t'approches trop, tu vas pas en revenir T'as capté ce stème-sy ? J'suis pas d'humeur à blaguer J'peux te smasher, attardé, si tu me respectes pas assez Avec ma horde de basanés, on va bien te fracasser MC, ramassez les mixtures sur le canapé, je m'immisce Merde, frère... J'ai rattrapé ces bitchs Qui m'parlaient d'un plan à 3, j'crois qu'ça se passe dans les bois Mon côté obscur a pris l'dessus, je t'assure, j'voulais ap' J'suis tombé dans les arcades de la folie, à l'agonie J'fais des arnaques à la Yonea4</t>
         </is>
       </c>
     </row>
@@ -1563,12 +1563,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Ouais Boy</t>
+          <t>Freestyle de Nekfeu, 17 minutes</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>B-Boy, B-Girl, scarla, scarlette T'es toujours à l'écoute de la Mixtape 2Fingz Et la 75ème Sess' te remercie Si t'as un truc à fumer, roule cette merde maintenant Si t'as une 'teille dans l'frigo, t'as juste le temps d'aller la chercher Et si tu kiffes juste l'oxygène, mets-toi à l'aise et écoute le son C'est parti, S-Crew, 2Fingz Il est temps d'leur montrer d'quoi vous êtes capables Mario, balance l'instru Framal Tu peux entendre mes balles dans l'gun, pas l'temps de dire ouf J'suis comme un battement d'cur, ta tempe se dissout Attends le discours d'un savant, j'suis vite saoulé Par les vacances, moi, j'veux de l'argent puis des foufs Mon passe-temps est pour l'appart des parents J'nique la France et les cours, qu'on parle franc Appelle-moi l'hémorroïde quand j'viens bloquer ta sortie Assorti au, fucking décor flamboyant, ça déborde sur la langue Tu viens d'sucker ma grosse bite, la grosse bitch prend la porte J'baise les porcs, on les prend comme un tarif à bon prix T'as compris, écoute le bruit des Ducati Sous les plumards y'a plus d'cash, j'me bute la nuit Ouais, j'me couche tard, les coups d'schlass te fourguent, l'ami Que des coups d'rage, écoute ça, que de l'outrage Sors mon pouchka, on nous regarde, sur tout Paris 2Zer Washington Quand mes pensées s'assombrissent, y'a danger, ça s'complique La vie m'a mutilé mais j'suis cultivé, je n'rangerai pas mon bic Ma vendetta s'combine pendant qu'ces sales cons friment J'suis déçu de la vie comme Une nympho devant des caleçons vides Ma vie, c'est rapper ou taffer l'développé-couché J'suis l'buf qui vient désosser et dévorer l'boucher J'ai les oreilles bouchées car le Rap met la pression On parlera d'mes agressions quand j'aurais dégommé Clooney Et détrôné tous mes adversaires J'suis un sale pervers car tes gars se laissent faire Quand j'leur fais des attouchements textuels J'rappe doucement car souvent ma Douce France est cruelle Mekra J'ai les pensées d'un polygame, j'aime trop les femmes, ma gueule J'suis pas comique mais trop bizarre, j'ai promis, j'cane la feuille C'est Mekra, j'aime pas l'État, fais gaffe, j'suis pas légal, pédale Je gratte des phases où le Sheitan m'accueille, c'est sale Tu veux lire dans mes pensées, fais bellek, c'est un film d'horreur Des trucs de psychopathes, ça passe du rire aux larmes Ça vire au drame quand j'me dis que les vigos meurent Tu trouve que j'suis fou, normal, je le suis Tu boudes là, petite zouz ? Goûte le bre-chi Ouais, j'ai des pensées perverses, j'ai dépensé De l'espèce pour des 'teilles pour que j'essaye De songer à des pensées pépères, faut m'laisser, les mecs Dans mes dièses, j'suis débranché, les frères KLM Dégomme des rangées d', des tonnes de pensées obscures Animent mon veau-cer mais je n'ai que faire Elle passe ap' le duo au stud' Des sons, d'la sape, ça bosse dur Sans borne, j'leur zappe leur posture Qui che-lâ ses shabs après une sale imposture Des post-it partout dans la breuch, un crachat dans une teuch Une overdose de geushs et ta clique de porcs à la broche Voilà c'que je vois quand Chivas est à l'approche Tétanisé sur la brèche, j'accélère et passe aux proches Un big up, ouais ! C'est qu'ils veulent çà A 19 time, j'serai peut-être toujours qué-cho par les loches Mais bref, j'me détends, j'rallume la téloche Les flammes du mal me lèchent J'peux t'dire qu'elles tarissent pas d'éloges Doum's Ça sent la merde, toi-même t'as senti Que mon esprit n'est pas tranquille Tard en ville, j'pars en vrille, ouais, presbyte, j'te garantis Que si tu t'approches trop, tu vas pas en revenir T'as capté ce stème-sy ? J'suis pas d'humeur à blaguer J'peux te smasher, attardé, si tu me respectes pas assez Avec ma horde de basanés, on va bien te fracasser MC, ramassez les mixtures sur le canapé, je m'immisce Merde, frère... J'ai rattrapé ces bitchs Qui m'parlaient d'un plan à 3, j'crois qu'ça se passe dans les bois Mon côté obscur a pris l'dessus, je t'assure, j'voulais ap' J'suis tombé dans les arcades de la folie, à l'agonie J'fais des arnaques à la Yonea4</t>
+          <t>C'est pas l'histoire d'un tox ou d'un gosse sur un champ d'bataille Ni celle d'un beauf ou d'un bobo qui s'encanaille Fidèle au poste, j'apporte trop d'flows qui sentent la maille J'dis des gros mots car y'a trop d'choses quand j'chante ma life Allez, j'squatte les palais, fuck les gens d'la hype Et fallait, pas m'faire déballer c'que ces vantards braillent Mais allez, j'suis inégalé par les gens d'leur taille Ils jouent à cache-cache et perdent leurs squelettes dans l'card-pla à balais Le poids des années te rend souvent seul, t'es rieur Oui, mais d'vant la foule, tu refoules tes souffrances intérieures Hier, j'aimais pas les corvées mais j'y allais quand maman m'disais Mon premier pote mort, j'ai chialé comme un môme 17 ans, j'étais un SDF, moi qui pourtant détestais perdre J'ai eu de l'aide et j'oublie pas les gestes des frères De sacrées têtes chaudes, la haine au ventre, on traîne au centre commercial Comme si y'avait les moyens de s'acheter quelque chose On m'a dit 2-Zer t'es pas éternel, faudra bien qu'tu partes un jour Tu recevras l'baiser d'la Mort, donc surtout tends pas ta joue Pour les jaloux, ce jour là sera sacré Ouais, le peu-Ra ça crée l'envie, d'se massacrer Si j'te fais du mal c'est pas gratuit car j'suis un gentil mec La richesse est loin mais pour l'succès, manque plus qu'un centimètre Étrangement, pas de coups d'main, que des étranglements J'préfère, être le mec demandé, ouais, qu'être en demande Posé, sur les strapontins, j'me dis, qu'j'suis déjà contraint On fait des débats, dont pleins provoquent des dégâts qu'on craint J'me sens comme un graffeur qui n'a pas gué-ta l'bon train J'te jure que j'irai mieux quand mon papa verra l'compte plein L'amour c'est dur, mais être seul, ça l'est dix fois plus Donne ta confiance, n'imagine pas que ta lady sois pute Comment une si belle bouche peut sortir trop d'mots vexants ? J'vais attraper la gangrène car j'me fais trop d'mauvais sang Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire a commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remord On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit dans l'originale mais c'était pas la nuit dernière Quand j'étais p'tit dans l'originale, on m'chantait Mamadou avait mal aux dents Maintenant qu'j'suis grand Ces mêmes personnes me sucent le gland Et puis fuck, maintenant j'brûle des scènes Avec mes potes pénards, on fuck le Code pénal Envoie la drogue, pétard à la bouche que j'brûle ces chèques Car j'suis un résident des villes les plus médiatisées Où les présidents débiles dépensent des méga-budgets Dans des élections stériles, fuck ça j'préfère la zik, lope-sa J'déverse ma iv' dans l'Rap, en récitant mes titres Tu sauras d'où j'viens, BKO, Dar es Salam Si mes salauds passent à l'acte C'est pour éviter l'génocide des shaolins Dharamsala De toute façon, j'sais qu'les kisdés comptent bien Nous encercler, enfermer loin d'ces dîners mondains C'est dans l'chantier qu'on doit taffer Mais pour mes frères ce n'est pas assez File-nous 10 000 au moins, pour mes Miguel de Pigwalle Avant d'commencer c'son, j'avais un thème Un truc sombre sur la vendetta dans la tête d'un jeune qui a la vingtaine Puis j'ai fumé un joint d'jaune avec untel Ou p't-être un joint d'zeb suivi d'un fond d'teille Et j'ai zappé, sa mère, faudrait qu'j'arrête cette merde avant d'dead On est seuls, c'qui fait qu'on est tristes Le mauvais il, ça l'fait kiffer qu'on s'détruise Dis-toi qu't'as tout pour toi, c'est important Quand est-ce qu'on va s'unir ? Il faut un temps pour tout, on forme un tout pourtant Faut qu'on soit formatés par l'système, ils disent Ça m'fait flipper comme la montée d'l'antisémitisme On va en boîte, on s'fait chier Alors on fout l'zbeul, on finit dans les fichiers des colboks Comportement à l'école bof On s'bute à Call of en buvant des alcools forts Et les filles, je ne sais pas c'qu'elles veulent Mais je m'en fiche tant que j'enfile des baskets neuves Mais dès qu'j'ai mis la paire, ça y est, elle est plus neuve Problème épineux, dans ce shop y'aura p't-être une mieux On est continuellement frustrés consommer pour s'consoler J'm'amuse jamais dans les soirées mais j'continue d'm'incruster C'est pas bénéfique, les voisins débarquent avec La ferme intention de dire La ferme, attention, j'appelle les flics ! Je compte même plus les moments d'absence Je t'aime ça compte plus, les mots n'ont pas d'sens J'agrippe un Scud pendant qu'mon groupuscule graille une crêpe au stud' Face à Dieu, mes têtes lisses et crépues scrutent le même crépuscule J'ai capturé ton attention, catapulté ma rage dans l'son J'rap pas pour monter mais pour assumer mon ascension Fils, on a ce groove technique Nique tes homies thug, tes OG's pleurent Notre tireur débarque déguisé en room-service QI criminel, des bruits militaires, les stups s'immiscent discrets Flashback d'une vie similaire Pour ça qu'j'suis vieux jeu, Stash House dans l'neuf deux Des reufs de, toutes les nationalités Check la flyness mixée avec le seum Plein de voyous se sont perdus en voulant s'éduquer tout seul Cousin, on reste fly on est seize dans la place Prends toi mon seize dans la face, ou bien De l'enfer serais-je exempté ? Trop de dealers les terrains sont segmentés Si tu veux passer crème il faut que tes faux papiers soient étrangers Manie l'crom facile, smoke massif Un squad no joke, j'm'active la coke attire, en tant que business Oui j'ai vendu du crack mais pas de poudre Mes gars rappent comme Nas dans Barbecue Gazeuses, plaques et matraques la capitale est yomb Ici ni fleuve ni lac, juste une Seine lasse-dèg donc allons-y, fuyons Entre les putes, les connasses, les gars, Nous trions dans l'originale Ville lassante mais nous rions Donc j'accomplis mon triomphe comme l'Arc Imagine la Tour Eiffel se faire amputer Boumbadaboum ! Encore un gosse vient d'se faire buter Le pognon, c'est l'thème L'opinion d'ces débiles n'est pas l'essentiel Sans gène, c'est l'défilé des pigeons avec ou sans ailes Certains, pris de dégout, deviendront des scélérats Sortis des égouts, les bourges nous regardent En s'disant C'est ça les rats... La street un mauvais ragout, passe tes thunes et ça l'aidera A assaisonner de plus de gout, ça vaut le coup mais, ça, c'est rare J'voulais porter le stard-co mais les keufs m'ont mis les pinces On n'écoute pas Sarko, ici, seul le Parc est un prince Au plus profond d'mes songes, j'ai vu cette lueur lunaire Sans aucune honte, j'vous présente le côté sombre de la ville lumière J'dîne avec deux nababs, j'discute d'un tas d'fric à faire Petite malette, cigarette, mitraillette de Vie la chaire en , big dans l'palace J'vie d'la guerre, des flics à terre, nique sa mère le travail Nique sa mère le travail Nique, nique, nique sa mère le travail.. Nique sa mère le travail, nique sa mère c'est habtai Moi j'arrive je kick ça et tu sais qu'negro c'est habtal Tu veux nous tester mon équipe c'est la meilleure de Paname En freestyle on va baiser ces tagas et ces tass C'est qu'ça s'passe, je reviens avec la flamme Ouais j'suis mon negro Feu, tu veux cracher des aah Vas-y dis leur, on est des putains de commandants Des dragons, écoute la flamme, on va kicker ça, dès maintenant Dès maintenant, on va kicker ça des flammes bleutées On est venus pour kicker pas venu pour bluffer C'est pour tous mes , complètement pétés Complètement hébétés, complètement éreintés Sur le rain-té ou pas c'est comme ça qu'on le fait Soupape, Nek le Fennec dans tous les concerts, le cancer nous concerne Il concerne tous les gens qui font la mal-bouffe C'est Nek le Fennec, si t'as mal l'ouvre Pas, car ici c'est pas comme ça, gars, faut fermer sa gueule C'est comme ça qu'je l'fait quand j'fous l'zbeul Je sais pas c'que j'dis c'est pas grave ça sort donc c'est l'inconscient qui parle, direct C'est Nek le Fennec pour muslims, porteurs de kippas, j'y vais C'est comme ça qu'je l'fait, c'est comme ça que j'réunis les gens J'veux pas être une légende, j'veux juste un être intelligent Ah, tu vois donc j'bafouille quand j'dis intelligent car Je mens un petit peu car je l'suis pas encore gars J'fais le truc, c'est comme ça qu'j'pars, j'pars en Corvette, nique les corvées C'est comme ça, on est encore frères On est là encore frère, fuck les corvées On part en Corvette, comment t'expliquer qu'mec c'est mortel On prend les rimes du reuf pour claquer quelques phases Rien à foutre des fuckin' keufs moi j'arrive je passe On fume la marijuanna devant le palais royal Demande à Alpha comment ça s'passe, ouais avais les khoyas On est toujours àl, on s'pose pour le Seine Zoo Eh, la réédition est àl, négro reste cool Et là c'est Doumams toujours en freestyle j'te lâche des phases Tu comprends ap comment ça s'passe mon négro ça sort de ma tête Je coupe des , ah, je coupe des plaquettes, ah Je marche en claquettes, toujours avec la tablette scoop, tu peux m'croiser dans l'métro Avec tous les frérots tu sais que Doumams fume le po-po Fuck la po-police, avec mes gavas on est àl on est en impro-pro Si tu nous testes j'ai...j'ai ta , vas-y Alpha reviens àl Je suis en train de ramer comme si j'étais Ok, àl, et 'jvais mettre une fuckin frappe Parle nous de..de Tony ou bien de Kraus Le business est maqué, Phily Flingue revient en claquettes Par d'or plaqué appelle moi Clark Kent Hein, il y a pas de problème on découpe le truc Découpe le 'uc, fume le shit en plaquette Il y a pas de problème, ramène le truc, le marocain J'fais qu'me rapprocher, Alph Lauren le mois prochain Eh, Phily Flingue les schneks vient les rrer-fou Comme si j'me faisais des perfusions de RedBull Trop d'énergie, je reste très speed Phily Flingue même face à treize skins J'fais la vitesse d'un Usain Bolt Phily Flingue, j'écoute leur truc, ces rappeurs c'est que..poubelles mortes Ça rime pas mais ça rime bien, petit chien Phily Flingue, technique practicien Parisien, sale petit chien, eh Phily Flingue, rendez-vous chez l'opticien Des meufs aux p'tits seins, nan Mais elles me traient aux petits soins Il y a pas de problème toi même tu sais Phily Flingue, hein, ya, impossible de sucer, pour le succès Eh, Je sais, toi tu sais, à quoi tu sers Il y a pas de problème, ramène des putains de chiennasses mais ramène pas des pucelles Hein, on s'met bien, très bien, sept cinq Je reste Phal, je reste Flingue On ramène ça, on ramène ça cul sec D'une traite, dans l'équipe il y a plus d'traitres Car ces petites pédales ont tous décalé Nek le Fennec, inégalé, pour sénégalais et tous les gens qui squattent sur les galets Sur les pavés, c'est comme ça qu'j'le fais la jeunesse dépravée Je l'ai pas fait, enfin si, maintenant c'est fini Balance une putain de phase sur les vinyls Séparés, on est parés, negro j'ai la dalle On est trois, on va lâcher six flingues, et c'est macabre Est-ce que vous êtes prêts pour le trois et demi Alpha est-ce que tu m'suis la mif, il faut mettre des baffes à ces bitches J'enchaine, la famille, Phily Flingue, il faut que tu m'trouves dans Trois chambres, dans trois suites, dans le catalogue des 3Suisses Phily Flingue, j'suis le prince, mais dès qu'je rap même le roi suis Hein hein, ouais le roi suis, je le fais ça pour mes petits mecs On balance le putain de triplex On fait le truc à trois on fait le truc en trio avec C'est Nek le Fennec j'suis chaud depuis l'embryon Depuis l'embryon, ouais, depuis le départ Rien à foutre de toutes ces pétasses, moi j'suis posé j'ai le pétard Avec mes négro on est àl et tu sais qu'on brillera, comme Les néons, ou les phares de ce xénon Ouais, ouais ça brille mec, puissance Madrillène Elles avalent le jus blanc et j'parle pas d'Actimel Et c'est facile mec, Phily Flingue au microphone toi même tu sais j'ai pas mis d' C'est comme ça, ça sort du cerveau c'est la donation J'viens d'me lever c'est comme si j'avais fait l'ovation Car c'est trop chaud, et je balance du love à fond C'est Nek le Fennec ouais mon gars en improvisation En improvisation, là c'est la BBC Tu veux nous tester mon negro fuck BBC RTL et toutes c'est conneries, àl c'est du freestyle On parle avec nos têtes, vas-y Phal mets des baffes Le flow est bien tacheté , j'ai bien agi, j'ai bien acté J'sais pas si c'est un mic ou bien un MAC-10 Car je flingue dans tous les sens C'est comme dans la partouze, du sperme dans toutes le franges Flingue dans tous les sens, ouais tu l'as dit et c'est tacheté Nous c'est le courage, eux c'est la lâcheté La ré-édition dans les bacs et tu vas l'acheter C'est Nek le Fennec ouais mon gars c'est comme ça qu'j'balance Yo le freestyle, c'est convivial! J'ai dit le freestyle, c'est convivial! Poto le freestyle, c'est convivial! J'ai dit le freestyle, c'est convivial! Nek Tout le monde le freestyle C'est convivial Nek Ouais ouais le cris.. Alpha..tal, c'est pas convivial Nek C'est transparent, le cristal Alpha Fuck les bijoux Quand j'serai grand j'veux habiter à la mer, avec mon père et ma mère Marcher dans le sable plus prendre le R.E.R Ces putains de tours j'veux plus les voir plus tard J'veux vivre autre part, j'ai même une idée si tu veux savoir J'ai même un idée quand j'écoute Fabe, quand j'écoute Nab Quand j'écoute tous mes gars qui fabriquent Des idées différentes un peu de c'qu'il y a C'est pour mes itinérants qu'est-ce qu'il y a? J'fais le truc, fumeur de Ihya ou pas Ceux qui qui pillavent, ceux qui mènent la vie droite C'est Nek le Fennec la vie d'oim, j'regarde le miroir Et j'aime pas trop ce que je vois, j'essaie d'pas vider les tiroirs Parce qu'il y a des trucs sombres, ouais mon gars j'aimerai bien t'y voir Ouais, ouais, ouais, fuck les voleurs d'ivoir C'est comme ça qu'on fait tu vois bien que j'y vais gars Hein, fin, vas-y balance la suite Moi j'y vais gars, comme si j't'ai vé-ga Sur la Sega, je sais qu'il y a toutes ces petites pétasses ouais c'est normal Les , avec la technique, toujours les mêmes rimes Mais c'est pas grave, ouais tu sais qu'ça sse-pa La sse-cla j'l'ai oubliée dans le hall Comment t'expliquer j'suis àl avec mes soss Belek à toi, ouais tu sais qu'on est onze Eh, moi j'arrive et je bronze Sur le soleil, j'aurai le disque de platine, la famille Avec mes gavas on arrive on applique Les meilleures techniques, les meilleures jutsu Si tu nous testes, bitch, tu vas gouter à la pure foudre Qu'on va concocter, mec désolé J'suis en train d'te quitter des phases obscures, dérobées I fucked up, c'est une rime de merde, ça n'veut rien dire Mais c'est pas grave je reviens, oui mamen je découpe ta tête On leur montre, à quoi le cro-mi sert Eh, tu sais qu'on est vicieux comme la police serbe Fait tourner l'micro comme le cul d'la fille du comissaire Pas d'problème, j'me mets bien Nouvelle structure, faut qu'le truc dure Phily Flingue dans des jolies voitures Des Dacia, j'fume des trucs bien, j'fume pas d'l'acacia A Paris y a, mes parias Phily Flingue, yes, hein Ambiance familiale, on veut des thunes par milliards Par milliers, tu sais qui c'est Phily Flingue alias Phil Phal Qui va enchainer, eh? Qui va rengainer, ais-je fais que gangréner, eh? Mes textes c'est d'la sueur et des larmes, d'la fureur et du love Faire du seille avec mes phases c'est faire du feu avec de l'eau Eff Gee fait si mal, le meurtre technique efficace Une balle et j'suis ti-par face à l'inévitable, pas d'délai Faut convertir chaque 16 en euros puis en dollar vite si je vise la villa à LA Et là ce n'est qu'un rêve C'est pas parce que tu fly que t'es un oiseau Auquel cas tu serais un moineau et moi j'serais un aigle Si si, j'volerais au-dessus des lois comme un ministre La vie est sinistre J'écris mon histoire, j'm'en tape de c'qu'ils disent Dans l'flow qu'j'administre Flow criminel qui nique les milices Pas près d'bouger d'là comme si on m'avait shooté l'dos À force de m'coucher tard j'finis par m'coucher tôt J'suis du-per, mec, pour m'repérer j'suis le vent Sachant qu'si tu parles derrière mon dos c'est qu'j'suis devant E deux F, G deux E, je te crève les deux yeux Je te sèche les cheveux, salope! E deux F, G deux E, je te crève les deux yeux Je te sèche les cheveux, salope! d'sample Mise mes billets, gars, car le buisness illégal en pleine journée provoque effusion d'sang Gamin j'n'ai plus ton temps sans nous la rue n'est plus contente Et nous n'avons qu'une seule question, negro, payes-tu ? On aime les voitures, les hoes, le pèse facile Le crew m'a dit qu'jétais plus fort que des têtes d'affiches Ça fait si si yo, Nasty Yass vous abimera en survêt' Adida Originals Les crises de , tant les criminals Ma rue est plutôt stricte, ici, negro, se faire du fric c'est le minimum On est venu coffrer, de-spee comme un faucon Pendant qu'mes gars se font coffrer sous des faux noms Vas-y paye la caution en vitesse avant qu'les empreintes digitales remontent Nigga j'frappe le son Et c'est facile comme les qu'on négocie C'est de l'or j'ai fini par traiter mes anciens comme des gosses Coupe à moitié pleine, le chargeur à moitié vide à moitié cassé, mon âme est à moitié clean Mon gars, le j'le baffe tranquille, jamais j'attends l'biff C'est tout bête, tu peux tout perde en un battement de cil Chez moi la zone n'est pas sensible, si tu restes pas attentif Le sang va couler comme Atlantis Ok check j'ai ça, ça fait Hein, hein, hein Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap, faut Arracher l'cro-mi des faux, chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout quand bas il y a les 'zins? La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes Tu vois comme ça s'passe, ça shoote comme dans Medal Of Honor Comme l'a dit Bazz, mec, Vos guerres, nos morts C'est comme ça qu'je l'fait, tu vois, c'est pour tous mes garnements Ceux qui ont planqués un petit peu d'armement Au cas où ça dérape, au cas où Marion Maréchal débarque C'est comme ça qu'on l'fait j'me tape des barres avec mes gars, ouais J'fais mon truc enfile ton cahouet, il pleut C'est Nek le Fennec il peut, kicker avec ses ty-pes Encore un soir où je tente d'écrire mais ma page reste blanche Peu d'inspi, le ventre vide, il me reste un sachet à vendre J'me dirige vers le 6, là bas un los-bar m'attend J'vais m'remplir le bide et l'frigo devant la banque On se voit, on monte chez Los', la transaction se passe en balle Puis j'fonce dans l'trom', rejoindre tous mes gars en bas Ça roule des cônes ou devrais-je plutôt dire des battes Goûte cette dope qui me fait relativiser Le mal La cam dans la chanson originale c'est mal, on l'sait tous mais cela dit j'y vais Fuck tes probabilités, je tenterais ce paris risqué Il m'faut des pepettes pour graille, j'suis pas du style lève tôt J'garde ma conscience pour moi donc fais de même, frérot</t>
         </is>
       </c>
     </row>
@@ -1580,12 +1580,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Freestyle de Nekfeu, 17 minutes</t>
+          <t>Dernière fois</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>C'est pas l'histoire d'un tox ou d'un gosse sur un champ d'bataille Ni celle d'un beauf ou d'un bobo qui s'encanaille Fidèle au poste, j'apporte trop d'flows qui sentent la maille J'dis des gros mots car y'a trop d'choses quand j'chante ma life Allez, j'squatte les palais, fuck les gens d'la hype Et fallait, pas m'faire déballer c'que ces vantards braillent Mais allez, j'suis inégalé par les gens d'leur taille Ils jouent à cache-cache et perdent leurs squelettes dans l'card-pla à balais Le poids des années te rend souvent seul, t'es rieur Oui, mais d'vant la foule, tu refoules tes souffrances intérieures Hier, j'aimais pas les corvées mais j'y allais quand maman m'disais Mon premier pote mort, j'ai chialé comme un môme 17 ans, j'étais un SDF, moi qui pourtant détestais perdre J'ai eu de l'aide et j'oublie pas les gestes des frères De sacrées têtes chaudes, la haine au ventre, on traîne au centre commercial Comme si y'avait les moyens de s'acheter quelque chose On m'a dit 2-Zer t'es pas éternel, faudra bien qu'tu partes un jour Tu recevras l'baiser d'la Mort, donc surtout tends pas ta joue Pour les jaloux, ce jour là sera sacré Ouais, le peu-Ra ça crée l'envie, d'se massacrer Si j'te fais du mal c'est pas gratuit car j'suis un gentil mec La richesse est loin mais pour l'succès, manque plus qu'un centimètre Étrangement, pas de coups d'main, que des étranglements J'préfère, être le mec demandé, ouais, qu'être en demande Posé, sur les strapontins, j'me dis, qu'j'suis déjà contraint On fait des débats, dont pleins provoquent des dégâts qu'on craint J'me sens comme un graffeur qui n'a pas gué-ta l'bon train J'te jure que j'irai mieux quand mon papa verra l'compte plein L'amour c'est dur, mais être seul, ça l'est dix fois plus Donne ta confiance, n'imagine pas que ta lady sois pute Comment une si belle bouche peut sortir trop d'mots vexants ? J'vais attraper la gangrène car j'me fais trop d'mauvais sang Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire a commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remord On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit dans l'originale mais c'était pas la nuit dernière Quand j'étais p'tit dans l'originale, on m'chantait Mamadou avait mal aux dents Maintenant qu'j'suis grand Ces mêmes personnes me sucent le gland Et puis fuck, maintenant j'brûle des scènes Avec mes potes pénards, on fuck le Code pénal Envoie la drogue, pétard à la bouche que j'brûle ces chèques Car j'suis un résident des villes les plus médiatisées Où les présidents débiles dépensent des méga-budgets Dans des élections stériles, fuck ça j'préfère la zik, lope-sa J'déverse ma iv' dans l'Rap, en récitant mes titres Tu sauras d'où j'viens, BKO, Dar es Salam Si mes salauds passent à l'acte C'est pour éviter l'génocide des shaolins Dharamsala De toute façon, j'sais qu'les kisdés comptent bien Nous encercler, enfermer loin d'ces dîners mondains C'est dans l'chantier qu'on doit taffer Mais pour mes frères ce n'est pas assez File-nous 10 000 au moins, pour mes Miguel de Pigwalle Avant d'commencer c'son, j'avais un thème Un truc sombre sur la vendetta dans la tête d'un jeune qui a la vingtaine Puis j'ai fumé un joint d'jaune avec untel Ou p't-être un joint d'zeb suivi d'un fond d'teille Et j'ai zappé, sa mère, faudrait qu'j'arrête cette merde avant d'dead On est seuls, c'qui fait qu'on est tristes Le mauvais il, ça l'fait kiffer qu'on s'détruise Dis-toi qu't'as tout pour toi, c'est important Quand est-ce qu'on va s'unir ? Il faut un temps pour tout, on forme un tout pourtant Faut qu'on soit formatés par l'système, ils disent Ça m'fait flipper comme la montée d'l'antisémitisme On va en boîte, on s'fait chier Alors on fout l'zbeul, on finit dans les fichiers des colboks Comportement à l'école bof On s'bute à Call of en buvant des alcools forts Et les filles, je ne sais pas c'qu'elles veulent Mais je m'en fiche tant que j'enfile des baskets neuves Mais dès qu'j'ai mis la paire, ça y est, elle est plus neuve Problème épineux, dans ce shop y'aura p't-être une mieux On est continuellement frustrés consommer pour s'consoler J'm'amuse jamais dans les soirées mais j'continue d'm'incruster C'est pas bénéfique, les voisins débarquent avec La ferme intention de dire La ferme, attention, j'appelle les flics ! Je compte même plus les moments d'absence Je t'aime ça compte plus, les mots n'ont pas d'sens J'agrippe un Scud pendant qu'mon groupuscule graille une crêpe au stud' Face à Dieu, mes têtes lisses et crépues scrutent le même crépuscule J'ai capturé ton attention, catapulté ma rage dans l'son J'rap pas pour monter mais pour assumer mon ascension Fils, on a ce groove technique Nique tes homies thug, tes OG's pleurent Notre tireur débarque déguisé en room-service QI criminel, des bruits militaires, les stups s'immiscent discrets Flashback d'une vie similaire Pour ça qu'j'suis vieux jeu, Stash House dans l'neuf deux Des reufs de, toutes les nationalités Check la flyness mixée avec le seum Plein de voyous se sont perdus en voulant s'éduquer tout seul Cousin, on reste fly on est seize dans la place Prends toi mon seize dans la face, ou bien De l'enfer serais-je exempté ? Trop de dealers les terrains sont segmentés Si tu veux passer crème il faut que tes faux papiers soient étrangers Manie l'crom facile, smoke massif Un squad no joke, j'm'active la coke attire, en tant que business Oui j'ai vendu du crack mais pas de poudre Mes gars rappent comme Nas dans Barbecue Gazeuses, plaques et matraques la capitale est yomb Ici ni fleuve ni lac, juste une Seine lasse-dèg donc allons-y, fuyons Entre les putes, les connasses, les gars, Nous trions dans l'originale Ville lassante mais nous rions Donc j'accomplis mon triomphe comme l'Arc Imagine la Tour Eiffel se faire amputer Boumbadaboum ! Encore un gosse vient d'se faire buter Le pognon, c'est l'thème L'opinion d'ces débiles n'est pas l'essentiel Sans gène, c'est l'défilé des pigeons avec ou sans ailes Certains, pris de dégout, deviendront des scélérats Sortis des égouts, les bourges nous regardent En s'disant C'est ça les rats... La street un mauvais ragout, passe tes thunes et ça l'aidera A assaisonner de plus de gout, ça vaut le coup mais, ça, c'est rare J'voulais porter le stard-co mais les keufs m'ont mis les pinces On n'écoute pas Sarko, ici, seul le Parc est un prince Au plus profond d'mes songes, j'ai vu cette lueur lunaire Sans aucune honte, j'vous présente le côté sombre de la ville lumière J'dîne avec deux nababs, j'discute d'un tas d'fric à faire Petite malette, cigarette, mitraillette de Vie la chaire en , big dans l'palace J'vie d'la guerre, des flics à terre, nique sa mère le travail Nique sa mère le travail Nique, nique, nique sa mère le travail.. Nique sa mère le travail, nique sa mère c'est habtai Moi j'arrive je kick ça et tu sais qu'negro c'est habtal Tu veux nous tester mon équipe c'est la meilleure de Paname En freestyle on va baiser ces tagas et ces tass C'est qu'ça s'passe, je reviens avec la flamme Ouais j'suis mon negro Feu, tu veux cracher des aah Vas-y dis leur, on est des putains de commandants Des dragons, écoute la flamme, on va kicker ça, dès maintenant Dès maintenant, on va kicker ça des flammes bleutées On est venus pour kicker pas venu pour bluffer C'est pour tous mes , complètement pétés Complètement hébétés, complètement éreintés Sur le rain-té ou pas c'est comme ça qu'on le fait Soupape, Nek le Fennec dans tous les concerts, le cancer nous concerne Il concerne tous les gens qui font la mal-bouffe C'est Nek le Fennec, si t'as mal l'ouvre Pas, car ici c'est pas comme ça, gars, faut fermer sa gueule C'est comme ça qu'je l'fait quand j'fous l'zbeul Je sais pas c'que j'dis c'est pas grave ça sort donc c'est l'inconscient qui parle, direct C'est Nek le Fennec pour muslims, porteurs de kippas, j'y vais C'est comme ça qu'je l'fait, c'est comme ça que j'réunis les gens J'veux pas être une légende, j'veux juste un être intelligent Ah, tu vois donc j'bafouille quand j'dis intelligent car Je mens un petit peu car je l'suis pas encore gars J'fais le truc, c'est comme ça qu'j'pars, j'pars en Corvette, nique les corvées C'est comme ça, on est encore frères On est là encore frère, fuck les corvées On part en Corvette, comment t'expliquer qu'mec c'est mortel On prend les rimes du reuf pour claquer quelques phases Rien à foutre des fuckin' keufs moi j'arrive je passe On fume la marijuanna devant le palais royal Demande à Alpha comment ça s'passe, ouais avais les khoyas On est toujours àl, on s'pose pour le Seine Zoo Eh, la réédition est àl, négro reste cool Et là c'est Doumams toujours en freestyle j'te lâche des phases Tu comprends ap comment ça s'passe mon négro ça sort de ma tête Je coupe des , ah, je coupe des plaquettes, ah Je marche en claquettes, toujours avec la tablette scoop, tu peux m'croiser dans l'métro Avec tous les frérots tu sais que Doumams fume le po-po Fuck la po-police, avec mes gavas on est àl on est en impro-pro Si tu nous testes j'ai...j'ai ta , vas-y Alpha reviens àl Je suis en train de ramer comme si j'étais Ok, àl, et 'jvais mettre une fuckin frappe Parle nous de..de Tony ou bien de Kraus Le business est maqué, Phily Flingue revient en claquettes Par d'or plaqué appelle moi Clark Kent Hein, il y a pas de problème on découpe le truc Découpe le 'uc, fume le shit en plaquette Il y a pas de problème, ramène le truc, le marocain J'fais qu'me rapprocher, Alph Lauren le mois prochain Eh, Phily Flingue les schneks vient les rrer-fou Comme si j'me faisais des perfusions de RedBull Trop d'énergie, je reste très speed Phily Flingue même face à treize skins J'fais la vitesse d'un Usain Bolt Phily Flingue, j'écoute leur truc, ces rappeurs c'est que..poubelles mortes Ça rime pas mais ça rime bien, petit chien Phily Flingue, technique practicien Parisien, sale petit chien, eh Phily Flingue, rendez-vous chez l'opticien Des meufs aux p'tits seins, nan Mais elles me traient aux petits soins Il y a pas de problème toi même tu sais Phily Flingue, hein, ya, impossible de sucer, pour le succès Eh, Je sais, toi tu sais, à quoi tu sers Il y a pas de problème, ramène des putains de chiennasses mais ramène pas des pucelles Hein, on s'met bien, très bien, sept cinq Je reste Phal, je reste Flingue On ramène ça, on ramène ça cul sec D'une traite, dans l'équipe il y a plus d'traitres Car ces petites pédales ont tous décalé Nek le Fennec, inégalé, pour sénégalais et tous les gens qui squattent sur les galets Sur les pavés, c'est comme ça qu'j'le fais la jeunesse dépravée Je l'ai pas fait, enfin si, maintenant c'est fini Balance une putain de phase sur les vinyls Séparés, on est parés, negro j'ai la dalle On est trois, on va lâcher six flingues, et c'est macabre Est-ce que vous êtes prêts pour le trois et demi Alpha est-ce que tu m'suis la mif, il faut mettre des baffes à ces bitches J'enchaine, la famille, Phily Flingue, il faut que tu m'trouves dans Trois chambres, dans trois suites, dans le catalogue des 3Suisses Phily Flingue, j'suis le prince, mais dès qu'je rap même le roi suis Hein hein, ouais le roi suis, je le fais ça pour mes petits mecs On balance le putain de triplex On fait le truc à trois on fait le truc en trio avec C'est Nek le Fennec j'suis chaud depuis l'embryon Depuis l'embryon, ouais, depuis le départ Rien à foutre de toutes ces pétasses, moi j'suis posé j'ai le pétard Avec mes négro on est àl et tu sais qu'on brillera, comme Les néons, ou les phares de ce xénon Ouais, ouais ça brille mec, puissance Madrillène Elles avalent le jus blanc et j'parle pas d'Actimel Et c'est facile mec, Phily Flingue au microphone toi même tu sais j'ai pas mis d' C'est comme ça, ça sort du cerveau c'est la donation J'viens d'me lever c'est comme si j'avais fait l'ovation Car c'est trop chaud, et je balance du love à fond C'est Nek le Fennec ouais mon gars en improvisation En improvisation, là c'est la BBC Tu veux nous tester mon negro fuck BBC RTL et toutes c'est conneries, àl c'est du freestyle On parle avec nos têtes, vas-y Phal mets des baffes Le flow est bien tacheté , j'ai bien agi, j'ai bien acté J'sais pas si c'est un mic ou bien un MAC-10 Car je flingue dans tous les sens C'est comme dans la partouze, du sperme dans toutes le franges Flingue dans tous les sens, ouais tu l'as dit et c'est tacheté Nous c'est le courage, eux c'est la lâcheté La ré-édition dans les bacs et tu vas l'acheter C'est Nek le Fennec ouais mon gars c'est comme ça qu'j'balance Yo le freestyle, c'est convivial! J'ai dit le freestyle, c'est convivial! Poto le freestyle, c'est convivial! J'ai dit le freestyle, c'est convivial! Nek Tout le monde le freestyle C'est convivial Nek Ouais ouais le cris.. Alpha..tal, c'est pas convivial Nek C'est transparent, le cristal Alpha Fuck les bijoux Quand j'serai grand j'veux habiter à la mer, avec mon père et ma mère Marcher dans le sable plus prendre le R.E.R Ces putains de tours j'veux plus les voir plus tard J'veux vivre autre part, j'ai même une idée si tu veux savoir J'ai même un idée quand j'écoute Fabe, quand j'écoute Nab Quand j'écoute tous mes gars qui fabriquent Des idées différentes un peu de c'qu'il y a C'est pour mes itinérants qu'est-ce qu'il y a? J'fais le truc, fumeur de Ihya ou pas Ceux qui qui pillavent, ceux qui mènent la vie droite C'est Nek le Fennec la vie d'oim, j'regarde le miroir Et j'aime pas trop ce que je vois, j'essaie d'pas vider les tiroirs Parce qu'il y a des trucs sombres, ouais mon gars j'aimerai bien t'y voir Ouais, ouais, ouais, fuck les voleurs d'ivoir C'est comme ça qu'on fait tu vois bien que j'y vais gars Hein, fin, vas-y balance la suite Moi j'y vais gars, comme si j't'ai vé-ga Sur la Sega, je sais qu'il y a toutes ces petites pétasses ouais c'est normal Les , avec la technique, toujours les mêmes rimes Mais c'est pas grave, ouais tu sais qu'ça sse-pa La sse-cla j'l'ai oubliée dans le hall Comment t'expliquer j'suis àl avec mes soss Belek à toi, ouais tu sais qu'on est onze Eh, moi j'arrive et je bronze Sur le soleil, j'aurai le disque de platine, la famille Avec mes gavas on arrive on applique Les meilleures techniques, les meilleures jutsu Si tu nous testes, bitch, tu vas gouter à la pure foudre Qu'on va concocter, mec désolé J'suis en train d'te quitter des phases obscures, dérobées I fucked up, c'est une rime de merde, ça n'veut rien dire Mais c'est pas grave je reviens, oui mamen je découpe ta tête On leur montre, à quoi le cro-mi sert Eh, tu sais qu'on est vicieux comme la police serbe Fait tourner l'micro comme le cul d'la fille du comissaire Pas d'problème, j'me mets bien Nouvelle structure, faut qu'le truc dure Phily Flingue dans des jolies voitures Des Dacia, j'fume des trucs bien, j'fume pas d'l'acacia A Paris y a, mes parias Phily Flingue, yes, hein Ambiance familiale, on veut des thunes par milliards Par milliers, tu sais qui c'est Phily Flingue alias Phil Phal Qui va enchainer, eh? Qui va rengainer, ais-je fais que gangréner, eh? Mes textes c'est d'la sueur et des larmes, d'la fureur et du love Faire du seille avec mes phases c'est faire du feu avec de l'eau Eff Gee fait si mal, le meurtre technique efficace Une balle et j'suis ti-par face à l'inévitable, pas d'délai Faut convertir chaque 16 en euros puis en dollar vite si je vise la villa à LA Et là ce n'est qu'un rêve C'est pas parce que tu fly que t'es un oiseau Auquel cas tu serais un moineau et moi j'serais un aigle Si si, j'volerais au-dessus des lois comme un ministre La vie est sinistre J'écris mon histoire, j'm'en tape de c'qu'ils disent Dans l'flow qu'j'administre Flow criminel qui nique les milices Pas près d'bouger d'là comme si on m'avait shooté l'dos À force de m'coucher tard j'finis par m'coucher tôt J'suis du-per, mec, pour m'repérer j'suis le vent Sachant qu'si tu parles derrière mon dos c'est qu'j'suis devant E deux F, G deux E, je te crève les deux yeux Je te sèche les cheveux, salope! E deux F, G deux E, je te crève les deux yeux Je te sèche les cheveux, salope! d'sample Mise mes billets, gars, car le buisness illégal en pleine journée provoque effusion d'sang Gamin j'n'ai plus ton temps sans nous la rue n'est plus contente Et nous n'avons qu'une seule question, negro, payes-tu ? On aime les voitures, les hoes, le pèse facile Le crew m'a dit qu'jétais plus fort que des têtes d'affiches Ça fait si si yo, Nasty Yass vous abimera en survêt' Adida Originals Les crises de , tant les criminals Ma rue est plutôt stricte, ici, negro, se faire du fric c'est le minimum On est venu coffrer, de-spee comme un faucon Pendant qu'mes gars se font coffrer sous des faux noms Vas-y paye la caution en vitesse avant qu'les empreintes digitales remontent Nigga j'frappe le son Et c'est facile comme les qu'on négocie C'est de l'or j'ai fini par traiter mes anciens comme des gosses Coupe à moitié pleine, le chargeur à moitié vide à moitié cassé, mon âme est à moitié clean Mon gars, le j'le baffe tranquille, jamais j'attends l'biff C'est tout bête, tu peux tout perde en un battement de cil Chez moi la zone n'est pas sensible, si tu restes pas attentif Le sang va couler comme Atlantis Ok check j'ai ça, ça fait Hein, hein, hein Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap, faut Arracher l'cro-mi des faux, chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout quand bas il y a les 'zins? La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes Tu vois comme ça s'passe, ça shoote comme dans Medal Of Honor Comme l'a dit Bazz, mec, Vos guerres, nos morts C'est comme ça qu'je l'fait, tu vois, c'est pour tous mes garnements Ceux qui ont planqués un petit peu d'armement Au cas où ça dérape, au cas où Marion Maréchal débarque C'est comme ça qu'on l'fait j'me tape des barres avec mes gars, ouais J'fais mon truc enfile ton cahouet, il pleut C'est Nek le Fennec il peut, kicker avec ses ty-pes Encore un soir où je tente d'écrire mais ma page reste blanche Peu d'inspi, le ventre vide, il me reste un sachet à vendre J'me dirige vers le 6, là bas un los-bar m'attend J'vais m'remplir le bide et l'frigo devant la banque On se voit, on monte chez Los', la transaction se passe en balle Puis j'fonce dans l'trom', rejoindre tous mes gars en bas Ça roule des cônes ou devrais-je plutôt dire des battes Goûte cette dope qui me fait relativiser Le mal La cam dans la chanson originale c'est mal, on l'sait tous mais cela dit j'y vais Fuck tes probabilités, je tenterais ce paris risqué Il m'faut des pepettes pour graille, j'suis pas du style lève tôt J'garde ma conscience pour moi donc fais de même, frérot</t>
+          <t>Grand Master Pouchki flashe ta cousine comme un projecteur Alexandre traduit protecteur XXX comme lecteur cassettes CD ou DVD j'ai mille facettes Tu risques de décéder A,B,C,D j'te kill avec 2-zer washington des MC's j'en bâche une tonne Convoité jusqu'en Asie même si je parle pas chintok' Groupie je te croque ta pomme putain je suis comme MacIntosh Tu braques une banque, je dragues une moche, pendant que je matte une teuch O pour le niveau U car dans le son je sue Double H pour le hip-hop, blaze complexe comme un digicode Z pour la 'sique XXL sur le beat ! Ouhhz le magicien des beats et c'est déjà un classique J'crache des bouts d'texte, regarde ma tête je boude là J'traîne sur le boulevard, Belleville c'est le zoo gars C'est bel et bien Bloopalooza, du 20 moins 1 cousin, le 20ème mon voisin J'arrive de loin avec de lourdes phrases Couplet en Ukrainien Les coups qui décapent, décapsulent des cannettes Traque en lâchant des cases en flinguant linche les ca- -davre de s'hrab qui pue donc envoie des claques Pas de MicMac, j'paye mon Big Mac deluxe c'est Doc Polux! Accro d'esthétique, peu catholique depuis le berceau J'ai forgé ma critique sous psychotrope dans des tunnels de métro Parle de l'éthique MC Soul Costik , ?? Authentique Approche, oui approche et tend l'oreille à la parole d'un gavroche des temps modernes Approche, oui approche et tend l'oreille,c'est l'étrange juste un gosse de plus qui vous dérange J'rappe tout le temps mais je rêve que derrière un cro-mi Si j'perce, je continuerai d'creuser voila ce que j'ai promis Que mon son laisse une trace comme une ain-m sans gants Qu'on sache que Meassane veut dire âme sanglante Au mic c'est Eff, éphémère j'ai les nerfs 4 mesures c'est éphémère Les mecs me disent -Eff il casse! Qu'est-ce qui se passe Si tu dis qu'Eff ? est efficace Ok, dis le qu'on est là que nos dégâts sont des foutaises Blessés dans nos âmes, le rap nos armes, et elles vous plaisent Alors écoute et laisse l'esprit espiègle J'repars et reste fier, c'était Espiiem Fuck la vie d'russe, un texte de plus sur papyrus Et ouais, Homme de l'est, spontané, comme un freestyle sous l'abri-bus Avec ses gus tarés, 'paraît qu'j'suis minus 'paraît qu'toi tu saignes des sinus Enfoiré... Je suis violent, sur ce son je viens te violer Les rappeurs fleur bleue ont dalle de Roast-beef pas de billets violets J'espère que tout le monde ici a son tube ami M-ELO, je suis le Tsunami M-E-L-O Dans ce rap jeu, je suis l'Alpha, l'Oméga Le mégalo que personne n'égale au micro Les narco kiffent l'art nautique écoutent d'un pédalo Il n'y a qu'un Alpha mec, lis entre les lignes ne soit pas analphabète Flap style MC, back on the beat Pack a hit for the street Make the sound uniques Beat for the lover music, just do it Get up on this mouvement! Move it... Move it... Passe mon shit, chut, c'est un one shot Les chattes jactent tandis que les corbeaux chuchotent C'est le danger, j'vais me venger, j'suis un bil-dè Trop dérangé le R.A.P on va manger Greenzli impossible à glisser Black re-noi est pour le rap c'est qu'un iceberg est pour Titanic J'attrape le mic, tout le monde met soupape, tout le monde panique Les grizzlis c'est les équipes qui sont venues prendre toute la place Comme Hitler on fera pas semblant de te niquer ta race B.A.K.S.T.E.R si tu veux me tester de-mer J'suis tellement cé-fran qu'il va bientôt plus me rester de verbes J'ai fâcher les bites, j'ai froisser les types pour fracasser ? Costard sélectif mon rap c'est l'élite quand ??? c'est l'équipe Couplet en Anglais. Nekfeu, Mc chevelu, sans cesse j'évolue Je veux lutter, guetter ce que je suis devenu Divine entité, entêté, hanté, endetté, embêté Tâter la facilité, antithèse Areno Jaz, un as des micros ouverts Face à mes phases, les nases deviennent bleus ou verts Hey boy, t'es ébahis quand je fais mes bails Lâche 4 mesures en baillant et bye Flav' au mic, nouvel exercice Guette mon lexique VR6 Un wack s'pointe j'en fais mon affaire lui pète le plexus J'déboule d'une autre galaxie, emmerde les gars laxistes Lâche le P.O.S sûr qu'ça s'finit en dent-acci J'arrive dans le game, en force comme un chouara de bécane De ma bite t'as le béguin je suis célèbre comme David Beckham Deux-trois pétasses, une 8-6, un niaks, un texte cru Mephis débarque, je suis la menace -nace... Regarde le ciel, je suis l'OVNI du rap Big-up à celles qui dans mon lit dérapent J'rattrape le temps perdu car je m'étais égaré J'étais déjà partis quand toi tu t'es gâré Vagabond c'est trop arabesque Tellement j'ai les crocs je suis presque un clebs trop en chien J'coupe la laisse, tribu de l'Est Qui peut test, sauve qui peut on est des ti-peu de tieks Si l'écriture c'est une go bah je nique le texte Appelle moi S.N.E.A. double Z.Y Sneazzy éblouis comme le Crystal Waw mon squad est organisé pire que le SWAT Jilly Jordan, Casquette et fat sweet Loveni Lyricalchimie on est les best Je reste blesse tout les MC qui veulent test J'agresse, trop balèze, tu retournes ta veste En guest, viens bouger ta graisse dans ma fiesta ????? et reste dans les normes en étant pudique Mais j'en impose tellement que les gens m'appelle trésor public J'applique ma rime active, ma crise ma vie d'artiste Jadis chétif, jamais factice, MC avant-gardiste Ah, j'suis tellement bon que c'est sur moi que je place ma thune Quand toi t'es embourbé, Clean passe la dune La nuit tellement j'brille je remplace la Lune J'ai pas de lacune céleste je surclasse Saturne Yo, je suis atteint du songe, je tombe alcoolique A la renverse la tête dans une relation platonique Si je suis là c'est que j'ai de bons acolytes J'défonce la chronique, Joe explose comme une bombe atomique Les MC ne jurent que par Jazzy Bazz Je suis dans l'hémicycle le vent se dissipe J'fais des disciples et des kamikazes Le régime présidentiel en saigne, j'm'inspire des récits existentiels que l'Egypte ancienne m'enseigne J'lâche un quatre, et ton crâne désenfle En cas de démence, mic check, j'braque l'aisance J'aime le luxe et mes guys se dépensent Esso roule et n'est jamais en panne d'essence Les mecs aiment parler de dépouiller des poulets, et de bourrer des poulettes Toujours à pousser des couplets avec le Pooch à la russe roulettes Moi c'est Kema qui fait que tu mouilles dans ton boum short Et j'fais lever plus de bras en l'air que la police de New York C'est Issa, j'vis ça pas le temps pour les vieux textes J'te check si tu met 6 zéros sur mes deux chèques Ils zieutent sec, mais pourtant je suis pas comme eux mec Et je pose un genou à terre c'est pour mieux les prendre en levrette Je suis celui qu'on appelle B-O-R-M-A-N L'un de vous aurait-il une allumette juste le temps de rallumer ma haine Quoi que tu fasses je sais bien que c'est pour devenir une star J'te bats à pied connard, même si toi t'es en McLaren Des années j'en ai plus de 20, dix ans déjà que je suis le Devin Devant les gens, j'prends les devants micro en main J'fais s'écarquiller les yeux comme l'accomplissement d'un effet divin Rajoute le 2 devant mon arrondissement, bah ça fait Devin Ça parle de Glock et de chneck De rhum et de sauter l'jack Appuie sur stop eject si ta gorge tente l'éjac' Casse des chromes, dans les ventes je serais pas au top certes Si on s'croisse pas toujours remets ça à tes obsèques SERVAL MC!1</t>
         </is>
       </c>
     </row>
@@ -1597,12 +1597,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Dernière fois</t>
+          <t>Oulala</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Grand Master Pouchki flashe ta cousine comme un projecteur Alexandre traduit protecteur XXX comme lecteur cassettes CD ou DVD j'ai mille facettes Tu risques de décéder A,B,C,D j'te kill avec 2-zer washington des MC's j'en bâche une tonne Convoité jusqu'en Asie même si je parle pas chintok' Groupie je te croque ta pomme putain je suis comme MacIntosh Tu braques une banque, je dragues une moche, pendant que je matte une teuch O pour le niveau U car dans le son je sue Double H pour le hip-hop, blaze complexe comme un digicode Z pour la 'sique XXL sur le beat ! Ouhhz le magicien des beats et c'est déjà un classique J'crache des bouts d'texte, regarde ma tête je boude là J'traîne sur le boulevard, Belleville c'est le zoo gars C'est bel et bien Bloopalooza, du 20 moins 1 cousin, le 20ème mon voisin J'arrive de loin avec de lourdes phrases Couplet en Ukrainien Les coups qui décapent, décapsulent des cannettes Traque en lâchant des cases en flinguant linche les ca- -davre de s'hrab qui pue donc envoie des claques Pas de MicMac, j'paye mon Big Mac deluxe c'est Doc Polux! Accro d'esthétique, peu catholique depuis le berceau J'ai forgé ma critique sous psychotrope dans des tunnels de métro Parle de l'éthique MC Soul Costik , ?? Authentique Approche, oui approche et tend l'oreille à la parole d'un gavroche des temps modernes Approche, oui approche et tend l'oreille,c'est l'étrange juste un gosse de plus qui vous dérange J'rappe tout le temps mais je rêve que derrière un cro-mi Si j'perce, je continuerai d'creuser voila ce que j'ai promis Que mon son laisse une trace comme une ain-m sans gants Qu'on sache que Meassane veut dire âme sanglante Au mic c'est Eff, éphémère j'ai les nerfs 4 mesures c'est éphémère Les mecs me disent -Eff il casse! Qu'est-ce qui se passe Si tu dis qu'Eff ? est efficace Ok, dis le qu'on est là que nos dégâts sont des foutaises Blessés dans nos âmes, le rap nos armes, et elles vous plaisent Alors écoute et laisse l'esprit espiègle J'repars et reste fier, c'était Espiiem Fuck la vie d'russe, un texte de plus sur papyrus Et ouais, Homme de l'est, spontané, comme un freestyle sous l'abri-bus Avec ses gus tarés, 'paraît qu'j'suis minus 'paraît qu'toi tu saignes des sinus Enfoiré... Je suis violent, sur ce son je viens te violer Les rappeurs fleur bleue ont dalle de Roast-beef pas de billets violets J'espère que tout le monde ici a son tube ami M-ELO, je suis le Tsunami M-E-L-O Dans ce rap jeu, je suis l'Alpha, l'Oméga Le mégalo que personne n'égale au micro Les narco kiffent l'art nautique écoutent d'un pédalo Il n'y a qu'un Alpha mec, lis entre les lignes ne soit pas analphabète Flap style MC, back on the beat Pack a hit for the street Make the sound uniques Beat for the lover music, just do it Get up on this mouvement! Move it... Move it... Passe mon shit, chut, c'est un one shot Les chattes jactent tandis que les corbeaux chuchotent C'est le danger, j'vais me venger, j'suis un bil-dè Trop dérangé le R.A.P on va manger Greenzli impossible à glisser Black re-noi est pour le rap c'est qu'un iceberg est pour Titanic J'attrape le mic, tout le monde met soupape, tout le monde panique Les grizzlis c'est les équipes qui sont venues prendre toute la place Comme Hitler on fera pas semblant de te niquer ta race B.A.K.S.T.E.R si tu veux me tester de-mer J'suis tellement cé-fran qu'il va bientôt plus me rester de verbes J'ai fâcher les bites, j'ai froisser les types pour fracasser ? Costard sélectif mon rap c'est l'élite quand ??? c'est l'équipe Couplet en Anglais. Nekfeu, Mc chevelu, sans cesse j'évolue Je veux lutter, guetter ce que je suis devenu Divine entité, entêté, hanté, endetté, embêté Tâter la facilité, antithèse Areno Jaz, un as des micros ouverts Face à mes phases, les nases deviennent bleus ou verts Hey boy, t'es ébahis quand je fais mes bails Lâche 4 mesures en baillant et bye Flav' au mic, nouvel exercice Guette mon lexique VR6 Un wack s'pointe j'en fais mon affaire lui pète le plexus J'déboule d'une autre galaxie, emmerde les gars laxistes Lâche le P.O.S sûr qu'ça s'finit en dent-acci J'arrive dans le game, en force comme un chouara de bécane De ma bite t'as le béguin je suis célèbre comme David Beckham Deux-trois pétasses, une 8-6, un niaks, un texte cru Mephis débarque, je suis la menace -nace... Regarde le ciel, je suis l'OVNI du rap Big-up à celles qui dans mon lit dérapent J'rattrape le temps perdu car je m'étais égaré J'étais déjà partis quand toi tu t'es gâré Vagabond c'est trop arabesque Tellement j'ai les crocs je suis presque un clebs trop en chien J'coupe la laisse, tribu de l'Est Qui peut test, sauve qui peut on est des ti-peu de tieks Si l'écriture c'est une go bah je nique le texte Appelle moi S.N.E.A. double Z.Y Sneazzy éblouis comme le Crystal Waw mon squad est organisé pire que le SWAT Jilly Jordan, Casquette et fat sweet Loveni Lyricalchimie on est les best Je reste blesse tout les MC qui veulent test J'agresse, trop balèze, tu retournes ta veste En guest, viens bouger ta graisse dans ma fiesta ????? et reste dans les normes en étant pudique Mais j'en impose tellement que les gens m'appelle trésor public J'applique ma rime active, ma crise ma vie d'artiste Jadis chétif, jamais factice, MC avant-gardiste Ah, j'suis tellement bon que c'est sur moi que je place ma thune Quand toi t'es embourbé, Clean passe la dune La nuit tellement j'brille je remplace la Lune J'ai pas de lacune céleste je surclasse Saturne Yo, je suis atteint du songe, je tombe alcoolique A la renverse la tête dans une relation platonique Si je suis là c'est que j'ai de bons acolytes J'défonce la chronique, Joe explose comme une bombe atomique Les MC ne jurent que par Jazzy Bazz Je suis dans l'hémicycle le vent se dissipe J'fais des disciples et des kamikazes Le régime présidentiel en saigne, j'm'inspire des récits existentiels que l'Egypte ancienne m'enseigne J'lâche un quatre, et ton crâne désenfle En cas de démence, mic check, j'braque l'aisance J'aime le luxe et mes guys se dépensent Esso roule et n'est jamais en panne d'essence Les mecs aiment parler de dépouiller des poulets, et de bourrer des poulettes Toujours à pousser des couplets avec le Pooch à la russe roulettes Moi c'est Kema qui fait que tu mouilles dans ton boum short Et j'fais lever plus de bras en l'air que la police de New York C'est Issa, j'vis ça pas le temps pour les vieux textes J'te check si tu met 6 zéros sur mes deux chèques Ils zieutent sec, mais pourtant je suis pas comme eux mec Et je pose un genou à terre c'est pour mieux les prendre en levrette Je suis celui qu'on appelle B-O-R-M-A-N L'un de vous aurait-il une allumette juste le temps de rallumer ma haine Quoi que tu fasses je sais bien que c'est pour devenir une star J'te bats à pied connard, même si toi t'es en McLaren Des années j'en ai plus de 20, dix ans déjà que je suis le Devin Devant les gens, j'prends les devants micro en main J'fais s'écarquiller les yeux comme l'accomplissement d'un effet divin Rajoute le 2 devant mon arrondissement, bah ça fait Devin Ça parle de Glock et de chneck De rhum et de sauter l'jack Appuie sur stop eject si ta gorge tente l'éjac' Casse des chromes, dans les ventes je serais pas au top certes Si on s'croisse pas toujours remets ça à tes obsèques SERVAL MC!1</t>
+          <t>On a grandi dans ce bloc, on a grandi tous ensemble Nous on va racheter le bloc, on va racheter toute la rue On a grandi dans ce bloc, on a grandi entre frères Nous on va racheter le bloc On a grandi dans ce bloc, on a grandi tous ensemble Nous on va racheter le bloc, on va racheter toute la rue On a grandi dans ce bloc, on a grandi entre frères Nous on va racheter le bloc M comme la mala qu'on vesqui F comme le fire qu'il faut cer-lan quand j'm'exprime D comme le système, me demande pas si j'aime Depuis Les chroniques du mystère, on daba les képis Ils veulent pécho la weed mais elle est pas dans les Teddy Planquée dans les yeu-cou, t'aventure pas dans l'récif Habitué aux yeu-dou, j'suis là-d'dans d'puis la tétine Eh eh, deux s'condes j't'explique Pas de P.O.R.C. dans mon C.O.R.P.S J'porte mon honneur jusqu'à la M.O.R.T J'm'appelle M.F.D., pas b'soin d'LSD pour gérer les miss C'est lundi, j'suis en R.L.P. le dimanche, en P.S.G Vu mes rêves, auprès d'mes frères, j'me dois d'faire mieux, L.O.R.D Dis-moi comment faire, fumer d'l'herbe et emmerder la B.R.B Si tu m'le permets Oulala oulala, les leurs veulent attraper les miens Mais le destin nous aura pas, je peux le voir de tout là-bas Oulala oulala, c'est 2zer et dou-Mama Le succès arrive à grands pas, je peux le voir de tout là-bas Oulala oulala, les leurs veulent attraper les miens Mais le destin nous aura pas, je peux le voir de tout là-bas Oulala oulala, c'est 2zer et dou-Mama Le succès arrive à grands pas, je peux le voir de tout là-bas J'me suis trompé de pellicule, j'vois tout en négatif Et mon seul sédatif c'est de recompter les thunes Pas facile d'être un artiste on charbonne, on est actif Après une tempête de sable, il faut remonter les dunes Je ne veux pas du monde à mes pieds Je veux, que mon nom, tout le monde sache l'épeler Ouais, j'ai un train de vie de fêlé La vie c'est pas la télé mais j'veux zapper quand ça me déplaît Ouais, j'vais pas rentrer dans l'détail mais on a plié de la féraille Que mon train de vie en déraille, yeah On m'avait dit Dans tes rêves mais j'ai la tête dure Comme sur Twitter, toujours en TT Sur l'passage de mon train de vie Toujours plus vite retiens la devise Trop de bons souvenirs, le stockage est bientôt saturé Donc j'ai déjà zappé tout ce que je viens de vivre J'essaie de bien m'tenir mais c'est rien de l'dire Un homme qui n'agit pas, il n'y a rien de pire Tu prends de l'âge et ça tu ne le vois pas venir Le temps qui passe te fera breaker comme une feinte de tir Oulala oulala, les leurs veulent attraper les miens Mais le destin nous aura pas, je peux le voir de tout là-bas Oulala oulala, c'est 2zer et Doumama Le succès arrive à grands pas, je peux le voir de tout là-bas Oulala oulala, les leurs veulent attraper les miens Mais le destin nous aura pas, je peux le voir de tout là-bas Oulala oulala, c'est 2zer et Doumama Le succès arrive à grands pas, je peux le voir de tout là-bas On a grandi dans ce bloc, on a grandi tous ensemble Nous on va racheter le bloc, on va racheter toute la rue On a grandi dans ce bloc, on a grandi entre frères Nous on va racheter le bloc On a grandi dans ce bloc, on a grandi tous ensemble Nous on va racheter le bloc, on va racheter toute la rue On a grandi dans ce bloc, on a grandi entre frères Nous on va racheter le bloc Hugz t'es en feu sur celle-là2</t>
         </is>
       </c>
     </row>
@@ -1614,12 +1614,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Oulala</t>
+          <t>#25 télé rap</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>On a grandi dans ce bloc, on a grandi tous ensemble Nous on va racheter le bloc, on va racheter toute la rue On a grandi dans ce bloc, on a grandi entre frères Nous on va racheter le bloc On a grandi dans ce bloc, on a grandi tous ensemble Nous on va racheter le bloc, on va racheter toute la rue On a grandi dans ce bloc, on a grandi entre frères Nous on va racheter le bloc M comme la mala qu'on vesqui F comme le fire qu'il faut cer-lan quand j'm'exprime D comme le système, me demande pas si j'aime Depuis Les chroniques du mystère, on daba les képis Ils veulent pécho la weed mais elle est pas dans les Teddy Planquée dans les yeu-cou, t'aventure pas dans l'récif Habitué aux yeu-dou, j'suis là-d'dans d'puis la tétine Eh eh, deux s'condes j't'explique Pas de P.O.R.C. dans mon C.O.R.P.S J'porte mon honneur jusqu'à la M.O.R.T J'm'appelle M.F.D., pas b'soin d'LSD pour gérer les miss C'est lundi, j'suis en R.L.P. le dimanche, en P.S.G Vu mes rêves, auprès d'mes frères, j'me dois d'faire mieux, L.O.R.D Dis-moi comment faire, fumer d'l'herbe et emmerder la B.R.B Si tu m'le permets Oulala oulala, les leurs veulent attraper les miens Mais le destin nous aura pas, je peux le voir de tout là-bas Oulala oulala, c'est 2zer et dou-Mama Le succès arrive à grands pas, je peux le voir de tout là-bas Oulala oulala, les leurs veulent attraper les miens Mais le destin nous aura pas, je peux le voir de tout là-bas Oulala oulala, c'est 2zer et dou-Mama Le succès arrive à grands pas, je peux le voir de tout là-bas J'me suis trompé de pellicule, j'vois tout en négatif Et mon seul sédatif c'est de recompter les thunes Pas facile d'être un artiste on charbonne, on est actif Après une tempête de sable, il faut remonter les dunes Je ne veux pas du monde à mes pieds Je veux, que mon nom, tout le monde sache l'épeler Ouais, j'ai un train de vie de fêlé La vie c'est pas la télé mais j'veux zapper quand ça me déplaît Ouais, j'vais pas rentrer dans l'détail mais on a plié de la féraille Que mon train de vie en déraille, yeah On m'avait dit Dans tes rêves mais j'ai la tête dure Comme sur Twitter, toujours en TT Sur l'passage de mon train de vie Toujours plus vite retiens la devise Trop de bons souvenirs, le stockage est bientôt saturé Donc j'ai déjà zappé tout ce que je viens de vivre J'essaie de bien m'tenir mais c'est rien de l'dire Un homme qui n'agit pas, il n'y a rien de pire Tu prends de l'âge et ça tu ne le vois pas venir Le temps qui passe te fera breaker comme une feinte de tir Oulala oulala, les leurs veulent attraper les miens Mais le destin nous aura pas, je peux le voir de tout là-bas Oulala oulala, c'est 2zer et Doumama Le succès arrive à grands pas, je peux le voir de tout là-bas Oulala oulala, les leurs veulent attraper les miens Mais le destin nous aura pas, je peux le voir de tout là-bas Oulala oulala, c'est 2zer et Doumama Le succès arrive à grands pas, je peux le voir de tout là-bas On a grandi dans ce bloc, on a grandi tous ensemble Nous on va racheter le bloc, on va racheter toute la rue On a grandi dans ce bloc, on a grandi entre frères Nous on va racheter le bloc On a grandi dans ce bloc, on a grandi tous ensemble Nous on va racheter le bloc, on va racheter toute la rue On a grandi dans ce bloc, on a grandi entre frères Nous on va racheter le bloc Hugz t'es en feu sur celle-là2</t>
+          <t>Maman, écoute je passe à la télé Mon son fait la B.O de ce reportage sur la cité Entre drogue, alcool, baston d'ivrogne Foye, c'est la seul place qu'on laisse à mon hip-hop Du pe-ra dans les tubes cathodiques Quoi, ils auraient peur qu'on dise des trucs pas très catholiques ? Dans l'immédiat, faut du Hip-Hop dans les médias, sérieux A force de voir des clips de merde j'vais devenir sourd des yeux Du rap à la télé ? Ma foi, mais pas n'importe lequel Faut surtout pas que ça soit les les wacks qui mattent le game J'veux voir du bon son, quand je zappe les chaînes Pas de MCs comédiennes qui s'crêpent le chignon comme des collégiennes J'n'allume plus ma télé car j'suis perdu dans tout ce pêle-mêle Besoin de changement donc parlez-en à monsieur Belmer Certains programmes me stressent autant qu'ma future belle-mère J'me permet d'en parler car j'peux pas cautionner de telles merdes Du rap sur Canal ou D8 ? Ils t'laissent espérer Font passer mes gars pour des types genre pestiférés Dis moi qu'est-ce qu't'y ferais toi ? des flows-syllabes ? La plupart pensent qu'on fait rimer que yo, zy-va Ça serait bien un jour de voir notre vraie culture sur ton écran Rien de crade dans nos écrits alors un cri d'alerte s'impose mon grand Gros, plein d'MCs d'talents attendent une chose c'est d'être choisis Eh oui y'en a marre des sosies nous pondant des morceaux moisis Pour être honnête on en a marre de vos sornettes Mettez-nous du bon Hip-Hop à la télé et non vos soupes Nan, nan du talent dans nos rues en soif de diffusion Mais vos starlettes qui chantent en boucle man à l'unisson J'ai beau croiser les mots, j'ai pas ma place à Mots croisés Tu fais du rap variété ? Y'a Pop Star pour faire jury Petit appel à Yves Calvi, invite-nous je t'en supplie Passe-nous chercher, on est bloqué de Sept à huit chez Harry Télé ma douce tu sais, t'as peur du H.I.P C'est fou c'que t'as choppé à force de debats peu futés Le marchand dans les prés XXX C'est qu'les plumes bien aiguisées doivent deranger Notez mon drop name, les gens d'la télé poto Zem' ? Non, non juste Naulleau, paix à Cyril et tout sa collo... ...nel blague de merde style Thierry Moreau Je sors mais j'compte sur Enora pour faire la promo Y'avait du H.I.P-H.O.P à l'époque sur TF1 Les chaînes ont déserté l'chantier, dans l'R.A.P mec on est pleins MTV, OFIVE, Trace TV j'veux plus de place pour péter l'blocus Plus de culte pour ma zic sur France Télé et Canal On veut du Hip-Hop à la télé, y'a plus d'Hip-Hop à la télé J'ai un tas d'CV, pas d'CB pour t'lâcher un Track TV Hip-Hop à la télé, y'a plus d'Hip-Hop à la télé On attend l'retour d'Maïté pour voir quelques carottes rappées On veut du Hip-Hop à la télé, qu'ça tourne en boucle dans les médias Dans l'immédiat te faire kiffer le rap même si tu l'aimais déjà Et boom, ça s'rait cool qu'ça chamboule tout le petit écran Pour faire kiffer notre culture, pour les petits et les grands On viens pour dominer l'gamin avec mon Armada d'félés On veut du rap à la télé, demande à Olivier Cachin On envahit les ondes, assieds-toi et détends-toi J'ammène des filles qui ont des formes même dans un écran plat Négro, y'a quoi sur l'écran plasma ? Rien de nouveau Pourtant, des trucs de oufs s'passe dans le rap mais on les passent pas Tu veux du Ghetto Blaster, du hip-hop dans les iPod Clique, clique c'est l'tour de passe-passe, tu m'verras dans ton poste Ici on rêve qu'le rideau s'lève, qu'le hip-hop crève l'écran Le rap innove, le PAF ignore, faut bien qu'on prenne les devants Ouais, on nous passe pas à la télé tant qu'on représente sur lasphalte Ils nous traitent comme des araignées donc nous on s'répend sur la toile On veut du hip hop au max, réalisé par Pullicino De vrais magazines, l'époque de Sear ou Texaco Qu'on nous redonne du power, interviews de Fabe et Hour T'imagines Lemdi Moax présentés par Roselmack J'demande un p'tit peu plus de vue , de rap dans les médias Immédiatement j'réclame toutes les images de la rime idéale La France d'en bas comme toi qui trime et bave On veut tous se voir ensemble, arrêtez-les comme crime et balle Trop mat pour France Télé', trop foncé pour M6 Black Malgrès les portes enfoncées et les blagues Or et platine, cherche ma rage dans l'paysage musical français Comme un mic en platine pour defoncer les barrages Sale rap, j'ai gâché ma vie, raté la tienne T'auras jamais eu d'JT J'aurai p't'être mieux fait d'caner aux Etats-Unis Au bout d'un cable ou à la TNT And I've been thinking and i'm done with the thinking of blinking XXX on bitches who rob me, you riches In fact XXX bringing back will never fade into black Hip-hop XXX on your screen Et tu zappes, et tu zappes, affalé dans le canap' Toujours les mêmes blabla que tu mattes, les mêmes salades qu'ils nous jactent Qui a dit qu'l'audimat, lui, ne voulait pas de rap ? C'est à la TNT, les gars, qu'on va faire péter le cable Depuis Zemmour et Naulleau, les chaînes éguisent leurs couteaux Tandis qu'la France aux fachos, attendent le dérapage de trop, oh Rap et télévision Rapport sous pression Il voudrait qu'on reste muet. Véronique Sanson Peu d'MCs sur M6 le canal est étroit, semble t-il Oui je pense qu'il est tant de franchir le détroit, simple type J'excelle, loin des strass et des Seychelles Avant de passer à l'écran, il faut se libérer de ses chaines Faut pas rêver, y'aura jamais d'hip-hop à la télé Ces salopes préfèrent les émissions sur les flics zélés Trop d'talk-show pour bobo, présenté par des homos Cesse ça, on veut des trucs pour les prolos Je garde des bases en vain Je suis partisan d'aucune démarche, tu t'occupes des masses et des débats sans fin Est-ce que la télé les pousse à la réflexion ? Non, elle séduit le vice dont elle est l'épouse Fait nous d'la place, on a la couleur, pas du noir et blanc Mate ma face, ouais non n'aie pas peur que je crève l'écran Ou bien, pas d'brasser du vent mon rap prend les devants On attend pas Vivement dimanche allongé sur le divan Yo, mon hip-hop est là, il n'veut pas bougé Il est pas couché, quand tu le vois tes enfants aiment bouger Mais crois moi il sait faire le taf Il a sa place sur le PAF, ouais il va pas t'faire de farce On mate pas la télé on veut qu'la télé nous matte, man Et trop d'rappeurs puent la merde mais ils sont dans les bacs Et trop d'rappeurs s'appellent chef mais ils font cuir des pâtes Alors diffuse nous sur le cable avant qu'on pète le cable Ca fait longtemps qu'les portes sont fermées Longtemps qu'ils nous on cernés, pour exister en marge faut savoir se démerder Mais pourtant, les miens on b'soin d'lumières et d'rêver Ammenez-les, gars, la télé et montrez-les qu'on peut s'aimer Ils veulent nos benefs comme des fils de vampes on est pas dans les plans On a des places mais passe pas à l'écran malgrès les chiffres de ventes On a la maitrise mais ces types là ils méprisent le genre Et ça m'déprime c'est c'qui m'épuise car ça métisse les gens On veut du rap sale des vrais trucs, pas d'la fiction J'veux qu'mes partitions squattent le générique d'Ardisson Soit, du rap sur les écrans pas leur parti d'con Rien qu'des fouines chanceux, tout ceux qui l'ont admis l'son Encore en bal pas d'bol alertez-les Mon quarties fédéral dans les rudes rues khoya fait qu'trainer Ils s'attelent à chuter pseudo-gang et fashion boy de mes couilles Pas qu'on ne m'écoute en boucle sans passer par la télé Malgré les boycotts, les vengeances on est toujours à jour Il faut qu'on provoque des tendances, allez le dire à Mouloud Achour Spécialiste en langue de bois, on les appelle les ébenistes Oubli Roland Garros, j'crois qu'j'f'rais mieux d'racketter des tennis K-Ly Impitoyable comme maître d'esclave Les médias ont ma sous-culture dans l'viseur et tente de la rendre détestable Plus de hip-hop en télé' ferait bander les jeunes Ferait kiffer la street et rendrait p't-être Morandini moins cheum Y'a plus de vérité, dans une boule magique ou une rette-ba Selon leurs dires j'suis une racaille, même moi j'l'e savait même pas Ça m'fédère car devant la télé j'tappe des barres des rires Moi j'ai l'impact des rimes, et de l'information d'vant l'JT d'Derka Comme tous les amateurs de hip-hop, j'veux plus de rap à la télé Demande à A2' ou Abraham, j'suis un négro fêlé J'suis recherché par Scully et Mulder, appelle moi E.T J'aimerais que MC soit considéré comme B.E.T Un peu de hip-hop de Paris à Memphis On voudrait entendre plus de vrais titres en playlist En bref, pour que tous mes gens relativisent Mettez-nous plus de hip-hop à la TV Du rap à la télé, faudrait s'y atteler Sans forcément avoir à se faire plus de blé qu'on est, ou rentré dans le moule imposé On veut des moyens de diffusion sans participer À l'abrutissement général, aujourd'hui plébiscité Youm Vas dire aux medias d'ici qu'on est les poetes des temps modernes Que la mort de Biggie me touche autant que celle de Jean Jaures On m'parle de sous culture franchement j'trouve ça abusé On s'battra pour qu'cet art prenne sa place, qu'on le grave dans les musées Elle passe ses soirées à les apaiser, ce qu'elle leur sert est pré-mâché Les enfants d'la télé sont maternés Elle pourrait leur offrir subversion, poésie, subtilité Mais n'a qu'un tas de chaînes pour les immobiliser Comme l'impression qu'nos rimes sont nées dans un corbillard Car Michel Druker veut rien lâcher comme Paul Bia Toujours à dénigrer le hip-hop de France Alors qu'on pourrait faire autant d'audience que l'dernier épisode de Friends Faut qu'on fasse quelque chose dans l'immédiat On voit pas assez nos gueules dans les médias Ca tombe bien, j'recherchai du boulot Ca paye combien pour remplacer Jean-Pierre Foucault ? Eh mais oh mais c'est fini la télé ci-gît la clef sur le palier Vos promos d'rats et d'rateliers le temps l'état T'inquiète qu'il s'aime le rap çais-fran bientôt 30 ans qu'il donne le la Donc vous réveillez pas maintenant vous avez déjà raté tout ça Je pense donc je suis, mais je ne suis pas ce qu'il pense J'ai qu'une seule direction, j'écris des phrases à double sens Discours monocorde, les médias ont la langue pendue Certains rappeurs ont craqués parce que percer d'vient tendu Le hip-hop est un art brut trainé dans la boue Avoue, les adjectifs négatifs fleurissent dans les bouches Le PAF taf et cliché au pif mis bout à bout Laissez-nous l'antenne avec qu'les téléspectateurs se couchent Pas de hip-hop à la télé, sont-ils félés ? Qui fait les ventes, fait les modes, les B.O d'leur docu' clichés ? Me parlez pas de sous-culture Ils crachaient sur le jazz, aujourd'hui s'astiquent dessus Bonne nouvelle madame Chazal, je lis Claire dans vos yeux Attention à la marche, nan le rap n'est pas un jeu Hey, on n'est pas couché et c'est pour ça qu'tout l'monde en parle Puis on trouv'ra le sommeil quand y'aura du hip-hop en prime En 84, y'avait des battles sur la une Aujourd'hui je zappe, matte ma gueule pas d'culture du bitume Pourant ont fait les thunes, nos raps les solvables Hip-hop soldat, nos concerts sold-out J'aspire à être un tueur, j'veux crever l'écran Etre sur la une, la deux comme l'ont fait les grands J'veut péter les cartes qu'on m'entende l'été dans les câbles Etre en grand dans l'journal, les jaloux vont péter un câble Chaque jours je constate qu'on nous boycotte, tant qu'on ne fait de la pop Vu l'peura que j'apporte, TF1 m'laisse pas passer près de la porte J'ai tout essayer, entêté comme Antoine, mais Le bon rap en télé est rare comme le soleil en ce mois de Mai</t>
         </is>
       </c>
     </row>
@@ -1631,12 +1631,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>#25 télé rap</t>
+          <t>L’ Freestyle</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Maman, écoute je passe à la télé Mon son fait la B.O de ce reportage sur la cité Entre drogue, alcool, baston d'ivrogne Foye, c'est la seul place qu'on laisse à mon hip-hop Du pe-ra dans les tubes cathodiques Quoi, ils auraient peur qu'on dise des trucs pas très catholiques ? Dans l'immédiat, faut du Hip-Hop dans les médias, sérieux A force de voir des clips de merde j'vais devenir sourd des yeux Du rap à la télé ? Ma foi, mais pas n'importe lequel Faut surtout pas que ça soit les les wacks qui mattent le game J'veux voir du bon son, quand je zappe les chaînes Pas de MCs comédiennes qui s'crêpent le chignon comme des collégiennes J'n'allume plus ma télé car j'suis perdu dans tout ce pêle-mêle Besoin de changement donc parlez-en à monsieur Belmer Certains programmes me stressent autant qu'ma future belle-mère J'me permet d'en parler car j'peux pas cautionner de telles merdes Du rap sur Canal ou D8 ? Ils t'laissent espérer Font passer mes gars pour des types genre pestiférés Dis moi qu'est-ce qu't'y ferais toi ? des flows-syllabes ? La plupart pensent qu'on fait rimer que yo, zy-va Ça serait bien un jour de voir notre vraie culture sur ton écran Rien de crade dans nos écrits alors un cri d'alerte s'impose mon grand Gros, plein d'MCs d'talents attendent une chose c'est d'être choisis Eh oui y'en a marre des sosies nous pondant des morceaux moisis Pour être honnête on en a marre de vos sornettes Mettez-nous du bon Hip-Hop à la télé et non vos soupes Nan, nan du talent dans nos rues en soif de diffusion Mais vos starlettes qui chantent en boucle man à l'unisson J'ai beau croiser les mots, j'ai pas ma place à Mots croisés Tu fais du rap variété ? Y'a Pop Star pour faire jury Petit appel à Yves Calvi, invite-nous je t'en supplie Passe-nous chercher, on est bloqué de Sept à huit chez Harry Télé ma douce tu sais, t'as peur du H.I.P C'est fou c'que t'as choppé à force de debats peu futés Le marchand dans les prés XXX C'est qu'les plumes bien aiguisées doivent deranger Notez mon drop name, les gens d'la télé poto Zem' ? Non, non juste Naulleau, paix à Cyril et tout sa collo... ...nel blague de merde style Thierry Moreau Je sors mais j'compte sur Enora pour faire la promo Y'avait du H.I.P-H.O.P à l'époque sur TF1 Les chaînes ont déserté l'chantier, dans l'R.A.P mec on est pleins MTV, OFIVE, Trace TV j'veux plus de place pour péter l'blocus Plus de culte pour ma zic sur France Télé et Canal On veut du Hip-Hop à la télé, y'a plus d'Hip-Hop à la télé J'ai un tas d'CV, pas d'CB pour t'lâcher un Track TV Hip-Hop à la télé, y'a plus d'Hip-Hop à la télé On attend l'retour d'Maïté pour voir quelques carottes rappées On veut du Hip-Hop à la télé, qu'ça tourne en boucle dans les médias Dans l'immédiat te faire kiffer le rap même si tu l'aimais déjà Et boom, ça s'rait cool qu'ça chamboule tout le petit écran Pour faire kiffer notre culture, pour les petits et les grands On viens pour dominer l'gamin avec mon Armada d'félés On veut du rap à la télé, demande à Olivier Cachin On envahit les ondes, assieds-toi et détends-toi J'ammène des filles qui ont des formes même dans un écran plat Négro, y'a quoi sur l'écran plasma ? Rien de nouveau Pourtant, des trucs de oufs s'passe dans le rap mais on les passent pas Tu veux du Ghetto Blaster, du hip-hop dans les iPod Clique, clique c'est l'tour de passe-passe, tu m'verras dans ton poste Ici on rêve qu'le rideau s'lève, qu'le hip-hop crève l'écran Le rap innove, le PAF ignore, faut bien qu'on prenne les devants Ouais, on nous passe pas à la télé tant qu'on représente sur lasphalte Ils nous traitent comme des araignées donc nous on s'répend sur la toile On veut du hip hop au max, réalisé par Pullicino De vrais magazines, l'époque de Sear ou Texaco Qu'on nous redonne du power, interviews de Fabe et Hour T'imagines Lemdi Moax présentés par Roselmack J'demande un p'tit peu plus de vue , de rap dans les médias Immédiatement j'réclame toutes les images de la rime idéale La France d'en bas comme toi qui trime et bave On veut tous se voir ensemble, arrêtez-les comme crime et balle Trop mat pour France Télé', trop foncé pour M6 Black Malgrès les portes enfoncées et les blagues Or et platine, cherche ma rage dans l'paysage musical français Comme un mic en platine pour defoncer les barrages Sale rap, j'ai gâché ma vie, raté la tienne T'auras jamais eu d'JT J'aurai p't'être mieux fait d'caner aux Etats-Unis Au bout d'un cable ou à la TNT And I've been thinking and i'm done with the thinking of blinking XXX on bitches who rob me, you riches In fact XXX bringing back will never fade into black Hip-hop XXX on your screen Et tu zappes, et tu zappes, affalé dans le canap' Toujours les mêmes blabla que tu mattes, les mêmes salades qu'ils nous jactent Qui a dit qu'l'audimat, lui, ne voulait pas de rap ? C'est à la TNT, les gars, qu'on va faire péter le cable Depuis Zemmour et Naulleau, les chaînes éguisent leurs couteaux Tandis qu'la France aux fachos, attendent le dérapage de trop, oh Rap et télévision Rapport sous pression Il voudrait qu'on reste muet. Véronique Sanson Peu d'MCs sur M6 le canal est étroit, semble t-il Oui je pense qu'il est tant de franchir le détroit, simple type J'excelle, loin des strass et des Seychelles Avant de passer à l'écran, il faut se libérer de ses chaines Faut pas rêver, y'aura jamais d'hip-hop à la télé Ces salopes préfèrent les émissions sur les flics zélés Trop d'talk-show pour bobo, présenté par des homos Cesse ça, on veut des trucs pour les prolos Je garde des bases en vain Je suis partisan d'aucune démarche, tu t'occupes des masses et des débats sans fin Est-ce que la télé les pousse à la réflexion ? Non, elle séduit le vice dont elle est l'épouse Fait nous d'la place, on a la couleur, pas du noir et blanc Mate ma face, ouais non n'aie pas peur que je crève l'écran Ou bien, pas d'brasser du vent mon rap prend les devants On attend pas Vivement dimanche allongé sur le divan Yo, mon hip-hop est là, il n'veut pas bougé Il est pas couché, quand tu le vois tes enfants aiment bouger Mais crois moi il sait faire le taf Il a sa place sur le PAF, ouais il va pas t'faire de farce On mate pas la télé on veut qu'la télé nous matte, man Et trop d'rappeurs puent la merde mais ils sont dans les bacs Et trop d'rappeurs s'appellent chef mais ils font cuir des pâtes Alors diffuse nous sur le cable avant qu'on pète le cable Ca fait longtemps qu'les portes sont fermées Longtemps qu'ils nous on cernés, pour exister en marge faut savoir se démerder Mais pourtant, les miens on b'soin d'lumières et d'rêver Ammenez-les, gars, la télé et montrez-les qu'on peut s'aimer Ils veulent nos benefs comme des fils de vampes on est pas dans les plans On a des places mais passe pas à l'écran malgrès les chiffres de ventes On a la maitrise mais ces types là ils méprisent le genre Et ça m'déprime c'est c'qui m'épuise car ça métisse les gens On veut du rap sale des vrais trucs, pas d'la fiction J'veux qu'mes partitions squattent le générique d'Ardisson Soit, du rap sur les écrans pas leur parti d'con Rien qu'des fouines chanceux, tout ceux qui l'ont admis l'son Encore en bal pas d'bol alertez-les Mon quarties fédéral dans les rudes rues khoya fait qu'trainer Ils s'attelent à chuter pseudo-gang et fashion boy de mes couilles Pas qu'on ne m'écoute en boucle sans passer par la télé Malgré les boycotts, les vengeances on est toujours à jour Il faut qu'on provoque des tendances, allez le dire à Mouloud Achour Spécialiste en langue de bois, on les appelle les ébenistes Oubli Roland Garros, j'crois qu'j'f'rais mieux d'racketter des tennis K-Ly Impitoyable comme maître d'esclave Les médias ont ma sous-culture dans l'viseur et tente de la rendre détestable Plus de hip-hop en télé' ferait bander les jeunes Ferait kiffer la street et rendrait p't-être Morandini moins cheum Y'a plus de vérité, dans une boule magique ou une rette-ba Selon leurs dires j'suis une racaille, même moi j'l'e savait même pas Ça m'fédère car devant la télé j'tappe des barres des rires Moi j'ai l'impact des rimes, et de l'information d'vant l'JT d'Derka Comme tous les amateurs de hip-hop, j'veux plus de rap à la télé Demande à A2' ou Abraham, j'suis un négro fêlé J'suis recherché par Scully et Mulder, appelle moi E.T J'aimerais que MC soit considéré comme B.E.T Un peu de hip-hop de Paris à Memphis On voudrait entendre plus de vrais titres en playlist En bref, pour que tous mes gens relativisent Mettez-nous plus de hip-hop à la TV Du rap à la télé, faudrait s'y atteler Sans forcément avoir à se faire plus de blé qu'on est, ou rentré dans le moule imposé On veut des moyens de diffusion sans participer À l'abrutissement général, aujourd'hui plébiscité Youm Vas dire aux medias d'ici qu'on est les poetes des temps modernes Que la mort de Biggie me touche autant que celle de Jean Jaures On m'parle de sous culture franchement j'trouve ça abusé On s'battra pour qu'cet art prenne sa place, qu'on le grave dans les musées Elle passe ses soirées à les apaiser, ce qu'elle leur sert est pré-mâché Les enfants d'la télé sont maternés Elle pourrait leur offrir subversion, poésie, subtilité Mais n'a qu'un tas de chaînes pour les immobiliser Comme l'impression qu'nos rimes sont nées dans un corbillard Car Michel Druker veut rien lâcher comme Paul Bia Toujours à dénigrer le hip-hop de France Alors qu'on pourrait faire autant d'audience que l'dernier épisode de Friends Faut qu'on fasse quelque chose dans l'immédiat On voit pas assez nos gueules dans les médias Ca tombe bien, j'recherchai du boulot Ca paye combien pour remplacer Jean-Pierre Foucault ? Eh mais oh mais c'est fini la télé ci-gît la clef sur le palier Vos promos d'rats et d'rateliers le temps l'état T'inquiète qu'il s'aime le rap çais-fran bientôt 30 ans qu'il donne le la Donc vous réveillez pas maintenant vous avez déjà raté tout ça Je pense donc je suis, mais je ne suis pas ce qu'il pense J'ai qu'une seule direction, j'écris des phrases à double sens Discours monocorde, les médias ont la langue pendue Certains rappeurs ont craqués parce que percer d'vient tendu Le hip-hop est un art brut trainé dans la boue Avoue, les adjectifs négatifs fleurissent dans les bouches Le PAF taf et cliché au pif mis bout à bout Laissez-nous l'antenne avec qu'les téléspectateurs se couchent Pas de hip-hop à la télé, sont-ils félés ? Qui fait les ventes, fait les modes, les B.O d'leur docu' clichés ? Me parlez pas de sous-culture Ils crachaient sur le jazz, aujourd'hui s'astiquent dessus Bonne nouvelle madame Chazal, je lis Claire dans vos yeux Attention à la marche, nan le rap n'est pas un jeu Hey, on n'est pas couché et c'est pour ça qu'tout l'monde en parle Puis on trouv'ra le sommeil quand y'aura du hip-hop en prime En 84, y'avait des battles sur la une Aujourd'hui je zappe, matte ma gueule pas d'culture du bitume Pourant ont fait les thunes, nos raps les solvables Hip-hop soldat, nos concerts sold-out J'aspire à être un tueur, j'veux crever l'écran Etre sur la une, la deux comme l'ont fait les grands J'veut péter les cartes qu'on m'entende l'été dans les câbles Etre en grand dans l'journal, les jaloux vont péter un câble Chaque jours je constate qu'on nous boycotte, tant qu'on ne fait de la pop Vu l'peura que j'apporte, TF1 m'laisse pas passer près de la porte J'ai tout essayer, entêté comme Antoine, mais Le bon rap en télé est rare comme le soleil en ce mois de Mai</t>
+          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
         </is>
       </c>
     </row>
@@ -1648,12 +1648,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>L’ Freestyle</t>
+          <t>20 mesures</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
+          <t>J'suis pas Escobar, j'aborde Paname pour refourguer ma came J'me sens rejeté, j'suis parano, les refoulés m'acclament J'ai plein d'choses à dire mais les mots ne veulent pas séchapper Y'a qu'face à moi-même que j'verse des larmes et je les sèche après J'suis un mec à l'ancienne, j'écoute des vinyles fossilisés Si t'es pas prêt faut s'initier, j'reste pas mais faut s'immiscer Pas s'y glisser, demande à Nekfeu, j'suis trop déterminé J'ai vu des frères ruinés, en une seconde tout était terminé Le peu-Ra, c'est toute ma vie, gros, j'ai ça dans l'ADN J'dois rester l'un des meilleurs même si j'sais pas où l'indé' mène J'aurai jamais d'beaux tarifs mais l'heure des comptes arrive Faut que j'me sorte de mon train de vie car cette pute me contrarie Ça dit que j'vais pas percer, moi, j'guette les sales gars parler Mon talent c'est toute ma vie et ça veut s'l'accaparer On reconnait bien la galère mais beaucoup moins la providence On s'en fout c'est l'omerta mais tire pas là où la police danse 'Tain, j'ai trop peur d'échouer, t'façon, y'aura pas d'coïncidences J'ai fait l'école d'un silence, face à moi, y'a trop d'insistance T'as les oreilles qui sanguinolent, mon son, c'est comme une injection Vas-y, remballe ton show, guignol, tu niques les oreilles de l'ingé-son Ma vie, c'est prendre des coups, les cons XXX, moi, je ne rêve que dans des coupes J'ai su rapper sans prendre des cours, moi, j'fais partie d'ceux qu'on découvre Ne t'étonne pas que l'on te dépouille, pour bien vivre faut qu'on s'débrouille Cherche l'argent par tous les moyens en attendant qu'mon ons' déboule 2-zer ! Toi-même tu sais comment ça aif' mon pote ! Fais ner-tour, fais ner-tour, fais ner-tour ! Tu connais, tu connais, tu connais ! OK, toi-même tu sais comment ça aif' mon pote !</t>
         </is>
       </c>
     </row>
@@ -1665,12 +1665,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>20 mesures</t>
+          <t>2zer - John Doe ∅ 19</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>J'suis pas Escobar, j'aborde Paname pour refourguer ma came J'me sens rejeté, j'suis parano, les refoulés m'acclament J'ai plein d'choses à dire mais les mots ne veulent pas séchapper Y'a qu'face à moi-même que j'verse des larmes et je les sèche après J'suis un mec à l'ancienne, j'écoute des vinyles fossilisés Si t'es pas prêt faut s'initier, j'reste pas mais faut s'immiscer Pas s'y glisser, demande à Nekfeu, j'suis trop déterminé J'ai vu des frères ruinés, en une seconde tout était terminé Le peu-Ra, c'est toute ma vie, gros, j'ai ça dans l'ADN J'dois rester l'un des meilleurs même si j'sais pas où l'indé' mène J'aurai jamais d'beaux tarifs mais l'heure des comptes arrive Faut que j'me sorte de mon train de vie car cette pute me contrarie Ça dit que j'vais pas percer, moi, j'guette les sales gars parler Mon talent c'est toute ma vie et ça veut s'l'accaparer On reconnait bien la galère mais beaucoup moins la providence On s'en fout c'est l'omerta mais tire pas là où la police danse 'Tain, j'ai trop peur d'échouer, t'façon, y'aura pas d'coïncidences J'ai fait l'école d'un silence, face à moi, y'a trop d'insistance T'as les oreilles qui sanguinolent, mon son, c'est comme une injection Vas-y, remballe ton show, guignol, tu niques les oreilles de l'ingé-son Ma vie, c'est prendre des coups, les cons XXX, moi, je ne rêve que dans des coupes J'ai su rapper sans prendre des cours, moi, j'fais partie d'ceux qu'on découvre Ne t'étonne pas que l'on te dépouille, pour bien vivre faut qu'on s'débrouille Cherche l'argent par tous les moyens en attendant qu'mon ons' déboule 2-zer ! Toi-même tu sais comment ça aif' mon pote ! Fais ner-tour, fais ner-tour, fais ner-tour ! Tu connais, tu connais, tu connais ! OK, toi-même tu sais comment ça aif' mon pote !</t>
+          <t>Tu connais t'façon John Doe J'pense un peu comme un raciste, on m'a trop discriminé Depuis mon enfance on me disait que c'est le vice qui m'irait Je pense que ma face les dégoûte comme si je sortais des canalisations Devant ça j'ai rien à dire, comme un sourd qui analyse un son On change pas de position même si ce qu'on pense a des nuances J'sens un vide quand je compense de circonstances atténuantes Mon flow est lourd, à chaque mot je compresse tes omoplates Non je suis pas homo, t'aurais pu croire vu que je baise des hommes au rap Si le rap ça paye, on te fait qué-cro demande à Doums Coulibaly Range tes plans pourris l'ami, on veut pas tous courir à vie Je m'en fou de tes propositions, tu n'es pas le pro du son Vise la pôle position, on est accro de production Pour percer, il n'y a pas trop de solution Tu dégoûtes comme un père qui s'accroche au dos de son fiston On est jamais inactif Pendant que t'écoutes ce morceau t'inquiètes y' d'autre son qui s'font Breeeeeeeh</t>
         </is>
       </c>
     </row>
@@ -1682,12 +1682,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2zer - John Doe ∅ 19</t>
+          <t>Anonymous</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Tu connais t'façon John Doe J'pense un peu comme un raciste, on m'a trop discriminé Depuis mon enfance on me disait que c'est le vice qui m'irait Je pense que ma face les dégoûte comme si je sortais des canalisations Devant ça j'ai rien à dire, comme un sourd qui analyse un son On change pas de position même si ce qu'on pense a des nuances J'sens un vide quand je compense de circonstances atténuantes Mon flow est lourd, à chaque mot je compresse tes omoplates Non je suis pas homo, t'aurais pu croire vu que je baise des hommes au rap Si le rap ça paye, on te fait qué-cro demande à Doums Coulibaly Range tes plans pourris l'ami, on veut pas tous courir à vie Je m'en fou de tes propositions, tu n'es pas le pro du son Vise la pôle position, on est accro de production Pour percer, il n'y a pas trop de solution Tu dégoûtes comme un père qui s'accroche au dos de son fiston On est jamais inactif Pendant que t'écoutes ce morceau t'inquiètes y' d'autre son qui s'font Breeeeeeeh</t>
+          <t>Georgio, Abou, 2-Zer C'est L'Entourage, S-Crew, boy Tu connais t'façon 75ème Session, girl Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Toutes les pétasses opèrent avec la même technique d'approche OK, j'suis le Roi des cons mais t'es la reine des p'tites salopes Ici, c'est Paris, la ville des soi-disant gangsters Qui manigancent pour te voir moisir en enfer C'est 2-Zer Washington et Georgio Armani Y'a d'la be-her, d'la picole et puis des morceaux d'cannabis Nos propos paralysent et font l'effet du tabagisme On t'attire comme une actrice porno amatrice Dans l'excellence, j'suis une référence textuelle Tes déchainements gestuels prouvent tes préférences sexuelles Errer dans des ruelles, nan, c'est pas l'paradis On fait qu'se plaindre car la vie est méchante et cruelle On fait pas d'Rap mais de la littérature moderne C'est ça l'dicton, pas d'addiction mais la rime et la rue m'obsèdent C'est pour Paris Nord mais c'couplet j'l'ai gratté dans l'15 Big up à mon S-Crew et ceux qui vont graffer dans l'train Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Assis dans l'métro, j'remercie Rosa Parks mais je serais heureux Quand on n'osera pas me dire non aux soirées hypes et grands apparts J'entends tellement de merdes, de faux Nekfeu J'ai peur qu'les gens vomissent, pas d'feat Je mélange pas mon champagne avec du Champomy Très loin des cours de catéchisme mes amis sombres, entre shit et garettes-ci J'ai quitté la maison, c'est la merde à vrai dire Quelques métaphores dans mes textes, on m'a dit Mets en d'autres En attendant on s'baise la tête, une chambre de bonne devenue maison close L'impression qu'tout le wagon m'fixe d'être à part Malgré qu'j'sois dans les normes avec mon pantalon-baskets-sweat bien sympa J'pense aux embrouilles d'hier, j'avais la tête vide à la base Et ma mère, j'comprends plus rien à c'qu'elle m'dit, v'la l'blabla Le monde s'achète, mets ton nom sous packaging, c'est tout pour la monnaie Alors qu'y'a qu'dans ces yeux qu'j'trouve un coin de paradis L'été, Paris sous les toits a des airs de Jamaïque J'ai fini d'rêver, j'aurais plus d'espoir si j'étais pas naïf x2 Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Oh qu'est-ce que tu fous, là !? Ça va pas ou quoi !? Quoi, j'fais rien d'mal ? J'veux juste réveiller le quartier ! Regarde, ouvre tes yeux, il est mort c'putain d'quartier !</t>
         </is>
       </c>
     </row>
@@ -1699,12 +1699,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Anonymous</t>
+          <t>Balle perdue #1 - Intestable</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Georgio, Abou, 2-Zer C'est L'Entourage, S-Crew, boy Tu connais t'façon 75ème Session, girl Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Toutes les pétasses opèrent avec la même technique d'approche OK, j'suis le Roi des cons mais t'es la reine des p'tites salopes Ici, c'est Paris, la ville des soi-disant gangsters Qui manigancent pour te voir moisir en enfer C'est 2-Zer Washington et Georgio Armani Y'a d'la be-her, d'la picole et puis des morceaux d'cannabis Nos propos paralysent et font l'effet du tabagisme On t'attire comme une actrice porno amatrice Dans l'excellence, j'suis une référence textuelle Tes déchainements gestuels prouvent tes préférences sexuelles Errer dans des ruelles, nan, c'est pas l'paradis On fait qu'se plaindre car la vie est méchante et cruelle On fait pas d'Rap mais de la littérature moderne C'est ça l'dicton, pas d'addiction mais la rime et la rue m'obsèdent C'est pour Paris Nord mais c'couplet j'l'ai gratté dans l'15 Big up à mon S-Crew et ceux qui vont graffer dans l'train Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Assis dans l'métro, j'remercie Rosa Parks mais je serais heureux Quand on n'osera pas me dire non aux soirées hypes et grands apparts J'entends tellement de merdes, de faux Nekfeu J'ai peur qu'les gens vomissent, pas d'feat Je mélange pas mon champagne avec du Champomy Très loin des cours de catéchisme mes amis sombres, entre shit et garettes-ci J'ai quitté la maison, c'est la merde à vrai dire Quelques métaphores dans mes textes, on m'a dit Mets en d'autres En attendant on s'baise la tête, une chambre de bonne devenue maison close L'impression qu'tout le wagon m'fixe d'être à part Malgré qu'j'sois dans les normes avec mon pantalon-baskets-sweat bien sympa J'pense aux embrouilles d'hier, j'avais la tête vide à la base Et ma mère, j'comprends plus rien à c'qu'elle m'dit, v'la l'blabla Le monde s'achète, mets ton nom sous packaging, c'est tout pour la monnaie Alors qu'y'a qu'dans ces yeux qu'j'trouve un coin de paradis L'été, Paris sous les toits a des airs de Jamaïque J'ai fini d'rêver, j'aurais plus d'espoir si j'étais pas naïf x2 Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Dans l'Rap, j'suis Anonymous pas un virus informatique Jyeah ! Tous mes textes se ressemblent, ma vie d'rue, ma force, ma tise Jyeah ! Alors on s'active dans les apparts de Paris Nord Milieu du Rap ça parait grand, mais ici c'est pas énorme Oh qu'est-ce que tu fous, là !? Ça va pas ou quoi !? Quoi, j'fais rien d'mal ? J'veux juste réveiller le quartier ! Regarde, ouvre tes yeux, il est mort c'putain d'quartier !</t>
+          <t>Intesté ne veut pas dire intestable, j'ai vu mes proches partir, j'ai la muerte en FaceTime Je traverse la Terre, poursuivi par le jet lag, j'ai vu des gens payés des kilos avec PayPal C'est ce putain d'ennui qui m'donne envie de bédave mais la vie ne récompense que celui qui se démarque J'ai rêvé que mon cur suivait le rythme des vagues, avec le temps, le paqu'bot est devenu une épave Nan, ne te prends surtout pas pour ce que tu n'es pas, tu sais que c'est l'instinct de survie qui guide mes pas Mon meilleur pote est mort, putain je m'en remets pas, le seul qui m'acceptait quand je n'étais qu'un renégat Et la haine se répand comme se répand le choléra, weed alcool et rap, faites attention aux dégâts L'élève dépasse le maître et il dit qu'il ne connait pas, souvent les gens se taisent et souvent la monnaie parle Je dois la vie à mes associés, ainsi va la vie, on a réussi à s'imposer Je dois la vie à mes associés, ainsi va la vie, on a réussi à s'imposer, ouais Car on vit nos vies à fond, rythmé par nos palpitations, je ne veux plus d'obligation eh, ouais Dans la vie y a pas d'à peu près, l'humanité est morte donc j'ai toute la Terre a peuplé Les crimes sont restés impunis, normal qu'on pète un fusible yeah Et leur conquête infinie commence par des lois intrusives On ne peut pas bosser ensemble, si ya aucun feeling Mais Paris et moi, c'est comme Iverson et Philly yeah J'ai la bague au doigt, c'est évident mademoiselle, tu t'intéresses à mon gent-ar mais cest kiffant, jdois ladmettre Plus de maille sur le compte courant mais vivement que j'vois la mer yeah J'ai pas de patron, j'me fais des virements à moi-même yeah Unité, s'il-te-plaît ne t'en vas pas, si y avait pas ma bande, moi je ferais bande à part J'représente les rejetés, tout ceux qui vivent de mandat cash yeah Pas ceux qui parlent dans ton dos sourient devant ta face, ouais Je dois la vie à mes associés, ainsi va la vie, on a réussi à s'imposer Je dois la vie à mes associés, ainsi va la vie, on a réussi à s'imposer, ouais Car on vit nos vies à fond, rythmé par nos palpitations, je ne veux plus d'obligation eh, ouais Dans la vie y a pas d'à peu près, l'humanité est morte donc j'ai toute la Terre a peuplé Intesté ne veut pas dire intestable, j'ai vu mes proches partir, j'ai la muerte en FaceTime</t>
         </is>
       </c>
     </row>
@@ -1716,12 +1716,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Balle perdue #1 - Intestable</t>
+          <t>Balle perdue #2</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Intesté ne veut pas dire intestable, j'ai vu mes proches partir, j'ai la muerte en FaceTime Je traverse la Terre, poursuivi par le jet lag, j'ai vu des gens payés des kilos avec PayPal C'est ce putain d'ennui qui m'donne envie de bédave mais la vie ne récompense que celui qui se démarque J'ai rêvé que mon cur suivait le rythme des vagues, avec le temps, le paqu'bot est devenu une épave Nan, ne te prends surtout pas pour ce que tu n'es pas, tu sais que c'est l'instinct de survie qui guide mes pas Mon meilleur pote est mort, putain je m'en remets pas, le seul qui m'acceptait quand je n'étais qu'un renégat Et la haine se répand comme se répand le choléra, weed alcool et rap, faites attention aux dégâts L'élève dépasse le maître et il dit qu'il ne connait pas, souvent les gens se taisent et souvent la monnaie parle Je dois la vie à mes associés, ainsi va la vie, on a réussi à s'imposer Je dois la vie à mes associés, ainsi va la vie, on a réussi à s'imposer, ouais Car on vit nos vies à fond, rythmé par nos palpitations, je ne veux plus d'obligation eh, ouais Dans la vie y a pas d'à peu près, l'humanité est morte donc j'ai toute la Terre a peuplé Les crimes sont restés impunis, normal qu'on pète un fusible yeah Et leur conquête infinie commence par des lois intrusives On ne peut pas bosser ensemble, si ya aucun feeling Mais Paris et moi, c'est comme Iverson et Philly yeah J'ai la bague au doigt, c'est évident mademoiselle, tu t'intéresses à mon gent-ar mais cest kiffant, jdois ladmettre Plus de maille sur le compte courant mais vivement que j'vois la mer yeah J'ai pas de patron, j'me fais des virements à moi-même yeah Unité, s'il-te-plaît ne t'en vas pas, si y avait pas ma bande, moi je ferais bande à part J'représente les rejetés, tout ceux qui vivent de mandat cash yeah Pas ceux qui parlent dans ton dos sourient devant ta face, ouais Je dois la vie à mes associés, ainsi va la vie, on a réussi à s'imposer Je dois la vie à mes associés, ainsi va la vie, on a réussi à s'imposer, ouais Car on vit nos vies à fond, rythmé par nos palpitations, je ne veux plus d'obligation eh, ouais Dans la vie y a pas d'à peu près, l'humanité est morte donc j'ai toute la Terre a peuplé Intesté ne veut pas dire intestable, j'ai vu mes proches partir, j'ai la muerte en FaceTime</t>
+          <t>Hugz, t'es en feu sur celle-là Yolop bitchies poulop, j'me fous d'vos critiques youh j'roule un gros blunt couleur Dickies ha-ha-ha J'suis le killeur, Mary Jane c'est la victime yeah, à cause de sa couleur et d'son odeur addictive brah Ma face à la télé, ma voix dans les enceintes yeah, sapé en noir et blanc comme un ancien ouais Ta montre vaut le prix d'une Renaud 5, nan, ta montre vaut le prix d'un voyage en train ha-ha-ha L'ennemi me serre la main, sa femme me fait du pied, ouais avant j'étais du-per, maintenant j'vais pas m'laisser duper T'as pas écouté ta mère, ouais bah moi j'vais t'éduquer J'vais ramener qui-tu-sais, ouais ouais ce soir faut que tu saignes J'peux t'envoyer dormir comme si j'étais ton père J'me souviens plus de mes bagarres, j'me souviens plus de mes conquêtes De toute façon c'est la même, c'est qu'une histoire de corps à corps Et comme dirait Mekra Il faut assumer ton sexe Hein belek, ne te questionne pas sur ton intellect, t'enlèves ce joint d'tes lèvres et demande-toi pourquoi t'es loin d'tes rêves Loin d'tes rêves car l'État t'impose sa réalité, il te trouve des défauts dans ce qui peut être des qualités Hein belek, ne te questionne pas sur ton intellect, t'enlèves ce joint d'tes lèvres et demande-toi pourquoi t'es loin d'tes rêves Loin d'tes rêves car l'État t'impose sa réalité, il te trouve des défauts dans ce qui peut être des qualités Heureux de vivre, y s'peut que j'meurs demain, les balles perdues ne demandent pas leur chemin hein, hein Dans la vie, t'as faim quand tu pars de rien, les balles perdues ne demandent pas leur chemin hein, hein Heureux de vivre, y s'peut que j'meurs demain yeah, les balles perdues ne demandent pas leur chemin ouais Dans la vie, t'as faim quand tu pars de rien, les balles perdues ne demandent pas leur chemin brah, brah, brah La vie c'est une pute, t'es bête, tu crois qu'elle t'aime, après t'avoir tirer dans les jambes, elle tire en pleine tête Y a des coupables qui s'baladent sur la Terre-Mère oui, y a des innocents qui prennent perpète Rien ne tire debout à part mes vertèbres, tu peux caner le jour de ton anniversaire brah Et même si t'as les poches remplis d'espèce, la solitude entraîne une mort quasi-certaine bête On chie du caviar, on pisse du Moët, on porte nos cojones dans des brouettes ha-ha-ha Jamais tu n'atteindras le crew-S lève la main, on fait la sieste sur le Piton de la Fournaise Hein belek, ne te questionne pas sur ton intellect, t'enlèves ce joint d'tes lèvres et demande-toi pourquoi t'es loin d'tes rêves Loin d'tes rêves car l'État t'impose sa réalité, il te trouve des défauts dans ce qui peut être des qualités Hein belek, ne te questionne pas sur ton intellect, t'enlèves ce joint d'tes lèvres et demande-toi pourquoi t'es loin d'tes rêves Loin d'tes rêves car l'État t'impose sa réalité, il te trouve des défauts dans ce qui peut être des qualités Heureux de vivre, y s'peut que j'meurs demain, les balles perdues ne demandent pas leur chemin hein, hein Dans la vie, t'as faim quand tu pars de rien, les balles perdues ne demandent pas leur chemin hein, hein Heureux de vivre, y s'peut que j'meurs demain yeah, les balles perdues ne demandent pas leur chemin ouais Dans la vie, t'as faim quand tu pars de rien, les balles perdues ne demandent pas leur chemin brah, brah, brah</t>
         </is>
       </c>
     </row>
@@ -1733,12 +1733,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Balle perdue #2</t>
+          <t>Balle perdue #3 - Mustang</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Hugz, t'es en feu sur celle-là Yolop bitchies poulop, j'me fous d'vos critiques youh j'roule un gros blunt couleur Dickies ha-ha-ha J'suis le killeur, Mary Jane c'est la victime yeah, à cause de sa couleur et d'son odeur addictive brah Ma face à la télé, ma voix dans les enceintes yeah, sapé en noir et blanc comme un ancien ouais Ta montre vaut le prix d'une Renaud 5, nan, ta montre vaut le prix d'un voyage en train ha-ha-ha L'ennemi me serre la main, sa femme me fait du pied, ouais avant j'étais du-per, maintenant j'vais pas m'laisser duper T'as pas écouté ta mère, ouais bah moi j'vais t'éduquer J'vais ramener qui-tu-sais, ouais ouais ce soir faut que tu saignes J'peux t'envoyer dormir comme si j'étais ton père J'me souviens plus de mes bagarres, j'me souviens plus de mes conquêtes De toute façon c'est la même, c'est qu'une histoire de corps à corps Et comme dirait Mekra Il faut assumer ton sexe Hein belek, ne te questionne pas sur ton intellect, t'enlèves ce joint d'tes lèvres et demande-toi pourquoi t'es loin d'tes rêves Loin d'tes rêves car l'État t'impose sa réalité, il te trouve des défauts dans ce qui peut être des qualités Hein belek, ne te questionne pas sur ton intellect, t'enlèves ce joint d'tes lèvres et demande-toi pourquoi t'es loin d'tes rêves Loin d'tes rêves car l'État t'impose sa réalité, il te trouve des défauts dans ce qui peut être des qualités Heureux de vivre, y s'peut que j'meurs demain, les balles perdues ne demandent pas leur chemin hein, hein Dans la vie, t'as faim quand tu pars de rien, les balles perdues ne demandent pas leur chemin hein, hein Heureux de vivre, y s'peut que j'meurs demain yeah, les balles perdues ne demandent pas leur chemin ouais Dans la vie, t'as faim quand tu pars de rien, les balles perdues ne demandent pas leur chemin brah, brah, brah La vie c'est une pute, t'es bête, tu crois qu'elle t'aime, après t'avoir tirer dans les jambes, elle tire en pleine tête Y a des coupables qui s'baladent sur la Terre-Mère oui, y a des innocents qui prennent perpète Rien ne tire debout à part mes vertèbres, tu peux caner le jour de ton anniversaire brah Et même si t'as les poches remplis d'espèce, la solitude entraîne une mort quasi-certaine bête On chie du caviar, on pisse du Moët, on porte nos cojones dans des brouettes ha-ha-ha Jamais tu n'atteindras le crew-S lève la main, on fait la sieste sur le Piton de la Fournaise Hein belek, ne te questionne pas sur ton intellect, t'enlèves ce joint d'tes lèvres et demande-toi pourquoi t'es loin d'tes rêves Loin d'tes rêves car l'État t'impose sa réalité, il te trouve des défauts dans ce qui peut être des qualités Hein belek, ne te questionne pas sur ton intellect, t'enlèves ce joint d'tes lèvres et demande-toi pourquoi t'es loin d'tes rêves Loin d'tes rêves car l'État t'impose sa réalité, il te trouve des défauts dans ce qui peut être des qualités Heureux de vivre, y s'peut que j'meurs demain, les balles perdues ne demandent pas leur chemin hein, hein Dans la vie, t'as faim quand tu pars de rien, les balles perdues ne demandent pas leur chemin hein, hein Heureux de vivre, y s'peut que j'meurs demain yeah, les balles perdues ne demandent pas leur chemin ouais Dans la vie, t'as faim quand tu pars de rien, les balles perdues ne demandent pas leur chemin brah, brah, brah</t>
+          <t>S-Crew L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine Je peux t'assurer que si t'es sous le ciel azuré, tu pourrais te mettre à sceller, l'essentiel c'est d'assumer On est pas des fortunés, infortunément, là pour pleurer même si on importune les gens On pète les plafonds malgré le refus des banques, toujours au bord du précipice pour ça qu'j'ai plus d'élan On est de ceux qui dérangent, à cause de nos différences, tu te grattes la tête, j'ai la gâchette qui démange J'prends de l'élan puis je m'élance au dessus de vos espérances, je m'inspire et je mélange On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître, j'peux pas dire qu'l'humanité n'est pas cruel Tu connais mon salaire annuel, j'peux flamber mais je me casse comme une allumette, ouais</t>
         </is>
       </c>
     </row>
@@ -1750,12 +1750,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Balle perdue #3 - Mustang</t>
+          <t>Balle perdue #4 - Excès</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>S-Crew L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine Je peux t'assurer que si t'es sous le ciel azuré, tu pourrais te mettre à sceller, l'essentiel c'est d'assumer On est pas des fortunés, infortunément, là pour pleurer même si on importune les gens On pète les plafonds malgré le refus des banques, toujours au bord du précipice pour ça qu'j'ai plus d'élan On est de ceux qui dérangent, à cause de nos différences, tu te grattes la tête, j'ai la gâchette qui démange J'prends de l'élan puis je m'élance au dessus de vos espérances, je m'inspire et je mélange On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître, j'peux pas dire qu'l'humanité n'est pas cruel Tu connais mon salaire annuel, j'peux flamber mais je me casse comme une allumette, ouais</t>
+          <t>Ah ah, c'est Zer-2 Balle perdue, Hugz t'es en feu sur celle-là ? Yeah Aura-t-on le droit à une deuxième chance si la vie n'est qu'un essai ? yah Excès de franchise, pas de filtre sur ma voix, non j'ai pas peur de vexer nop, nop J'continuerais de célébrer ma vie jusqu'au jour de mon décès ouais Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh J'continuerais de célébrer ma vie jusqu'au jour de mon décès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais J'fume la zèb, c'est fini le shit, c'est fini la 'sère, c'est fini le SMIC Certains se connaissent depuis 1998, y'a que sur notre label qu'on a signé de suite J'fume la zèb, c'est fini le shit, c'est fini la 'sère, c'est fini le SMIC Certains se connaissent depuis 1998, y'a que sur notre label qu'on a signé de suite Montagne de pasta, faut pas qu'j'tombe à plat, direction Meuda si l'pochton n'est pas plein Mon égo me dit que tu n'es qu'une tapin, faut d'jeter des fleurs pour qu'tu mettes au parfum Pet, pet, pet, je les roule un par un, Super Silver Haze Block fait l'effet d'un parpaing wouh, wouh Mon destin m'appartient, j'ai atteint mon but, maintenant j'ai besoin d'un gardien Aura-t-on le droit à une deuxième chance si la vie n'est qu'un essai ? j'sais as-p Excès de franchise, pas de filtre sur ma voix, non j'ai pas peur de vexer hell no J'continuerais de célébrer ma vie jusqu'au jour de mon décès wouh Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh J'continuerais de célébrer ma vie jusqu'au jour de mon décès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais Tu m'en crois pas capable, j'le fais devant toi, j'deviens le boss si j'ai pas la gueule de l'emploi Et quand j'ai la dalle, je me sers, j'demande pas, on m'a dit Zer-2, ça me choque venant d'toi Besoin de bédave pour réguler mes émotions, pour certains c'est le venin, pour certains c'est la potion Si t'es pas intéressant, tu perds mon attention, j'te dis que j'ai pas le temps quand je perds la notion Si t'es ma go, j'connais ton anatomie, t'es contente de me voir, fais pas la tho-my T'as mis de la crème, tu t'es fait belle cousine, y a que sur les meufs que j'aime la peau lisse On est impoli de Paname à Napoli, flow du futur, ouais j'suis anachronique Fume pas la chronique, plutôt la cookie, j'ai besoin de rédemption à la Tookie Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh J'continuerais de célébrer ma vie jusqu'au jour de mon décès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais J'fume la zèb, c'est fini le shit, c'est fini la 'sère, c'est fini le SMIC Certains se connaissent depuis 1998, y'a que sur notre label qu'on a signé de suite J'fume la zèb, c'est fini le shit, c'est fini la 'sère, c'est fini le SMIC Certains se connaissent depuis 1998, y'a que sur notre label qu'on a signé de suite Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Hugz est toujours dans l'excès, eh Zer-2 toujours dans l'excès, eh S-Crew toujours dans l'excès, ouais</t>
         </is>
       </c>
     </row>
@@ -1767,12 +1767,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Balle perdue #4 - Excès</t>
+          <t>Balle perdue #5 - Blood Diamonds</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Ah ah, c'est Zer-2 Balle perdue, Hugz t'es en feu sur celle-là ? Yeah Aura-t-on le droit à une deuxième chance si la vie n'est qu'un essai ? yah Excès de franchise, pas de filtre sur ma voix, non j'ai pas peur de vexer nop, nop J'continuerais de célébrer ma vie jusqu'au jour de mon décès ouais Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh J'continuerais de célébrer ma vie jusqu'au jour de mon décès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais J'fume la zèb, c'est fini le shit, c'est fini la 'sère, c'est fini le SMIC Certains se connaissent depuis 1998, y'a que sur notre label qu'on a signé de suite J'fume la zèb, c'est fini le shit, c'est fini la 'sère, c'est fini le SMIC Certains se connaissent depuis 1998, y'a que sur notre label qu'on a signé de suite Montagne de pasta, faut pas qu'j'tombe à plat, direction Meuda si l'pochton n'est pas plein Mon égo me dit que tu n'es qu'une tapin, faut d'jeter des fleurs pour qu'tu mettes au parfum Pet, pet, pet, je les roule un par un, Super Silver Haze Block fait l'effet d'un parpaing wouh, wouh Mon destin m'appartient, j'ai atteint mon but, maintenant j'ai besoin d'un gardien Aura-t-on le droit à une deuxième chance si la vie n'est qu'un essai ? j'sais as-p Excès de franchise, pas de filtre sur ma voix, non j'ai pas peur de vexer hell no J'continuerais de célébrer ma vie jusqu'au jour de mon décès wouh Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh J'continuerais de célébrer ma vie jusqu'au jour de mon décès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais Tu m'en crois pas capable, j'le fais devant toi, j'deviens le boss si j'ai pas la gueule de l'emploi Et quand j'ai la dalle, je me sers, j'demande pas, on m'a dit Zer-2, ça me choque venant d'toi Besoin de bédave pour réguler mes émotions, pour certains c'est le venin, pour certains c'est la potion Si t'es pas intéressant, tu perds mon attention, j'te dis que j'ai pas le temps quand je perds la notion Si t'es ma go, j'connais ton anatomie, t'es contente de me voir, fais pas la tho-my T'as mis de la crème, tu t'es fait belle cousine, y a que sur les meufs que j'aime la peau lisse On est impoli de Paname à Napoli, flow du futur, ouais j'suis anachronique Fume pas la chronique, plutôt la cookie, j'ai besoin de rédemption à la Tookie Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh J'continuerais de célébrer ma vie jusqu'au jour de mon décès, ouais Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Excès de confiance, si on t'manque de respect, bah c'est qu'on l'a fait exprès, ouais J'fume la zèb, c'est fini le shit, c'est fini la 'sère, c'est fini le SMIC Certains se connaissent depuis 1998, y'a que sur notre label qu'on a signé de suite J'fume la zèb, c'est fini le shit, c'est fini la 'sère, c'est fini le SMIC Certains se connaissent depuis 1998, y'a que sur notre label qu'on a signé de suite Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Ouais j'suis toujours dans l'excès, eh Hugz est toujours dans l'excès, eh Zer-2 toujours dans l'excès, eh S-Crew toujours dans l'excès, ouais</t>
+          <t>Trop d'émotions mais des mots y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin, tout ira bien nan, nan, nan Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais brh, brh, brh, yeah Le temps fait que passer, j'ai pas de futur, il ne m'attend pas il ne m'attends pas C'est le même refrain, c'est les mêmes reufrés, c'est les mêmes en bas, ouais Tu l'sais, c'est à Paname que j'ai pris racine, j'ai les pieds sous terre j'ai les pieds sous terre C'est là qu'j'ai grandi, c'est là qu'j'ai gole-ri, c'est là qu'j'ai souffert Ils ont voulu voler nos parts, normal on évolue à part Ils ont bien vu qu'on venait d'autre part, ferme te gueule quand les frérots parlent Vrai, on s'connait depuis dix ans mais même avant, tu médisais Donc, jamais de mon vivant, ma haine pour toi sera maîtrisée, ouais Nos liaisons sont dangereuses, j'me barre de Paname quand je veux L'élimination, c'est la seule sortie si tu rentres dans le jeu Pour être généreux, faut le cur sportif, borderline, j'effleure leur piste Dieu merci, destin fortuit, pourtant j'en demandais peu Trop d'émotions mais des mots y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin tout ira bien très, très, très Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais brh, brh, brh, yeah Trop d'émotions mais d'emo y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin tout ira bien nan, nan, nan Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais Le temps fait que passer, on perd la rage, on s'assagit doucement La faim s'est estompée, Dieu merci, on se rassasie On s'est ressaisi comme des hustlers, faut nous le dire quand on s'lélé J'taffe les épaules, ils haussent les leurs, pourtant l'Gelato est dans l'OCB Bébé, bouge ton postérieur comme si t'avais pas d'rempart Entre toi et moi, y a pas d'rempart, t'arrives fraîche, tu repars bancale Fuck les tains-p et les tes-traî, on fait pas dans l'à-peu-près nan On débarque, chacun sa proie, ouais, les loups sont dans le pré ah, ah, ah Sans la mort, y a pas d'enjeu, tu joues mieux quand tu peux pas respawner Avant dans ma vie, tout était gris, si tout est écrit, viens pas spoiler Sans la mort, y a pas d'enjeu, tu joues mieux quand tu peux pas respawner Avant dans ma vie, tout était gris, si tout est écrit, viens pas spoiler Trop d'émotions mais des mots y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin tout ira bien très, très, très Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais brh, brh, brh, yeah Trop d'émotions mais d'emo y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin tout ira bien nan, nan, nan Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais Hugz, t'es en feu sur celle-là</t>
         </is>
       </c>
     </row>
@@ -1784,12 +1784,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Balle perdue #5 - Blood Diamonds</t>
+          <t>Balle perdue #6 - NMI</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Trop d'émotions mais des mots y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin, tout ira bien nan, nan, nan Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais brh, brh, brh, yeah Le temps fait que passer, j'ai pas de futur, il ne m'attend pas il ne m'attends pas C'est le même refrain, c'est les mêmes reufrés, c'est les mêmes en bas, ouais Tu l'sais, c'est à Paname que j'ai pris racine, j'ai les pieds sous terre j'ai les pieds sous terre C'est là qu'j'ai grandi, c'est là qu'j'ai gole-ri, c'est là qu'j'ai souffert Ils ont voulu voler nos parts, normal on évolue à part Ils ont bien vu qu'on venait d'autre part, ferme te gueule quand les frérots parlent Vrai, on s'connait depuis dix ans mais même avant, tu médisais Donc, jamais de mon vivant, ma haine pour toi sera maîtrisée, ouais Nos liaisons sont dangereuses, j'me barre de Paname quand je veux L'élimination, c'est la seule sortie si tu rentres dans le jeu Pour être généreux, faut le cur sportif, borderline, j'effleure leur piste Dieu merci, destin fortuit, pourtant j'en demandais peu Trop d'émotions mais des mots y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin tout ira bien très, très, très Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais brh, brh, brh, yeah Trop d'émotions mais d'emo y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin tout ira bien nan, nan, nan Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais Le temps fait que passer, on perd la rage, on s'assagit doucement La faim s'est estompée, Dieu merci, on se rassasie On s'est ressaisi comme des hustlers, faut nous le dire quand on s'lélé J'taffe les épaules, ils haussent les leurs, pourtant l'Gelato est dans l'OCB Bébé, bouge ton postérieur comme si t'avais pas d'rempart Entre toi et moi, y a pas d'rempart, t'arrives fraîche, tu repars bancale Fuck les tains-p et les tes-traî, on fait pas dans l'à-peu-près nan On débarque, chacun sa proie, ouais, les loups sont dans le pré ah, ah, ah Sans la mort, y a pas d'enjeu, tu joues mieux quand tu peux pas respawner Avant dans ma vie, tout était gris, si tout est écrit, viens pas spoiler Sans la mort, y a pas d'enjeu, tu joues mieux quand tu peux pas respawner Avant dans ma vie, tout était gris, si tout est écrit, viens pas spoiler Trop d'émotions mais des mots y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin tout ira bien très, très, très Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais brh, brh, brh, yeah Trop d'émotions mais d'emo y en a pas suffisamment nan, nan, nan Je ferme les yeux et j'me dis qu'à la fin tout ira bien nan, nan, nan Du mal à ignorer tout c'qui s'passe mondialement nan, nan, nan T'as du sang sur les mains quand t'achètes un diamant, ouais Hugz, t'es en feu sur celle-là</t>
+          <t>Oh my god J'ai perdu la notion du temps du temps J'ai perdu la notion du temps yah, pas de soucis, nos destins sont liés quoi ? J'fais pas ça juste pour prendre un bon billet nan, rien à prouver, d'toute façon, ça s'entend nan Peu parfumé ,mon teh, je m'en perds, je me barre, nan, ils vont pas me traiter de la sorte yeah J't'ai vu sniffer ta merde dans les toilettes, t'ouvres ta bouche mais t'as pas fermé la porte Ouais, grumpy, sale humeur, c'est comme ça, pas d'rumeurs, soit tu vis, soit tu meurs yeah, yeah, yeah Yeah, c'est simple, efficace, cache ton vrai visage, le mensonge ou la pudeur Yeah, y a quoi que tu comprends pas ? Satisfait du vécu, tu sais qu'on s'rend pas jamais Hey, j'suis pas dans vos bails de jouer en douceur, je vise et je fonce dans l'tas On s'connait pas, t'as dû t'tromper, j'suis pas d'ici, t'es mal tombé Me sers pas la main, on part pas du bon pied, j'assume mes problèmes, j'ai pas d'plan B Braquer la banque, brûler la caisse, vendre l'afghan, buter la hess Ces tentations sont dans ma tête, j'sais pas c'que j'ferai sans la verte Ouais, mon gava, tu sais quoi gava, tu sais quoi ? ? T'as qu'un ennemi, c'est toi l'ennemi, c'est toi Plus tu prends du recul sur toi-même du recul sur toi-même, plus les ennuis s'éloignent les ennuis s'éloignent, eh Ouais, mon gava, tu sais quoi gava, tu sais quoi ? ? T'as qu'un ennemi, c'est toi l'ennemi, c'est toi T'as du plomb dans la cabeza dans la cabeza, y a du sang sur la camiseta sur la camiseta J'ai pas répondu, j'ai dû m'assoupir eh, sur mon téléphone, j'ai mis la sourdine eh J'suis pas sorti, j'ai dû m'assombrir eh, le bonheur, je le reçois sous vide, ouais bleh À la base, j'ai fait tout ça pour les rendre fiers quoi ?, les chicos acérés comme des mange-pierres ouais Physiquement, on est bien mais nos âmes saignent yeah, pour désinfecter, on boit le rhum pêche Rien d'étonnant, tout est banal ouais, c'est excellent, on dit pas mal ouais Si j't'aime pas, j'te le dis frontal wouh avec l'insolence de Framal bleh, bleh Les jetons sont misés, j'emporte la mise et les curs sont brisés ouais Ouais, l'erreur est humaine, ton esprit un bolide mais ta peur conduisait haha On s'connait pas, t'as dû t'tromper, j'suis pas d'ici, t'es mal tombé Me sers pas la main, on part pas du bon pied, j'assume mes problèmes, j'ai pas d'plan B Braquer la banque, brûler la caisse, vendre l'afghan, buter la hess Ces tentations sont dans ma tête, j'sais pas c'que j'ferai sans la verte Ouais, mon gava, tu sais quoi gava, tu sais quoi ? ? T'as qu'un ennemi, c'est toi l'ennemi, c'est toi Plus tu prends du recul sur toi-même du recul sur toi-même, plus les ennuis s'éloignent les ennuis s'éloignent, eh Ouais, mon gava, tu sais quoi gava, tu sais quoi ? ? T'as qu'un ennemi, c'est toi l'ennemi, c'est toi T'as du plomb dans la cabeza dans la cabeza, y a du sang sur la camiseta sur la camiseta</t>
         </is>
       </c>
     </row>
@@ -1801,12 +1801,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Balle perdue #6 - NMI</t>
+          <t>Big Emceeing Freestyle</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Oh my god J'ai perdu la notion du temps du temps J'ai perdu la notion du temps yah, pas de soucis, nos destins sont liés quoi ? J'fais pas ça juste pour prendre un bon billet nan, rien à prouver, d'toute façon, ça s'entend nan Peu parfumé ,mon teh, je m'en perds, je me barre, nan, ils vont pas me traiter de la sorte yeah J't'ai vu sniffer ta merde dans les toilettes, t'ouvres ta bouche mais t'as pas fermé la porte Ouais, grumpy, sale humeur, c'est comme ça, pas d'rumeurs, soit tu vis, soit tu meurs yeah, yeah, yeah Yeah, c'est simple, efficace, cache ton vrai visage, le mensonge ou la pudeur Yeah, y a quoi que tu comprends pas ? Satisfait du vécu, tu sais qu'on s'rend pas jamais Hey, j'suis pas dans vos bails de jouer en douceur, je vise et je fonce dans l'tas On s'connait pas, t'as dû t'tromper, j'suis pas d'ici, t'es mal tombé Me sers pas la main, on part pas du bon pied, j'assume mes problèmes, j'ai pas d'plan B Braquer la banque, brûler la caisse, vendre l'afghan, buter la hess Ces tentations sont dans ma tête, j'sais pas c'que j'ferai sans la verte Ouais, mon gava, tu sais quoi gava, tu sais quoi ? ? T'as qu'un ennemi, c'est toi l'ennemi, c'est toi Plus tu prends du recul sur toi-même du recul sur toi-même, plus les ennuis s'éloignent les ennuis s'éloignent, eh Ouais, mon gava, tu sais quoi gava, tu sais quoi ? ? T'as qu'un ennemi, c'est toi l'ennemi, c'est toi T'as du plomb dans la cabeza dans la cabeza, y a du sang sur la camiseta sur la camiseta J'ai pas répondu, j'ai dû m'assoupir eh, sur mon téléphone, j'ai mis la sourdine eh J'suis pas sorti, j'ai dû m'assombrir eh, le bonheur, je le reçois sous vide, ouais bleh À la base, j'ai fait tout ça pour les rendre fiers quoi ?, les chicos acérés comme des mange-pierres ouais Physiquement, on est bien mais nos âmes saignent yeah, pour désinfecter, on boit le rhum pêche Rien d'étonnant, tout est banal ouais, c'est excellent, on dit pas mal ouais Si j't'aime pas, j'te le dis frontal wouh avec l'insolence de Framal bleh, bleh Les jetons sont misés, j'emporte la mise et les curs sont brisés ouais Ouais, l'erreur est humaine, ton esprit un bolide mais ta peur conduisait haha On s'connait pas, t'as dû t'tromper, j'suis pas d'ici, t'es mal tombé Me sers pas la main, on part pas du bon pied, j'assume mes problèmes, j'ai pas d'plan B Braquer la banque, brûler la caisse, vendre l'afghan, buter la hess Ces tentations sont dans ma tête, j'sais pas c'que j'ferai sans la verte Ouais, mon gava, tu sais quoi gava, tu sais quoi ? ? T'as qu'un ennemi, c'est toi l'ennemi, c'est toi Plus tu prends du recul sur toi-même du recul sur toi-même, plus les ennuis s'éloignent les ennuis s'éloignent, eh Ouais, mon gava, tu sais quoi gava, tu sais quoi ? ? T'as qu'un ennemi, c'est toi l'ennemi, c'est toi T'as du plomb dans la cabeza dans la cabeza, y a du sang sur la camiseta sur la camiseta</t>
+          <t>Eff Gee, han ! Melo, han ! On ride Paris en trom', en caisse ou en vélo, han ! On t'fait beaucoup d'effet, sur c'disque y'a tous mes frères Au bout d'mes rêves, on serait sur scène du haut d'la Tour Eiffel Pas d'quartier, t'as cramé que j'apparais chaque année Pour t'apporter du son rare comme XXX J'réchauffe les thermomètres dans les curs glacés Un peu comme Père Noël, c'est ma face cachée La face cachée, Eff Gee et Melo Maintenant qu'on est là, tu veux plus dire que tu aimais l'autre Attention, c'est du lourd donc laisse pas ber-tom On ve-ri à pas de loups sur du putain d'béton Des rimes de velours, dures, pures, obscures Il faut que t'assures, si tu pues tu t'drogues, sûr Y'a pas de part de lâcheté, on est des félins tachetés Qui découpent ton son, on déboule, tu tombes Mon ectoplasme porte lestocade même si j'rétrograde Il t'estomaque, depuis le berceau j'rappe donc viens pas test au mic Rap jurassique, furie climatique avec les multisyllabiques Les puristes m'imaginent en Nubi B-Rabbit Flow trop fat, MC Cosmocat, mes propos t'cassent l'omoplate J'suis sociopathe, intouchable en Rap comme un hologramme Hip-hopeur assidu d'habitude d'attitude taciturne, gaffe À ton matricule, j'articule et tape les particules grave J'ai des mots plein la tête sur un XXX Big flow comme Ill-G, tu veux une démo, tiens la tape Des MC's qui squattent Paris, fou à lier pour allier Le swagg, la rime, ceux sur qui les squales parient Mon squad arrive profond comme la face cachée L'homme Jaz trace, fâché sur l'asphalte glacé Pour des tas d'phases lâchées donc avale cachets Cours, détale, va t'cacher, va t'cacher Wesh, tu connais l'origine certifiée par la clique Un Double Neuf Cinq, Eff Gee, Melo, un mic et les MC's s'agitent Lance un beat, j'envoie la démo beaucoup de débutants prennent la fuite Les freestylers montent au créneau, ma zik tu l'aimes ou tu la quittes Mes parents s'doutent de rien, pensent que la school me tient par les couilles Donc j'taffe la née-jour et le soir devient l'idole des foules Le sampleur chauffe alors pousse encore le volume Flav' Fonky, j'balance un 8, tu finis sous l'bitume J'fume un spliff de bon matin, j'kiffe 'vec acharnement J'astique mon armement, j'suis c'garnement qui gifle les bons gamins J'ai la rime fat, homie, les autres sont plutôt maigres Et je n'ai jamais vu un ovni ou une pute honnête J'horrifie les mecs soporifiques qui m'horripilent glorifie-moi C'est horrible fils, les jolies filles au lit dilatent leurs orifices J'ai plein de stories peace mais y'a trop d'XXX J'suis Captain America, t'as capté la me-ri gars ? Hé yo Eff Gee, Melo, quoi d'neuf la mif ? Non non pas d'bluff j'arrive et les rappeurs pâlissent Fuck leurs récits d'blaireaux, ils gâchent leur salive S'ils font du rap thug moi j'veux voir leur calibre J'entends leur merde malgré moi comme un fumeur passif Mes kho's aiguisent leur canines pire que des leaders d'manifs Si t'es une sister câline je deviens killer d'manix Allez dites leur que j'arrive, ils sont pris d'peur, panique Voilà le boss des boss, le chef des freestylers Le best des nique la peur, le mec qui piste ta sur Écrire des classiques est automatique Violer la 'zik, voilà ce que mes potos pratiquent J'rappe sur le fil du rasoir appelle-moi Wilkinson J'ai ken le mic et j'ai laissé des preuves comme Bill Clinton Bref ! C'est moi l'best, j'crois qu'j'ai raison J'suis le MC qui vient tagger ton pâté d'maisons Allez va dire aux mecs, que j'écris des styles aux maîtres Que dorénavant tu m'verras plus avec un spliff au bec Check ! Sango pyroman, j'aime tout ceux qui remettent La rime précédente qui donne le sourire aux lèvres Jusqu'aux Antilles même, demande même à Philomène J'décolle cent kilos d'herbe, merde j'suis un phénomène Horreur de c'que les autres aiment, pas pour autant schizophrène J'ken tout ceux qui me freinent, voilà c'que j'explique aux frères XXX on attend pas qu'un manager me tend la patte Me propose un contrat pour faire du rap qui met des baffes Sans arrêt je taffe, pour les week-ends pas de place 100 indé, intestable, j'n'ai toujours pas de fan XXX est mon tier-quar où les rookies me backent Hauts-de-Seine j'habite àl, tout près de la capitale Où ça vole à l'étalage, faire l'effet d'un Kalach J'voulais attendre pour me lancer, LAX m'a dit c'est bon t'as l'âge Ok bienvenue dans mon esprit si vous aimez les vents d'folie Qui dit mieux ? Personne fait seul, moi j'dois côtoyer la mélancolie D'office donc petit si tu m'cherches, suis l'orage et tu l'auras Quoi ? Toi, j'vois qu'tu voulais la guerre, tu l'auras Aah, j'finis par croire en peu de personnes sérieux, ai-je tort ? Celui qui m'escorte, m'escroque, sort et me laisse mort XXX ça, est-ce l'or qui divisera ? C'est les p'tits qui parlent de sexe, drogue, XXX J'fais acte de présence, les mecs trouvent ça affolant J'dégage tellement d'aisance, ça en devient insolent Mon hobby c'est la drogue, finis les autocollants J'suis haut toute la journée, je n'me déplace plus qu'en volant Ça plane... J'me sens privilégié J'arpente Paname les paupières lourdes et l'esprit léger Pourtant quand t'écoutes mon son, j'sens qu'ça t'éveille Mon savoir est une arme, j'te mets du plomb dans la cervelle J'suis l'ingé son mais j'n'ai pas oublié l'plaisir de rapper L'désir de backer, le 8 mesures, saisir et frapper, l'instrumentale Tu m'entends même sur off, je suis l'intrus mental Non tu mens, sache que je compte percer comme Rohff Et j'veux que les XXX m'empalent Les sceptiques à la fosse septique, on tire la chasse et basta V'nez pas casser la star, à c'stade on n'a plus l'âge des lascars Mais celui d'un homme adulte qui s'donne qu'à ceux qui assument Malgré un nombre d'cassures, j't'assure Chérie, j'reviendrai pour qu'ensemble ça dure Moi j'ai la dalle, je pense à graille, j'vais surement pas lâcher les steaks Et si le rap ne me nourrit pas, ben on ira lyncher ce traître Devant ma voix l'ingé stresse, impossible de la compresser XXX un déstress, ils disent tous qu'ils sont pressés La joie te chauffe mais se retire avant qu'elle te fasse cracher Finies les phases gâchées, on va pas se crasher, on nous sort la face cachée Ne t'attache pas trop, sache que même ce 8 est éphémère Au mic' c'est 2Zer qui pe-ra pour la tête des Femens XXX XXX J'éclate la track je n'vais pas m'tâter Ça va s'gâter, j'viens m'imposer, placer l'rap carré J'suis v'là l'taré avec des phases plus fortes qu'un shot de rhum J'agite mon lexique j't'explique, j'excite plus qu'une hot mom Je n'parle pas de pistolet ni de shotgun Juste d'la vie qu'j'connais pour l'instant je bosse j'me donne J'peux pas l'cacher j'viens m'installer fini l'bal masqué J'viens exceller, accélérer, révéler ma face cachée RETRANSCRIPTION EN COURS</t>
         </is>
       </c>
     </row>
@@ -1818,12 +1818,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Big Emceeing Freestyle</t>
+          <t>Bizi’N The Hood #2 - 4x4 Noir</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Eff Gee, han ! Melo, han ! On ride Paris en trom', en caisse ou en vélo, han ! On t'fait beaucoup d'effet, sur c'disque y'a tous mes frères Au bout d'mes rêves, on serait sur scène du haut d'la Tour Eiffel Pas d'quartier, t'as cramé que j'apparais chaque année Pour t'apporter du son rare comme XXX J'réchauffe les thermomètres dans les curs glacés Un peu comme Père Noël, c'est ma face cachée La face cachée, Eff Gee et Melo Maintenant qu'on est là, tu veux plus dire que tu aimais l'autre Attention, c'est du lourd donc laisse pas ber-tom On ve-ri à pas de loups sur du putain d'béton Des rimes de velours, dures, pures, obscures Il faut que t'assures, si tu pues tu t'drogues, sûr Y'a pas de part de lâcheté, on est des félins tachetés Qui découpent ton son, on déboule, tu tombes Mon ectoplasme porte lestocade même si j'rétrograde Il t'estomaque, depuis le berceau j'rappe donc viens pas test au mic Rap jurassique, furie climatique avec les multisyllabiques Les puristes m'imaginent en Nubi B-Rabbit Flow trop fat, MC Cosmocat, mes propos t'cassent l'omoplate J'suis sociopathe, intouchable en Rap comme un hologramme Hip-hopeur assidu d'habitude d'attitude taciturne, gaffe À ton matricule, j'articule et tape les particules grave J'ai des mots plein la tête sur un XXX Big flow comme Ill-G, tu veux une démo, tiens la tape Des MC's qui squattent Paris, fou à lier pour allier Le swagg, la rime, ceux sur qui les squales parient Mon squad arrive profond comme la face cachée L'homme Jaz trace, fâché sur l'asphalte glacé Pour des tas d'phases lâchées donc avale cachets Cours, détale, va t'cacher, va t'cacher Wesh, tu connais l'origine certifiée par la clique Un Double Neuf Cinq, Eff Gee, Melo, un mic et les MC's s'agitent Lance un beat, j'envoie la démo beaucoup de débutants prennent la fuite Les freestylers montent au créneau, ma zik tu l'aimes ou tu la quittes Mes parents s'doutent de rien, pensent que la school me tient par les couilles Donc j'taffe la née-jour et le soir devient l'idole des foules Le sampleur chauffe alors pousse encore le volume Flav' Fonky, j'balance un 8, tu finis sous l'bitume J'fume un spliff de bon matin, j'kiffe 'vec acharnement J'astique mon armement, j'suis c'garnement qui gifle les bons gamins J'ai la rime fat, homie, les autres sont plutôt maigres Et je n'ai jamais vu un ovni ou une pute honnête J'horrifie les mecs soporifiques qui m'horripilent glorifie-moi C'est horrible fils, les jolies filles au lit dilatent leurs orifices J'ai plein de stories peace mais y'a trop d'XXX J'suis Captain America, t'as capté la me-ri gars ? Hé yo Eff Gee, Melo, quoi d'neuf la mif ? Non non pas d'bluff j'arrive et les rappeurs pâlissent Fuck leurs récits d'blaireaux, ils gâchent leur salive S'ils font du rap thug moi j'veux voir leur calibre J'entends leur merde malgré moi comme un fumeur passif Mes kho's aiguisent leur canines pire que des leaders d'manifs Si t'es une sister câline je deviens killer d'manix Allez dites leur que j'arrive, ils sont pris d'peur, panique Voilà le boss des boss, le chef des freestylers Le best des nique la peur, le mec qui piste ta sur Écrire des classiques est automatique Violer la 'zik, voilà ce que mes potos pratiquent J'rappe sur le fil du rasoir appelle-moi Wilkinson J'ai ken le mic et j'ai laissé des preuves comme Bill Clinton Bref ! C'est moi l'best, j'crois qu'j'ai raison J'suis le MC qui vient tagger ton pâté d'maisons Allez va dire aux mecs, que j'écris des styles aux maîtres Que dorénavant tu m'verras plus avec un spliff au bec Check ! Sango pyroman, j'aime tout ceux qui remettent La rime précédente qui donne le sourire aux lèvres Jusqu'aux Antilles même, demande même à Philomène J'décolle cent kilos d'herbe, merde j'suis un phénomène Horreur de c'que les autres aiment, pas pour autant schizophrène J'ken tout ceux qui me freinent, voilà c'que j'explique aux frères XXX on attend pas qu'un manager me tend la patte Me propose un contrat pour faire du rap qui met des baffes Sans arrêt je taffe, pour les week-ends pas de place 100 indé, intestable, j'n'ai toujours pas de fan XXX est mon tier-quar où les rookies me backent Hauts-de-Seine j'habite àl, tout près de la capitale Où ça vole à l'étalage, faire l'effet d'un Kalach J'voulais attendre pour me lancer, LAX m'a dit c'est bon t'as l'âge Ok bienvenue dans mon esprit si vous aimez les vents d'folie Qui dit mieux ? Personne fait seul, moi j'dois côtoyer la mélancolie D'office donc petit si tu m'cherches, suis l'orage et tu l'auras Quoi ? Toi, j'vois qu'tu voulais la guerre, tu l'auras Aah, j'finis par croire en peu de personnes sérieux, ai-je tort ? Celui qui m'escorte, m'escroque, sort et me laisse mort XXX ça, est-ce l'or qui divisera ? C'est les p'tits qui parlent de sexe, drogue, XXX J'fais acte de présence, les mecs trouvent ça affolant J'dégage tellement d'aisance, ça en devient insolent Mon hobby c'est la drogue, finis les autocollants J'suis haut toute la journée, je n'me déplace plus qu'en volant Ça plane... J'me sens privilégié J'arpente Paname les paupières lourdes et l'esprit léger Pourtant quand t'écoutes mon son, j'sens qu'ça t'éveille Mon savoir est une arme, j'te mets du plomb dans la cervelle J'suis l'ingé son mais j'n'ai pas oublié l'plaisir de rapper L'désir de backer, le 8 mesures, saisir et frapper, l'instrumentale Tu m'entends même sur off, je suis l'intrus mental Non tu mens, sache que je compte percer comme Rohff Et j'veux que les XXX m'empalent Les sceptiques à la fosse septique, on tire la chasse et basta V'nez pas casser la star, à c'stade on n'a plus l'âge des lascars Mais celui d'un homme adulte qui s'donne qu'à ceux qui assument Malgré un nombre d'cassures, j't'assure Chérie, j'reviendrai pour qu'ensemble ça dure Moi j'ai la dalle, je pense à graille, j'vais surement pas lâcher les steaks Et si le rap ne me nourrit pas, ben on ira lyncher ce traître Devant ma voix l'ingé stresse, impossible de la compresser XXX un déstress, ils disent tous qu'ils sont pressés La joie te chauffe mais se retire avant qu'elle te fasse cracher Finies les phases gâchées, on va pas se crasher, on nous sort la face cachée Ne t'attache pas trop, sache que même ce 8 est éphémère Au mic' c'est 2Zer qui pe-ra pour la tête des Femens XXX XXX J'éclate la track je n'vais pas m'tâter Ça va s'gâter, j'viens m'imposer, placer l'rap carré J'suis v'là l'taré avec des phases plus fortes qu'un shot de rhum J'agite mon lexique j't'explique, j'excite plus qu'une hot mom Je n'parle pas de pistolet ni de shotgun Juste d'la vie qu'j'connais pour l'instant je bosse j'me donne J'peux pas l'cacher j'viens m'installer fini l'bal masqué J'viens exceller, accélérer, révéler ma face cachée RETRANSCRIPTION EN COURS</t>
+          <t>Deux négros dans un 4x4 noir, pas de panique, y aura pas de 4-4-2 Et le taro, mon poto, ne tient qu'à moi, ça va t'arranger quand c'est le sin-c' à Zeu La rue, c'est l'feu, belek à ta sur, pas de coup de foudre, que des coups d'taser Je côtoie des pélos qui se foutent d'ta gueule pendant que devant mon négro, tu leur bouffes la queue Ouais, fuck ces putes solidaires, j'marche seul dans la rue comme un loup solitaire Toujours un il sur ta relation, les charos sur le coup quand ta go' se libère On m'a dit Ne traîne pas avec ces gens, Saïdou, fais belek, ces gars sont méchants Ça dit Psartek la nouvelle caisse, Merco-Benz, va dormir, on va s'faire tes jantes, ouais Demain, j'me casse à Miami, je maille, je danse sur le mia D'vant les keufs, je nie à vie, nan nan, y a pas d'ami-ami Demain, j'me casse à Miami, je maille, je danse sur le mia D'vant les keufs, je nie à vie, nan nan, y a pas d'ami-ami Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Deux gars du 9-4, mon négro, c'est tactique, leur faire du sale, mon négro, c'est technique Tous, tous les malheurs du monde, toi et ta team, va te faire enculer par Toutatis J'n'aime pas les michtos, ni les deurs-vi, j'n'aime pas les mythos, tu le devines Un verre, un frère, un noir déter', grand cur, grosses couilles mais tous les deux sont vides, ah Je la ramène dans une chambre d'hôtel, c'est une vraie bataille, c'est comme dans le maquis Jeune demoiselle a trouvé son mec mortel, elle m'a dit Merci comme Michel et Jacquie On m'a demandé John, pourquoi tu parles ainsi ? pourquoi ?, j'ai répondu Mon frérot, c'est la vie ouais L'argent facile n'est pas le plus facile mais paraît-il que cette putain d'rue les fascine, oh À c'qu'il paraît, t'es tout déter', alors vas-y montre nous, fais-le T'as beaucoup parlé, poto, t'aurais dû t'taire, chut, maintenant, la ville veut t'voir en vrette-le Oui, je suis 9-4, oui, je suis Vitry, oui, je suis 113, je suis Mafia K'1 Fry Oui, je suis Pour ceux, Les Princes de la city, oui je représente Phénomène Bizi, oh Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent et les filles faciles, j'pose pas avec n'importe qui en feat' J'vis ma vie sans savoir qui m'envie, chaque jour, ma liste d'ennemis s'remplit Pas pour la guerre, foutez-moi la paix, ta meuf est en chien, pas une couille à gratter Elle roule des yeux quand tu mets tes sons, elle a dit La prod est lourde mais tu l'as gâtée Mort aux adversaires, j'fais tout dans l'excès, mort aux associés qui vont me vexer En vrai, j'suis paro, faut me relaxer, toujours parano, j'me sens désaxé Qui manie l'acier mourra par l'acier, qui sniffe la C mourra par la C Fumer la Sherbert et deviens cher bête, j'suis rempli d'espèces, j'me sens menacé Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine</t>
         </is>
       </c>
     </row>
@@ -1835,12 +1835,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Bizi’N The Hood #2 - 4x4 Noir</t>
+          <t>Bon débarras</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Deux négros dans un 4x4 noir, pas de panique, y aura pas de 4-4-2 Et le taro, mon poto, ne tient qu'à moi, ça va t'arranger quand c'est le sin-c' à Zeu La rue, c'est l'feu, belek à ta sur, pas de coup de foudre, que des coups d'taser Je côtoie des pélos qui se foutent d'ta gueule pendant que devant mon négro, tu leur bouffes la queue Ouais, fuck ces putes solidaires, j'marche seul dans la rue comme un loup solitaire Toujours un il sur ta relation, les charos sur le coup quand ta go' se libère On m'a dit Ne traîne pas avec ces gens, Saïdou, fais belek, ces gars sont méchants Ça dit Psartek la nouvelle caisse, Merco-Benz, va dormir, on va s'faire tes jantes, ouais Demain, j'me casse à Miami, je maille, je danse sur le mia D'vant les keufs, je nie à vie, nan nan, y a pas d'ami-ami Demain, j'me casse à Miami, je maille, je danse sur le mia D'vant les keufs, je nie à vie, nan nan, y a pas d'ami-ami Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Deux gars du 9-4, mon négro, c'est tactique, leur faire du sale, mon négro, c'est technique Tous, tous les malheurs du monde, toi et ta team, va te faire enculer par Toutatis J'n'aime pas les michtos, ni les deurs-vi, j'n'aime pas les mythos, tu le devines Un verre, un frère, un noir déter', grand cur, grosses couilles mais tous les deux sont vides, ah Je la ramène dans une chambre d'hôtel, c'est une vraie bataille, c'est comme dans le maquis Jeune demoiselle a trouvé son mec mortel, elle m'a dit Merci comme Michel et Jacquie On m'a demandé John, pourquoi tu parles ainsi ? pourquoi ?, j'ai répondu Mon frérot, c'est la vie ouais L'argent facile n'est pas le plus facile mais paraît-il que cette putain d'rue les fascine, oh À c'qu'il paraît, t'es tout déter', alors vas-y montre nous, fais-le T'as beaucoup parlé, poto, t'aurais dû t'taire, chut, maintenant, la ville veut t'voir en vrette-le Oui, je suis 9-4, oui, je suis Vitry, oui, je suis 113, je suis Mafia K'1 Fry Oui, je suis Pour ceux, Les Princes de la city, oui je représente Phénomène Bizi, oh Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent et les filles faciles, j'pose pas avec n'importe qui en feat' J'vis ma vie sans savoir qui m'envie, chaque jour, ma liste d'ennemis s'remplit Pas pour la guerre, foutez-moi la paix, ta meuf est en chien, pas une couille à gratter Elle roule des yeux quand tu mets tes sons, elle a dit La prod est lourde mais tu l'as gâtée Mort aux adversaires, j'fais tout dans l'excès, mort aux associés qui vont me vexer En vrai, j'suis paro, faut me relaxer, toujours parano, j'me sens désaxé Qui manie l'acier mourra par l'acier, qui sniffe la C mourra par la C Fumer la Sherbert et deviens cher bête, j'suis rempli d'espèces, j'me sens menacé Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine Attiré par l'argent facile, attiré par l'argent facile Attiré par l'argent facile, paraît que la rue les fascine</t>
+          <t>Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Tu sais me piquer, tu fais monter ma rage monter ma rage, monter ma rage Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras J'ai zappé que j'suis serein quand t'es dans les parages dans les parages, dans les parages T'étais la seule immunisée dans ce monde de malade de malade, de malade Mais quand tu m'énervais, je conduis comme un fou dans Paname sku, sku, sku Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Mais quand t'es partie, t'as pris une partie de moi de moi, de moi J'te faisais des cachotteries maintenant je sais plus à qui parler parler, parler T'es rester à mes côtés même quand y avait le biff qui partait partait, partait Ne pleure pas quand la colère parle tu sais bien qu'c'est pas vrai pas vrai, bébé À la baraque, ça part en embrouille, personne pour séparer séparer, yeah Donc on dit des choses qu'on aurait pas dû dire et on fait des choses qu'on aurait pas dû faire yo J'y croyais pas quand tu m'as dit La prochaine, tu t'tires, j'ai rien senti venir, j'pensais avoir du flair Mon sin-cou m'a dit zer-2, ton cur, t'as dû l'perdre, tu passes dans ta bulle à bédave du teh comment, comment ? Comment v'-esqui l'adultère ? Comment v'-esqui l'adultère ? Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Tu sais me piquer, tu fais monter ma rage monter ma rage, monter ma rage Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras J'ai zappé que j'suis serein quand t'es dans les parages dans les parages, dans les parages T'étais la seule immunisée dans ce monde de malade de malade, de malade Mais quand tu m'énervais, je conduis comme un fou dans Paname sku, sku, sku Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Mais quand t'es partie, t'as pris une partie de moi de moi, de moi L'amour, c'est comme le bus', y a conflit d'intérêt mais si tu guettes le contrat y a pas marqué que j'dois t'aimer Fais bellek à ta conscience, elle pourrait t'étonner, avant la détonation, je savais pas c'que j'détenais Y a que du vice autour de moi, forcément, j'm'y connais, quand t'as dit oui devant le maire, est-ce que tu mythonnais ? L'amour, c'est pas un film, y a rien d'édulcoré, on répète sans cesse les mêmes erreurs, on dirait une choré' sku, sku On s'moquait des autres quand ils se disputaient, parmi les tes-bê, combien se disent futés ? On a ouvert les portes, le respect a failli fuiter, c'est cause perdue comme mon assiduité On s'est réconciliés mais putain comme on a pris du temps, c'est vrai que des fois le célibat est alléchant On s'est réconciliés mais putain, c'était d'jà trop tard, le physique et les sentiments avaient d'jà gés-chan Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Tu sais me piquer, tu fais monter ma rage monter ma rage, monter ma rage Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras J'ai zappé que j'suis serein quand t'es dans les parages dans les parages, dans les parages T'étais la seule immunisée dans ce monde de malade de malade, de malade Mais quand tu m'énervais, je conduis comme un fou dans Paname sku, sku, sku Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Mais quand t'es partie, t'as pris une partie de moi de moi, de moi Tu veux des réponses et j'en ai plus, tu veux des réponses et j'en ai plus pour toi Ouais, ton comportement m'a déçu, surtout quand tu me dis c'est la musique ou moi Tu veux des réponses et j'en ai plus, tu veux des réponses et j'en ai plus pour toi Ouais, ton comportement m'a déçu, surtout quand tu me dis c'est la musique ou moi</t>
         </is>
       </c>
     </row>
@@ -1852,12 +1852,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Bon débarras</t>
+          <t>Bulle</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Tu sais me piquer, tu fais monter ma rage monter ma rage, monter ma rage Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras J'ai zappé que j'suis serein quand t'es dans les parages dans les parages, dans les parages T'étais la seule immunisée dans ce monde de malade de malade, de malade Mais quand tu m'énervais, je conduis comme un fou dans Paname sku, sku, sku Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Mais quand t'es partie, t'as pris une partie de moi de moi, de moi J'te faisais des cachotteries maintenant je sais plus à qui parler parler, parler T'es rester à mes côtés même quand y avait le biff qui partait partait, partait Ne pleure pas quand la colère parle tu sais bien qu'c'est pas vrai pas vrai, bébé À la baraque, ça part en embrouille, personne pour séparer séparer, yeah Donc on dit des choses qu'on aurait pas dû dire et on fait des choses qu'on aurait pas dû faire yo J'y croyais pas quand tu m'as dit La prochaine, tu t'tires, j'ai rien senti venir, j'pensais avoir du flair Mon sin-cou m'a dit zer-2, ton cur, t'as dû l'perdre, tu passes dans ta bulle à bédave du teh comment, comment ? Comment v'-esqui l'adultère ? Comment v'-esqui l'adultère ? Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Tu sais me piquer, tu fais monter ma rage monter ma rage, monter ma rage Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras J'ai zappé que j'suis serein quand t'es dans les parages dans les parages, dans les parages T'étais la seule immunisée dans ce monde de malade de malade, de malade Mais quand tu m'énervais, je conduis comme un fou dans Paname sku, sku, sku Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Mais quand t'es partie, t'as pris une partie de moi de moi, de moi L'amour, c'est comme le bus', y a conflit d'intérêt mais si tu guettes le contrat y a pas marqué que j'dois t'aimer Fais bellek à ta conscience, elle pourrait t'étonner, avant la détonation, je savais pas c'que j'détenais Y a que du vice autour de moi, forcément, j'm'y connais, quand t'as dit oui devant le maire, est-ce que tu mythonnais ? L'amour, c'est pas un film, y a rien d'édulcoré, on répète sans cesse les mêmes erreurs, on dirait une choré' sku, sku On s'moquait des autres quand ils se disputaient, parmi les tes-bê, combien se disent futés ? On a ouvert les portes, le respect a failli fuiter, c'est cause perdue comme mon assiduité On s'est réconciliés mais putain comme on a pris du temps, c'est vrai que des fois le célibat est alléchant On s'est réconciliés mais putain, c'était d'jà trop tard, le physique et les sentiments avaient d'jà gés-chan Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Tu sais me piquer, tu fais monter ma rage monter ma rage, monter ma rage Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras J'ai zappé que j'suis serein quand t'es dans les parages dans les parages, dans les parages T'étais la seule immunisée dans ce monde de malade de malade, de malade Mais quand tu m'énervais, je conduis comme un fou dans Paname sku, sku, sku Quand t'es partie, j'me suis dit Bon débarras bon débarras, bon débarras Mais quand t'es partie, t'as pris une partie de moi de moi, de moi Tu veux des réponses et j'en ai plus, tu veux des réponses et j'en ai plus pour toi Ouais, ton comportement m'a déçu, surtout quand tu me dis c'est la musique ou moi Tu veux des réponses et j'en ai plus, tu veux des réponses et j'en ai plus pour toi Ouais, ton comportement m'a déçu, surtout quand tu me dis c'est la musique ou moi</t>
+          <t>Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse</t>
         </is>
       </c>
     </row>
@@ -1869,12 +1869,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Bulle</t>
+          <t>Capitale sale</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse</t>
+          <t>OK, L'Animal S-Crew, 14ème, 15ème, brah ! Yeah Appelle moi scientifique quand j'fais jouer les mots pour faire des rimes Pas pour faire rire, tu t'en rends compte quand dans ton froc t'urines Y'a pas d'tulipes, ça parle de mort alors avoue tu flippes Et l'foutu vide, y'a des tueurs à gage comme dans les films Et, dans ma ville, y'a des trucs sales mais rien arrive au vent Donc il faut vaincre et pas échouer, bah, j'ai mis des feintes Sans mettre de freins, j'crois que j'arrêterai quand j'aurais 20 000 textes Ouais, j'arrêterai quand dans la salle y aura 200 000 têtes Les ennuis m'guettent, j'ai vu qu'les deks étaient des photographes Pour cé-per vite, dans l'rap français faut être une pornstar Mes potos s'marrent mais, au final, j'ai vu qu'on à tous mal Et ouais, ma couille, tout l'monde magouille pour se per-sa en marque En marge de tous, mais sur ma vie que j'ai jamais fait la pute La vie, la rue, c'est comme une bite, cousin, parfois c'est dur Bah ouais, c'est dur, quand l'téléphone sonne à 7h du mat' Mauvaise nouvelle, mais pour mon pote j'suis là une heure plus tard Nekfeu est dur comme la gaule matinale, j'fais jouir les gos vaginales Y'a plus d'espoir, j'bois tous les soirs, j'arrête quand l'alcool m'a mis mal J'enchaîne les comas minables et j'en redemande, j'emmerde le monde Le genre de môme qui gère des bombes sauvages comme l'Animal En cash, le barge qu'on manie mal qui marche vers le combat final Sois cash, t'as pas dix balles ? Il m'faut du hasch pour le tabac que j'inhale Et j'suis pas Dany Dan, terrain miné si t'es rappeur J'suis le kinésithérapeute, j'viens te masser pour qu'ma famille dame Donc j'use mes amygdales pour mon habitat crade La capitale sale, quand t'as mis d'la came, les amis t'acclament Vite, tape m'en 5, t'a repéré la mif J'veux serrer d'la miche avant d'avoir un bide de femme enceinte Fuck les petits toutous, on plie tout, nous, même avec un flow lent C'est affolant comme quitte ou double, on vis toujours en insolent Les coups de crasse, moi, j'les crains plus, j'suis un peu comme anesthésié Gros, j'ouvre ma bouche pour ceux qui pendant toutes ces années s'taisaient T'as linstinct animal, t'es comme un chien, tu sens la peur T'es pas technique alors qu'une de mes phases tue cent rappeurs La vérité blesse mais l'mensonge tue, les grandes gueules sont sermentées Moi, sur le podium, faut m'faire monter, toi, laisse ton flow à fermenter Écoute la consonance, les cons s'élancent et vers le Front tire Le pire c'est qu'on sait quand les conséquences dépasse les frontières Tu parles trop mal, j'aime pas ta langue, t'as tout ce qu'il faut mais pas l'talent T'as trop baisser ton pantalon, mon flow te laisse les bras balants Pas besoin d'bosa nova ni d'faire l'Casanova Si on m'ferme Générations bah la vie d'moi j'passe à Nova Le succès passera nous voir, moi, je déploie ça pour voir J'lève mon verre au jour où la mifa dépassera l'pouvoir J'vois c'qui s'passe autour de moi, oui, lucide mais parano J'ai trop peur, genre ma femme mise enceinte par un autre Salope !</t>
         </is>
       </c>
     </row>
@@ -1886,12 +1886,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Capitale sale</t>
+          <t>Comment faire</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>OK, L'Animal S-Crew, 14ème, 15ème, brah ! Yeah Appelle moi scientifique quand j'fais jouer les mots pour faire des rimes Pas pour faire rire, tu t'en rends compte quand dans ton froc t'urines Y'a pas d'tulipes, ça parle de mort alors avoue tu flippes Et l'foutu vide, y'a des tueurs à gage comme dans les films Et, dans ma ville, y'a des trucs sales mais rien arrive au vent Donc il faut vaincre et pas échouer, bah, j'ai mis des feintes Sans mettre de freins, j'crois que j'arrêterai quand j'aurais 20 000 textes Ouais, j'arrêterai quand dans la salle y aura 200 000 têtes Les ennuis m'guettent, j'ai vu qu'les deks étaient des photographes Pour cé-per vite, dans l'rap français faut être une pornstar Mes potos s'marrent mais, au final, j'ai vu qu'on à tous mal Et ouais, ma couille, tout l'monde magouille pour se per-sa en marque En marge de tous, mais sur ma vie que j'ai jamais fait la pute La vie, la rue, c'est comme une bite, cousin, parfois c'est dur Bah ouais, c'est dur, quand l'téléphone sonne à 7h du mat' Mauvaise nouvelle, mais pour mon pote j'suis là une heure plus tard Nekfeu est dur comme la gaule matinale, j'fais jouir les gos vaginales Y'a plus d'espoir, j'bois tous les soirs, j'arrête quand l'alcool m'a mis mal J'enchaîne les comas minables et j'en redemande, j'emmerde le monde Le genre de môme qui gère des bombes sauvages comme l'Animal En cash, le barge qu'on manie mal qui marche vers le combat final Sois cash, t'as pas dix balles ? Il m'faut du hasch pour le tabac que j'inhale Et j'suis pas Dany Dan, terrain miné si t'es rappeur J'suis le kinésithérapeute, j'viens te masser pour qu'ma famille dame Donc j'use mes amygdales pour mon habitat crade La capitale sale, quand t'as mis d'la came, les amis t'acclament Vite, tape m'en 5, t'a repéré la mif J'veux serrer d'la miche avant d'avoir un bide de femme enceinte Fuck les petits toutous, on plie tout, nous, même avec un flow lent C'est affolant comme quitte ou double, on vis toujours en insolent Les coups de crasse, moi, j'les crains plus, j'suis un peu comme anesthésié Gros, j'ouvre ma bouche pour ceux qui pendant toutes ces années s'taisaient T'as linstinct animal, t'es comme un chien, tu sens la peur T'es pas technique alors qu'une de mes phases tue cent rappeurs La vérité blesse mais l'mensonge tue, les grandes gueules sont sermentées Moi, sur le podium, faut m'faire monter, toi, laisse ton flow à fermenter Écoute la consonance, les cons s'élancent et vers le Front tire Le pire c'est qu'on sait quand les conséquences dépasse les frontières Tu parles trop mal, j'aime pas ta langue, t'as tout ce qu'il faut mais pas l'talent T'as trop baisser ton pantalon, mon flow te laisse les bras balants Pas besoin d'bosa nova ni d'faire l'Casanova Si on m'ferme Générations bah la vie d'moi j'passe à Nova Le succès passera nous voir, moi, je déploie ça pour voir J'lève mon verre au jour où la mifa dépassera l'pouvoir J'vois c'qui s'passe autour de moi, oui, lucide mais parano J'ai trop peur, genre ma femme mise enceinte par un autre Salope !</t>
+          <t>Jécris des particules de textes noires En coste-La Jmets pas mon avenir en pause moi Jmimpose moi Cest différent quand la prose parle Sur dla grosse la basse Jpourrais facilement faire autre chose Mais jose ap Jdois dêtre précis quand jsuis dans cdel Jsuis dans lthème Souvent les vieux démons mencerclent Veulent danser Jregarde devant moi même quand je doute Ou quand jétouff Savent que cest différnt quand cest nous Le temps fait tout Jsuis sur lnavire quand on prend la mer Le gang samène Moi, jdois v'-esqui quand ça mprend la tête Faut quon sarrête Quand la haine me suit, je prends sur moi Jfais face au mal Elle ma dit jsuis la même quand cest noir Ne ten fais pas, eh Je sais pas comment faire Même quand jvide ma tête Jvois tout à lenvers yeah yeah eh eh Je sais pas comment faire Même quand jvide ma tête Jvois tout à lenvers yeah yeah eh eh Toi, dis-moi s'tu sais toi, dis-moi s'tu sais Toi, dis-moi s'tu sais mieux qu'moi Toi, dis-moi s'tu sais si tu sais mieux Yeah yeah, eh eh Pas là pour remplir les quotas J'fais partie des gens qui côtoient Les vilains, les bandits dGotham Où la vie vaut un lo-ki dcoca Ces temps-ci, cest couci-couça Je ne sais pas quoi faire de tout ça On mdit Fais loseille en silence Donc je létouffe sous un coussin J'sais pas comment faire donc j'te dis cash daller t'faire enculer Il ma dit Sans rancune mais c'fils de pute a lair très rancunier Jme rappelle de cette scène filmée par mes globes oculaires Bizarrement dans cmonde, rester à larrêt t'fait reculer, ouais Je sais pas comment faire Même quand jvide ma tête Jvois tout à lenvers yeah yeah eh eh Je sais pas comment faire Même quand jvide ma tête Jvois tout à lenvers yeah yeah eh eh Toi, dis-moi s'tu sais toi, dis-moi s'tu sais Toi, dis-moi s'tu sais mieux qu'moi Toi, dis-moi s'tu sais si tu sais mieux Yeah yeah, eh eh Toi, dis-moi s'tu sais Toi, dis-moi s'tu sais mieux qu'moi Toi, dis-moi s'tu sais Yeah yeah eh eh</t>
         </is>
       </c>
     </row>
@@ -1903,12 +1903,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Comment faire</t>
+          <t>Conscience tranquille</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Jécris des particules de textes noires En coste-La Jmets pas mon avenir en pause moi Jmimpose moi Cest différent quand la prose parle Sur dla grosse la basse Jpourrais facilement faire autre chose Mais jose ap Jdois dêtre précis quand jsuis dans cdel Jsuis dans lthème Souvent les vieux démons mencerclent Veulent danser Jregarde devant moi même quand je doute Ou quand jétouff Savent que cest différnt quand cest nous Le temps fait tout Jsuis sur lnavire quand on prend la mer Le gang samène Moi, jdois v'-esqui quand ça mprend la tête Faut quon sarrête Quand la haine me suit, je prends sur moi Jfais face au mal Elle ma dit jsuis la même quand cest noir Ne ten fais pas, eh Je sais pas comment faire Même quand jvide ma tête Jvois tout à lenvers yeah yeah eh eh Je sais pas comment faire Même quand jvide ma tête Jvois tout à lenvers yeah yeah eh eh Toi, dis-moi s'tu sais toi, dis-moi s'tu sais Toi, dis-moi s'tu sais mieux qu'moi Toi, dis-moi s'tu sais si tu sais mieux Yeah yeah, eh eh Pas là pour remplir les quotas J'fais partie des gens qui côtoient Les vilains, les bandits dGotham Où la vie vaut un lo-ki dcoca Ces temps-ci, cest couci-couça Je ne sais pas quoi faire de tout ça On mdit Fais loseille en silence Donc je létouffe sous un coussin J'sais pas comment faire donc j'te dis cash daller t'faire enculer Il ma dit Sans rancune mais c'fils de pute a lair très rancunier Jme rappelle de cette scène filmée par mes globes oculaires Bizarrement dans cmonde, rester à larrêt t'fait reculer, ouais Je sais pas comment faire Même quand jvide ma tête Jvois tout à lenvers yeah yeah eh eh Je sais pas comment faire Même quand jvide ma tête Jvois tout à lenvers yeah yeah eh eh Toi, dis-moi s'tu sais toi, dis-moi s'tu sais Toi, dis-moi s'tu sais mieux qu'moi Toi, dis-moi s'tu sais si tu sais mieux Yeah yeah, eh eh Toi, dis-moi s'tu sais Toi, dis-moi s'tu sais mieux qu'moi Toi, dis-moi s'tu sais Yeah yeah eh eh</t>
+          <t>J'ai la rage et j'aime bien le crier sur tous les toits C'est la de-mer, avant d'aider les autres, surtout aide-toi Fais ton chemin car t'es seul, issu d'un d'ces quartiers cheums Pour tout c'qu'on m'a fait y a prescription mais j'ai gardé l'seum J'confonds pas les potes occasionnels et les mecs sincères Si tu m'trahis, j'vais te montrer à quoi les médecins servent J'fume l'ignorance sans filtres, mon innocence s'enfuit J'ai la conscience tranquille, faut pas qu'on s'lance sans fil Moi j'en ai marre du rap de merde, j'écouterai plus qu'le son d'l'horloge Faut pas qu'tu pollues mes oreilles, j'les couperai comme Vincent Van Gogh Tu m'bouffes de l'intérieur, tu m'fais l'effet d'une bactérie Tu veux qu'j'te fasse des tofs, t'veux pas aussi que j'backe tes rimes ? Suivre son coeur c'est dangereux, mon cerveau, quand ça craint, j'l'en mêle Mes sentiments s'emmêlent, faut que j'transforme mon chagrin en haine Dans ma tête j'me fais des films ou c'est les films qui s'font ma tête À donner des leçons, j'm'apprête Les ghettos mentent, le son j'maltraite Ici les poulets t'cuisinent, putain c'est l'monde à l'envers Quand je pense à m'évader, gros, j'ai l'moral en baisse Si ton malheur m'affecte, c'est par peur que ça m'arrive Les tueurs ont la conscience aussi vierge que Sainte-Marie Les poulets t'cuisinent, putain c'est l'monde à l'envers Quand je pense à m'évader, gros, j'ai l'moral en baisse Si ton malheur m'affecte, c'est par peur que ça m'arrive Les tueurs ont la conscience aussi vierge que Sainte-Marie Que j'perce dans l'peura, c'est ça ma prophétie Moi j'en ai marre, ça y est j'me lance, le bonheur m'a trop fait signe Dans ma vie, en général, moi j'suis d'humeur pas trop festive On arrive pour gêner l'rap, pour que tu dise 'Tain trop frais l'style Si j'suis un pro, j'fais skill, me paie Les mecs faux, meskine, se plaignent Depuis que ça rap y en a même qui, pour Mesrine, se prennent J'ai pas de compte à t'rendre, espère même pas qu'on t'attende Si j'veux pas t'voir, j'te verrai pas j'suis un maître en esquive suprême J'suis pas d'ceux qui font le mal et qui en font l'apologie Ni d'ceux qui disent que font la religion n'est que d'la biologie Fini l'temps du fitness, j'ai une balance pour peser l'herbe grasse Marie-Jeanne me fait planer mais j'l'aime malgré son air de garce Beaucoup plus qu'une guerre de classe Là où j'vais, il n'y a guère de grâce Comment cer-per dans faire de crasse ? Y en a même qui à terre t'écrasent J'veux réussir mais j'fais parti d'ces jeunes qui poussent des cris en cours Ma vision du succès c'est plus qu'un stand aux puces de Clignancourt Ici les poulets t'cuisinent, putain c'est l'monde à l'envers Quand je pense à m'évader, gros, j'ai l'moral en baisse Si ton malheur m'affecte, c'est par peur que ça m'arrive Les tueurs ont la conscience aussi vierge que Sainte-Marie Les poulets t'cuisinent, putain c'est l'monde à l'envers Quand je pense à m'évader, gros, j'ai l'moral en baisse Si ton malheur m'affecte, c'est par peur que ça m'arrive Les tueurs ont la conscience aussi vierge que Sainte-Marie</t>
         </is>
       </c>
     </row>
@@ -1920,12 +1920,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Conscience tranquille</t>
+          <t>Crise de nerf</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>J'ai la rage et j'aime bien le crier sur tous les toits C'est la de-mer, avant d'aider les autres, surtout aide-toi Fais ton chemin car t'es seul, issu d'un d'ces quartiers cheums Pour tout c'qu'on m'a fait y a prescription mais j'ai gardé l'seum J'confonds pas les potes occasionnels et les mecs sincères Si tu m'trahis, j'vais te montrer à quoi les médecins servent J'fume l'ignorance sans filtres, mon innocence s'enfuit J'ai la conscience tranquille, faut pas qu'on s'lance sans fil Moi j'en ai marre du rap de merde, j'écouterai plus qu'le son d'l'horloge Faut pas qu'tu pollues mes oreilles, j'les couperai comme Vincent Van Gogh Tu m'bouffes de l'intérieur, tu m'fais l'effet d'une bactérie Tu veux qu'j'te fasse des tofs, t'veux pas aussi que j'backe tes rimes ? Suivre son coeur c'est dangereux, mon cerveau, quand ça craint, j'l'en mêle Mes sentiments s'emmêlent, faut que j'transforme mon chagrin en haine Dans ma tête j'me fais des films ou c'est les films qui s'font ma tête À donner des leçons, j'm'apprête Les ghettos mentent, le son j'maltraite Ici les poulets t'cuisinent, putain c'est l'monde à l'envers Quand je pense à m'évader, gros, j'ai l'moral en baisse Si ton malheur m'affecte, c'est par peur que ça m'arrive Les tueurs ont la conscience aussi vierge que Sainte-Marie Les poulets t'cuisinent, putain c'est l'monde à l'envers Quand je pense à m'évader, gros, j'ai l'moral en baisse Si ton malheur m'affecte, c'est par peur que ça m'arrive Les tueurs ont la conscience aussi vierge que Sainte-Marie Que j'perce dans l'peura, c'est ça ma prophétie Moi j'en ai marre, ça y est j'me lance, le bonheur m'a trop fait signe Dans ma vie, en général, moi j'suis d'humeur pas trop festive On arrive pour gêner l'rap, pour que tu dise 'Tain trop frais l'style Si j'suis un pro, j'fais skill, me paie Les mecs faux, meskine, se plaignent Depuis que ça rap y en a même qui, pour Mesrine, se prennent J'ai pas de compte à t'rendre, espère même pas qu'on t'attende Si j'veux pas t'voir, j'te verrai pas j'suis un maître en esquive suprême J'suis pas d'ceux qui font le mal et qui en font l'apologie Ni d'ceux qui disent que font la religion n'est que d'la biologie Fini l'temps du fitness, j'ai une balance pour peser l'herbe grasse Marie-Jeanne me fait planer mais j'l'aime malgré son air de garce Beaucoup plus qu'une guerre de classe Là où j'vais, il n'y a guère de grâce Comment cer-per dans faire de crasse ? Y en a même qui à terre t'écrasent J'veux réussir mais j'fais parti d'ces jeunes qui poussent des cris en cours Ma vision du succès c'est plus qu'un stand aux puces de Clignancourt Ici les poulets t'cuisinent, putain c'est l'monde à l'envers Quand je pense à m'évader, gros, j'ai l'moral en baisse Si ton malheur m'affecte, c'est par peur que ça m'arrive Les tueurs ont la conscience aussi vierge que Sainte-Marie Les poulets t'cuisinent, putain c'est l'monde à l'envers Quand je pense à m'évader, gros, j'ai l'moral en baisse Si ton malheur m'affecte, c'est par peur que ça m'arrive Les tueurs ont la conscience aussi vierge que Sainte-Marie</t>
+          <t>Longue est l'éternité, déter' est le vocabulaire Et j'casse des crânes et j'claque des faces comme Müller Je ne veux pas être adulé, j'm'en bats les couilles de toutes vos suceries C'est la tête dans une tass' que je noie mes soucis Dans la débilité, fuck la stupidité L'oseille, qu'une idée souvent victime de la cupidité, mais Ciblé par les autres, refusé par les patrons Pas venu par accident mais j'suis né pour faire un carton L'argent divise les potes et les proches sur le Porsche Dans ce monde de porcs, ya foye dans les poches et mes frères qui me portent Au-delà des yeux, shoote-les au peu-pom La beu-bom dans cette Dounia triste où il y a peu de bons N'écoute pas les ministres et milites avec ton millimètre Fuck les millis, mec, trop occupé à sauver Willy, han Harcelé par mes démons, je ne suis qu'une part d'homme Fuck-les tous, et pour mes péchés, que Dieu me pardonne Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien, on agit comme des cancres Mais si j'arrête pas, mon ange de gauche n'aura plus d'encre Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien, on agit comme des cancres Bientôt, mon ange de gauche n'aura plus d'encre Ici c'est gadjis et bouts de shit, latinas bitches Maquillage qui brille, taille fine, vrai booty Des Malika divines qui assassinent tes groupies Pas de gamines, c'est pourri, que des sales biatches qui sniffent Cadillac, bling-bling, ça m'intéresse pas J'veux la vie à Biggie, flingues et belles femmes On bataille pour mes sauvages et mes tou-bab Avec Saï-Saï, John Hash et Doumams Pour eux, la vie c'était philo', dictionnaire Moi, mes amis, on terminait schizos, bipolaires J'ai toujours pas besoin de tes strass et paillettes Si t'effaces mes galères, j'fais que sser-froi des canettes Des fois, j'vais l'admettre que j'm'écarte des tapettes qui déçoivent On a des swags qui décoiffent les starlettes J'suis pas un escroc, j'laisse vos bails se dérouler À vrai dire, Marie-Jeanne est la seule que j'ai roulé Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé, la vie est une vaste mer On y comprend rien, on agit comme des cancres Mais si j'arrête pas mon ange de gauche n'aura plus d'encre Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien on agit comme des cancres Bientôt mon ange de gauche n'aura plus d'encre On serait à l'époque, ce serait nous les gueux C'est depuis que j'suis né que On s'obstine à croire que notre destinée sera dégueu' Mais j'admets que j'ai plus souvent la flemme Que j'assume le cliché grosse queue Yes, I'm a real nigga Pour revenir à mon avenir, j'me dis qu'il est pas beau Mais trop d'appétit petit bateau veut devenir paquebot Un titan, nique s'ils aiment pas nos blazes On brise la glace Phénomène n'est pas le Titanic J'accumule les risques, qu'ils disent qu'on est paros Le cerveau rayé comme un disque qui tourne pas rond C'est pour mes mauvais garçons, nos whiskys n'ont pas de glaçons Gare à son vice, miss, on sait comment les garces sont Ils cherchent le succès, font tout pour qu'on les mette bien C'est bien si tu suces, c'est encore mieux si tu suces bien Sans couilles, t'as pas de valeur sans valeur, aucun ennemi Donc mes ennemis viennent voir ce que valent mes couilles Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé, la vie est une vaste mer On y comprend rien, on agit comme des cancres Mais si j'arrête pas mon ange de gauche n'aura plus d'encre Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien on agit comme des cancres Bientôt mon ange de gauche n'aura plus d'encre Ouais, tu sais qui c'est le boss Salope, enlève ton gloss Pète le second d'un second rôle d'une série B Yo, dawg, tu veux tester mon crew ? J'te parle pas du ... Mais de mes frères qui charbonnent tous les jours dans Bruce Sept-Cinq-Double-Zéro-Neuf, Sept-Cinq Zéro-Quinze Sans oublier les bavons qui barodent dans le Vingt-Moins-Un C'est simple on marche en meute, à deux ou bien solitaire Mais quoi qu'il arrive, on est tous àl' si y a conflit, frère Donc on se met mleh dans le sud de Bruxelles jusqu'à Bordeaux On se met mleh dans le stud', pas de pucelles, que des prolos Bordeaux et un tas de stups Sur le terrain, ça se bute à la came, fréro J't'assure qu'on ne baisse pas nos frocs, que des blunts pour mes ninjas On s'en ... de tes hoes et toutes tes offres On ouvre tes portes avec des pieds d'bitchs Wassup ? De nos jours, y a plus de grands ou de petits Si t'es pas de la mif, on te nique ta mère Clic-baw sur tes types Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé, la vie est une vaste mer On y comprend rien, on agit comme des cancres Mais si j'arrête pas mon ange de gauche n'aura plus d'encre Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien on agit comme des cancres Bientôt mon ange de gauche n'aura plus d'encre</t>
         </is>
       </c>
     </row>
@@ -1937,12 +1937,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Crise de nerf</t>
+          <t>Décisions</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Longue est l'éternité, déter' est le vocabulaire Et j'casse des crânes et j'claque des faces comme Müller Je ne veux pas être adulé, j'm'en bats les couilles de toutes vos suceries C'est la tête dans une tass' que je noie mes soucis Dans la débilité, fuck la stupidité L'oseille, qu'une idée souvent victime de la cupidité, mais Ciblé par les autres, refusé par les patrons Pas venu par accident mais j'suis né pour faire un carton L'argent divise les potes et les proches sur le Porsche Dans ce monde de porcs, ya foye dans les poches et mes frères qui me portent Au-delà des yeux, shoote-les au peu-pom La beu-bom dans cette Dounia triste où il y a peu de bons N'écoute pas les ministres et milites avec ton millimètre Fuck les millis, mec, trop occupé à sauver Willy, han Harcelé par mes démons, je ne suis qu'une part d'homme Fuck-les tous, et pour mes péchés, que Dieu me pardonne Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien, on agit comme des cancres Mais si j'arrête pas, mon ange de gauche n'aura plus d'encre Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien, on agit comme des cancres Bientôt, mon ange de gauche n'aura plus d'encre Ici c'est gadjis et bouts de shit, latinas bitches Maquillage qui brille, taille fine, vrai booty Des Malika divines qui assassinent tes groupies Pas de gamines, c'est pourri, que des sales biatches qui sniffent Cadillac, bling-bling, ça m'intéresse pas J'veux la vie à Biggie, flingues et belles femmes On bataille pour mes sauvages et mes tou-bab Avec Saï-Saï, John Hash et Doumams Pour eux, la vie c'était philo', dictionnaire Moi, mes amis, on terminait schizos, bipolaires J'ai toujours pas besoin de tes strass et paillettes Si t'effaces mes galères, j'fais que sser-froi des canettes Des fois, j'vais l'admettre que j'm'écarte des tapettes qui déçoivent On a des swags qui décoiffent les starlettes J'suis pas un escroc, j'laisse vos bails se dérouler À vrai dire, Marie-Jeanne est la seule que j'ai roulé Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé, la vie est une vaste mer On y comprend rien, on agit comme des cancres Mais si j'arrête pas mon ange de gauche n'aura plus d'encre Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien on agit comme des cancres Bientôt mon ange de gauche n'aura plus d'encre On serait à l'époque, ce serait nous les gueux C'est depuis que j'suis né que On s'obstine à croire que notre destinée sera dégueu' Mais j'admets que j'ai plus souvent la flemme Que j'assume le cliché grosse queue Yes, I'm a real nigga Pour revenir à mon avenir, j'me dis qu'il est pas beau Mais trop d'appétit petit bateau veut devenir paquebot Un titan, nique s'ils aiment pas nos blazes On brise la glace Phénomène n'est pas le Titanic J'accumule les risques, qu'ils disent qu'on est paros Le cerveau rayé comme un disque qui tourne pas rond C'est pour mes mauvais garçons, nos whiskys n'ont pas de glaçons Gare à son vice, miss, on sait comment les garces sont Ils cherchent le succès, font tout pour qu'on les mette bien C'est bien si tu suces, c'est encore mieux si tu suces bien Sans couilles, t'as pas de valeur sans valeur, aucun ennemi Donc mes ennemis viennent voir ce que valent mes couilles Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé, la vie est une vaste mer On y comprend rien, on agit comme des cancres Mais si j'arrête pas mon ange de gauche n'aura plus d'encre Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien on agit comme des cancres Bientôt mon ange de gauche n'aura plus d'encre Ouais, tu sais qui c'est le boss Salope, enlève ton gloss Pète le second d'un second rôle d'une série B Yo, dawg, tu veux tester mon crew ? J'te parle pas du ... Mais de mes frères qui charbonnent tous les jours dans Bruce Sept-Cinq-Double-Zéro-Neuf, Sept-Cinq Zéro-Quinze Sans oublier les bavons qui barodent dans le Vingt-Moins-Un C'est simple on marche en meute, à deux ou bien solitaire Mais quoi qu'il arrive, on est tous àl' si y a conflit, frère Donc on se met mleh dans le sud de Bruxelles jusqu'à Bordeaux On se met mleh dans le stud', pas de pucelles, que des prolos Bordeaux et un tas de stups Sur le terrain, ça se bute à la came, fréro J't'assure qu'on ne baisse pas nos frocs, que des blunts pour mes ninjas On s'en ... de tes hoes et toutes tes offres On ouvre tes portes avec des pieds d'bitchs Wassup ? De nos jours, y a plus de grands ou de petits Si t'es pas de la mif, on te nique ta mère Clic-baw sur tes types Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé, la vie est une vaste mer On y comprend rien, on agit comme des cancres Mais si j'arrête pas mon ange de gauche n'aura plus d'encre Le biff, la mif, les daronnes et leurs crises de nerf Déter', isolé la vie est une vaste mer On y comprend rien on agit comme des cancres Bientôt mon ange de gauche n'aura plus d'encre</t>
+          <t>Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions À la fin, nous périssons, tourne tout en dérision Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions Tourne tout en dérision, tourne tout en dérision Même si ton choix n'est pas le bon, ne regrette pas, fais pas le con, mmh Même si ton choix n'est pas le bon, ne regrette pas, fais pas le con, brr, brr J'suis ce genre de mec avec le spleef au coin des lèvres, tu connais pas Seine Zoo, c'est soit t'es bête ou soit t'es dead Chez nous soit t'es la bitch, soit t'es le proxénète, n'écoute pas tes sentiments pour que ton business soit propre et net Soit t'es dans la foule ou soit t'es sur le postscaenium, j'suis ce genre de lion qui saute dans la fosse aux lionnes Soit t'es toujours au summum, indépendant et autonome, soit t'as pas le choix, t'apprends à apprécier les fausses notes, eh Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions À la fin, nous périssons, tourne tout en dérision Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions Tourne tout en dérision, tourne tout en dérision Même si ton choix n'est pas le bon, ne regrette pas, fais pas le con, mmh Même si ton choix n'est pas le bon, ne regrette pas, fais pas le con, brr, brr On a posé nos couilles sur la table, on est organisés comme les cartels de Culiacan Fais attention à qui tu secoues la patte, tu lui dis Viens tout seul, mais ils déboulent à quatre Certaines décisions t'amènent à la perquisition ou t'amènes à voir ta te-tê à la télévision Même quand t'as pas le choix, y a toujours une solution, c'est juste que notre vision est brouillée par la pollution Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions À la fin, nous périssons, tourne tout en dérision Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions Tourne tout en dérision, tourne tout en dérision</t>
         </is>
       </c>
     </row>
@@ -1954,12 +1954,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Décisions</t>
+          <t>De l’autre côté de la Seine (Épisode II)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions À la fin, nous périssons, tourne tout en dérision Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions Tourne tout en dérision, tourne tout en dérision Même si ton choix n'est pas le bon, ne regrette pas, fais pas le con, mmh Même si ton choix n'est pas le bon, ne regrette pas, fais pas le con, brr, brr J'suis ce genre de mec avec le spleef au coin des lèvres, tu connais pas Seine Zoo, c'est soit t'es bête ou soit t'es dead Chez nous soit t'es la bitch, soit t'es le proxénète, n'écoute pas tes sentiments pour que ton business soit propre et net Soit t'es dans la foule ou soit t'es sur le postscaenium, j'suis ce genre de lion qui saute dans la fosse aux lionnes Soit t'es toujours au summum, indépendant et autonome, soit t'as pas le choix, t'apprends à apprécier les fausses notes, eh Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions À la fin, nous périssons, tourne tout en dérision Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions Tourne tout en dérision, tourne tout en dérision Même si ton choix n'est pas le bon, ne regrette pas, fais pas le con, mmh Même si ton choix n'est pas le bon, ne regrette pas, fais pas le con, brr, brr On a posé nos couilles sur la table, on est organisés comme les cartels de Culiacan Fais attention à qui tu secoues la patte, tu lui dis Viens tout seul, mais ils déboulent à quatre Certaines décisions t'amènent à la perquisition ou t'amènes à voir ta te-tê à la télévision Même quand t'as pas le choix, y a toujours une solution, c'est juste que notre vision est brouillée par la pollution Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, beaucoup de choix, une seule décision J'suis sûr de quoi si j'suis pas sûr de moi ? Décisions, décisions Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions À la fin, nous périssons, tourne tout en dérision Décisions, décisions, décisions, décisions J'dois les prendre même sans la moindre précision Décisions, décisions, décisions, décisions Tourne tout en dérision, tourne tout en dérision</t>
+          <t>Blackbird, bébé, 2-Zer S-Crew, on est trop mleh ! Seine Zoo, le 30 Septembre dans les bacs J'ai la gorge serrée Et la peur du futur comme un gosse Qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules et pas quand des vieux cons te parlent Car la France est en décadence dès que tombe la nuit Avec ce son, le navire est battu par les flots mais ne sombre pas Les poulets font des guet-apens car j'fais que pondre ma rime Mon Rap ne peut pas s'épanouir sans affinité Un peu comme l'agilité d'une bête en captivité J'laisse le stress s'évanouir, j'efface mes fragilités J'ai gardé ma dignité, rapper n'est pas une facilité T'es prévisible comme une bagarre à l'open-bar Tu vois 2-Zer avec ta femme ? C'est qu'ce bâtard à trop bédave Nos vies c'est l'anarchie, le succès est pas là par magie Tu nous as croisé dans les open-mics de Paname à Rotterdam Petit rageux Ta langue est plus pendue qu'un gars qui vole du bétail au XIXème siècle Crois pas que mon posse te respecte Barre-toi avant qu'on t'vise en pleine tête Bye, bye...</t>
         </is>
       </c>
     </row>
@@ -1971,12 +1971,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>De l’autre côté de la Seine (Épisode II)</t>
+          <t>Deux comme toi</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Blackbird, bébé, 2-Zer S-Crew, on est trop mleh ! Seine Zoo, le 30 Septembre dans les bacs J'ai la gorge serrée Et la peur du futur comme un gosse Qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules et pas quand des vieux cons te parlent Car la France est en décadence dès que tombe la nuit Avec ce son, le navire est battu par les flots mais ne sombre pas Les poulets font des guet-apens car j'fais que pondre ma rime Mon Rap ne peut pas s'épanouir sans affinité Un peu comme l'agilité d'une bête en captivité J'laisse le stress s'évanouir, j'efface mes fragilités J'ai gardé ma dignité, rapper n'est pas une facilité T'es prévisible comme une bagarre à l'open-bar Tu vois 2-Zer avec ta femme ? C'est qu'ce bâtard à trop bédave Nos vies c'est l'anarchie, le succès est pas là par magie Tu nous as croisé dans les open-mics de Paname à Rotterdam Petit rageux Ta langue est plus pendue qu'un gars qui vole du bétail au XIXème siècle Crois pas que mon posse te respecte Barre-toi avant qu'on t'vise en pleine tête Bye, bye...</t>
+          <t>Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Tu peux avoir le monde si c'est bien demandé mais maman m'a dit C'est pas bien de quémander Tu fais les choses à ta façon, ils veulent te réprimander, c'est grâce à GTA si j'maîtrise l'anglais J'vais les ignorer, j'ai fermé tous les onglets, ils ont le seum, je n'accepte pas leurs invit' C'est tous des clones, ouais, c'est tous des zombies, leur caractère est limité comme un tweet Ça y est, t'en as pas marre de côtoyer la 'sère ? Surtout que la tristesse dure le temps d'une averse Faut rattraper l'retard, remettre les pendules à l'heure, surtout que le bonheur dure le temps du malheur Ils pouvaient pas me voir en face, ils m'ont tourné le dos, maintenant, je prends du cash même pour les journées repos J'ai tourné la page mais c'est resté dans ma tête, je ne ferai pas l'album ou la tournée de trop Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Tu te plains de ta situation mais tu passes tes journées à rêvasser devant la télé Un cauchemar éveillé, j'en vois pas l'intérêt, nan, tu vis pas, tu fais d'la figuration, ouais Et tu te plains de ta situation mais tu choisis ton destin c'est de l'automutilation T'en as d'jà marre mais t'as pas vécu assez, ouais, n'en parle pas si t'as pas vécu la scène, hey Ta vie est sens dessus dessous, ton compte n'a jamais vu tes sous Dans la vie, tout a un prix mais tu ne tiens pas le coup L'État nous tient par les couilles, il faut que les gens soient à l'écoute T'es même pas encore bé-tom, t'es qu'un numéro d'écrou Ça paraît loin mais tout ça, c'est dans la tête Et ça vaut pas la peine de s'attarder sur des choses bêtes Prends pas trop ton temps avant de régler tes dettes Ouais, si ta pendule interne est déréglée, t'es dead Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Tout ça, c'est dans la tête Pourquoi ta conscience te maltraite ? Qu'est-ce qui te différencie d'un athlète ? Faut te battre contre toi-même Dans ce monde, c'est dur de rester soi-même Mais si t'es pas toi-même, t'es personne Faut faire des Washington et des Jefferson Mais si tu restes pas toi-même, t'es personne</t>
         </is>
       </c>
     </row>
@@ -1988,12 +1988,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Deux comme toi</t>
+          <t>Dis-leur</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Tu peux avoir le monde si c'est bien demandé mais maman m'a dit C'est pas bien de quémander Tu fais les choses à ta façon, ils veulent te réprimander, c'est grâce à GTA si j'maîtrise l'anglais J'vais les ignorer, j'ai fermé tous les onglets, ils ont le seum, je n'accepte pas leurs invit' C'est tous des clones, ouais, c'est tous des zombies, leur caractère est limité comme un tweet Ça y est, t'en as pas marre de côtoyer la 'sère ? Surtout que la tristesse dure le temps d'une averse Faut rattraper l'retard, remettre les pendules à l'heure, surtout que le bonheur dure le temps du malheur Ils pouvaient pas me voir en face, ils m'ont tourné le dos, maintenant, je prends du cash même pour les journées repos J'ai tourné la page mais c'est resté dans ma tête, je ne ferai pas l'album ou la tournée de trop Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Tu te plains de ta situation mais tu passes tes journées à rêvasser devant la télé Un cauchemar éveillé, j'en vois pas l'intérêt, nan, tu vis pas, tu fais d'la figuration, ouais Et tu te plains de ta situation mais tu choisis ton destin c'est de l'automutilation T'en as d'jà marre mais t'as pas vécu assez, ouais, n'en parle pas si t'as pas vécu la scène, hey Ta vie est sens dessus dessous, ton compte n'a jamais vu tes sous Dans la vie, tout a un prix mais tu ne tiens pas le coup L'État nous tient par les couilles, il faut que les gens soient à l'écoute T'es même pas encore bé-tom, t'es qu'un numéro d'écrou Ça paraît loin mais tout ça, c'est dans la tête Et ça vaut pas la peine de s'attarder sur des choses bêtes Prends pas trop ton temps avant de régler tes dettes Ouais, si ta pendule interne est déréglée, t'es dead Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Pour eux, t'as pas la gueule de l'emploi, n'essaye même pas d'leur ressembler Y en a pas deux comme toi, tu peux avoir le monde si c'est bien demandé Tout ça, c'est dans la tête Pourquoi ta conscience te maltraite ? Qu'est-ce qui te différencie d'un athlète ? Faut te battre contre toi-même Dans ce monde, c'est dur de rester soi-même Mais si t'es pas toi-même, t'es personne Faut faire des Washington et des Jefferson Mais si tu restes pas toi-même, t'es personne</t>
+          <t>T'en a pas marre de menacer ? Il sera temps que tu passes à l'action T'as pas retenu la leçon ? Tu vas finir par me lasser Deuspi, deuspi, j'ai tout lâcher Mais t'es revenue vers moi On a pris les mêmes, on l'a refait Le sexe fait perdre la mémoire La douleur fait perdre les sentiments Donc difficile que je m'émoie Et moi, j'm'aime plus que toi, t'auras beau donner tout c'que t'as Que des disputes et des reproches On va jamais finir au top Nombres d'insultes dans la même phrase On a battu tous les records J'ai révisé, j'connais toutes les parties d'ton anatomie Mais t'as fait la meuf, maintenant tous mes reufs te traitent comme une inconnue T'as voulu m'entuber, bébé, j'suis pire que rancunier On peut plus reculer, dis leur, on peut plus reculer Dis leur, dis leur, dis leur, dis leur, que j'suis tellement sombre Depuis qu'je sais que ton intention n'était que mensongère Ma tristesse est contagieuse et même la Terre en pleure N'ose même pas songer À ce qu'on prenne de l'ampleur Dis leur, dis leur, dis leur, dis leur, que j'suis tellement sombre Depuis qu'je sais que ton intention n'était que mensongère Ma colère est contagieuse et même la Terre en tremble N'ose même pas songer À ce qu'on se remette ensembles J'ai perdu la vue pour tes beaux yeux Tout est devenu bressom Le temps passe, je retiens les leçons Maintenant les neus-je m'appellent Monsieur On a jamais finis au top J'compte plus le nombres de fois Qu'à cause de toi De tes histoires J'ai faillis finir au post Bien sûr, j'respecte toujours ta mif' Même si tu changes de continent J'fais abstraction d'mes sentiments Comme du draille, je l'ai tamise Ne m'attends pas, j'fais mes valises Qu'est-ce que t'as pas fais pour le khalis ? Au moins, j'aurai dit c'que j'ai à dire Avant qu'la balle me neutralise J'ai révisé, j'connais toutes les parties d'ton anatomie Mais t'as fait la meuf, maintenant tous mes reufs te traitent comme une inconnue T'as voulu m'entuber, bébé, j'suis pire que rancunier On peut plus reculer, dis leur, on peut plus reculer Dis leur, dis leur, dis leur, dis leur, que j'suis tellement sombre Depuis qu'je sais que ton intention n'était que mensongère Ma tristesse est contagieuse et même la Terre en pleure N'ose même pas songer À ce qu'on prenne de l'ampleur Dis leur, dis leur, dis leur, dis leur, que j'suis tellement sombre Depuis qu'je sais que ton intention n'était que mensongère Ma colère est contagieuse et même la Terre en tremble N'ose même pas songer À ce qu'on se remette ensembles</t>
         </is>
       </c>
     </row>
@@ -2005,12 +2005,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Dis-leur</t>
+          <t>DLC</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>T'en a pas marre de menacer ? Il sera temps que tu passes à l'action T'as pas retenu la leçon ? Tu vas finir par me lasser Deuspi, deuspi, j'ai tout lâcher Mais t'es revenue vers moi On a pris les mêmes, on l'a refait Le sexe fait perdre la mémoire La douleur fait perdre les sentiments Donc difficile que je m'émoie Et moi, j'm'aime plus que toi, t'auras beau donner tout c'que t'as Que des disputes et des reproches On va jamais finir au top Nombres d'insultes dans la même phrase On a battu tous les records J'ai révisé, j'connais toutes les parties d'ton anatomie Mais t'as fait la meuf, maintenant tous mes reufs te traitent comme une inconnue T'as voulu m'entuber, bébé, j'suis pire que rancunier On peut plus reculer, dis leur, on peut plus reculer Dis leur, dis leur, dis leur, dis leur, que j'suis tellement sombre Depuis qu'je sais que ton intention n'était que mensongère Ma tristesse est contagieuse et même la Terre en pleure N'ose même pas songer À ce qu'on prenne de l'ampleur Dis leur, dis leur, dis leur, dis leur, que j'suis tellement sombre Depuis qu'je sais que ton intention n'était que mensongère Ma colère est contagieuse et même la Terre en tremble N'ose même pas songer À ce qu'on se remette ensembles J'ai perdu la vue pour tes beaux yeux Tout est devenu bressom Le temps passe, je retiens les leçons Maintenant les neus-je m'appellent Monsieur On a jamais finis au top J'compte plus le nombres de fois Qu'à cause de toi De tes histoires J'ai faillis finir au post Bien sûr, j'respecte toujours ta mif' Même si tu changes de continent J'fais abstraction d'mes sentiments Comme du draille, je l'ai tamise Ne m'attends pas, j'fais mes valises Qu'est-ce que t'as pas fais pour le khalis ? Au moins, j'aurai dit c'que j'ai à dire Avant qu'la balle me neutralise J'ai révisé, j'connais toutes les parties d'ton anatomie Mais t'as fait la meuf, maintenant tous mes reufs te traitent comme une inconnue T'as voulu m'entuber, bébé, j'suis pire que rancunier On peut plus reculer, dis leur, on peut plus reculer Dis leur, dis leur, dis leur, dis leur, que j'suis tellement sombre Depuis qu'je sais que ton intention n'était que mensongère Ma tristesse est contagieuse et même la Terre en pleure N'ose même pas songer À ce qu'on prenne de l'ampleur Dis leur, dis leur, dis leur, dis leur, que j'suis tellement sombre Depuis qu'je sais que ton intention n'était que mensongère Ma colère est contagieuse et même la Terre en tremble N'ose même pas songer À ce qu'on se remette ensembles</t>
+          <t>-Crew, toujours la même, rien n'a changé, toujours la même Toujours les mêmes ons-s, toujours la même cons' Ouais, toujours les mêmes têtes Seine Zoo, Don dada, L', Saboteur gang Hugz, fuego, fuego J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite</t>
         </is>
       </c>
     </row>
@@ -2022,12 +2022,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>DLC</t>
+          <t>Don ZooZoo</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>-Crew, toujours la même, rien n'a changé, toujours la même Toujours les mêmes ons-s, toujours la même cons' Ouais, toujours les mêmes têtes Seine Zoo, Don dada, L', Saboteur gang Hugz, fuego, fuego J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite</t>
+          <t>Sisi Philly Flingo Zerzer Hugz lets go Ya trop dputes dans ce monde, au féminin comme au masculin des putes Il agit comme un chien et ce bâtard se croit humain Ok, ouais ya trop dputes dans cmonde, au féminin comme au masculin Cest qui ? Et quand tas tout perdu tu sais vraiment à quoi tu tiens Ouais cest comme ça Trop de supercheries, j'les ponctionne Avec moi voyelles consonnes fonctionnent Ils attendent que jles valide, jsuis un sponsor J'suis dans les 22, j'suis dans l'11 d'or Malcom X derrière mon stor 24 sur 7 non stop Guette les vines de mon front sortent Trop d'putes qui trichent, je sais reconnaître les bluffs Trouver les plus p'tits prix comme au duty free Maintenant j'connecte les plugs, appelle moi la multiprise Ceux qui ne s'en sortent pas sans michtonner devraient être emprisonnés Big Flingue aka grand pistolet Fuck les p'tites tains-p' et les gens pistonnés Quand tu fais mieux queux, ils te critiquent bitch Tu veux casser ton tête, tentends clic clic bitch no Que des cauchemars, pas de dream team bitch Chez nous, shit, weed pas de chic types Ya celui qui parle, celui qui tire hey Cest no limit, no future whoo Choisi bien ceux qui tentourent whoo tauras déjà fait le plus dur hey Sappé comme Peter Griffin En bas d'ton bat, j'péta l'Wi-fi Quand ma salive sera acide, là jpourrais faire du lèche vitrine Ok Ya trop dputes dans ce monde, au féminin comme au masculin des putes Il agit comme un chien et ce bâtard se croit humain Ok, ouais ya trop dputes dans cmonde, au féminin comme au masculin Cest qui ? Et quand tas tout perdu tu sais vraiment à quoi tu tiens La plupart des gens cest des putas Si tes pas leur pimp, ils técoutent pas Pas de coups de foudre, que des coups d'tas' Jentends que des flows qui découpent pas, et tous leurs principes cest des foutaises Jpeux te faire un coup dtraitre sur un coup dtête Pas dpeace and love que des coups dserpe Chez nous que des flows qui découpent sec Don Dada pas d'foutaises Inch'allah plus tard dans les boutiques L' comme Wu Tang, pratique le marathon pas l'footing J'en suis seulement au niveau 2 mais ils trouvent déjà que j'suis trop deuss Dans c'rap FR j'suis important comment ? comme Dubaï pour une michtoneuse Zer2 Washington Philadelphia Flingue Pennsylvanie Carte de crédit comme joujou, Seine Dada Don Zoozoo Y'a trop d'putes dans c'monde au féminin comme au masculin Hein, des démons avec des masques humains let's get it Ya trop dputes dans ce monde, au féminin comme au masculin des putes Il agit comme un chien et ce bâtard se croit humain Ok, ouais ya trop dputes dans cmonde, au féminin comme au masculin Cest qui ? Et quand tas tout perdu tu sais vraiment à quoi tu tiens Ouais cest comme ça2</t>
         </is>
       </c>
     </row>
@@ -2039,12 +2039,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Don ZooZoo</t>
+          <t>Double turbo</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Sisi Philly Flingo Zerzer Hugz lets go Ya trop dputes dans ce monde, au féminin comme au masculin des putes Il agit comme un chien et ce bâtard se croit humain Ok, ouais ya trop dputes dans cmonde, au féminin comme au masculin Cest qui ? Et quand tas tout perdu tu sais vraiment à quoi tu tiens Ouais cest comme ça Trop de supercheries, j'les ponctionne Avec moi voyelles consonnes fonctionnent Ils attendent que jles valide, jsuis un sponsor J'suis dans les 22, j'suis dans l'11 d'or Malcom X derrière mon stor 24 sur 7 non stop Guette les vines de mon front sortent Trop d'putes qui trichent, je sais reconnaître les bluffs Trouver les plus p'tits prix comme au duty free Maintenant j'connecte les plugs, appelle moi la multiprise Ceux qui ne s'en sortent pas sans michtonner devraient être emprisonnés Big Flingue aka grand pistolet Fuck les p'tites tains-p' et les gens pistonnés Quand tu fais mieux queux, ils te critiquent bitch Tu veux casser ton tête, tentends clic clic bitch no Que des cauchemars, pas de dream team bitch Chez nous, shit, weed pas de chic types Ya celui qui parle, celui qui tire hey Cest no limit, no future whoo Choisi bien ceux qui tentourent whoo tauras déjà fait le plus dur hey Sappé comme Peter Griffin En bas d'ton bat, j'péta l'Wi-fi Quand ma salive sera acide, là jpourrais faire du lèche vitrine Ok Ya trop dputes dans ce monde, au féminin comme au masculin des putes Il agit comme un chien et ce bâtard se croit humain Ok, ouais ya trop dputes dans cmonde, au féminin comme au masculin Cest qui ? Et quand tas tout perdu tu sais vraiment à quoi tu tiens La plupart des gens cest des putas Si tes pas leur pimp, ils técoutent pas Pas de coups de foudre, que des coups d'tas' Jentends que des flows qui découpent pas, et tous leurs principes cest des foutaises Jpeux te faire un coup dtraitre sur un coup dtête Pas dpeace and love que des coups dserpe Chez nous que des flows qui découpent sec Don Dada pas d'foutaises Inch'allah plus tard dans les boutiques L' comme Wu Tang, pratique le marathon pas l'footing J'en suis seulement au niveau 2 mais ils trouvent déjà que j'suis trop deuss Dans c'rap FR j'suis important comment ? comme Dubaï pour une michtoneuse Zer2 Washington Philadelphia Flingue Pennsylvanie Carte de crédit comme joujou, Seine Dada Don Zoozoo Y'a trop d'putes dans c'monde au féminin comme au masculin Hein, des démons avec des masques humains let's get it Ya trop dputes dans ce monde, au féminin comme au masculin des putes Il agit comme un chien et ce bâtard se croit humain Ok, ouais ya trop dputes dans cmonde, au féminin comme au masculin Cest qui ? Et quand tas tout perdu tu sais vraiment à quoi tu tiens Ouais cest comme ça2</t>
+          <t>Eh, eh-eh Wouh-wouh, wouh Zer2 Eh Tu connais t'façon Uh-huh -Crew, Seine Zoo, Saboteur Gang Hugz Wouh-wouh, wouh Yeah Si ça tenait qu'à moi Eh J'aurais pas d'taf mais j'me paierai chaque moi Uh-huh Double turbo, quatre pots d'échappements Eh Double canon, des morceaux, des fragments Wouh-wouh, wouh De quoi choquer ta bande Si ça tenait qu'à moi Eh On resterait soudés comme des siamois Uh-huh Nos soldats seraient armer que de savoir Eh Un monde imaginaire que j'suis pas seul à voir Wouh-wouh, wouh Voir, voir Chez nous l'appétit vient en fumant Smoke, smoke J'me barre à l'étranger le temps d'un confinement Salam Quand la vie n'a pas de goût, la weed en condiment Ceux qui voulaient changer les choses, combien sont vivant? Eh, eh Quand y a trop d'enjeux, ça devient confidentiel Wouh On vit dans cette putain de mise en scène Okay Ils sont trop à l'ancienne, n'écoute pas ce qu'ils t'enseignent Jamais, jamais Pour eux c'est normal que tout un continent saigne Goddamn On fait la guerre mais à la base on s'aimait Eh Combien de cadavres sous le ciment? Uh-huh En France depuis l'enfance on nous apprend Eh Vit dans la modestie et meurt en silence Uh-huh Au collège le CPE faisait le sévère Wouh J'l'écoute pas, j'vois qu'un bâtard qui remue ses lèvres Hahaha J'dépense tant que je peux m'le permettre, avant c'putain d'repos éternel Si ça tenait qu'à moi Eh J'aurais pas d'taffe mais j'me paierai chaque moi Uh-huh Double turbo, quatre pots d'échappements Eh Double canon, des morceaux, des fragments Wouh-wouh, wouh De quoi choquer ta bande Si ça tenait qu'à moi Eh On resterait souder comme des siamois Uh-huh Nos soldats seraient armer que de savoir Eh Un monde imaginaire que j'suis pas seul à voir Wouh-wouh, wouh Voir, voir T'es rien tant que tu n'as pas ton bout de terrain Non Et ton foyer construit à la force de tes mains Okay Chaque fois que tu manques une opportunité Ouais Fait que tu retires le pain d'la bouche de quelqu'un Ouh, ouh L'état veut me punir parce que je suis moi-même Long, longtemps que j'ai compris qu'ils ne veulent plus de nous No, no J'en ai plus rien à foutre des valeurs citoyennes Le loup mange les porcs et le chassuer tue le loup Wouh, wouh J'suis dans le studio, booth, j'avance, tu suis le mouv' On cuisine, tu le bouffes, fait pas la fine bouche On était tous poser chez Pouch, à l'époque on faisaient les poches de tout ceux qui faisaient les fous Vu que personne répondait, on à péter la porte Ici bas y a que mon stylo qui m'a prêter main forte J'ai fait l'effort de rester vrai et j'ai perdu plus d'un pote Y a que la miff qui m'importe, eh Premier d'la classe envie le mauvais élève Eh Il doit taffer dur le très devenu célèbre Uh-huh Ça fait du bien de savoir que t'as vécu tes rêves Eh Et qu'en plus avec ça t'es revenu Uh-huh Au collège le CPE faisait le sévère Wouh J'l'écoute pas, j'vois qu'un bâtard qui remue ses lèvres Hahaha J'dépense tant que je peux m'le permettre, avant c'putain d'repos éternel Si ça tenait qu'à moi Eh J'aurais pas d'taffe mais j'me paierai chaque moi Uh-huh Double turbo, quatre pots d'échappements Eh Double canon, des morceaux, des fragments Wouh-wouh, wouh De quoi choquer ta bande Si ça tenait qu'à moi Eh On resterait souder comme des siamois Uh-huh Nos soldats seraient armer que de savoir Eh Un monde imaginaire que j'suis pas seul à voir Wouh-wouh, wouh Voir, voir Eh Uh-huh Eh Wouh-wouh, wouh</t>
         </is>
       </c>
     </row>
@@ -2056,12 +2056,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Double turbo</t>
+          <t>Doucement</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Eh, eh-eh Wouh-wouh, wouh Zer2 Eh Tu connais t'façon Uh-huh -Crew, Seine Zoo, Saboteur Gang Hugz Wouh-wouh, wouh Yeah Si ça tenait qu'à moi Eh J'aurais pas d'taf mais j'me paierai chaque moi Uh-huh Double turbo, quatre pots d'échappements Eh Double canon, des morceaux, des fragments Wouh-wouh, wouh De quoi choquer ta bande Si ça tenait qu'à moi Eh On resterait soudés comme des siamois Uh-huh Nos soldats seraient armer que de savoir Eh Un monde imaginaire que j'suis pas seul à voir Wouh-wouh, wouh Voir, voir Chez nous l'appétit vient en fumant Smoke, smoke J'me barre à l'étranger le temps d'un confinement Salam Quand la vie n'a pas de goût, la weed en condiment Ceux qui voulaient changer les choses, combien sont vivant? Eh, eh Quand y a trop d'enjeux, ça devient confidentiel Wouh On vit dans cette putain de mise en scène Okay Ils sont trop à l'ancienne, n'écoute pas ce qu'ils t'enseignent Jamais, jamais Pour eux c'est normal que tout un continent saigne Goddamn On fait la guerre mais à la base on s'aimait Eh Combien de cadavres sous le ciment? Uh-huh En France depuis l'enfance on nous apprend Eh Vit dans la modestie et meurt en silence Uh-huh Au collège le CPE faisait le sévère Wouh J'l'écoute pas, j'vois qu'un bâtard qui remue ses lèvres Hahaha J'dépense tant que je peux m'le permettre, avant c'putain d'repos éternel Si ça tenait qu'à moi Eh J'aurais pas d'taffe mais j'me paierai chaque moi Uh-huh Double turbo, quatre pots d'échappements Eh Double canon, des morceaux, des fragments Wouh-wouh, wouh De quoi choquer ta bande Si ça tenait qu'à moi Eh On resterait souder comme des siamois Uh-huh Nos soldats seraient armer que de savoir Eh Un monde imaginaire que j'suis pas seul à voir Wouh-wouh, wouh Voir, voir T'es rien tant que tu n'as pas ton bout de terrain Non Et ton foyer construit à la force de tes mains Okay Chaque fois que tu manques une opportunité Ouais Fait que tu retires le pain d'la bouche de quelqu'un Ouh, ouh L'état veut me punir parce que je suis moi-même Long, longtemps que j'ai compris qu'ils ne veulent plus de nous No, no J'en ai plus rien à foutre des valeurs citoyennes Le loup mange les porcs et le chassuer tue le loup Wouh, wouh J'suis dans le studio, booth, j'avance, tu suis le mouv' On cuisine, tu le bouffes, fait pas la fine bouche On était tous poser chez Pouch, à l'époque on faisaient les poches de tout ceux qui faisaient les fous Vu que personne répondait, on à péter la porte Ici bas y a que mon stylo qui m'a prêter main forte J'ai fait l'effort de rester vrai et j'ai perdu plus d'un pote Y a que la miff qui m'importe, eh Premier d'la classe envie le mauvais élève Eh Il doit taffer dur le très devenu célèbre Uh-huh Ça fait du bien de savoir que t'as vécu tes rêves Eh Et qu'en plus avec ça t'es revenu Uh-huh Au collège le CPE faisait le sévère Wouh J'l'écoute pas, j'vois qu'un bâtard qui remue ses lèvres Hahaha J'dépense tant que je peux m'le permettre, avant c'putain d'repos éternel Si ça tenait qu'à moi Eh J'aurais pas d'taffe mais j'me paierai chaque moi Uh-huh Double turbo, quatre pots d'échappements Eh Double canon, des morceaux, des fragments Wouh-wouh, wouh De quoi choquer ta bande Si ça tenait qu'à moi Eh On resterait souder comme des siamois Uh-huh Nos soldats seraient armer que de savoir Eh Un monde imaginaire que j'suis pas seul à voir Wouh-wouh, wouh Voir, voir Eh Uh-huh Eh Wouh-wouh, wouh</t>
+          <t>Hugz, t'es en feu sur celle-là Bébé, détends-toi, c'est un détournement C'est comment ? C'est comment ? Fais doucement Tu tires sur le joint jusqu'à l'étouffement Prends ton temps, prends ton temps, fais doucement Ton boule provoque des éboulements C'est comment ? C'est comment ? Fais doucement J'voulais te ramener, tu m'as dit Tout se vend Prends ton temps, prends ton temps, fais doucement Seul sur le boulevard, jamais la boule au ventre, t'as perdu ton rêve, moi, j'suis là pour le vendre Banane Seine Zoo en-d'ssous du coupe-vent, vas-y, fais doucement, poto, y a tout dedans Quantité, quantité mais de quoi tu te vantes ? Qualité, qualité, tu feras plus de ventes Mentir dans le buss' mais faut pas qu'tu te mentes, soit tu te sers, soit tu demandes On veut la mettre à ton gouvernement collabo, le sol est couvert de sang Quand tu parles au phone, igo, fais doucement, t'es fermé d'esprit, j'le dis ouvertement Je sens que la pression ne fait que ter-mon Plus y a du de-mon et plus j'ai le démon Besoin d'espace, j'agite les foules Fais doucement, bébé, même si t'es douce Je sens que la pression ne fait que ter-mon Plus y a du de-mon et plus j'ai le démon Besoin d'espace, j'agite les foules Bébé, fais doucement même si t'es douce Bébé, détends-toi, c'est un détournement C'est comment ? C'est comment ? Fais doucement Tu tires sur le joint jusqu'à l'étouffement Prends ton temps, prends ton temps, fais doucement Ton boule provoque des éboulements C'est comment ? C'est comment ? Fais doucement J'voulais te ramener, tu m'as dit Tout se vend Prends ton temps, prends ton temps, fais doucement T'assumes pas la boisson, petite corpulence, bébé, faut qu'tu danses, oublie tabou, prudence Autour de toi, la foule est de plus en plus dense, on est là pour durer comme l'accoutumance Je rêve, je rêve, je rêve, j'hallucine, tu roules mes joints et tu fais la cuisine Je rêve, je rêve, je rêve, j'hallucine, harcèlement, ouais, ton boule est abusif Fais doucement ou j'vais foutre le camp, j'vais foutre le camp s'tu fais pas doucement J'sais pas comment te le dire autrement tes formes débordent de ton accoutrement Tu connais mon blase, t'es bien renseignée, peut-être que tu taffes pour les renseignements T'as pris ta leçon, on peut rien t'enseigner, ouvert d'esprit et j'le dis fermement Je sens que la pression ne fait que ter-mon Plus y a du de-mon et plus j'ai le démon Besoin d'espace, j'agite les foules Fais doucement, bébé, même si t'es douce Je sens que la pression ne fait que ter-mon Plus y a du de-mon et plus j'ai le démon Besoin d'espace, j'agite les foules Bébé, fais doucement même si t'es douce Bébé, détends-toi, c'est un détournement C'est comment ? C'est comment ? Fais doucement Tu tires sur le joint jusqu'à l'étouffement Prends ton temps, prends ton temps, fais doucement Ton boule provoque des éboulements C'est comment ? C'est comment ? Fais doucement J'voulais te ramener, tu m'as dit Tout se vend Prends ton temps, prends ton temps, fais doucement</t>
         </is>
       </c>
     </row>
@@ -2073,12 +2073,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Doucement</t>
+          <t>Électron libre</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Hugz, t'es en feu sur celle-là Bébé, détends-toi, c'est un détournement C'est comment ? C'est comment ? Fais doucement Tu tires sur le joint jusqu'à l'étouffement Prends ton temps, prends ton temps, fais doucement Ton boule provoque des éboulements C'est comment ? C'est comment ? Fais doucement J'voulais te ramener, tu m'as dit Tout se vend Prends ton temps, prends ton temps, fais doucement Seul sur le boulevard, jamais la boule au ventre, t'as perdu ton rêve, moi, j'suis là pour le vendre Banane Seine Zoo en-d'ssous du coupe-vent, vas-y, fais doucement, poto, y a tout dedans Quantité, quantité mais de quoi tu te vantes ? Qualité, qualité, tu feras plus de ventes Mentir dans le buss' mais faut pas qu'tu te mentes, soit tu te sers, soit tu demandes On veut la mettre à ton gouvernement collabo, le sol est couvert de sang Quand tu parles au phone, igo, fais doucement, t'es fermé d'esprit, j'le dis ouvertement Je sens que la pression ne fait que ter-mon Plus y a du de-mon et plus j'ai le démon Besoin d'espace, j'agite les foules Fais doucement, bébé, même si t'es douce Je sens que la pression ne fait que ter-mon Plus y a du de-mon et plus j'ai le démon Besoin d'espace, j'agite les foules Bébé, fais doucement même si t'es douce Bébé, détends-toi, c'est un détournement C'est comment ? C'est comment ? Fais doucement Tu tires sur le joint jusqu'à l'étouffement Prends ton temps, prends ton temps, fais doucement Ton boule provoque des éboulements C'est comment ? C'est comment ? Fais doucement J'voulais te ramener, tu m'as dit Tout se vend Prends ton temps, prends ton temps, fais doucement T'assumes pas la boisson, petite corpulence, bébé, faut qu'tu danses, oublie tabou, prudence Autour de toi, la foule est de plus en plus dense, on est là pour durer comme l'accoutumance Je rêve, je rêve, je rêve, j'hallucine, tu roules mes joints et tu fais la cuisine Je rêve, je rêve, je rêve, j'hallucine, harcèlement, ouais, ton boule est abusif Fais doucement ou j'vais foutre le camp, j'vais foutre le camp s'tu fais pas doucement J'sais pas comment te le dire autrement tes formes débordent de ton accoutrement Tu connais mon blase, t'es bien renseignée, peut-être que tu taffes pour les renseignements T'as pris ta leçon, on peut rien t'enseigner, ouvert d'esprit et j'le dis fermement Je sens que la pression ne fait que ter-mon Plus y a du de-mon et plus j'ai le démon Besoin d'espace, j'agite les foules Fais doucement, bébé, même si t'es douce Je sens que la pression ne fait que ter-mon Plus y a du de-mon et plus j'ai le démon Besoin d'espace, j'agite les foules Bébé, fais doucement même si t'es douce Bébé, détends-toi, c'est un détournement C'est comment ? C'est comment ? Fais doucement Tu tires sur le joint jusqu'à l'étouffement Prends ton temps, prends ton temps, fais doucement Ton boule provoque des éboulements C'est comment ? C'est comment ? Fais doucement J'voulais te ramener, tu m'as dit Tout se vend Prends ton temps, prends ton temps, fais doucement</t>
+          <t>Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Ouais Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Jamais, jamais, jamais, jamais Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Ouais Électron libre qu'on essaie de calr dans la file File, file Suivr les ordres ne m'a jamais vraiment rien appris Jamais, jamais, jamais, jamais 3.14 scellé, minuit, j'prends le volant Libre dans la foulée, rouler, rouler Ce monde est violent, ma ville l'illustre assez souvent Beaucoup pensent à se sauver, rouler, rouler Et je n'fais que ça, j'bouge au studio quelques fois Met sur beat les dièses que j'vois, seul, taffer rend fier de soi Ouais, j'te parle de tout c'que j'vois, tout ce dont les rêves s'éloignent Cette jeune mère qu'est presque à poil dans la rue malgré le froid J'rêve d'un monde beaucoup moins vieux jeu, du respect pour toutes les feumeus Pas d'diff' entre feu-js et rebeus, comme dans l'squad un jour, si Dieu veut J'mate dehors, j'me dis qu'en deux-deux, tu dors où les oiseaux chient Dans ce monde, j'envie les masochistes car seuls eux peuvent être heureux, hey Hey Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Ouais Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Jamais, jamais, jamais, jamais Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Ouais Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Pas né pour suivre les ordres Hein, hein, nope, ni même pour les donner Nan, nan On a pas choisi c'décor No, j'ai la flemme de le rénover Le monde est à nous, est à vous, est à tous, la joie dans le stade, j'ai goûté la p'louse Hey 'teille de champagne dans la foule j'éclabousse, si j'me tourne les pouces, c'est pour compter le flouse L'oseille, les femmes et la santé d'abord Hey, j'reste focus sur les plans qu'j'élabore Hey-oh, hey-oh, hey-oh, hey-oh, la bonne carte peut changer la donne Nos rents-pa ont charbonné, ouais, nous-même, on a donné On est restés longtemps dans la rue à zoner, ouais, beaucoup trop d'erreurs à gommer Fait longtemps que tu t'es pas fait gauler, ouais, et c'qu'on a bâti, frère, on l'a pas volé On court tous après la money, ouais, tout le squad a croqué On est débrouillards comme tous ceux qui naissent pauvres, pas l'temps d'être mesquin On construit nos propres prisons comme Esco, pour le reste, on s'en remet au destin Hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Besoin de rien d'autre quand t'es là Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Jamais, jamais, jamais, jamais Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Besoin de rien d'autre quand t'es là Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Hey Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh</t>
         </is>
       </c>
     </row>
@@ -2090,12 +2090,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Électron libre</t>
+          <t>En attendant Seine Zoo #2</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Ouais Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Jamais, jamais, jamais, jamais Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Ouais Électron libre qu'on essaie de calr dans la file File, file Suivr les ordres ne m'a jamais vraiment rien appris Jamais, jamais, jamais, jamais 3.14 scellé, minuit, j'prends le volant Libre dans la foulée, rouler, rouler Ce monde est violent, ma ville l'illustre assez souvent Beaucoup pensent à se sauver, rouler, rouler Et je n'fais que ça, j'bouge au studio quelques fois Met sur beat les dièses que j'vois, seul, taffer rend fier de soi Ouais, j'te parle de tout c'que j'vois, tout ce dont les rêves s'éloignent Cette jeune mère qu'est presque à poil dans la rue malgré le froid J'rêve d'un monde beaucoup moins vieux jeu, du respect pour toutes les feumeus Pas d'diff' entre feu-js et rebeus, comme dans l'squad un jour, si Dieu veut J'mate dehors, j'me dis qu'en deux-deux, tu dors où les oiseaux chient Dans ce monde, j'envie les masochistes car seuls eux peuvent être heureux, hey Hey Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Ouais Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Jamais, jamais, jamais, jamais Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Ouais Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Pas né pour suivre les ordres Hein, hein, nope, ni même pour les donner Nan, nan On a pas choisi c'décor No, j'ai la flemme de le rénover Le monde est à nous, est à vous, est à tous, la joie dans le stade, j'ai goûté la p'louse Hey 'teille de champagne dans la foule j'éclabousse, si j'me tourne les pouces, c'est pour compter le flouse L'oseille, les femmes et la santé d'abord Hey, j'reste focus sur les plans qu'j'élabore Hey-oh, hey-oh, hey-oh, hey-oh, la bonne carte peut changer la donne Nos rents-pa ont charbonné, ouais, nous-même, on a donné On est restés longtemps dans la rue à zoner, ouais, beaucoup trop d'erreurs à gommer Fait longtemps que tu t'es pas fait gauler, ouais, et c'qu'on a bâti, frère, on l'a pas volé On court tous après la money, ouais, tout le squad a croqué On est débrouillards comme tous ceux qui naissent pauvres, pas l'temps d'être mesquin On construit nos propres prisons comme Esco, pour le reste, on s'en remet au destin Hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Besoin de rien d'autre quand t'es là Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Jamais, jamais, jamais, jamais Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Besoin de rien d'autre quand t'es là Électron libre qu'on essaie de caler dans la file File, file Suivre les ordres ne m'a jamais vraiment rien appris Hey Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Besoin de rien d'autre quand t'es là Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh Hey-oh, hey-oh, hey-oh, hey-oh</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -2107,12 +2107,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>En attendant Seine Zoo #2</t>
+          <t>Esquive suprême</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
+          <t>Ouais, allô ! Tranquille ou quoi, poto ? Ah, le son ? Nan, j'ai même pas gratté... J'te jure, j'ai pas eu le temps. Y'a l'taff, tout ça, c'est chaud. Ouais mais t'inquiète, t'inquiète, vas-y... En plus, j'te jure, en c'moment, j'ai plus d'inspi', j'ai rien du tout, j'ai pas d'beat pour le studio... Chaque MC voulant feater se découvre des talents d'lover J'reste fidèle au tro-mé, j'boycotte Land Rover Dans l'Hip-Hop, ça pue, j'rappe mais j'me porte pas garant d'l'odeur Voyant les gars d'avance se bagarrant j'avance comme 40 moteurs J'les vois bavardant, guette si c'est pas navrant, généreux soit disant Mais rien qu'ça parle d'argent, c'est chiant qu'ces wacks vénéneux soient vivants Vas-y laisse tenter un dièse, j'vis aller chanter un 16 Dans l'peu-Ra, t'es inconnu, j'peux t'appeler 31 On est des hommes beaufs qui veulent des femmes à fricpuis des fanatiques On veut des tas d'articles dans l'journal car les gars d'la clique En ont marre des wacks qui roulent les mots, c'est trop facile À paumer des mots, mon flow fascine Des phases de malades et les faux s'vaccinent Les quettes-pla arrondissent le mois, garantissent un bon glissement À bon prix se vendent autour des arrondissements J'lache des vilains couplets, chouf J'ai une vie à couper l'souffle Toi, tu veux rapper mais tes darons disent Nan.</t>
         </is>
       </c>
     </row>
@@ -2124,12 +2124,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Esquive suprême</t>
+          <t>Fast life</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Ouais, allô ! Tranquille ou quoi, poto ? Ah, le son ? Nan, j'ai même pas gratté... J'te jure, j'ai pas eu le temps. Y'a l'taff, tout ça, c'est chaud. Ouais mais t'inquiète, t'inquiète, vas-y... En plus, j'te jure, en c'moment, j'ai plus d'inspi', j'ai rien du tout, j'ai pas d'beat pour le studio... Chaque MC voulant feater se découvre des talents d'lover J'reste fidèle au tro-mé, j'boycotte Land Rover Dans l'Hip-Hop, ça pue, j'rappe mais j'me porte pas garant d'l'odeur Voyant les gars d'avance se bagarrant j'avance comme 40 moteurs J'les vois bavardant, guette si c'est pas navrant, généreux soit disant Mais rien qu'ça parle d'argent, c'est chiant qu'ces wacks vénéneux soient vivants Vas-y laisse tenter un dièse, j'vis aller chanter un 16 Dans l'peu-Ra, t'es inconnu, j'peux t'appeler 31 On est des hommes beaufs qui veulent des femmes à fricpuis des fanatiques On veut des tas d'articles dans l'journal car les gars d'la clique En ont marre des wacks qui roulent les mots, c'est trop facile À paumer des mots, mon flow fascine Des phases de malades et les faux s'vaccinent Les quettes-pla arrondissent le mois, garantissent un bon glissement À bon prix se vendent autour des arrondissements J'lache des vilains couplets, chouf J'ai une vie à couper l'souffle Toi, tu veux rapper mais tes darons disent Nan.</t>
+          <t>15h du mat', j'me réveille car mon téléphone sonne J'ai la gaule comme tous les matins , j'peux pas dompter mes hormones J'ai passé ma nuit précédente avec une miss élégante Jamais fatiguée qui agissait selon mes préférences J'rêve de quitter la France et faire la fête en vacances Bref, je check mon téléphone j'ai des appels en absence Mec, j'ai au moins 10 messages vocaux XXX XXX avec des tiss-mé à gogo ! J'ferai pas l'Salam Aleikoum On côtoiera pas la galère Mais avant tout j'passe voir ma mère qui est à l'hosto Si t'es pas costaud, surtout si t'es basané lai-laisse tomber T'auras jamais une vie d'rêve à l'eau d'rose Faut que tu sâches que ma beuh vient de Jamaïque Et mon chit à fumer c'est Marocain, là j'arrive Si tu t'interroges sur mon retard Sache que ma ponctualité n'est pas au point A la ligne Framal et Crapo, on mène tous la Fast Life Nekfeu et Mekhra, on mène tous la Fast Life Quand j'parle du ghetto, on mène tous la Fast Life XXXXX et Mamadou, on mène tous la Fast Life Deen et Jazzy Bazz, on mène tous la Fast Life Alpha Fonky Flav', on mène tous la Fast Life Dizme, Eff Gee, on mène tous la Fast Life Neefa et Margue', on mène tous la Fast Life ...</t>
         </is>
       </c>
     </row>
@@ -2141,12 +2141,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Fast life</t>
+          <t>FEUX ARRIERES</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>15h du mat', j'me réveille car mon téléphone sonne J'ai la gaule comme tous les matins , j'peux pas dompter mes hormones J'ai passé ma nuit précédente avec une miss élégante Jamais fatiguée qui agissait selon mes préférences J'rêve de quitter la France et faire la fête en vacances Bref, je check mon téléphone j'ai des appels en absence Mec, j'ai au moins 10 messages vocaux XXX XXX avec des tiss-mé à gogo ! J'ferai pas l'Salam Aleikoum On côtoiera pas la galère Mais avant tout j'passe voir ma mère qui est à l'hosto Si t'es pas costaud, surtout si t'es basané lai-laisse tomber T'auras jamais une vie d'rêve à l'eau d'rose Faut que tu sâches que ma beuh vient de Jamaïque Et mon chit à fumer c'est Marocain, là j'arrive Si tu t'interroges sur mon retard Sache que ma ponctualité n'est pas au point A la ligne Framal et Crapo, on mène tous la Fast Life Nekfeu et Mekhra, on mène tous la Fast Life Quand j'parle du ghetto, on mène tous la Fast Life XXXXX et Mamadou, on mène tous la Fast Life Deen et Jazzy Bazz, on mène tous la Fast Life Alpha Fonky Flav', on mène tous la Fast Life Dizme, Eff Gee, on mène tous la Fast Life Neefa et Margue', on mène tous la Fast Life ...</t>
+          <t>J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte Toi, tu vois qu'mes feux arrières Tu vois qu'mes feux arrières Saboteur Records J'ai tout investi, bien labouré la terre, tous ces billets me font tourner la tête let's go Y a le taff, les sous qui viennent après, tout va de pair comme la guerre et la paix Il m'faut plus qu'un million et mes gars pareil, faut provoquer l'occas' et s'l'accaparer On fait pas le grossiste avec quatre barrettes, on fera pas d'affaires si t'es pas carré J'ai cramé des caisses comme un p'tit con ptit con, un ami décède, j'ai des frissons frissons J'vesqui les keufs, j'suis dans les buissons buisson, y a un tho-m' a péter, j'envoie les p'tits sauvages J'ai du rhum dans le breuvage, la même mentale du 9.3. à Beauval oh oui J'réécoute mes maps dans la gova let's guill, son à fond j'arrive en R à Total Y a le coupe-coupe, fait pas deffort, Stutt me dit coupe tout faut pas qu'ça foire On a fait les comptes, on a vendu a la foi, j'suis sur FIFA avec Eff on aime faire aléatoire oh oui On m'a dit fais belek à toi, fais belek aux gens, fais belek à qui tu racontes ta vie T'inquiètes, j'ai les idées claires, j'ai mis sur pause l'illégal mais j'ai toujours les contacts avides J'actionne, sur mon passage tous les klaxons, dégaine de mauvais garçon, bre-som comme un Jackson Personne, dans le noir ne maperçoit, solo, j'roule un perso et c'est là que jperforme Pleine forme, même si y a tout dans le pack son, c'est pour tous les tieksons de Paname jusqu'à Belfort Belles formes, te calcule pas si t'as pas les fonds, plus personne ne répond, quand s'agit d'faire un effort J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte, toi, tu vois qu'mes feux arrières J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte, toi, tu vois qu'mes feux arrières Le premier, à tirer, c'est souvent le dernier à tourner le dos On prépare ta future playlist, pendant que tu fais le beau J'ai encore du mal à retrouver la paix donc tu sais, j'mets gelato dans les bédos quand je saigne dans le cur, encore dans les bas-fonds de ma tête mais j'essaye De trouver le zen en moi, retrouver le frère en toi J'ai cherché la luz dans la pénombre, on sonne mais on s'présente pas Ride dans l'averse la nuit, essuie le sang quand c'est fini Pas les mêmes plav', mêmes bails, pas les mêmes démons de minuit Action entraîne réaction, pourquoi t'es chelou à chaque interaction ? T'étais pas là, t'as raté l'action, on est ensemble comme Paname et rap sombre T'sais qu'on traîne là où les rats sont, on a pris les munitions et les rations Qui le, qui le fait monter le ratio ? Zer2, tu connais, d't'façon J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte, toi, tu vois qu'mes feux arrières J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte, toi, tu vois qu'mes feux arrières</t>
         </is>
       </c>
     </row>
@@ -2158,12 +2158,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>FEUX ARRIERES</t>
+          <t>Focus</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte Toi, tu vois qu'mes feux arrières Tu vois qu'mes feux arrières Saboteur Records J'ai tout investi, bien labouré la terre, tous ces billets me font tourner la tête let's go Y a le taff, les sous qui viennent après, tout va de pair comme la guerre et la paix Il m'faut plus qu'un million et mes gars pareil, faut provoquer l'occas' et s'l'accaparer On fait pas le grossiste avec quatre barrettes, on fera pas d'affaires si t'es pas carré J'ai cramé des caisses comme un p'tit con ptit con, un ami décède, j'ai des frissons frissons J'vesqui les keufs, j'suis dans les buissons buisson, y a un tho-m' a péter, j'envoie les p'tits sauvages J'ai du rhum dans le breuvage, la même mentale du 9.3. à Beauval oh oui J'réécoute mes maps dans la gova let's guill, son à fond j'arrive en R à Total Y a le coupe-coupe, fait pas deffort, Stutt me dit coupe tout faut pas qu'ça foire On a fait les comptes, on a vendu a la foi, j'suis sur FIFA avec Eff on aime faire aléatoire oh oui On m'a dit fais belek à toi, fais belek aux gens, fais belek à qui tu racontes ta vie T'inquiètes, j'ai les idées claires, j'ai mis sur pause l'illégal mais j'ai toujours les contacts avides J'actionne, sur mon passage tous les klaxons, dégaine de mauvais garçon, bre-som comme un Jackson Personne, dans le noir ne maperçoit, solo, j'roule un perso et c'est là que jperforme Pleine forme, même si y a tout dans le pack son, c'est pour tous les tieksons de Paname jusqu'à Belfort Belles formes, te calcule pas si t'as pas les fonds, plus personne ne répond, quand s'agit d'faire un effort J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte, toi, tu vois qu'mes feux arrières J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte, toi, tu vois qu'mes feux arrières Le premier, à tirer, c'est souvent le dernier à tourner le dos On prépare ta future playlist, pendant que tu fais le beau J'ai encore du mal à retrouver la paix donc tu sais, j'mets gelato dans les bédos quand je saigne dans le cur, encore dans les bas-fonds de ma tête mais j'essaye De trouver le zen en moi, retrouver le frère en toi J'ai cherché la luz dans la pénombre, on sonne mais on s'présente pas Ride dans l'averse la nuit, essuie le sang quand c'est fini Pas les mêmes plav', mêmes bails, pas les mêmes démons de minuit Action entraîne réaction, pourquoi t'es chelou à chaque interaction ? T'étais pas là, t'as raté l'action, on est ensemble comme Paname et rap sombre T'sais qu'on traîne là où les rats sont, on a pris les munitions et les rations Qui le, qui le fait monter le ratio ? Zer2, tu connais, d't'façon J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte, toi, tu vois qu'mes feux arrières J'suis vrai avec toi mais tu fais d'la merde, tu marches de travers J'passe le feu rouge sous l'effet d'la verte, toi, tu vois qu'mes feux arrières</t>
+          <t>Eh yeah Eh yeah yeah Zer-2 hein, eh T'oublies pas quand tu dépannes un frère Ça ne vaut rien si tu n'es pas sincère On sort pas du même placenta mais ils étaient là pendant toutes mes années de galère De ta façon, de ma façon, ouais de toutes manières Pas peur de la police mais je redoute ma mère Nan le mauvais rap ne m'atteint pas Difficile de me capter, je voyage toute l'année, ouais On m'appelle Monsieur que depuis le platine, j'ai le meuseu Ils me détestaient comme si j'avais tartiné leur reusseu Quand t'as dit que la gloire ne t'affecterait pas, je sentais que tu mentais Pourtant on se connaît depuis l'époque des boucles d'oreilles aimantée Une équipe originale Mes gars me soutiennent comme ma ceinture abdominale Demande à Boogie Down, on sait faire de la monnaie depuis l'anonymat Hugz en copilote, ça roule l'antidote Mon corps est la machine, mon âme est le ventriloque Est-ce que tu vois la hype ? On est à l'antipode C'est souvent la jalousie qui anéantit l'Homme Un jour le karma vient te reprendre tous les bails que t'as pas donnés Pour toi c'est des gues-bla, tu jettes ton repas quand tu te sens ballonné Faut que tu tiennes le coup Je sais pourquoi tu baves parce que tu dors debout Seine Zoo, ces gars ils sortent d'où ? Tu secoues pas la tête sur les sons, tu te tords le cou C'est moi devant le mic, c'est moi qui fais la prod Toujours focus, je veux pas rater le coche Tranquillement, c'est qu'une annonce d'album Je récupère le ballon, je slalome Salam ou shalom, on repousse nos limites Les jaloux se jalonnent mais kiffent nos lyrics Pas b'soin de mobile, toute l'équipe se mobilise Quand j'suis avec eux même le temps s'immobilise Pas le temps pour vos bails, faut rester focus L'histoire de mon ascension, le premier opus Ouais, pas le temps pour vos bails, faut rester focus, ouais ouais J'ai roulé ma Marie-Jeanne dans une feuille de lotus1</t>
         </is>
       </c>
     </row>
@@ -2175,12 +2175,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Focus</t>
+          <t>Formatage erroné</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Eh yeah Eh yeah yeah Zer-2 hein, eh T'oublies pas quand tu dépannes un frère Ça ne vaut rien si tu n'es pas sincère On sort pas du même placenta mais ils étaient là pendant toutes mes années de galère De ta façon, de ma façon, ouais de toutes manières Pas peur de la police mais je redoute ma mère Nan le mauvais rap ne m'atteint pas Difficile de me capter, je voyage toute l'année, ouais On m'appelle Monsieur que depuis le platine, j'ai le meuseu Ils me détestaient comme si j'avais tartiné leur reusseu Quand t'as dit que la gloire ne t'affecterait pas, je sentais que tu mentais Pourtant on se connaît depuis l'époque des boucles d'oreilles aimantée Une équipe originale Mes gars me soutiennent comme ma ceinture abdominale Demande à Boogie Down, on sait faire de la monnaie depuis l'anonymat Hugz en copilote, ça roule l'antidote Mon corps est la machine, mon âme est le ventriloque Est-ce que tu vois la hype ? On est à l'antipode C'est souvent la jalousie qui anéantit l'Homme Un jour le karma vient te reprendre tous les bails que t'as pas donnés Pour toi c'est des gues-bla, tu jettes ton repas quand tu te sens ballonné Faut que tu tiennes le coup Je sais pourquoi tu baves parce que tu dors debout Seine Zoo, ces gars ils sortent d'où ? Tu secoues pas la tête sur les sons, tu te tords le cou C'est moi devant le mic, c'est moi qui fais la prod Toujours focus, je veux pas rater le coche Tranquillement, c'est qu'une annonce d'album Je récupère le ballon, je slalome Salam ou shalom, on repousse nos limites Les jaloux se jalonnent mais kiffent nos lyrics Pas b'soin de mobile, toute l'équipe se mobilise Quand j'suis avec eux même le temps s'immobilise Pas le temps pour vos bails, faut rester focus L'histoire de mon ascension, le premier opus Ouais, pas le temps pour vos bails, faut rester focus, ouais ouais J'ai roulé ma Marie-Jeanne dans une feuille de lotus1</t>
+          <t>x2 Les médias sont des commères, ils vendent du cauchemar pour qu'on ait peur d'affronter nos rêves Avoir son opinion, c'est la meilleure façon d'être honnête Ils s'font des frayeurs, veulent voir le seigneur annoncer l'tonnerre N'aie pas l'air étonné Comment prendre parti quand tu n'es pas au cur du conflit Difficile de mettre tout l'monde d'accord comme l'odeur du bon shit On a la même vie, les mêmes envies et les mêmes passions Si ça dégénère, c'est qu'les médias nous poussent à la défenestration Ils voudraient nous diviser alors qu'on a grandit ensemble Ils t'inculquent leurs principes en disant c'que t'as envie d'entendre Ils ralentissent l'entente ne parlent que de l'horreur des gens Et pour masquer l'odeur de sang, ils ont l'cigare en guise d'encens La vie nous a spoilé, on connaît tous la fin mais aucun de nous n'aura la chance de voir le film entier Seigneur, guide ma colère, j'suis pas le plus à plaindre mais j'apprécie tellement l'absence des problèmes financiers Qu'on en commet des délits relayés par des médias, c'est vert et sans gènes Demande à Mouss' ce que ça fait de prendre une peine exemplaire Si le mensonge est élégant, la vérité est-elle essentielle ? Enfermé dans une tour d'Ivoire car elle a la gueule d'éléphant-man x2 N'aie pas l'air étonné, mentalité bétonnée 2zer et R.O.N, le formatage est erroné x2 Les médias sont des commères, ils vendent du cauchemar pour qu'on ait peur d'affronter nos rêves Avoir son opinion, c'est la meilleure façon d'être honnête Ils s'font des frayeurs, veulent voir le seigneur annoncer l'tonnerre N'aie pas l'air étonné Face aux médias, tu t'électrocutes, tu laisses place au diable et dégaines ton cutter Tu t'laisses manipuler, vider de toute pudeur, stupeur Ça découpe des têtes sur le net et chaque scène te plombe les yeux Des fascistes pris sur le fait, blasphémant le nom de Dieu Y a pas que les mythos de la presse, y a ton veau-cer qui se rétrécit C'est répressif, tu prends parti sans savoir réfléchir, parfait bouc émissaire, ça t'arrange de nous détester Entre doutes et mystères, la vérité pourrait te blesser, le plus dur pour toi, serait d'reconnaître tes torts Mec t'es tordu, tu t'accordes de ber-tom dans des sombres décors et encore, sur le bien, c'est le mal qui l'emporte J'ai beau déblatérer mais l'interêt que j'te porte est quasiment mort Tu doutes de la margination, est-ce élémentaire ? C'n'est que les manches vers la presse Ne manque que l'imagination, puis, du coup, tu t'lances en plein dans la de-mer 2zer dis-leurs, simple message de paix, dans un élan de guerre, Ron x2 Les médias sont des commères, ils vendent du cauchemar pour qu'on ait peur d'affronter nos rêves Avoir son opinion, c'est la meilleure façon d'être honnête Ils s'font des frayeurs, veulent voir le seigneur annoncer l'tonnerre N'aie pas l'air étonné x2 N'aie pas l'air étonné, mentalité bétonnée 2zer et R.O.N, le formatage est erroné</t>
         </is>
       </c>
     </row>
@@ -2192,12 +2192,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Formatage erroné</t>
+          <t>Fraternité</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>x2 Les médias sont des commères, ils vendent du cauchemar pour qu'on ait peur d'affronter nos rêves Avoir son opinion, c'est la meilleure façon d'être honnête Ils s'font des frayeurs, veulent voir le seigneur annoncer l'tonnerre N'aie pas l'air étonné Comment prendre parti quand tu n'es pas au cur du conflit Difficile de mettre tout l'monde d'accord comme l'odeur du bon shit On a la même vie, les mêmes envies et les mêmes passions Si ça dégénère, c'est qu'les médias nous poussent à la défenestration Ils voudraient nous diviser alors qu'on a grandit ensemble Ils t'inculquent leurs principes en disant c'que t'as envie d'entendre Ils ralentissent l'entente ne parlent que de l'horreur des gens Et pour masquer l'odeur de sang, ils ont l'cigare en guise d'encens La vie nous a spoilé, on connaît tous la fin mais aucun de nous n'aura la chance de voir le film entier Seigneur, guide ma colère, j'suis pas le plus à plaindre mais j'apprécie tellement l'absence des problèmes financiers Qu'on en commet des délits relayés par des médias, c'est vert et sans gènes Demande à Mouss' ce que ça fait de prendre une peine exemplaire Si le mensonge est élégant, la vérité est-elle essentielle ? Enfermé dans une tour d'Ivoire car elle a la gueule d'éléphant-man x2 N'aie pas l'air étonné, mentalité bétonnée 2zer et R.O.N, le formatage est erroné x2 Les médias sont des commères, ils vendent du cauchemar pour qu'on ait peur d'affronter nos rêves Avoir son opinion, c'est la meilleure façon d'être honnête Ils s'font des frayeurs, veulent voir le seigneur annoncer l'tonnerre N'aie pas l'air étonné Face aux médias, tu t'électrocutes, tu laisses place au diable et dégaines ton cutter Tu t'laisses manipuler, vider de toute pudeur, stupeur Ça découpe des têtes sur le net et chaque scène te plombe les yeux Des fascistes pris sur le fait, blasphémant le nom de Dieu Y a pas que les mythos de la presse, y a ton veau-cer qui se rétrécit C'est répressif, tu prends parti sans savoir réfléchir, parfait bouc émissaire, ça t'arrange de nous détester Entre doutes et mystères, la vérité pourrait te blesser, le plus dur pour toi, serait d'reconnaître tes torts Mec t'es tordu, tu t'accordes de ber-tom dans des sombres décors et encore, sur le bien, c'est le mal qui l'emporte J'ai beau déblatérer mais l'interêt que j'te porte est quasiment mort Tu doutes de la margination, est-ce élémentaire ? C'n'est que les manches vers la presse Ne manque que l'imagination, puis, du coup, tu t'lances en plein dans la de-mer 2zer dis-leurs, simple message de paix, dans un élan de guerre, Ron x2 Les médias sont des commères, ils vendent du cauchemar pour qu'on ait peur d'affronter nos rêves Avoir son opinion, c'est la meilleure façon d'être honnête Ils s'font des frayeurs, veulent voir le seigneur annoncer l'tonnerre N'aie pas l'air étonné x2 N'aie pas l'air étonné, mentalité bétonnée 2zer et R.O.N, le formatage est erroné</t>
+          <t>La vrai fraternité, c'est déjà terminé On voit si t'as l'sang chaud une fois tes artères vidées C'est la guerre contre ces réfractaires givrés J'les met à terre s'ils déblatèrent sur mes affaires privées C'est la merde! Non j'veux pas m'faire des idées Détailler c'est risqué mais j'ai pas l'air d'hésiter Mais là frère c'que je vis c'est la célébrité J'lai mérité pour ça pas d'sérénité J'baise ta cacophonie j'vis ma vie Et j'te rends dingue comme une pathologie psychiatrique Putain y'as trop d'folies! Mais face aux phobies j'y arrive Tu cherches la merde, c'est que c'est la sodomie qui t'attire! Mon clan t'rentre dedans, sans prendre de gants C'est sanglant nan nan franchement Il est grand temps que j'me venge! Nekfeu, Framal et Mekra, S-Crew, nerveux f'ra vla les dégâts On va tout niquer, et j'le pense amplement! Faut pas nous banaliser, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Analisez, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Si ton malheur m'affecte, c'est par peur que ça m'arrive J'combat je maltraite, ceux qui condamnent le faciès Mes sons d'ailleurs achètent, les rappeurs que t'analyse Saveurs de cannabis, ces vapeurs me canalisent! Le diable est dans ton déhanché miss J'vais pas m'estomper j'vais dompter et plomber l'antéchrist, non c'est triste! Avant y'avait les meufs qui m'bâchaient et ces chiens qui m'ignoraient Maintenant j'me fais draguer par des bitchs aux seins siliconés! Unis dans l'biz mais on ne sait plus à qui se référencer Comme un uni-jambiste qui veut choisir sur quel pied danser Pas là pour plaisanter, ou bien quémander Ne propose pas un steak à un édenté! J'ai fréquenter les pires endroits J'ai vu des dérangés qui étranglaient des filles dans l'bois! Quand ta vie s'en va, t'es pris de l'angoisse Que ta miss conçoit, l'avenir sans toi! La vie d'rêve frangin, c'est 2zer Washington! Tu connais t'façons, L'Entourage bébé S-Crew booy! Framal est dans la place! Crapo', toujours monosourcilé! Blackbird bébé, Blackbirdddd, tu connais t'façons! Mekra, j'sais pas t'es où t'es toujours en retard Et Fennek, t'es en tournée, et Bsahtek, on va tout baiser ! S-Crew!1</t>
         </is>
       </c>
     </row>
@@ -2209,12 +2209,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Fraternité</t>
+          <t>Freestyle Planète Rap - Deen Burbigo, Nekfeu, 2-Zer, Jazzy Bazz, Doums &amp;Co</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>La vrai fraternité, c'est déjà terminé On voit si t'as l'sang chaud une fois tes artères vidées C'est la guerre contre ces réfractaires givrés J'les met à terre s'ils déblatèrent sur mes affaires privées C'est la merde! Non j'veux pas m'faire des idées Détailler c'est risqué mais j'ai pas l'air d'hésiter Mais là frère c'que je vis c'est la célébrité J'lai mérité pour ça pas d'sérénité J'baise ta cacophonie j'vis ma vie Et j'te rends dingue comme une pathologie psychiatrique Putain y'as trop d'folies! Mais face aux phobies j'y arrive Tu cherches la merde, c'est que c'est la sodomie qui t'attire! Mon clan t'rentre dedans, sans prendre de gants C'est sanglant nan nan franchement Il est grand temps que j'me venge! Nekfeu, Framal et Mekra, S-Crew, nerveux f'ra vla les dégâts On va tout niquer, et j'le pense amplement! Faut pas nous banaliser, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Analisez, on est des calamitées On compte pas sur l'amitié pour sortir de la misère! Mais Dieu merci mes potes ne cesseront pas de m'épauler Le succès nous fait décoller Oh oui j'veux la vie d'rêve! Si ton malheur m'affecte, c'est par peur que ça m'arrive J'combat je maltraite, ceux qui condamnent le faciès Mes sons d'ailleurs achètent, les rappeurs que t'analyse Saveurs de cannabis, ces vapeurs me canalisent! Le diable est dans ton déhanché miss J'vais pas m'estomper j'vais dompter et plomber l'antéchrist, non c'est triste! Avant y'avait les meufs qui m'bâchaient et ces chiens qui m'ignoraient Maintenant j'me fais draguer par des bitchs aux seins siliconés! Unis dans l'biz mais on ne sait plus à qui se référencer Comme un uni-jambiste qui veut choisir sur quel pied danser Pas là pour plaisanter, ou bien quémander Ne propose pas un steak à un édenté! J'ai fréquenter les pires endroits J'ai vu des dérangés qui étranglaient des filles dans l'bois! Quand ta vie s'en va, t'es pris de l'angoisse Que ta miss conçoit, l'avenir sans toi! La vie d'rêve frangin, c'est 2zer Washington! Tu connais t'façons, L'Entourage bébé S-Crew booy! Framal est dans la place! Crapo', toujours monosourcilé! Blackbird bébé, Blackbirdddd, tu connais t'façons! Mekra, j'sais pas t'es où t'es toujours en retard Et Fennek, t'es en tournée, et Bsahtek, on va tout baiser ! S-Crew!1</t>
+          <t>Débranche le distributeur de canette, branche le poste cassette Je fais mon premier style-free dans une laverie avec Khyde Alcoolisés à deux pas de mon lycée Sans le savoir, je suis à deux doigts d'm'enliser Le casque est vissé, les leçons ne sont pas révisées J'cours après les femmes métissées et les plats épicés J'savais que jamais ça m'ferait vibrer mais qu'il fallait tricher Ou bien aller trimer jusqu'à s'épuiser Faire du liquide à la sueur de mon front Car taffer pour les autres j'trouvais qu'y avait pas d'sens J'voulais acquérir des biens en vitesse J'ai dû apprendre à prendre mon mal en patience Plus d'une fois j'ai failli baisser les bras Comme tous ceux qui croient qu'ils n'ont pas d'chance Mais je suis déterminé comme les athlètes Arrogant, j'monte sur scène, j'ai pas l'track J'ai des mauvaises idées derrière la tête Et je cours comme un taré pour pas qu'elles m'rattrapent J'ai dû croire en moi, comme ceux qui naissent à la DASS C'est comme manger ou chier, personne va le faire à ma place J'fixais l'atlas, rêvant qu'c'est lui qui me regardait J'ai pris mon temps pour mieux le marquer Je te rappe ma vie boy 95 c'est la d'ou je viens la ou j'ai grandi la ou sur le terrain on casse tes reins sportif de haut niveau on aime le sport et la compète Négro check Le matin j'ai la tête dans l'cul J'ai la tête dans l'cul, réveillé par un 69 J'ai rêvé que j'abattais froidement c'keuf On connait le papier qu'ils mettent dans l'urne Film pornographique sur le laptop J'suis noyé par les vapeurs que j'absorbe Dans c'putain de monde où les valeurs peu rapportent Où les sénateurs et les violeurs se galochent Mes revenus sont en hausse massive Navré pour les rappeurs que j'amoche J'suis de confiance donc les soss me suivent Aucun d'eux ne dit qu'il a peur de la mort Ouais mais tous espèrent qu'c'est une autre vie Car on n'fait que de perdre au jeu Tu mets d'la cocaïne dans tes narines mais ton assurance n'est que d'la poudre aux yeux Mec, ici rien n'a changé Toujours les mêmes connards à l'Assemblée qui disent vouloir nous voir avancer Font mine de trinquer à la santé des gamins qu'ont que dalle à manger Face à cette vie j'ai du mal à bander Comme un gigolo qui doit baiser une vieille J'suis pas dealer mais je sais ce que c'est quand, la nuit, pour maintenir ton biz, tu veilles J'écris des danses macabres et je prends de la maille Il faut qu'je les stoppe comme un défenseur axial J'suis pas zoophile mais tu m'as vu dans le Canard Tu m'as vu dans le Canard, j'ai cru que j'y passais quand je fonçais dans ce platane Tu ressembles à cette fillette suintant le napalm et te jettes à l'avant de la rame Caillera de haut standing, que la concurrence se jette dans lvide Jeune criminel, CV polyvalent dans le bolide allemand mes négros visent la banque Dans ltrap jai festoyé. Grande, baffe si tu fais ldoyen Jai des négros riches qui, bicravent comme sils étaient en retard sur le loyer Street nigga check le répertoire Ghetto français, ghetto cain-ri jsuis lcroisement Les keufs passent au ralenti en me toisant Jcompte les plonger dans ldésespoir Nos ptits sont des adultes, on trime tôt, faut lbif gros Ils veulent juste assez dfric pour acheter des flingues au prix dgros Jsuis dans les cyphers où mes négros du-per posent Mes schémas drimes se superposent Jfais des rêves où la voiture de la brigade des stups explose Ta clique à lagonie, je nte respecterais jamais si tu sais pas mentir à la police! Viva la money ! Dans le hood ! Très très loin des lieux qui tinspirent la fête Face à nous tu ferais bien ddisparaître Négro, ton gilet pare-balle sert à rien jvise la tête! Je mène pas une vie hyper saine, même si j'ai percé J'aperçois des personnes derrière les persiennes Seul dans mon appart sale, ma sur révise un partiel Y'a pas d'loi impartiale à part l'Ciel J'suis entouré de zonards sur le sonar Mais c'est trop tard quand les ennuis sont là Les accusés sont sur l'banc et transpirent comme au sauna Les mères pleurent comme Solaar T'es jamais à l'abri, le mal me l'a appris La me-la brille, une maman prie Pourquoi tu me l'as pris ? Ô Dieu, c'est pas le Ciel, c'est les Hommes Odieux, leur âme est scellée par le sexe et les sommes J'ai vu le seum, donner du sale C'est comme si leur cur avait regardé les deux yeux de Médusa Le courage et la peur, ensemble, sont mes deux armes Quand je me sens déraciné, je monte au sommet des arbres De là-haut, j'vois la mort, faut être prêt si elle approche La vie, c'est apprécier la vue, après scier la branche Couplet 6 2Zer J'veux d'la maille, j'veux d'la maille dans mes poches Toujours dans ma chrysalide, j'ai pas l'temps d'éclore J'suis devant l'arbre de la vie et je gratte son écorce Bientôt j'pourrai la vendre, ouais la patience est d'or Pour la monnaie c'est la guerre, tu peux soulever des haltères C'est foutre ton nez dans mes affaires qui va provoquer ta perte La tête dans les nuages, toi t'es un peu trop terre à terre Comment veux-tu gagner si tu n'es toujours pas prêt à perdre ? Ouais Investir pour générer des bénéfices J'm'éloigne de mes bons côtés mais je reste près d'mes vices La monnaie fait dérailler, ouais la monnaie fait comploter À quoi bon être blindé si t'as l'destin d'un Kennedy ? Mon négro j'fume que la moula donc pas le temps pour le grand cru il faut qu'on strike c'est quoi les diez donc j'ai pas de couplet je pars en impro je vais mettre des gifles t'a compris c'est quoi les bails sort le gilet comme l'adit luxe on vise la tète t'as pas compris mes négros gèrent les tecs tu lèche des schnecks putain c'est crade rase les murs et laisse nous passer on va tous les écraser Grand cru est dans les bacs es que tu capte le putain de bail on est en impro le structure se superpose on lâche que des flammes et dragons les commendants sont dans la place minimum 25k si tu veux le pass! 25 c'est le grand cru bienvenu si t'as un grand cul on rentre dans la place pour le bigo c'est nek le fenek mec parle pas trop surtout au bigo envo les lingots on est dingo on veux se tailler ou? a saint domingue Yeah a saint domingue voir la mif avec mes gavas on va se barrer d'ici ouais tu sais que c'est dingue donc on part en freestyle comme a notre habitude donc on va gâtez le coin mais y'a pas de souci moi j'arrive je te donne toujours la bonne phase la bonne flamme tu captes les diez avec mes gavas on se pavane j'ai la belle femme</t>
         </is>
       </c>
     </row>
@@ -2226,12 +2226,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Freestyle Planète Rap - Deen Burbigo, Nekfeu, 2-Zer, Jazzy Bazz, Doums &amp;Co</t>
+          <t>Galérer</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Débranche le distributeur de canette, branche le poste cassette Je fais mon premier style-free dans une laverie avec Khyde Alcoolisés à deux pas de mon lycée Sans le savoir, je suis à deux doigts d'm'enliser Le casque est vissé, les leçons ne sont pas révisées J'cours après les femmes métissées et les plats épicés J'savais que jamais ça m'ferait vibrer mais qu'il fallait tricher Ou bien aller trimer jusqu'à s'épuiser Faire du liquide à la sueur de mon front Car taffer pour les autres j'trouvais qu'y avait pas d'sens J'voulais acquérir des biens en vitesse J'ai dû apprendre à prendre mon mal en patience Plus d'une fois j'ai failli baisser les bras Comme tous ceux qui croient qu'ils n'ont pas d'chance Mais je suis déterminé comme les athlètes Arrogant, j'monte sur scène, j'ai pas l'track J'ai des mauvaises idées derrière la tête Et je cours comme un taré pour pas qu'elles m'rattrapent J'ai dû croire en moi, comme ceux qui naissent à la DASS C'est comme manger ou chier, personne va le faire à ma place J'fixais l'atlas, rêvant qu'c'est lui qui me regardait J'ai pris mon temps pour mieux le marquer Je te rappe ma vie boy 95 c'est la d'ou je viens la ou j'ai grandi la ou sur le terrain on casse tes reins sportif de haut niveau on aime le sport et la compète Négro check Le matin j'ai la tête dans l'cul J'ai la tête dans l'cul, réveillé par un 69 J'ai rêvé que j'abattais froidement c'keuf On connait le papier qu'ils mettent dans l'urne Film pornographique sur le laptop J'suis noyé par les vapeurs que j'absorbe Dans c'putain de monde où les valeurs peu rapportent Où les sénateurs et les violeurs se galochent Mes revenus sont en hausse massive Navré pour les rappeurs que j'amoche J'suis de confiance donc les soss me suivent Aucun d'eux ne dit qu'il a peur de la mort Ouais mais tous espèrent qu'c'est une autre vie Car on n'fait que de perdre au jeu Tu mets d'la cocaïne dans tes narines mais ton assurance n'est que d'la poudre aux yeux Mec, ici rien n'a changé Toujours les mêmes connards à l'Assemblée qui disent vouloir nous voir avancer Font mine de trinquer à la santé des gamins qu'ont que dalle à manger Face à cette vie j'ai du mal à bander Comme un gigolo qui doit baiser une vieille J'suis pas dealer mais je sais ce que c'est quand, la nuit, pour maintenir ton biz, tu veilles J'écris des danses macabres et je prends de la maille Il faut qu'je les stoppe comme un défenseur axial J'suis pas zoophile mais tu m'as vu dans le Canard Tu m'as vu dans le Canard, j'ai cru que j'y passais quand je fonçais dans ce platane Tu ressembles à cette fillette suintant le napalm et te jettes à l'avant de la rame Caillera de haut standing, que la concurrence se jette dans lvide Jeune criminel, CV polyvalent dans le bolide allemand mes négros visent la banque Dans ltrap jai festoyé. Grande, baffe si tu fais ldoyen Jai des négros riches qui, bicravent comme sils étaient en retard sur le loyer Street nigga check le répertoire Ghetto français, ghetto cain-ri jsuis lcroisement Les keufs passent au ralenti en me toisant Jcompte les plonger dans ldésespoir Nos ptits sont des adultes, on trime tôt, faut lbif gros Ils veulent juste assez dfric pour acheter des flingues au prix dgros Jsuis dans les cyphers où mes négros du-per posent Mes schémas drimes se superposent Jfais des rêves où la voiture de la brigade des stups explose Ta clique à lagonie, je nte respecterais jamais si tu sais pas mentir à la police! Viva la money ! Dans le hood ! Très très loin des lieux qui tinspirent la fête Face à nous tu ferais bien ddisparaître Négro, ton gilet pare-balle sert à rien jvise la tête! Je mène pas une vie hyper saine, même si j'ai percé J'aperçois des personnes derrière les persiennes Seul dans mon appart sale, ma sur révise un partiel Y'a pas d'loi impartiale à part l'Ciel J'suis entouré de zonards sur le sonar Mais c'est trop tard quand les ennuis sont là Les accusés sont sur l'banc et transpirent comme au sauna Les mères pleurent comme Solaar T'es jamais à l'abri, le mal me l'a appris La me-la brille, une maman prie Pourquoi tu me l'as pris ? Ô Dieu, c'est pas le Ciel, c'est les Hommes Odieux, leur âme est scellée par le sexe et les sommes J'ai vu le seum, donner du sale C'est comme si leur cur avait regardé les deux yeux de Médusa Le courage et la peur, ensemble, sont mes deux armes Quand je me sens déraciné, je monte au sommet des arbres De là-haut, j'vois la mort, faut être prêt si elle approche La vie, c'est apprécier la vue, après scier la branche Couplet 6 2Zer J'veux d'la maille, j'veux d'la maille dans mes poches Toujours dans ma chrysalide, j'ai pas l'temps d'éclore J'suis devant l'arbre de la vie et je gratte son écorce Bientôt j'pourrai la vendre, ouais la patience est d'or Pour la monnaie c'est la guerre, tu peux soulever des haltères C'est foutre ton nez dans mes affaires qui va provoquer ta perte La tête dans les nuages, toi t'es un peu trop terre à terre Comment veux-tu gagner si tu n'es toujours pas prêt à perdre ? Ouais Investir pour générer des bénéfices J'm'éloigne de mes bons côtés mais je reste près d'mes vices La monnaie fait dérailler, ouais la monnaie fait comploter À quoi bon être blindé si t'as l'destin d'un Kennedy ? Mon négro j'fume que la moula donc pas le temps pour le grand cru il faut qu'on strike c'est quoi les diez donc j'ai pas de couplet je pars en impro je vais mettre des gifles t'a compris c'est quoi les bails sort le gilet comme l'adit luxe on vise la tète t'as pas compris mes négros gèrent les tecs tu lèche des schnecks putain c'est crade rase les murs et laisse nous passer on va tous les écraser Grand cru est dans les bacs es que tu capte le putain de bail on est en impro le structure se superpose on lâche que des flammes et dragons les commendants sont dans la place minimum 25k si tu veux le pass! 25 c'est le grand cru bienvenu si t'as un grand cul on rentre dans la place pour le bigo c'est nek le fenek mec parle pas trop surtout au bigo envo les lingots on est dingo on veux se tailler ou? a saint domingue Yeah a saint domingue voir la mif avec mes gavas on va se barrer d'ici ouais tu sais que c'est dingue donc on part en freestyle comme a notre habitude donc on va gâtez le coin mais y'a pas de souci moi j'arrive je te donne toujours la bonne phase la bonne flamme tu captes les diez avec mes gavas on se pavane j'ai la belle femme</t>
+          <t>Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains</t>
         </is>
       </c>
     </row>
@@ -2243,12 +2243,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Galérer</t>
+          <t>Gros freestyle de L’Entourage en live dans Planète Rap !</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains</t>
+          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
         </is>
       </c>
     </row>
@@ -2260,12 +2260,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Gros freestyle de L’Entourage en live dans Planète Rap !</t>
+          <t>Grünt d’Or #17</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
+          <t>Yeah, Zerzer Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour ds choses abominables, sèche ms larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais ZerZer volume 1 dispo partout la miff' DJ Élite aux platines Eh, eh Ok, ok, yeah Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Nique ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce gosse en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Brrrr Comme d'habitude, Hugz à la prod Eh, eh, eh Depuis l'époque de Décisions Yeah, yeah, yeah Han, han, Zerzer Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Ok, yeah, yeah, yeah Ça, c'est pour les anciens, ceux qui étaient là depuis l'époque Eh, eh Yeah Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie Yeah, yeah, yeah, yeah Ok, Reeko à la prod Hahaha, tu connais les bails Ouais, ouais, yeah Eh L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais Wooouh ! Han, han Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Yeah, yeah Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woouuh, -Crew, 2zer, Framal Brrraaa Brreh, brreh, brreh, brreh Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Letsguill ! Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Letsguill, Letsguill Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle 2zer Washington Ça sent la lorage, ca sent laverse jsuis dans ma tête Saboteurs Je ne bouge pas' jattends quca vienne Eh, eh, eh Sur le droit chemin, en sens inverse Grozomozo, Ratu, Saboteur gang Yeah, yeah, yeah Letsguill DJ Elite, balance la suite Han, han, tu connais Toujours la même, rien n'a changé Toujours les mêmes ons-s, toujours la même cons', eh Ouais, toujours les mêmes têtes Blackbird, Saboteur, Seine Zoo Hugz, ça dit quoi mon pote ? J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Eh, Grünt, sisi Han, han, ZerZer volume 1, dispo partout la miff' Yeah, han, han, han Saboteur gang, Seine Zoo Saboteur gang, Seine Zoo Hugz, ça dit quoi ? Yeah</t>
         </is>
       </c>
     </row>
@@ -2277,12 +2277,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Grünt d’Or #17</t>
+          <t>Horloge biologique</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Yeah, Zerzer Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour ds choses abominables, sèche ms larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais ZerZer volume 1 dispo partout la miff' DJ Élite aux platines Eh, eh Ok, ok, yeah Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Nique ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce gosse en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Brrrr Comme d'habitude, Hugz à la prod Eh, eh, eh Depuis l'époque de Décisions Yeah, yeah, yeah Han, han, Zerzer Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles et plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Tu n'apprends pas la violence aux incultes, tu choisis pas la couleur d'ton linceul Souvent le meurtre succède une insulte, j'fais des morceaux pour rester en un seul Facilité, c'est la vie criminelle pour obtenir toutes ces choses qu'on n'a pas Tous ces rappeurs font l'apogée du mal, moi, j'ai pêché pour pas servir d'appât Beaucoup peut changer en un millénaire, on a recommencé mais on a pris les mêmes Cette planète, c'est aussi la nôtre, on a peu d'influence donc à qui la faute ? La fin du monde, c'est les préliminaires, limité par des États militaires Imiter les U.S.A, c'est la mode, un nouvel air mais triste est la note Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Pour t'apprécier, j'ai besoin d'un effort mais la voix dans ma tête n'est pas d'accord Ma parano' et ma haine en essor, pas comme si j'pouvais les mettre à la porte Mon courage fait des grimaces à la peur, rien ne m'effraie à part l'taff d'amateur Enfant sauvage mais perfectionniste, éduqué par l'univers des comics J'viens d'un monde imaginaire, on a tous grandi dans le déni Suffit que tu perdes tes attaches pour que toutes les langues se délient J'ai tourné, tourné, tourné, tourné dans tous les recoins de Bériz Tourné, tourné, tourné, tourné comme un de mes sons dans ta playlist Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies ennemies, ennemies Galérer, galérer, galérer pour enfin me sentir aimé galérer, galérer Quand la parano prend les devants, la voix dans ta tête est ton ennemi ennemi, ennemi Galérer, galérer, galérer pour des choses qui valaient pas la peine galérer, galérer Plus les choix sont difficiles, plus tes émotions sont tes ennemies Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains pour n'en faire qu'à ma tête, ouais Toi et moi, c'est pas la même, ouais, j'suis guidé par la haine, ouais J'ai fait des pieds et des mains Ok, yeah, yeah, yeah Ça, c'est pour les anciens, ceux qui étaient là depuis l'époque Eh, eh Yeah Y'a pas d'erreur dans la vie, y'a que des leçons Quand j'gagne la mise, j'te claque la bise, je rejoue et j'claque mes jetons A quoi bon monter le ton ? Si tout le monde gueule, on s'entend plus Ça se traite d'enfant d'pute, ensuite ça se serre la main et sans rancune Du chantage pour une fellation le monde part en sucette La pratique de la délation, que de nombreux agents suggèrent Aux simples battements d'une aile, ta destinée peut changer L'effet papillon fait que c'est toi-même qui provoque le danger Et moi, quand maman me questionne, j'ai honte de lui répondre Elle pense que j'pense qu'elle m'espionne et que j'dois lui rendre des comptes C'est juste que c'est dur de dire à sa mère qu'on va pas fort Elle sera la première à le savoir si la gloire frappe à ma porte A la recherche du biff pour assumer une progéniture Mais si ton contrat c'est une biture, à quoi bon bosser si dur ? Alors que dans la rue j'me fais ton salaire en une semaine Pour l'instant je suis mon chemin mais c'est vers une impasse que la rue me mène x2 Bébé, tes belles fesses bougent sur le son de ma team Que tu sois blonde platine ou une bombe latine Mais on sait que tu cesses de rayonner quand revient la pluie C'est qu'on a bien appris les leçons de la vie Yeah, yeah, yeah, yeah Ok, Reeko à la prod Hahaha, tu connais les bails Ouais, ouais, yeah Eh L'homme n'est fidèle qu'à lui-même, c'est typique de la race humaine yeah Aucune raison rationnel, constamment dans le viseur d'un fusil à lunette, hey Ton tueur te connaît et t'as vu naître yeah, j'peux pas dire qu'l'humanité n'est pas cruel nan, nan, nan Tu connais mon salaire annuel écoute, j'peux flamber mais je me casse comme une allumette, ouais brah Ouais fuck toutes vos fédérations, on fait des rations au frais des nations yeah C'est toujours l'époque de la ségrégation, fuck vos délégués, vos délégations brah Que des vérités, pas de révélations ah, tiens la canne-à-pêche, laisse-moi gérer l'hameçon bitch T'entendais pas ma voix qui venait des bas fond yeah, maintenant tu fais tourner mon CD à fond eh-eh On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On parle de disrespect, même plus envie d's'aimer, on passe nos vies stresser, entre le jour et la nuit on est vite cerné On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri hey, hey On veut changer le colorie de nos vies, je te le dis, pas le temps de gole-ri ouais, ouais Wooouh ! Han, han Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Yeah, yeah Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woouuh, -Crew, 2zer, Framal Brrraaa Brreh, brreh, brreh, brreh Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas' jattends quca vienne Sur le droit chemin, en sens inverse Triple 6 quand ca vend la S Non faut pas suivre ou le vent tamène Que du THC dans le sang dla veine Vainqueur ou mort si jsors dlarène, oh Ya ma conscience qui veut rprendre sa place Jvois mes démons devant la glace, je roule un gros joint ltemps qusa passe Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Jsuis dans ma bulle, jsuis dans ma bulle Droit au but comme quand jsuis dans ma pute Ca roule des potences jsuis dans labus Jaime ni le beau temps ni la nature Ouais tu parles , jeune immature si tu veux devenir immortel comme Balladur Ca roule des vortex quand ya la bulle, jsuis dans un Scorsese quand yen a plus Pelo, jamais on a signé, jamais on va signé, ya que pour la fa-fa quon est prêt a signer Dpuis qujsuis papa, ils font tous quhalluciné Ils parlent drogue et de braquages mais cest que du ciné Jsuis né dans le ciment, jvais mourir dans le ciment La concu peut mourir en silence Tu découpais des souris en sciences, moi jécrivais déjà des couplets dOG en free-lance Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle Ça sent la lorage, ca sent laverse jsuis dans ma tête Je ne bouge pas, jattends quca vienne Sur le droit chemin, en sens inverse Taimes nous coller quand on effrites moula Jpartirais pas comme Boutefli-ka Ya pas plus technique sur lterrain ya pas Ya Dojo et OG sur lR1 motard Ta dope ma pas cassé la gueule, ton produit est guez car le crew est gang saboteur Les yeux collés devant lordinateur, en 2h cest plié aucun bégaye lets gi Mets moi du sucre dans mon coffee sugar Nouveau prétendant comme les Toffees Everton De lor dans les mains et les pieds neuf Jsuis devant, j'empile les buts comme Etoo fils avant-centre Dans lgame entouré des meilleurs sabo Jsuis Meyer Lansky pour les comptes Le cerveau bouillant jfais des pompes toujours Jsuis Luciano pour tes frayeurs Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Mais dans ma tête, hey ca fais un bail qucest plus la fête Jsuis dans ma bulle, hey jsuis dans ma bulle, jsuis dans ma tête Letsguill ! Jsuis dans labus, jsuis dans labus Aucune lumière sort de la brume Ca peut te fumer pour de la fumette Envoie la thune et hors de ma vue Élevé à la dure, élevé à la dure Taff mental et musculature Dure davoir une vue sur la mer, quand tas de loseille mais que tu pues la ur Faut que jassure, faut que jassure Personne va remplir mon assiette Pour mes hindous, pour mes asiat, mange quand ca peut fait pas la diette Sur la A6 dans le A7, ya le haschich dans la cachette Contrôle d'police, délit de faciès, c'était seulement pour une kassded, woah Letsguill, Letsguill Jsuis dans ma bulle, jsuis dans ma tête jsuis dans ma bulle 2zer Washington Ça sent la lorage, ca sent laverse jsuis dans ma tête Saboteurs Je ne bouge pas' jattends quca vienne Eh, eh, eh Sur le droit chemin, en sens inverse Grozomozo, Ratu, Saboteur gang Yeah, yeah, yeah Letsguill DJ Elite, balance la suite Han, han, tu connais Toujours la même, rien n'a changé Toujours les mêmes ons-s, toujours la même cons', eh Ouais, toujours les mêmes têtes Blackbird, Saboteur, Seine Zoo Hugz, ça dit quoi mon pote ? J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Faut faire en scred, la gova est wanted J'suis à Vondelpark, j'appelle Hugz au phone-tel Il descend d'l'hôtel, toujours en feu comme Ken Bientôt y'a -Crew tout en haut du top ten Pour toi et ta go, du bon sons pour ta gov' J'allume le moteur, ça rugit comme un fauve Pour info, j'bouge pas pour un faux Pour un frère, j'bombarde comme un fou Monte dans la chop, demande pas où on va Fais pas de manières, ralentis pas le convoi J'récupère c'qu'on m'doit, de quoi tenir tout le mois Mets le coco et on démarre, la liberté, c'est tout droit Et sur la route, c'est toujours mouvementé J'attends le moment Et la vitesse est augmentée Trop fumée de cal' il m'faut l'hollandaise J'ai la bonne hollandaise, mets les potos à l'aise Toujours les mêmes têtes toute la nuit dans la caisse Pour les rues d'Bélize, j'ai la bonne playlist Toujours les mêmes sons toute la nuit dans la caisse Un délit d'faciès, ouais on roule en classe S Lumière de ma qui brille dans la caisse Beaucoup d'appels, beaucoup d'adresses On ride, on ride, toute la nuit dans la caisse Ouais, ouais, ouais, ouais gros J'pensais que tout allait mieux quand tu quittais l'bendo J'évite les blems-pro, j'évite les filatures Paris est miniature, mais j'fais jamais la même chose Ouais, ouais, ouais, ouais gros Dis-moi, c'est qui le gars de l'autre côté du miroir ? J'ai dû ranger tous mes sentiments dans un tiroir J'ai perdu mon chemin pourtant, c'était une ligne droite Eh, Grünt, sisi Han, han, ZerZer volume 1, dispo partout la miff' Yeah, han, han, han Saboteur gang, Seine Zoo Saboteur gang, Seine Zoo Hugz, ça dit quoi ? Yeah</t>
+          <t>Eh Don, Don, Don Dada 2zer Washington Don, Don, Don Dada Seine Zoo Records, ouais ouais ouais Faut qu'tu niques tout, personne va l'faire à ta place Si les négros étaient des caisses On sort du concessionnaire et vous êtes à la casse dawg Faux billet plug en Uganda pas d'extradition Copyright le flow Seine Zoo sur la partition Technique comme Harlem, tu connais la tradition sisi Profil New York MCs, fuck les imitratrices De retour dans l'BX on aime quand les vils-ci balisent Sisi la team, huit heures de conduite Chauffeur haïtien, traphouse à Cincinnati Business de faux chèques, vacances à Aspen Cigare cubain comme le bracelet Escroc de luxe, j'en ai l'aspect Billets de toutes les couleurs, mon négro vas-y brasse-les Style de killa pour qui chaque vie se paie Ta meuf imagine le game okay Négro, t'es pas OG juste parce que t'étais là back in the days À la limite, et au-delà, jusqu'à l'au-delà J'vendrai le parfum du hood, j'appellerais ça Eau De Larmes Balance l'instru', j'me comporte comme un boucher avec Sors un disque, j'sais pas combien j'vais toucher avec La meuf à mon bras, j'vais t'faire loucher avec J'en ai marre d'elle même avant d'avoir couché avec Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage T'approches pas de mon cur si t'as peur du vide Mon horloge biologique indique l'heure du crime, hmm Petit opportuniste, écoute ce son faut pas qu'tu meurs stupide Mon cur comme stylo, mon sang en guise d'ancre Plus j'vide mes veines, plus j'me sens vivant Sans ça, je n'ai plus de sentiments Pourtant, on est tous nés en criant Trois heures du mat' dans une ruelle parisienne L'odeur te gene, dans la rue, y'a pas d'hygiène Como esta si esta bien Même si la vie m'a prouvé qu'il n'y a jamais d'happy end Pas d'heures précises pour les criminels Qui ont le cur assez froid pour aimer l'hiver Pas de rappeurs pressés pour les midinettes Qui veulent éliminer les préliminaires Le début d'la fin, négro l'alpha et l'oméga t'inflige des gros dégâts Démarre le biz devant l'entrée du Bodega, déter' comme Gogeta ouais ouais Tu veux d'l'automatique, tu trafiques le jouet Esclave du système, c'est pour mieux te contrôler qu'il agite le fouet Les faux passeports sont fournis par des zaïrois Les cheques lavés par mes gars d'l'Afrique de l'Ouest Seine Zoo perception, parle pas d'règles négro, j'suis l'exception J'arrive LuXe comme, tu connais l'expression Rappe à la perfection Hustla, couche tard, y'aura qu'mes frérots là où j'pars J'suis né réfugié politique, la Syrie Comment tu veux qu'ça m'touche pas ? Tes démons sont trop visibles mais le succès les maquillera Accompagné d'une Shakira sur la moto rouge d'Akira LuuuXe Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage Yeah, Seine Zoo Records Don Dada on dit quoi ? VM le Don, disquette le proc, lui fais croire qu'j'suis légal Qu'y'a pas d'business de drogues</t>
         </is>
       </c>
     </row>
@@ -2294,12 +2294,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Horloge biologique</t>
+          <t>Inévitable</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Eh Don, Don, Don Dada 2zer Washington Don, Don, Don Dada Seine Zoo Records, ouais ouais ouais Faut qu'tu niques tout, personne va l'faire à ta place Si les négros étaient des caisses On sort du concessionnaire et vous êtes à la casse dawg Faux billet plug en Uganda pas d'extradition Copyright le flow Seine Zoo sur la partition Technique comme Harlem, tu connais la tradition sisi Profil New York MCs, fuck les imitratrices De retour dans l'BX on aime quand les vils-ci balisent Sisi la team, huit heures de conduite Chauffeur haïtien, traphouse à Cincinnati Business de faux chèques, vacances à Aspen Cigare cubain comme le bracelet Escroc de luxe, j'en ai l'aspect Billets de toutes les couleurs, mon négro vas-y brasse-les Style de killa pour qui chaque vie se paie Ta meuf imagine le game okay Négro, t'es pas OG juste parce que t'étais là back in the days À la limite, et au-delà, jusqu'à l'au-delà J'vendrai le parfum du hood, j'appellerais ça Eau De Larmes Balance l'instru', j'me comporte comme un boucher avec Sors un disque, j'sais pas combien j'vais toucher avec La meuf à mon bras, j'vais t'faire loucher avec J'en ai marre d'elle même avant d'avoir couché avec Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage T'approches pas de mon cur si t'as peur du vide Mon horloge biologique indique l'heure du crime, hmm Petit opportuniste, écoute ce son faut pas qu'tu meurs stupide Mon cur comme stylo, mon sang en guise d'ancre Plus j'vide mes veines, plus j'me sens vivant Sans ça, je n'ai plus de sentiments Pourtant, on est tous nés en criant Trois heures du mat' dans une ruelle parisienne L'odeur te gene, dans la rue, y'a pas d'hygiène Como esta si esta bien Même si la vie m'a prouvé qu'il n'y a jamais d'happy end Pas d'heures précises pour les criminels Qui ont le cur assez froid pour aimer l'hiver Pas de rappeurs pressés pour les midinettes Qui veulent éliminer les préliminaires Le début d'la fin, négro l'alpha et l'oméga t'inflige des gros dégâts Démarre le biz devant l'entrée du Bodega, déter' comme Gogeta ouais ouais Tu veux d'l'automatique, tu trafiques le jouet Esclave du système, c'est pour mieux te contrôler qu'il agite le fouet Les faux passeports sont fournis par des zaïrois Les cheques lavés par mes gars d'l'Afrique de l'Ouest Seine Zoo perception, parle pas d'règles négro, j'suis l'exception J'arrive LuXe comme, tu connais l'expression Rappe à la perfection Hustla, couche tard, y'aura qu'mes frérots là où j'pars J'suis né réfugié politique, la Syrie Comment tu veux qu'ça m'touche pas ? Tes démons sont trop visibles mais le succès les maquillera Accompagné d'une Shakira sur la moto rouge d'Akira LuuuXe Les refrés le savent, on est venu faire le cash Action d'anthologie, mon horloge biologique me rappelle que le temps n'est qu'un mirage C'est pour ça que tous les refrés le savent LuXe On est venu faire le cash, action d'anthologie Mon horloge biologique me rappelle que le temps n'est qu'un mirage Yeah, Seine Zoo Records Don Dada on dit quoi ? VM le Don, disquette le proc, lui fais croire qu'j'suis légal Qu'y'a pas d'business de drogues</t>
+          <t>Ça vaut le cout de bien faire Toujours là quand t'as besoin dun coup de main frère Même quand il pleut des balles J'ai le pare-balles planqué sous mon imper' Ils ont retourné leur veste Une mauvaise étiquette cest tout ce qui leur reste On a pas besoin de leur aide Pour changer les choses tu dois rester le même On a fait avec le butin du larcin Ils se sont déployés tôt au lever 6h du matin Il y a pas de sortie de prison comme dans GTA5 Il n'y a qu'autour du poignet qu'elles peuvent me serrer la pince On a quitté les études pour vivre nos rêves Plus d'heures de vécu, moins d'heures de sommeil Un jour en Lexus, un jour en Citroen Un petit verre de Redbull Un petit verre de Mohet Toutes ces journées qui défilent avant que ma réussite me semblent interminables Pourtant les signes qui me guident vers la réussite me semblent indéniables Avec mon système auditif j'ai atteins des objectifs qui te semblent inatteignables Toutes ces journées qui défilent avant que ma réussite me semblent interminables Ne fais pas l'imbécile Faut rester vrai pour pouvoir dégager un vrai style Faut que tu restes investi Et nécoutes pas les soit disant saint desprits Quand ta vie te lance un défi Ne prends pas la décision d'être indécis Pour éviter le précipice Faut rester précis comme X2 Je vois les journées qui passent Des images et des visages Des lignes droites et des virages Besoin dun autre paysage Tu veux me mener en bateau T'as besoin d'un équipage L'amour cest mon seul héritage Mais la mort est inévitable Toutes ces journées qui défilent avant que ma réussite me semblent interminables Avec mon système auditif j'ai atteins des objectifs qui te semblent inatteignables X2 Toutes ces journées qui défilent avant que ma réussite me semblent interminables Pourtant les signes qui me guident vers la réussite me semblent indéniables Avec mon système auditif j'ai atteins des objectifs qui te semblent inatteignables Toutes ces journées qui défilent avant que ma réussite me semblent interminables</t>
         </is>
       </c>
     </row>
@@ -2311,12 +2311,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Inévitable</t>
+          <t>Je plairais aux types</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Ça vaut le cout de bien faire Toujours là quand t'as besoin dun coup de main frère Même quand il pleut des balles J'ai le pare-balles planqué sous mon imper' Ils ont retourné leur veste Une mauvaise étiquette cest tout ce qui leur reste On a pas besoin de leur aide Pour changer les choses tu dois rester le même On a fait avec le butin du larcin Ils se sont déployés tôt au lever 6h du matin Il y a pas de sortie de prison comme dans GTA5 Il n'y a qu'autour du poignet qu'elles peuvent me serrer la pince On a quitté les études pour vivre nos rêves Plus d'heures de vécu, moins d'heures de sommeil Un jour en Lexus, un jour en Citroen Un petit verre de Redbull Un petit verre de Mohet Toutes ces journées qui défilent avant que ma réussite me semblent interminables Pourtant les signes qui me guident vers la réussite me semblent indéniables Avec mon système auditif j'ai atteins des objectifs qui te semblent inatteignables Toutes ces journées qui défilent avant que ma réussite me semblent interminables Ne fais pas l'imbécile Faut rester vrai pour pouvoir dégager un vrai style Faut que tu restes investi Et nécoutes pas les soit disant saint desprits Quand ta vie te lance un défi Ne prends pas la décision d'être indécis Pour éviter le précipice Faut rester précis comme X2 Je vois les journées qui passent Des images et des visages Des lignes droites et des virages Besoin dun autre paysage Tu veux me mener en bateau T'as besoin d'un équipage L'amour cest mon seul héritage Mais la mort est inévitable Toutes ces journées qui défilent avant que ma réussite me semblent interminables Avec mon système auditif j'ai atteins des objectifs qui te semblent inatteignables X2 Toutes ces journées qui défilent avant que ma réussite me semblent interminables Pourtant les signes qui me guident vers la réussite me semblent indéniables Avec mon système auditif j'ai atteins des objectifs qui te semblent inatteignables Toutes ces journées qui défilent avant que ma réussite me semblent interminables</t>
+          <t>J'maudit vos critiques c'est pas joli joli quand j'te décime Trop dhypocrisie c'est la folie faut lire entre les lignes J'était inconscient, le feu ça brûle, mais j'y met ma main J'mérite des débris mais j'dérivait car j'm'estimais malin Ça fera mailler, j'attend pas ce qui n'arrivera jamais La gloire, c'est une pute qui est naïve, là je la met J'suis un mec en chien qui n'as plus d'os a mordiller On m'dit oublie les amours d'hier, et tout les coups amortis les J'compte me battre, dans la rue avec mes frères de sons On brille tellement tout ce qu'on fera, c'est te faire de l'ombre Met moi une balle si j'trahis mes compères C'est que vous êtes con si vous pariez qu'on perds J'suis un gars gentil mais j'garantis que j'percerai sans galanterie Pas d'couvert en plastique j'bouffe le succès avec de l'argenterie Pas envie de taffer, mais j'suis en vie, parfait Comment être heureux ma mère est handicapée x2 J'suis sur que je plairait aux types, sans ces stéréotypes Chanter c'est frais, sampler des vrais son stéréo, j'kiffe J'vais répéter qu'on est des vrais trop détestés nocifs Toute la journée je t'avouerai qu'on est pété au spliff' La nuit je m'endort sans songer C'est mon congé avant que le soleil apparaisse Je zappe le sommeil la paresse Je prend tout l'oseille y'a pas d'restes Le pe-ra est déblin je viens, savourer sa thune Ça veut toucher l'espace mais j'ai passer les XXX et Saturne Ici ça roule et ça fume car la journée sera dure Viens pas jouer j't'assure, gars, j't'avouerai qu'je sature J'rappe, en tapant les basses, viens, je t'apprend les bases Les MC veulent feater mais rien que ça prend des bâches Devant moi tu t'chie dessus et maintenant te met a ssé-pi Tu veux m'enculer a sec ? Nan tu m'encule mais accepte T'as les oreilles qui sanguillent Même mon son c'est comme une injection Va faire en bas ton jeune guignol Tu niques les oreilles de l'ingé Son On graille ton flow, c'est des friandises tes rimes J'suis un mec tu ne m'écoute pas, c'est des friand d'hystérie J'bicrave mes son comme des rettes-ba Tout les clients m'disent terrible J'vis en me disant Dans 10 ans fils t'est riche Oubliant le vice très vite... x31</t>
         </is>
       </c>
     </row>
@@ -2328,12 +2328,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Je plairais aux types</t>
+          <t>La biffle</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>J'maudit vos critiques c'est pas joli joli quand j'te décime Trop dhypocrisie c'est la folie faut lire entre les lignes J'était inconscient, le feu ça brûle, mais j'y met ma main J'mérite des débris mais j'dérivait car j'm'estimais malin Ça fera mailler, j'attend pas ce qui n'arrivera jamais La gloire, c'est une pute qui est naïve, là je la met J'suis un mec en chien qui n'as plus d'os a mordiller On m'dit oublie les amours d'hier, et tout les coups amortis les J'compte me battre, dans la rue avec mes frères de sons On brille tellement tout ce qu'on fera, c'est te faire de l'ombre Met moi une balle si j'trahis mes compères C'est que vous êtes con si vous pariez qu'on perds J'suis un gars gentil mais j'garantis que j'percerai sans galanterie Pas d'couvert en plastique j'bouffe le succès avec de l'argenterie Pas envie de taffer, mais j'suis en vie, parfait Comment être heureux ma mère est handicapée x2 J'suis sur que je plairait aux types, sans ces stéréotypes Chanter c'est frais, sampler des vrais son stéréo, j'kiffe J'vais répéter qu'on est des vrais trop détestés nocifs Toute la journée je t'avouerai qu'on est pété au spliff' La nuit je m'endort sans songer C'est mon congé avant que le soleil apparaisse Je zappe le sommeil la paresse Je prend tout l'oseille y'a pas d'restes Le pe-ra est déblin je viens, savourer sa thune Ça veut toucher l'espace mais j'ai passer les XXX et Saturne Ici ça roule et ça fume car la journée sera dure Viens pas jouer j't'assure, gars, j't'avouerai qu'je sature J'rappe, en tapant les basses, viens, je t'apprend les bases Les MC veulent feater mais rien que ça prend des bâches Devant moi tu t'chie dessus et maintenant te met a ssé-pi Tu veux m'enculer a sec ? Nan tu m'encule mais accepte T'as les oreilles qui sanguillent Même mon son c'est comme une injection Va faire en bas ton jeune guignol Tu niques les oreilles de l'ingé Son On graille ton flow, c'est des friandises tes rimes J'suis un mec tu ne m'écoute pas, c'est des friand d'hystérie J'bicrave mes son comme des rettes-ba Tout les clients m'disent terrible J'vis en me disant Dans 10 ans fils t'est riche Oubliant le vice très vite... x31</t>
+          <t>Que je perce dans le pe-ra c'est ça ma prophétie Moi j'en ai marre ça y est je me lance le bonheur m'a trop fait signe Dans ma vie en général moi je suis d'humeur pas trop festive On arrive pour géner le rap pour que tu dises que t'aime trop frais le style Si je suis impro je fais ce qu'il me plait Les mecs font meskines, se plaignent Depuis que ca rappe y en a même qui pour Mesrine se prennent J'ai pas de compte a te rendre, n'espére même pas qu'on t'attente Si je veux pas te voir je te verrais pas je suis un maitre en esquive suprême Je suis pas de ceux qui font le mal et qui en font l'apologie Ni de ceux qui disent qu'au fond la religion n'est que de la biologie Fini le temps du fitness j'ai une balance pour peser l'herbe grasse Marie Jeanne me fait planer mais je l'aime malgré son air de garce Beaucoup plus qu'une guerre de classes La où je vis il n'y a guère de grâce Comment cé-per sans faire de crasses Il y en a même qui à terre t'écrasent Je veux réussir mais je fais parti de ces jeunes qui poussent des cris en cours Ma vision du succès c'est plus qu'un stand aux puces de Clignancourt La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelé un rgard en coin, une patate sur le nez Nan pas dtaf, fuir le néant FatCap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos Toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Toujours des tas d'pervers et dans nos verres plus de lait maternel J'en ai marre d'errer loin des tam-tams de l'Afrique Y a pas d'drame ma bite, un tas de femmes me l'astiquent Mais je ne suis pas heureux comme Befa je reste impertinent Je t'emmerde sinon je suis pas un mec qui tremble J'ai un père til-gen, je fuis le vertige en négligent mes grosses cernes Et c'est évident, mec je vous défie sans me prosterner Je reste vivant, j'observe et je me défile dans cette existence Textes immensément dément, résident dans nos cervelles Trop excitent faut s'faire belle, tass, sinon t'assures plus J'veux pas de surplus, j'invite le président à s'faire mettre1</t>
         </is>
       </c>
     </row>
@@ -2345,12 +2345,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>La biffle</t>
+          <t>Laisse-moi</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Que je perce dans le pe-ra c'est ça ma prophétie Moi j'en ai marre ça y est je me lance le bonheur m'a trop fait signe Dans ma vie en général moi je suis d'humeur pas trop festive On arrive pour géner le rap pour que tu dises que t'aime trop frais le style Si je suis impro je fais ce qu'il me plait Les mecs font meskines, se plaignent Depuis que ca rappe y en a même qui pour Mesrine se prennent J'ai pas de compte a te rendre, n'espére même pas qu'on t'attente Si je veux pas te voir je te verrais pas je suis un maitre en esquive suprême Je suis pas de ceux qui font le mal et qui en font l'apologie Ni de ceux qui disent qu'au fond la religion n'est que de la biologie Fini le temps du fitness j'ai une balance pour peser l'herbe grasse Marie Jeanne me fait planer mais je l'aime malgré son air de garce Beaucoup plus qu'une guerre de classes La où je vis il n'y a guère de grâce Comment cé-per sans faire de crasses Il y en a même qui à terre t'écrasent Je veux réussir mais je fais parti de ces jeunes qui poussent des cris en cours Ma vision du succès c'est plus qu'un stand aux puces de Clignancourt La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelé un rgard en coin, une patate sur le nez Nan pas dtaf, fuir le néant FatCap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos Toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Toujours des tas d'pervers et dans nos verres plus de lait maternel J'en ai marre d'errer loin des tam-tams de l'Afrique Y a pas d'drame ma bite, un tas de femmes me l'astiquent Mais je ne suis pas heureux comme Befa je reste impertinent Je t'emmerde sinon je suis pas un mec qui tremble J'ai un père til-gen, je fuis le vertige en négligent mes grosses cernes Et c'est évident, mec je vous défie sans me prosterner Je reste vivant, j'observe et je me défile dans cette existence Textes immensément dément, résident dans nos cervelles Trop excitent faut s'faire belle, tass, sinon t'assures plus J'veux pas de surplus, j'invite le président à s'faire mettre1</t>
+          <t>Hé Yo 2zer Je te vois Yo la vibe est bonne Tes pétasses t'escortent Bien accompagné même si tu fais pas d'efforts Je suis dans le N-.Y.C Pousse le son à fond dans la caisse, en warning Vas-y vite secoue tes fesses, darling Poto roule un pers et laisse-moi vivre Yo yo C'est vrai que des fois je suis paro Laisse-moi ah ah ah J'ai juste besoin d'une tass' et d'un spliff Navré d'insister sur des faces B cainri Ces mecs me déçoivent et sont des fardeaux Y'a pas d'espoi a a ar Je te laisse haïr donc laisse-moi rire Les mamacitas m'disent you the best, papi Très bien entourés on a le pur Gildas flow T'as des fringues et t'as des chaussures de marque luuuXe Même si t'as des flingues on est au-dessus de ça Donc tu n'peux pas nous toucher car tu ne vise pas haut J'te vole ton goûter avec un fusil dassaut Un allez simple, pour les côtés obscurs de Paname viens! V'là les feintes pour enfiler leurs costumes de canards Pour eux le rap n'est rien de plus qu'une crise d'ado Yo la vibe est bonne Tes pétasses t'escortent Bien accompagné même si tu fais pas d'efforts Tu vois des Flammes partout on est les Nérons de ma ville Rien ne'change à part le prénom de ma bitch OK ça fait un pour le S, deux pour le L Trois pour la caisse et quatre pour la grâce du ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington mon reufré thug zer d'Paris Nord Seine Zooooooo On est 25 dans le club, style prince dans le club Mon break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veut pas que la peur te rejette Fais pas l'dingue dans le club Jeune vétéran, swerve élégant Blunt excellent nigga je pête les dents J'ai dis à mes G's qui y en a marre d'l'orgueil Quand le système est à poil j'ai la barre comme Deuil Ca fait one two, one two mic check T'es pas un hustler si tu t'es jamais retrouvé à sec Homie Yo la vibe est bonne Tes pétasses t'escortent Bien accompagné même si tu fais pas d'efforts Je suis dans le N-.Y.C Pousse le son à fond dans la caisse, en warning Vas-y vite secoue tes fesses, darling Poto roule un pers et laisse-moi vivre Yo yo C'est vrai que des fois je suis paro Laisse-moi ah ah ah J'ai juste besoin d'une tass' et d'un spliff Navré d'insister sur des faces B cainri Ces mecs me déçoivent et sont des fardeaux Y'a pas d'espoi a a ar Je te laisse haïr donc laisse-moi rire Les mamacitas m'disent you the best, papi LuuuuuuuuuuXe2</t>
         </is>
       </c>
     </row>
@@ -2362,12 +2362,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Laisse-moi</t>
+          <t>La vie n’est pas cirrhose</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Hé Yo 2zer Je te vois Yo la vibe est bonne Tes pétasses t'escortent Bien accompagné même si tu fais pas d'efforts Je suis dans le N-.Y.C Pousse le son à fond dans la caisse, en warning Vas-y vite secoue tes fesses, darling Poto roule un pers et laisse-moi vivre Yo yo C'est vrai que des fois je suis paro Laisse-moi ah ah ah J'ai juste besoin d'une tass' et d'un spliff Navré d'insister sur des faces B cainri Ces mecs me déçoivent et sont des fardeaux Y'a pas d'espoi a a ar Je te laisse haïr donc laisse-moi rire Les mamacitas m'disent you the best, papi Très bien entourés on a le pur Gildas flow T'as des fringues et t'as des chaussures de marque luuuXe Même si t'as des flingues on est au-dessus de ça Donc tu n'peux pas nous toucher car tu ne vise pas haut J'te vole ton goûter avec un fusil dassaut Un allez simple, pour les côtés obscurs de Paname viens! V'là les feintes pour enfiler leurs costumes de canards Pour eux le rap n'est rien de plus qu'une crise d'ado Yo la vibe est bonne Tes pétasses t'escortent Bien accompagné même si tu fais pas d'efforts Tu vois des Flammes partout on est les Nérons de ma ville Rien ne'change à part le prénom de ma bitch OK ça fait un pour le S, deux pour le L Trois pour la caisse et quatre pour la grâce du ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington mon reufré thug zer d'Paris Nord Seine Zooooooo On est 25 dans le club, style prince dans le club Mon break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veut pas que la peur te rejette Fais pas l'dingue dans le club Jeune vétéran, swerve élégant Blunt excellent nigga je pête les dents J'ai dis à mes G's qui y en a marre d'l'orgueil Quand le système est à poil j'ai la barre comme Deuil Ca fait one two, one two mic check T'es pas un hustler si tu t'es jamais retrouvé à sec Homie Yo la vibe est bonne Tes pétasses t'escortent Bien accompagné même si tu fais pas d'efforts Je suis dans le N-.Y.C Pousse le son à fond dans la caisse, en warning Vas-y vite secoue tes fesses, darling Poto roule un pers et laisse-moi vivre Yo yo C'est vrai que des fois je suis paro Laisse-moi ah ah ah J'ai juste besoin d'une tass' et d'un spliff Navré d'insister sur des faces B cainri Ces mecs me déçoivent et sont des fardeaux Y'a pas d'espoi a a ar Je te laisse haïr donc laisse-moi rire Les mamacitas m'disent you the best, papi LuuuuuuuuuuXe2</t>
+          <t>La vie n'est pas si rose à part si tu te noies dans l'alcool J'suis qu'un parigot, j'ai mon sse-di de hash dans la poche T'façon c'est soit le Rap, soit je vis de l'argent d'la drogue Y'a que la foi qui te guidera devant la mort Approche, peu importe tes infos ou tes intox Y'a pas de doutes, j'ai plein d'potes On parle de foufs, on parle de flouze On parle de toucher l'jackpot mais jamais de ce qu'il adviendrait Si l'un de nous disparaissait, des couplets j'en gratterais Au moins dix par décès, ainsi, j'trouverai la force On a rien sans rien, en principe, on est d'accord Mais, toi, t'es prêt à tout et t'en oublies ta fierté Ton respect, tu l'as laissé mourir à tes pieds Constamment en crise existentielle Peu importe tes malheurs, ma gueule, tu te dois de sourire S'te plait stoppe tes vices et tes mises en scènes Tu penses avec ton ventre mais t'as jamais su de quoi te nourrir J'ai dit constamment en crise existentielle Peu importe tes malheurs, ma gueule, tu te dois de sourire S'te plait stoppe tes vices et tes mises en scènes Tu penses avec ton ventre mais t'as jamais su de quoi te nourrir Je m'en beurre de tes foutus ces-vi J'ai plus envie de perdre des potes pour du teu-shi Emballer du shit sous cello C'est le destin de tous les gars du ghetto C'est ce caramelo mielleux le nerf de la guerre pour les loves C'est ce caramelo mielleux le nerf de la guerre pour les loves Le nerf de la guerre pour les loves c'est ce caramelo mielleux Quand j'partais, y'avait la madre qui s'inquiétait J'vivais en marge, pas à la page, pire qu'un illettré Tu comprendras mon malaise si j'te décris les faits Et gestes et là tu comprendras c'que j'ai décidé d'être Et j'reste le même avec tout le monde en dépit des traîtres Paradoxal, c'est ces hommes sales qui embellissent mes textes Forcément, la vie change quand t'as pris des pépètes Finie l'époque des tête-têtes et des grèves lycéenes J'bicravais en étant insouciant et naïf Mais autour d'un mafé au foyer, un jour, Candy m'a dit ×2 Les flics se fondent dans la masse, surveille ton voisinage Ils te prennent en photo sans se soucier d'tes droits d'images Emballer du shit sous cello C'est le destin de tous les gars du ghetto C'est ce caramelo mielleux le nerf de la guerre pour les loves C'est ce caramelo mielleux le nerf de la guerre pour les loves Le nerf de la guerre pour les loves c'est ce caramelo mielleux Constamment en crise existentielle Peu importe tes malheurs, ma gueule, tu te dois de sourire S'te plait stoppe tes vices et tes mises en scènes Tu penses avec ton ventre mais t'as jamais su de quoi te nourrir J'ai dit constamment en crise existentielle Peu importe tes malheurs, ma gueule, tu te dois de sourire S'te plait stoppe tes vices et tes mises en scènes Tu penses avec ton ventre mais t'as jamais su de quoi te nourrir Je m'en beurre de tes foutus ces-vi J'ai plus envie de perdre des potes pour du teu-shi1</t>
         </is>
       </c>
     </row>
@@ -2379,12 +2379,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>La vie n’est pas cirrhose</t>
+          <t>La zezer</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>La vie n'est pas si rose à part si tu te noies dans l'alcool J'suis qu'un parigot, j'ai mon sse-di de hash dans la poche T'façon c'est soit le Rap, soit je vis de l'argent d'la drogue Y'a que la foi qui te guidera devant la mort Approche, peu importe tes infos ou tes intox Y'a pas de doutes, j'ai plein d'potes On parle de foufs, on parle de flouze On parle de toucher l'jackpot mais jamais de ce qu'il adviendrait Si l'un de nous disparaissait, des couplets j'en gratterais Au moins dix par décès, ainsi, j'trouverai la force On a rien sans rien, en principe, on est d'accord Mais, toi, t'es prêt à tout et t'en oublies ta fierté Ton respect, tu l'as laissé mourir à tes pieds Constamment en crise existentielle Peu importe tes malheurs, ma gueule, tu te dois de sourire S'te plait stoppe tes vices et tes mises en scènes Tu penses avec ton ventre mais t'as jamais su de quoi te nourrir J'ai dit constamment en crise existentielle Peu importe tes malheurs, ma gueule, tu te dois de sourire S'te plait stoppe tes vices et tes mises en scènes Tu penses avec ton ventre mais t'as jamais su de quoi te nourrir Je m'en beurre de tes foutus ces-vi J'ai plus envie de perdre des potes pour du teu-shi Emballer du shit sous cello C'est le destin de tous les gars du ghetto C'est ce caramelo mielleux le nerf de la guerre pour les loves C'est ce caramelo mielleux le nerf de la guerre pour les loves Le nerf de la guerre pour les loves c'est ce caramelo mielleux Quand j'partais, y'avait la madre qui s'inquiétait J'vivais en marge, pas à la page, pire qu'un illettré Tu comprendras mon malaise si j'te décris les faits Et gestes et là tu comprendras c'que j'ai décidé d'être Et j'reste le même avec tout le monde en dépit des traîtres Paradoxal, c'est ces hommes sales qui embellissent mes textes Forcément, la vie change quand t'as pris des pépètes Finie l'époque des tête-têtes et des grèves lycéenes J'bicravais en étant insouciant et naïf Mais autour d'un mafé au foyer, un jour, Candy m'a dit ×2 Les flics se fondent dans la masse, surveille ton voisinage Ils te prennent en photo sans se soucier d'tes droits d'images Emballer du shit sous cello C'est le destin de tous les gars du ghetto C'est ce caramelo mielleux le nerf de la guerre pour les loves C'est ce caramelo mielleux le nerf de la guerre pour les loves Le nerf de la guerre pour les loves c'est ce caramelo mielleux Constamment en crise existentielle Peu importe tes malheurs, ma gueule, tu te dois de sourire S'te plait stoppe tes vices et tes mises en scènes Tu penses avec ton ventre mais t'as jamais su de quoi te nourrir J'ai dit constamment en crise existentielle Peu importe tes malheurs, ma gueule, tu te dois de sourire S'te plait stoppe tes vices et tes mises en scènes Tu penses avec ton ventre mais t'as jamais su de quoi te nourrir Je m'en beurre de tes foutus ces-vi J'ai plus envie de perdre des potes pour du teu-shi1</t>
+          <t>Hugz, t'es en feu sur celle-là J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées J'ai l'air différent, jugé au premier regard, moins de droits que de devoirs, t'façon, c'est tous des crevards Y a pas d'meufs car sans le bus', y a pas d'monnaie, cercle vicieux t'es connu mais plus personne te connait J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées C'est la zezer, la zezer, la zezer, la zezer, la zezer, la zer, oh, yo C'est la zezer, la zezer, la zezer, la zezer, la zezer, la zer, mmh Un gros doobie et je chante à la Bob Marley, j'connais la map de mon cerveau, j'évite les sombres allées J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées J'm'accroche au peu de bonheur, au peu des gens qui me restent J'aurais pu m'en sortir mais la haine m'a dit je t'aime Fais tourner le mot ils m'ont tous tourné le dos Parmi tous les vrais comment trouver le faux ? J'm'accroche au peu de bonheur, au peu des gens qui me restent J'aurais pu m'en sortir mais la haine m'a dit je t'aime Fais tourner le mot ils m'ont tous tourné le dos Si j'sais que j'suis vrai, qui est le faux ? Mauvais équipage, le navire a chaloupé, au milieu de la scène, c'est pas les plages de la Guadaloupe Les pirates échoués sur les rivages de l'Île-de-France, j'ai usé d'la violence, j'ai perdu mon innocence J'ai vu des choses qu'on n'devrait pas voir, heureusement qu'j'étais naïf, tu peux pas souffrir sans le savoir, nan, nan Le bonheur est parti, bon débarras, j'suis bien dans ma zezer, seul comme CJ contre les Ballas Ils m'ont dit C'est que du bus', ne le prends pas personnel Mais ce bus', c'est toute ma vie, j'me transforme en mercenaire J'suis comme toi, j'ai fait du sale avant qu'le soleil se lève J'ai marché dans tout Paname, j'ai vu quel monde sous mes semelles, eh J'suis dans l'vaisseau mère mais j'ai nulle part où aller Dans ma tête, j'ai fait le vide, j'entends ma voix résonner C'est la zezer, faut faire des provisions mais on a tout graillé Si être sain, c'est suivre les règles, on est des fous à lier J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées J'ai l'air différent, jugé au premier regard, moins de droits que de devoirs, t'façon, c'est tous des crevards Y a pas d'meufs car sans le bus', y a pas d'monnaie, cercle vicieux t'es connu mais plus personne te connait J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées C'est la zezer, la zezer, la zezer, la zezer, la zezer, la zer, oh, yo C'est la zezer, la zezer, la zezer, la zezer, la zezer, la zer, mmh Un gros doobie et je chante à la Bob Marley, j'connais la map de mon cerveau, j'évite les sombres allées J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées J'm'accroche au peu de bonheur, au peu des gens qui me restent J'aurais pu m'en sortir mais la haine m'a dit je t'aime Fais tourner le mot ils m'ont tous tourné le dos Parmi tous les vrais comment trouver le faux ? J'm'accroche au peu de bonheur, au peu des gens qui me restent J'aurais pu m'en sortir mais la haine m'a dit je t'aime Fais tourner le mot ils m'ont tous tourné le dos Si j'sais que j'suis vrai, qui est le faux ?</t>
         </is>
       </c>
     </row>
@@ -2396,12 +2396,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>La zezer</t>
+          <t>Le gong</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Hugz, t'es en feu sur celle-là J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées J'ai l'air différent, jugé au premier regard, moins de droits que de devoirs, t'façon, c'est tous des crevards Y a pas d'meufs car sans le bus', y a pas d'monnaie, cercle vicieux t'es connu mais plus personne te connait J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées C'est la zezer, la zezer, la zezer, la zezer, la zezer, la zer, oh, yo C'est la zezer, la zezer, la zezer, la zezer, la zezer, la zer, mmh Un gros doobie et je chante à la Bob Marley, j'connais la map de mon cerveau, j'évite les sombres allées J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées J'm'accroche au peu de bonheur, au peu des gens qui me restent J'aurais pu m'en sortir mais la haine m'a dit je t'aime Fais tourner le mot ils m'ont tous tourné le dos Parmi tous les vrais comment trouver le faux ? J'm'accroche au peu de bonheur, au peu des gens qui me restent J'aurais pu m'en sortir mais la haine m'a dit je t'aime Fais tourner le mot ils m'ont tous tourné le dos Si j'sais que j'suis vrai, qui est le faux ? Mauvais équipage, le navire a chaloupé, au milieu de la scène, c'est pas les plages de la Guadaloupe Les pirates échoués sur les rivages de l'Île-de-France, j'ai usé d'la violence, j'ai perdu mon innocence J'ai vu des choses qu'on n'devrait pas voir, heureusement qu'j'étais naïf, tu peux pas souffrir sans le savoir, nan, nan Le bonheur est parti, bon débarras, j'suis bien dans ma zezer, seul comme CJ contre les Ballas Ils m'ont dit C'est que du bus', ne le prends pas personnel Mais ce bus', c'est toute ma vie, j'me transforme en mercenaire J'suis comme toi, j'ai fait du sale avant qu'le soleil se lève J'ai marché dans tout Paname, j'ai vu quel monde sous mes semelles, eh J'suis dans l'vaisseau mère mais j'ai nulle part où aller Dans ma tête, j'ai fait le vide, j'entends ma voix résonner C'est la zezer, faut faire des provisions mais on a tout graillé Si être sain, c'est suivre les règles, on est des fous à lier J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées J'ai l'air différent, jugé au premier regard, moins de droits que de devoirs, t'façon, c'est tous des crevards Y a pas d'meufs car sans le bus', y a pas d'monnaie, cercle vicieux t'es connu mais plus personne te connait J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées C'est la zezer, la zezer, la zezer, la zezer, la zezer, la zer, oh, yo C'est la zezer, la zezer, la zezer, la zezer, la zezer, la zer, mmh Un gros doobie et je chante à la Bob Marley, j'connais la map de mon cerveau, j'évite les sombres allées J'me sens pas chez moi, j'ai nulle part où aller, si Dieu veut, ça va aller si j'évite les sombres allées J'm'accroche au peu de bonheur, au peu des gens qui me restent J'aurais pu m'en sortir mais la haine m'a dit je t'aime Fais tourner le mot ils m'ont tous tourné le dos Parmi tous les vrais comment trouver le faux ? J'm'accroche au peu de bonheur, au peu des gens qui me restent J'aurais pu m'en sortir mais la haine m'a dit je t'aime Fais tourner le mot ils m'ont tous tourné le dos Si j'sais que j'suis vrai, qui est le faux ?</t>
+          <t>J'ai pas le même destin que Giscard J'parle pas la même langue que Jack J'prends le micro, toi tu jactes, j'prends le micro, toi tu jactes On rentre dans la salle, on est 1000 squa Ça bédave comme à la fac J'prends le micro, toi tu jactes, j'prends le micro, toi tu jactes Mets le que-tru dans le sac, mets le que-tru dans le sac J'ai des blessures sous les straps Y'a mes gars sûrs sur l'estrade On est high, on est ailleurs Et m'a ceinture elle est noire comme Teddy Riner, Teddy Riner Tous ces motherfuckers le savent, tous ces motherfuckers le savent Quelle est la taille de mon cur ? Il est pas plus grand qu'un grain de sable La monnaie j'ai besoin de ça, la monnaie j'ai besoin de ça J'suis pas né dans les sous, j'ai pas chié dans la soie Ramène le cash, on a froid hey Ramène le cash, on a froid J'ai crié mes textes, j'me suis cassé la voix Vas-y roule dans la caisse, on a passé la douane Je suis né pour embrasser la gloire Je la vois, je me dis que je pourrais l'avoir Mais que pour y arriver, j'ai toute la mer à boire Ramène le cash, on a soif On veut niquer des mères, tu comprends le message Une équipe de fer, on va squatter les ondes Ce qui coule dans mes veines, c'est le sang des esclaves Je me gratte la tête, j'ai de l'or sous les ongles M'a dit Bagdadi depuis le départ J'suis dans ma fusée, je fiste le monde Tu pourras pas dire que tu savais pas Nan, la seule chose qui peut nous sauver c'est le gong ah-ah-ah ah-ah-ah-ah-ah-ah M'a dit Bagdadi depuis le départ J'suis dans ma fusée, je fixe le monde Tu pourras pas dire que tu savais pas Nan, la seule chose qui peut nous sauver c'est le gong Ohohohoh on voit la vie en rouge, en vert, en violet Marche ou crève, je veux m'envoler tout là-haut J'vais braquer la banque avec mon pistolet à flo-ow Fais tourner l'info-o-o Paralysé par la peur, sur une main j'ai cur et dans l'autre j'ai l'détonateur Écoute pas c'que disent les rappeurs, y'a pas plus faux Ah, j'mets des billets de té-cô J'dois me coucher tard, j'dois me lever tôt On se retrouver au Zénith, j'ai juré sur la vie de mama T'inquiète pas pour l'avenir, j'écris toutes mes rimes sur les lignes de ma main On veut quitter la terre, vas-y fume tout le zder, j'ai pas mis de tabac Hier je mordais la poussière, aujourd'hui j'ai ce grain dans la voix T'inquiète pas, si t'es là, on va pas t'oublier T'étais pas dans les bails, c'est que tu devais roupiller Pas de noblesse, nan nan, j'ai le sang d'ouvrier J'ai dû me reprendre, la monnaie m'avait bousillé J'ai pas choisi ma voie, non, des voix m'ont guidé Ouais j'ai gardé la foi, et ça, quoi qu'on disait Marre de dépenser des sommes et des sommes et des sommes Tout l'monde veut gratter son billet Certain profite de ta gentillesse, y'a que des croix sur le calendrier On est que des hommes et des hommes et des hommes et, des fois, nos destins sont liés L'adversité ne m'impressionne pas, j'suis le seul qui l'ouvre quand personne ne parle Ne me questionne pas, j'sais pourquoi je m'allume Entre l'homme et la lune, il n'y a qu'un seul pas Cercle vicieux, les anneaux de Saturne J'suis en apesanteur et pourvu que ça dure Ouais, l'atterrissage est plus dur que la chute Entre l'homme et la lune, il n'y a qu'un seul pas Ohohohoh on voit la vie en rouge, en vert, en violet Marche ou crève, je veux m'envoler tout là-haut J'vais braquer la banque avec mon pistolet à flo-ow Fais tourner l'info-o-o Paralysé par la peur, sur une main j'ai cur et dans l'autre j'ai l'détonateur Ecoute pas c'que disent les rappeurs, y'a pas plus faux Ah, j'mets des billets de té-cô J'dois me coucher tard, j'dois me lever tôt On se retrouver au Zénith, j'ai juré sur la vie de mama T'inquiète pas pour l'avenir, j'écris toutes mes rimes sur les lignes de ma main On veut quitter la terre, vas-y fume tout le zder, j'ai pas mis de tabac Hier je mordais la poussière, aujourd'hui j'ai ce grain dans la voix</t>
         </is>
       </c>
     </row>
@@ -2413,12 +2413,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Le gong</t>
+          <t>L’Entourage en live dans Planète Rap</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>J'ai pas le même destin que Giscard J'parle pas la même langue que Jack J'prends le micro, toi tu jactes, j'prends le micro, toi tu jactes On rentre dans la salle, on est 1000 squa Ça bédave comme à la fac J'prends le micro, toi tu jactes, j'prends le micro, toi tu jactes Mets le que-tru dans le sac, mets le que-tru dans le sac J'ai des blessures sous les straps Y'a mes gars sûrs sur l'estrade On est high, on est ailleurs Et m'a ceinture elle est noire comme Teddy Riner, Teddy Riner Tous ces motherfuckers le savent, tous ces motherfuckers le savent Quelle est la taille de mon cur ? Il est pas plus grand qu'un grain de sable La monnaie j'ai besoin de ça, la monnaie j'ai besoin de ça J'suis pas né dans les sous, j'ai pas chié dans la soie Ramène le cash, on a froid hey Ramène le cash, on a froid J'ai crié mes textes, j'me suis cassé la voix Vas-y roule dans la caisse, on a passé la douane Je suis né pour embrasser la gloire Je la vois, je me dis que je pourrais l'avoir Mais que pour y arriver, j'ai toute la mer à boire Ramène le cash, on a soif On veut niquer des mères, tu comprends le message Une équipe de fer, on va squatter les ondes Ce qui coule dans mes veines, c'est le sang des esclaves Je me gratte la tête, j'ai de l'or sous les ongles M'a dit Bagdadi depuis le départ J'suis dans ma fusée, je fiste le monde Tu pourras pas dire que tu savais pas Nan, la seule chose qui peut nous sauver c'est le gong ah-ah-ah ah-ah-ah-ah-ah-ah M'a dit Bagdadi depuis le départ J'suis dans ma fusée, je fixe le monde Tu pourras pas dire que tu savais pas Nan, la seule chose qui peut nous sauver c'est le gong Ohohohoh on voit la vie en rouge, en vert, en violet Marche ou crève, je veux m'envoler tout là-haut J'vais braquer la banque avec mon pistolet à flo-ow Fais tourner l'info-o-o Paralysé par la peur, sur une main j'ai cur et dans l'autre j'ai l'détonateur Écoute pas c'que disent les rappeurs, y'a pas plus faux Ah, j'mets des billets de té-cô J'dois me coucher tard, j'dois me lever tôt On se retrouver au Zénith, j'ai juré sur la vie de mama T'inquiète pas pour l'avenir, j'écris toutes mes rimes sur les lignes de ma main On veut quitter la terre, vas-y fume tout le zder, j'ai pas mis de tabac Hier je mordais la poussière, aujourd'hui j'ai ce grain dans la voix T'inquiète pas, si t'es là, on va pas t'oublier T'étais pas dans les bails, c'est que tu devais roupiller Pas de noblesse, nan nan, j'ai le sang d'ouvrier J'ai dû me reprendre, la monnaie m'avait bousillé J'ai pas choisi ma voie, non, des voix m'ont guidé Ouais j'ai gardé la foi, et ça, quoi qu'on disait Marre de dépenser des sommes et des sommes et des sommes Tout l'monde veut gratter son billet Certain profite de ta gentillesse, y'a que des croix sur le calendrier On est que des hommes et des hommes et des hommes et, des fois, nos destins sont liés L'adversité ne m'impressionne pas, j'suis le seul qui l'ouvre quand personne ne parle Ne me questionne pas, j'sais pourquoi je m'allume Entre l'homme et la lune, il n'y a qu'un seul pas Cercle vicieux, les anneaux de Saturne J'suis en apesanteur et pourvu que ça dure Ouais, l'atterrissage est plus dur que la chute Entre l'homme et la lune, il n'y a qu'un seul pas Ohohohoh on voit la vie en rouge, en vert, en violet Marche ou crève, je veux m'envoler tout là-haut J'vais braquer la banque avec mon pistolet à flo-ow Fais tourner l'info-o-o Paralysé par la peur, sur une main j'ai cur et dans l'autre j'ai l'détonateur Ecoute pas c'que disent les rappeurs, y'a pas plus faux Ah, j'mets des billets de té-cô J'dois me coucher tard, j'dois me lever tôt On se retrouver au Zénith, j'ai juré sur la vie de mama T'inquiète pas pour l'avenir, j'écris toutes mes rimes sur les lignes de ma main On veut quitter la terre, vas-y fume tout le zder, j'ai pas mis de tabac Hier je mordais la poussière, aujourd'hui j'ai ce grain dans la voix</t>
+          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
         </is>
       </c>
     </row>
@@ -2430,12 +2430,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>L’Entourage en live dans Planète Rap</t>
+          <t>L’homme Wanted</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>J'me sens hypocrite, j'plonge dans les tentations volontairement Un péché en plus, un billet en moins J'tue doucement la concurrence, tous habillés en noir On n'a pas l'temps d'attendre ton enterrement J'pense à ceux qu'on s'est mis à dos, j'vois mon seum s'émietter C'est mieux de s'aimer que sortir le semi-auto On est tous responsables, en partie, du monde que l'on bâtit L'égoïsme et le manque d'empathie, tout le monde en pâtit C'qu'on vole, on le reperd De quoi tomber pour recel dans le repère Dans la jungle urbaine Sous tenue camouflage pour qu'on me repère J'ai percé en indé', j'suis frais C'monde est régi par des chiffres Et, pour comprendre, faut déchiffrer Ton patron t'a jeté, tu galères pour t'acheter Les nouvelles paires en étant berné par les reportages télé Tu vis dans un monde où l'État peut te piller ou t'épier T'as pigé en regardant un dollar, garde un il sur tes billets Le biz' est flambant neuf depuis qu'on a verni les langues de bois Le passé, j'y peux rien, mec, mais l'avenir dépend de moi Bienvenu dans l'pays des relations extra-conjugales Ta femme et son amant festoient et baisent dans ton plumard... Enlève ton autotune, nous, on est plutôt talkbox L apostrophe, on est nos propres boss, l'indé nous colle au cul Jamais de drogues dures, juste la douceur d'un bon joint Chérie, t'as besoin d'un conjoint, S-Crew t'en offre plus d'un Faites de la place à la Chevrolet, va garer ton Opel ailleurs T'inquiète, j'ai des poches sous les yeux pour garder mon oseille à lil On est loin des villas de Cannes et d'la bronzette On boit la gasolina, chez Yass, dans le Bronx C'est quand y'a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Ça chante, mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on a l'affiche Les fachos sont fâchés, on vivra Me parle plus d'amitié, pour dire vrai, tout ça ça m'dépasse Donc laisse-moi avec ma miff, j'ai l'espoir de les mettre bien à vie Nan, j'veux pas d'ta pitié, ni d'ta grognasse dans l'huitième En fait moi, c'est pour ma miff que j'bicrave Pour les mettre bien à vie Marie-Jeanne c'est ma femme, la nicotine c'est ma p'tite copine En partant de c'point d'vue, tu sauras que j'suis plutôt clean Mais j'ai mes vices comme tout l'monde J'essaie de vivre comme tout l'monde On m'a dit Faut qu'tu tes-mon Sans sucer d'bites comme tout l'monde J'suis prêt à caner pour ma cause, pas pour une dose de plus On n'est pas pareil, t'es dans l'paraitre, t'es qu'une hoes de plus Moi, c'est décidé, dans moins d'une décennie, j'aurais la destinée Dessinée par le guide à moins qu'on s'désunissent J'vois la dérive et des humains décimés pour du liquide Aux valeurs décimales face aux décédés J'reste indécis, man, j'suis qu'un specimen dissipé pas les décibels Pourquoi les deks, ces dep's, me regardaient si mal ? Motherfucker, t'as pas pigé ? J'suis pas d'ici, moi Je t'avais promis qu'un jour tu te rappellerais de nos têtes Je ne suis pas prêt de me taire De la primaire au lycée, déprimé, je me sentais prisonnier Parce que les professeurs voulaient toujours me noter Pourtant, j'aimais les cours, j'étais différent De tous ceux qui me disaient Soit tu subis, soit tu mets les coups Moi, je rêvais d'aventure, griffonnais les devantures J'attaquais tout ce qui m'était défendu Rien à péter de toutes leurs émissions de télé de vendus Je voulais voir le monde avant d'être rappelé devant Dieu Et, pour ne pas qu'on se moque de moi, je bouquinais en cachette Pendant que les gamins de mon âge parlaient de voitures Un des gars de l'époque bicravait des Armani Code Et, un beau jour, il a ramené une arme à l'école J'étais choqué de le voir avec un glock Oui ! J'en ai rien à foutre de vos putains de codes Oui ! J'avais peur, je l'ai dit, mais j'ai un cur, je le dis Mais je suis toujours là pour mes putains de potes Maintenant, pour lui, le bruit des balles est imprimé dans le crâne Ceux qui traînaient dans le bât' l'ont entraîné vers le bas On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Ramène pas ton grain d'sel, il nous manque pas d'grain Quand t'entends qu'ça grince, c'est que j'baise avec ta princesse J'les entend tous, ils font crari ils sont pleins d'règles Mais vont trahir de leur plein gré Sur mes cicatrices, pas d'pansements J'me méfie des pensées, bah, ouais, les gens mentent Un penchant pour le gent-gent, mon fric j'fais que l'dépenser Plein d'rêves, on veut tous faire des dingueries Pour tout niquer y'a qu'un siècle, S-Crew On prend les mêmes et on recommence L'histoire à commencé dans l'quinzième Des films d'horreur et des romans, on n'a jamais d'remords On fait que des effondrements, revient arc-en-ciel La date de ton bum-al, personne se demande quand c'est Toujours corcé, le pe-Ra part en couille, man J'écoute des trucs à l'ancienne Chaque jour de l'honneur comme un samouraï Peut-être qu'un beau jour ça m'aura J'ai pas besoin d'sa morale, on fera plus rien quand ça mourra Pour ça qu'faut faire que des sans faute, jamais dans l'faux Il m'en faut pas beaucoup pour sortir mes dents de fauve Ici, dans l'quinze, quand on appuie, ça fait pas d'bruit derrière J'suis venu au monde la nuit mais c'était pas la nuit dernière L'intelligence bat des records, on lit à travers l'regard Au Blackbird on record, on fait apparaitre le cash Peut-être que les mecs te mentent Et, nan y'a pas que les vêtements Je n'pense pas que les rêves de grands Me correspondent honnêtement Des centaines de kilomètres de gens dehors J'aimerais qu'on les mette devant Ceux qui respectent le règlement Ne le respectent pas correctement Compter les miettes de temps C'est entêtant mais les mecs se pendent Cependant tout le monde s'étend Quand c'est le dernier temps mort Tcheck le bête de gang quand j'entre en transe Phénomène étrange, quand j'entends tant de tendance Dans les têtes de vente, je les traite ouvertement, tonton Oui, j'ai la flemme de Rantanplan quand j'guette le béton armé Faut pas dégainer ton arme ou la BAC te pète bêtement Je resterai ce tendre mec, je sais que j'ai le cran Si ça transperce, c'est qu'tu pensais Qu'la balle serait peut-être blanche Feu, feu dans les bacs, la balle était pas blanche, fils de putain C'est comme ça qu'ça s'passe, j'vise le butin J'vise le cur des frères et surs, c'est comme ça qu'ça s'passe Comme mes prédecesseurs, le truc est nécessaire Laissez-faire, c'est comme ça qu'ça s'passe en impro Les gars s'rapprochent du mic, Ali, Phénomène Bizness C'est comme ça qu'ça s'passe Balance une petite phase direct du 9.4 A la limite du coma les galères me prennent la tête C'est pas la fête et j'me répète encore une soirée comme d'hab Hanté par des faits divers des bails de weed en tess Sortez les k-way l'hiver arrive a Winterfell Alors j'me renferme sur moi même comme un collier de perle Ou j'me sens à létroit comme dans une chatte de coréenne Leurs phases de grandes blagues, des rimes de farces et attrapes S'réfugie dans l'futur mais sache qu'un jour le passé te rattrape Quand la bonne étoile s'dérobe la chance est prise de gangrène Des phases et des phases à t'écouler par centaines J'ai démarré mon couplet au départ sans thème Depuis têtard toujours têtu mes pensées sont lointaines, merde Il s'fait tard, toujours une heure d'retard, j'vis à l'heure londonienne Sous leurs apparences chic l'argent sera leur seul parachute Les apparatchiks plus rien ne les choque à part la chute Le destin est-il voué à mourir comme des prolétaires Laisse-moi devenir propriétaire, il n'y a que Dieu qu'je dois louer La vie se fait de défaites, je les regarde se battre pour gagner Merde, ils sont tous à l'ouest comme Kanye Une ville étrange où je réside plongé dans la résine, parfois Je me résigne mais pourtant combien sont déjà condamnés ? Prends les valises, direction Brésil ou bien Chicago Perdu dans Beriz, si j'analyse je crois que je suis carbo Blindés par le vécu au final on veut l'palace J'ai vu, je vaincrai, j'suis pas venu, j'suis déjà là I dont know if you understand but Imma fucking kill it All these other niggas know we chilling in the building Right now in Skyrock, Planet Rap These niggas better know me because Im in that trap Bring up that money, nothing is funny All these other niggas looking at me they bummy All these other niggas know that I get bunnies Fucking them, loving them, all these niggas know I do it Everywhere they see us so these niggas know Im fluid All these niggas truant, they aint even go to school And these niggas know Im young but Im not a fucking fool Watch me, watch me, watch my back All these niggas better sit it cause Im with the S-crew Lentourage dawg, killing it with that 1995, 86 gang Niggas know its my thing dawg and I dont really sing All niggas know what I really bring Im hot on the mic so yall better see Goddamn and niggas yall just wannabes Im nice, nigga Im nice And youd better cool me off dawg I need ice Got a little ice on my neck golden chain Niggas know I do it and its not a fucking game Watch out right now Thank you Nekfeu on the beat J'aimerais sourire plus souvent mais ça n'serait pas sincère Quand j'fais semblant, j'ai très vite mal au visage Mes zygomatiques se bloquent Igo, ma clique te botte, mes bicots trafiquent le pops Les renois sont rarement les grossistes Même dans le drogue game, on a rien, on n'a pas le droit de dîner C'est pour tous mes Haalpulaar Gales-sène ou maliens, moi, j'suis d'la Guinée La science de la survie est innée, il faut que tu m'ressentes Même si on a pas d'lien, mon rap c'est pour tout l'monde J'en ai rien à foutre, si t'es tous les jours au skate park Si tu shootes pour des quettes-pla ou si tu joues au sket-ba J'veux juste que tu sois respectable Et qu'tu deviennes le spectateur de mon spectacle Jouez aux insomniaques, ouais Venez on teste, on verra qui veillera l'plus Dans leurs clips, ils chantent, ils dansent mais ils rappent plus Quand faut faire de la thune J'ai juste besoin de mon oreiller et de ma plume Je marche dans la brume, toujours prêt à monnayer de la pure J'suis pas un négro philosophe ou un négro qui joue au singe, nan Pendant qu'tu achètes des diamants pour la chaîne de ta chienne Je schématise, je complote pour la chair de ma chair Ceux qui vont pleurer si j'pars, ouais, si mon récit t'parle Achète pour que j'les achève mais n'me félicite pas, nan Les compliments, c'est comme la caillasse Qu'est-ce que tu veux que j'fasse avec ? Aucun d'nous retournera sa veste Pas d'veste réversible, Phaal fait et persiste A la fois brillant et flottant j'suis l'averse et l'éclaircie Je suis celui qui ne supporte pas l'idée de taffer On m'a tellement dit Dommage, on le déduira de ta paye Je suis celui qui arrive avant que tu te mettes à rêver Je suis la scène que tu refais quand tu viens de te faire taper Y'a quelque chose entre Paname et moi Nek le Fenek est un cavalier noir A bas les lois, avale mes noix Pardonnez-moi si je perds la mémoire Un pilier de bar depuis le départ L'envie de me battre guide mes pas Un filet de bave, en piteux état J'espère que cette pétasse s'épile le bas Le studio est allemand, italiennes sont les bagnoles Les concerts sont américains, les branlettes sont espagnoles On va découper pour la miff On part en freestyle, c'est de-spee Rien à foutre, je baise ces bitchs Gars, neuvième zone, oui, c'est l'inspi Posé avec mon gava à droite, c'est Joon, nan, c'est pas un jnoun Le gava vient de L.A., tu sais qu'il est calibré Il a ramené la wax et la weed Tu vois c'que j'veux dire avec la miff On s'est posés, on a tisé, on a fait l'spleech Rien à foutre, on est des jins, on était fuckin clean Pourquoi tu veux tester mes négros ? C'est comme ça, mec C'est comme ça que j'me pose sur la melo Ça s'passe comme les cheveux de Doums Ce soir, c'est Black Yellow Ouais, on se pose, l'album Est dans les bacs donc j'm'essaie au impros Ouais, mon gars, si tu veux jouer, fais pas le pro Je m'en bats les couilles J'essaie de gagner du temps avant que Saï pose C'est comme ça qu'ça s'passe Tu vois bien que le mic chauffe Mets le dans le iPod, le iPad et le iPhone C'est comme ça qu'ça s'passe C'est pour ça que les 'tasses font Paris, nul ne nous compare... Qui veut la paix devra combattre Peine capitale, pas de compassion pour les fonblards Viol dans les geôles, starfoullah Flow convoité par les kideb Feinté par une meuf en hijeb Victime du coup du foulard Envahi par des pensées maussades, fasciné par les gros cas ? Je ne cours qu'après une femme Dans le seul but de lui déposséder d'son sac Têtu dans le calme, renoi qui n'aime pas la fête Dois-je leur mettre des balles dans le crâne Pour qu'ils aient du plomb dans la tête ? En quête du bonheur de l'amour Dans la vie, c'est la mort qui peine à m'accoster Dounia fait la gueule dans la détresse C'est dans l'alcool que mes gars vont s'arroser Au bord de la falaise, divertis par les interactions de la life Perdu dans la sphère, fais c'que t'as à faire Lâche les tass et pète ta wife Prise de conscience, c'est la solitude qui m'a dit Compte sur toi Vise la victoire, débloque le trône par la force brute Mec, c'est le mal que tu soudoies J'ai autant de potes que je compte sur mes dix doigts Je me devais bien de lire entre les signes Je m'efforce à égorger un noich' du 13 Pour écrire mon 16 à l'encre de Chine 1, 2, 3, 4, levez les bras 5, 6, 7, 8, levez les brink's Puis semez les flics et posez les briques 9, 10, 11, 12, courez là-bas Les filles savent tout, n'en doutez pas Nafissatou baise Dominique, elle a le beau boraba Elle m'a dit Tu me niques Mais trop d'timiniks donc je t'en voulais pas Comme Alejandro, ne m'enculez pas Vous ne nous aurez pas, vrais négros comme Aimé Césaire Partez à point, ne courez pas Vous ne comprenez pas comment ne pas aimer sévère La boisson vient d'Ecosse ou bien de Pologne La trahison sent l'eau de Cologne Ces putes sont des menteurs Ils utilisent la langue de Bois d'Boulogne Donne-moi du biff ! La zik, on la fait nous même Sûr que tu kiffes, Bizi Bizi Phénomène L'avenir, j'en fais mon thème, j'te l'ai déjà dit dans Mayday Il n'y a pas de je t'aime, j'te prie de m'excuser, baby De la haine et de la rancur Super vulgaires seront toutes mes ballades Tu gouteras toute ma fureur Parle à ma bite, mon cur est malade Niveau rap toi tu n'es pas là, tu n'as ni le rythme ni le mental Dis-moi c'que t'as rappé à part de l'emmental La main sur le mic, la tête ailleurs comme mon papa surmené Un plat dpâtes surgelées, un regard en coin, une patate sur le nez Nan, pas dtaff, fuir le néant, Fat Cap sous les néons La BAC passe soulever quand ça stape sous le préau Backpack vissé au dos, toujours le même schéma ternaire Toujours la même haine dans les veines, les mêmes débats fermés Toujours les même thèmes, les mêmes scènes que lÉtat permet Ouais, des tas dpervers et dans nos verres plus de lait maternel Et jen ai marre derrer loin des tam-tams de lAfrique Y'a pas ddrame, ma bite, un tas dfemmes me lastique Mais je nsuis pas heureux, comme be-Fa, j'reste impertinent Je temmerde sinon, jsuis pas un mec qui tremble Mais jai un père til-gen et jfuis le vertige en Négligeant mes grosses cernes et cest évident Mec, j'te défie sans me prosterner Je reste vivant, jobserve et je mexile dans cette existence Tu peux m'croiser au coin d'la rue, toujours à laffût De toutes ces putes qui veulent nous voir finir en garde à vue Sache car c'est dead, on a la rime catapulte C'est l'invasion, ouais, nique les clones, on fera du sale je t'assure On roule des cônes, on 'lume des go Est-ce que tu captes, t'as vu ? Et même les gars d'ta rue Viennent chez nous puis tapent d'la pure Bande de loss' pour une dose sont prêts à pep's, t'abuses Et dans mon coin d'rue, c'est pas la même, t'as vu Tu verras toujours les mêmes gars posés Pas de petite frappe dopée 'vec sa petite 'tasse cokée Pute vénale, checke ce freestyle codée Faudrait qu'tu vives dans mon coin d'rue Pour comprendre mon point d'vue Chut, pédale, j'ai pas l'temps pour les on-dits T'es qu'un fuckin fanatique, t'fais pas passer pour un homie Dans mon coin d'rue, plein d'gus s'adonnent au mic Et j'en ai plein l'cul d'ces incultes paranoïaques J'ai le même regard qu'un canon d'calibre Comme une grosse baffe de maçon j'arrive J'suis devenu fou, que des mecs de l'ombre, Paris M'a rendu sombre, accro du son mais quand j'affronte, high kick Pour les keufs, le pompe sera vide Fonce dans les catacombes quand les matons rappliquent Et c'est mes péripéties, j'excite les filles en passant Appelle-moi l'ennemi des flics, j'aiguise des rimes, j'prends l'argent Pire qu'une épidémie, j'vesqui les schmits, l'équipe est vive Terrible, et oui, j'débite des lignes d'épileptique, j'tente ma chance Et y'a pas d'autotune, que des phases qui claquent ton gros cul Tu cherches un endroit où me taper ? Va sur Youtube On débarque, on est quatre, on t'épate, faut des liasses Qu'on démarrent des gamos Lotus J'ai la gorge serrée et la peur du futur Comme un gosse qui élabore ses rêves Et j'adore mes frères mais, à force, je les perds Car cette vie rapide est éphémère, la mort se dépêche Et même si ta clique est téméraire, esquive l'abysse et les ténèbres La fille facile et les pervers, la drogue les berce 1, 2, 1, 2, mic check ! Plein de rageux, plein de blèmes Mais mon posse, flingue le Rap jeu à l'aise Les leçons de la vie s'apprennent seules Et pas quand des vieux cons te parlent A la tombée d'la nuit, la tour Eiffel Enfile sa plus belle roba à paillettes On saute les barrières de la boite pour pas yep' A la nique sa mère, on sort et on boit, j'en ai vu claquer Un an d'salaire en une soirée en boite et rentrer à iep' J'suis issu d'la mixité, fuck tes aprioris J'vais chercher un d'mes potes dans sa cité On s'retrouve après au Ritz Si, si, tout est possible, sérieux, tu pensais quoi, bitch ? Passe un peu sur Paname, ici, les opposées cohabitent OK, ça parle en G pour terminer en 4K 6D peut t'arranger des meufs tah Jason Statham Putain de lifestyle, nan, je n'm'en lasse pas Mais dans un pavtar, nique sa mère, je graille le plat d'pâte Tas d'lascards, la comédie pour que Madame paye mes dédicaces Aujourd'hui, j'm'extasie, j'ai peut-être les mains sales Mais y'a qu'les gens extrêmes qui ne voulaient pas que j'm'installe C'est Gang, le freestyle est convivial Rien qu'on inhale, chez moi c'est pire que l'Burning J'ai dit, c'est Gang, prêt à rentrer dans des anneaux Si l'plan tombe à l'eau, allô, j'ai besoin du magot J'porte l'espoir de mes soss sur mes jeunes épaules Pas question d'décevoir, on grandit 'vec le seum d'être pauvre J'te jure qu'ça forge le caractère, quand tu sors d'l'école Pour les sentiers battus ou les bagarres règnent Les stups sont sur ma trace et ces tass' veulent ma maille Donc j'me déplace qu'en silence entre ces rapaces Je smoke la came, à l'impasse Cité Véron On vit là-bas avec mes gars sûrs on a calciné des Frémont Descendu des Gildas possédés par le démon Enfoiré, passe le chivas quand j'suis posé dans la pénombre La miff' c'est le principal, le beat, c'est secondaire Les bitchs ont la dernière place Ainsi que les traitres de leurs compères Voici mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'ai dit, mes principes, yo, juste quelques mots Non, n'aie pas peur, ça vient du cur, danse sur ma démo J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ J'voudrais refaire ma vie sans qu'on m'parle de contrat Le temps passe trop vite ou pas assez donc il ne compte pas Reufré, la miff, c'est c'qui fait tenir mes gars 7.5, double 0, 9 depuis le top départ3</t>
+          <t>J'm'appelle 2-Zer, enchanté, dans ma vie j'ai perdu trop d'chicos Mon tier-quar est en chantier XXX que des toxicos Pas d'coquelicots mais mon moral et au ras des pâquerettes Tu veux bicrave ? Viens nous voir et t'auras des plaquettes Je sais qui est fauché et quel gus a d'l'oseille J'ai pas besoin d'téléphone car j'ai la puce à l'oreille T'es, t'es comme un vicelard qui trace des miss fines J'suis armé jusqu'aux dents car j'crache des missiles Y'a plus d'hospitalité, j'suis le gosse qui t'as niqué Moi, j'te crosse si t'as l'idée de nous hospitaliser Toi, tes soss tétanisés XXX détalent, sale grosse pédale Retourne t'amuser, casse-toi ou j'sors le gros pétard J'ai des crocs d'blédard mais je n'traîne qu'avec des mecs sincères Viens m'tester et j'te montrerai à quoi un médecin sert J'ai pas pris d'cours de chant mais, sur ma vie, qu'j'ai trouvé ma voie J'ai rien à t'prouver, j'aurais du biff si j'pouvais XXX J'ai boycotte l'école pour m'occuper de ma carrière Comme si j'étais sur l'périph', j'peux pas faire marche arrière J'essaye de m'ouvrir au monde mais j'ai pas d'charnière J'm'acharne pour montrer qu'j'réussis à ceux qui m'charriaient J'veux qu'les cons s'tirent donc conquérir ma ville Tout m'porte malheur, j'te l'répète si tu m'as pas compris ma XXXXX J'ai merdé, j'ai choisi l'peu-Ra sans demander l'avis d'ma mère Bien avant que Nekfeu me dise Connais-tu la vie d'galère ? Wesh, Candy Cotton, j'suis un bandit Qu'est-ce t'en dis, cochonne ? Devant moi y'a rien à faire comme un manche-di d'automne Reste gentil, bonhomme... 2-Zer ! Dédicace, Candy Cotton, j'suis un bandit Qu'est-ce t'en dis, cochonne ? Devant moi y'a rien à faire comme un manche-di d'automne Reste gentil, bonhomme ou...</t>
         </is>
       </c>
     </row>
@@ -2447,12 +2447,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>L’homme Wanted</t>
+          <t>L’ignorance</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>J'm'appelle 2-Zer, enchanté, dans ma vie j'ai perdu trop d'chicos Mon tier-quar est en chantier XXX que des toxicos Pas d'coquelicots mais mon moral et au ras des pâquerettes Tu veux bicrave ? Viens nous voir et t'auras des plaquettes Je sais qui est fauché et quel gus a d'l'oseille J'ai pas besoin d'téléphone car j'ai la puce à l'oreille T'es, t'es comme un vicelard qui trace des miss fines J'suis armé jusqu'aux dents car j'crache des missiles Y'a plus d'hospitalité, j'suis le gosse qui t'as niqué Moi, j'te crosse si t'as l'idée de nous hospitaliser Toi, tes soss tétanisés XXX détalent, sale grosse pédale Retourne t'amuser, casse-toi ou j'sors le gros pétard J'ai des crocs d'blédard mais je n'traîne qu'avec des mecs sincères Viens m'tester et j'te montrerai à quoi un médecin sert J'ai pas pris d'cours de chant mais, sur ma vie, qu'j'ai trouvé ma voie J'ai rien à t'prouver, j'aurais du biff si j'pouvais XXX J'ai boycotte l'école pour m'occuper de ma carrière Comme si j'étais sur l'périph', j'peux pas faire marche arrière J'essaye de m'ouvrir au monde mais j'ai pas d'charnière J'm'acharne pour montrer qu'j'réussis à ceux qui m'charriaient J'veux qu'les cons s'tirent donc conquérir ma ville Tout m'porte malheur, j'te l'répète si tu m'as pas compris ma XXXXX J'ai merdé, j'ai choisi l'peu-Ra sans demander l'avis d'ma mère Bien avant que Nekfeu me dise Connais-tu la vie d'galère ? Wesh, Candy Cotton, j'suis un bandit Qu'est-ce t'en dis, cochonne ? Devant moi y'a rien à faire comme un manche-di d'automne Reste gentil, bonhomme... 2-Zer ! Dédicace, Candy Cotton, j'suis un bandit Qu'est-ce t'en dis, cochonne ? Devant moi y'a rien à faire comme un manche-di d'automne Reste gentil, bonhomme ou...</t>
+          <t>Le temps a plus de valeur que l'dollar et l'euro, j'm'en occuperai quand j'aurai quelques années de trop J'sais pas si j'me trompe mais pour l'instant, j'suis heureux, l'ignorance fait l'bonheur, woho J'te connais même pas, tu m'prends la tête, laisse-moi vivre le bon moment À fond sens interdit, meufs assorties avec ma Benz, l'ignorance fait l'bonheur, woho Chez nous, c'est donnant-donnant, ce quotidien est trop lent Il est temps que j'prenne le volant, personne peut m'arrêter Enfermé entre quatre murs, tout est écrit donc j'm'allume Faut lire entre les ratures, comment ça, j'peux pas rêver ? Slalom entre les voitures, à deux pas de la droiture On mélange pas nos sentiments donc l'ignorance, on la boit pure L'inquiétude est dans ma nature, le seul remède, c'est le danger On part en équipe à l'aventure, on se sent chez nous à l'étranger C'est autour de l'oseille que tout tourne, ici bas, c'est quitte ou double C'est pas grave de se faire dépasser tant que tu sais qui te double J'regarderai pas le temps passer, j'laisse pas les années me tabasser Comment ça, mon destin est cadenassé ? Pass-PTT dans la doudoune Le temps a plus de valeur que l'dollar et l'euro, j'm'en occuperai quand j'aurai quelques années de trop J'sais pas si j'me trompe mais pour l'instant, j'suis heureux, l'ignorance fait l'bonheur, woho J'te connais même pas, tu m'prends la tête, laisse-moi vivre le moment À fond sens interdit, meufs assorties avec ma Benz, l'ignorance fait l'bonheur, woho J'suis pas de ceux qui font les choses bien pour les mauvaises raisons Mais de ceux qui agissent par impulsion et après, s'posent des questions J'étais tranquille mais rien ne pouvait donc ça n'allait pas Leur philosophie et tous leurs intérêts ne mimpressionnaient pas Tous ces gens peuvent zapper les leurs pour une opportunité Ils font dans la proximité, ils ont l'esprit limité J'ai mis du temps mais mon arrivée va faire un gros coup d'éclat Si c'est pas moi, c'est mes gars j'suis vainqueur dans tous les cas Le temps a plus de valeur que l'dollar et l'euro, j'm'en occuperai quand j'aurai quelques années de trop J'sais pas si j'me trompe mais pour l'instant, j'suis heureux, l'ignorance fait l'bonheur, woho J'te connais même pas, tu m'prends la tête, laisse-moi vivre le bon moment À fond sens interdit, meufs assorties avec ma Benz, l'ignorance fait l'bonheur, woho</t>
         </is>
       </c>
     </row>
@@ -2464,12 +2464,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>L’ignorance</t>
+          <t>Médaille</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Le temps a plus de valeur que l'dollar et l'euro, j'm'en occuperai quand j'aurai quelques années de trop J'sais pas si j'me trompe mais pour l'instant, j'suis heureux, l'ignorance fait l'bonheur, woho J'te connais même pas, tu m'prends la tête, laisse-moi vivre le bon moment À fond sens interdit, meufs assorties avec ma Benz, l'ignorance fait l'bonheur, woho Chez nous, c'est donnant-donnant, ce quotidien est trop lent Il est temps que j'prenne le volant, personne peut m'arrêter Enfermé entre quatre murs, tout est écrit donc j'm'allume Faut lire entre les ratures, comment ça, j'peux pas rêver ? Slalom entre les voitures, à deux pas de la droiture On mélange pas nos sentiments donc l'ignorance, on la boit pure L'inquiétude est dans ma nature, le seul remède, c'est le danger On part en équipe à l'aventure, on se sent chez nous à l'étranger C'est autour de l'oseille que tout tourne, ici bas, c'est quitte ou double C'est pas grave de se faire dépasser tant que tu sais qui te double J'regarderai pas le temps passer, j'laisse pas les années me tabasser Comment ça, mon destin est cadenassé ? Pass-PTT dans la doudoune Le temps a plus de valeur que l'dollar et l'euro, j'm'en occuperai quand j'aurai quelques années de trop J'sais pas si j'me trompe mais pour l'instant, j'suis heureux, l'ignorance fait l'bonheur, woho J'te connais même pas, tu m'prends la tête, laisse-moi vivre le moment À fond sens interdit, meufs assorties avec ma Benz, l'ignorance fait l'bonheur, woho J'suis pas de ceux qui font les choses bien pour les mauvaises raisons Mais de ceux qui agissent par impulsion et après, s'posent des questions J'étais tranquille mais rien ne pouvait donc ça n'allait pas Leur philosophie et tous leurs intérêts ne mimpressionnaient pas Tous ces gens peuvent zapper les leurs pour une opportunité Ils font dans la proximité, ils ont l'esprit limité J'ai mis du temps mais mon arrivée va faire un gros coup d'éclat Si c'est pas moi, c'est mes gars j'suis vainqueur dans tous les cas Le temps a plus de valeur que l'dollar et l'euro, j'm'en occuperai quand j'aurai quelques années de trop J'sais pas si j'me trompe mais pour l'instant, j'suis heureux, l'ignorance fait l'bonheur, woho J'te connais même pas, tu m'prends la tête, laisse-moi vivre le bon moment À fond sens interdit, meufs assorties avec ma Benz, l'ignorance fait l'bonheur, woho</t>
+          <t>J'ai fermé les volets, je ne voulais pas laisser passer la lumière, je compte mes pas Dans le noir de la pièce, c'est là qu'j'écris mes phases quand tu parles de la bête à chaque coup de métal Capuché dans les bails et on fait en scred, t'as les Ça parle de la fin du monde mais pas de la famine, on entend les sirènes et les dits-ban s'taisent J'm'en suis pris dans la tête et ça dès le départ, ils vont dire que j'abuse et raconte des histoires La misère dans le luxe, t'as pas finis d'y croire, j'ai toujours l'impression que c'est la même image Moi, mes priorités, c'est d'abord la famille, t'as su qui on était quand t'as vu mes amis La guerre pour l'anneau, cette année, c'est la nôtre, on s'est préparé Les guignols qui s'amusent mais c'est pas mardi gras, parlent de la fin du monde mais pas d'la faim dans l'monde Mes reufrés sont là, blottit dans l'habitat, parlent de l'appât du gain mais pas d'la faim dans l'monde On fréquente les abîmes, si j'y réponds à l'appel, c'est qu'il le fallait J'ai des preuves à l'appuie, on aura la médaille l'addition s'ra salée J'fais le mal, j'fais le bien, j'suis qu'un homme mais pas comme tout ces camés, pour nous comprendre, il suffit d'un mot On mets l'ambiance comme l'éthanol, mélange de rimes et tu finis accro J'fais le mal, j'fais le bien, j'suis qu'un homme mais pas comme tout ces camés, pour nous comprendre, il suffit d'un mot On met l'ambiance comme l'éthanol mélange de rimes et tu finis accro Dansera pour nos pères, on fait ça pour la médaille Pour t'raconter nos vies avec très peu de détails Dansera pour nos pères, on fait ça pour la médaille Malade est la vie, on veut pas devenir l'bétail Dansera pour nos pères, on fait ça pour la médaille Pour t'raconter nos vies avec très peu de détails Dansera pour nos pères, on fait ça pour la médaille Malade est la vie, on veut pas devenir l'bétail Ces temps-ci, je n'ai pas le sourire, certaines portes ne veulent pas s'ouvrir J'ai l'impression qu'on a sauté mon tour, j'ai peur de tomber dans l'oubli On n'a pas la même rage à la base, personne ne prendra ma place À l'avant de l'avion première classe, avant, c'était fond de la classe On crache le feu, on fait fondre la glace, le tour du net et le tour de l'Atlas Guette dans mes yeux, tu vois l'il de la seum, j'ai le full dans les mains y a la foule dans la salle On m'a dit fais pas ci, on m'a dit fais pas ça, quand j'étais p'tit on m'a dit fais passer Comment aimer sans s'attacher ? Ici, on est que de passage Pas question d'quitter c'monde sans laisser nos marques Toujours pas prêt à porter vos marques, partez Pas question d'quitter c'monde, sans laisser nos marques Toujours pas prêt à porter vos marques Dansera pour nos pères, on fait ça pour la médaille Pour t'raconter nos vies avec très peu de détails Dansera pour nos pères, on fait ça pour la médaille Malade est la vie, on veut pas devenir l'bétail Dansera pour nos pères, on fait ça pour la médaille Pour t'raconter nos vies avec très peu de détails Dansera pour nos pères, on fait ça pour la médaille Malade est la vie, on veut pas devenir l'bétail</t>
         </is>
       </c>
     </row>
@@ -2481,12 +2481,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Médaille</t>
+          <t>Monopole</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>J'ai fermé les volets, je ne voulais pas laisser passer la lumière, je compte mes pas Dans le noir de la pièce, c'est là qu'j'écris mes phases quand tu parles de la bête à chaque coup de métal Capuché dans les bails et on fait en scred, t'as les Ça parle de la fin du monde mais pas de la famine, on entend les sirènes et les dits-ban s'taisent J'm'en suis pris dans la tête et ça dès le départ, ils vont dire que j'abuse et raconte des histoires La misère dans le luxe, t'as pas finis d'y croire, j'ai toujours l'impression que c'est la même image Moi, mes priorités, c'est d'abord la famille, t'as su qui on était quand t'as vu mes amis La guerre pour l'anneau, cette année, c'est la nôtre, on s'est préparé Les guignols qui s'amusent mais c'est pas mardi gras, parlent de la fin du monde mais pas d'la faim dans l'monde Mes reufrés sont là, blottit dans l'habitat, parlent de l'appât du gain mais pas d'la faim dans l'monde On fréquente les abîmes, si j'y réponds à l'appel, c'est qu'il le fallait J'ai des preuves à l'appuie, on aura la médaille l'addition s'ra salée J'fais le mal, j'fais le bien, j'suis qu'un homme mais pas comme tout ces camés, pour nous comprendre, il suffit d'un mot On mets l'ambiance comme l'éthanol, mélange de rimes et tu finis accro J'fais le mal, j'fais le bien, j'suis qu'un homme mais pas comme tout ces camés, pour nous comprendre, il suffit d'un mot On met l'ambiance comme l'éthanol mélange de rimes et tu finis accro Dansera pour nos pères, on fait ça pour la médaille Pour t'raconter nos vies avec très peu de détails Dansera pour nos pères, on fait ça pour la médaille Malade est la vie, on veut pas devenir l'bétail Dansera pour nos pères, on fait ça pour la médaille Pour t'raconter nos vies avec très peu de détails Dansera pour nos pères, on fait ça pour la médaille Malade est la vie, on veut pas devenir l'bétail Ces temps-ci, je n'ai pas le sourire, certaines portes ne veulent pas s'ouvrir J'ai l'impression qu'on a sauté mon tour, j'ai peur de tomber dans l'oubli On n'a pas la même rage à la base, personne ne prendra ma place À l'avant de l'avion première classe, avant, c'était fond de la classe On crache le feu, on fait fondre la glace, le tour du net et le tour de l'Atlas Guette dans mes yeux, tu vois l'il de la seum, j'ai le full dans les mains y a la foule dans la salle On m'a dit fais pas ci, on m'a dit fais pas ça, quand j'étais p'tit on m'a dit fais passer Comment aimer sans s'attacher ? Ici, on est que de passage Pas question d'quitter c'monde sans laisser nos marques Toujours pas prêt à porter vos marques, partez Pas question d'quitter c'monde, sans laisser nos marques Toujours pas prêt à porter vos marques Dansera pour nos pères, on fait ça pour la médaille Pour t'raconter nos vies avec très peu de détails Dansera pour nos pères, on fait ça pour la médaille Malade est la vie, on veut pas devenir l'bétail Dansera pour nos pères, on fait ça pour la médaille Pour t'raconter nos vies avec très peu de détails Dansera pour nos pères, on fait ça pour la médaille Malade est la vie, on veut pas devenir l'bétail</t>
+          <t>Zer 2 , S crew, boy L'entourage bébé Si Dieu le veut, jusqu'à 120 ans Voilà mon espérance de vie Toujours dans lexcellence, tu connais les préférences, on est vraiment des références de style Dans l'équipe aucune défiance, nan On ne tolère pas la médisance, nan On est méfiants, choisis ton camp, au lieu de rester entre deux files, nan Tant que je n'ai pas le million, tous mes égotrips resteront de l'autodérision Besoin de second degré pour quitter ce monde de merde Je me laisse aller avant de prendre une autre décision Trop de menaces et de coup de crasse pour des loves Je le sens tout de suite quand un traître tape mon épaule Ne le vois tu pas, de quoi tu parles à part de ton écho Rester à ma place ce n'est pas dans mon créneau x2 La musique me procure certains sentiments Que je ne pourrais trouver chez aucune femme Même au plumard je reste intransigeant Si t'as pas de son, tu vas lécher mes chaussures sales x2 Peut-être que je commet trop d'erreurs Je peux mentir aussitôt pour ton cul de rêve Peut-être qu'on m'a jeté le mauvais sort Y'a pas que les toxicos qui n'ont plus de veine J'ai l'art desquiver l'angoisse, mais faut que je guette la vérité en face Personne te dévisage, laisse moi guetter le paysage où tu te prends la baie vitrée dans le crane Je n'ai jamais posé mon cul sur les bancs de la fac, bâtiment délabré fallait sauter pour descendre la marche Pendant des années, dans les allées, on vendait de la came Y'avait des enfants de la DASS, cherchant de la maille Qu'il investissait dans le crack ! Je pense que tout le monde veut le monopole Même tes deux nouveaux potes veulent le monopole Donc jespère que tu as bien compris que c'est chacun pour sa peau Même le lapin sous le chapeau veut le monopole Je pense que tout le monde veut le monopole Même tes deux nouveaux potes veulent le monopole Donc jespère que tu as bien compris que c'est chacun pour sa peau Même le lapin sous le chapeau veut le monopole x2 x2</t>
         </is>
       </c>
     </row>
@@ -2498,12 +2498,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Monopole</t>
+          <t>Néon</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Zer 2 , S crew, boy L'entourage bébé Si Dieu le veut, jusqu'à 120 ans Voilà mon espérance de vie Toujours dans lexcellence, tu connais les préférences, on est vraiment des références de style Dans l'équipe aucune défiance, nan On ne tolère pas la médisance, nan On est méfiants, choisis ton camp, au lieu de rester entre deux files, nan Tant que je n'ai pas le million, tous mes égotrips resteront de l'autodérision Besoin de second degré pour quitter ce monde de merde Je me laisse aller avant de prendre une autre décision Trop de menaces et de coup de crasse pour des loves Je le sens tout de suite quand un traître tape mon épaule Ne le vois tu pas, de quoi tu parles à part de ton écho Rester à ma place ce n'est pas dans mon créneau x2 La musique me procure certains sentiments Que je ne pourrais trouver chez aucune femme Même au plumard je reste intransigeant Si t'as pas de son, tu vas lécher mes chaussures sales x2 Peut-être que je commet trop d'erreurs Je peux mentir aussitôt pour ton cul de rêve Peut-être qu'on m'a jeté le mauvais sort Y'a pas que les toxicos qui n'ont plus de veine J'ai l'art desquiver l'angoisse, mais faut que je guette la vérité en face Personne te dévisage, laisse moi guetter le paysage où tu te prends la baie vitrée dans le crane Je n'ai jamais posé mon cul sur les bancs de la fac, bâtiment délabré fallait sauter pour descendre la marche Pendant des années, dans les allées, on vendait de la came Y'avait des enfants de la DASS, cherchant de la maille Qu'il investissait dans le crack ! Je pense que tout le monde veut le monopole Même tes deux nouveaux potes veulent le monopole Donc jespère que tu as bien compris que c'est chacun pour sa peau Même le lapin sous le chapeau veut le monopole Je pense que tout le monde veut le monopole Même tes deux nouveaux potes veulent le monopole Donc jespère que tu as bien compris que c'est chacun pour sa peau Même le lapin sous le chapeau veut le monopole x2 x2</t>
+          <t>S-Crew, tiens Tiens, tiens, tiens La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, cest le néant, quand dans ma tête, c'est le néant La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, cest le néant, quand dans ma tête, c'est le néant La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts Jai accepté la facilité, plus de questions jai réponse à tout J'surveille mon intonation, je filtre les informations Non, ne me prends pas pour un con, tu ne me suivras pas dans ma tombe Je sais qut'étais sur le point de lâcher, t'étais perdu sur le chemin de la paix Le respect t'étais sur le point de lacheter, preuve de lâcheté, maintenant t'es H.S Bientôt, j'me barre au Japon, bientôt, j'me barre au Mexique Normal, on pète les plafonds, élévation stratosphérique Ne crois pas que je me la raconte j'suis juste fier de mon équipe On prend de la place sur la map-monde Plus j'grandis, plus c'monde est petit La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, c'est le néant, quand dans ma tête, c'est le néant La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, c'est le néant, quand dans ma tête, c'est le néant La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout La vérité est dure à digérer mais je ne vais pas cracher le morceau Écrasé par le poids de mes pêchés, ça me fait juste taffer les dorsaux, hey Moi, je n'ai jamais considéré la défaite comme une fatalité Je tourne la page comme un illettré, rien ne m'inquiète, c'est une calamité Si tu me vois douter, c'est qu'à la mi-temps, j'vendais des sachets y a même pas dix ans Si t'as pas d'opinion, je m'en fous d'ce que tu penses, c'est que t'approuves si t'as pas dit nan Pas de ma faute si Paname m'inspire, Paname est sombre comme l'âme d'un flic Tu sais qu'l'État coulera le navire, j'veux rien dire de mal mais c'est mal de rien dire La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, c'est le néant, quand dans ma tête, c'est le néant La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, c'est le néant, quand dans ma tête, c'est le néant La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout</t>
         </is>
       </c>
     </row>
@@ -2515,12 +2515,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Néon</t>
+          <t>Noor</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>S-Crew, tiens Tiens, tiens, tiens La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, cest le néant, quand dans ma tête, c'est le néant La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, cest le néant, quand dans ma tête, c'est le néant La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts Jai accepté la facilité, plus de questions jai réponse à tout J'surveille mon intonation, je filtre les informations Non, ne me prends pas pour un con, tu ne me suivras pas dans ma tombe Je sais qut'étais sur le point de lâcher, t'étais perdu sur le chemin de la paix Le respect t'étais sur le point de lacheter, preuve de lâcheté, maintenant t'es H.S Bientôt, j'me barre au Japon, bientôt, j'me barre au Mexique Normal, on pète les plafonds, élévation stratosphérique Ne crois pas que je me la raconte j'suis juste fier de mon équipe On prend de la place sur la map-monde Plus j'grandis, plus c'monde est petit La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, c'est le néant, quand dans ma tête, c'est le néant La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, c'est le néant, quand dans ma tête, c'est le néant La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout La vérité est dure à digérer mais je ne vais pas cracher le morceau Écrasé par le poids de mes pêchés, ça me fait juste taffer les dorsaux, hey Moi, je n'ai jamais considéré la défaite comme une fatalité Je tourne la page comme un illettré, rien ne m'inquiète, c'est une calamité Si tu me vois douter, c'est qu'à la mi-temps, j'vendais des sachets y a même pas dix ans Si t'as pas d'opinion, je m'en fous d'ce que tu penses, c'est que t'approuves si t'as pas dit nan Pas de ma faute si Paname m'inspire, Paname est sombre comme l'âme d'un flic Tu sais qu'l'État coulera le navire, j'veux rien dire de mal mais c'est mal de rien dire La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, c'est le néant, quand dans ma tête, c'est le néant La nuit tombée, j'aime bien promener ma gova sous les néons Quand dans ma tête, c'est le néant, quand dans ma tête, c'est le néant La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout La vie voudrait me déstabiliser mais j'suis bien dans ma tête, j'ai les bons atouts J'ai accepté la facilité, plus de questions j'ai réponse à tout</t>
+          <t>C'est vrai qu'souvent, la peur m'a neutralisé Si j'suis pas sûr de gagner, je n'veux pas miser Tout seul dans mon salon, lumière tamisée J'me dis qu'il est grand temps de m'organiser J'veux quitter ma dépendance, créer les modes, les tendances Influencer les gens chaque fois qu'mon humeur est changeante La paresse est tentante mais si tu t'tais, personne t'entends Influencer les gens chaque fois qu'mon humeur est changeante Tu gardes les poches vides si ta tête n'est pas remplie Mais sache que si tu réfléchis trop, ça te ralentit Comment avancer sans zapper les dégâts d'hier ? Tout est dans le veau-cer, c'est toi qui crées tes barrières Les problèmes ont de l'importance seulement si t'en donnes T'as même pas vu le gros chèque, t'as jugé la p'tite enveloppe Tu peux pas plaire à tout l'monde, tu peux pas donner quand t'as pas Nique le regard des gens, nan, y en a pas tant qui pensent à toi On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, négro, bah ouais On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, hey On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, négro, bah ouais On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, hey On a grandi dans tous les sens Tu m'as trahi une fois, frérot, honte à toi toi Tu m'as trahi deux fois, toujours honte à toi Quand on donne c'est sans retour, pas de honte à avoir J'veux pas être comme ces vautours, j'veux pas d'cette honte en moi On a grandi dans la 'sère, dis-moi qu'est-c'que tu connais ? J'laisse mes affaires entre tes mains pour voir qu'est-c'que tu commets J'ai dit J'ai grandi dans la 'sère, dis-moi qu'est-c'que tu connais ? J'laisse mes affaires entre tes mains pour voir qu'est-c'que tu commets C'est vrai qu'souvent la peur m'a neutralisé Si j'suis pas sûr de gagner, je n'veux pas miser Tout seul dans mon salon, lumière tamisée J'me dis qu'il est grand temps de m'organiser J'veux quitter ma dépendance, créer les modes, les tendances Influencer les gens chaque fois qu'mon humeur est changeante La paresse est tentante mais si tu t'tais, personne t'entends Influencer les gens chaque fois qu'mon humeur est changeante On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, négro, bah ouais On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, hey On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, négro, bah ouais On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, hey On a grandi dans tous les sens</t>
         </is>
       </c>
     </row>
@@ -2532,12 +2532,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Noor</t>
+          <t>NTDGG</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>C'est vrai qu'souvent, la peur m'a neutralisé Si j'suis pas sûr de gagner, je n'veux pas miser Tout seul dans mon salon, lumière tamisée J'me dis qu'il est grand temps de m'organiser J'veux quitter ma dépendance, créer les modes, les tendances Influencer les gens chaque fois qu'mon humeur est changeante La paresse est tentante mais si tu t'tais, personne t'entends Influencer les gens chaque fois qu'mon humeur est changeante Tu gardes les poches vides si ta tête n'est pas remplie Mais sache que si tu réfléchis trop, ça te ralentit Comment avancer sans zapper les dégâts d'hier ? Tout est dans le veau-cer, c'est toi qui crées tes barrières Les problèmes ont de l'importance seulement si t'en donnes T'as même pas vu le gros chèque, t'as jugé la p'tite enveloppe Tu peux pas plaire à tout l'monde, tu peux pas donner quand t'as pas Nique le regard des gens, nan, y en a pas tant qui pensent à toi On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, négro, bah ouais On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, hey On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, négro, bah ouais On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, hey On a grandi dans tous les sens Tu m'as trahi une fois, frérot, honte à toi toi Tu m'as trahi deux fois, toujours honte à toi Quand on donne c'est sans retour, pas de honte à avoir J'veux pas être comme ces vautours, j'veux pas d'cette honte en moi On a grandi dans la 'sère, dis-moi qu'est-c'que tu connais ? J'laisse mes affaires entre tes mains pour voir qu'est-c'que tu commets J'ai dit J'ai grandi dans la 'sère, dis-moi qu'est-c'que tu connais ? J'laisse mes affaires entre tes mains pour voir qu'est-c'que tu commets C'est vrai qu'souvent la peur m'a neutralisé Si j'suis pas sûr de gagner, je n'veux pas miser Tout seul dans mon salon, lumière tamisée J'me dis qu'il est grand temps de m'organiser J'veux quitter ma dépendance, créer les modes, les tendances Influencer les gens chaque fois qu'mon humeur est changeante La paresse est tentante mais si tu t'tais, personne t'entends Influencer les gens chaque fois qu'mon humeur est changeante On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, négro, bah ouais On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, hey On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, négro, bah ouais On a grandi dans tous les sens, si j't'ai menti, c'est pour t'défendre, hey On a grandi dans tous les sens</t>
+          <t>Zerzer, Hugz Wollop wollop j'suis là depuis l'époque, RIP Nate Dogg Wollop wollop j'suis là depuis l'époque Des fois la vie t'envoie dans les cordes, faut tout détruire changer le décor Prendre racine, durcir ton écorce Rien n'a changé, ouais, depuis l'exode Dans la rue entre potes, des concours d'anecdotes Attends deuspi des couplets j'en ai d'autres Mais avant de commencer RIP Nate Dogg Qui m'a appris à ré-pleu tout en restant thug J'suis parano je garde ma veste dans le club On s'est formé quand c'était la misère donc si c'est mal visser on agresse ton plug T'as du mal à capter si t'es pas dans le délire Faut remplir le belly du baby imbécile Ca nous colle à la peau pas besoin de casting Comme Ray Liotta, De Niro et Joe Pesci J'aime quand l'eau pétille, quand le s'effrite tout seul Parapluie semi-auto pour quand les coups pleuvent J'me sens pas coupable même quand c'est moi le coupable Plaquette découpée dans la Mini Cooper Dans mes écouteurs la prod en rotation J'baise les que-mar j'achète contrefaçon Comme dit Clément nos corps c'est des locations Tu veux t'faire pardonner, maintenant c'est l'occasion Wollop wollop j'suis là depuis l'époque Des fois la vie t'envoie dans les cordes, faut tout détruire changer le décor Prendre racine, durcir ton écorce Rien n'a changé, ouais, depuis l'exode Dans la rue entre potes, des concours d'anecdotes Attends deuspi des couplets j'en ai d'autres Mais avant de commencer RIP Nate Dogg J'ai demandé ma direction hun, ils m'ont indiqué le mur Ils m'ont demandé la discrétion, j'ai tout fait dans la démesure J'ai taffé mon bail dans la pénombre T'es mieux que moi faut que tu l'démontres Si j'connais même pas ton blase Ne m'appelle pas par mon prénom Eduqué par Tupac Amaru, tu veux nous tracer mais ton truc tiens pas la route A Panam' à chaque fois qu'on sort on se camoufle Cur de glace non détecté par l'infrarouge Le passé est à vous, l'avenir est à nous Sale quand tu mens, qu'on te crame et que t'avoue Fais ta monnaie, vaut mieux la jouer soum soum En France l'argent est un sujet tabou Wollop wollop j'suis là depuis l'époque Des fois la vie t'envoie dans les cordes, faut tout détruire changer le décor Prendre racine, durcir ton écorce Rien n'a changé, ouais, depuis l'exode Dans la rue entre potes, des concours d'anecdotes Attends deuspi des couplets j'en ai d'autres Mais avant de terminer RIP Nate Dogg Avant de terminer RIP Nate Dogg ZerZer Wollop wollop j'suis là depuis l'époque Hugzer Hun Hun SZR Putain d'enculé d'ta mère</t>
         </is>
       </c>
     </row>
@@ -2549,12 +2549,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>NTDGG</t>
+          <t>On ne fait qu’avancer</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Zerzer, Hugz Wollop wollop j'suis là depuis l'époque, RIP Nate Dogg Wollop wollop j'suis là depuis l'époque Des fois la vie t'envoie dans les cordes, faut tout détruire changer le décor Prendre racine, durcir ton écorce Rien n'a changé, ouais, depuis l'exode Dans la rue entre potes, des concours d'anecdotes Attends deuspi des couplets j'en ai d'autres Mais avant de commencer RIP Nate Dogg Qui m'a appris à ré-pleu tout en restant thug J'suis parano je garde ma veste dans le club On s'est formé quand c'était la misère donc si c'est mal visser on agresse ton plug T'as du mal à capter si t'es pas dans le délire Faut remplir le belly du baby imbécile Ca nous colle à la peau pas besoin de casting Comme Ray Liotta, De Niro et Joe Pesci J'aime quand l'eau pétille, quand le s'effrite tout seul Parapluie semi-auto pour quand les coups pleuvent J'me sens pas coupable même quand c'est moi le coupable Plaquette découpée dans la Mini Cooper Dans mes écouteurs la prod en rotation J'baise les que-mar j'achète contrefaçon Comme dit Clément nos corps c'est des locations Tu veux t'faire pardonner, maintenant c'est l'occasion Wollop wollop j'suis là depuis l'époque Des fois la vie t'envoie dans les cordes, faut tout détruire changer le décor Prendre racine, durcir ton écorce Rien n'a changé, ouais, depuis l'exode Dans la rue entre potes, des concours d'anecdotes Attends deuspi des couplets j'en ai d'autres Mais avant de commencer RIP Nate Dogg J'ai demandé ma direction hun, ils m'ont indiqué le mur Ils m'ont demandé la discrétion, j'ai tout fait dans la démesure J'ai taffé mon bail dans la pénombre T'es mieux que moi faut que tu l'démontres Si j'connais même pas ton blase Ne m'appelle pas par mon prénom Eduqué par Tupac Amaru, tu veux nous tracer mais ton truc tiens pas la route A Panam' à chaque fois qu'on sort on se camoufle Cur de glace non détecté par l'infrarouge Le passé est à vous, l'avenir est à nous Sale quand tu mens, qu'on te crame et que t'avoue Fais ta monnaie, vaut mieux la jouer soum soum En France l'argent est un sujet tabou Wollop wollop j'suis là depuis l'époque Des fois la vie t'envoie dans les cordes, faut tout détruire changer le décor Prendre racine, durcir ton écorce Rien n'a changé, ouais, depuis l'exode Dans la rue entre potes, des concours d'anecdotes Attends deuspi des couplets j'en ai d'autres Mais avant de terminer RIP Nate Dogg Avant de terminer RIP Nate Dogg ZerZer Wollop wollop j'suis là depuis l'époque Hugzer Hun Hun SZR Putain d'enculé d'ta mère</t>
+          <t>The most XXX shit on the planet right now, brah ! 2009, 2010, c'est pareil, moi, je m'en fous d'tes millénaires J'ai voulu croire en mes amis mais leur lâcheté m'a mis les nerfs Pour me détendre, je manie les vers, je sors le Rap de convalescence Mon son, c'est un bolide, tu veux qu'je fonce ? Envoie l'essence ! Je vois qu'mes potes XXX, y a trop d'mythos qui XXX XXX ta maille ne m'atteint pas même si la somme semble alléchante T'as survécu sans valet d'chambre, arrête d'te plaindre, sois pas méchant J'profite jamais des occasions, depuis tout petit, j'vois pas mes chances J'étais l'meilleur dans la galère pendant qu't'étais l'meilleur en ski Moi, j'veux faire d'l'argent brillamment un peu comme Meyer Lansky Depuis que le Rap est à la mode, elles veulent toutes un bébé métis Mais bon, les gos, ça s'met faya, moi, j'suis déjà imbibé mais j'tise J'ai pas trop d'chances de m'en sortir mais j'suis pas d'ceux qui perdent la foi Heureusement dans l'peu-Ra j'ai un don et je suis si fier de l'avoir La musique passe en premier, tout le reste, c'est secondaire J'te l'arrache dessous les pieds, c'est pour ça qu'j'ai ma seconde herbe On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors on n'fait qu'avancer ! Vers le droit chemin ou celui qui est à gauche À ma destinée j'm'accroche donc, poto, on n'fait qu'avancer ! On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors on n'fait qu'avancer ! J'tape des chorés avec le Diable même si j'sais pas danser Sur le chemin du succès, je n'fais qu'avancer La piété m'sourit pas, pourtant perdu j'casse des barres J'compte avancer dans l'peu-Ra, j'ai déjà vé-squi la case départ C'est bientôt la fin du monde, c'est pour ça qu'j'fais des rations J'nique vos fédérations, j'veux grailler aux frais des nations Moi, c'est 2-zer, j'suis postiché et j'ai la dégaine à l'Antéchrist Peur de personne, ma seule phobie c'est d'avoir une ville hantée triste Métro-boulot-dodo, c'est monotone comme dans Tetris C'est la vue de la tentation et j'ai le vice comme Tentatrice Ne t'attache pas à leurs promesses, tu vas être fortement déçu Ici, les boloss se cachent et les plus forts te montent dessus Pour le biff, tout part en couille, même tes amis veulent t'escroquer Ça veut rentrer dans tes bails mais, eux, c'est rare qu'ils t'laissent croquer Les études, c'est pas pour moi, j'aurai jamais de Bac Litté' Mais j'continue de palpiter, nan, moi, ce monde j'veux pas l'quitter J'veux que mon Rap rapporte du biff, c'est pas une uvre caritative Tu vis l'cauchemar français mais le rêve cain-ri t'attire On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors on n'fait qu'avancer ! Vers le droit chemin ou celui qui est à gauche À ma destinée j'm'accroche donc, poto, on n'fait qu'avancer ! On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors on n'fait qu'avancer ! J'tape des chorés avec le Diable même si j'sais pas danser Sur le chemin du succès, je n'fais qu'avancer On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors... Vers le droit chemin ou celui qui est à gauche À ma destinée j'm'accroche donc, poto... On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors... J'tape des chorés avec le Diable même si j'sais pas danser Sur le chemin du succès, je n'fais qu'avancer</t>
         </is>
       </c>
     </row>
@@ -2566,12 +2566,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>On ne fait qu’avancer</t>
+          <t>PASSWORD</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>The most XXX shit on the planet right now, brah ! 2009, 2010, c'est pareil, moi, je m'en fous d'tes millénaires J'ai voulu croire en mes amis mais leur lâcheté m'a mis les nerfs Pour me détendre, je manie les vers, je sors le Rap de convalescence Mon son, c'est un bolide, tu veux qu'je fonce ? Envoie l'essence ! Je vois qu'mes potes XXX, y a trop d'mythos qui XXX XXX ta maille ne m'atteint pas même si la somme semble alléchante T'as survécu sans valet d'chambre, arrête d'te plaindre, sois pas méchant J'profite jamais des occasions, depuis tout petit, j'vois pas mes chances J'étais l'meilleur dans la galère pendant qu't'étais l'meilleur en ski Moi, j'veux faire d'l'argent brillamment un peu comme Meyer Lansky Depuis que le Rap est à la mode, elles veulent toutes un bébé métis Mais bon, les gos, ça s'met faya, moi, j'suis déjà imbibé mais j'tise J'ai pas trop d'chances de m'en sortir mais j'suis pas d'ceux qui perdent la foi Heureusement dans l'peu-Ra j'ai un don et je suis si fier de l'avoir La musique passe en premier, tout le reste, c'est secondaire J'te l'arrache dessous les pieds, c'est pour ça qu'j'ai ma seconde herbe On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors on n'fait qu'avancer ! Vers le droit chemin ou celui qui est à gauche À ma destinée j'm'accroche donc, poto, on n'fait qu'avancer ! On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors on n'fait qu'avancer ! J'tape des chorés avec le Diable même si j'sais pas danser Sur le chemin du succès, je n'fais qu'avancer La piété m'sourit pas, pourtant perdu j'casse des barres J'compte avancer dans l'peu-Ra, j'ai déjà vé-squi la case départ C'est bientôt la fin du monde, c'est pour ça qu'j'fais des rations J'nique vos fédérations, j'veux grailler aux frais des nations Moi, c'est 2-zer, j'suis postiché et j'ai la dégaine à l'Antéchrist Peur de personne, ma seule phobie c'est d'avoir une ville hantée triste Métro-boulot-dodo, c'est monotone comme dans Tetris C'est la vue de la tentation et j'ai le vice comme Tentatrice Ne t'attache pas à leurs promesses, tu vas être fortement déçu Ici, les boloss se cachent et les plus forts te montent dessus Pour le biff, tout part en couille, même tes amis veulent t'escroquer Ça veut rentrer dans tes bails mais, eux, c'est rare qu'ils t'laissent croquer Les études, c'est pas pour moi, j'aurai jamais de Bac Litté' Mais j'continue de palpiter, nan, moi, ce monde j'veux pas l'quitter J'veux que mon Rap rapporte du biff, c'est pas une uvre caritative Tu vis l'cauchemar français mais le rêve cain-ri t'attire On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors on n'fait qu'avancer ! Vers le droit chemin ou celui qui est à gauche À ma destinée j'm'accroche donc, poto, on n'fait qu'avancer ! On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors on n'fait qu'avancer ! J'tape des chorés avec le Diable même si j'sais pas danser Sur le chemin du succès, je n'fais qu'avancer On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors... Vers le droit chemin ou celui qui est à gauche À ma destinée j'm'accroche donc, poto... On a la mort à nos trousses, jamais on aura nous ouss Et la morale nous pousse alors... J'tape des chorés avec le Diable même si j'sais pas danser Sur le chemin du succès, je n'fais qu'avancer</t>
+          <t>Yeah yah, yeah yah, yeah, yah, yah Han, han, han, han, han, han, han Et c'est ton numéro qui s'affiche, hey, celui qui finit par trois fois 6 Ici, le soleil paraît si près Elle a des valeurs et des principes, moi j'é- moi j'essaie de falsifié C'est danger, danger, les cicatrices n'ont rien changés, j'suis le même Tu connais bien mon name, c'est dans ta bouche qu'il est salé J'ai maladie sans remède, donc j'vais jamais m'en remettre M'appelle pas, j'suis sur messageri Ça prendra deux-trois seconds pour qu'on monte à 100 J'envoie haine sur le monde, moi, j'suis bon qu'à ça Titulaire sur le terrain, j'suis pas remplaçant Tout qui brûle à l'intérieur, j'suis bien qu'en facade Et moi, je n'vole pas, j'tombe et moi, je n'vole pas, j'tombe Sans jamais toucher terre, j'm'endormirai dans la tombe et j'm'endormirai dans la tombe Tous mes res-frè font la même Mamacita veut le password, tous les codes elle veut, elle veut le password De mon cur, de mon téléphone Mamacita veut le password, tous les codes, ouais, ouais, ouais Elle veut savoir combien j'touche et dans mon MDP, combien d'touches Sur combien de meufs, je louche, elle m'prend pour un FDP, elle voit rouge Bête sauvage plutôt farouche, tu vois mes cicatrices aux phalanges J'peux tout plaquer tout d'un coup, comme toujours, j'fais comme ça m'arrange C'est notre nature, on fait la guerre, on parle après J'ai voulu la peau de la tigresse et puis, j'ai fini balafré ouais, ouais J'suis remplis de haine mais j'veux qu'on m'aime très fort Être un bonhomme c'est aussi savoir reconnaître ses torts Et ton humeur est versatile mais t'as gardé ton sex-appeal Quand on se met sur la même ligne, inarrêtable, tu sais qu'ça kill Si t'en as marre, on laisse tomber mais les sentiments vont s'estomper woaw Mon password c'est ma liberté donc j'pourrais jamais t'le donner Et moi, je n'vole pas, j'tombe et moi, je n'vole pas, j'tombe Sans jamais toucher terre, j'm'endormirai dans la tombe et j'm'endormirai dans la tombe Tous mes res-frè font la même Mamacita veut le password, tous les codes ouais, ouais, ouais De mon cur, de mon téléphone Mamacita veut le password, tous les codes, ouais, ouais, ouais Et moi, je n'vole pas, j'tombe et moi, je n'vole pas, j'tombe Sans jamais toucher terre, j'm'endormirai dans la tombe et j'm'endormirai dans la tombe Tous mes res-frè font la même Mamacita veut le password, tous les codes ouais, ouais, ouais De mon cur, de mon téléphone Mamacita veut le password, tous les codes, ouais, ouais, ouais La lune est presque pleine Pourquoi tu doubles le prix ? Moi, j'suis qu'une goûte de pluie Dans une averse d'été Ah ouais, une averse d'été</t>
         </is>
       </c>
     </row>
@@ -2583,12 +2583,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>PASSWORD</t>
+          <t>Peace &amp; Love</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Yeah yah, yeah yah, yeah, yah, yah Han, han, han, han, han, han, han Et c'est ton numéro qui s'affiche, hey, celui qui finit par trois fois 6 Ici, le soleil paraît si près Elle a des valeurs et des principes, moi j'é- moi j'essaie de falsifié C'est danger, danger, les cicatrices n'ont rien changés, j'suis le même Tu connais bien mon name, c'est dans ta bouche qu'il est salé J'ai maladie sans remède, donc j'vais jamais m'en remettre M'appelle pas, j'suis sur messageri Ça prendra deux-trois seconds pour qu'on monte à 100 J'envoie haine sur le monde, moi, j'suis bon qu'à ça Titulaire sur le terrain, j'suis pas remplaçant Tout qui brûle à l'intérieur, j'suis bien qu'en facade Et moi, je n'vole pas, j'tombe et moi, je n'vole pas, j'tombe Sans jamais toucher terre, j'm'endormirai dans la tombe et j'm'endormirai dans la tombe Tous mes res-frè font la même Mamacita veut le password, tous les codes elle veut, elle veut le password De mon cur, de mon téléphone Mamacita veut le password, tous les codes, ouais, ouais, ouais Elle veut savoir combien j'touche et dans mon MDP, combien d'touches Sur combien de meufs, je louche, elle m'prend pour un FDP, elle voit rouge Bête sauvage plutôt farouche, tu vois mes cicatrices aux phalanges J'peux tout plaquer tout d'un coup, comme toujours, j'fais comme ça m'arrange C'est notre nature, on fait la guerre, on parle après J'ai voulu la peau de la tigresse et puis, j'ai fini balafré ouais, ouais J'suis remplis de haine mais j'veux qu'on m'aime très fort Être un bonhomme c'est aussi savoir reconnaître ses torts Et ton humeur est versatile mais t'as gardé ton sex-appeal Quand on se met sur la même ligne, inarrêtable, tu sais qu'ça kill Si t'en as marre, on laisse tomber mais les sentiments vont s'estomper woaw Mon password c'est ma liberté donc j'pourrais jamais t'le donner Et moi, je n'vole pas, j'tombe et moi, je n'vole pas, j'tombe Sans jamais toucher terre, j'm'endormirai dans la tombe et j'm'endormirai dans la tombe Tous mes res-frè font la même Mamacita veut le password, tous les codes ouais, ouais, ouais De mon cur, de mon téléphone Mamacita veut le password, tous les codes, ouais, ouais, ouais Et moi, je n'vole pas, j'tombe et moi, je n'vole pas, j'tombe Sans jamais toucher terre, j'm'endormirai dans la tombe et j'm'endormirai dans la tombe Tous mes res-frè font la même Mamacita veut le password, tous les codes ouais, ouais, ouais De mon cur, de mon téléphone Mamacita veut le password, tous les codes, ouais, ouais, ouais La lune est presque pleine Pourquoi tu doubles le prix ? Moi, j'suis qu'une goûte de pluie Dans une averse d'été Ah ouais, une averse d'été</t>
+          <t>Nekfeu 342 - 427 Quand tout à coup le coup bas, suis-je le coupable ou pas? On s'en fout y'a toute la troupe la pour le Bloopalooza On t'encercle comme un hula hoop Écoute ça sous ta tour, j'avoue Dès que j'ouvre la bouche les loux-ja bougent Mes tou-bab fous leurs foutent la frousse J'parcours la foule et roule un bout Les poules accourent et j'touche un boule C'est nous les bougs de l'entourage Les groupies faites nous l'amour A chaque fois j'entend des Oura tour à tour au rendez yo Nous savourant l'goût d'la bouda et les Humm back de youra J'suis la preuve vivante que les rappeurs ont une peur immense Pas faire des skeuds à la hauteur de vos curs vibrants C'est pour les reufs plein d'honneur dans l'horreur piquante J'pense à un son dont j'suis l'auteur à peine l'heure suivante Remerciment au mec figé sur le même divant Qui m'estime quand j'fais le mec dis mais qu'est ce qui te prend Je t'explique je reste technique et excitant Je mène le flow, j'amène le show jamais je reste quil-tran</t>
         </is>
       </c>
     </row>
@@ -2600,12 +2600,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Peace &amp; Love</t>
+          <t>Place aux vices</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Nekfeu 342 - 427 Quand tout à coup le coup bas, suis-je le coupable ou pas? On s'en fout y'a toute la troupe la pour le Bloopalooza On t'encercle comme un hula hoop Écoute ça sous ta tour, j'avoue Dès que j'ouvre la bouche les loux-ja bougent Mes tou-bab fous leurs foutent la frousse J'parcours la foule et roule un bout Les poules accourent et j'touche un boule C'est nous les bougs de l'entourage Les groupies faites nous l'amour A chaque fois j'entend des Oura tour à tour au rendez yo Nous savourant l'goût d'la bouda et les Humm back de youra J'suis la preuve vivante que les rappeurs ont une peur immense Pas faire des skeuds à la hauteur de vos curs vibrants C'est pour les reufs plein d'honneur dans l'horreur piquante J'pense à un son dont j'suis l'auteur à peine l'heure suivante Remerciment au mec figé sur le même divant Qui m'estime quand j'fais le mec dis mais qu'est ce qui te prend Je t'explique je reste technique et excitant Je mène le flow, j'amène le show jamais je reste quil-tran</t>
+          <t>J'suis mauvais joueur mais pas mauvais perdant J'me perds dans mes phases avant de té-sau j'prends mon élan J'dois laisser mes traces Des enflures m'ont niqué à coup de flux monétaires A quoi bon communiquer ? J'veux pas finir prolétaire J'ferai simple, trop de complexité Fais d'la compèt' si t'es beaucoup trop excité J'te l'expliquen mon lexique n'est pas celui d'un amateur C'est d'ma vie que j'te parle j'ai la technique d'un narrateur J'ai l'flow a Bénabar, j'vois flou j'ai peine à croire Trop d'gens se baisent à Paris pour une Porsche ou des appart' La musique me désempare, pour le son des gens partent J'voudrais qu'ce soit rentable mais devant moi j'vois des remparts Malgré tout je n'change pas, j'fais du mal aux semblables Poto j'te l'dis sans blague Calme toi si ça s'emballe Face à toi j'me sens mal, tu tuerais pour cent balles Et la plupart s'en bat les couilles de niquer son bail Les gens me débectent, j'te l'dis, j'le crie et j'le répète Si tu m'respectes, tâche d'oublier tes vieux réflexes Face à nous des barrières qu'on peut franchir mais trop peu d'franchise La galère me vise mais elle se trompe de cible J'confonds mes rêves et mes souvenirs Les yeux fermés n'ont qu'à s'ouvrir Mes cauchemars souvent aux films de Mathieu Kassovitz Mes rêves et mes souvenirs, les yeux fermés n'ont qu'à s'ouvrir Mes cauchemars ressemblent souvent aux films de Mathieu Kassovitz Tu vois la haine dans nos prunelles comme le sang sur l'opinel Vas y expose ton opinion y'à que les anges qui n'ont plus d'ailes La vie est belle, mais de loin, moi je lève mes deux doigts Pas besoin d'un médecin même si je hurlais de mort Si je peu-ra c'est pour la gloire mais j'me contenterai d'un fan Tu t'vantes de tes histoires pendant que par ici y'a foy Y'en a qui baise des putes pendant la journée de la femme Je vis à 100 à l'heure, devant moi les radars s'affolent De Panam à Los Angelès poto j'ai le sang gelé Tu pourras trouver tout mes sons près du rayon surgelé C'est pour les prolétaires, les mots j'déterre, j'suis trop déter', y'a pas d'été Içi ça galère d't'façon j'resterai sur la planète Terre Pourquoi l'économie nécrologique n'fait qu'augmenter, c'est pas logique Les go dominent, l'écologie te font virer de tologie L'anorexie morphologique te pousse à faire des morceaux logiques Les MC tombent dans la folie et pensent que la mort communique J'vois les boloss parler d'AK car j'leur ai dit que j'parlerai ap' La vengeance se mange très froide, pour l'instant j'avance par étape J'suis innocent, croyez moi, j'ai la dalle d'un foyer man J'pète un câble à cause du biff qui m'force à côtoyer l'mal J'touche aucun euro par mois, les keufs trop chauds parlent mal Ma vie n'a pas changé après la victoire d'Obama C'est le H pour la Haine et le V pour Vendetta Ouais poto j'viens du 20ème, élevé près d'Gambetta Les yeux d'ma mère m'amènent souvent à prendre le droit chemin 18 piges toujours aussi bête, l'école n'a plus de droit sur moi J'fais des conneries et j'assume pas depuis l'époque Jurassic Park J'fais des promesses et je les tiens, enfin du moins jusqu'à c'qu'ils partent Ouais poto j'suis dans ma bulle j'regarde à peine les alentours J'veux pas foutre ma vie en l'air bah malgré tout faut que j'aille en cours Mon objectif Toujours mieux, il faut percer les horizons Ceux qui sont dans le faux penseront toujours qu'ils ont raison</t>
         </is>
       </c>
     </row>
@@ -2617,12 +2617,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Place aux vices</t>
+          <t>Plus que toi</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>J'suis mauvais joueur mais pas mauvais perdant J'me perds dans mes phases avant de té-sau j'prends mon élan J'dois laisser mes traces Des enflures m'ont niqué à coup de flux monétaires A quoi bon communiquer ? J'veux pas finir prolétaire J'ferai simple, trop de complexité Fais d'la compèt' si t'es beaucoup trop excité J'te l'expliquen mon lexique n'est pas celui d'un amateur C'est d'ma vie que j'te parle j'ai la technique d'un narrateur J'ai l'flow a Bénabar, j'vois flou j'ai peine à croire Trop d'gens se baisent à Paris pour une Porsche ou des appart' La musique me désempare, pour le son des gens partent J'voudrais qu'ce soit rentable mais devant moi j'vois des remparts Malgré tout je n'change pas, j'fais du mal aux semblables Poto j'te l'dis sans blague Calme toi si ça s'emballe Face à toi j'me sens mal, tu tuerais pour cent balles Et la plupart s'en bat les couilles de niquer son bail Les gens me débectent, j'te l'dis, j'le crie et j'le répète Si tu m'respectes, tâche d'oublier tes vieux réflexes Face à nous des barrières qu'on peut franchir mais trop peu d'franchise La galère me vise mais elle se trompe de cible J'confonds mes rêves et mes souvenirs Les yeux fermés n'ont qu'à s'ouvrir Mes cauchemars souvent aux films de Mathieu Kassovitz Mes rêves et mes souvenirs, les yeux fermés n'ont qu'à s'ouvrir Mes cauchemars ressemblent souvent aux films de Mathieu Kassovitz Tu vois la haine dans nos prunelles comme le sang sur l'opinel Vas y expose ton opinion y'à que les anges qui n'ont plus d'ailes La vie est belle, mais de loin, moi je lève mes deux doigts Pas besoin d'un médecin même si je hurlais de mort Si je peu-ra c'est pour la gloire mais j'me contenterai d'un fan Tu t'vantes de tes histoires pendant que par ici y'a foy Y'en a qui baise des putes pendant la journée de la femme Je vis à 100 à l'heure, devant moi les radars s'affolent De Panam à Los Angelès poto j'ai le sang gelé Tu pourras trouver tout mes sons près du rayon surgelé C'est pour les prolétaires, les mots j'déterre, j'suis trop déter', y'a pas d'été Içi ça galère d't'façon j'resterai sur la planète Terre Pourquoi l'économie nécrologique n'fait qu'augmenter, c'est pas logique Les go dominent, l'écologie te font virer de tologie L'anorexie morphologique te pousse à faire des morceaux logiques Les MC tombent dans la folie et pensent que la mort communique J'vois les boloss parler d'AK car j'leur ai dit que j'parlerai ap' La vengeance se mange très froide, pour l'instant j'avance par étape J'suis innocent, croyez moi, j'ai la dalle d'un foyer man J'pète un câble à cause du biff qui m'force à côtoyer l'mal J'touche aucun euro par mois, les keufs trop chauds parlent mal Ma vie n'a pas changé après la victoire d'Obama C'est le H pour la Haine et le V pour Vendetta Ouais poto j'viens du 20ème, élevé près d'Gambetta Les yeux d'ma mère m'amènent souvent à prendre le droit chemin 18 piges toujours aussi bête, l'école n'a plus de droit sur moi J'fais des conneries et j'assume pas depuis l'époque Jurassic Park J'fais des promesses et je les tiens, enfin du moins jusqu'à c'qu'ils partent Ouais poto j'suis dans ma bulle j'regarde à peine les alentours J'veux pas foutre ma vie en l'air bah malgré tout faut que j'aille en cours Mon objectif Toujours mieux, il faut percer les horizons Ceux qui sont dans le faux penseront toujours qu'ils ont raison</t>
+          <t>Je débarque avec v'là l'équipe On balance toute notre Amérique Si tu nous croises dans le carré VIP C'est qu'on mouille le maillot à la Lavezzi Sur scène, en stud, vois l'esprit C'est l'bordel comme en Palestine Même mes potes qui fument pas de weed Face aux flics deviennent amnésique Tu veux test, sois pas débile, trop dappétit pour être athlétique Ta destinée paraît si pathétique Pourquoi ? Car t'as pas d'éthique Mamen, j'arrête la résine, Paris, on dit quoi ? Je t'achève avec ma rétine Eff Gee Uchiwa ×4 Qui va test Killa Eff ? Un pour toi, deux pour moi J'en veux toujours plus que toi Trois pour toi, quatre pour moi J'en veux toujours plus que toi Dix pour toi, cent pour moi J'en veux toujours plus que toi Mille pour toi, dix mille pour moi J'en veux toujours plus que toi Mon, gars, j'ai pas d'patron, j'suis sur d'mes plans De la scène à la tombe, j'reste sur les planches Gare à Gee Eff car j'arrive, mec, ça va vite faire badabim J'gagne la mise et j'pars habiter sur la cote au paradis ×4 Pour mes pistoleros qui veulent toujours plus que les autres Toujours plus de dineros, connecté à tous les réseaux Marre de rouler des joints sous les préaux Donc on t'envoie de lAmérique Ouais, tu peux chier dans les quartiers riches C'que tu bouffes dans les ghettos Si tu montes à bord du vaisseau, la fast life est garantie Aucun dos dâne ne nous ralentit, on voit les jaloux dans le rétro T'as de l'ambition, on se connaît, on a des atomes crochus Tous les rappeurs que je connais sont des rappeurs connus Souvent je suis sous gros spliff mais j'suis un futur nouveau riche Nouveau riche, vous pouvez garder tous vos speechs Souvent je suis sous gros spliff mais j'suis un futur nouveau riche Nouveau riche, courez acheter tous nos disques Un pour toi, deux pour moi J'en veux toujours plus que toi Trois pour toi, quatre pour moi J'en veux toujours plus que toi Cinquante pour toi, dix mille pour moi J'en veux toujours plus que toi Un million pour toi, trois millions pour moi J'en veux toujours plus que toi ×6</t>
         </is>
       </c>
     </row>
@@ -2634,12 +2634,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Plus que toi</t>
+          <t>Pop</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Je débarque avec v'là l'équipe On balance toute notre Amérique Si tu nous croises dans le carré VIP C'est qu'on mouille le maillot à la Lavezzi Sur scène, en stud, vois l'esprit C'est l'bordel comme en Palestine Même mes potes qui fument pas de weed Face aux flics deviennent amnésique Tu veux test, sois pas débile, trop dappétit pour être athlétique Ta destinée paraît si pathétique Pourquoi ? Car t'as pas d'éthique Mamen, j'arrête la résine, Paris, on dit quoi ? Je t'achève avec ma rétine Eff Gee Uchiwa ×4 Qui va test Killa Eff ? Un pour toi, deux pour moi J'en veux toujours plus que toi Trois pour toi, quatre pour moi J'en veux toujours plus que toi Dix pour toi, cent pour moi J'en veux toujours plus que toi Mille pour toi, dix mille pour moi J'en veux toujours plus que toi Mon, gars, j'ai pas d'patron, j'suis sur d'mes plans De la scène à la tombe, j'reste sur les planches Gare à Gee Eff car j'arrive, mec, ça va vite faire badabim J'gagne la mise et j'pars habiter sur la cote au paradis ×4 Pour mes pistoleros qui veulent toujours plus que les autres Toujours plus de dineros, connecté à tous les réseaux Marre de rouler des joints sous les préaux Donc on t'envoie de lAmérique Ouais, tu peux chier dans les quartiers riches C'que tu bouffes dans les ghettos Si tu montes à bord du vaisseau, la fast life est garantie Aucun dos dâne ne nous ralentit, on voit les jaloux dans le rétro T'as de l'ambition, on se connaît, on a des atomes crochus Tous les rappeurs que je connais sont des rappeurs connus Souvent je suis sous gros spliff mais j'suis un futur nouveau riche Nouveau riche, vous pouvez garder tous vos speechs Souvent je suis sous gros spliff mais j'suis un futur nouveau riche Nouveau riche, courez acheter tous nos disques Un pour toi, deux pour moi J'en veux toujours plus que toi Trois pour toi, quatre pour moi J'en veux toujours plus que toi Cinquante pour toi, dix mille pour moi J'en veux toujours plus que toi Un million pour toi, trois millions pour moi J'en veux toujours plus que toi ×6</t>
+          <t>How to you fricken crap face get out here You suck your so stupid Holy crap you do not no What you are holy crap crap Holy lot crap Look you got nothing to me You suck your crap Oh my gosh you idiot who are you yoy you piece of crap You suck crap Holy crap holy crap Repeat me frick you holy crap</t>
         </is>
       </c>
     </row>
@@ -2651,12 +2651,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Pop</t>
+          <t>PROCHAINE VAGUE</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>How to you fricken crap face get out here You suck your so stupid Holy crap you do not no What you are holy crap crap Holy lot crap Look you got nothing to me You suck your crap Oh my gosh you idiot who are you yoy you piece of crap You suck crap Holy crap holy crap Repeat me frick you holy crap</t>
+          <t>Et j'ai fini par m'y faire Jsuis défoncé comme hier Mmmm je veux pas m'réveiller Mmmm j'en ai marre dessayer Jsuis sur Paname et on s'tue pour la monnaie, ah ouais Jsuis sur le terrain et au stud toi tu connais, ah ouais Mmmm j'en ai marre d'essayer Mmmm mais j'ai fini par m'y faire Toujours à lheure comme la muerte De vendredi à vendredi Rien à graille à part ma fierté Donc j'me rendort le ventre vide Demain j'y retourne encore et encore et encore, ouais Pourquoi j'y retourne encore et encore et encore Et j'suis carré comme Elle m'a demandé du love mais j'ai pas vraiment l'time Mais j'ai pas vraiment ltime Elle m'a demandé du love mais bon c'est pas rentable Aussi carré comme d'hab J'me rallume une garette-ci mais ça passe pas J'fais des cauchemars très précis, j'rêve en 4K J'attends la passe décisive Mon coeur est devenu muet j'pleure des larmes invisibles Que des larmes J'suis dans l'pe-ra ça fait 10 ans, qu'est-ce qu'une minute ? Va t'faire enculo j'bois au goulot pour mieux faire passer la pilule Faut pas clubber 9-10 minutes Donc ne mattends pas pour diner Dans ce milieu trop d'putes Moi faut pas m'assimiler J'suis presque mort j'ai l'air en forme à côté d'eux ouais Giro giro dans l'tieks tout est bleu ouais Dans la cabine c'est le fuego Mes gars démarrent quand j'dis le'go La première goutte annonce lorage La conso large mais j'coule sans nager Bébé faut stopper l'hémorragie Ou le H faut qu'on gravite La fin est courte et tragique Faire son cash comme tour de magie, yeah</t>
         </is>
       </c>
     </row>
@@ -2668,12 +2668,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>PROCHAINE VAGUE</t>
+          <t>Puff Puff</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Et j'ai fini par m'y faire Jsuis défoncé comme hier Mmmm je veux pas m'réveiller Mmmm j'en ai marre dessayer Jsuis sur Paname et on s'tue pour la monnaie, ah ouais Jsuis sur le terrain et au stud toi tu connais, ah ouais Mmmm j'en ai marre d'essayer Mmmm mais j'ai fini par m'y faire Toujours à lheure comme la muerte De vendredi à vendredi Rien à graille à part ma fierté Donc j'me rendort le ventre vide Demain j'y retourne encore et encore et encore, ouais Pourquoi j'y retourne encore et encore et encore Et j'suis carré comme Elle m'a demandé du love mais j'ai pas vraiment l'time Mais j'ai pas vraiment ltime Elle m'a demandé du love mais bon c'est pas rentable Aussi carré comme d'hab J'me rallume une garette-ci mais ça passe pas J'fais des cauchemars très précis, j'rêve en 4K J'attends la passe décisive Mon coeur est devenu muet j'pleure des larmes invisibles Que des larmes J'suis dans l'pe-ra ça fait 10 ans, qu'est-ce qu'une minute ? Va t'faire enculo j'bois au goulot pour mieux faire passer la pilule Faut pas clubber 9-10 minutes Donc ne mattends pas pour diner Dans ce milieu trop d'putes Moi faut pas m'assimiler J'suis presque mort j'ai l'air en forme à côté d'eux ouais Giro giro dans l'tieks tout est bleu ouais Dans la cabine c'est le fuego Mes gars démarrent quand j'dis le'go La première goutte annonce lorage La conso large mais j'coule sans nager Bébé faut stopper l'hémorragie Ou le H faut qu'on gravite La fin est courte et tragique Faire son cash comme tour de magie, yeah</t>
+          <t>x4 Allume ce joint Tire sur ce joint Une taffe de plus Un taf de moins Puff puff, comme dirai le Z.E.U Pas d'bluff, que des bédos purs dans l'obscurité C'est absurde je sais mais trouve pas le sommeil sans Ce zbar de fumée dans lequel mes frérots suent J'opère le truc avec mes connaissances Épauler mes collègues pour décoller, faut canaliser l'instant Appelant le H et parait paro Et pour l'occas' j'ai caler mes galos entre les jambes de ta vierge frère Trop d'flow pour serpillière Fier jusqu'au bout le Panama s'écartera du trou S'approchera du palace on vous écarte tous Finir à Dallas, on contemple le flouz, fou Pour le L apostrophe Lache le balai pour le juice avale la phase avec tes gosses, fuck Crache la haine sur l'anti-pop Ouais depuis toujours anti-cops J'veux pas du garde du corps, du compte à Bill Gates Ni porter le roro dans les peu-cli, faire le petit d'tess Défoncé j'essaie de voir le bout du tunnel vite, fait Le vide avant qu'un bâtard t'fume en ville et qu'aucun type t'aide Solo j'ai du faire avec des regrets dans ma ville, j'reste Blessé par ceux qui voulaient qu'on fasse le truc en briques, bref J'ai prouvé la force en moi en maniant la plume, j'laisse Le temps maquiller les drames, té-ma mes scards-la vite naissent Hé, avec mes gavas j'cherche les billets vite Rappe des frappes à l'occas', les cris remplacent la peine au mic Apprécié par les vrais, les rageux parlent on crée le mythe Tu payes le prix l'ivresse, les vrais ennuis remplacent la paix, le rire Partir et voir la mer une fois par an c'est pas la vie Certains voudraient qu'on tombe mais nique on connait pas la suite 7.5 on fait les bails en soum le soir sous cannabis Quand trop d'eux parlent en mime mes scards-la vivent attirés par la rime x2 Allume ce joint Tire sur ce joint Une taffe de plus Un taf de moins Dans l'équipe, on est tous tête d'affiche Pour nous cotoyer, tu trouves des tactiques C'est pratique, car vos cartes de visite Me servent de ton-car pour rouler ma weed Mon crew les fascine C'est mérité ne croie pas que tout est facile Merde, tu ne pourras pas t'envoler Temps que tu n'auras pas goûter l'tapis Ton honnêteté reste à vérifier Qui dit que t'as pas jeté mes disques à la poubelle Fais confiance à ceux qui cherchent la vérité Mais doute de ceux qui te disent l'avoir trouvé Wesh D6, wesh Hakim, wesh Ormaz On mérite les Grammy, les Awards Des livres sterling, des dollars Pour faire demi-tour c'est trop tard XXX J'en ferai d'la fumée J'rentre dans l'jeu Les dés sont jetés J'gratte mes pensées sombres durant mes nuits blanches Si je marche au pas c'est simple, c'est que l'herbe est dense, boy Tu sais c'est pas si dur de sortir le com-com les palaces Hormis les bails de hasch', j'mets 2 heures à faire mon khaliss J'glisse, miss, j'ai besoin d'un fils Viens pas m'sucer la bite si j'n'ai qu'une galère de feat J'surine pour mettre bien la miff On veut tous des palaces mais le tout c'est de le remplir x3 Allume ce joint Tire sur ce joint Une taffe de plus Un taf de moins2</t>
         </is>
       </c>
     </row>
@@ -2685,12 +2685,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Puff Puff</t>
+          <t>Rien ne va plus</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>x4 Allume ce joint Tire sur ce joint Une taffe de plus Un taf de moins Puff puff, comme dirai le Z.E.U Pas d'bluff, que des bédos purs dans l'obscurité C'est absurde je sais mais trouve pas le sommeil sans Ce zbar de fumée dans lequel mes frérots suent J'opère le truc avec mes connaissances Épauler mes collègues pour décoller, faut canaliser l'instant Appelant le H et parait paro Et pour l'occas' j'ai caler mes galos entre les jambes de ta vierge frère Trop d'flow pour serpillière Fier jusqu'au bout le Panama s'écartera du trou S'approchera du palace on vous écarte tous Finir à Dallas, on contemple le flouz, fou Pour le L apostrophe Lache le balai pour le juice avale la phase avec tes gosses, fuck Crache la haine sur l'anti-pop Ouais depuis toujours anti-cops J'veux pas du garde du corps, du compte à Bill Gates Ni porter le roro dans les peu-cli, faire le petit d'tess Défoncé j'essaie de voir le bout du tunnel vite, fait Le vide avant qu'un bâtard t'fume en ville et qu'aucun type t'aide Solo j'ai du faire avec des regrets dans ma ville, j'reste Blessé par ceux qui voulaient qu'on fasse le truc en briques, bref J'ai prouvé la force en moi en maniant la plume, j'laisse Le temps maquiller les drames, té-ma mes scards-la vite naissent Hé, avec mes gavas j'cherche les billets vite Rappe des frappes à l'occas', les cris remplacent la peine au mic Apprécié par les vrais, les rageux parlent on crée le mythe Tu payes le prix l'ivresse, les vrais ennuis remplacent la paix, le rire Partir et voir la mer une fois par an c'est pas la vie Certains voudraient qu'on tombe mais nique on connait pas la suite 7.5 on fait les bails en soum le soir sous cannabis Quand trop d'eux parlent en mime mes scards-la vivent attirés par la rime x2 Allume ce joint Tire sur ce joint Une taffe de plus Un taf de moins Dans l'équipe, on est tous tête d'affiche Pour nous cotoyer, tu trouves des tactiques C'est pratique, car vos cartes de visite Me servent de ton-car pour rouler ma weed Mon crew les fascine C'est mérité ne croie pas que tout est facile Merde, tu ne pourras pas t'envoler Temps que tu n'auras pas goûter l'tapis Ton honnêteté reste à vérifier Qui dit que t'as pas jeté mes disques à la poubelle Fais confiance à ceux qui cherchent la vérité Mais doute de ceux qui te disent l'avoir trouvé Wesh D6, wesh Hakim, wesh Ormaz On mérite les Grammy, les Awards Des livres sterling, des dollars Pour faire demi-tour c'est trop tard XXX J'en ferai d'la fumée J'rentre dans l'jeu Les dés sont jetés J'gratte mes pensées sombres durant mes nuits blanches Si je marche au pas c'est simple, c'est que l'herbe est dense, boy Tu sais c'est pas si dur de sortir le com-com les palaces Hormis les bails de hasch', j'mets 2 heures à faire mon khaliss J'glisse, miss, j'ai besoin d'un fils Viens pas m'sucer la bite si j'n'ai qu'une galère de feat J'surine pour mettre bien la miff On veut tous des palaces mais le tout c'est de le remplir x3 Allume ce joint Tire sur ce joint Une taffe de plus Un taf de moins2</t>
+          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
         </is>
       </c>
     </row>
@@ -2702,12 +2702,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Rien ne va plus</t>
+          <t>Routine</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Han, vive mon rap, mon label, vive mon tieks, mon squa, mon équipe Si t'as pas réparé ta faute et qu'tu t'excuses, crois pas qu'on est quittes Yo, yo, vive mon cash, mon liquide, vive les clashs, nique la politique Vive le sucre, le gras saturé, les truffes râpées sur ma purée C'est au PSG que j'voulais jouer, pas à Joué-lès-Tours Pour cer-per', crois pas qu'le tour est joué ou ça va t'jouer des tours, hey Ma mère séchait mes affaires pendant qu'j'séchais les cours Je bosse pour la moula mais, n attendant, j'la fais ner-tour', hey On graill pas chez Courtepaille, on est un cauchemar pour ces chefs Chez nous, personne ne tire la courte paille, on préfère la courte échelle J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème Cheff Gee, James Deen, Framal Pacino, 2zer Washington Baby, on sort du casino pour braquer Babylone On met l'blase en capital sur l'Capitol, hey, hey Deux cent à l'heure, le cabriolet fait des cabrioles Le navire a sombré, le ciel s'est assombri Loin des terrasses, les rats sont rassemblés et Dieu fera son tri Ouais, ouais, ouais, tout l'monde veut faire son blé, 's ont toujours pas compris Qu'à la fin, tout l'monde paiera son prix, et c'est pour ça qu'on prie Rien n'est gratuit, j'parle comme un ayatollah, vit comme un mécréant La vie que je mène n'amène que paranoïa, le nez dans mes créances Un cur de glace sous la Patagonia, le savoir d'un vétéran Frais comme un rookie, ppe-fra sur la pookie, j'bricole, j'ai pas d'outil J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème J'graille du gastro, j'graille du grec, j'écoute du Pusha, j'écoute du Drake En fait, j't'emmerde j'suis comme ta grand-mère, ça fait déjà longtemps que j'ai plus d'règles J'traîne avec des cas soc' et des bac' plus, des dealers et des cadres sup' Des braqueurs et un banquier, tous ont la mentale de contrebandiers Haut les mains, j'braque ces comédiens déguisés en rappeurs Mais, quand faut kicker, ça parle coréen, norvégien ou indonésien On coupe la parole ou la langue aux témoins, j'devrais m'droguer moins Les bitchs ou l'amour en voilà un choix cornélien Demain, tout ira mieux, pas l'temps d'se chamailler Pour pas qu'nos femmes s'habillent chez Camaïeu, il reste plus qu'à mailler Mes saboteurs veulent que je sois mafieux, ma mère que je sois marié J'suis là, j'profite, d'façon, j'me vois pas vieux, j'ai pas l'temps d'être casanier Ouais, ouais, ouais, même si j'pars travailler en survêt' à damier Crois-moi, je cravache comme un cavalier, taffe plus qu'un salarié J'arrive à l'hôtel et j'vide mon sac, j'arrive en cabine et j'vide mon sac Trop dans la tête pour écrire un thème, trop dans la tête pour écrire un thème On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom On veut les fonds, la caisse, on roule à fond la caisse, vroom, vroom On roule à fond la caisse, on veut les fonds, la caisse, vroom, vroom1</t>
+          <t>Besoin de ta tise hein, besoin de ta weed hein Besoin de te rassasier faut qu'tu te ressaisisses hein Ils veulent que tu restes assis et que tobéisses bien L'État te vend sa dope, cette vie t'épuise hein J'appelle au boycott de ce système, pour la richesse on a pas les critères Pendant que tu fais du Lollipop, on pousse des cris de guerre On taffe avec des émissaires des deux hémisphères Balance une clope hein, si t'as le mal de vivre On a l'antidote hein Des millions de lions, pas trop d'antilopes hein Moi j'me porte bien, personne me manipule même si j'viens d'la porte de Pantin Pour résoudre des 'blèmes, suffit d'imprimer plus de dollars Mais l'égalité va nuire à leur équilibre On a les épaules larges, poto on a trop vu de polars On sait que la banque a créé l'Etat à son effigie Demande à Eff Gee, dans le 19 y a des petits qui ont perdu l'appétit Peu à peu, arrêtent de vivre Car la déprime vient souvent avec le crime Mélangé à du haschich, accompagné de nicotine J'enterre la paix comme un cri de guerre Aucun rescapé, ennemi au cimetière Parmi les miens, mille et une vies de merde Donc j'enterre la paix comme un cri de guerre Tu roules ton pers' alors qu'y a des potes à côté T'es trop gâté, personne te force à bosser Demande à JB, deux barres on fait tourner Espèce de crevard, on va devoir te dépouiller Nos plans soirées, en vrai c'est que des bourbiers Donc ça freestyle, tu ferais mieux d'écouter Comme à me-Da, tu peux en prendre de la graine Tu comprendras que l'amour engendre la haine Et la paix engendre la guerre Aucune justice pour les enfants de la terre Moi j'veux traverser le monde sans prendre d'affaires Fuck le rap game, marre d'entendre de la merde À quoi bon vivre, hein, si personne n'est libre hein Tous les habitants du monde sont mes riverains Petit Parisien survole les méridiens Ma vie, un livre hein, Dieu en est l'écrivain Hein.. Nan, naaaan x2 J'enterre la paix comme un cri de guerre Aucun rescapé, ennemi au cimetière Parmi les miens, mille et une vies de merde Donc j'enterre la paix comme un cri de guerre J'constate que Paris n'est pas le centre du monde Quand je regarde l'horizon sur une colline de Mexico Pour vivre ce que je vis, combien s'entretueront Des gens rêvent d'être avec moi comme les copines de mes rivaux Rien n'est impossible accompagné de mes apôtres On peut échapper à la Gestapo par un tunnel comme El Chapo J'avoue, j'ai dérapé quand mamacita m'a dit papi que padre Nan j'étais pas prêt J'parcours la calle, j'me dis que j'suis prêt à caner Pour palper le million avant mes 30 balais Nan y a pas de quoi s'emballer, si tu passes ton temps à bailler Faut palper le million avant de s'en aller, yeah J'enterre la paix comme un cri de guerre Aucun rescapé, ennemi au cimetière Parmi les miens, mille et une vies de merde Donc j'enterre la paix comme un cri de guerre2</t>
         </is>
       </c>
     </row>
@@ -2719,12 +2719,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Routine</t>
+          <t>Sans demander</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Besoin de ta tise hein, besoin de ta weed hein Besoin de te rassasier faut qu'tu te ressaisisses hein Ils veulent que tu restes assis et que tobéisses bien L'État te vend sa dope, cette vie t'épuise hein J'appelle au boycott de ce système, pour la richesse on a pas les critères Pendant que tu fais du Lollipop, on pousse des cris de guerre On taffe avec des émissaires des deux hémisphères Balance une clope hein, si t'as le mal de vivre On a l'antidote hein Des millions de lions, pas trop d'antilopes hein Moi j'me porte bien, personne me manipule même si j'viens d'la porte de Pantin Pour résoudre des 'blèmes, suffit d'imprimer plus de dollars Mais l'égalité va nuire à leur équilibre On a les épaules larges, poto on a trop vu de polars On sait que la banque a créé l'Etat à son effigie Demande à Eff Gee, dans le 19 y a des petits qui ont perdu l'appétit Peu à peu, arrêtent de vivre Car la déprime vient souvent avec le crime Mélangé à du haschich, accompagné de nicotine J'enterre la paix comme un cri de guerre Aucun rescapé, ennemi au cimetière Parmi les miens, mille et une vies de merde Donc j'enterre la paix comme un cri de guerre Tu roules ton pers' alors qu'y a des potes à côté T'es trop gâté, personne te force à bosser Demande à JB, deux barres on fait tourner Espèce de crevard, on va devoir te dépouiller Nos plans soirées, en vrai c'est que des bourbiers Donc ça freestyle, tu ferais mieux d'écouter Comme à me-Da, tu peux en prendre de la graine Tu comprendras que l'amour engendre la haine Et la paix engendre la guerre Aucune justice pour les enfants de la terre Moi j'veux traverser le monde sans prendre d'affaires Fuck le rap game, marre d'entendre de la merde À quoi bon vivre, hein, si personne n'est libre hein Tous les habitants du monde sont mes riverains Petit Parisien survole les méridiens Ma vie, un livre hein, Dieu en est l'écrivain Hein.. Nan, naaaan x2 J'enterre la paix comme un cri de guerre Aucun rescapé, ennemi au cimetière Parmi les miens, mille et une vies de merde Donc j'enterre la paix comme un cri de guerre J'constate que Paris n'est pas le centre du monde Quand je regarde l'horizon sur une colline de Mexico Pour vivre ce que je vis, combien s'entretueront Des gens rêvent d'être avec moi comme les copines de mes rivaux Rien n'est impossible accompagné de mes apôtres On peut échapper à la Gestapo par un tunnel comme El Chapo J'avoue, j'ai dérapé quand mamacita m'a dit papi que padre Nan j'étais pas prêt J'parcours la calle, j'me dis que j'suis prêt à caner Pour palper le million avant mes 30 balais Nan y a pas de quoi s'emballer, si tu passes ton temps à bailler Faut palper le million avant de s'en aller, yeah J'enterre la paix comme un cri de guerre Aucun rescapé, ennemi au cimetière Parmi les miens, mille et une vies de merde Donc j'enterre la paix comme un cri de guerre2</t>
+          <t>Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah1</t>
         </is>
       </c>
     </row>
@@ -2736,12 +2736,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Sans demander</t>
+          <t>Satoshi Nakamoto</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Nan, nan, nan, nan, eh Nan, nan, nan, nan J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Je suis le seul au guidon, seules les étoiles me guident pah Personne me passe le filon, la vie n'tient qu'à un fil eh Rebeu, la voile nous hissons, direction une autre vie pah Une question de vision, une question de fric ouh Je voulais être honnête mais je pouvais pas m'le permettre Rendre fiers père et mère mais dans nos têtes, c'est un pêle-mêle La vie me prend par le col, oh, pas d'école, pas d'heures de colle, oh Entre les bagarres, les vols, oh, la proviseur devient folle, oh Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Dans les sacs à gravats, un peu de bicrava, demande pas si ça va, je vais bien Rode parmi les cafards, pas beaucoup d'états d'âme, ouais ce monde est fatale, on sait rien Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah Woh, woh, je pense à demain, s'agit pas de maintenant Waouh, rien à foutre des gens si j'dois l'dire honnêtement Woh, woh, moi et mon égo, on va canner en même temps Waouh, si j'dois l'dire honnêtement J'ai peur de moi-même peur de moi-même Peur de ma colère, peur de ma folie Peur de ma haine peur de ma haine Devant l'inconnu, fais des insomnies J'suis dans ma tête j'suis dans ma tête J'suis dans la zone libre, pas d'all eyes on me J'suis sous l'averse j'suis sous l'averse J'marche sur des lames de couteaux en esquivant les gouttes d'eau Sans demander Sans demander, sans demander, nan, nan J'me suis servis J'me suis servis sans demander, nan, nan Et le talent Talent naturel, ouais, sans me vanter C'est tout c'que j'ai, ça veut me l'enlever Donc je l'ai pris, ouais, sans demander J'peux pas rester conscient, j'suis bloqué dans mes pensées On m'a dit C'est pas bon signe, toi, dis-moi, qu'est-ce t'en sais ? Nan, j'suis pas présent, nan, j'suis pas présent, j'suis bloqué dans mes pensées Tous les jours, on traîne ensemble, mais dis-moi, qu'est-ce t'en sais ? Yeah1</t>
+          <t>Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Niqu ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce goss en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto</t>
         </is>
       </c>
     </row>
@@ -2753,12 +2753,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Satoshi Nakamoto</t>
+          <t>Selfreestyle 1 #Paris</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto On n'est pas des Superman, on investit dans la crypto' Neuf têtes cramées dans le Vitto, gyro', poursuivis par une vie d'pauvre Bitcoin ou PayPal, ça ne prend plus le cash Faut que tu le saches, on n'est pas du bétail et les banques ne sont plus de taille Quand c'est en baisse, on mise, quand c'est en hausse, on garde, hey, hey Niqu ton haut standing, j'suis pas dans vos standards, hey, hey J'étais ce goss en ville avec de grosses envies mais qui venait d'en bas Catalogué zonard mais pourtant, j'étais loin d'un ke-mé lambda J'fais toujours de mon mieux et pour le reste, c'est le destin Depuis l'enfance, on est retreints, il est temps qu'on s'invite au festin La monnaie te va mieux, j'te souhaite d'être dé-blin Même si l'économie est en déclin et que la crise en fera tomber plein Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto J'suis dans l'bull, t'es dans l'bear, j'suis dans l'mouv', t'es sédentaire T'es dans l'rouge, j'suis dans l'vert, parcours de vie exemplaire Toi, sous tes pieds, c'est l'enfer, j'détruis l'décor, c'est l'enfer Mets-toi en garde, on est en guerre, le vainqueur sera légendaire Vous le voulez ? Venez le prendre, vous avez le temps Si t'as la monnaie, on peut s'arranger, tu peux passer devant monnaie À part la passion, y a pas de talent, que des facilités quoi ? Et dans la rue, y a pas de mensonge, que de l'habilité y a rien Ton pire ennemi, c'est l'inflation, mais c'n'est pas mentionner dans la narration Même si y a que des gros poissons, ça finira bien par mordre à l'hameçon Changer les choses sans discrétion, tu finis en cours de cassation Fils, savais-tu que les gens qui dirigent s'enfoutent de la nation ? Eh Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto Quand tu bosses pour un tron-pa, t'as des soucis, t'as mal au dos Fais la moula, la vraie de vrai, la Satoshi Nakamoto</t>
+          <t>Flânons tout le long, tout le long des rues de Paris Flânons tout le long, tout le long des rues de Paris Flânons tout le long, tout le long des rues de Paris Yeah yeah 2Zer-Washington, Selfreestyle S-Crew Booooy, L'Entourage Bébé Je me balade le long des rues À Paname le monde est rude Pas fameux Mais y'a de la beuh C'est pas mal Bon début Paris est froid Mais je parle pas d'hiver, Frère Plein de potes Mais combien zappent ma date d'anniversaire Pas de balivernes, merde Paris va t'envoûter Vas-y va t'en couper Si t'arrives à en douter Akhi, tu palisses sur ma vie T'as tant loupé Quand t'arrives dans ma ville T'es archi mal entouré Ici c'est la canicule Paris brûle Ouais je te manipule Tu capitules Quand j'articule T'en prends pour ton matricule Avec ma tribu Je m'attribue le track Et puis ta tribune C'est archi dur de se battre Quand dans le rap T'es qu'une particule Flânons tout le long, tout le long des rues de Paris Poto, c'est ici que je puise ma puissance Sans mes soces et Paris Mon peura n'a plus de sens Flânons tout le long, tout le long des rues de Paris Flânons tout le long, tout le long des rues de Paris Flânons tout le long, tout le long des rues de Paris Flânons tout le long, yeah yeah, brrrrrruh !</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2770,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Selfreestyle 1 #Paris</t>
+          <t>#SELFREESTYLE 27.06.2016</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Flânons tout le long, tout le long des rues de Paris Flânons tout le long, tout le long des rues de Paris Flânons tout le long, tout le long des rues de Paris Yeah yeah 2Zer-Washington, Selfreestyle S-Crew Booooy, L'Entourage Bébé Je me balade le long des rues À Paname le monde est rude Pas fameux Mais y'a de la beuh C'est pas mal Bon début Paris est froid Mais je parle pas d'hiver, Frère Plein de potes Mais combien zappent ma date d'anniversaire Pas de balivernes, merde Paris va t'envoûter Vas-y va t'en couper Si t'arrives à en douter Akhi, tu palisses sur ma vie T'as tant loupé Quand t'arrives dans ma ville T'es archi mal entouré Ici c'est la canicule Paris brûle Ouais je te manipule Tu capitules Quand j'articule T'en prends pour ton matricule Avec ma tribu Je m'attribue le track Et puis ta tribune C'est archi dur de se battre Quand dans le rap T'es qu'une particule Flânons tout le long, tout le long des rues de Paris Poto, c'est ici que je puise ma puissance Sans mes soces et Paris Mon peura n'a plus de sens Flânons tout le long, tout le long des rues de Paris Flânons tout le long, tout le long des rues de Paris Flânons tout le long, tout le long des rues de Paris Flânons tout le long, yeah yeah, brrrrrruh !</t>
+          <t>Tu connais les bails Tu connais les bails Zer-2, -Crew, Seine Zoo La vérité est dure à digérer Mais je ne vais pas cracher le morceau Écrasé par le poids de mes péchés Ça me fait juste taffer les dorsaux Moi je n'ai jamais considéré La défaite est comme une fatalité Je tourne la page comme un illéttré Rien ne m'inquiète c'est une calamité Et si tu me vois douter c'est calamitant J'vendais des sachets y'a même pas dix ans Si t'as pas d'opinion je m'en fous de ce que tu penses Ç'est que t'approuves si tu n'as pas dit non Pas de ma faute si Paname m'inspire Paname est sombre comme l'âme d'un flic Et l'État coulera le navire J'veux rien dire de mal mais c'est mal de rien dire</t>
         </is>
       </c>
     </row>
@@ -2787,12 +2787,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>#SELFREESTYLE 27.06.2016</t>
+          <t>Selfreestyle 2 #RegardeÀlHorizonTuVerras2zerSeLever</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Tu connais les bails Tu connais les bails Zer-2, -Crew, Seine Zoo La vérité est dure à digérer Mais je ne vais pas cracher le morceau Écrasé par le poids de mes péchés Ça me fait juste taffer les dorsaux Moi je n'ai jamais considéré La défaite est comme une fatalité Je tourne la page comme un illéttré Rien ne m'inquiète c'est une calamité Et si tu me vois douter c'est calamitant J'vendais des sachets y'a même pas dix ans Si t'as pas d'opinion je m'en fous de ce que tu penses Ç'est que t'approuves si tu n'as pas dit non Pas de ma faute si Paname m'inspire Paname est sombre comme l'âme d'un flic Et l'État coulera le navire J'veux rien dire de mal mais c'est mal de rien dire</t>
+          <t>C'est un nouveau départ, le passé j'vais le dilapider Ferme ta bouche, c'est ton comportement qui me dira qui t'es J'ai plein d'vitalité, jeune d'âge mental mais là j'm'en tape, j'deviens vite agité quand l'argent s'taille, c'est lamentable J'pose et j'réfléchi après, j'dois vite avancer, toi ton flow s'est fait kidnapper, j't'invite à penser J'dois dépasser cette ligne qui sépare le ciel et la Terre, ouais ça y est c'est dit, j'kiff les femmes, le sexe et la bière La vie est moche, mais j'l'ai échappé belle, j'me souviens plus de la tristesse, ouais j'ai tout effacé d'elle J'veux des sous, des femmes, des belles, passer des journées à les ken, rester cloué ça m'vénere, j'me serait coupé déjà les veines J'vais débouler, vous dérouillez, allez courez ça m'déchaîne, l'avenir est à moi ce que la Tour est à Eiffel Faites place à ce gosse qui sous Beuher veut gueuler, regarde à l'horizon tu verra 2Zer se lever Bleh2</t>
         </is>
       </c>
     </row>
@@ -2804,12 +2804,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Selfreestyle 2 #RegardeÀlHorizonTuVerras2zerSeLever</t>
+          <t>Seulement</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>C'est un nouveau départ, le passé j'vais le dilapider Ferme ta bouche, c'est ton comportement qui me dira qui t'es J'ai plein d'vitalité, jeune d'âge mental mais là j'm'en tape, j'deviens vite agité quand l'argent s'taille, c'est lamentable J'pose et j'réfléchi après, j'dois vite avancer, toi ton flow s'est fait kidnapper, j't'invite à penser J'dois dépasser cette ligne qui sépare le ciel et la Terre, ouais ça y est c'est dit, j'kiff les femmes, le sexe et la bière La vie est moche, mais j'l'ai échappé belle, j'me souviens plus de la tristesse, ouais j'ai tout effacé d'elle J'veux des sous, des femmes, des belles, passer des journées à les ken, rester cloué ça m'vénere, j'me serait coupé déjà les veines J'vais débouler, vous dérouillez, allez courez ça m'déchaîne, l'avenir est à moi ce que la Tour est à Eiffel Faites place à ce gosse qui sous Beuher veut gueuler, regarde à l'horizon tu verra 2Zer se lever Bleh2</t>
+          <t>Hugz t'es en feu sur celle-là J'ai le business à gérer, elle m'dit Bébé, faudrait que tu penses à m'appeler Y a toute la mif à gérer, il m'dit Poto, faudrait que tu penses à m'appeler À quel moment j'pense à moi-même ? À quel moment j'pense à ma paie ? Mais si tu m'dois un billet, sérieux poto faudrait que tu penses à m'appeler Seulement, seulement, seulement, seulement si tu m'appelais Seulement, seulement, seulement, seulement si tu répondais On devait s'capter dans la journée, depuis la nuit est tombée Le temps passe et t'es parti, si seulement je t'avais rappelé Y avait des choses que j'aurais pu t'dire, j'repense à tous ces moments ratés J'savais pas que c'était déductible, c'est sûr j'vais m'en rappeler Une excuse de merde, RDV annulé juste pour rester sur l'rrain-te J'oublie souvent les meilleurs moments, c'est avec la mif autour d'un thé Y avait des choses qu'on aurait pu vivre, qu'on aurait pu éviter T'es pas là, tout paraît futile, j'regarde nos vidéos en replay Si seulement j'avais décroché, respecté tes projets, j'aurais pas ces regrets Cerveau micro-processeur, j'suis mon propre professeur, ouais j'fais que m'interroger J'ai le business à gérer, elle m'dit Bébé, faudrait que tu penses à m'appeler Y a toute la mif à gérer, il m'dit Poto, faudrait que tu penses à m'appeler À quel moment j'pense à moi-même ? À quel moment j'pense à ma paie ? Mais si tu m'dois un billet, sérieux poto faudrait que tu penses à m'appeler Seulement, seulement, seulement, seulement si tu m'appelais Seulement, seulement, seulement, seulement si tu répondais On devait s'capter dans la journée, depuis la nuit est tombée Le temps passe et t'es parti, si seulement je t'avais rappelé Pour la galère, j'suis rodé, achète le bonheur à l'unité Ma vie en édition limitée, mes xe-té sont numérotés Ne choisis pas un camp si le combat n'est pas le tien, fais pas le délinquant, on s'connaît pas donc parle bien Profite de ta journée, c'est pas sûr que tu voies demain, les rues d'Paris sont tordues, non y'a pas de droit chemin Ici c'est la galère, y a pas de vida loca, mets la vodka dans la bouteille comme si tu bois de l'eau plate Pas du genre à faire du boucan même pendant les embrouilles, j'parlerai après ma ... dans ta boîte vocale Si seulement j'avais décroché, respecté tes projets, j'aurais pas ces regrets Cerveau micro-processeur, j'suis mon propre professeur, ouais j'fais que m'interroger J'ai le business à gérer, elle m'dit Bébé, faudrait que tu penses à m'appeler Y a toute la mif à gérer, il m'dit Poto, faudrait que tu penses à m'appeler À quel moment j'pense à moi-même ? À quel moment j'pense à ma paie ? Mais si tu m'dois un billet, sérieux poto faudrait que tu penses à m'appeler Seulement, seulement, seulement, seulement si tu m'appelais Seulement, seulement, seulement, seulement si tu répondais On devait s'capter dans la journée, depuis la nuit est tombée Le temps passe et t'es parti, si seulement je t'avais rappelé</t>
         </is>
       </c>
     </row>
@@ -2821,12 +2821,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Seulement</t>
+          <t>Si c’était facile</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Hugz t'es en feu sur celle-là J'ai le business à gérer, elle m'dit Bébé, faudrait que tu penses à m'appeler Y a toute la mif à gérer, il m'dit Poto, faudrait que tu penses à m'appeler À quel moment j'pense à moi-même ? À quel moment j'pense à ma paie ? Mais si tu m'dois un billet, sérieux poto faudrait que tu penses à m'appeler Seulement, seulement, seulement, seulement si tu m'appelais Seulement, seulement, seulement, seulement si tu répondais On devait s'capter dans la journée, depuis la nuit est tombée Le temps passe et t'es parti, si seulement je t'avais rappelé Y avait des choses que j'aurais pu t'dire, j'repense à tous ces moments ratés J'savais pas que c'était déductible, c'est sûr j'vais m'en rappeler Une excuse de merde, RDV annulé juste pour rester sur l'rrain-te J'oublie souvent les meilleurs moments, c'est avec la mif autour d'un thé Y avait des choses qu'on aurait pu vivre, qu'on aurait pu éviter T'es pas là, tout paraît futile, j'regarde nos vidéos en replay Si seulement j'avais décroché, respecté tes projets, j'aurais pas ces regrets Cerveau micro-processeur, j'suis mon propre professeur, ouais j'fais que m'interroger J'ai le business à gérer, elle m'dit Bébé, faudrait que tu penses à m'appeler Y a toute la mif à gérer, il m'dit Poto, faudrait que tu penses à m'appeler À quel moment j'pense à moi-même ? À quel moment j'pense à ma paie ? Mais si tu m'dois un billet, sérieux poto faudrait que tu penses à m'appeler Seulement, seulement, seulement, seulement si tu m'appelais Seulement, seulement, seulement, seulement si tu répondais On devait s'capter dans la journée, depuis la nuit est tombée Le temps passe et t'es parti, si seulement je t'avais rappelé Pour la galère, j'suis rodé, achète le bonheur à l'unité Ma vie en édition limitée, mes xe-té sont numérotés Ne choisis pas un camp si le combat n'est pas le tien, fais pas le délinquant, on s'connaît pas donc parle bien Profite de ta journée, c'est pas sûr que tu voies demain, les rues d'Paris sont tordues, non y'a pas de droit chemin Ici c'est la galère, y a pas de vida loca, mets la vodka dans la bouteille comme si tu bois de l'eau plate Pas du genre à faire du boucan même pendant les embrouilles, j'parlerai après ma ... dans ta boîte vocale Si seulement j'avais décroché, respecté tes projets, j'aurais pas ces regrets Cerveau micro-processeur, j'suis mon propre professeur, ouais j'fais que m'interroger J'ai le business à gérer, elle m'dit Bébé, faudrait que tu penses à m'appeler Y a toute la mif à gérer, il m'dit Poto, faudrait que tu penses à m'appeler À quel moment j'pense à moi-même ? À quel moment j'pense à ma paie ? Mais si tu m'dois un billet, sérieux poto faudrait que tu penses à m'appeler Seulement, seulement, seulement, seulement si tu m'appelais Seulement, seulement, seulement, seulement si tu répondais On devait s'capter dans la journée, depuis la nuit est tombée Le temps passe et t'es parti, si seulement je t'avais rappelé</t>
+          <t>Le peura ne m'dit pas tout pourtant je l'suis depuis la case départ On a fait l'gâteau ensemble mais ce batard me cache des parts En essayant d'stopper la merde c'est là qu'tu la vois s'amplifier Accroche toi à l'apparence mais utilise là sans t'y fier En regardant j'ai vu l'mal dans les yeuz de cette sse-mi Comme un excès d'ce-vi c'est d'sa rage qu'elle se vide J'étouffe j'fais des conneries car mon cerveau est mal oxygéné Soit pas aussi gêné car mon train d'vie bah moi aussi j'l'aimais Refrain x2 Les gens font ce qu'ils veulent Pour leurs plans te marchent dessus J'ai beau sprinter derrière eux Maintenant j'en ai marre je sue Y a plus d'impunité Même tes frères te manipulent L'avenir fait frissonner moi j'm'en fous j'ai pas mis d'pull Moi au fond j'suis un peu sportif Car l'instru c'est mon terrain de jeu Moi j'veux cer-per autant qu'une vieille voudrait monter un ne-jeu J'veux tellement récolter ce que j'ai semé comme un Kétama Tu m'as zappé mais quand j'serais parti tu comprendras que t'as mal Quand ça va pas faut qu'j'me rappelle que ma vie fut un temps festive Mais chérie tu m'fais trop mal avec tes fuites intempestives Non j'kiff pas trop les mensonges donc je zappe l'Odyssée Pour soulager mon égo j'kifferais que vous applaudissiez 11 janvier 91 j'vois le jour en pleine nuit J'ai d'la peine oui D'être après tout c'temps en pénurie A part rappeur j'ai pas trouvé ma vocation C'est auch pour cer-per vous baissez tous vos caleçons Moi Paris c'limité au XXème arrondissement Comment découvrir d'autres horizons quand tes darons disent nan J'suis parano moi depuis tout petit j'prépare ma vendetta Nan j'me vendais pas j'suis juste un jeune élevé près de Gambetta J'fais du mal à mes proches mais j'les aime très fort Comment faire pour être til-gen alors qu'la haine me dévore J'suis un mec haineux, en aucun cas j'tolère la défaite J'suis un vénéneux, guettes comment ma colère a de l'effet J'ai d'la peine bien sûr à mes 20 ans j'me serais vu sur une péninsule Mais putain ma vie ressemble à une lettre pleine d'insultes Elle ne tient qu'à un fil, mais c'est un fil de fer Sache que beaucoup partiraient si c'était facile de l'faire frère Sache que beaucoup partiraient si c'était facile de l'faire</t>
         </is>
       </c>
     </row>
@@ -2838,12 +2838,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Si c’était facile</t>
+          <t>Teteille</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Le peura ne m'dit pas tout pourtant je l'suis depuis la case départ On a fait l'gâteau ensemble mais ce batard me cache des parts En essayant d'stopper la merde c'est là qu'tu la vois s'amplifier Accroche toi à l'apparence mais utilise là sans t'y fier En regardant j'ai vu l'mal dans les yeuz de cette sse-mi Comme un excès d'ce-vi c'est d'sa rage qu'elle se vide J'étouffe j'fais des conneries car mon cerveau est mal oxygéné Soit pas aussi gêné car mon train d'vie bah moi aussi j'l'aimais Refrain x2 Les gens font ce qu'ils veulent Pour leurs plans te marchent dessus J'ai beau sprinter derrière eux Maintenant j'en ai marre je sue Y a plus d'impunité Même tes frères te manipulent L'avenir fait frissonner moi j'm'en fous j'ai pas mis d'pull Moi au fond j'suis un peu sportif Car l'instru c'est mon terrain de jeu Moi j'veux cer-per autant qu'une vieille voudrait monter un ne-jeu J'veux tellement récolter ce que j'ai semé comme un Kétama Tu m'as zappé mais quand j'serais parti tu comprendras que t'as mal Quand ça va pas faut qu'j'me rappelle que ma vie fut un temps festive Mais chérie tu m'fais trop mal avec tes fuites intempestives Non j'kiff pas trop les mensonges donc je zappe l'Odyssée Pour soulager mon égo j'kifferais que vous applaudissiez 11 janvier 91 j'vois le jour en pleine nuit J'ai d'la peine oui D'être après tout c'temps en pénurie A part rappeur j'ai pas trouvé ma vocation C'est auch pour cer-per vous baissez tous vos caleçons Moi Paris c'limité au XXème arrondissement Comment découvrir d'autres horizons quand tes darons disent nan J'suis parano moi depuis tout petit j'prépare ma vendetta Nan j'me vendais pas j'suis juste un jeune élevé près de Gambetta J'fais du mal à mes proches mais j'les aime très fort Comment faire pour être til-gen alors qu'la haine me dévore J'suis un mec haineux, en aucun cas j'tolère la défaite J'suis un vénéneux, guettes comment ma colère a de l'effet J'ai d'la peine bien sûr à mes 20 ans j'me serais vu sur une péninsule Mais putain ma vie ressemble à une lettre pleine d'insultes Elle ne tient qu'à un fil, mais c'est un fil de fer Sache que beaucoup partiraient si c'était facile de l'faire frère Sache que beaucoup partiraient si c'était facile de l'faire</t>
+          <t>Ouh, ouh, ouh beat, wow wow Zer-2 Ouh, ouh Eh, eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille C'est le froid de l'hiver, on a besoin de la chaleur d'un flash Personne t'entend, t'as peu d'impact, c'est qu'tu gardes tes valeurs intactes ouh, ouh Des millions sont détournés mais tu pourrais ber-tom pour une quette-pla Pendant qu'certains jouent les gangstas, certains tirent pour un poulet kefta bleh Ouais, j't'ai menti, j'voulais pas te blesser, nan, j'avais pas le choix no La vérité peut m'écarter de toi et les remords ne faisaient pas le poids Touche à la mif', j'vais te pister et trouver ta cachette eh Faut trouver la force de presser la gâchette, ramasser les douilles, effacer la cassette eh, eh, eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille J'étais dans la merde, j'ai fait des choses atroces des choses atroces J'ai fait pleurer ma mère, j'voulais devenir le boss devenir le boss Comment font-ils pour avoir autant d'vices ? Wah En vrai, j'déteste ces mecs, faut qu'on s'le dise C'était la hess là, on trinque nous, pas d'salade Avec mes hustlers, on a triplé l'salaire ouh J'croyais qu't'étais mon frère, t'étais qu'un te-traî, mince alors paw Maintenant, j'fais du biff, j'veux un palace avec plein d'salopes plein d'salopes Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille Je regarde le ciel allongé sur le sol J'serais toujours le dernier à pleurer sur mon sort Si j'ai la santé, ouais, c'est sûr, j'm'en sors Si t'es l'seul à penser ça, c'est que t'as sûrement tort</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Teteille</t>
+          <t>TLN</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Ouh, ouh, ouh beat, wow wow Zer-2 Ouh, ouh Eh, eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille C'est le froid de l'hiver, on a besoin de la chaleur d'un flash Personne t'entend, t'as peu d'impact, c'est qu'tu gardes tes valeurs intactes ouh, ouh Des millions sont détournés mais tu pourrais ber-tom pour une quette-pla Pendant qu'certains jouent les gangstas, certains tirent pour un poulet kefta bleh Ouais, j't'ai menti, j'voulais pas te blesser, nan, j'avais pas le choix no La vérité peut m'écarter de toi et les remords ne faisaient pas le poids Touche à la mif', j'vais te pister et trouver ta cachette eh Faut trouver la force de presser la gâchette, ramasser les douilles, effacer la cassette eh, eh, eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille J'étais dans la merde, j'ai fait des choses atroces des choses atroces J'ai fait pleurer ma mère, j'voulais devenir le boss devenir le boss Comment font-ils pour avoir autant d'vices ? Wah En vrai, j'déteste ces mecs, faut qu'on s'le dise C'était la hess là, on trinque nous, pas d'salade Avec mes hustlers, on a triplé l'salaire ouh J'croyais qu't'étais mon frère, t'étais qu'un te-traî, mince alors paw Maintenant, j'fais du biff, j'veux un palace avec plein d'salopes plein d'salopes Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille eh Po-pow, tire sur le oint-j, viens qu'on s'évade avant qu'ces putains d'blèmes nous crament la te-tê Oh, oh, on fait du bien, on fait du mal, les soucis viennent, on s'cache derrière la 'te-'teille Je regarde le ciel allongé sur le sol J'serais toujours le dernier à pleurer sur mon sort Si j'ai la santé, ouais, c'est sûr, j'm'en sors Si t'es l'seul à penser ça, c'est que t'as sûrement tort</t>
+          <t>Et j'ai tourné, tourné toute la night toute la night Grosse caisse, grosse basse réveillent tout Paname tout Paname T'as pas capté, bats les couilles d'ta life bats les couilles Grosse caisse, grosse basse, voisins sous Xanax voisins sous Xanax Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night toute la night, j'ai dit Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night ouais, ouais, ouais S'ils te fabriquent, ils pourront te détruire Pour ça que le calibre est toujours dans l'étui Pour ça qu'on s'est faits nous-mêmes, cent pourcents Seine Zoo Qu'on brille ou qu'on s'éteigne, cent pourcents -Crew On a toujours la dalle, toujours pas la paix eh On n'est jamais à l'heure, on fait toujours scandale Comme quand y avait que dalle, leur biz' est plutôt casse-gueule J'ai Hugz dans le casque, Seine Zoo a plusieurs casquettes Et chacune d'elles t'encastrent, t'en chopes des problèmes gastriques Qu'est-ce qu'ils connaissent de la street ceux qui connaissent s'angoissent Jarrive comme Bernadette pour collecter les thunes Dès que je perds la tête, j'me connecte à Neptune Ouais, le local et ptit, sent pas leucalyptus Te-ma le collectif, comme on les connait tous Paraît qu'le calibre tue, parait qu'le feu, je lai Toujours libre, jsuis entraîné s'il faut jeûner Sur-sollicité, je gère tout y a ma sueur sur les CD Seine Zoo, tu connais, maintenant, jsuis dans tous les journaux comme un fish and chips Cest pour tous mes G's quon a fichés Et jsuis dans tout les journaux comme un fish and chips Cest pour tous mes G's quon a fichés Et j'ai tourné, tourné toute la night toute la night Grosse caisse, grosse basse réveillent tout Paname tout Paname T'as pas capté, bats les couilles d'ta life bats les couilles Grosse caisse, grosse basse, voisins sous Xanax voisins sous Xanax Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night toute la night, j'ai dit Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night ouais, ouais, ouais Dans la caisse en paix, cool-al dans l'Sanpe' Tu fais rien sans blé, toujours un qui veut nuire à ta santé Mekra, faut pas l'fréquenter, traîne avec traficante Même les putes t'ont fécondé, jamais croisé de vrais condés J'garde ma place comme Corona, que de la frappe comme For Honor Toi, tu mérites la mort aux rats, on t'pardonne pas, t'es comme Rollo hey Que des fuites en roue arrière, no stress Le rap FR n'a rien à envier aux States nan, nan Tout se fait à Paname, le prestige intemporel On a la Tour Eiffel, ils ont la coupe aux grandes oreilles Oh, oh Fais les bails en deuss', deuss' deuss', deuss' Médicale à haute dose haute dose Fumée ressort par les deux yeuz, à part nous, qui l'fait mieux ? Appelle-nous si sérieux, y a Paname qui s'fait vieux Mets le son dans la caisse, coffrer toute la rée-s' Bre-som sous l'averse, devant ton adresse J'vais où le vent m'emmène, j'me sens lég' dans ma Benz On débarque dans ta rée-s', te corrige comme Antares Et j'ai tourné, tourné toute la night toute la night Grosse caisse, grosse basse réveillent tout Paname tout Paname T'as pas capté, bats les couilles d'ta life bats les couilles Grosse caisse, grosse basse, voisins sous Xanax voisins sous Xanax Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night toute la night, j'ai dit Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night ouais, ouais, ouais</t>
         </is>
       </c>
     </row>
@@ -2872,12 +2872,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>TLN</t>
+          <t>Venez</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Et j'ai tourné, tourné toute la night toute la night Grosse caisse, grosse basse réveillent tout Paname tout Paname T'as pas capté, bats les couilles d'ta life bats les couilles Grosse caisse, grosse basse, voisins sous Xanax voisins sous Xanax Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night toute la night, j'ai dit Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night ouais, ouais, ouais S'ils te fabriquent, ils pourront te détruire Pour ça que le calibre est toujours dans l'étui Pour ça qu'on s'est faits nous-mêmes, cent pourcents Seine Zoo Qu'on brille ou qu'on s'éteigne, cent pourcents -Crew On a toujours la dalle, toujours pas la paix eh On n'est jamais à l'heure, on fait toujours scandale Comme quand y avait que dalle, leur biz' est plutôt casse-gueule J'ai Hugz dans le casque, Seine Zoo a plusieurs casquettes Et chacune d'elles t'encastrent, t'en chopes des problèmes gastriques Qu'est-ce qu'ils connaissent de la street ceux qui connaissent s'angoissent Jarrive comme Bernadette pour collecter les thunes Dès que je perds la tête, j'me connecte à Neptune Ouais, le local et ptit, sent pas leucalyptus Te-ma le collectif, comme on les connait tous Paraît qu'le calibre tue, parait qu'le feu, je lai Toujours libre, jsuis entraîné s'il faut jeûner Sur-sollicité, je gère tout y a ma sueur sur les CD Seine Zoo, tu connais, maintenant, jsuis dans tous les journaux comme un fish and chips Cest pour tous mes G's quon a fichés Et jsuis dans tout les journaux comme un fish and chips Cest pour tous mes G's quon a fichés Et j'ai tourné, tourné toute la night toute la night Grosse caisse, grosse basse réveillent tout Paname tout Paname T'as pas capté, bats les couilles d'ta life bats les couilles Grosse caisse, grosse basse, voisins sous Xanax voisins sous Xanax Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night toute la night, j'ai dit Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night ouais, ouais, ouais Dans la caisse en paix, cool-al dans l'Sanpe' Tu fais rien sans blé, toujours un qui veut nuire à ta santé Mekra, faut pas l'fréquenter, traîne avec traficante Même les putes t'ont fécondé, jamais croisé de vrais condés J'garde ma place comme Corona, que de la frappe comme For Honor Toi, tu mérites la mort aux rats, on t'pardonne pas, t'es comme Rollo hey Que des fuites en roue arrière, no stress Le rap FR n'a rien à envier aux States nan, nan Tout se fait à Paname, le prestige intemporel On a la Tour Eiffel, ils ont la coupe aux grandes oreilles Oh, oh Fais les bails en deuss', deuss' deuss', deuss' Médicale à haute dose haute dose Fumée ressort par les deux yeuz, à part nous, qui l'fait mieux ? Appelle-nous si sérieux, y a Paname qui s'fait vieux Mets le son dans la caisse, coffrer toute la rée-s' Bre-som sous l'averse, devant ton adresse J'vais où le vent m'emmène, j'me sens lég' dans ma Benz On débarque dans ta rée-s', te corrige comme Antares Et j'ai tourné, tourné toute la night toute la night Grosse caisse, grosse basse réveillent tout Paname tout Paname T'as pas capté, bats les couilles d'ta life bats les couilles Grosse caisse, grosse basse, voisins sous Xanax voisins sous Xanax Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night toute la night, j'ai dit Pour mes khos qui dorment la journée et qui font que tourner Tourner toute la night ouais, ouais, ouais</t>
+          <t>Pas du genre à m'cacher, pas du genre à cacher les blem' Pas de gâchis, j'me sers de ma peine et j'utilise ma haine J'ai vu la roue tourner, j'pilote, tu sais où m'trouver Venez m'chercher, venez, venez, venez Sentiments sans limite, que les miens qu'on imite pas Peu d'limites, limites, limites, y'a pas de polémique y'a que les miens qu'on imite pas Que les miens, que les miens, bien entouré, tu sais où m'trouver aha Venez m'chercher Elle occupe mes pensées, son corps est élancé Devant son déhanché j'sais pas sur quel pied danser yeah Mais j'suis infréquentable, j'vais la blesser comme d'hab Parigot pas français, toujours les sourcils froncés Le temps t'efface, pas le temps, pas le temps,elle laisse pas d'traces Les gens qui passent font que passer quoi que tu fasses Pas du genre à m'cacher, pas du genre à cacher les blem' Pas de gâchis, j'me sers de ma peine et j'utilise ma haine J'ai vu la roue tourner, j'pilote, tu sais où m'trouver Venez m'chercher, venez, venez, venez Sentiments sans limite, que les miens qu'on imite pas Peu d'limites, limites, limites, y'a pas de polémique y'a que les miens qu'on imite pas Que les miens, que les miens, bien entouré, tu sais où m'trouver aha Venez m'chercher Change pas, reste comme t'es, c'est l'effet escompté Peux pas me laisser dompter, sauvage c'est donc vrai yeah Peux pas la laisser tomber, j'combats mes démons ouais, yeah Bébé t'as les fesses bombées, ? s'est trompé Et le chaud qui fâche Y'a le sang, le sang, le sang qui tâche fait que couler ? Et j'me casse quoi que tu fasses on le fait, on le fait, on le fait Pas du genre à m'cacher, pas du genre à cacher les blem' Pas de gâchis, j'me sers de ma peine et j'utilise ma haine J'ai vu la roue tourner, j'pilote, tu sais où m'trouver Venez m'chercher, venez, venez, venez Sentiments sans limite, que les miens qu'on imite pas Peu d'limites, limites, limites, y'a pas de polémique y'a que les miens qu'on imite pas Que les miens, que les miens, bien entouré, tu sais où m'trouver aha Venez m'chercher, venez me chercher, venez me chercher, venez me chercher, venez me chercher</t>
         </is>
       </c>
     </row>
@@ -2889,12 +2889,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Venez</t>
+          <t>Vie de galère</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Pas du genre à m'cacher, pas du genre à cacher les blem' Pas de gâchis, j'me sers de ma peine et j'utilise ma haine J'ai vu la roue tourner, j'pilote, tu sais où m'trouver Venez m'chercher, venez, venez, venez Sentiments sans limite, que les miens qu'on imite pas Peu d'limites, limites, limites, y'a pas de polémique y'a que les miens qu'on imite pas Que les miens, que les miens, bien entouré, tu sais où m'trouver aha Venez m'chercher Elle occupe mes pensées, son corps est élancé Devant son déhanché j'sais pas sur quel pied danser yeah Mais j'suis infréquentable, j'vais la blesser comme d'hab Parigot pas français, toujours les sourcils froncés Le temps t'efface, pas le temps, pas le temps,elle laisse pas d'traces Les gens qui passent font que passer quoi que tu fasses Pas du genre à m'cacher, pas du genre à cacher les blem' Pas de gâchis, j'me sers de ma peine et j'utilise ma haine J'ai vu la roue tourner, j'pilote, tu sais où m'trouver Venez m'chercher, venez, venez, venez Sentiments sans limite, que les miens qu'on imite pas Peu d'limites, limites, limites, y'a pas de polémique y'a que les miens qu'on imite pas Que les miens, que les miens, bien entouré, tu sais où m'trouver aha Venez m'chercher Change pas, reste comme t'es, c'est l'effet escompté Peux pas me laisser dompter, sauvage c'est donc vrai yeah Peux pas la laisser tomber, j'combats mes démons ouais, yeah Bébé t'as les fesses bombées, ? s'est trompé Et le chaud qui fâche Y'a le sang, le sang, le sang qui tâche fait que couler ? Et j'me casse quoi que tu fasses on le fait, on le fait, on le fait Pas du genre à m'cacher, pas du genre à cacher les blem' Pas de gâchis, j'me sers de ma peine et j'utilise ma haine J'ai vu la roue tourner, j'pilote, tu sais où m'trouver Venez m'chercher, venez, venez, venez Sentiments sans limite, que les miens qu'on imite pas Peu d'limites, limites, limites, y'a pas de polémique y'a que les miens qu'on imite pas Que les miens, que les miens, bien entouré, tu sais où m'trouver aha Venez m'chercher, venez me chercher, venez me chercher, venez me chercher, venez me chercher</t>
+          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
         </is>
       </c>
     </row>
@@ -2906,27 +2906,10 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Vie de galère</t>
+          <t>ViperGts</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
-        <is>
-          <t>Vu que c'était la débandade, on a du agir comme des panthères De vive voix, l'envie de vaincre comme si ma vie en dépendait J'étais petit je voulais me faire la terre entière C'est quand tu te laisses aller que ça devient de pire en pire T'y crois plus depuis que t'as raté, car la vie joue sur ton caractère On a du resserrer pour pas faire de grosses erreurs Certains sont enterrés, on va venger leurs âmes On bannit les traîtres, les éléments cancéreux Faut croire en ses rêves, c'est comme ça qu'on s'est inséré On te sert comme l'équipe des Lakers 2-zer, Mekra, Framal, Nek Hey hey Pour eux, je sortirais les guns Hey hey La vérité se cache dans les coeurs J'étais naïf, j'ai bien appris à pas leur parler Ma grand-mère m'a dit Faut pas cramer sa tanière J'suis méfiant c'est pas la peine de la ramener Pour baiser un gros poisson ma gueule faut l'art et la manière Les groupies c'est fatiguant, ça veut pas lâcher Les concerts c'est pas là-bas que t'auras ta cavalière Le business faut pas croire, c'est pas la scène Faut pas croire ce que tu vois sur la bannière Dis pas qu't'aimes pas les sous quand on sait qu't'habites à Vincennes La meilleure façon de faire du fric c'est de fuir à Marseille Belek c'est facile, on peut t'effacer J'ai la mif à rincer, le reste je m'en bats les couilles Comme ôter la vie d'un insecte En vrai la vie c'est qu'un essai J'prendrai les armes s'il faut sauver mes marmots En vrai la vie c'est qu'un essai De mon point de vue, je me dis ça va, ça vient Mais quand tu me vois tu me dis Ça va, ça vit, hein Jvois que le monde du peu-ra ça rassasie bien Pour les gens honnêtes et pas les bâtards à chiens Avant 2010, ma musique n'avait pas la côte Sans diplôme on me conseille de taffer à La Poste Enlève ton bob rappeur n'est pas un job Tu ne verras jamais le succès frapper à ta porte Mais j'avais la tête aussi dure que les murs que je tenais L'enfant passionné devient l'homme le plus fort Donc aucune chute n'a fait que je n'ai pu me relever 2zer déter comme ça que mes potes me surnomment Est-ce que c'est possible d'aimer la musique plus que les femmes ? Ce qui me fait bander, c'est quand le public me réclame Quand jkicke, je t'inflige de multiple dégâts Repris de justice qui critique l'Etat Quand le feu est allumé, impossible de l'éteindre Tu m'envies, t'as tort, de pire en pire ma gueule Comment imaginer ma consommation se restreindre ? 50 centimes la clope, 10 centimes la feuille Qu'est-ce que j'entends ? Paraît qu'on veux me rentrer dedans Je souris même quand mes ennemis montrent les dents Je ne vais pas prendre de gants ni même attendre demain L'avenir entre nos mains, je pars à l'entrainement Quand j'pense que des enfants s'élèvent en France seuls Je rentre le ventre et j'affronte le vent Pense en te levant qu'il faut prendre le temps Quand les gens te demandent, faut engendrer le manque Peu importe la manche, il m'reste encore des cartes, yo Mon cur est immense, ça aide pas pour le cardio Dans la de-mer jusqu'au cou Mais j'irai, j'irai jusqu'au bout ! Sur la vie d'ma mère J'réagirai juste aux coups J'en veux toujours plus comme vous ! Ouais, ouais, ouais, ouais J'ai pas la patience, je n'ai pas la sympathie J'tise deux litres, ce n'est pas la Saint Patrick J'ai d'quoi les épater, les béliers sont de sortie ma gueule et c'est parti Peut foutre le bordel ma gueule, à volonté Les cocktails m'accueillent À la base on avait parlé d'un lieu Où c'est la classe et rien est à l'il C'est normal alors passe la tise On fait place à notre anarchie Tu fais l'blarf' à nous alarmer Tu nous fous la honte comme un sac Tati Mets-moi des glaçons dans le rosé J'vais tout faire pour avoir leur oseille J'donne tout dans les p'tites ou les grandes scènes Peu importe le vol ou le recel Fais gaffe à ta reuseu si t'as hassa j'peux te manquer de respect La race on la reçoit, la réussite se fait avec la rage alors essaie Fais les thunes et toi ? On sort les lunettes noires Tu nous as vu festoyer, dans ton hôtel on t'enlève une étoile On fait les thunes et toi ? On sort les lunettes noires Maintenant j'mets les voiles, remercie-nous il t'reste une étoile Qualité street comme Doc Gyneco Desert Eagle si ton OG fait l'beau, torpille les faux Le premier d'la classe va faire en sorte que tu n'copies qu'les fautes Tu vois c'que j'veux dire Y'a le meilleur, on n'voit pas que le pire Chacun d'mes négros pourra te le dire Y'a le meilleur, on n'voit pas que le pire C'est Yass, négro Ta clique panique, nique un taf réglo Tes négros ne savent plus comment agir donc parle-nous bien ou j'te fracasse l'épaule Tu vois c'que j'veux dire Il m'en faut quatre j'suis du signe de la vierge Je lui ramène quand Idriss veut ta tête J'fais ma fête avant qu'il puisse me la mettre Car ce bon, l'destin connaît l'pourvoir d'mes crimes J'étudie l'histoire pour pouvoir l'écrire Yes, nique les fédéraux, c'est tous les frères que j'viens fédérer J'suis resté frais, même quand j'me suis fait déferrer Real talk dans ma tête, chiffrer des tas d'rouages Les fraîcheurs du Queens veulent déchiffrer mes tatouages Soirée aquarium, pas d'maximum Mon regard transperce la fumée On m'regarde, je n'fais qu'm'allumer J'rentre dans le club, les négros s'agrippent à leurs meufs Ne t'inquiète pas, je ne fais que passer Vas-y ramène un MC que j'vienne le casser Ça t'fait pareil quand tu pètes de la C Louanges à Dieu, l'imprévisible, ceux qui suivent son chemin tant bien que mal Jeune vrai rappeur quand j'ai blindé l'splizzif Imprévisible comme le Drunken Master Quand j'suis là l're-frè n'a peur de rien Mes actions sont vraies donc elles nous hantent jamais T'es trop sensible, avant qu'j'naisse mon arme préparait déjà l'offensive On est tous ratal, on t'envoie des rafales Mais toi tu crois quoi, on a la dalle ici Complètement habta, t'inquiètes pas que je ferais tout pour pas finir à Sainte-Anne ou à Oued-Aïssi On attrape le deal avec mes gars d'rebelles Propose tout les défis j'prends n'importe lequel Je veux mourir sur le ring comme Apollo Creed Démarrage américain quand la Polo crie Tu prends l'titre à l'aise, à l'aide de tous ce seille-o T'es riche psartek mais tes seuls amis sont que des zéros J'suis avec mes frères on gagne c'est l'équipe qui perce Et dans le cas contraire Malgré les défaites on ne change pas l'équipe qui perd, ma gueule Mon négro j'fume que la moula Pour les ients-cli y'a le molly Une chose est sûre, j'plaiderai sûrement coupable Face à Mounkar et Nakir, je vois les coupables s'évanouir A l'époque ça rackettait comme dans GTO Maintenant j'appelle mon chauffeur comme dans GTA Le jeune bandit a bien grandi, évite d'être comme les autres Ces fake niggies qui bavent sur tes côtes pour des loves 4 black, pas d'plaque dans la GTT Fucked up là je m'suis décalé Mais je peux revenir en impro préparée C'est quoi les bails bafouillés ? On fait des trucs de merde puis on revient mon frère C'est ça les djizz, je gère le 'sness C'est de l'impro, ouais je coupe des têtes Pendant qu'tu penses que nous on lèche des verges Nan, on n'est pas de votre clique Nan, on n'est pas de votre bord Teste ma clique puis on va t'couper la tête Teste-les, nan, c'est dead, vas-y mon soss, balance Hey, depuis lécole élémentaire, la haine elle est monté C'est quand ta rien qu'tu soulèves des montagnes État second, sur l'avenue Monte' Ma clique est ininterrompable Mes rencards ont les reporte, on n'est jamais sur pause J'ai les deux pieds sur l'hoverboard Je taffe et je prends du repos là où les autres ne s'aventurent pas Y'a les tamponnés, le rap c'est temporaire Ils me disent Merci, je leurs réponds Autant pour moi C'est la grisaille dans notre tête mais on sera là tant que l'on pourra Être à la hauteur de mes envies ça nous a laissé des traces Comme tout les secrets dÉtats on est tous encré dedans Les têtes sont concentrées de drogues mais si un jour je tue ce sera pour rester en vie Le jour où j'aurai d'l'argent j'f'rai peut-être des implants Donc s'il y a du biff à faire, il faut le faire dès maint'nant Pas b'soin de stéroïde, le mic révèle mes tas d'pouvoirs Et j't'ap'rai dans l'héroïne quand j'aurai baisé Catwoman Tu joues le fou mais tu devrais taffer Si vous êtes plusieurs dans ta tête, y'en a pas un qui sait rapper Allez ça dégage J'connais cette fille du 4, un missile, tu craques Qui cherche une idylle durable Mais n'kiff que ceux qui dealent du crack Le studio c'est mon lieu, on m'demande c'que j'fais dans la vie J'réponds que j'fais d'mon mieux Eff Gee n'est pas présomptueux Mais il est très somptueux, pas b'soin d'une voix grave Si ces mecs envoient du pâté moi du foie gras C'est qu'une question d'jeu J'suis c'que mes potos sont, cur noyé dans des eaux profondes On s'morfond, car il n'reste plus qu'des souv'nirs sur des photos sombres Des meufs, d'la beuh, ce soir on va ram'ner les deux Je lis en elle comme si ma queue avait des yeux Tu vois des flammes partout, on est les Néron d'ma ville Rien n'change à part le prénom d'ma bitch Ok, ça fait 1 pour le S, 2 pour le L, 3 pour la caisse et 4 pour la Grâce du Ciel Tes rappeurs de merde ne me servent pas d'idoles Y'a 2zer Washington, mon re-frè On est 25 dans le club, style prince dans le club On break flingue dans le club Amateur de beurettes, arnaqueur de vedettes Si tu veux pas qu'la peur te rejette fais pas l'dingue dans le club Jeune vétéran, swerve élégant, blunt excellent Nigga j'pète les dents J'ai dit à mes G's Qui en a marre d'l'orgueil ? Quand le système est à poil j'ai la barre comme Deuil Ça fait one two, one two, mic check T'es pas un hustler si tu t'es jamais retrouvé à sec, homie Le manque d'adversaire, on t'fait ta fête le 31 Tape un sourire pour un incroyable anniversaire Paraît qu'ton frère serre, à part des verres Trêve de balivernes et j'XXX comme cascade dans Berzerk Négro retourne pas ta veste, ici le temps s'dégrade Et j'gratte sous l'inspi d'l'averse Opinion controversé Dans ma tête c'est XXX contre Persée XXX devant ta porte, chacun ses affaires-zer Un trou dans la tête si tu comptais percer Mon avenir dans la tess est dérisoire comme les seins d'XXX J'ai vu tant de mecs briser leurs vies au tiercé Faire la une, négro faudra t'y faire Quitte à crever en été, pour vesqui la rubrique faits divers Leurs ambitions ne sont qu'des fantasmes Dans la vie c'est noir ou blanc donc on adopte le flow panda C'est quand il y a danger qu'tu vois la vraie nature de l'Homme Ça fait la pute dehors, t'sais, ce n'est pas dur de s'pendre J'kiffe tout c'qui vient d'ailleurs, rappeur à plein temps Sachant qu'mon équipe s'élève très vite, on marche à l'instinct À tout moment, la balle peut surgir On survit, on surine, on subit les supplices Mais, bon, c'est l'mektoub qui nous l'dira Mecton, j'suis peut-être fou comme les bougs d'Irak On connaît pas nos voisins, on connaît pas nos potes Toujours dans l'vrai, dans l'droit chemin, on reconnaît pas nos torts À quoi ça sert d'monter, hein ? À baiser toutes ces petites putes qui sont assermentées J'ai vu la mort sur un lit d'hôpital, y'a plus d'pitié Poto, j'te fais mon speech sur un beat official Y'a plus d'ficha, on est à l'affiche Les fachos sont fâchés, on vivra Ici, survivre est un exploit, faut pas lâcher Leur modèle, c'est le travail à la chaîne, moi, j'suis pas un esclave Ils sont déjà malheureux, les jeunes, alors les vieux... On a le relais, je ne rejette pas le religieux, nan J'ai des yeux meilleurs, tout m'perturbe J'ai vu des jeunes voyous perdus devenir des mecs de ur' jnounés Loin de ces frayeurs, j'recouvre d'une couverture Ma deuxième mère qui dort sur le canapé après une dure journée Un jour, elle m'a dit je t'aime et mes yeux scintillèrent J'me sens apaisé par sa voix pendant les cinq prières Pourtant, j'suis loin d'être un modèle de vertu, bordel de merde Dure vie moderne, faut qu'je modère la verdure Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme Pendant qu'le Diable embrouille encore une âme, la mort arrive Muette comme une tombe, bruyante comme une arme On m'annonce ta mort au téléphone alors qu'j'étais dans le métro C'est pas comme si j'étais sé-po, peinard auprès de mes potes Mon cur perd son tempo, le malheur du monde sur mes épaules J'me rappelle de tous nos jets-pro et de la belle époque Étant bébé, on se lavait dans la même bassine Mal dans ma peau, ta gentillesse était ma terre d'asile À quoi ça sert la vie ? A voir ses frères partir ? Mais on m'a dit Que Dieu cueille les plus belles fleurs qui prennent racine Parfois, j'ai l'impression de t'apercevoir dans la pénombre Quand ça ? Quand j'galère le soir Tu sais ici, on est tous tes frères Ta mort me pousse au bout de mes nerfs Tellement pleuré que la coupe est pleine T'aurais voulu que j'épouse mes rêves Donc j'écris des couplets, j'me force à faire des concerts Minute de silence, s'il vous plaît C'est pour mon zin décédé qu'on s'lève Tout l'monde disait qu'on se ressemblait Le même sang coulait dans nos veines On s'racontait nos cauchemars Maintenant t'apparais dans mes rêves Un vrai repère le Rap, y'a trop de faux-amis Peu de perles rares, instinct de volatile Hors-la-loi, postiché comme le Corbeau Noir Même si la vie ne vaut rien, rien ne vaut la vie À toutes les heures, la mort peut te heurter Si eux, ils sont pas des hommes, c'est parce qu'ils ont peur d'l'être Y'a pas d'issues pour s'échapper Le sang versé ne sèche jamais Y'a des os, des larmes quand un proche va dans l'au-delà Ils sont là pour de l'or, c'qu'on aime, au fond, c'est l'âme C'est pas la peau de l'homme, révolté comme Mandela Entre parenthèses, toujours là quand ça part en guerre Mes tortionnaires se mettent torse-nu comme la race des Saiyen On attend son heure à part entière On était forcés d'être forcenés Forcément, fallait qu'ça brille tah les phares xénon Faudrait qu'j'pense à faire des mômes Il faut rendre fier les nôtres avant qu'on enterre mes côtes J'veux qu'ils écoutent mes derniers mots Joue pas les so-per, merde, le monde est à nous, frère C'est pas qu'des foutaises ni des délires posés sur la braise Tu vois c'que j'veux dire donc je fuck mon putain d'couplet D'puis t'à l'heure il arrête pas d'déconner donc j'vais rebondir Et revenir, venir vous parler De c'qu'on peut faire seine Zoo, l'17 juin on est parés Déjà dans les bacs et les 'tasses se parlent mal Rien à foutre, vous êtes des chattes, vous avez pas compris on n'a pas l'time Donc j'essaye de faire des roulements en même temps d'improviser C'est un peu difficile mais y'a pas d'souci j'peux t'apprendre A atomiser la prod, à atomiser le mic Avec mes gavas on est àl et tu sais qu'on est trop haut Rien à foutre de ces 'tasses qui parlent mal Vas-y Fennek balance-leur des flammes pour qu'ils captent En plus ouais j'suis prêt c'est Destins liés, il est dans les bacs J'fais tourner si jamais il m'reste un billet C'est comme ça qu'je l'fais Et puis quand j'ai la dalle, man, tu connais Comme un chacal j'pense au festin d'hier C'est comme ça qu'j'le aif, en improvi Quand t'es chaud qu'tu balances des roulements C'est comme ça qu'j'le fais, le déroulement, du putain d'truc C'est comme ça qu'ça s'passe dans l'espace C'est Nek le Fenek, laisse-moi j'bébar J'm'arrache en Vespa, n'est-ce pas C'est comme ça qu'on l'fait avec la vraie classe Mes gars le savent depuis l'époque de la Sega C'est comme ça qu'on l'fait mais personne n'égale mes gars Mes gars, ouais on XXX Comment t'expliquer qu'on est là, ouais, depuis bas âge ? Pour mes gavas du ze-qui, pour mes gavas du 19 9 PC dans les khos, 9 PC dans les eaux Ouais c'est ça les G's depuis longtemps, on est àl Rien à foutre des 'tasses qui parlent mal de l'équipe On va les cramer comme la Pall Mall ou la Gitane sans filtre Est-ce que tu captes les G's ? On te parle sans filtre On te parle sans rime On te parle juste avec des idées qui sortent, j'empile Toutes sortes de techniques, toutes sortes de flammes ouais Toutes sortes de phases, Seine Zoo est dans les bacs Mohofucker Seine Zoo est dans les bacs, faut qu'tu l'achètes, frère C'est comme ça qu'on l'fait, c'est un lâché d'verses On lâche plein d'trucs ouais on déconne frère J'ai appris plus de trucs avec les potes que à l'école frère J'ai mis le Seine Zoo, t'as le col V C'est comme ça qu'on l'fait, même y'a des décolletés De l'autre côté C'est comme ça qu'on l'fait, trop souvent boycottés Maintenant on est des boys cotés S-Crew boy Comment t'expliquer qu'on arrive, on va t'désosser Tous ces putains d'enfoirés tels des bouchers Le buf, rappelle-toi de la phase de mon reuf zer-2 On peut t'coucher comme si c'était d'la peuf Ou bien juste quelques rimes Ouais, ah fucked up j'n'ai plus l'temps pour terminer aç Donc c'est déjà l'17 là, il faut pécher l'bail Il faut pécher l'bail, Doums et Nek tuent en impro On t'regarde derrière les nettes-lu et ouais gros C'est comme ça qu'on l'fait, j'ai la berlu Comique comme Berlusconi C'est comme ça qu'on l'fait, ouais ouais homie C'est comme ça que j'passe, y'a le Jack Honey Les filles au lit, c'est comme ça qu'on l'fait Mon gars on fidélise, c'est comme ça qu'on l'fait On fuit la lice-po, ouais gros, en impro Avec mes frérots, c'est toujours réglo On fume le matos, on fait tourner le micro avec les frérots Seine Zoo, Destins Liés, reste cool ou j'vais te briser Le peuple est endetté mais ceux qui gèrent les banques ils s'font Des couilles en or sur ta tête pendant que la banquise fond Éparpillés sur l'avenue, ça y est on y est parvenus Bienvenu aux nouveaux venus mais les groupies c'est farfelu Tous ces clones, écartez-les, surtout quand ça parle de rap Faut arracher l'cro-mi des faux chroniqueurs télé T'as vu l'atmosphère qu'on s'prend ? Obsédés par les morts C'est comme si on parlait morse vu qu'on tape pour s'faire comprendre Sur l'amour tire un trait, j'te fais pas de dessin Mon cur, pas facile d'y rentrer, surtout qu'en bas y'a les zins La vie, un voyage compliqué, pourtant y'a qu'un aller simple C'est pas net, j'me sens comme un humain sur la Planète des singes J'aimerais regarder le passé et me dire Putain, ce fut dur Et regarder devant, que Dieu m'accorde un futur Tirer entre la foi, la folie et la fortune L'équation est simple si je n'réussis pas, j'suis foutu Je fais pas du rap que pour moi, ça c'est vrai Quand je m'imagine devenant esclave de la machine J'ai le pouls qui s'accélère Après la crise cardiaque ils diront que j'avais du cur Ou attendront que j'dead pour dire que j'étais le meilleur Mon âme titube, la faucheuse demande De quelle origine es-tu ? Je suis métisse mi-ange mi-démon Parce que la banlieue démonte Faut faire face à toute mise à l'amende Apparemment pour la guerre il leurs faut deux mots Debout, prenez vos bitches, vos bifs, vos teilles-bou Portez vos les-bou ou barrez vous à l'autre bout du monde Juste avant de mourir je leur dirai ni comment ni pourquoi En chuchotant seulement à l'oreille John, c'est moi !1</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>2zer Washington</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>ViperGts</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
         <is>
           <t>Ouais ouais, ouais ouais, ouais ouais, ouais ouais Ouais ouais, ouais ouais, ouais ouais, ouais ouais Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de style, pas d'image, pas de robot, même pas dimanche Et des comme moi pas des masses, je fais du son, je m'alimente Dans les recoins de Paris Nord, j'ai le micro et le maniement On fait parti des monuments, y a pas de race dominante Gole-ri, travail, abdominaux, mes potos tombent comme dominos Pleure pour des choses abominables, sèche mes larmes avec money, man Ils volent nos terres en no limit, je me sens comme Geronimo Trahi comme dans Many Men, mon cur mesure 9 millimètres Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais T'as pas de team, pas d'équipe, tes meilleurs sons, c'est que des feats Ouais, si tu quittes, on est quittes, tu payes tes flows en liquide Passe les rapports salement, ça embrebouille calmement Y a les 22 droit devant, bombe, ils passent en coup de vent T'allumes une clope, ça fout le mort, la prochaine fois, j'te fous dehors Que les gros spliffs autorisés, dans mon salon motorisé Très peu de frères, plein d'ennemis, dans les deux cas, t'en paye le prix 11.01.91, j'ai vu le jour en pleine nuit Rien n'me ralenti comme argent blanchi J'arrive en bande, ce soir, le capot d'la Banji Rien n'me ralenti, arrivederci J'suis dans la Viper GTS ou dans la Banji Turbo ouais, mets les voiles ouais Turbo ouais, mets les voiles ouais1</t>
         </is>

</xml_diff>